<commit_message>
Okno serwisowe - aktualizacja plików Excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_OiDanych\_SDG\_dyzur\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1486,7 +1486,7 @@
     <t>17.3.1 Official development assistance (ODA) as a proportion of total domestic budget</t>
   </si>
   <si>
-    <t>Ministry of Finance Republic of Poland / Ministry of Foreign Affairs Republic of Poland</t>
+    <t>Ministry of Finance Republic of Poland / Ministry of Foreign Affairs Republic  of Poland</t>
   </si>
   <si>
     <t>17.3.2 Volume of remittances (in United States dollars) as a proportion of total GDP</t>
@@ -1534,10 +1534,10 @@
     <t>macroeconomic indicator</t>
   </si>
   <si>
-    <t>GDP per capita in EUR (current prices)</t>
-  </si>
-  <si>
-    <t>euro</t>
+    <t>GDP per capita in PLN (current prices)</t>
+  </si>
+  <si>
+    <t>PLN, [-], percent [%]</t>
   </si>
   <si>
     <t>indices of GDP (constant prices)</t>
@@ -1591,7 +1591,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 07-04-2020, 13:55</t>
+    <t>Last update: 21-04-2020, 13:22</t>
   </si>
 </sst>
 </file>
@@ -2139,7 +2139,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3196,7 +3196,9 @@
       <c r="M24" s="4">
         <v>63.3</v>
       </c>
-      <c r="N24" s="3"/>
+      <c r="N24" s="4">
+        <v>62.6</v>
+      </c>
       <c r="O24" s="3"/>
       <c r="P24" s="2" t="s">
         <v>22</v>
@@ -3242,7 +3244,9 @@
       <c r="M25" s="4">
         <v>11.4</v>
       </c>
-      <c r="N25" s="3"/>
+      <c r="N25" s="4">
+        <v>11.6</v>
+      </c>
       <c r="O25" s="3"/>
       <c r="P25" s="2" t="s">
         <v>22</v>
@@ -3288,7 +3292,9 @@
       <c r="M26" s="4">
         <v>11.9</v>
       </c>
-      <c r="N26" s="3"/>
+      <c r="N26" s="4">
+        <v>12</v>
+      </c>
       <c r="O26" s="3"/>
       <c r="P26" s="2" t="s">
         <v>22</v>
@@ -3334,7 +3340,9 @@
       <c r="M27" s="4">
         <v>40</v>
       </c>
-      <c r="N27" s="3"/>
+      <c r="N27" s="4">
+        <v>39</v>
+      </c>
       <c r="O27" s="3"/>
       <c r="P27" s="2" t="s">
         <v>22</v>
@@ -3866,7 +3874,9 @@
       <c r="M39" s="5">
         <v>0.36</v>
       </c>
-      <c r="N39" s="3"/>
+      <c r="N39" s="5">
+        <v>0.57999999999999996</v>
+      </c>
       <c r="O39" s="3"/>
       <c r="P39" s="2" t="s">
         <v>76</v>
@@ -3954,7 +3964,9 @@
       <c r="M41" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="N41" s="3"/>
+      <c r="N41" s="4">
+        <v>1.3</v>
+      </c>
       <c r="O41" s="3"/>
       <c r="P41" s="2" t="s">
         <v>22</v>
@@ -4243,7 +4255,9 @@
       <c r="N47" s="6">
         <v>28</v>
       </c>
-      <c r="O47" s="3"/>
+      <c r="O47" s="6">
+        <v>25</v>
+      </c>
       <c r="P47" s="2" t="s">
         <v>86</v>
       </c>
@@ -4384,7 +4398,9 @@
       <c r="M50" s="4">
         <v>434.8</v>
       </c>
-      <c r="N50" s="3"/>
+      <c r="N50" s="4">
+        <v>437.2</v>
+      </c>
       <c r="O50" s="3"/>
       <c r="P50" s="2" t="s">
         <v>22</v>
@@ -4430,7 +4446,9 @@
       <c r="M51" s="4">
         <v>22.9</v>
       </c>
-      <c r="N51" s="3"/>
+      <c r="N51" s="4">
+        <v>23.5</v>
+      </c>
       <c r="O51" s="3"/>
       <c r="P51" s="2" t="s">
         <v>22</v>
@@ -4476,7 +4494,9 @@
       <c r="M52" s="4">
         <v>259.3</v>
       </c>
-      <c r="N52" s="3"/>
+      <c r="N52" s="4">
+        <v>263.89999999999998</v>
+      </c>
       <c r="O52" s="3"/>
       <c r="P52" s="2" t="s">
         <v>22</v>
@@ -4522,7 +4542,9 @@
       <c r="M53" s="4">
         <v>26.4</v>
       </c>
-      <c r="N53" s="3"/>
+      <c r="N53" s="4">
+        <v>24.6</v>
+      </c>
       <c r="O53" s="3"/>
       <c r="P53" s="2" t="s">
         <v>22</v>
@@ -4568,7 +4590,9 @@
       <c r="M54" s="4">
         <v>11.7</v>
       </c>
-      <c r="N54" s="3"/>
+      <c r="N54" s="4">
+        <v>11.6</v>
+      </c>
       <c r="O54" s="3"/>
       <c r="P54" s="2" t="s">
         <v>22</v>
@@ -4614,7 +4638,9 @@
       <c r="M55" s="4">
         <v>20.9</v>
       </c>
-      <c r="N55" s="3"/>
+      <c r="N55" s="4">
+        <v>20.8</v>
+      </c>
       <c r="O55" s="3"/>
       <c r="P55" s="2" t="s">
         <v>22</v>
@@ -4660,7 +4686,9 @@
       <c r="M56" s="4">
         <v>3</v>
       </c>
-      <c r="N56" s="3"/>
+      <c r="N56" s="4">
+        <v>2.9</v>
+      </c>
       <c r="O56" s="3"/>
       <c r="P56" s="2" t="s">
         <v>22</v>
@@ -4980,7 +5008,9 @@
       <c r="M63" s="4">
         <v>0.6</v>
       </c>
-      <c r="N63" s="3"/>
+      <c r="N63" s="4">
+        <v>0.8</v>
+      </c>
       <c r="O63" s="3"/>
       <c r="P63" s="2" t="s">
         <v>22</v>
@@ -9259,8 +9289,12 @@
       <c r="L175" s="6">
         <v>145185</v>
       </c>
-      <c r="M175" s="3"/>
-      <c r="N175" s="3"/>
+      <c r="M175" s="6">
+        <v>153374</v>
+      </c>
+      <c r="N175" s="6">
+        <v>153374</v>
+      </c>
       <c r="O175" s="3"/>
       <c r="P175" s="2" t="s">
         <v>225</v>
@@ -9904,7 +9938,9 @@
         <v>26.37</v>
       </c>
       <c r="M190" s="3"/>
-      <c r="N190" s="3"/>
+      <c r="N190" s="5">
+        <v>27.79</v>
+      </c>
       <c r="O190" s="3"/>
       <c r="P190" s="2" t="s">
         <v>22</v>
@@ -9942,7 +9978,9 @@
         <v>27.79</v>
       </c>
       <c r="M191" s="3"/>
-      <c r="N191" s="3"/>
+      <c r="N191" s="5">
+        <v>29.47</v>
+      </c>
       <c r="O191" s="3"/>
       <c r="P191" s="2" t="s">
         <v>22</v>
@@ -9980,7 +10018,9 @@
         <v>24.79</v>
       </c>
       <c r="M192" s="3"/>
-      <c r="N192" s="3"/>
+      <c r="N192" s="5">
+        <v>25.94</v>
+      </c>
       <c r="O192" s="3"/>
       <c r="P192" s="2" t="s">
         <v>22</v>
@@ -10018,7 +10058,9 @@
         <v>52.11</v>
       </c>
       <c r="M193" s="3"/>
-      <c r="N193" s="3"/>
+      <c r="N193" s="5">
+        <v>51.95</v>
+      </c>
       <c r="O193" s="3"/>
       <c r="P193" s="2" t="s">
         <v>22</v>
@@ -10056,7 +10098,9 @@
         <v>36.17</v>
       </c>
       <c r="M194" s="3"/>
-      <c r="N194" s="3"/>
+      <c r="N194" s="5">
+        <v>37.49</v>
+      </c>
       <c r="O194" s="3"/>
       <c r="P194" s="2" t="s">
         <v>22</v>
@@ -10094,7 +10138,9 @@
         <v>26.12</v>
       </c>
       <c r="M195" s="3"/>
-      <c r="N195" s="3"/>
+      <c r="N195" s="5">
+        <v>26.78</v>
+      </c>
       <c r="O195" s="3"/>
       <c r="P195" s="2" t="s">
         <v>22</v>
@@ -10132,7 +10178,9 @@
         <v>20.8</v>
       </c>
       <c r="M196" s="3"/>
-      <c r="N196" s="3"/>
+      <c r="N196" s="5">
+        <v>21.85</v>
+      </c>
       <c r="O196" s="3"/>
       <c r="P196" s="2" t="s">
         <v>22</v>
@@ -10170,7 +10218,9 @@
         <v>15.93</v>
       </c>
       <c r="M197" s="3"/>
-      <c r="N197" s="3"/>
+      <c r="N197" s="5">
+        <v>16.91</v>
+      </c>
       <c r="O197" s="3"/>
       <c r="P197" s="2" t="s">
         <v>22</v>
@@ -10208,7 +10258,9 @@
         <v>17.29</v>
       </c>
       <c r="M198" s="3"/>
-      <c r="N198" s="3"/>
+      <c r="N198" s="5">
+        <v>18.309999999999999</v>
+      </c>
       <c r="O198" s="3"/>
       <c r="P198" s="2" t="s">
         <v>22</v>
@@ -10246,7 +10298,9 @@
         <v>19.84</v>
       </c>
       <c r="M199" s="3"/>
-      <c r="N199" s="3"/>
+      <c r="N199" s="5">
+        <v>21.98</v>
+      </c>
       <c r="O199" s="3"/>
       <c r="P199" s="2" t="s">
         <v>22</v>
@@ -10284,7 +10338,9 @@
         <v>20.2</v>
       </c>
       <c r="M200" s="3"/>
-      <c r="N200" s="3"/>
+      <c r="N200" s="5">
+        <v>21.7</v>
+      </c>
       <c r="O200" s="3"/>
       <c r="P200" s="2" t="s">
         <v>22</v>
@@ -10322,7 +10378,9 @@
         <v>15.35</v>
       </c>
       <c r="M201" s="3"/>
-      <c r="N201" s="3"/>
+      <c r="N201" s="5">
+        <v>16.22</v>
+      </c>
       <c r="O201" s="3"/>
       <c r="P201" s="2" t="s">
         <v>22</v>
@@ -10360,7 +10418,9 @@
         <v>17.14</v>
       </c>
       <c r="M202" s="3"/>
-      <c r="N202" s="3"/>
+      <c r="N202" s="5">
+        <v>18.809999999999999</v>
+      </c>
       <c r="O202" s="3"/>
       <c r="P202" s="2" t="s">
         <v>22</v>
@@ -10398,7 +10458,9 @@
         <v>24.29</v>
       </c>
       <c r="M203" s="3"/>
-      <c r="N203" s="3"/>
+      <c r="N203" s="5">
+        <v>25.91</v>
+      </c>
       <c r="O203" s="3"/>
       <c r="P203" s="2" t="s">
         <v>22</v>
@@ -10436,7 +10498,9 @@
         <v>28.98</v>
       </c>
       <c r="M204" s="3"/>
-      <c r="N204" s="3"/>
+      <c r="N204" s="5">
+        <v>30.29</v>
+      </c>
       <c r="O204" s="3"/>
       <c r="P204" s="2" t="s">
         <v>22</v>
@@ -10474,7 +10538,9 @@
         <v>27.63</v>
       </c>
       <c r="M205" s="3"/>
-      <c r="N205" s="3"/>
+      <c r="N205" s="5">
+        <v>29.02</v>
+      </c>
       <c r="O205" s="3"/>
       <c r="P205" s="2" t="s">
         <v>22</v>
@@ -10512,7 +10578,9 @@
         <v>25.87</v>
       </c>
       <c r="M206" s="3"/>
-      <c r="N206" s="3"/>
+      <c r="N206" s="5">
+        <v>26.84</v>
+      </c>
       <c r="O206" s="3"/>
       <c r="P206" s="2" t="s">
         <v>22</v>
@@ -10550,7 +10618,9 @@
         <v>27.61</v>
       </c>
       <c r="M207" s="3"/>
-      <c r="N207" s="3"/>
+      <c r="N207" s="5">
+        <v>28.28</v>
+      </c>
       <c r="O207" s="3"/>
       <c r="P207" s="2" t="s">
         <v>22</v>
@@ -10588,7 +10658,9 @@
         <v>34.18</v>
       </c>
       <c r="M208" s="3"/>
-      <c r="N208" s="3"/>
+      <c r="N208" s="5">
+        <v>38.65</v>
+      </c>
       <c r="O208" s="3"/>
       <c r="P208" s="2" t="s">
         <v>22</v>
@@ -10637,7 +10709,9 @@
       <c r="N209" s="4">
         <v>3.8</v>
       </c>
-      <c r="O209" s="3"/>
+      <c r="O209" s="4">
+        <v>3.3</v>
+      </c>
       <c r="P209" s="2" t="s">
         <v>22</v>
       </c>
@@ -10685,7 +10759,9 @@
       <c r="N210" s="4">
         <v>3.8</v>
       </c>
-      <c r="O210" s="3"/>
+      <c r="O210" s="4">
+        <v>3</v>
+      </c>
       <c r="P210" s="2" t="s">
         <v>22</v>
       </c>
@@ -10733,7 +10809,9 @@
       <c r="N211" s="4">
         <v>3.8</v>
       </c>
-      <c r="O211" s="3"/>
+      <c r="O211" s="4">
+        <v>3.6</v>
+      </c>
       <c r="P211" s="2" t="s">
         <v>22</v>
       </c>
@@ -10781,7 +10859,9 @@
       <c r="N212" s="4">
         <v>11.7</v>
       </c>
-      <c r="O212" s="3"/>
+      <c r="O212" s="4">
+        <v>9.9</v>
+      </c>
       <c r="P212" s="2" t="s">
         <v>22</v>
       </c>
@@ -10829,7 +10909,9 @@
       <c r="N213" s="4">
         <v>4.3</v>
       </c>
-      <c r="O213" s="3"/>
+      <c r="O213" s="4">
+        <v>3.7</v>
+      </c>
       <c r="P213" s="2" t="s">
         <v>22</v>
       </c>
@@ -10877,7 +10959,9 @@
       <c r="N214" s="4">
         <v>2.9</v>
       </c>
-      <c r="O214" s="3"/>
+      <c r="O214" s="4">
+        <v>2.6</v>
+      </c>
       <c r="P214" s="2" t="s">
         <v>22</v>
       </c>
@@ -10925,7 +11009,9 @@
       <c r="N215" s="4">
         <v>2.9</v>
       </c>
-      <c r="O215" s="3"/>
+      <c r="O215" s="4">
+        <v>2.4</v>
+      </c>
       <c r="P215" s="2" t="s">
         <v>22</v>
       </c>
@@ -10973,7 +11059,9 @@
       <c r="N216" s="4">
         <v>2.5</v>
       </c>
-      <c r="O216" s="3"/>
+      <c r="O216" s="4">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="P216" s="2" t="s">
         <v>22</v>
       </c>
@@ -11021,7 +11109,9 @@
       <c r="N217" s="4">
         <v>6.5</v>
       </c>
-      <c r="O217" s="3"/>
+      <c r="O217" s="4">
+        <v>6.5</v>
+      </c>
       <c r="P217" s="2" t="s">
         <v>22</v>
       </c>
@@ -14175,7 +14265,9 @@
       <c r="N287" s="5">
         <v>6.19</v>
       </c>
-      <c r="O287" s="3"/>
+      <c r="O287" s="5">
+        <v>9.5299999999999994</v>
+      </c>
       <c r="P287" s="2" t="s">
         <v>337</v>
       </c>
@@ -14223,7 +14315,9 @@
       <c r="N288" s="5">
         <v>766.04</v>
       </c>
-      <c r="O288" s="3"/>
+      <c r="O288" s="5">
+        <v>684.46</v>
+      </c>
       <c r="P288" s="2" t="s">
         <v>341</v>
       </c>
@@ -14271,7 +14365,9 @@
       <c r="N289" s="5">
         <v>244.93</v>
       </c>
-      <c r="O289" s="3"/>
+      <c r="O289" s="5">
+        <v>144.66999999999999</v>
+      </c>
       <c r="P289" s="2" t="s">
         <v>341</v>
       </c>
@@ -17822,7 +17918,9 @@
       <c r="M364" s="7">
         <v>0.19800000000000001</v>
       </c>
-      <c r="N364" s="3"/>
+      <c r="N364" s="7">
+        <v>0.19800000000000001</v>
+      </c>
       <c r="O364" s="3"/>
       <c r="P364" s="2" t="s">
         <v>429</v>
@@ -18318,7 +18416,9 @@
       <c r="M377" s="5">
         <v>0.68</v>
       </c>
-      <c r="N377" s="3"/>
+      <c r="N377" s="5">
+        <v>0.53</v>
+      </c>
       <c r="O377" s="3"/>
       <c r="P377" s="2" t="s">
         <v>22</v>
@@ -18479,15 +18579,17 @@
       <c r="J381" s="3"/>
       <c r="K381" s="3"/>
       <c r="L381" s="6">
-        <v>1429</v>
+        <v>1426</v>
       </c>
       <c r="M381" s="6">
-        <v>1424</v>
+        <v>1421</v>
       </c>
       <c r="N381" s="6">
         <v>1475</v>
       </c>
-      <c r="O381" s="3"/>
+      <c r="O381" s="6">
+        <v>1603</v>
+      </c>
       <c r="P381" s="2" t="s">
         <v>451</v>
       </c>
@@ -18518,12 +18620,14 @@
         <v>212</v>
       </c>
       <c r="M382" s="6">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N382" s="6">
-        <v>198</v>
-      </c>
-      <c r="O382" s="3"/>
+        <v>204</v>
+      </c>
+      <c r="O382" s="6">
+        <v>236</v>
+      </c>
       <c r="P382" s="2" t="s">
         <v>451</v>
       </c>
@@ -18551,15 +18655,17 @@
       <c r="J383" s="3"/>
       <c r="K383" s="3"/>
       <c r="L383" s="6">
-        <v>1214</v>
+        <v>1208</v>
       </c>
       <c r="M383" s="6">
-        <v>1200</v>
+        <v>1197</v>
       </c>
       <c r="N383" s="6">
-        <v>1233</v>
-      </c>
-      <c r="O383" s="3"/>
+        <v>1264</v>
+      </c>
+      <c r="O383" s="6">
+        <v>1359</v>
+      </c>
       <c r="P383" s="2" t="s">
         <v>451</v>
       </c>
@@ -18587,15 +18693,17 @@
       <c r="J384" s="3"/>
       <c r="K384" s="3"/>
       <c r="L384" s="6">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="M384" s="6">
-        <v>1193</v>
+        <v>1211</v>
       </c>
       <c r="N384" s="6">
+        <v>1270</v>
+      </c>
+      <c r="O384" s="6">
         <v>1379</v>
       </c>
-      <c r="O384" s="3"/>
       <c r="P384" s="2" t="s">
         <v>451</v>
       </c>
@@ -18626,12 +18734,14 @@
         <v>153</v>
       </c>
       <c r="M385" s="6">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N385" s="6">
-        <v>195</v>
-      </c>
-      <c r="O385" s="3"/>
+        <v>186</v>
+      </c>
+      <c r="O385" s="6">
+        <v>196</v>
+      </c>
       <c r="P385" s="2" t="s">
         <v>451</v>
       </c>
@@ -18662,12 +18772,14 @@
         <v>879</v>
       </c>
       <c r="M386" s="6">
-        <v>1025</v>
+        <v>1021</v>
       </c>
       <c r="N386" s="6">
-        <v>1178</v>
-      </c>
-      <c r="O386" s="3"/>
+        <v>1078</v>
+      </c>
+      <c r="O386" s="6">
+        <v>1175</v>
+      </c>
       <c r="P386" s="2" t="s">
         <v>451</v>
       </c>
@@ -18695,7 +18807,7 @@
       <c r="J387" s="3"/>
       <c r="K387" s="3"/>
       <c r="L387" s="6">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M387" s="6">
         <v>116</v>
@@ -18703,7 +18815,9 @@
       <c r="N387" s="6">
         <v>159</v>
       </c>
-      <c r="O387" s="3"/>
+      <c r="O387" s="6">
+        <v>110</v>
+      </c>
       <c r="P387" s="2" t="s">
         <v>451</v>
       </c>
@@ -18731,7 +18845,7 @@
       <c r="J388" s="3"/>
       <c r="K388" s="3"/>
       <c r="L388" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M388" s="3"/>
       <c r="N388" s="3"/>
@@ -18763,15 +18877,17 @@
       <c r="J389" s="3"/>
       <c r="K389" s="3"/>
       <c r="L389" s="6">
-        <v>1274</v>
+        <v>1277</v>
       </c>
       <c r="M389" s="6">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="N389" s="6">
         <v>1259</v>
       </c>
-      <c r="O389" s="3"/>
+      <c r="O389" s="6">
+        <v>1400</v>
+      </c>
       <c r="P389" s="2" t="s">
         <v>451</v>
       </c>
@@ -18802,12 +18918,14 @@
         <v>67</v>
       </c>
       <c r="M390" s="6">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="N390" s="6">
         <v>57</v>
       </c>
-      <c r="O390" s="3"/>
+      <c r="O390" s="6">
+        <v>93</v>
+      </c>
       <c r="P390" s="2" t="s">
         <v>451</v>
       </c>
@@ -18903,7 +19021,9 @@
       <c r="N392" s="6">
         <v>13407</v>
       </c>
-      <c r="O392" s="3"/>
+      <c r="O392" s="6">
+        <v>9367</v>
+      </c>
       <c r="P392" s="2" t="s">
         <v>467</v>
       </c>
@@ -19657,7 +19777,9 @@
       <c r="N411" s="4">
         <v>0.7</v>
       </c>
-      <c r="O411" s="3"/>
+      <c r="O411" s="4">
+        <v>0.7</v>
+      </c>
       <c r="P411" s="2" t="s">
         <v>487</v>
       </c>
@@ -19753,7 +19875,9 @@
       <c r="N413" s="4">
         <v>2.5</v>
       </c>
-      <c r="O413" s="3"/>
+      <c r="O413" s="4">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="P413" s="2" t="s">
         <v>490</v>
       </c>
@@ -19776,7 +19900,7 @@
       </c>
       <c r="F414" s="3"/>
       <c r="G414" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H414" s="6">
         <v>2</v>
@@ -19799,7 +19923,9 @@
       <c r="N414" s="6">
         <v>1</v>
       </c>
-      <c r="O414" s="3"/>
+      <c r="O414" s="6">
+        <v>2</v>
+      </c>
       <c r="P414" s="2" t="s">
         <v>492</v>
       </c>
@@ -19980,10 +20106,10 @@
         <v>62.3</v>
       </c>
       <c r="I418" s="4">
-        <v>63.9</v>
+        <v>62.8</v>
       </c>
       <c r="J418" s="4">
-        <v>67.2</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="K418" s="4">
         <v>68</v>
@@ -19994,8 +20120,12 @@
       <c r="M418" s="4">
         <v>76</v>
       </c>
-      <c r="N418" s="3"/>
-      <c r="O418" s="3"/>
+      <c r="N418" s="4">
+        <v>77.5</v>
+      </c>
+      <c r="O418" s="4">
+        <v>80.400000000000006</v>
+      </c>
       <c r="P418" s="2" t="s">
         <v>22</v>
       </c>
@@ -20043,7 +20173,9 @@
       <c r="N419" s="4">
         <v>766</v>
       </c>
-      <c r="O419" s="3"/>
+      <c r="O419" s="4">
+        <v>684.5</v>
+      </c>
       <c r="P419" s="2" t="s">
         <v>79</v>
       </c>
@@ -20091,7 +20223,9 @@
       <c r="N420" s="5">
         <v>1.27</v>
       </c>
-      <c r="O420" s="3"/>
+      <c r="O420" s="5">
+        <v>1.26</v>
+      </c>
       <c r="P420" s="2" t="s">
         <v>441</v>
       </c>
@@ -20113,35 +20247,35 @@
         <v>504</v>
       </c>
       <c r="F421" s="6">
-        <v>9400</v>
+        <v>37524</v>
       </c>
       <c r="G421" s="6">
-        <v>9900</v>
+        <v>40669</v>
       </c>
       <c r="H421" s="6">
-        <v>10100</v>
+        <v>42285</v>
       </c>
       <c r="I421" s="6">
-        <v>10300</v>
+        <v>43034</v>
       </c>
       <c r="J421" s="6">
-        <v>10700</v>
+        <v>44705</v>
       </c>
       <c r="K421" s="6">
-        <v>11200</v>
+        <v>46814</v>
       </c>
       <c r="L421" s="6">
-        <v>11100</v>
+        <v>48433</v>
       </c>
       <c r="M421" s="6">
-        <v>12200</v>
+        <v>51776</v>
       </c>
       <c r="N421" s="6">
-        <v>12900</v>
+        <v>55066</v>
       </c>
       <c r="O421" s="3"/>
       <c r="P421" s="2" t="s">
-        <v>240</v>
+        <v>22</v>
       </c>
     </row>
     <row r="422" spans="1:16" ht="27" x14ac:dyDescent="0.25">
@@ -20182,14 +20316,16 @@
         <v>103.1</v>
       </c>
       <c r="M422" s="4">
-        <v>104.8</v>
+        <v>104.9</v>
       </c>
       <c r="N422" s="4">
         <v>105.1</v>
       </c>
-      <c r="O422" s="3"/>
+      <c r="O422" s="4">
+        <v>104.1</v>
+      </c>
       <c r="P422" s="2" t="s">
-        <v>240</v>
+        <v>22</v>
       </c>
     </row>
     <row r="423" spans="1:16" ht="18" x14ac:dyDescent="0.25">
@@ -20230,14 +20366,14 @@
         <v>18</v>
       </c>
       <c r="M423" s="4">
-        <v>17.7</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="N423" s="4">
         <v>18.2</v>
       </c>
       <c r="O423" s="3"/>
       <c r="P423" s="2" t="s">
-        <v>240</v>
+        <v>22</v>
       </c>
     </row>
     <row r="424" spans="1:16" ht="36" x14ac:dyDescent="0.25">
@@ -20280,10 +20416,14 @@
       <c r="M424" s="4">
         <v>102</v>
       </c>
-      <c r="N424" s="3"/>
-      <c r="O424" s="3"/>
+      <c r="N424" s="4">
+        <v>101.6</v>
+      </c>
+      <c r="O424" s="4">
+        <v>102.3</v>
+      </c>
       <c r="P424" s="2" t="s">
-        <v>240</v>
+        <v>22</v>
       </c>
     </row>
     <row r="425" spans="1:16" ht="36" x14ac:dyDescent="0.25">
@@ -20331,7 +20471,7 @@
       </c>
       <c r="O425" s="3"/>
       <c r="P425" s="2" t="s">
-        <v>240</v>
+        <v>22</v>
       </c>
     </row>
     <row r="426" spans="1:16" ht="36" x14ac:dyDescent="0.25">
@@ -20351,35 +20491,35 @@
         <v>504</v>
       </c>
       <c r="F426" s="4">
-        <v>-7.3</v>
+        <v>-7.4</v>
       </c>
       <c r="G426" s="4">
-        <v>-4.8</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="H426" s="4">
         <v>-3.7</v>
       </c>
       <c r="I426" s="4">
-        <v>-4.0999999999999996</v>
+        <v>-4.2</v>
       </c>
       <c r="J426" s="4">
-        <v>-3.7</v>
+        <v>-3.6</v>
       </c>
       <c r="K426" s="4">
-        <v>-2.7</v>
+        <v>-2.6</v>
       </c>
       <c r="L426" s="4">
-        <v>-2.2000000000000002</v>
+        <v>-2.4</v>
       </c>
       <c r="M426" s="4">
         <v>-1.5</v>
       </c>
       <c r="N426" s="4">
-        <v>-0.4</v>
+        <v>-0.2</v>
       </c>
       <c r="O426" s="3"/>
       <c r="P426" s="2" t="s">
-        <v>240</v>
+        <v>22</v>
       </c>
     </row>
     <row r="427" spans="1:16" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
okno serwisowe xlsx, api
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -1652,7 +1652,7 @@
     <t xml:space="preserve">100% deaths registration</t>
   </si>
   <si>
-    <t xml:space="preserve">Last update: 08-06-2021, 08:32</t>
+    <t xml:space="preserve">Last update: 13-07-2021, 08:08</t>
   </si>
 </sst>
 </file>
@@ -4002,7 +4002,9 @@
       <c r="O43" s="6" t="n">
         <v>99.8</v>
       </c>
-      <c r="P43" s="5"/>
+      <c r="P43" s="6" t="n">
+        <v>99.7</v>
+      </c>
       <c r="Q43" s="4" t="s">
         <v>22</v>
       </c>
@@ -4051,7 +4053,9 @@
       <c r="O44" s="6" t="n">
         <v>4.4</v>
       </c>
-      <c r="P44" s="5"/>
+      <c r="P44" s="6" t="n">
+        <v>4.2</v>
+      </c>
       <c r="Q44" s="4" t="s">
         <v>22</v>
       </c>
@@ -4100,7 +4104,9 @@
       <c r="O45" s="6" t="n">
         <v>2.7</v>
       </c>
-      <c r="P45" s="5"/>
+      <c r="P45" s="6" t="n">
+        <v>2.6</v>
+      </c>
       <c r="Q45" s="4" t="s">
         <v>22</v>
       </c>
@@ -4890,7 +4896,9 @@
       <c r="O61" s="6" t="n">
         <v>4.5</v>
       </c>
-      <c r="P61" s="5"/>
+      <c r="P61" s="6" t="n">
+        <v>3.8</v>
+      </c>
       <c r="Q61" s="4" t="s">
         <v>22</v>
       </c>
@@ -4941,7 +4949,9 @@
       <c r="O62" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="P62" s="5"/>
+      <c r="P62" s="6" t="n">
+        <v>0</v>
+      </c>
       <c r="Q62" s="4" t="s">
         <v>22</v>
       </c>
@@ -4990,9 +5000,11 @@
         <v>10.2</v>
       </c>
       <c r="O63" s="6" t="n">
-        <v>9.4</v>
-      </c>
-      <c r="P63" s="5"/>
+        <v>9.3</v>
+      </c>
+      <c r="P63" s="6" t="n">
+        <v>8.1</v>
+      </c>
       <c r="Q63" s="4" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Okno serwisowe 24.08.2021, aktualizacja
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1663,7 +1663,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 10-08-2021, 12:23</t>
+    <t>Last update: 24-08-2021, 09:56</t>
   </si>
 </sst>
 </file>
@@ -2211,7 +2211,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23168,7 +23168,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="78" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="77" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
okno serwisowe - 21.09.2021
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="549">
   <si>
     <t>sdg.gov.pl/en</t>
   </si>
@@ -1237,7 +1237,7 @@
     <t>Wroclaw Agglomeration</t>
   </si>
   <si>
-    <t>PM 2.5 - by agglomeration</t>
+    <t xml:space="preserve"> PM 2.5 - by agglomeration</t>
   </si>
   <si>
     <t>11.a.1 Proportion of population living in gminas that have valid local spatial development plans or valid study of local spatial planning directions and determinants, by type of gminas - PROXY!</t>
@@ -1306,7 +1306,7 @@
     <t>12.6.1 The number of the signatories of the Partnership for the Implementation of the SDGs in Poland - PROXY!</t>
   </si>
   <si>
-    <t>the Ministry of Economic Development, Labour and Technology</t>
+    <t>the Ministry of Economic Development and Technology</t>
   </si>
   <si>
     <t>12.7.1 Number of countries implementing sustainable public procurement policies and action plans</t>
@@ -1636,9 +1636,6 @@
     <t>17.14.1 Number of countries with mechanisms in place to enhance policy coherence of sustainable development</t>
   </si>
   <si>
-    <t>the Ministry of Economic Development and Technology</t>
-  </si>
-  <si>
     <t>17.18.2 Number of countries that have national statistical legislation that complies with the Fundamental Principles of Official Statistics</t>
   </si>
   <si>
@@ -1672,7 +1669,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 07-09-2021, 13:39</t>
+    <t>Last update: 21-09-2021, 08:24</t>
   </si>
 </sst>
 </file>
@@ -2224,7 +2221,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22900,7 +22897,7 @@
       </c>
       <c r="Q443" s="3"/>
       <c r="R443" s="2" t="s">
-        <v>537</v>
+        <v>427</v>
       </c>
     </row>
     <row r="444" spans="1:18" ht="27" x14ac:dyDescent="0.25">
@@ -22908,7 +22905,7 @@
         <v>510</v>
       </c>
       <c r="B444" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>21</v>
@@ -22962,7 +22959,7 @@
         <v>510</v>
       </c>
       <c r="B445" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C445" s="2" t="s">
         <v>21</v>
@@ -23016,7 +23013,7 @@
         <v>510</v>
       </c>
       <c r="B446" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C446" s="2" t="s">
         <v>21</v>
@@ -23025,7 +23022,7 @@
         <v>22</v>
       </c>
       <c r="E446" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F446" s="3"/>
       <c r="G446" s="3"/>
@@ -23056,7 +23053,7 @@
       </c>
       <c r="Q446" s="3"/>
       <c r="R446" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="447" spans="1:18" ht="36" x14ac:dyDescent="0.25">
@@ -23064,13 +23061,13 @@
         <v>510</v>
       </c>
       <c r="B447" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C447" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="C447" s="2" t="s">
+      <c r="D447" s="3" t="s">
         <v>544</v>
-      </c>
-      <c r="D447" s="3" t="s">
-        <v>545</v>
       </c>
       <c r="E447" s="3" t="s">
         <v>176</v>
@@ -23092,7 +23089,7 @@
         <v>1</v>
       </c>
       <c r="R447" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="448" spans="1:18" ht="36" x14ac:dyDescent="0.25">
@@ -23100,13 +23097,13 @@
         <v>510</v>
       </c>
       <c r="B448" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C448" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="C448" s="2" t="s">
-        <v>544</v>
-      </c>
       <c r="D448" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E448" s="3" t="s">
         <v>176</v>
@@ -23148,7 +23145,7 @@
         <v>1</v>
       </c>
       <c r="R448" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="449" spans="1:18" ht="36" x14ac:dyDescent="0.25">
@@ -23156,13 +23153,13 @@
         <v>510</v>
       </c>
       <c r="B449" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C449" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="C449" s="2" t="s">
-        <v>544</v>
-      </c>
       <c r="D449" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E449" s="3" t="s">
         <v>176</v>
@@ -23204,13 +23201,13 @@
         <v>1</v>
       </c>
       <c r="R449" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="450" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="451" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A451" s="12" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B451" s="10"/>
     </row>
@@ -23225,7 +23222,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="78" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="77" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okno serwisowe - 19.10.2021
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1669,7 +1669,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 12-10-2021, 14:03</t>
+    <t>Last update: 19-10-2021, 08:27</t>
   </si>
 </sst>
 </file>
@@ -2221,7 +2221,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23222,7 +23222,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="78" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="77" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okno serwisowe - 23.11.2021
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1447,7 +1447,7 @@
     <t>15.b.1 Official development assistance and public expenditure on conservation and sustainable use of biodiversity and ecosystems</t>
   </si>
   <si>
-    <t>15.c.1 Proportion of traded wildlife that was poached or illicitly trafficked</t>
+    <t>15.c.1 The number of CITES individuals detained by custom officers</t>
   </si>
   <si>
     <t>Goal 16. Peace, justice and strong institutions</t>
@@ -1669,7 +1669,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 09-11-2021, 11:05</t>
+    <t>Last update: 24-11-2021, 11:15</t>
   </si>
 </sst>
 </file>
@@ -2221,7 +2221,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20718,7 +20718,7 @@
         <v>22</v>
       </c>
       <c r="E393" s="3" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="F393" s="7">
         <v>8495</v>
@@ -20755,7 +20755,7 @@
       </c>
       <c r="Q393" s="3"/>
       <c r="R393" s="2" t="s">
-        <v>21</v>
+        <v>470</v>
       </c>
     </row>
     <row r="394" spans="1:18" ht="27" x14ac:dyDescent="0.25">
@@ -21472,7 +21472,9 @@
       <c r="O409" s="7">
         <v>9367</v>
       </c>
-      <c r="P409" s="3"/>
+      <c r="P409" s="7">
+        <v>10438</v>
+      </c>
       <c r="Q409" s="3"/>
       <c r="R409" s="2" t="s">
         <v>497</v>
@@ -23414,7 +23416,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="78" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="77" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
aktualizacja - okno serwisowe 18.01.2022
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -178,7 +178,7 @@
     <t>by adoption and implementation of the national strategy</t>
   </si>
   <si>
-    <t>number</t>
+    <t>(0,1)</t>
   </si>
   <si>
     <t>Government Centre for Security (RCB)</t>
@@ -1693,7 +1693,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 18-01-2022, 08:15</t>
+    <t>Last update: 18-01-2022, 12:29</t>
   </si>
 </sst>
 </file>
@@ -2244,7 +2244,7 @@
   <dimension ref="A1:R455"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
@@ -2372,7 +2372,9 @@
       <c r="O4" s="4">
         <v>0.4</v>
       </c>
-      <c r="P4" s="3"/>
+      <c r="P4" s="4">
+        <v>0.2</v>
+      </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="2" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Wskaźnik 12-2-2 Aktualizacja PDF i Excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2828" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2828" uniqueCount="560">
   <si>
     <t>sdg.gov.pl/en</t>
   </si>
@@ -1303,6 +1303,9 @@
     <t>12.2.2 Domestic Material Consumption (DMC)</t>
   </si>
   <si>
+    <t>thous. tonnes, tonnes</t>
+  </si>
+  <si>
     <t>12.4.1 Number of parties to international multilateral environmental agreements on hazardous waste, and other chemicals that meet their commitments and obligations in transmitting information as required by each relevant agreement</t>
   </si>
   <si>
@@ -1699,7 +1702,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 07-06-2022, 09:55</t>
+    <t>Last update: 06-07-2022, 07:59</t>
   </si>
 </sst>
 </file>
@@ -20144,7 +20147,7 @@
         <v>22</v>
       </c>
       <c r="E375" s="3" t="s">
-        <v>280</v>
+        <v>426</v>
       </c>
       <c r="F375" s="4">
         <v>644835</v>
@@ -20198,7 +20201,7 @@
         <v>281</v>
       </c>
       <c r="E376" s="3" t="s">
-        <v>280</v>
+        <v>426</v>
       </c>
       <c r="F376" s="5">
         <v>16.95</v>
@@ -20243,7 +20246,7 @@
         <v>423</v>
       </c>
       <c r="B377" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>21</v>
@@ -20289,7 +20292,7 @@
       </c>
       <c r="Q377" s="3"/>
       <c r="R377" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="378" spans="1:18" ht="27" x14ac:dyDescent="0.25">
@@ -20297,16 +20300,16 @@
         <v>423</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D378" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E378" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F378" s="6">
         <v>39</v>
@@ -20331,7 +20334,7 @@
       <c r="P378" s="3"/>
       <c r="Q378" s="3"/>
       <c r="R378" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="379" spans="1:18" ht="27" x14ac:dyDescent="0.25">
@@ -20339,16 +20342,16 @@
         <v>423</v>
       </c>
       <c r="B379" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D379" s="3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E379" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F379" s="6">
         <v>75</v>
@@ -20373,7 +20376,7 @@
       <c r="P379" s="3"/>
       <c r="Q379" s="3"/>
       <c r="R379" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="380" spans="1:18" ht="27" x14ac:dyDescent="0.25">
@@ -20381,16 +20384,16 @@
         <v>423</v>
       </c>
       <c r="B380" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D380" s="3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E380" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F380" s="6">
         <v>21</v>
@@ -20415,7 +20418,7 @@
       <c r="P380" s="3"/>
       <c r="Q380" s="3"/>
       <c r="R380" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="381" spans="1:18" ht="27" x14ac:dyDescent="0.25">
@@ -20423,10 +20426,10 @@
         <v>423</v>
       </c>
       <c r="B381" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C381" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D381" s="3" t="s">
         <v>22</v>
@@ -20467,7 +20470,7 @@
       <c r="P381" s="3"/>
       <c r="Q381" s="3"/>
       <c r="R381" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="382" spans="1:18" ht="27" x14ac:dyDescent="0.25">
@@ -20475,7 +20478,7 @@
         <v>423</v>
       </c>
       <c r="B382" s="2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>21</v>
@@ -20507,7 +20510,7 @@
       </c>
       <c r="Q382" s="3"/>
       <c r="R382" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="383" spans="1:18" ht="27" x14ac:dyDescent="0.25">
@@ -20515,7 +20518,7 @@
         <v>423</v>
       </c>
       <c r="B383" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>21</v>
@@ -20563,7 +20566,7 @@
         <v>1</v>
       </c>
       <c r="R383" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="384" spans="1:18" ht="36" x14ac:dyDescent="0.25">
@@ -20571,7 +20574,7 @@
         <v>423</v>
       </c>
       <c r="B384" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>21</v>
@@ -20624,10 +20627,10 @@
     </row>
     <row r="385" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B385" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C385" s="2" t="s">
         <v>45</v>
@@ -20678,10 +20681,10 @@
     </row>
     <row r="386" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B386" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C386" s="2" t="s">
         <v>45</v>
@@ -20732,10 +20735,10 @@
     </row>
     <row r="387" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B387" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C387" s="2" t="s">
         <v>21</v>
@@ -20783,15 +20786,15 @@
         <v>1</v>
       </c>
       <c r="R387" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="388" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B388" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C388" s="2" t="s">
         <v>21</v>
@@ -20800,7 +20803,7 @@
         <v>22</v>
       </c>
       <c r="E388" s="3" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="F388" s="5">
         <v>413501.55</v>
@@ -20835,15 +20838,15 @@
       <c r="P388" s="3"/>
       <c r="Q388" s="3"/>
       <c r="R388" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="389" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B389" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C389" s="2" t="s">
         <v>21</v>
@@ -20852,7 +20855,7 @@
         <v>22</v>
       </c>
       <c r="E389" s="3" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F389" s="6">
         <v>1</v>
@@ -20896,10 +20899,10 @@
     </row>
     <row r="390" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C390" s="2" t="s">
         <v>21</v>
@@ -20944,16 +20947,16 @@
     </row>
     <row r="391" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B391" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C391" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D391" s="3" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E391" s="3" t="s">
         <v>23</v>
@@ -20993,21 +20996,21 @@
       </c>
       <c r="Q391" s="3"/>
       <c r="R391" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="392" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C392" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D392" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E392" s="3" t="s">
         <v>23</v>
@@ -21047,21 +21050,21 @@
       </c>
       <c r="Q392" s="3"/>
       <c r="R392" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="393" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B393" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C393" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D393" s="3" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="E393" s="3" t="s">
         <v>23</v>
@@ -21101,21 +21104,21 @@
       </c>
       <c r="Q393" s="3"/>
       <c r="R393" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="394" spans="1:18" ht="54" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C394" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D394" s="3" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="E394" s="3" t="s">
         <v>23</v>
@@ -21155,15 +21158,15 @@
       </c>
       <c r="Q394" s="3"/>
       <c r="R394" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="395" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B395" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>21</v>
@@ -21209,15 +21212,15 @@
       </c>
       <c r="Q395" s="3"/>
       <c r="R395" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="396" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>21</v>
@@ -21268,10 +21271,10 @@
     </row>
     <row r="397" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B397" s="2" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>21</v>
@@ -21322,10 +21325,10 @@
     </row>
     <row r="398" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B398" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C398" s="2" t="s">
         <v>21</v>
@@ -21371,18 +21374,18 @@
       </c>
       <c r="Q398" s="3"/>
       <c r="R398" s="2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="399" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B399" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C399" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D399" s="3" t="s">
         <v>22</v>
@@ -21409,21 +21412,21 @@
         <v>95</v>
       </c>
       <c r="R399" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="400" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B400" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C400" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D400" s="3" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E400" s="3" t="s">
         <v>23</v>
@@ -21441,21 +21444,21 @@
       <c r="P400" s="3"/>
       <c r="Q400" s="3"/>
       <c r="R400" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="401" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B401" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C401" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D401" s="3" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E401" s="3" t="s">
         <v>23</v>
@@ -21473,21 +21476,21 @@
       <c r="P401" s="3"/>
       <c r="Q401" s="3"/>
       <c r="R401" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="402" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A402" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B402" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C402" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D402" s="3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E402" s="3" t="s">
         <v>23</v>
@@ -21505,21 +21508,21 @@
       <c r="P402" s="3"/>
       <c r="Q402" s="3"/>
       <c r="R402" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="403" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B403" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C403" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D403" s="3" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E403" s="3" t="s">
         <v>23</v>
@@ -21543,21 +21546,21 @@
         <v>66.599999999999994</v>
       </c>
       <c r="R403" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="404" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B404" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C404" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D404" s="3" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="E404" s="3" t="s">
         <v>23</v>
@@ -21581,21 +21584,21 @@
         <v>99.2</v>
       </c>
       <c r="R404" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="405" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B405" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C405" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D405" s="3" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E405" s="3" t="s">
         <v>23</v>
@@ -21619,15 +21622,15 @@
         <v>94.4</v>
       </c>
       <c r="R405" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="406" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B406" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C406" s="2" t="s">
         <v>21</v>
@@ -21675,15 +21678,15 @@
         <v>1</v>
       </c>
       <c r="R406" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="407" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B407" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>21</v>
@@ -21729,15 +21732,15 @@
       </c>
       <c r="Q407" s="3"/>
       <c r="R407" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="408" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B408" s="2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C408" s="2" t="s">
         <v>21</v>
@@ -21785,15 +21788,15 @@
         <v>1</v>
       </c>
       <c r="R408" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="409" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B409" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C409" s="2" t="s">
         <v>21</v>
@@ -21838,10 +21841,10 @@
     </row>
     <row r="410" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B410" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C410" s="2" t="s">
         <v>21</v>
@@ -21886,10 +21889,10 @@
     </row>
     <row r="411" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A411" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B411" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>21</v>
@@ -21935,15 +21938,15 @@
       </c>
       <c r="Q411" s="3"/>
       <c r="R411" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="412" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A412" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B412" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C412" s="2" t="s">
         <v>21</v>
@@ -21994,10 +21997,10 @@
     </row>
     <row r="413" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B413" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>21</v>
@@ -22045,15 +22048,15 @@
         <v>0</v>
       </c>
       <c r="R413" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="414" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B414" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C414" s="2" t="s">
         <v>21</v>
@@ -22092,10 +22095,10 @@
     </row>
     <row r="415" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B415" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C415" s="2" t="s">
         <v>21</v>
@@ -22137,24 +22140,24 @@
       </c>
       <c r="Q415" s="3"/>
       <c r="R415" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="416" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B416" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C416" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D416" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E416" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F416" s="3"/>
       <c r="G416" s="3"/>
@@ -22179,24 +22182,24 @@
       </c>
       <c r="Q416" s="3"/>
       <c r="R416" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="417" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A417" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B417" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C417" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D417" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E417" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F417" s="3"/>
       <c r="G417" s="3"/>
@@ -22221,24 +22224,24 @@
       </c>
       <c r="Q417" s="3"/>
       <c r="R417" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="418" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B418" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C418" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D418" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="E418" s="3" t="s">
         <v>493</v>
-      </c>
-      <c r="E418" s="3" t="s">
-        <v>492</v>
       </c>
       <c r="F418" s="3"/>
       <c r="G418" s="3"/>
@@ -22263,24 +22266,24 @@
       </c>
       <c r="Q418" s="3"/>
       <c r="R418" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="419" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B419" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C419" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D419" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E419" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F419" s="3"/>
       <c r="G419" s="3"/>
@@ -22305,24 +22308,24 @@
       </c>
       <c r="Q419" s="3"/>
       <c r="R419" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="420" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B420" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C420" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D420" s="3" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E420" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F420" s="3"/>
       <c r="G420" s="3"/>
@@ -22347,24 +22350,24 @@
       </c>
       <c r="Q420" s="3"/>
       <c r="R420" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="421" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B421" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C421" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="D421" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="D421" s="3" t="s">
+      <c r="E421" s="3" t="s">
         <v>493</v>
-      </c>
-      <c r="E421" s="3" t="s">
-        <v>492</v>
       </c>
       <c r="F421" s="3"/>
       <c r="G421" s="3"/>
@@ -22389,24 +22392,24 @@
       </c>
       <c r="Q421" s="3"/>
       <c r="R421" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="422" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B422" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C422" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D422" s="3" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E422" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F422" s="3"/>
       <c r="G422" s="3"/>
@@ -22431,24 +22434,24 @@
       </c>
       <c r="Q422" s="3"/>
       <c r="R422" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="423" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B423" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C423" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D423" s="3" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E423" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F423" s="3"/>
       <c r="G423" s="3"/>
@@ -22473,24 +22476,24 @@
       </c>
       <c r="Q423" s="3"/>
       <c r="R423" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="424" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B424" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C424" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D424" s="3" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="E424" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F424" s="3"/>
       <c r="G424" s="3"/>
@@ -22515,24 +22518,24 @@
       </c>
       <c r="Q424" s="3"/>
       <c r="R424" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="425" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B425" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C425" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D425" s="3" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E425" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F425" s="3"/>
       <c r="G425" s="3"/>
@@ -22557,15 +22560,15 @@
       </c>
       <c r="Q425" s="3"/>
       <c r="R425" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="426" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A426" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B426" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>29</v>
@@ -22611,15 +22614,15 @@
       </c>
       <c r="Q426" s="3"/>
       <c r="R426" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="427" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B427" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>29</v>
@@ -22665,15 +22668,15 @@
       </c>
       <c r="Q427" s="3"/>
       <c r="R427" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="428" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B428" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C428" s="2" t="s">
         <v>29</v>
@@ -22719,21 +22722,21 @@
       </c>
       <c r="Q428" s="3"/>
       <c r="R428" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="429" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A429" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B429" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C429" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D429" s="3" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="E429" s="3" t="s">
         <v>23</v>
@@ -22773,21 +22776,21 @@
       </c>
       <c r="Q429" s="3"/>
       <c r="R429" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="430" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A430" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B430" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D430" s="3" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="E430" s="3" t="s">
         <v>23</v>
@@ -22827,15 +22830,15 @@
       </c>
       <c r="Q430" s="3"/>
       <c r="R430" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="431" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B431" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>21</v>
@@ -22844,7 +22847,7 @@
         <v>22</v>
       </c>
       <c r="E431" s="3" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="F431" s="6">
         <v>12487</v>
@@ -22881,18 +22884,18 @@
       </c>
       <c r="Q431" s="3"/>
       <c r="R431" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="432" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A432" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B432" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C432" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D432" s="3" t="s">
         <v>219</v>
@@ -22919,18 +22922,18 @@
       <c r="P432" s="3"/>
       <c r="Q432" s="3"/>
       <c r="R432" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="433" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A433" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B433" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C433" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D433" s="3" t="s">
         <v>221</v>
@@ -22957,21 +22960,21 @@
       <c r="P433" s="3"/>
       <c r="Q433" s="3"/>
       <c r="R433" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="434" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A434" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B434" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C434" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D434" s="3" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E434" s="3" t="s">
         <v>23</v>
@@ -22995,21 +22998,21 @@
       <c r="P434" s="3"/>
       <c r="Q434" s="3"/>
       <c r="R434" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="435" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A435" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B435" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C435" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D435" s="3" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E435" s="3" t="s">
         <v>23</v>
@@ -23033,21 +23036,21 @@
       <c r="P435" s="3"/>
       <c r="Q435" s="3"/>
       <c r="R435" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="436" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A436" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B436" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C436" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D436" s="3" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E436" s="3" t="s">
         <v>23</v>
@@ -23071,21 +23074,21 @@
       <c r="P436" s="3"/>
       <c r="Q436" s="3"/>
       <c r="R436" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="437" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A437" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B437" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C437" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D437" s="3" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E437" s="3" t="s">
         <v>23</v>
@@ -23109,18 +23112,18 @@
       <c r="P437" s="3"/>
       <c r="Q437" s="3"/>
       <c r="R437" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="438" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A438" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B438" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C438" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D438" s="3" t="s">
         <v>37</v>
@@ -23147,21 +23150,21 @@
       <c r="P438" s="3"/>
       <c r="Q438" s="3"/>
       <c r="R438" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="439" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A439" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B439" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C439" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D439" s="3" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E439" s="3" t="s">
         <v>23</v>
@@ -23185,21 +23188,21 @@
       <c r="P439" s="3"/>
       <c r="Q439" s="3"/>
       <c r="R439" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="440" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B440" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C440" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D440" s="3" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E440" s="3" t="s">
         <v>23</v>
@@ -23223,21 +23226,21 @@
       <c r="P440" s="3"/>
       <c r="Q440" s="3"/>
       <c r="R440" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="441" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B441" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C441" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D441" s="3" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E441" s="3" t="s">
         <v>23</v>
@@ -23261,21 +23264,21 @@
       <c r="P441" s="3"/>
       <c r="Q441" s="3"/>
       <c r="R441" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="442" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B442" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C442" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="D442" s="3" t="s">
         <v>516</v>
-      </c>
-      <c r="D442" s="3" t="s">
-        <v>515</v>
       </c>
       <c r="E442" s="3" t="s">
         <v>23</v>
@@ -23299,18 +23302,18 @@
       <c r="P442" s="3"/>
       <c r="Q442" s="3"/>
       <c r="R442" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="443" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A443" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B443" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C443" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D443" s="3" t="s">
         <v>37</v>
@@ -23337,15 +23340,15 @@
       <c r="P443" s="3"/>
       <c r="Q443" s="3"/>
       <c r="R443" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="444" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A444" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B444" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>21</v>
@@ -23393,15 +23396,15 @@
         <v>100</v>
       </c>
       <c r="R444" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="445" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A445" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B445" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C445" s="2" t="s">
         <v>21</v>
@@ -23436,10 +23439,10 @@
     </row>
     <row r="446" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A446" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B446" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C446" s="2" t="s">
         <v>21</v>
@@ -23485,15 +23488,15 @@
       </c>
       <c r="Q446" s="3"/>
       <c r="R446" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="447" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B447" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C447" s="2" t="s">
         <v>21</v>
@@ -23539,18 +23542,18 @@
       </c>
       <c r="Q447" s="3"/>
       <c r="R447" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="448" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B448" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C448" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D448" s="3" t="s">
         <v>22</v>
@@ -23598,16 +23601,16 @@
     </row>
     <row r="449" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A449" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B449" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C449" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D449" s="3" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E449" s="3" t="s">
         <v>23</v>
@@ -23652,10 +23655,10 @@
     </row>
     <row r="450" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A450" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B450" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C450" s="2" t="s">
         <v>21</v>
@@ -23701,15 +23704,15 @@
       </c>
       <c r="Q450" s="3"/>
       <c r="R450" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="451" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A451" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B451" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C451" s="2" t="s">
         <v>21</v>
@@ -23760,10 +23763,10 @@
     </row>
     <row r="452" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A452" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B452" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C452" s="2" t="s">
         <v>21</v>
@@ -23809,21 +23812,21 @@
       </c>
       <c r="Q452" s="3"/>
       <c r="R452" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="453" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A453" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B453" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C453" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D453" s="3" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E453" s="3" t="s">
         <v>46</v>
@@ -23868,16 +23871,16 @@
     </row>
     <row r="454" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A454" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B454" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C454" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D454" s="3" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E454" s="3" t="s">
         <v>46</v>
@@ -23922,16 +23925,16 @@
     </row>
     <row r="455" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A455" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B455" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C455" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D455" s="3" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E455" s="3" t="s">
         <v>46</v>
@@ -23976,10 +23979,10 @@
     </row>
     <row r="456" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A456" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B456" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C456" s="2" t="s">
         <v>21</v>
@@ -24030,10 +24033,10 @@
     </row>
     <row r="457" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B457" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C457" s="2" t="s">
         <v>21</v>
@@ -24084,10 +24087,10 @@
     </row>
     <row r="458" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A458" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C458" s="2" t="s">
         <v>21</v>
@@ -24133,21 +24136,21 @@
       </c>
       <c r="Q458" s="3"/>
       <c r="R458" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="459" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B459" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C459" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D459" s="3" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E459" s="3" t="s">
         <v>283</v>
@@ -24192,16 +24195,16 @@
     </row>
     <row r="460" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C460" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D460" s="3" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="E460" s="3" t="s">
         <v>283</v>
@@ -24248,16 +24251,16 @@
     </row>
     <row r="461" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B461" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C461" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D461" s="3" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E461" s="3" t="s">
         <v>283</v>
@@ -24304,16 +24307,16 @@
     </row>
     <row r="462" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C462" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D462" s="3" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E462" s="3" t="s">
         <v>283</v>
@@ -24360,16 +24363,16 @@
     </row>
     <row r="463" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B463" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C463" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D463" s="3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E463" s="3" t="s">
         <v>283</v>
@@ -24416,16 +24419,16 @@
     </row>
     <row r="464" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B464" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C464" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D464" s="3" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="E464" s="3" t="s">
         <v>283</v>
@@ -24472,10 +24475,10 @@
     </row>
     <row r="465" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B465" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C465" s="2" t="s">
         <v>21</v>
@@ -24509,15 +24512,15 @@
         <v>1</v>
       </c>
       <c r="R465" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="466" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B466" s="2" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C466" s="2" t="s">
         <v>21</v>
@@ -24570,10 +24573,10 @@
     </row>
     <row r="467" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B467" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C467" s="2" t="s">
         <v>21</v>
@@ -24626,10 +24629,10 @@
     </row>
     <row r="468" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B468" s="2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C468" s="2" t="s">
         <v>21</v>
@@ -24638,7 +24641,7 @@
         <v>22</v>
       </c>
       <c r="E468" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="F468" s="3"/>
       <c r="G468" s="3"/>
@@ -24669,21 +24672,21 @@
       </c>
       <c r="Q468" s="3"/>
       <c r="R468" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="469" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A469" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B469" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C469" s="2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D469" s="3" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E469" s="3" t="s">
         <v>187</v>
@@ -24705,21 +24708,21 @@
         <v>1</v>
       </c>
       <c r="R469" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="470" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B470" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C470" s="2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D470" s="3" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E470" s="3" t="s">
         <v>187</v>
@@ -24761,21 +24764,21 @@
         <v>1</v>
       </c>
       <c r="R470" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="471" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A471" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B471" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C471" s="2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D471" s="3" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E471" s="3" t="s">
         <v>187</v>
@@ -24817,14 +24820,14 @@
         <v>1</v>
       </c>
       <c r="R471" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="472" spans="1:18" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="473" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="474" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A474" s="12" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B474" s="10"/>
     </row>

</xml_diff>

<commit_message>
Okno serwisowe - 06.09.2022
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1711,7 +1711,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 30-08-2022, 14:25</t>
+    <t>Last update: 06-09-2022, 11:44</t>
   </si>
 </sst>
 </file>
@@ -2262,8 +2262,8 @@
   <dimension ref="A1:S472"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Okno serwisowe - 11.10.2022
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1711,7 +1711,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 20-09-2022, 13:32</t>
+    <t>Last update: 11-10-2022, 10:20</t>
   </si>
 </sst>
 </file>
@@ -2262,8 +2262,8 @@
   <dimension ref="A1:S472"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5381,7 +5381,7 @@
         <v>24</v>
       </c>
       <c r="P61" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q61" s="6">
         <v>15</v>
@@ -5438,9 +5438,11 @@
         <v>4</v>
       </c>
       <c r="P62" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q62" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="Q62" s="6">
+        <v>2</v>
+      </c>
       <c r="R62" s="3"/>
       <c r="S62" s="2" t="s">
         <v>101</v>
@@ -5495,7 +5497,9 @@
       <c r="P63" s="6">
         <v>6</v>
       </c>
-      <c r="Q63" s="3"/>
+      <c r="Q63" s="6">
+        <v>13</v>
+      </c>
       <c r="R63" s="3"/>
       <c r="S63" s="2" t="s">
         <v>101</v>
@@ -5662,7 +5666,9 @@
       <c r="P66" s="6">
         <v>19</v>
       </c>
-      <c r="Q66" s="3"/>
+      <c r="Q66" s="6">
+        <v>21</v>
+      </c>
       <c r="R66" s="3"/>
       <c r="S66" s="2" t="s">
         <v>101</v>
@@ -5717,7 +5723,9 @@
       <c r="P67" s="6">
         <v>9</v>
       </c>
-      <c r="Q67" s="3"/>
+      <c r="Q67" s="6">
+        <v>9</v>
+      </c>
       <c r="R67" s="3"/>
       <c r="S67" s="2" t="s">
         <v>101</v>
@@ -6907,7 +6915,9 @@
       <c r="P91" s="5">
         <v>1.93</v>
       </c>
-      <c r="Q91" s="3"/>
+      <c r="Q91" s="5">
+        <v>56.63</v>
+      </c>
       <c r="R91" s="3"/>
       <c r="S91" s="2" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Aktualizacja eOkno serwisowe 13.12.2022 - aktualizacja plików excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -1706,7 +1706,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 15-11-2022, 08:47</t>
+    <t>Last update: 13-12-2022, 09:49</t>
   </si>
 </sst>
 </file>
@@ -3639,7 +3639,9 @@
       <c r="P28" s="7">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="Q28" s="3"/>
+      <c r="Q28" s="7">
+        <v>9.0000000000000006E-5</v>
+      </c>
       <c r="R28" s="3"/>
       <c r="S28" s="2" t="s">
         <v>60</v>
@@ -11560,7 +11562,7 @@
         <v>87.6</v>
       </c>
       <c r="H199" s="4">
-        <v>87.9</v>
+        <v>87.8</v>
       </c>
       <c r="I199" s="4">
         <v>88</v>
@@ -11578,16 +11580,16 @@
         <v>92</v>
       </c>
       <c r="N199" s="4">
-        <v>92.1</v>
+        <v>92</v>
       </c>
       <c r="O199" s="4">
         <v>92.2</v>
       </c>
       <c r="P199" s="4">
-        <v>92.3</v>
+        <v>92.7</v>
       </c>
       <c r="Q199" s="4">
-        <v>62.4</v>
+        <v>92.8</v>
       </c>
       <c r="R199" s="3"/>
       <c r="S199" s="2" t="s">

</xml_diff>

<commit_message>
Okno serwisowe 07.02.2023 - aktualizacja plików excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="18060" windowHeight="7050"/>
   </bookViews>
@@ -1705,13 +1700,13 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 02-02-2023, 14:25</t>
+    <t>Last update: 07-02-2023, 10:17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$-10809]0.0;\-0.0;0.0"/>
     <numFmt numFmtId="165" formatCode="[$-10809]0.00;\-0.00;0.00"/>
@@ -1720,7 +1715,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000;\-0.000;0.000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1918,14 +1913,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1946,7 +1933,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="0" name="Picture 1"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2009,7 +1996,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2041,10 +2028,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2076,7 +2062,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -2252,7 +2237,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S472"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
@@ -2260,7 +2245,7 @@
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2272,17 +2257,17 @@
     <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="36" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2341,7 +2326,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="19.5">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2396,7 +2381,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="15">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2451,7 +2436,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -2506,7 +2491,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="15">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -2561,7 +2546,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="15">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -2616,7 +2601,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="15">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -2671,7 +2656,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -2726,7 +2711,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2781,7 +2766,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -2836,7 +2821,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2891,7 +2876,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="19.5">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -2946,7 +2931,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="19.5">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -3001,7 +2986,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="15">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -3040,7 +3025,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="29.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -3097,7 +3082,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="97.5">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -3152,7 +3137,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="97.5">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -3207,7 +3192,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="97.5">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -3262,7 +3247,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="19.5">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -3317,7 +3302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="29.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -3374,7 +3359,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="29.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -3431,7 +3416,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="29.25">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -3476,7 +3461,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="68.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -3521,7 +3506,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="29.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
@@ -3566,7 +3551,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="29.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -3611,7 +3596,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="29.25">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
@@ -3662,7 +3647,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="39">
       <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
@@ -3719,7 +3704,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="39">
       <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
@@ -3776,7 +3761,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="39">
       <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
@@ -3833,7 +3818,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="39">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -3890,7 +3875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="19.5">
       <c r="A33" s="2" t="s">
         <v>66</v>
       </c>
@@ -3945,7 +3930,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="29.25">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -3990,7 +3975,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="29.25">
       <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
@@ -4035,7 +4020,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="29.25">
       <c r="A36" s="2" t="s">
         <v>66</v>
       </c>
@@ -4080,7 +4065,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="29.25">
       <c r="A37" s="2" t="s">
         <v>66</v>
       </c>
@@ -4125,7 +4110,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="29.25">
       <c r="A38" s="2" t="s">
         <v>66</v>
       </c>
@@ -4170,7 +4155,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="29.25">
       <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
@@ -4215,7 +4200,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="39">
       <c r="A40" s="2" t="s">
         <v>66</v>
       </c>
@@ -4254,7 +4239,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="97.5">
       <c r="A41" s="2" t="s">
         <v>66</v>
       </c>
@@ -4313,7 +4298,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="97.5">
       <c r="A42" s="2" t="s">
         <v>66</v>
       </c>
@@ -4372,7 +4357,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="97.5">
       <c r="A43" s="2" t="s">
         <v>66</v>
       </c>
@@ -4431,7 +4416,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="97.5">
       <c r="A44" s="2" t="s">
         <v>66</v>
       </c>
@@ -4490,7 +4475,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="97.5">
       <c r="A45" s="2" t="s">
         <v>66</v>
       </c>
@@ -4549,7 +4534,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="97.5">
       <c r="A46" s="2" t="s">
         <v>66</v>
       </c>
@@ -4608,7 +4593,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="48.75">
       <c r="A47" s="2" t="s">
         <v>66</v>
       </c>
@@ -4657,7 +4642,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="48.75">
       <c r="A48" s="2" t="s">
         <v>66</v>
       </c>
@@ -4706,7 +4691,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="19.5">
       <c r="A49" s="2" t="s">
         <v>66</v>
       </c>
@@ -4761,7 +4746,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="29.25">
       <c r="A50" s="2" t="s">
         <v>66</v>
       </c>
@@ -4812,7 +4797,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="19.5">
       <c r="A51" s="2" t="s">
         <v>95</v>
       </c>
@@ -4867,7 +4852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="19.5">
       <c r="A52" s="2" t="s">
         <v>95</v>
       </c>
@@ -4924,7 +4909,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>95</v>
       </c>
@@ -4981,7 +4966,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>95</v>
       </c>
@@ -5038,7 +5023,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>95</v>
       </c>
@@ -5095,7 +5080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>95</v>
       </c>
@@ -5152,7 +5137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>95</v>
       </c>
@@ -5209,7 +5194,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>95</v>
       </c>
@@ -5266,7 +5251,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="29.25">
       <c r="A59" s="2" t="s">
         <v>95</v>
       </c>
@@ -5323,7 +5308,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>95</v>
       </c>
@@ -5380,7 +5365,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="29.25">
       <c r="A61" s="2" t="s">
         <v>95</v>
       </c>
@@ -5437,7 +5422,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="29.25">
       <c r="A62" s="2" t="s">
         <v>95</v>
       </c>
@@ -5494,7 +5479,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="29.25">
       <c r="A63" s="2" t="s">
         <v>95</v>
       </c>
@@ -5551,7 +5536,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="19.5">
       <c r="A64" s="2" t="s">
         <v>95</v>
       </c>
@@ -5608,7 +5593,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="29.25">
       <c r="A65" s="2" t="s">
         <v>95</v>
       </c>
@@ -5665,7 +5650,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="29.25">
       <c r="A66" s="2" t="s">
         <v>95</v>
       </c>
@@ -5722,7 +5707,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="29.25">
       <c r="A67" s="2" t="s">
         <v>95</v>
       </c>
@@ -5779,7 +5764,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="29.25">
       <c r="A68" s="2" t="s">
         <v>95</v>
       </c>
@@ -5834,7 +5819,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="29.25">
       <c r="A69" s="2" t="s">
         <v>95</v>
       </c>
@@ -5889,7 +5874,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" ht="29.25">
       <c r="A70" s="2" t="s">
         <v>95</v>
       </c>
@@ -5944,7 +5929,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" ht="29.25">
       <c r="A71" s="2" t="s">
         <v>95</v>
       </c>
@@ -5999,7 +5984,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" ht="19.5">
       <c r="A72" s="2" t="s">
         <v>95</v>
       </c>
@@ -6054,7 +6039,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="19.5">
       <c r="A73" s="2" t="s">
         <v>95</v>
       </c>
@@ -6109,7 +6094,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="19.5">
       <c r="A74" s="2" t="s">
         <v>95</v>
       </c>
@@ -6164,7 +6149,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="19.5">
       <c r="A75" s="2" t="s">
         <v>95</v>
       </c>
@@ -6221,7 +6206,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" ht="29.25">
       <c r="A76" s="2" t="s">
         <v>95</v>
       </c>
@@ -6278,7 +6263,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" ht="29.25">
       <c r="A77" s="2" t="s">
         <v>95</v>
       </c>
@@ -6317,7 +6302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" ht="19.5">
       <c r="A78" s="2" t="s">
         <v>95</v>
       </c>
@@ -6374,7 +6359,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="19.5">
       <c r="A79" s="2" t="s">
         <v>95</v>
       </c>
@@ -6431,7 +6416,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" ht="19.5">
       <c r="A80" s="2" t="s">
         <v>95</v>
       </c>
@@ -6488,7 +6473,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="19.5">
       <c r="A81" s="2" t="s">
         <v>95</v>
       </c>
@@ -6529,7 +6514,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="29.25">
       <c r="A82" s="2" t="s">
         <v>95</v>
       </c>
@@ -6574,7 +6559,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="29.25">
       <c r="A83" s="2" t="s">
         <v>95</v>
       </c>
@@ -6619,7 +6604,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="19.5">
       <c r="A84" s="2" t="s">
         <v>95</v>
       </c>
@@ -6654,7 +6639,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="29.25">
       <c r="A85" s="2" t="s">
         <v>95</v>
       </c>
@@ -6689,7 +6674,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="19.5">
       <c r="A86" s="2" t="s">
         <v>95</v>
       </c>
@@ -6744,7 +6729,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="19.5">
       <c r="A87" s="2" t="s">
         <v>95</v>
       </c>
@@ -6783,7 +6768,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" ht="19.5">
       <c r="A88" s="2" t="s">
         <v>95</v>
       </c>
@@ -6840,7 +6825,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="19.5">
       <c r="A89" s="2" t="s">
         <v>95</v>
       </c>
@@ -6897,7 +6882,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="19.5">
       <c r="A90" s="2" t="s">
         <v>95</v>
       </c>
@@ -6938,7 +6923,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="29.25">
       <c r="A91" s="2" t="s">
         <v>95</v>
       </c>
@@ -6989,7 +6974,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" ht="19.5">
       <c r="A92" s="2" t="s">
         <v>95</v>
       </c>
@@ -7028,7 +7013,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" ht="19.5">
       <c r="A93" s="2" t="s">
         <v>95</v>
       </c>
@@ -7067,7 +7052,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" ht="19.5">
       <c r="A94" s="2" t="s">
         <v>95</v>
       </c>
@@ -7106,7 +7091,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" ht="19.5">
       <c r="A95" s="2" t="s">
         <v>95</v>
       </c>
@@ -7159,7 +7144,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" ht="48.75">
       <c r="A96" s="2" t="s">
         <v>149</v>
       </c>
@@ -7196,7 +7181,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" ht="48.75">
       <c r="A97" s="2" t="s">
         <v>149</v>
       </c>
@@ -7233,7 +7218,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" ht="48.75">
       <c r="A98" s="2" t="s">
         <v>149</v>
       </c>
@@ -7270,7 +7255,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" ht="48.75">
       <c r="A99" s="2" t="s">
         <v>149</v>
       </c>
@@ -7311,7 +7296,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" ht="48.75">
       <c r="A100" s="2" t="s">
         <v>149</v>
       </c>
@@ -7352,7 +7337,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" ht="48.75">
       <c r="A101" s="2" t="s">
         <v>149</v>
       </c>
@@ -7393,7 +7378,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" ht="48.75">
       <c r="A102" s="2" t="s">
         <v>149</v>
       </c>
@@ -7434,7 +7419,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" ht="48.75">
       <c r="A103" s="2" t="s">
         <v>149</v>
       </c>
@@ -7475,7 +7460,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" ht="48.75">
       <c r="A104" s="2" t="s">
         <v>149</v>
       </c>
@@ -7516,7 +7501,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" ht="29.25">
       <c r="A105" s="2" t="s">
         <v>149</v>
       </c>
@@ -7553,7 +7538,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" ht="19.5">
       <c r="A106" s="2" t="s">
         <v>149</v>
       </c>
@@ -7610,7 +7595,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" ht="19.5">
       <c r="A107" s="2" t="s">
         <v>149</v>
       </c>
@@ -7667,7 +7652,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" ht="19.5">
       <c r="A108" s="2" t="s">
         <v>149</v>
       </c>
@@ -7724,7 +7709,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" ht="19.5">
       <c r="A109" s="2" t="s">
         <v>149</v>
       </c>
@@ -7761,7 +7746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" ht="19.5">
       <c r="A110" s="2" t="s">
         <v>149</v>
       </c>
@@ -7798,7 +7783,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" ht="19.5">
       <c r="A111" s="2" t="s">
         <v>149</v>
       </c>
@@ -7835,7 +7820,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" ht="29.25">
       <c r="A112" s="2" t="s">
         <v>149</v>
       </c>
@@ -7880,7 +7865,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" ht="19.5">
       <c r="A113" s="2" t="s">
         <v>149</v>
       </c>
@@ -7927,7 +7912,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" ht="39">
       <c r="A114" s="2" t="s">
         <v>149</v>
       </c>
@@ -7974,7 +7959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" ht="48.75">
       <c r="A115" s="2" t="s">
         <v>149</v>
       </c>
@@ -8021,7 +8006,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" ht="58.5">
       <c r="A116" s="2" t="s">
         <v>149</v>
       </c>
@@ -8068,7 +8053,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" ht="29.25">
       <c r="A117" s="2" t="s">
         <v>149</v>
       </c>
@@ -8115,7 +8100,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" ht="29.25">
       <c r="A118" s="2" t="s">
         <v>149</v>
       </c>
@@ -8160,7 +8145,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" ht="19.5">
       <c r="A119" s="2" t="s">
         <v>149</v>
       </c>
@@ -8207,7 +8192,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" ht="39">
       <c r="A120" s="2" t="s">
         <v>149</v>
       </c>
@@ -8254,7 +8239,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" ht="48.75">
       <c r="A121" s="2" t="s">
         <v>149</v>
       </c>
@@ -8301,7 +8286,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" ht="58.5">
       <c r="A122" s="2" t="s">
         <v>149</v>
       </c>
@@ -8348,7 +8333,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" ht="29.25">
       <c r="A123" s="2" t="s">
         <v>149</v>
       </c>
@@ -8395,7 +8380,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" ht="48.75">
       <c r="A124" s="2" t="s">
         <v>149</v>
       </c>
@@ -8434,7 +8419,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" ht="48.75">
       <c r="A125" s="2" t="s">
         <v>149</v>
       </c>
@@ -8473,7 +8458,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" ht="29.25">
       <c r="A126" s="2" t="s">
         <v>149</v>
       </c>
@@ -8530,7 +8515,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" ht="29.25">
       <c r="A127" s="2" t="s">
         <v>149</v>
       </c>
@@ -8565,7 +8550,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" ht="29.25">
       <c r="A128" s="2" t="s">
         <v>149</v>
       </c>
@@ -8600,7 +8585,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" ht="29.25">
       <c r="A129" s="2" t="s">
         <v>149</v>
       </c>
@@ -8635,7 +8620,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" ht="29.25">
       <c r="A130" s="2" t="s">
         <v>149</v>
       </c>
@@ -8670,7 +8655,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" ht="29.25">
       <c r="A131" s="2" t="s">
         <v>149</v>
       </c>
@@ -8705,7 +8690,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" ht="29.25">
       <c r="A132" s="2" t="s">
         <v>149</v>
       </c>
@@ -8740,7 +8725,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" ht="29.25">
       <c r="A133" s="2" t="s">
         <v>149</v>
       </c>
@@ -8775,7 +8760,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" ht="29.25">
       <c r="A134" s="2" t="s">
         <v>149</v>
       </c>
@@ -8810,7 +8795,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" ht="29.25">
       <c r="A135" s="2" t="s">
         <v>149</v>
       </c>
@@ -8845,7 +8830,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" ht="29.25">
       <c r="A136" s="2" t="s">
         <v>149</v>
       </c>
@@ -8880,7 +8865,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" ht="29.25">
       <c r="A137" s="2" t="s">
         <v>149</v>
       </c>
@@ -8915,7 +8900,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" ht="29.25">
       <c r="A138" s="2" t="s">
         <v>149</v>
       </c>
@@ -8950,7 +8935,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" ht="29.25">
       <c r="A139" s="2" t="s">
         <v>149</v>
       </c>
@@ -8985,7 +8970,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" ht="29.25">
       <c r="A140" s="2" t="s">
         <v>149</v>
       </c>
@@ -9020,7 +9005,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" ht="29.25">
       <c r="A141" s="2" t="s">
         <v>149</v>
       </c>
@@ -9055,7 +9040,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" ht="29.25">
       <c r="A142" s="2" t="s">
         <v>149</v>
       </c>
@@ -9090,7 +9075,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" ht="48.75">
       <c r="A143" s="2" t="s">
         <v>149</v>
       </c>
@@ -9149,7 +9134,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" ht="58.5">
       <c r="A144" s="2" t="s">
         <v>149</v>
       </c>
@@ -9208,7 +9193,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" ht="58.5">
       <c r="A145" s="2" t="s">
         <v>149</v>
       </c>
@@ -9243,7 +9228,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" ht="58.5">
       <c r="A146" s="2" t="s">
         <v>149</v>
       </c>
@@ -9278,7 +9263,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" ht="58.5">
       <c r="A147" s="2" t="s">
         <v>149</v>
       </c>
@@ -9337,7 +9322,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" ht="58.5">
       <c r="A148" s="2" t="s">
         <v>149</v>
       </c>
@@ -9396,7 +9381,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" ht="58.5">
       <c r="A149" s="2" t="s">
         <v>149</v>
       </c>
@@ -9455,7 +9440,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" ht="29.25">
       <c r="A150" s="2" t="s">
         <v>149</v>
       </c>
@@ -9506,7 +9491,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" ht="58.5">
       <c r="A151" s="2" t="s">
         <v>149</v>
       </c>
@@ -9561,7 +9546,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" ht="58.5">
       <c r="A152" s="2" t="s">
         <v>149</v>
       </c>
@@ -9616,7 +9601,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" ht="58.5">
       <c r="A153" s="2" t="s">
         <v>149</v>
       </c>
@@ -9671,7 +9656,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" ht="58.5">
       <c r="A154" s="2" t="s">
         <v>149</v>
       </c>
@@ -9726,7 +9711,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" ht="29.25">
       <c r="A155" s="2" t="s">
         <v>205</v>
       </c>
@@ -9761,7 +9746,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" ht="19.5">
       <c r="A156" s="2" t="s">
         <v>205</v>
       </c>
@@ -9818,7 +9803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" ht="39">
       <c r="A157" s="2" t="s">
         <v>205</v>
       </c>
@@ -9853,7 +9838,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" ht="39">
       <c r="A158" s="2" t="s">
         <v>205</v>
       </c>
@@ -9888,7 +9873,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" ht="39">
       <c r="A159" s="2" t="s">
         <v>205</v>
       </c>
@@ -9923,7 +9908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="160" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" ht="39">
       <c r="A160" s="2" t="s">
         <v>205</v>
       </c>
@@ -9958,7 +9943,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" ht="39">
       <c r="A161" s="2" t="s">
         <v>205</v>
       </c>
@@ -9993,7 +9978,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" ht="19.5">
       <c r="A162" s="2" t="s">
         <v>205</v>
       </c>
@@ -10028,7 +10013,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:19" ht="19.5">
       <c r="A163" s="2" t="s">
         <v>205</v>
       </c>
@@ -10063,7 +10048,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" ht="19.5">
       <c r="A164" s="2" t="s">
         <v>205</v>
       </c>
@@ -10098,7 +10083,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:19" ht="19.5">
       <c r="A165" s="2" t="s">
         <v>205</v>
       </c>
@@ -10133,7 +10118,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" ht="19.5">
       <c r="A166" s="2" t="s">
         <v>205</v>
       </c>
@@ -10168,7 +10153,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" ht="19.5">
       <c r="A167" s="2" t="s">
         <v>205</v>
       </c>
@@ -10203,7 +10188,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:19" ht="19.5">
       <c r="A168" s="2" t="s">
         <v>205</v>
       </c>
@@ -10238,7 +10223,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" ht="19.5">
       <c r="A169" s="2" t="s">
         <v>205</v>
       </c>
@@ -10273,7 +10258,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:19" ht="29.25">
       <c r="A170" s="2" t="s">
         <v>205</v>
       </c>
@@ -10312,7 +10297,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:19" ht="29.25">
       <c r="A171" s="2" t="s">
         <v>205</v>
       </c>
@@ -10351,7 +10336,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:19" ht="29.25">
       <c r="A172" s="2" t="s">
         <v>205</v>
       </c>
@@ -10408,7 +10393,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:19" ht="29.25">
       <c r="A173" s="2" t="s">
         <v>205</v>
       </c>
@@ -10465,7 +10450,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:19" ht="29.25">
       <c r="A174" s="2" t="s">
         <v>205</v>
       </c>
@@ -10522,7 +10507,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:19" ht="29.25">
       <c r="A175" s="2" t="s">
         <v>205</v>
       </c>
@@ -10579,7 +10564,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:19" ht="29.25">
       <c r="A176" s="2" t="s">
         <v>205</v>
       </c>
@@ -10636,7 +10621,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="177" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:19" ht="19.5">
       <c r="A177" s="2" t="s">
         <v>205</v>
       </c>
@@ -10681,7 +10666,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="178" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:19" ht="39">
       <c r="A178" s="2" t="s">
         <v>205</v>
       </c>
@@ -10726,7 +10711,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:19" ht="19.5">
       <c r="A179" s="2" t="s">
         <v>205</v>
       </c>
@@ -10771,7 +10756,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:19" ht="39">
       <c r="A180" s="2" t="s">
         <v>205</v>
       </c>
@@ -10816,7 +10801,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:19" ht="39">
       <c r="A181" s="2" t="s">
         <v>205</v>
       </c>
@@ -10861,7 +10846,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="182" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:19" ht="39">
       <c r="A182" s="2" t="s">
         <v>205</v>
       </c>
@@ -10906,7 +10891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:19" ht="39">
       <c r="A183" s="2" t="s">
         <v>205</v>
       </c>
@@ -10951,7 +10936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:19" ht="39">
       <c r="A184" s="2" t="s">
         <v>205</v>
       </c>
@@ -10990,7 +10975,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:19" ht="39">
       <c r="A185" s="2" t="s">
         <v>205</v>
       </c>
@@ -11029,7 +11014,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="186" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:19" ht="39">
       <c r="A186" s="2" t="s">
         <v>205</v>
       </c>
@@ -11068,7 +11053,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:19" ht="39">
       <c r="A187" s="2" t="s">
         <v>205</v>
       </c>
@@ -11107,7 +11092,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:19" ht="39">
       <c r="A188" s="2" t="s">
         <v>205</v>
       </c>
@@ -11146,7 +11131,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:19" ht="39">
       <c r="A189" s="2" t="s">
         <v>205</v>
       </c>
@@ -11185,7 +11170,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:19" ht="39">
       <c r="A190" s="2" t="s">
         <v>205</v>
       </c>
@@ -11224,7 +11209,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:19" ht="39">
       <c r="A191" s="2" t="s">
         <v>205</v>
       </c>
@@ -11263,7 +11248,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:19" ht="39">
       <c r="A192" s="2" t="s">
         <v>205</v>
       </c>
@@ -11302,7 +11287,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="193" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:19" ht="39">
       <c r="A193" s="2" t="s">
         <v>205</v>
       </c>
@@ -11341,7 +11326,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:19" ht="39">
       <c r="A194" s="2" t="s">
         <v>205</v>
       </c>
@@ -11380,7 +11365,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="195" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:19" ht="39">
       <c r="A195" s="2" t="s">
         <v>205</v>
       </c>
@@ -11419,7 +11404,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="196" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:19" ht="19.5">
       <c r="A196" s="2" t="s">
         <v>205</v>
       </c>
@@ -11460,7 +11445,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:19" ht="19.5">
       <c r="A197" s="2" t="s">
         <v>205</v>
       </c>
@@ -11515,7 +11500,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:19" ht="19.5">
       <c r="A198" s="2" t="s">
         <v>205</v>
       </c>
@@ -11570,7 +11555,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:19" ht="19.5">
       <c r="A199" s="2" t="s">
         <v>245</v>
       </c>
@@ -11627,7 +11612,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="200" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:19" ht="29.25">
       <c r="A200" s="2" t="s">
         <v>245</v>
       </c>
@@ -11684,7 +11669,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="201" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:19" ht="19.5">
       <c r="A201" s="2" t="s">
         <v>245</v>
       </c>
@@ -11741,7 +11726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="202" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:19" ht="19.5">
       <c r="A202" s="2" t="s">
         <v>245</v>
       </c>
@@ -11776,7 +11761,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="203" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:19" ht="19.5">
       <c r="A203" s="2" t="s">
         <v>245</v>
       </c>
@@ -11811,7 +11796,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="204" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:19" ht="29.25">
       <c r="A204" s="2" t="s">
         <v>245</v>
       </c>
@@ -11866,7 +11851,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="205" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:19" ht="19.5">
       <c r="A205" s="2" t="s">
         <v>245</v>
       </c>
@@ -11921,7 +11906,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="206" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:19" ht="19.5">
       <c r="A206" s="2" t="s">
         <v>245</v>
       </c>
@@ -11966,7 +11951,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="207" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:19" ht="29.25">
       <c r="A207" s="2" t="s">
         <v>245</v>
       </c>
@@ -12021,7 +12006,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="208" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:19" ht="29.25">
       <c r="A208" s="2" t="s">
         <v>245</v>
       </c>
@@ -12072,7 +12057,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="209" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:19" ht="39">
       <c r="A209" s="2" t="s">
         <v>245</v>
       </c>
@@ -12129,7 +12114,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="210" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:19" ht="19.5">
       <c r="A210" s="2" t="s">
         <v>266</v>
       </c>
@@ -12164,7 +12149,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="211" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:19" ht="19.5">
       <c r="A211" s="2" t="s">
         <v>266</v>
       </c>
@@ -12219,7 +12204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="212" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:19" ht="29.25">
       <c r="A212" s="2" t="s">
         <v>266</v>
       </c>
@@ -12274,7 +12259,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="213" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:19" ht="29.25">
       <c r="A213" s="2" t="s">
         <v>266</v>
       </c>
@@ -12325,7 +12310,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="214" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:19" ht="29.25">
       <c r="A214" s="2" t="s">
         <v>272</v>
       </c>
@@ -12382,7 +12367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:19" ht="29.25">
       <c r="A215" s="2" t="s">
         <v>272</v>
       </c>
@@ -12439,7 +12424,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="216" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:19" ht="29.25">
       <c r="A216" s="2" t="s">
         <v>272</v>
       </c>
@@ -12478,7 +12463,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="217" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:19" ht="29.25">
       <c r="A217" s="2" t="s">
         <v>272</v>
       </c>
@@ -12517,7 +12502,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="218" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:19" ht="29.25">
       <c r="A218" s="2" t="s">
         <v>272</v>
       </c>
@@ -12556,7 +12541,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="219" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:19" ht="29.25">
       <c r="A219" s="2" t="s">
         <v>272</v>
       </c>
@@ -12613,7 +12598,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="220" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:19" ht="29.25">
       <c r="A220" s="2" t="s">
         <v>272</v>
       </c>
@@ -12670,7 +12655,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="221" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:19" ht="29.25">
       <c r="A221" s="2" t="s">
         <v>272</v>
       </c>
@@ -12727,7 +12712,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="222" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:19" ht="29.25">
       <c r="A222" s="2" t="s">
         <v>272</v>
       </c>
@@ -12772,7 +12757,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="223" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:19" ht="29.25">
       <c r="A223" s="2" t="s">
         <v>272</v>
       </c>
@@ -12817,7 +12802,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="224" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:19" ht="29.25">
       <c r="A224" s="2" t="s">
         <v>272</v>
       </c>
@@ -12862,7 +12847,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="225" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:19" ht="29.25">
       <c r="A225" s="2" t="s">
         <v>272</v>
       </c>
@@ -12907,7 +12892,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="226" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:19" ht="29.25">
       <c r="A226" s="2" t="s">
         <v>272</v>
       </c>
@@ -12952,7 +12937,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="227" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:19" ht="29.25">
       <c r="A227" s="2" t="s">
         <v>272</v>
       </c>
@@ -12997,7 +12982,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="228" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:19" ht="29.25">
       <c r="A228" s="2" t="s">
         <v>272</v>
       </c>
@@ -13042,7 +13027,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="229" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:19" ht="29.25">
       <c r="A229" s="2" t="s">
         <v>272</v>
       </c>
@@ -13087,7 +13072,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="230" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:19" ht="39">
       <c r="A230" s="2" t="s">
         <v>272</v>
       </c>
@@ -13132,7 +13117,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="231" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:19" ht="29.25">
       <c r="A231" s="2" t="s">
         <v>272</v>
       </c>
@@ -13177,7 +13162,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="232" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:19" ht="39">
       <c r="A232" s="2" t="s">
         <v>272</v>
       </c>
@@ -13222,7 +13207,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="233" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:19" ht="29.25">
       <c r="A233" s="2" t="s">
         <v>272</v>
       </c>
@@ -13267,7 +13252,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="234" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:19" ht="29.25">
       <c r="A234" s="2" t="s">
         <v>272</v>
       </c>
@@ -13312,7 +13297,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="235" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:19" ht="29.25">
       <c r="A235" s="2" t="s">
         <v>272</v>
       </c>
@@ -13357,7 +13342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="236" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:19" ht="29.25">
       <c r="A236" s="2" t="s">
         <v>272</v>
       </c>
@@ -13402,7 +13387,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="237" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:19" ht="29.25">
       <c r="A237" s="2" t="s">
         <v>272</v>
       </c>
@@ -13447,7 +13432,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="238" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:19" ht="29.25">
       <c r="A238" s="2" t="s">
         <v>272</v>
       </c>
@@ -13492,7 +13477,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:19" ht="29.25">
       <c r="A239" s="2" t="s">
         <v>272</v>
       </c>
@@ -13537,7 +13522,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="240" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:19" ht="29.25">
       <c r="A240" s="2" t="s">
         <v>272</v>
       </c>
@@ -13582,7 +13567,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="241" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:19" ht="29.25">
       <c r="A241" s="2" t="s">
         <v>272</v>
       </c>
@@ -13639,7 +13624,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="242" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:19" ht="29.25">
       <c r="A242" s="2" t="s">
         <v>272</v>
       </c>
@@ -13696,7 +13681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="243" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:19" ht="29.25">
       <c r="A243" s="2" t="s">
         <v>272</v>
       </c>
@@ -13753,7 +13738,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="244" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:19" ht="29.25">
       <c r="A244" s="2" t="s">
         <v>272</v>
       </c>
@@ -13810,7 +13795,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="245" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:19" ht="29.25">
       <c r="A245" s="2" t="s">
         <v>272</v>
       </c>
@@ -13867,7 +13852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="246" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:19" ht="29.25">
       <c r="A246" s="2" t="s">
         <v>272</v>
       </c>
@@ -13924,7 +13909,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="247" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:19" ht="29.25">
       <c r="A247" s="2" t="s">
         <v>272</v>
       </c>
@@ -13981,7 +13966,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="248" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:19" ht="29.25">
       <c r="A248" s="2" t="s">
         <v>272</v>
       </c>
@@ -14038,7 +14023,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="249" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:19" ht="29.25">
       <c r="A249" s="2" t="s">
         <v>272</v>
       </c>
@@ -14095,7 +14080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="250" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:19" ht="29.25">
       <c r="A250" s="2" t="s">
         <v>272</v>
       </c>
@@ -14152,7 +14137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="251" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:19" ht="29.25">
       <c r="A251" s="2" t="s">
         <v>272</v>
       </c>
@@ -14209,7 +14194,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="252" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:19" ht="29.25">
       <c r="A252" s="2" t="s">
         <v>272</v>
       </c>
@@ -14266,7 +14251,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="253" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:19" ht="39">
       <c r="A253" s="2" t="s">
         <v>272</v>
       </c>
@@ -14307,7 +14292,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="254" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:19" ht="39">
       <c r="A254" s="2" t="s">
         <v>272</v>
       </c>
@@ -14348,7 +14333,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="255" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:19" ht="39">
       <c r="A255" s="2" t="s">
         <v>272</v>
       </c>
@@ -14389,7 +14374,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="256" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:19" ht="29.25">
       <c r="A256" s="2" t="s">
         <v>272</v>
       </c>
@@ -14446,7 +14431,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="257" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:19" ht="48.75">
       <c r="A257" s="2" t="s">
         <v>272</v>
       </c>
@@ -14503,7 +14488,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="258" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:19" ht="29.25">
       <c r="A258" s="2" t="s">
         <v>272</v>
       </c>
@@ -14538,7 +14523,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="259" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:19" ht="29.25">
       <c r="A259" s="2" t="s">
         <v>272</v>
       </c>
@@ -14573,7 +14558,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="260" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:19" ht="29.25">
       <c r="A260" s="2" t="s">
         <v>272</v>
       </c>
@@ -14608,7 +14593,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="261" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:19" ht="29.25">
       <c r="A261" s="2" t="s">
         <v>272</v>
       </c>
@@ -14643,7 +14628,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="262" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:19" ht="29.25">
       <c r="A262" s="2" t="s">
         <v>272</v>
       </c>
@@ -14678,7 +14663,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="263" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:19" ht="29.25">
       <c r="A263" s="2" t="s">
         <v>272</v>
       </c>
@@ -14713,7 +14698,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="264" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:19" ht="29.25">
       <c r="A264" s="2" t="s">
         <v>272</v>
       </c>
@@ -14748,7 +14733,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="265" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:19" ht="29.25">
       <c r="A265" s="2" t="s">
         <v>272</v>
       </c>
@@ -14783,7 +14768,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="266" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:19" ht="29.25">
       <c r="A266" s="2" t="s">
         <v>272</v>
       </c>
@@ -14834,7 +14819,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="267" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:19" ht="29.25">
       <c r="A267" s="2" t="s">
         <v>318</v>
       </c>
@@ -14891,7 +14876,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="268" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:19" ht="29.25">
       <c r="A268" s="2" t="s">
         <v>318</v>
       </c>
@@ -14948,7 +14933,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="269" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:19" ht="29.25">
       <c r="A269" s="2" t="s">
         <v>318</v>
       </c>
@@ -15005,7 +14990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="270" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:19" ht="29.25">
       <c r="A270" s="2" t="s">
         <v>318</v>
       </c>
@@ -15062,7 +15047,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="271" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:19" ht="29.25">
       <c r="A271" s="2" t="s">
         <v>318</v>
       </c>
@@ -15119,7 +15104,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="272" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:19" ht="29.25">
       <c r="A272" s="2" t="s">
         <v>318</v>
       </c>
@@ -15176,7 +15161,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="273" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:19" ht="29.25">
       <c r="A273" s="2" t="s">
         <v>318</v>
       </c>
@@ -15233,7 +15218,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="274" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:19" ht="29.25">
       <c r="A274" s="2" t="s">
         <v>318</v>
       </c>
@@ -15290,7 +15275,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="275" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:19" ht="29.25">
       <c r="A275" s="2" t="s">
         <v>318</v>
       </c>
@@ -15347,7 +15332,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="276" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:19" ht="29.25">
       <c r="A276" s="2" t="s">
         <v>318</v>
       </c>
@@ -15404,7 +15389,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="277" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:19" ht="29.25">
       <c r="A277" s="2" t="s">
         <v>318</v>
       </c>
@@ -15461,7 +15446,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="278" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:19" ht="29.25">
       <c r="A278" s="2" t="s">
         <v>318</v>
       </c>
@@ -15518,7 +15503,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="279" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:19" ht="29.25">
       <c r="A279" s="2" t="s">
         <v>318</v>
       </c>
@@ -15575,7 +15560,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="280" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:19" ht="29.25">
       <c r="A280" s="2" t="s">
         <v>318</v>
       </c>
@@ -15632,7 +15617,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="281" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:19" ht="29.25">
       <c r="A281" s="2" t="s">
         <v>318</v>
       </c>
@@ -15689,7 +15674,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="282" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:19" ht="29.25">
       <c r="A282" s="2" t="s">
         <v>318</v>
       </c>
@@ -15746,7 +15731,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="283" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:19" ht="29.25">
       <c r="A283" s="2" t="s">
         <v>318</v>
       </c>
@@ -15803,7 +15788,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="284" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:19" ht="29.25">
       <c r="A284" s="2" t="s">
         <v>318</v>
       </c>
@@ -15860,7 +15845,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="285" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:19" ht="29.25">
       <c r="A285" s="2" t="s">
         <v>318</v>
       </c>
@@ -15917,7 +15902,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="286" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:19" ht="29.25">
       <c r="A286" s="2" t="s">
         <v>318</v>
       </c>
@@ -15974,7 +15959,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="287" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:19" ht="29.25">
       <c r="A287" s="2" t="s">
         <v>318</v>
       </c>
@@ -16025,7 +16010,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="288" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:19" ht="29.25">
       <c r="A288" s="2" t="s">
         <v>318</v>
       </c>
@@ -16082,7 +16067,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="289" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:19" ht="29.25">
       <c r="A289" s="2" t="s">
         <v>318</v>
       </c>
@@ -16139,7 +16124,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="290" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:19" ht="29.25">
       <c r="A290" s="2" t="s">
         <v>318</v>
       </c>
@@ -16190,7 +16175,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="291" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:19" ht="29.25">
       <c r="A291" s="2" t="s">
         <v>318</v>
       </c>
@@ -16243,7 +16228,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="292" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:19" ht="39">
       <c r="A292" s="2" t="s">
         <v>318</v>
       </c>
@@ -16292,7 +16277,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="293" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:19" ht="39">
       <c r="A293" s="2" t="s">
         <v>318</v>
       </c>
@@ -16341,7 +16326,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="294" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:19" ht="19.5">
       <c r="A294" s="2" t="s">
         <v>350</v>
       </c>
@@ -16398,7 +16383,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="295" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:19" ht="68.25">
       <c r="A295" s="2" t="s">
         <v>350</v>
       </c>
@@ -16455,7 +16440,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="296" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:19" ht="19.5">
       <c r="A296" s="2" t="s">
         <v>350</v>
       </c>
@@ -16512,7 +16497,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="297" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:19" ht="19.5">
       <c r="A297" s="2" t="s">
         <v>350</v>
       </c>
@@ -16569,7 +16554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="298" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:19" ht="19.5">
       <c r="A298" s="2" t="s">
         <v>350</v>
       </c>
@@ -16626,7 +16611,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="299" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:19" ht="19.5">
       <c r="A299" s="2" t="s">
         <v>350</v>
       </c>
@@ -16683,7 +16668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="300" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:19" ht="19.5">
       <c r="A300" s="2" t="s">
         <v>350</v>
       </c>
@@ -16740,7 +16725,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="301" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:19" ht="19.5">
       <c r="A301" s="2" t="s">
         <v>350</v>
       </c>
@@ -16797,7 +16782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="302" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:19" ht="19.5">
       <c r="A302" s="2" t="s">
         <v>350</v>
       </c>
@@ -16854,7 +16839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="303" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:19" ht="19.5">
       <c r="A303" s="2" t="s">
         <v>350</v>
       </c>
@@ -16911,7 +16896,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="304" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:19" ht="19.5">
       <c r="A304" s="2" t="s">
         <v>350</v>
       </c>
@@ -16968,7 +16953,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="305" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:19" ht="19.5">
       <c r="A305" s="2" t="s">
         <v>350</v>
       </c>
@@ -17007,7 +16992,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="306" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:19" ht="19.5">
       <c r="A306" s="2" t="s">
         <v>350</v>
       </c>
@@ -17064,7 +17049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="307" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:19" ht="39">
       <c r="A307" s="2" t="s">
         <v>350</v>
       </c>
@@ -17121,7 +17106,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="308" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:19" ht="48.75">
       <c r="A308" s="2" t="s">
         <v>350</v>
       </c>
@@ -17178,7 +17163,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="309" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:19" ht="39">
       <c r="A309" s="2" t="s">
         <v>350</v>
       </c>
@@ -17235,7 +17220,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="310" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:19" ht="39">
       <c r="A310" s="2" t="s">
         <v>350</v>
       </c>
@@ -17292,7 +17277,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="311" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:19" ht="29.25">
       <c r="A311" s="2" t="s">
         <v>350</v>
       </c>
@@ -17349,7 +17334,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="312" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:19" ht="39">
       <c r="A312" s="2" t="s">
         <v>350</v>
       </c>
@@ -17404,7 +17389,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="313" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:19" ht="29.25">
       <c r="A313" s="2" t="s">
         <v>350</v>
       </c>
@@ -17461,7 +17446,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="314" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:19" ht="29.25">
       <c r="A314" s="2" t="s">
         <v>350</v>
       </c>
@@ -17518,7 +17503,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="315" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:19" ht="39">
       <c r="A315" s="2" t="s">
         <v>350</v>
       </c>
@@ -17575,7 +17560,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="316" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:19" ht="29.25">
       <c r="A316" s="2" t="s">
         <v>350</v>
       </c>
@@ -17632,7 +17617,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="317" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:19" ht="39">
       <c r="A317" s="2" t="s">
         <v>350</v>
       </c>
@@ -17689,7 +17674,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="318" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:19" ht="29.25">
       <c r="A318" s="2" t="s">
         <v>350</v>
       </c>
@@ -17746,7 +17731,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="319" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:19" ht="29.25">
       <c r="A319" s="2" t="s">
         <v>350</v>
       </c>
@@ -17803,7 +17788,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="320" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:19" ht="39">
       <c r="A320" s="2" t="s">
         <v>350</v>
       </c>
@@ -17860,7 +17845,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="321" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:19" ht="39">
       <c r="A321" s="2" t="s">
         <v>350</v>
       </c>
@@ -17917,7 +17902,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="322" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:19" ht="68.25">
       <c r="A322" s="2" t="s">
         <v>350</v>
       </c>
@@ -17974,7 +17959,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="323" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:19" ht="58.5">
       <c r="A323" s="2" t="s">
         <v>350</v>
       </c>
@@ -18031,7 +18016,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="324" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:19" ht="68.25">
       <c r="A324" s="2" t="s">
         <v>350</v>
       </c>
@@ -18088,7 +18073,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="325" spans="1:19" ht="72" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:19" ht="68.25">
       <c r="A325" s="2" t="s">
         <v>350</v>
       </c>
@@ -18145,7 +18130,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="326" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:19" ht="39">
       <c r="A326" s="2" t="s">
         <v>350</v>
       </c>
@@ -18202,7 +18187,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="327" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:19" ht="68.25">
       <c r="A327" s="2" t="s">
         <v>350</v>
       </c>
@@ -18259,7 +18244,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="328" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:19" ht="58.5">
       <c r="A328" s="2" t="s">
         <v>350</v>
       </c>
@@ -18316,7 +18301,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="329" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:19" ht="68.25">
       <c r="A329" s="2" t="s">
         <v>350</v>
       </c>
@@ -18373,7 +18358,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="330" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:19" ht="68.25">
       <c r="A330" s="2" t="s">
         <v>350</v>
       </c>
@@ -18430,7 +18415,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="331" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:19" ht="29.25">
       <c r="A331" s="2" t="s">
         <v>391</v>
       </c>
@@ -18485,7 +18470,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="332" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:19" ht="29.25">
       <c r="A332" s="2" t="s">
         <v>391</v>
       </c>
@@ -18540,7 +18525,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="333" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:19" ht="29.25">
       <c r="A333" s="2" t="s">
         <v>391</v>
       </c>
@@ -18595,7 +18580,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="334" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:19" ht="29.25">
       <c r="A334" s="2" t="s">
         <v>391</v>
       </c>
@@ -18652,7 +18637,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="335" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:19" ht="29.25">
       <c r="A335" s="2" t="s">
         <v>391</v>
       </c>
@@ -18709,7 +18694,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="336" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:19" ht="29.25">
       <c r="A336" s="2" t="s">
         <v>391</v>
       </c>
@@ -18766,7 +18751,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="337" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:19" ht="29.25">
       <c r="A337" s="2" t="s">
         <v>391</v>
       </c>
@@ -18823,7 +18808,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="338" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:19" ht="29.25">
       <c r="A338" s="2" t="s">
         <v>391</v>
       </c>
@@ -18880,7 +18865,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="339" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:19" ht="29.25">
       <c r="A339" s="2" t="s">
         <v>391</v>
       </c>
@@ -18937,7 +18922,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="340" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:19" ht="29.25">
       <c r="A340" s="2" t="s">
         <v>391</v>
       </c>
@@ -18987,14 +18972,14 @@
         <v>20.7</v>
       </c>
       <c r="Q340" s="4">
-        <v>1</v>
+        <v>22.5</v>
       </c>
       <c r="R340" s="3"/>
       <c r="S340" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="341" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:19" ht="29.25">
       <c r="A341" s="2" t="s">
         <v>391</v>
       </c>
@@ -19051,7 +19036,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="342" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:19" ht="29.25">
       <c r="A342" s="2" t="s">
         <v>391</v>
       </c>
@@ -19108,7 +19093,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="343" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:19" ht="29.25">
       <c r="A343" s="2" t="s">
         <v>391</v>
       </c>
@@ -19165,7 +19150,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="344" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:19" ht="29.25">
       <c r="A344" s="2" t="s">
         <v>391</v>
       </c>
@@ -19222,7 +19207,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="345" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:19" ht="29.25">
       <c r="A345" s="2" t="s">
         <v>391</v>
       </c>
@@ -19279,7 +19264,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="346" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:19" ht="29.25">
       <c r="A346" s="2" t="s">
         <v>391</v>
       </c>
@@ -19336,7 +19321,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="347" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:19" ht="29.25">
       <c r="A347" s="2" t="s">
         <v>391</v>
       </c>
@@ -19393,7 +19378,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="348" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:19" ht="29.25">
       <c r="A348" s="2" t="s">
         <v>391</v>
       </c>
@@ -19450,7 +19435,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="349" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:19" ht="29.25">
       <c r="A349" s="2" t="s">
         <v>391</v>
       </c>
@@ -19507,7 +19492,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="350" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:19" ht="29.25">
       <c r="A350" s="2" t="s">
         <v>391</v>
       </c>
@@ -19564,7 +19549,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="351" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:19" ht="29.25">
       <c r="A351" s="2" t="s">
         <v>391</v>
       </c>
@@ -19621,7 +19606,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="352" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:19" ht="29.25">
       <c r="A352" s="2" t="s">
         <v>391</v>
       </c>
@@ -19678,7 +19663,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="353" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:19" ht="29.25">
       <c r="A353" s="2" t="s">
         <v>391</v>
       </c>
@@ -19735,7 +19720,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="354" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:19" ht="29.25">
       <c r="A354" s="2" t="s">
         <v>391</v>
       </c>
@@ -19792,7 +19777,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="355" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:19" ht="29.25">
       <c r="A355" s="2" t="s">
         <v>391</v>
       </c>
@@ -19849,7 +19834,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="356" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:19" ht="29.25">
       <c r="A356" s="2" t="s">
         <v>391</v>
       </c>
@@ -19906,7 +19891,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="357" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:19" ht="29.25">
       <c r="A357" s="2" t="s">
         <v>391</v>
       </c>
@@ -19963,7 +19948,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="358" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:19" ht="29.25">
       <c r="A358" s="2" t="s">
         <v>391</v>
       </c>
@@ -20018,7 +20003,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="359" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:19" ht="29.25">
       <c r="A359" s="2" t="s">
         <v>391</v>
       </c>
@@ -20075,7 +20060,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="360" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:19" ht="29.25">
       <c r="A360" s="2" t="s">
         <v>391</v>
       </c>
@@ -20132,7 +20117,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="361" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:19" ht="29.25">
       <c r="A361" s="2" t="s">
         <v>391</v>
       </c>
@@ -20189,7 +20174,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="362" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:19" ht="29.25">
       <c r="A362" s="2" t="s">
         <v>391</v>
       </c>
@@ -20246,7 +20231,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="363" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:19" ht="29.25">
       <c r="A363" s="2" t="s">
         <v>391</v>
       </c>
@@ -20303,7 +20288,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="364" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:19" ht="39">
       <c r="A364" s="2" t="s">
         <v>391</v>
       </c>
@@ -20360,7 +20345,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="365" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:19" ht="39">
       <c r="A365" s="2" t="s">
         <v>391</v>
       </c>
@@ -20417,7 +20402,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="366" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:19" ht="39">
       <c r="A366" s="2" t="s">
         <v>391</v>
       </c>
@@ -20474,7 +20459,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="367" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:19" ht="39">
       <c r="A367" s="2" t="s">
         <v>391</v>
       </c>
@@ -20531,7 +20516,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="368" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:19" ht="39">
       <c r="A368" s="2" t="s">
         <v>391</v>
       </c>
@@ -20588,7 +20573,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="369" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:19" ht="39">
       <c r="A369" s="2" t="s">
         <v>391</v>
       </c>
@@ -20645,7 +20630,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="370" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:19" ht="39">
       <c r="A370" s="2" t="s">
         <v>391</v>
       </c>
@@ -20702,7 +20687,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="371" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:19" ht="39">
       <c r="A371" s="2" t="s">
         <v>391</v>
       </c>
@@ -20759,7 +20744,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="372" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:19" ht="39">
       <c r="A372" s="2" t="s">
         <v>424</v>
       </c>
@@ -20816,7 +20801,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="373" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:19" ht="39">
       <c r="A373" s="2" t="s">
         <v>424</v>
       </c>
@@ -20873,7 +20858,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="374" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:19" ht="39">
       <c r="A374" s="2" t="s">
         <v>424</v>
       </c>
@@ -20930,7 +20915,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="375" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:19" ht="48.75">
       <c r="A375" s="2" t="s">
         <v>424</v>
       </c>
@@ -20989,7 +20974,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="376" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:19" ht="39">
       <c r="A376" s="2" t="s">
         <v>424</v>
       </c>
@@ -21034,7 +21019,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="377" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:19" ht="39">
       <c r="A377" s="2" t="s">
         <v>424</v>
       </c>
@@ -21079,7 +21064,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="378" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:19" ht="39">
       <c r="A378" s="2" t="s">
         <v>424</v>
       </c>
@@ -21124,7 +21109,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="379" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:19" ht="39">
       <c r="A379" s="2" t="s">
         <v>424</v>
       </c>
@@ -21177,7 +21162,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="380" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:19" ht="39">
       <c r="A380" s="2" t="s">
         <v>424</v>
       </c>
@@ -21222,7 +21207,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="381" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:19" ht="39">
       <c r="A381" s="2" t="s">
         <v>424</v>
       </c>
@@ -21281,7 +21266,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="382" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:19" ht="48.75">
       <c r="A382" s="2" t="s">
         <v>424</v>
       </c>
@@ -21340,7 +21325,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="383" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:19" ht="29.25">
       <c r="A383" s="2" t="s">
         <v>444</v>
       </c>
@@ -21397,7 +21382,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="384" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:19" ht="29.25">
       <c r="A384" s="2" t="s">
         <v>444</v>
       </c>
@@ -21454,7 +21439,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="385" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:19" ht="39">
       <c r="A385" s="2" t="s">
         <v>444</v>
       </c>
@@ -21513,7 +21498,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="386" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:19" ht="39">
       <c r="A386" s="2" t="s">
         <v>444</v>
       </c>
@@ -21568,7 +21553,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="387" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:19" ht="48.75">
       <c r="A387" s="2" t="s">
         <v>444</v>
       </c>
@@ -21627,7 +21612,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="388" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:19" ht="29.25">
       <c r="A388" s="2" t="s">
         <v>444</v>
       </c>
@@ -21678,7 +21663,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="389" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:19" ht="39">
       <c r="A389" s="2" t="s">
         <v>454</v>
       </c>
@@ -21737,7 +21722,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="390" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:19" ht="48.75">
       <c r="A390" s="2" t="s">
         <v>454</v>
       </c>
@@ -21796,7 +21781,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="391" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:19" ht="48.75">
       <c r="A391" s="2" t="s">
         <v>454</v>
       </c>
@@ -21855,7 +21840,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="392" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:19" ht="58.5">
       <c r="A392" s="2" t="s">
         <v>454</v>
       </c>
@@ -21914,7 +21899,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="393" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:19" ht="58.5">
       <c r="A393" s="2" t="s">
         <v>454</v>
       </c>
@@ -21969,7 +21954,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="394" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:19" ht="19.5">
       <c r="A394" s="2" t="s">
         <v>464</v>
       </c>
@@ -22024,7 +22009,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="395" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:19" ht="19.5">
       <c r="A395" s="2" t="s">
         <v>464</v>
       </c>
@@ -22079,7 +22064,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="396" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:19" ht="39">
       <c r="A396" s="2" t="s">
         <v>464</v>
       </c>
@@ -22136,7 +22121,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="397" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:19" ht="19.5">
       <c r="A397" s="2" t="s">
         <v>464</v>
       </c>
@@ -22175,7 +22160,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="398" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:19" ht="19.5">
       <c r="A398" s="2" t="s">
         <v>464</v>
       </c>
@@ -22208,7 +22193,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="399" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:19" ht="19.5">
       <c r="A399" s="2" t="s">
         <v>464</v>
       </c>
@@ -22241,7 +22226,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="400" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:19" ht="19.5">
       <c r="A400" s="2" t="s">
         <v>464</v>
       </c>
@@ -22274,7 +22259,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="401" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:19" ht="19.5">
       <c r="A401" s="2" t="s">
         <v>464</v>
       </c>
@@ -22313,7 +22298,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="402" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:19" ht="19.5">
       <c r="A402" s="2" t="s">
         <v>464</v>
       </c>
@@ -22352,7 +22337,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="403" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:19" ht="19.5">
       <c r="A403" s="2" t="s">
         <v>464</v>
       </c>
@@ -22391,7 +22376,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="404" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:19" ht="29.25">
       <c r="A404" s="2" t="s">
         <v>464</v>
       </c>
@@ -22450,7 +22435,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="405" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:19" ht="19.5">
       <c r="A405" s="2" t="s">
         <v>464</v>
       </c>
@@ -22507,7 +22492,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="406" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:19" ht="29.25">
       <c r="A406" s="2" t="s">
         <v>464</v>
       </c>
@@ -22566,7 +22551,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="407" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:19" ht="29.25">
       <c r="A407" s="2" t="s">
         <v>464</v>
       </c>
@@ -22617,7 +22602,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="408" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:19" ht="29.25">
       <c r="A408" s="2" t="s">
         <v>464</v>
       </c>
@@ -22668,7 +22653,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="409" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:19" ht="19.5">
       <c r="A409" s="2" t="s">
         <v>464</v>
       </c>
@@ -22725,7 +22710,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="410" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:19" ht="29.25">
       <c r="A410" s="2" t="s">
         <v>485</v>
       </c>
@@ -22780,7 +22765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="411" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:19" ht="29.25">
       <c r="A411" s="2" t="s">
         <v>485</v>
       </c>
@@ -22839,7 +22824,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="412" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:19" ht="29.25">
       <c r="A412" s="2" t="s">
         <v>485</v>
       </c>
@@ -22882,7 +22867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="413" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:19" ht="29.25">
       <c r="A413" s="2" t="s">
         <v>485</v>
       </c>
@@ -22935,7 +22920,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="414" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:19" ht="29.25">
       <c r="A414" s="2" t="s">
         <v>485</v>
       </c>
@@ -22980,7 +22965,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="415" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:19" ht="29.25">
       <c r="A415" s="2" t="s">
         <v>485</v>
       </c>
@@ -23025,7 +23010,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="416" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:19" ht="29.25">
       <c r="A416" s="2" t="s">
         <v>485</v>
       </c>
@@ -23070,7 +23055,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="417" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:19" ht="29.25">
       <c r="A417" s="2" t="s">
         <v>485</v>
       </c>
@@ -23115,7 +23100,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="418" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:19" ht="29.25">
       <c r="A418" s="2" t="s">
         <v>485</v>
       </c>
@@ -23160,7 +23145,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="419" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:19" ht="29.25">
       <c r="A419" s="2" t="s">
         <v>485</v>
       </c>
@@ -23205,7 +23190,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="420" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:19" ht="39">
       <c r="A420" s="2" t="s">
         <v>485</v>
       </c>
@@ -23250,7 +23235,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="421" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:19" ht="48.75">
       <c r="A421" s="2" t="s">
         <v>485</v>
       </c>
@@ -23295,7 +23280,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="422" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:19" ht="39">
       <c r="A422" s="2" t="s">
         <v>485</v>
       </c>
@@ -23340,7 +23325,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="423" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:19" ht="39">
       <c r="A423" s="2" t="s">
         <v>485</v>
       </c>
@@ -23385,7 +23370,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="424" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:19" ht="29.25">
       <c r="A424" s="2" t="s">
         <v>485</v>
       </c>
@@ -23442,7 +23427,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="425" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:19" ht="29.25">
       <c r="A425" s="2" t="s">
         <v>485</v>
       </c>
@@ -23497,7 +23482,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="426" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:19" ht="29.25">
       <c r="A426" s="2" t="s">
         <v>485</v>
       </c>
@@ -23552,7 +23537,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="427" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:19" ht="29.25">
       <c r="A427" s="2" t="s">
         <v>485</v>
       </c>
@@ -23607,7 +23592,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="428" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:19" ht="29.25">
       <c r="A428" s="2" t="s">
         <v>485</v>
       </c>
@@ -23664,7 +23649,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="429" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:19" ht="29.25">
       <c r="A429" s="2" t="s">
         <v>485</v>
       </c>
@@ -23721,7 +23706,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="430" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:19" ht="39">
       <c r="A430" s="2" t="s">
         <v>485</v>
       </c>
@@ -23760,7 +23745,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="431" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:19" ht="39">
       <c r="A431" s="2" t="s">
         <v>485</v>
       </c>
@@ -23799,7 +23784,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="432" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:19" ht="39">
       <c r="A432" s="2" t="s">
         <v>485</v>
       </c>
@@ -23838,7 +23823,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="433" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:19" ht="39">
       <c r="A433" s="2" t="s">
         <v>485</v>
       </c>
@@ -23877,7 +23862,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="434" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:19" ht="39">
       <c r="A434" s="2" t="s">
         <v>485</v>
       </c>
@@ -23916,7 +23901,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="435" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:19" ht="39">
       <c r="A435" s="2" t="s">
         <v>485</v>
       </c>
@@ -23955,7 +23940,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="436" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:19" ht="39">
       <c r="A436" s="2" t="s">
         <v>485</v>
       </c>
@@ -23994,7 +23979,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="437" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:19" ht="39">
       <c r="A437" s="2" t="s">
         <v>485</v>
       </c>
@@ -24033,7 +24018,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="438" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:19" ht="39">
       <c r="A438" s="2" t="s">
         <v>485</v>
       </c>
@@ -24072,7 +24057,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="439" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:19" ht="39">
       <c r="A439" s="2" t="s">
         <v>485</v>
       </c>
@@ -24111,7 +24096,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="440" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:19" ht="39">
       <c r="A440" s="2" t="s">
         <v>485</v>
       </c>
@@ -24150,7 +24135,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="441" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:19" ht="39">
       <c r="A441" s="2" t="s">
         <v>485</v>
       </c>
@@ -24189,7 +24174,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="442" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:19" ht="29.25">
       <c r="A442" s="2" t="s">
         <v>485</v>
       </c>
@@ -24248,7 +24233,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="443" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:19" ht="29.25">
       <c r="A443" s="2" t="s">
         <v>485</v>
       </c>
@@ -24287,7 +24272,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="444" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:19" ht="29.25">
       <c r="A444" s="2" t="s">
         <v>522</v>
       </c>
@@ -24344,7 +24329,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="445" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:19" ht="29.25">
       <c r="A445" s="2" t="s">
         <v>522</v>
       </c>
@@ -24401,7 +24386,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="446" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:19" ht="29.25">
       <c r="A446" s="2" t="s">
         <v>522</v>
       </c>
@@ -24458,7 +24443,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="447" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:19" ht="29.25">
       <c r="A447" s="2" t="s">
         <v>522</v>
       </c>
@@ -24515,7 +24500,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="448" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:19" ht="48.75">
       <c r="A448" s="2" t="s">
         <v>522</v>
       </c>
@@ -24572,7 +24557,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="449" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:19" ht="29.25">
       <c r="A449" s="2" t="s">
         <v>522</v>
       </c>
@@ -24629,7 +24614,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="450" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:19" ht="29.25">
       <c r="A450" s="2" t="s">
         <v>522</v>
       </c>
@@ -24686,7 +24671,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="451" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:19" ht="29.25">
       <c r="A451" s="2" t="s">
         <v>522</v>
       </c>
@@ -24745,7 +24730,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="452" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:19" ht="29.25">
       <c r="A452" s="2" t="s">
         <v>522</v>
       </c>
@@ -24804,7 +24789,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="453" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:19" ht="29.25">
       <c r="A453" s="2" t="s">
         <v>522</v>
       </c>
@@ -24863,7 +24848,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="454" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:19" ht="29.25">
       <c r="A454" s="2" t="s">
         <v>522</v>
       </c>
@@ -24920,7 +24905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="455" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:19" ht="29.25">
       <c r="A455" s="2" t="s">
         <v>522</v>
       </c>
@@ -24977,7 +24962,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="456" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:19" ht="29.25">
       <c r="A456" s="2" t="s">
         <v>522</v>
       </c>
@@ -25034,7 +25019,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="457" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:19" ht="29.25">
       <c r="A457" s="2" t="s">
         <v>522</v>
       </c>
@@ -25091,7 +25076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="458" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:19" ht="29.25">
       <c r="A458" s="2" t="s">
         <v>522</v>
       </c>
@@ -25150,7 +25135,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="459" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:19" ht="48.75">
       <c r="A459" s="2" t="s">
         <v>522</v>
       </c>
@@ -25209,7 +25194,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="460" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:19" ht="29.25">
       <c r="A460" s="2" t="s">
         <v>522</v>
       </c>
@@ -25268,7 +25253,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="461" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:19" ht="39">
       <c r="A461" s="2" t="s">
         <v>522</v>
       </c>
@@ -25325,7 +25310,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="462" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:19" ht="39">
       <c r="A462" s="2" t="s">
         <v>522</v>
       </c>
@@ -25382,7 +25367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="463" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:19" ht="29.25">
       <c r="A463" s="2" t="s">
         <v>522</v>
       </c>
@@ -25425,7 +25410,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="464" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:19" ht="29.25">
       <c r="A464" s="2" t="s">
         <v>522</v>
       </c>
@@ -25484,7 +25469,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="465" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:19" ht="29.25">
       <c r="A465" s="2" t="s">
         <v>522</v>
       </c>
@@ -25543,7 +25528,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="466" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:19" ht="29.25">
       <c r="A466" s="2" t="s">
         <v>522</v>
       </c>
@@ -25594,7 +25579,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="467" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:19" ht="39">
       <c r="A467" s="2" t="s">
         <v>522</v>
       </c>
@@ -25631,7 +25616,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="468" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:19" ht="39">
       <c r="A468" s="2" t="s">
         <v>522</v>
       </c>
@@ -25688,7 +25673,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="469" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:19" ht="39">
       <c r="A469" s="2" t="s">
         <v>522</v>
       </c>
@@ -25745,9 +25730,9 @@
         <v>557</v>
       </c>
     </row>
-    <row r="470" spans="1:19" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:19" ht="0" hidden="1" customHeight="1"/>
+    <row r="471" spans="1:19" ht="18" customHeight="1"/>
+    <row r="472" spans="1:19" ht="17.100000000000001" customHeight="1">
       <c r="A472" s="12" t="s">
         <v>560</v>
       </c>

</xml_diff>

<commit_message>
Okno serwisowe - 28.02.2023
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="18060" windowHeight="7050"/>
   </bookViews>
@@ -1700,13 +1705,13 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 07-02-2023, 13:42</t>
+    <t>Last update: 28-02-2023, 09:55</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$-10809]0.0;\-0.0;0.0"/>
     <numFmt numFmtId="165" formatCode="[$-10809]0.00;\-0.00;0.00"/>
@@ -1715,7 +1720,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000;\-0.000;0.000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1913,6 +1918,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1933,7 +1946,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1996,7 +2009,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2028,9 +2041,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2062,6 +2076,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -2237,15 +2252,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S472"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2257,17 +2272,17 @@
     <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="36" customHeight="1">
+    <row r="1" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:19" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:19" ht="25.5">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2326,7 +2341,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="19.5">
+    <row r="4" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2381,7 +2396,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2436,7 +2451,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -2491,7 +2506,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -2546,7 +2561,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -2601,7 +2616,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -2656,7 +2671,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -2711,7 +2726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2766,7 +2781,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -2821,7 +2836,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2876,7 +2891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="19.5">
+    <row r="14" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -2931,7 +2946,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="19.5">
+    <row r="15" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -2986,7 +3001,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -3025,7 +3040,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="29.25">
+    <row r="17" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -3082,7 +3097,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="97.5">
+    <row r="18" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -3137,7 +3152,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="97.5">
+    <row r="19" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -3192,7 +3207,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="97.5">
+    <row r="20" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -3247,7 +3262,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="19.5">
+    <row r="21" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -3302,7 +3317,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="29.25">
+    <row r="22" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -3359,7 +3374,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="29.25">
+    <row r="23" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -3416,7 +3431,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="29.25">
+    <row r="24" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -3461,7 +3476,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="68.25">
+    <row r="25" spans="1:19" ht="63" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -3506,7 +3521,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="29.25">
+    <row r="26" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
@@ -3551,7 +3566,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="29.25">
+    <row r="27" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -3596,7 +3611,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="29.25">
+    <row r="28" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
@@ -3647,7 +3662,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="39">
+    <row r="29" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
@@ -3704,7 +3719,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="39">
+    <row r="30" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
@@ -3761,7 +3776,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="39">
+    <row r="31" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
@@ -3818,7 +3833,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="39">
+    <row r="32" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -3875,7 +3890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="19.5">
+    <row r="33" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>66</v>
       </c>
@@ -3930,7 +3945,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="29.25">
+    <row r="34" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -3975,7 +3990,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="29.25">
+    <row r="35" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
@@ -4020,7 +4035,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="29.25">
+    <row r="36" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>66</v>
       </c>
@@ -4065,7 +4080,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="29.25">
+    <row r="37" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>66</v>
       </c>
@@ -4110,7 +4125,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="29.25">
+    <row r="38" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>66</v>
       </c>
@@ -4155,7 +4170,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="29.25">
+    <row r="39" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
@@ -4200,7 +4215,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="39">
+    <row r="40" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>66</v>
       </c>
@@ -4239,7 +4254,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="97.5">
+    <row r="41" spans="1:19" ht="81" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>66</v>
       </c>
@@ -4298,7 +4313,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="97.5">
+    <row r="42" spans="1:19" ht="81" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>66</v>
       </c>
@@ -4357,7 +4372,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="97.5">
+    <row r="43" spans="1:19" ht="81" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>66</v>
       </c>
@@ -4416,7 +4431,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="97.5">
+    <row r="44" spans="1:19" ht="81" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>66</v>
       </c>
@@ -4475,7 +4490,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="97.5">
+    <row r="45" spans="1:19" ht="81" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>66</v>
       </c>
@@ -4534,7 +4549,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="97.5">
+    <row r="46" spans="1:19" ht="81" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>66</v>
       </c>
@@ -4593,7 +4608,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="48.75">
+    <row r="47" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>66</v>
       </c>
@@ -4642,7 +4657,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="48.75">
+    <row r="48" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>66</v>
       </c>
@@ -4691,7 +4706,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="19.5">
+    <row r="49" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>66</v>
       </c>
@@ -4746,7 +4761,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="29.25">
+    <row r="50" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>66</v>
       </c>
@@ -4797,7 +4812,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="19.5">
+    <row r="51" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>95</v>
       </c>
@@ -4852,7 +4867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="19.5">
+    <row r="52" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>95</v>
       </c>
@@ -4909,7 +4924,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="19.5">
+    <row r="53" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>95</v>
       </c>
@@ -4966,7 +4981,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="19.5">
+    <row r="54" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>95</v>
       </c>
@@ -5023,7 +5038,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="19.5">
+    <row r="55" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>95</v>
       </c>
@@ -5080,7 +5095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="19.5">
+    <row r="56" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>95</v>
       </c>
@@ -5137,7 +5152,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="19.5">
+    <row r="57" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>95</v>
       </c>
@@ -5194,7 +5209,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="19.5">
+    <row r="58" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>95</v>
       </c>
@@ -5251,7 +5266,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="29.25">
+    <row r="59" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>95</v>
       </c>
@@ -5308,7 +5323,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="19.5">
+    <row r="60" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>95</v>
       </c>
@@ -5365,7 +5380,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="29.25">
+    <row r="61" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>95</v>
       </c>
@@ -5422,7 +5437,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="29.25">
+    <row r="62" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>95</v>
       </c>
@@ -5479,7 +5494,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="29.25">
+    <row r="63" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>95</v>
       </c>
@@ -5536,7 +5551,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="19.5">
+    <row r="64" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>95</v>
       </c>
@@ -5593,7 +5608,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="29.25">
+    <row r="65" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>95</v>
       </c>
@@ -5650,7 +5665,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="29.25">
+    <row r="66" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>95</v>
       </c>
@@ -5707,7 +5722,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="29.25">
+    <row r="67" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>95</v>
       </c>
@@ -5764,7 +5779,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="29.25">
+    <row r="68" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>95</v>
       </c>
@@ -5811,15 +5826,17 @@
         <v>421</v>
       </c>
       <c r="P68" s="4">
-        <v>455.1</v>
-      </c>
-      <c r="Q68" s="3"/>
+        <v>457.2</v>
+      </c>
+      <c r="Q68" s="4">
+        <v>475.8</v>
+      </c>
       <c r="R68" s="3"/>
       <c r="S68" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="29.25">
+    <row r="69" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>95</v>
       </c>
@@ -5866,15 +5883,17 @@
         <v>24.2</v>
       </c>
       <c r="P69" s="4">
-        <v>31.7</v>
-      </c>
-      <c r="Q69" s="3"/>
+        <v>31.9</v>
+      </c>
+      <c r="Q69" s="4">
+        <v>28.5</v>
+      </c>
       <c r="R69" s="3"/>
       <c r="S69" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="29.25">
+    <row r="70" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>95</v>
       </c>
@@ -5921,15 +5940,17 @@
         <v>261.3</v>
       </c>
       <c r="P70" s="4">
-        <v>260.39999999999998</v>
-      </c>
-      <c r="Q70" s="3"/>
+        <v>261.60000000000002</v>
+      </c>
+      <c r="Q70" s="4">
+        <v>246.5</v>
+      </c>
       <c r="R70" s="3"/>
       <c r="S70" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="29.25">
+    <row r="71" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>95</v>
       </c>
@@ -5976,15 +5997,17 @@
         <v>22.6</v>
       </c>
       <c r="P71" s="4">
-        <v>22.8</v>
-      </c>
-      <c r="Q71" s="3"/>
+        <v>22.9</v>
+      </c>
+      <c r="Q71" s="4">
+        <v>25.4</v>
+      </c>
       <c r="R71" s="3"/>
       <c r="S71" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="19.5">
+    <row r="72" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>95</v>
       </c>
@@ -6039,7 +6062,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="19.5">
+    <row r="73" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>95</v>
       </c>
@@ -6094,7 +6117,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="19.5">
+    <row r="74" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>95</v>
       </c>
@@ -6149,7 +6172,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="19.5">
+    <row r="75" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>95</v>
       </c>
@@ -6206,7 +6229,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="29.25">
+    <row r="76" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>95</v>
       </c>
@@ -6263,7 +6286,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="29.25">
+    <row r="77" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>95</v>
       </c>
@@ -6302,7 +6325,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="19.5">
+    <row r="78" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>95</v>
       </c>
@@ -6359,7 +6382,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="19.5">
+    <row r="79" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>95</v>
       </c>
@@ -6416,7 +6439,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="19.5">
+    <row r="80" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>95</v>
       </c>
@@ -6473,7 +6496,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="19.5">
+    <row r="81" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>95</v>
       </c>
@@ -6514,7 +6537,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="29.25">
+    <row r="82" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>95</v>
       </c>
@@ -6559,7 +6582,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="29.25">
+    <row r="83" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>95</v>
       </c>
@@ -6604,7 +6627,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="19.5">
+    <row r="84" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>95</v>
       </c>
@@ -6639,7 +6662,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="29.25">
+    <row r="85" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>95</v>
       </c>
@@ -6674,7 +6697,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="19.5">
+    <row r="86" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>95</v>
       </c>
@@ -6729,7 +6752,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="19.5">
+    <row r="87" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>95</v>
       </c>
@@ -6768,7 +6791,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="19.5">
+    <row r="88" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>95</v>
       </c>
@@ -6825,7 +6848,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="19.5">
+    <row r="89" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>95</v>
       </c>
@@ -6882,7 +6905,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="19.5">
+    <row r="90" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>95</v>
       </c>
@@ -6923,7 +6946,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="29.25">
+    <row r="91" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>95</v>
       </c>
@@ -6974,7 +6997,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="19.5">
+    <row r="92" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>95</v>
       </c>
@@ -7013,7 +7036,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="19.5">
+    <row r="93" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>95</v>
       </c>
@@ -7052,7 +7075,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="19.5">
+    <row r="94" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>95</v>
       </c>
@@ -7091,7 +7114,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="19.5">
+    <row r="95" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>95</v>
       </c>
@@ -7144,7 +7167,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="48.75">
+    <row r="96" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>149</v>
       </c>
@@ -7181,7 +7204,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="48.75">
+    <row r="97" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>149</v>
       </c>
@@ -7218,7 +7241,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="48.75">
+    <row r="98" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>149</v>
       </c>
@@ -7255,7 +7278,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="48.75">
+    <row r="99" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>149</v>
       </c>
@@ -7296,7 +7319,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="48.75">
+    <row r="100" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>149</v>
       </c>
@@ -7337,7 +7360,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="48.75">
+    <row r="101" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>149</v>
       </c>
@@ -7378,7 +7401,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="48.75">
+    <row r="102" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>149</v>
       </c>
@@ -7419,7 +7442,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="48.75">
+    <row r="103" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>149</v>
       </c>
@@ -7460,7 +7483,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="48.75">
+    <row r="104" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>149</v>
       </c>
@@ -7501,7 +7524,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="29.25">
+    <row r="105" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>149</v>
       </c>
@@ -7538,7 +7561,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="19.5">
+    <row r="106" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>149</v>
       </c>
@@ -7595,7 +7618,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="19.5">
+    <row r="107" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>149</v>
       </c>
@@ -7652,7 +7675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="19.5">
+    <row r="108" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>149</v>
       </c>
@@ -7709,7 +7732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="19.5">
+    <row r="109" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>149</v>
       </c>
@@ -7746,7 +7769,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="19.5">
+    <row r="110" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>149</v>
       </c>
@@ -7783,7 +7806,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="19.5">
+    <row r="111" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>149</v>
       </c>
@@ -7820,7 +7843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="29.25">
+    <row r="112" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>149</v>
       </c>
@@ -7865,7 +7888,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="19.5">
+    <row r="113" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>149</v>
       </c>
@@ -7912,7 +7935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="39">
+    <row r="114" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>149</v>
       </c>
@@ -7959,7 +7982,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="48.75">
+    <row r="115" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>149</v>
       </c>
@@ -8006,7 +8029,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="58.5">
+    <row r="116" spans="1:19" ht="54" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>149</v>
       </c>
@@ -8053,7 +8076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="29.25">
+    <row r="117" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>149</v>
       </c>
@@ -8100,7 +8123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="29.25">
+    <row r="118" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>149</v>
       </c>
@@ -8145,7 +8168,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="19.5">
+    <row r="119" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>149</v>
       </c>
@@ -8192,7 +8215,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="39">
+    <row r="120" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>149</v>
       </c>
@@ -8239,7 +8262,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="48.75">
+    <row r="121" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>149</v>
       </c>
@@ -8286,7 +8309,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="58.5">
+    <row r="122" spans="1:19" ht="54" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>149</v>
       </c>
@@ -8333,7 +8356,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="29.25">
+    <row r="123" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>149</v>
       </c>
@@ -8380,7 +8403,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="48.75">
+    <row r="124" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>149</v>
       </c>
@@ -8419,7 +8442,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="48.75">
+    <row r="125" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>149</v>
       </c>
@@ -8458,7 +8481,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="29.25">
+    <row r="126" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>149</v>
       </c>
@@ -8515,7 +8538,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="29.25">
+    <row r="127" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>149</v>
       </c>
@@ -8550,7 +8573,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="29.25">
+    <row r="128" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>149</v>
       </c>
@@ -8585,7 +8608,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="29.25">
+    <row r="129" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>149</v>
       </c>
@@ -8620,7 +8643,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="29.25">
+    <row r="130" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>149</v>
       </c>
@@ -8655,7 +8678,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="29.25">
+    <row r="131" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>149</v>
       </c>
@@ -8690,7 +8713,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="29.25">
+    <row r="132" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>149</v>
       </c>
@@ -8725,7 +8748,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="29.25">
+    <row r="133" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>149</v>
       </c>
@@ -8760,7 +8783,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="29.25">
+    <row r="134" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>149</v>
       </c>
@@ -8795,7 +8818,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="29.25">
+    <row r="135" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>149</v>
       </c>
@@ -8830,7 +8853,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="29.25">
+    <row r="136" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>149</v>
       </c>
@@ -8865,7 +8888,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="29.25">
+    <row r="137" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>149</v>
       </c>
@@ -8900,7 +8923,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="29.25">
+    <row r="138" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>149</v>
       </c>
@@ -8935,7 +8958,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="29.25">
+    <row r="139" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>149</v>
       </c>
@@ -8970,7 +8993,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="29.25">
+    <row r="140" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>149</v>
       </c>
@@ -9005,7 +9028,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="29.25">
+    <row r="141" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>149</v>
       </c>
@@ -9040,7 +9063,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="29.25">
+    <row r="142" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>149</v>
       </c>
@@ -9075,7 +9098,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="48.75">
+    <row r="143" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>149</v>
       </c>
@@ -9134,7 +9157,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="58.5">
+    <row r="144" spans="1:19" ht="54" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>149</v>
       </c>
@@ -9193,7 +9216,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="58.5">
+    <row r="145" spans="1:19" ht="54" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>149</v>
       </c>
@@ -9228,7 +9251,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="58.5">
+    <row r="146" spans="1:19" ht="54" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>149</v>
       </c>
@@ -9263,7 +9286,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="58.5">
+    <row r="147" spans="1:19" ht="54" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>149</v>
       </c>
@@ -9322,7 +9345,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="58.5">
+    <row r="148" spans="1:19" ht="54" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>149</v>
       </c>
@@ -9381,7 +9404,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="58.5">
+    <row r="149" spans="1:19" ht="54" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>149</v>
       </c>
@@ -9440,7 +9463,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="29.25">
+    <row r="150" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>149</v>
       </c>
@@ -9491,7 +9514,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="58.5">
+    <row r="151" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>149</v>
       </c>
@@ -9546,7 +9569,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="58.5">
+    <row r="152" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>149</v>
       </c>
@@ -9601,7 +9624,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="58.5">
+    <row r="153" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>149</v>
       </c>
@@ -9656,7 +9679,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="58.5">
+    <row r="154" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>149</v>
       </c>
@@ -9711,7 +9734,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="29.25">
+    <row r="155" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>205</v>
       </c>
@@ -9746,7 +9769,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="19.5">
+    <row r="156" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>205</v>
       </c>
@@ -9803,7 +9826,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="39">
+    <row r="157" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>205</v>
       </c>
@@ -9838,7 +9861,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="39">
+    <row r="158" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>205</v>
       </c>
@@ -9873,7 +9896,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="39">
+    <row r="159" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>205</v>
       </c>
@@ -9908,7 +9931,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="160" spans="1:19" ht="39">
+    <row r="160" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>205</v>
       </c>
@@ -9943,7 +9966,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="39">
+    <row r="161" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>205</v>
       </c>
@@ -9978,7 +10001,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="19.5">
+    <row r="162" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>205</v>
       </c>
@@ -10013,7 +10036,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="19.5">
+    <row r="163" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>205</v>
       </c>
@@ -10048,7 +10071,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="19.5">
+    <row r="164" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>205</v>
       </c>
@@ -10083,7 +10106,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="19.5">
+    <row r="165" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>205</v>
       </c>
@@ -10118,7 +10141,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="19.5">
+    <row r="166" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>205</v>
       </c>
@@ -10153,7 +10176,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="19.5">
+    <row r="167" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>205</v>
       </c>
@@ -10188,7 +10211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="19.5">
+    <row r="168" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>205</v>
       </c>
@@ -10223,7 +10246,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="19.5">
+    <row r="169" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>205</v>
       </c>
@@ -10258,7 +10281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="29.25">
+    <row r="170" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>205</v>
       </c>
@@ -10297,7 +10320,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="29.25">
+    <row r="171" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>205</v>
       </c>
@@ -10336,7 +10359,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="29.25">
+    <row r="172" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>205</v>
       </c>
@@ -10393,7 +10416,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="29.25">
+    <row r="173" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>205</v>
       </c>
@@ -10450,7 +10473,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="29.25">
+    <row r="174" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>205</v>
       </c>
@@ -10507,7 +10530,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="29.25">
+    <row r="175" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>205</v>
       </c>
@@ -10564,7 +10587,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="29.25">
+    <row r="176" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>205</v>
       </c>
@@ -10621,7 +10644,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="177" spans="1:19" ht="19.5">
+    <row r="177" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>205</v>
       </c>
@@ -10666,7 +10689,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="178" spans="1:19" ht="39">
+    <row r="178" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>205</v>
       </c>
@@ -10711,7 +10734,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="19.5">
+    <row r="179" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>205</v>
       </c>
@@ -10756,7 +10779,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="39">
+    <row r="180" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>205</v>
       </c>
@@ -10801,7 +10824,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="39">
+    <row r="181" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>205</v>
       </c>
@@ -10846,7 +10869,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="182" spans="1:19" ht="39">
+    <row r="182" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>205</v>
       </c>
@@ -10891,7 +10914,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:19" ht="39">
+    <row r="183" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>205</v>
       </c>
@@ -10936,7 +10959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="39">
+    <row r="184" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>205</v>
       </c>
@@ -10975,7 +10998,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="39">
+    <row r="185" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>205</v>
       </c>
@@ -11014,7 +11037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="186" spans="1:19" ht="39">
+    <row r="186" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>205</v>
       </c>
@@ -11053,7 +11076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="39">
+    <row r="187" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>205</v>
       </c>
@@ -11092,7 +11115,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="39">
+    <row r="188" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>205</v>
       </c>
@@ -11131,7 +11154,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="39">
+    <row r="189" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>205</v>
       </c>
@@ -11170,7 +11193,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="39">
+    <row r="190" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>205</v>
       </c>
@@ -11209,7 +11232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="39">
+    <row r="191" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>205</v>
       </c>
@@ -11248,7 +11271,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="39">
+    <row r="192" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>205</v>
       </c>
@@ -11287,7 +11310,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="193" spans="1:19" ht="39">
+    <row r="193" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>205</v>
       </c>
@@ -11326,7 +11349,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="39">
+    <row r="194" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>205</v>
       </c>
@@ -11365,7 +11388,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="195" spans="1:19" ht="39">
+    <row r="195" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>205</v>
       </c>
@@ -11404,7 +11427,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="196" spans="1:19" ht="19.5">
+    <row r="196" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>205</v>
       </c>
@@ -11445,7 +11468,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="19.5">
+    <row r="197" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>205</v>
       </c>
@@ -11500,7 +11523,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="19.5">
+    <row r="198" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>205</v>
       </c>
@@ -11555,7 +11578,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="19.5">
+    <row r="199" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>245</v>
       </c>
@@ -11612,7 +11635,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="200" spans="1:19" ht="29.25">
+    <row r="200" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>245</v>
       </c>
@@ -11669,7 +11692,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="201" spans="1:19" ht="19.5">
+    <row r="201" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>245</v>
       </c>
@@ -11726,7 +11749,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="202" spans="1:19" ht="19.5">
+    <row r="202" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>245</v>
       </c>
@@ -11761,7 +11784,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="203" spans="1:19" ht="19.5">
+    <row r="203" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>245</v>
       </c>
@@ -11796,7 +11819,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="204" spans="1:19" ht="29.25">
+    <row r="204" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>245</v>
       </c>
@@ -11851,7 +11874,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="205" spans="1:19" ht="19.5">
+    <row r="205" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>245</v>
       </c>
@@ -11906,7 +11929,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="206" spans="1:19" ht="19.5">
+    <row r="206" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>245</v>
       </c>
@@ -11951,7 +11974,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="207" spans="1:19" ht="29.25">
+    <row r="207" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>245</v>
       </c>
@@ -12006,7 +12029,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="208" spans="1:19" ht="29.25">
+    <row r="208" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>245</v>
       </c>
@@ -12057,7 +12080,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="209" spans="1:19" ht="39">
+    <row r="209" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>245</v>
       </c>
@@ -12114,7 +12137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="210" spans="1:19" ht="19.5">
+    <row r="210" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>266</v>
       </c>
@@ -12149,7 +12172,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="211" spans="1:19" ht="19.5">
+    <row r="211" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>266</v>
       </c>
@@ -12204,7 +12227,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="212" spans="1:19" ht="29.25">
+    <row r="212" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>266</v>
       </c>
@@ -12259,7 +12282,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="213" spans="1:19" ht="29.25">
+    <row r="213" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>266</v>
       </c>
@@ -12310,7 +12333,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="214" spans="1:19" ht="29.25">
+    <row r="214" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>272</v>
       </c>
@@ -12367,7 +12390,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:19" ht="29.25">
+    <row r="215" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>272</v>
       </c>
@@ -12424,7 +12447,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="216" spans="1:19" ht="29.25">
+    <row r="216" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>272</v>
       </c>
@@ -12463,7 +12486,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="217" spans="1:19" ht="29.25">
+    <row r="217" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>272</v>
       </c>
@@ -12502,7 +12525,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="218" spans="1:19" ht="29.25">
+    <row r="218" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>272</v>
       </c>
@@ -12541,7 +12564,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="219" spans="1:19" ht="29.25">
+    <row r="219" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>272</v>
       </c>
@@ -12598,7 +12621,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="220" spans="1:19" ht="29.25">
+    <row r="220" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>272</v>
       </c>
@@ -12655,7 +12678,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="221" spans="1:19" ht="29.25">
+    <row r="221" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>272</v>
       </c>
@@ -12712,7 +12735,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="222" spans="1:19" ht="29.25">
+    <row r="222" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>272</v>
       </c>
@@ -12757,7 +12780,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="223" spans="1:19" ht="29.25">
+    <row r="223" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>272</v>
       </c>
@@ -12802,7 +12825,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="224" spans="1:19" ht="29.25">
+    <row r="224" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>272</v>
       </c>
@@ -12847,7 +12870,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="225" spans="1:19" ht="29.25">
+    <row r="225" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>272</v>
       </c>
@@ -12892,7 +12915,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="226" spans="1:19" ht="29.25">
+    <row r="226" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>272</v>
       </c>
@@ -12937,7 +12960,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="227" spans="1:19" ht="29.25">
+    <row r="227" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>272</v>
       </c>
@@ -12982,7 +13005,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="228" spans="1:19" ht="29.25">
+    <row r="228" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>272</v>
       </c>
@@ -13027,7 +13050,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="229" spans="1:19" ht="29.25">
+    <row r="229" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>272</v>
       </c>
@@ -13072,7 +13095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="230" spans="1:19" ht="39">
+    <row r="230" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>272</v>
       </c>
@@ -13117,7 +13140,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="231" spans="1:19" ht="29.25">
+    <row r="231" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>272</v>
       </c>
@@ -13162,7 +13185,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="232" spans="1:19" ht="39">
+    <row r="232" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>272</v>
       </c>
@@ -13207,7 +13230,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="233" spans="1:19" ht="29.25">
+    <row r="233" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>272</v>
       </c>
@@ -13252,7 +13275,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="234" spans="1:19" ht="29.25">
+    <row r="234" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>272</v>
       </c>
@@ -13297,7 +13320,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="235" spans="1:19" ht="29.25">
+    <row r="235" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>272</v>
       </c>
@@ -13342,7 +13365,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="236" spans="1:19" ht="29.25">
+    <row r="236" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>272</v>
       </c>
@@ -13387,7 +13410,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="237" spans="1:19" ht="29.25">
+    <row r="237" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>272</v>
       </c>
@@ -13432,7 +13455,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="238" spans="1:19" ht="29.25">
+    <row r="238" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>272</v>
       </c>
@@ -13477,7 +13500,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="29.25">
+    <row r="239" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>272</v>
       </c>
@@ -13522,7 +13545,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="240" spans="1:19" ht="29.25">
+    <row r="240" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>272</v>
       </c>
@@ -13567,7 +13590,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="241" spans="1:19" ht="29.25">
+    <row r="241" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>272</v>
       </c>
@@ -13624,7 +13647,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="242" spans="1:19" ht="29.25">
+    <row r="242" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>272</v>
       </c>
@@ -13681,7 +13704,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="243" spans="1:19" ht="29.25">
+    <row r="243" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>272</v>
       </c>
@@ -13738,7 +13761,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="244" spans="1:19" ht="29.25">
+    <row r="244" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>272</v>
       </c>
@@ -13795,7 +13818,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="245" spans="1:19" ht="29.25">
+    <row r="245" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>272</v>
       </c>
@@ -13852,7 +13875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="246" spans="1:19" ht="29.25">
+    <row r="246" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>272</v>
       </c>
@@ -13909,7 +13932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="247" spans="1:19" ht="29.25">
+    <row r="247" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>272</v>
       </c>
@@ -13966,7 +13989,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="248" spans="1:19" ht="29.25">
+    <row r="248" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>272</v>
       </c>
@@ -14023,7 +14046,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="249" spans="1:19" ht="29.25">
+    <row r="249" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>272</v>
       </c>
@@ -14080,7 +14103,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="250" spans="1:19" ht="29.25">
+    <row r="250" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>272</v>
       </c>
@@ -14137,7 +14160,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="251" spans="1:19" ht="29.25">
+    <row r="251" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>272</v>
       </c>
@@ -14194,7 +14217,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="252" spans="1:19" ht="29.25">
+    <row r="252" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>272</v>
       </c>
@@ -14251,7 +14274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="253" spans="1:19" ht="39">
+    <row r="253" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>272</v>
       </c>
@@ -14292,7 +14315,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="254" spans="1:19" ht="39">
+    <row r="254" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>272</v>
       </c>
@@ -14333,7 +14356,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="255" spans="1:19" ht="39">
+    <row r="255" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>272</v>
       </c>
@@ -14374,7 +14397,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="256" spans="1:19" ht="29.25">
+    <row r="256" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>272</v>
       </c>
@@ -14431,7 +14454,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="257" spans="1:19" ht="48.75">
+    <row r="257" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>272</v>
       </c>
@@ -14488,7 +14511,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="258" spans="1:19" ht="29.25">
+    <row r="258" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>272</v>
       </c>
@@ -14523,7 +14546,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="259" spans="1:19" ht="29.25">
+    <row r="259" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>272</v>
       </c>
@@ -14558,7 +14581,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="260" spans="1:19" ht="29.25">
+    <row r="260" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>272</v>
       </c>
@@ -14593,7 +14616,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="261" spans="1:19" ht="29.25">
+    <row r="261" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>272</v>
       </c>
@@ -14628,7 +14651,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="262" spans="1:19" ht="29.25">
+    <row r="262" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>272</v>
       </c>
@@ -14663,7 +14686,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="263" spans="1:19" ht="29.25">
+    <row r="263" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>272</v>
       </c>
@@ -14698,7 +14721,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="264" spans="1:19" ht="29.25">
+    <row r="264" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>272</v>
       </c>
@@ -14733,7 +14756,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="265" spans="1:19" ht="29.25">
+    <row r="265" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>272</v>
       </c>
@@ -14768,7 +14791,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="266" spans="1:19" ht="29.25">
+    <row r="266" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>272</v>
       </c>
@@ -14819,7 +14842,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="267" spans="1:19" ht="29.25">
+    <row r="267" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>318</v>
       </c>
@@ -14876,7 +14899,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="268" spans="1:19" ht="29.25">
+    <row r="268" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>318</v>
       </c>
@@ -14933,7 +14956,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="269" spans="1:19" ht="29.25">
+    <row r="269" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>318</v>
       </c>
@@ -14990,7 +15013,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="270" spans="1:19" ht="29.25">
+    <row r="270" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>318</v>
       </c>
@@ -15047,7 +15070,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="271" spans="1:19" ht="29.25">
+    <row r="271" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>318</v>
       </c>
@@ -15104,7 +15127,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="272" spans="1:19" ht="29.25">
+    <row r="272" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>318</v>
       </c>
@@ -15161,7 +15184,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="273" spans="1:19" ht="29.25">
+    <row r="273" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>318</v>
       </c>
@@ -15218,7 +15241,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="274" spans="1:19" ht="29.25">
+    <row r="274" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>318</v>
       </c>
@@ -15275,7 +15298,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="275" spans="1:19" ht="29.25">
+    <row r="275" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>318</v>
       </c>
@@ -15332,7 +15355,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="276" spans="1:19" ht="29.25">
+    <row r="276" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>318</v>
       </c>
@@ -15389,7 +15412,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="277" spans="1:19" ht="29.25">
+    <row r="277" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>318</v>
       </c>
@@ -15446,7 +15469,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="278" spans="1:19" ht="29.25">
+    <row r="278" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>318</v>
       </c>
@@ -15503,7 +15526,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="279" spans="1:19" ht="29.25">
+    <row r="279" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>318</v>
       </c>
@@ -15560,7 +15583,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="280" spans="1:19" ht="29.25">
+    <row r="280" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>318</v>
       </c>
@@ -15617,7 +15640,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="281" spans="1:19" ht="29.25">
+    <row r="281" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>318</v>
       </c>
@@ -15674,7 +15697,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="282" spans="1:19" ht="29.25">
+    <row r="282" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>318</v>
       </c>
@@ -15731,7 +15754,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="283" spans="1:19" ht="29.25">
+    <row r="283" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>318</v>
       </c>
@@ -15788,7 +15811,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="284" spans="1:19" ht="29.25">
+    <row r="284" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>318</v>
       </c>
@@ -15845,7 +15868,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="285" spans="1:19" ht="29.25">
+    <row r="285" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>318</v>
       </c>
@@ -15902,7 +15925,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="286" spans="1:19" ht="29.25">
+    <row r="286" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>318</v>
       </c>
@@ -15959,7 +15982,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="287" spans="1:19" ht="29.25">
+    <row r="287" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>318</v>
       </c>
@@ -16010,7 +16033,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="288" spans="1:19" ht="29.25">
+    <row r="288" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>318</v>
       </c>
@@ -16067,7 +16090,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="289" spans="1:19" ht="29.25">
+    <row r="289" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>318</v>
       </c>
@@ -16124,7 +16147,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="290" spans="1:19" ht="29.25">
+    <row r="290" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>318</v>
       </c>
@@ -16175,7 +16198,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="291" spans="1:19" ht="29.25">
+    <row r="291" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>318</v>
       </c>
@@ -16228,7 +16251,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="292" spans="1:19" ht="39">
+    <row r="292" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>318</v>
       </c>
@@ -16277,7 +16300,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="293" spans="1:19" ht="39">
+    <row r="293" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>318</v>
       </c>
@@ -16326,7 +16349,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="294" spans="1:19" ht="19.5">
+    <row r="294" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>350</v>
       </c>
@@ -16383,7 +16406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="295" spans="1:19" ht="68.25">
+    <row r="295" spans="1:19" ht="63" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>350</v>
       </c>
@@ -16440,7 +16463,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="296" spans="1:19" ht="19.5">
+    <row r="296" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>350</v>
       </c>
@@ -16497,7 +16520,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="297" spans="1:19" ht="19.5">
+    <row r="297" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>350</v>
       </c>
@@ -16554,7 +16577,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="298" spans="1:19" ht="19.5">
+    <row r="298" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>350</v>
       </c>
@@ -16611,7 +16634,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="299" spans="1:19" ht="19.5">
+    <row r="299" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>350</v>
       </c>
@@ -16668,7 +16691,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="300" spans="1:19" ht="19.5">
+    <row r="300" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>350</v>
       </c>
@@ -16725,7 +16748,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="301" spans="1:19" ht="19.5">
+    <row r="301" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>350</v>
       </c>
@@ -16782,7 +16805,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="302" spans="1:19" ht="19.5">
+    <row r="302" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
         <v>350</v>
       </c>
@@ -16839,7 +16862,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="303" spans="1:19" ht="19.5">
+    <row r="303" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
         <v>350</v>
       </c>
@@ -16896,7 +16919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="304" spans="1:19" ht="19.5">
+    <row r="304" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>350</v>
       </c>
@@ -16953,7 +16976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="305" spans="1:19" ht="19.5">
+    <row r="305" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>350</v>
       </c>
@@ -16992,7 +17015,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="306" spans="1:19" ht="19.5">
+    <row r="306" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
         <v>350</v>
       </c>
@@ -17049,7 +17072,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="307" spans="1:19" ht="39">
+    <row r="307" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
         <v>350</v>
       </c>
@@ -17106,7 +17129,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="308" spans="1:19" ht="48.75">
+    <row r="308" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
         <v>350</v>
       </c>
@@ -17163,7 +17186,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="309" spans="1:19" ht="39">
+    <row r="309" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
         <v>350</v>
       </c>
@@ -17220,7 +17243,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="310" spans="1:19" ht="39">
+    <row r="310" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
         <v>350</v>
       </c>
@@ -17277,7 +17300,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="311" spans="1:19" ht="29.25">
+    <row r="311" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
         <v>350</v>
       </c>
@@ -17334,7 +17357,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="312" spans="1:19" ht="39">
+    <row r="312" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
         <v>350</v>
       </c>
@@ -17389,7 +17412,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="313" spans="1:19" ht="29.25">
+    <row r="313" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
         <v>350</v>
       </c>
@@ -17446,7 +17469,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="314" spans="1:19" ht="29.25">
+    <row r="314" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
         <v>350</v>
       </c>
@@ -17503,7 +17526,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="315" spans="1:19" ht="39">
+    <row r="315" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
         <v>350</v>
       </c>
@@ -17560,7 +17583,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="316" spans="1:19" ht="29.25">
+    <row r="316" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
         <v>350</v>
       </c>
@@ -17617,7 +17640,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="317" spans="1:19" ht="39">
+    <row r="317" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
         <v>350</v>
       </c>
@@ -17674,7 +17697,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="318" spans="1:19" ht="29.25">
+    <row r="318" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
         <v>350</v>
       </c>
@@ -17731,7 +17754,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="319" spans="1:19" ht="29.25">
+    <row r="319" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
         <v>350</v>
       </c>
@@ -17788,7 +17811,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="320" spans="1:19" ht="39">
+    <row r="320" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
         <v>350</v>
       </c>
@@ -17845,7 +17868,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="321" spans="1:19" ht="39">
+    <row r="321" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
         <v>350</v>
       </c>
@@ -17902,7 +17925,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="322" spans="1:19" ht="68.25">
+    <row r="322" spans="1:19" ht="54" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
         <v>350</v>
       </c>
@@ -17959,7 +17982,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="323" spans="1:19" ht="58.5">
+    <row r="323" spans="1:19" ht="63" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
         <v>350</v>
       </c>
@@ -18016,7 +18039,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="324" spans="1:19" ht="68.25">
+    <row r="324" spans="1:19" ht="63" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
         <v>350</v>
       </c>
@@ -18073,7 +18096,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="325" spans="1:19" ht="68.25">
+    <row r="325" spans="1:19" ht="72" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>350</v>
       </c>
@@ -18130,7 +18153,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="326" spans="1:19" ht="39">
+    <row r="326" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
         <v>350</v>
       </c>
@@ -18187,7 +18210,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="327" spans="1:19" ht="68.25">
+    <row r="327" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
         <v>350</v>
       </c>
@@ -18244,7 +18267,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="328" spans="1:19" ht="58.5">
+    <row r="328" spans="1:19" ht="54" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
         <v>350</v>
       </c>
@@ -18301,7 +18324,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="329" spans="1:19" ht="68.25">
+    <row r="329" spans="1:19" ht="54" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
         <v>350</v>
       </c>
@@ -18358,7 +18381,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="330" spans="1:19" ht="68.25">
+    <row r="330" spans="1:19" ht="63" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
         <v>350</v>
       </c>
@@ -18415,7 +18438,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="331" spans="1:19" ht="29.25">
+    <row r="331" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
         <v>391</v>
       </c>
@@ -18470,7 +18493,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="332" spans="1:19" ht="29.25">
+    <row r="332" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
         <v>391</v>
       </c>
@@ -18525,7 +18548,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="333" spans="1:19" ht="29.25">
+    <row r="333" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
         <v>391</v>
       </c>
@@ -18580,7 +18603,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="334" spans="1:19" ht="29.25">
+    <row r="334" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
         <v>391</v>
       </c>
@@ -18637,7 +18660,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="335" spans="1:19" ht="29.25">
+    <row r="335" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
         <v>391</v>
       </c>
@@ -18694,7 +18717,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="336" spans="1:19" ht="29.25">
+    <row r="336" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
         <v>391</v>
       </c>
@@ -18751,7 +18774,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="337" spans="1:19" ht="29.25">
+    <row r="337" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
         <v>391</v>
       </c>
@@ -18808,7 +18831,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="338" spans="1:19" ht="29.25">
+    <row r="338" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
         <v>391</v>
       </c>
@@ -18865,7 +18888,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="339" spans="1:19" ht="29.25">
+    <row r="339" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
         <v>391</v>
       </c>
@@ -18922,7 +18945,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="340" spans="1:19" ht="29.25">
+    <row r="340" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
         <v>391</v>
       </c>
@@ -18979,7 +19002,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="341" spans="1:19" ht="29.25">
+    <row r="341" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
         <v>391</v>
       </c>
@@ -19036,7 +19059,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="342" spans="1:19" ht="29.25">
+    <row r="342" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
         <v>391</v>
       </c>
@@ -19093,7 +19116,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="343" spans="1:19" ht="29.25">
+    <row r="343" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
         <v>391</v>
       </c>
@@ -19150,7 +19173,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="344" spans="1:19" ht="29.25">
+    <row r="344" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
         <v>391</v>
       </c>
@@ -19207,7 +19230,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="345" spans="1:19" ht="29.25">
+    <row r="345" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
         <v>391</v>
       </c>
@@ -19264,7 +19287,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="346" spans="1:19" ht="29.25">
+    <row r="346" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
         <v>391</v>
       </c>
@@ -19321,7 +19344,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="347" spans="1:19" ht="29.25">
+    <row r="347" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
         <v>391</v>
       </c>
@@ -19378,7 +19401,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="348" spans="1:19" ht="29.25">
+    <row r="348" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
         <v>391</v>
       </c>
@@ -19435,7 +19458,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="349" spans="1:19" ht="29.25">
+    <row r="349" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
         <v>391</v>
       </c>
@@ -19492,7 +19515,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="350" spans="1:19" ht="29.25">
+    <row r="350" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
         <v>391</v>
       </c>
@@ -19549,7 +19572,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="351" spans="1:19" ht="29.25">
+    <row r="351" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
         <v>391</v>
       </c>
@@ -19606,7 +19629,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="352" spans="1:19" ht="29.25">
+    <row r="352" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
         <v>391</v>
       </c>
@@ -19663,7 +19686,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="353" spans="1:19" ht="29.25">
+    <row r="353" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
         <v>391</v>
       </c>
@@ -19720,7 +19743,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="354" spans="1:19" ht="29.25">
+    <row r="354" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
         <v>391</v>
       </c>
@@ -19777,7 +19800,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="355" spans="1:19" ht="29.25">
+    <row r="355" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
         <v>391</v>
       </c>
@@ -19834,7 +19857,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="356" spans="1:19" ht="29.25">
+    <row r="356" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
         <v>391</v>
       </c>
@@ -19891,7 +19914,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="357" spans="1:19" ht="29.25">
+    <row r="357" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
         <v>391</v>
       </c>
@@ -19948,7 +19971,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="358" spans="1:19" ht="29.25">
+    <row r="358" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
         <v>391</v>
       </c>
@@ -20003,7 +20026,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="359" spans="1:19" ht="29.25">
+    <row r="359" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
         <v>391</v>
       </c>
@@ -20060,7 +20083,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="360" spans="1:19" ht="29.25">
+    <row r="360" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
         <v>391</v>
       </c>
@@ -20117,7 +20140,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="361" spans="1:19" ht="29.25">
+    <row r="361" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
         <v>391</v>
       </c>
@@ -20174,7 +20197,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="362" spans="1:19" ht="29.25">
+    <row r="362" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
         <v>391</v>
       </c>
@@ -20231,7 +20254,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="363" spans="1:19" ht="29.25">
+    <row r="363" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
         <v>391</v>
       </c>
@@ -20288,7 +20311,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="364" spans="1:19" ht="39">
+    <row r="364" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
         <v>391</v>
       </c>
@@ -20345,7 +20368,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="365" spans="1:19" ht="39">
+    <row r="365" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
         <v>391</v>
       </c>
@@ -20402,7 +20425,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="366" spans="1:19" ht="39">
+    <row r="366" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
         <v>391</v>
       </c>
@@ -20459,7 +20482,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="367" spans="1:19" ht="39">
+    <row r="367" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
         <v>391</v>
       </c>
@@ -20516,7 +20539,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="368" spans="1:19" ht="39">
+    <row r="368" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
         <v>391</v>
       </c>
@@ -20573,7 +20596,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="369" spans="1:19" ht="39">
+    <row r="369" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
         <v>391</v>
       </c>
@@ -20630,7 +20653,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="370" spans="1:19" ht="39">
+    <row r="370" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
         <v>391</v>
       </c>
@@ -20687,7 +20710,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="371" spans="1:19" ht="39">
+    <row r="371" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
         <v>391</v>
       </c>
@@ -20744,7 +20767,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="372" spans="1:19" ht="39">
+    <row r="372" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
         <v>424</v>
       </c>
@@ -20801,7 +20824,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="373" spans="1:19" ht="39">
+    <row r="373" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
         <v>424</v>
       </c>
@@ -20858,7 +20881,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="374" spans="1:19" ht="39">
+    <row r="374" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
         <v>424</v>
       </c>
@@ -20915,7 +20938,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="375" spans="1:19" ht="48.75">
+    <row r="375" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
         <v>424</v>
       </c>
@@ -20974,7 +20997,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="376" spans="1:19" ht="39">
+    <row r="376" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
         <v>424</v>
       </c>
@@ -21019,7 +21042,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="377" spans="1:19" ht="39">
+    <row r="377" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
         <v>424</v>
       </c>
@@ -21064,7 +21087,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="378" spans="1:19" ht="39">
+    <row r="378" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
         <v>424</v>
       </c>
@@ -21109,7 +21132,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="379" spans="1:19" ht="39">
+    <row r="379" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
         <v>424</v>
       </c>
@@ -21162,7 +21185,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="380" spans="1:19" ht="39">
+    <row r="380" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
         <v>424</v>
       </c>
@@ -21207,7 +21230,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="381" spans="1:19" ht="39">
+    <row r="381" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
         <v>424</v>
       </c>
@@ -21266,7 +21289,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="382" spans="1:19" ht="48.75">
+    <row r="382" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
         <v>424</v>
       </c>
@@ -21325,7 +21348,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="383" spans="1:19" ht="29.25">
+    <row r="383" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
         <v>444</v>
       </c>
@@ -21382,7 +21405,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="384" spans="1:19" ht="29.25">
+    <row r="384" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
         <v>444</v>
       </c>
@@ -21439,7 +21462,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="385" spans="1:19" ht="39">
+    <row r="385" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
         <v>444</v>
       </c>
@@ -21498,7 +21521,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="386" spans="1:19" ht="39">
+    <row r="386" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
         <v>444</v>
       </c>
@@ -21553,7 +21576,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="387" spans="1:19" ht="48.75">
+    <row r="387" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
         <v>444</v>
       </c>
@@ -21612,7 +21635,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="388" spans="1:19" ht="29.25">
+    <row r="388" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
         <v>444</v>
       </c>
@@ -21663,7 +21686,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="389" spans="1:19" ht="39">
+    <row r="389" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
         <v>454</v>
       </c>
@@ -21722,7 +21745,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="390" spans="1:19" ht="48.75">
+    <row r="390" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
         <v>454</v>
       </c>
@@ -21781,7 +21804,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="391" spans="1:19" ht="48.75">
+    <row r="391" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
         <v>454</v>
       </c>
@@ -21840,7 +21863,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="392" spans="1:19" ht="58.5">
+    <row r="392" spans="1:19" ht="54" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
         <v>454</v>
       </c>
@@ -21899,7 +21922,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="393" spans="1:19" ht="58.5">
+    <row r="393" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
         <v>454</v>
       </c>
@@ -21954,7 +21977,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="394" spans="1:19" ht="19.5">
+    <row r="394" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
         <v>464</v>
       </c>
@@ -22009,7 +22032,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="395" spans="1:19" ht="19.5">
+    <row r="395" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
         <v>464</v>
       </c>
@@ -22064,7 +22087,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="396" spans="1:19" ht="39">
+    <row r="396" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
         <v>464</v>
       </c>
@@ -22121,7 +22144,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="397" spans="1:19" ht="19.5">
+    <row r="397" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
         <v>464</v>
       </c>
@@ -22160,7 +22183,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="398" spans="1:19" ht="19.5">
+    <row r="398" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
         <v>464</v>
       </c>
@@ -22193,7 +22216,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="399" spans="1:19" ht="19.5">
+    <row r="399" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
         <v>464</v>
       </c>
@@ -22226,7 +22249,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="400" spans="1:19" ht="19.5">
+    <row r="400" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
         <v>464</v>
       </c>
@@ -22259,7 +22282,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="401" spans="1:19" ht="19.5">
+    <row r="401" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
         <v>464</v>
       </c>
@@ -22298,7 +22321,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="402" spans="1:19" ht="19.5">
+    <row r="402" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A402" s="2" t="s">
         <v>464</v>
       </c>
@@ -22337,7 +22360,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="403" spans="1:19" ht="19.5">
+    <row r="403" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
         <v>464</v>
       </c>
@@ -22376,7 +22399,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="404" spans="1:19" ht="29.25">
+    <row r="404" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
         <v>464</v>
       </c>
@@ -22435,7 +22458,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="405" spans="1:19" ht="19.5">
+    <row r="405" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
         <v>464</v>
       </c>
@@ -22492,7 +22515,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="406" spans="1:19" ht="29.25">
+    <row r="406" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
         <v>464</v>
       </c>
@@ -22551,7 +22574,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="407" spans="1:19" ht="29.25">
+    <row r="407" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
         <v>464</v>
       </c>
@@ -22602,7 +22625,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="408" spans="1:19" ht="29.25">
+    <row r="408" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
         <v>464</v>
       </c>
@@ -22653,7 +22676,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="409" spans="1:19" ht="19.5">
+    <row r="409" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
         <v>464</v>
       </c>
@@ -22710,7 +22733,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="410" spans="1:19" ht="29.25">
+    <row r="410" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
         <v>485</v>
       </c>
@@ -22765,7 +22788,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="411" spans="1:19" ht="29.25">
+    <row r="411" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A411" s="2" t="s">
         <v>485</v>
       </c>
@@ -22824,7 +22847,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="412" spans="1:19" ht="29.25">
+    <row r="412" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A412" s="2" t="s">
         <v>485</v>
       </c>
@@ -22867,7 +22890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="413" spans="1:19" ht="29.25">
+    <row r="413" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
         <v>485</v>
       </c>
@@ -22920,7 +22943,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="414" spans="1:19" ht="29.25">
+    <row r="414" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
         <v>485</v>
       </c>
@@ -22965,7 +22988,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="415" spans="1:19" ht="29.25">
+    <row r="415" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
         <v>485</v>
       </c>
@@ -23010,7 +23033,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="416" spans="1:19" ht="29.25">
+    <row r="416" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
         <v>485</v>
       </c>
@@ -23055,7 +23078,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="417" spans="1:19" ht="29.25">
+    <row r="417" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A417" s="2" t="s">
         <v>485</v>
       </c>
@@ -23100,7 +23123,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="418" spans="1:19" ht="29.25">
+    <row r="418" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
         <v>485</v>
       </c>
@@ -23145,7 +23168,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="419" spans="1:19" ht="29.25">
+    <row r="419" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
         <v>485</v>
       </c>
@@ -23190,7 +23213,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="420" spans="1:19" ht="39">
+    <row r="420" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
         <v>485</v>
       </c>
@@ -23235,7 +23258,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="421" spans="1:19" ht="48.75">
+    <row r="421" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
         <v>485</v>
       </c>
@@ -23280,7 +23303,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="422" spans="1:19" ht="39">
+    <row r="422" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
         <v>485</v>
       </c>
@@ -23325,7 +23348,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="423" spans="1:19" ht="39">
+    <row r="423" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
         <v>485</v>
       </c>
@@ -23370,7 +23393,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="424" spans="1:19" ht="29.25">
+    <row r="424" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
         <v>485</v>
       </c>
@@ -23427,7 +23450,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="425" spans="1:19" ht="29.25">
+    <row r="425" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
         <v>485</v>
       </c>
@@ -23482,7 +23505,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="426" spans="1:19" ht="29.25">
+    <row r="426" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A426" s="2" t="s">
         <v>485</v>
       </c>
@@ -23537,7 +23560,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="427" spans="1:19" ht="29.25">
+    <row r="427" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
         <v>485</v>
       </c>
@@ -23592,7 +23615,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="428" spans="1:19" ht="29.25">
+    <row r="428" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
         <v>485</v>
       </c>
@@ -23649,7 +23672,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="429" spans="1:19" ht="29.25">
+    <row r="429" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A429" s="2" t="s">
         <v>485</v>
       </c>
@@ -23706,7 +23729,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="430" spans="1:19" ht="39">
+    <row r="430" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A430" s="2" t="s">
         <v>485</v>
       </c>
@@ -23745,7 +23768,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="431" spans="1:19" ht="39">
+    <row r="431" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
         <v>485</v>
       </c>
@@ -23784,7 +23807,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="432" spans="1:19" ht="39">
+    <row r="432" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A432" s="2" t="s">
         <v>485</v>
       </c>
@@ -23823,7 +23846,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="433" spans="1:19" ht="39">
+    <row r="433" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A433" s="2" t="s">
         <v>485</v>
       </c>
@@ -23862,7 +23885,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="434" spans="1:19" ht="39">
+    <row r="434" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A434" s="2" t="s">
         <v>485</v>
       </c>
@@ -23901,7 +23924,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="435" spans="1:19" ht="39">
+    <row r="435" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A435" s="2" t="s">
         <v>485</v>
       </c>
@@ -23940,7 +23963,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="436" spans="1:19" ht="39">
+    <row r="436" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A436" s="2" t="s">
         <v>485</v>
       </c>
@@ -23979,7 +24002,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="437" spans="1:19" ht="39">
+    <row r="437" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A437" s="2" t="s">
         <v>485</v>
       </c>
@@ -24018,7 +24041,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="438" spans="1:19" ht="39">
+    <row r="438" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A438" s="2" t="s">
         <v>485</v>
       </c>
@@ -24057,7 +24080,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="439" spans="1:19" ht="39">
+    <row r="439" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A439" s="2" t="s">
         <v>485</v>
       </c>
@@ -24096,7 +24119,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="440" spans="1:19" ht="39">
+    <row r="440" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
         <v>485</v>
       </c>
@@ -24135,7 +24158,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="441" spans="1:19" ht="39">
+    <row r="441" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
         <v>485</v>
       </c>
@@ -24174,7 +24197,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="442" spans="1:19" ht="29.25">
+    <row r="442" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
         <v>485</v>
       </c>
@@ -24233,7 +24256,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="443" spans="1:19" ht="29.25">
+    <row r="443" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A443" s="2" t="s">
         <v>485</v>
       </c>
@@ -24272,7 +24295,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="444" spans="1:19" ht="29.25">
+    <row r="444" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A444" s="2" t="s">
         <v>522</v>
       </c>
@@ -24329,7 +24352,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="445" spans="1:19" ht="29.25">
+    <row r="445" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A445" s="2" t="s">
         <v>522</v>
       </c>
@@ -24386,7 +24409,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="446" spans="1:19" ht="29.25">
+    <row r="446" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A446" s="2" t="s">
         <v>522</v>
       </c>
@@ -24443,7 +24466,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="447" spans="1:19" ht="29.25">
+    <row r="447" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
         <v>522</v>
       </c>
@@ -24500,7 +24523,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="448" spans="1:19" ht="48.75">
+    <row r="448" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
         <v>522</v>
       </c>
@@ -24557,7 +24580,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="449" spans="1:19" ht="29.25">
+    <row r="449" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A449" s="2" t="s">
         <v>522</v>
       </c>
@@ -24614,7 +24637,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="450" spans="1:19" ht="29.25">
+    <row r="450" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A450" s="2" t="s">
         <v>522</v>
       </c>
@@ -24671,7 +24694,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="451" spans="1:19" ht="29.25">
+    <row r="451" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A451" s="2" t="s">
         <v>522</v>
       </c>
@@ -24730,7 +24753,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="452" spans="1:19" ht="29.25">
+    <row r="452" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A452" s="2" t="s">
         <v>522</v>
       </c>
@@ -24789,7 +24812,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="453" spans="1:19" ht="29.25">
+    <row r="453" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A453" s="2" t="s">
         <v>522</v>
       </c>
@@ -24848,7 +24871,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="454" spans="1:19" ht="29.25">
+    <row r="454" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A454" s="2" t="s">
         <v>522</v>
       </c>
@@ -24905,7 +24928,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="455" spans="1:19" ht="29.25">
+    <row r="455" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A455" s="2" t="s">
         <v>522</v>
       </c>
@@ -24962,7 +24985,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="456" spans="1:19" ht="29.25">
+    <row r="456" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A456" s="2" t="s">
         <v>522</v>
       </c>
@@ -25019,7 +25042,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="457" spans="1:19" ht="29.25">
+    <row r="457" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
         <v>522</v>
       </c>
@@ -25076,7 +25099,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="458" spans="1:19" ht="29.25">
+    <row r="458" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A458" s="2" t="s">
         <v>522</v>
       </c>
@@ -25135,7 +25158,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="459" spans="1:19" ht="48.75">
+    <row r="459" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
         <v>522</v>
       </c>
@@ -25194,7 +25217,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="460" spans="1:19" ht="29.25">
+    <row r="460" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
         <v>522</v>
       </c>
@@ -25253,7 +25276,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="461" spans="1:19" ht="39">
+    <row r="461" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
         <v>522</v>
       </c>
@@ -25310,7 +25333,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="462" spans="1:19" ht="39">
+    <row r="462" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
         <v>522</v>
       </c>
@@ -25367,7 +25390,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="463" spans="1:19" ht="29.25">
+    <row r="463" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
         <v>522</v>
       </c>
@@ -25410,7 +25433,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="464" spans="1:19" ht="29.25">
+    <row r="464" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
         <v>522</v>
       </c>
@@ -25469,7 +25492,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="465" spans="1:19" ht="29.25">
+    <row r="465" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
         <v>522</v>
       </c>
@@ -25528,7 +25551,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="466" spans="1:19" ht="29.25">
+    <row r="466" spans="1:19" ht="18" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
         <v>522</v>
       </c>
@@ -25579,7 +25602,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="467" spans="1:19" ht="39">
+    <row r="467" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
         <v>522</v>
       </c>
@@ -25616,7 +25639,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="468" spans="1:19" ht="39">
+    <row r="468" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
         <v>522</v>
       </c>
@@ -25673,7 +25696,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="469" spans="1:19" ht="39">
+    <row r="469" spans="1:19" ht="36" x14ac:dyDescent="0.25">
       <c r="A469" s="2" t="s">
         <v>522</v>
       </c>
@@ -25730,9 +25753,9 @@
         <v>557</v>
       </c>
     </row>
-    <row r="470" spans="1:19" ht="0" hidden="1" customHeight="1"/>
-    <row r="471" spans="1:19" ht="18" customHeight="1"/>
-    <row r="472" spans="1:19" ht="17.100000000000001" customHeight="1">
+    <row r="470" spans="1:19" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A472" s="12" t="s">
         <v>560</v>
       </c>

</xml_diff>

<commit_message>
Okno serwisowe - 07.03.2023
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -1705,7 +1705,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 28-02-2023, 09:55</t>
+    <t>Last update: 07-03-2023, 11:33</t>
   </si>
 </sst>
 </file>
@@ -1716,8 +1716,8 @@
     <numFmt numFmtId="164" formatCode="[$-10809]0.0;\-0.0;0.0"/>
     <numFmt numFmtId="165" formatCode="[$-10809]0.00;\-0.00;0.00"/>
     <numFmt numFmtId="166" formatCode="[$-10809]0;\-0;0"/>
-    <numFmt numFmtId="167" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
-    <numFmt numFmtId="168" formatCode="[$-10809]0.000;\-0.000;0.000"/>
+    <numFmt numFmtId="167" formatCode="[$-10809]0.000;\-0.000;0.000"/>
+    <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
@@ -2255,7 +2255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S472"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
@@ -2390,7 +2390,9 @@
       <c r="P4" s="4">
         <v>0.2</v>
       </c>
-      <c r="Q4" s="3"/>
+      <c r="Q4" s="4">
+        <v>0.2</v>
+      </c>
       <c r="R4" s="3"/>
       <c r="S4" s="2" t="s">
         <v>25</v>
@@ -3470,8 +3472,12 @@
       <c r="P24" s="6">
         <v>1</v>
       </c>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
+      <c r="Q24" s="6">
+        <v>1</v>
+      </c>
+      <c r="R24" s="6">
+        <v>1</v>
+      </c>
       <c r="S24" s="2" t="s">
         <v>53</v>
       </c>
@@ -3497,26 +3503,30 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="5">
+      <c r="K25" s="7">
         <v>0.8</v>
       </c>
-      <c r="L25" s="5">
+      <c r="L25" s="7">
         <v>0.8</v>
       </c>
-      <c r="M25" s="5">
+      <c r="M25" s="7">
         <v>0.8</v>
       </c>
-      <c r="N25" s="5">
+      <c r="N25" s="7">
         <v>0.85</v>
       </c>
-      <c r="O25" s="5">
+      <c r="O25" s="7">
         <v>0.85</v>
       </c>
-      <c r="P25" s="5">
+      <c r="P25" s="7">
         <v>0.85</v>
       </c>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
+      <c r="Q25" s="7">
+        <v>0.875</v>
+      </c>
+      <c r="R25" s="7">
+        <v>0.875</v>
+      </c>
       <c r="S25" s="2" t="s">
         <v>53</v>
       </c>
@@ -3560,8 +3570,12 @@
       <c r="P26" s="6">
         <v>16</v>
       </c>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
+      <c r="Q26" s="6">
+        <v>16</v>
+      </c>
+      <c r="R26" s="6">
+        <v>16</v>
+      </c>
       <c r="S26" s="2" t="s">
         <v>53</v>
       </c>
@@ -3605,8 +3619,12 @@
       <c r="P27" s="6">
         <v>100</v>
       </c>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
+      <c r="Q27" s="6">
+        <v>100</v>
+      </c>
+      <c r="R27" s="6">
+        <v>100</v>
+      </c>
       <c r="S27" s="2" t="s">
         <v>53</v>
       </c>
@@ -3630,31 +3648,31 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="7">
+      <c r="I28" s="8">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="J28" s="7">
+      <c r="J28" s="8">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="K28" s="7">
+      <c r="K28" s="8">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="L28" s="7">
+      <c r="L28" s="8">
         <v>7.9999999999999996E-6</v>
       </c>
-      <c r="M28" s="7">
+      <c r="M28" s="8">
         <v>2.0999999999999999E-5</v>
       </c>
-      <c r="N28" s="7">
+      <c r="N28" s="8">
         <v>6.0000000000000002E-6</v>
       </c>
-      <c r="O28" s="7">
+      <c r="O28" s="8">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="P28" s="7">
+      <c r="P28" s="8">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="Q28" s="7">
+      <c r="Q28" s="8">
         <v>9.0000000000000006E-5</v>
       </c>
       <c r="R28" s="3"/>
@@ -12221,7 +12239,9 @@
       <c r="P211" s="5">
         <v>16.100000000000001</v>
       </c>
-      <c r="Q211" s="3"/>
+      <c r="Q211" s="5">
+        <v>15.62</v>
+      </c>
       <c r="R211" s="3"/>
       <c r="S211" s="2" t="s">
         <v>25</v>
@@ -12243,37 +12263,37 @@
       <c r="E212" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="F212" s="8">
+      <c r="F212" s="7">
         <v>0.36799999999999999</v>
       </c>
-      <c r="G212" s="8">
+      <c r="G212" s="7">
         <v>0.35399999999999998</v>
       </c>
-      <c r="H212" s="8">
+      <c r="H212" s="7">
         <v>0.33800000000000002</v>
       </c>
-      <c r="I212" s="8">
+      <c r="I212" s="7">
         <v>0.33300000000000002</v>
       </c>
-      <c r="J212" s="8">
+      <c r="J212" s="7">
         <v>0.31</v>
       </c>
-      <c r="K212" s="8">
+      <c r="K212" s="7">
         <v>0.30099999999999999</v>
       </c>
-      <c r="L212" s="8">
+      <c r="L212" s="7">
         <v>0.30499999999999999</v>
       </c>
-      <c r="M212" s="8">
+      <c r="M212" s="7">
         <v>0.30499999999999999</v>
       </c>
-      <c r="N212" s="8">
+      <c r="N212" s="7">
         <v>0.30299999999999999</v>
       </c>
-      <c r="O212" s="8">
+      <c r="O212" s="7">
         <v>0.28199999999999997</v>
       </c>
-      <c r="P212" s="8">
+      <c r="P212" s="7">
         <v>0.27600000000000002</v>
       </c>
       <c r="Q212" s="3"/>
@@ -22103,40 +22123,40 @@
       <c r="E396" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F396" s="8">
+      <c r="F396" s="7">
         <v>0.19600000000000001</v>
       </c>
-      <c r="G396" s="8">
+      <c r="G396" s="7">
         <v>0.20499999999999999</v>
       </c>
-      <c r="H396" s="8">
+      <c r="H396" s="7">
         <v>0.20599999999999999</v>
       </c>
-      <c r="I396" s="8">
+      <c r="I396" s="7">
         <v>0.19800000000000001</v>
       </c>
-      <c r="J396" s="8">
+      <c r="J396" s="7">
         <v>0.20100000000000001</v>
       </c>
-      <c r="K396" s="8">
+      <c r="K396" s="7">
         <v>0.20300000000000001</v>
       </c>
-      <c r="L396" s="8">
+      <c r="L396" s="7">
         <v>0.20699999999999999</v>
       </c>
-      <c r="M396" s="8">
+      <c r="M396" s="7">
         <v>0.19800000000000001</v>
       </c>
-      <c r="N396" s="8">
+      <c r="N396" s="7">
         <v>0.19800000000000001</v>
       </c>
-      <c r="O396" s="8">
+      <c r="O396" s="7">
         <v>0.19900000000000001</v>
       </c>
-      <c r="P396" s="8">
+      <c r="P396" s="7">
         <v>0.2</v>
       </c>
-      <c r="Q396" s="8">
+      <c r="Q396" s="7">
         <v>0.19900000000000001</v>
       </c>
       <c r="R396" s="3"/>

</xml_diff>

<commit_message>
Okno serwisowe 21.03.2023 - aktualizacja excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="18060" windowHeight="7050"/>
   </bookViews>
@@ -1705,13 +1700,13 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 07-03-2023, 11:33</t>
+    <t>Last update: 22-03-2023, 08:35</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$-10809]0.0;\-0.0;0.0"/>
     <numFmt numFmtId="165" formatCode="[$-10809]0.00;\-0.00;0.00"/>
@@ -1720,7 +1715,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1918,14 +1913,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1946,7 +1933,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="0" name="Picture 1"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2009,7 +1996,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2041,10 +2028,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2076,7 +2062,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -2252,15 +2237,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S472"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2272,17 +2257,17 @@
     <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="36" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2341,7 +2326,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="19.5">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2398,7 +2383,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="15">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2453,7 +2438,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -2508,7 +2493,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="15">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -2563,7 +2548,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="15">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -2618,7 +2603,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="15">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -2673,7 +2658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -2728,7 +2713,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2783,7 +2768,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -2838,7 +2823,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2893,7 +2878,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="19.5">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -2948,7 +2933,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="19.5">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -3003,7 +2988,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="15">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -3042,7 +3027,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="29.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -3099,7 +3084,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="97.5">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -3154,7 +3139,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="97.5">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -3209,7 +3194,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="97.5">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -3264,7 +3249,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="19.5">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -3319,7 +3304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="29.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -3376,7 +3361,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="29.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -3433,7 +3418,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="29.25">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -3482,7 +3467,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="68.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -3531,7 +3516,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="29.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
@@ -3580,7 +3565,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="29.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -3629,7 +3614,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="29.25">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
@@ -3680,7 +3665,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="39">
       <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
@@ -3737,7 +3722,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="39">
       <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
@@ -3794,7 +3779,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="39">
       <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
@@ -3851,7 +3836,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="39">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -3908,7 +3893,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="19.5">
       <c r="A33" s="2" t="s">
         <v>66</v>
       </c>
@@ -3963,7 +3948,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="29.25">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -4008,7 +3993,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="29.25">
       <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
@@ -4053,7 +4038,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="29.25">
       <c r="A36" s="2" t="s">
         <v>66</v>
       </c>
@@ -4098,7 +4083,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="29.25">
       <c r="A37" s="2" t="s">
         <v>66</v>
       </c>
@@ -4143,7 +4128,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="29.25">
       <c r="A38" s="2" t="s">
         <v>66</v>
       </c>
@@ -4188,7 +4173,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="29.25">
       <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
@@ -4233,7 +4218,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="39">
       <c r="A40" s="2" t="s">
         <v>66</v>
       </c>
@@ -4272,7 +4257,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="97.5">
       <c r="A41" s="2" t="s">
         <v>66</v>
       </c>
@@ -4331,7 +4316,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="97.5">
       <c r="A42" s="2" t="s">
         <v>66</v>
       </c>
@@ -4390,7 +4375,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="97.5">
       <c r="A43" s="2" t="s">
         <v>66</v>
       </c>
@@ -4449,7 +4434,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="97.5">
       <c r="A44" s="2" t="s">
         <v>66</v>
       </c>
@@ -4508,7 +4493,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="97.5">
       <c r="A45" s="2" t="s">
         <v>66</v>
       </c>
@@ -4567,7 +4552,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="97.5">
       <c r="A46" s="2" t="s">
         <v>66</v>
       </c>
@@ -4626,7 +4611,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="48.75">
       <c r="A47" s="2" t="s">
         <v>66</v>
       </c>
@@ -4675,7 +4660,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="48.75">
       <c r="A48" s="2" t="s">
         <v>66</v>
       </c>
@@ -4724,7 +4709,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="19.5">
       <c r="A49" s="2" t="s">
         <v>66</v>
       </c>
@@ -4779,7 +4764,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="29.25">
       <c r="A50" s="2" t="s">
         <v>66</v>
       </c>
@@ -4830,7 +4815,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="19.5">
       <c r="A51" s="2" t="s">
         <v>95</v>
       </c>
@@ -4885,7 +4870,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="19.5">
       <c r="A52" s="2" t="s">
         <v>95</v>
       </c>
@@ -4942,7 +4927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>95</v>
       </c>
@@ -4999,7 +4984,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>95</v>
       </c>
@@ -5056,7 +5041,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>95</v>
       </c>
@@ -5113,7 +5098,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>95</v>
       </c>
@@ -5170,7 +5155,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>95</v>
       </c>
@@ -5227,7 +5212,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>95</v>
       </c>
@@ -5284,7 +5269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="29.25">
       <c r="A59" s="2" t="s">
         <v>95</v>
       </c>
@@ -5341,7 +5326,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>95</v>
       </c>
@@ -5398,7 +5383,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="29.25">
       <c r="A61" s="2" t="s">
         <v>95</v>
       </c>
@@ -5455,7 +5440,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="29.25">
       <c r="A62" s="2" t="s">
         <v>95</v>
       </c>
@@ -5512,7 +5497,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="29.25">
       <c r="A63" s="2" t="s">
         <v>95</v>
       </c>
@@ -5569,7 +5554,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="19.5">
       <c r="A64" s="2" t="s">
         <v>95</v>
       </c>
@@ -5626,7 +5611,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="29.25">
       <c r="A65" s="2" t="s">
         <v>95</v>
       </c>
@@ -5683,7 +5668,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="29.25">
       <c r="A66" s="2" t="s">
         <v>95</v>
       </c>
@@ -5740,7 +5725,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="29.25">
       <c r="A67" s="2" t="s">
         <v>95</v>
       </c>
@@ -5797,7 +5782,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="29.25">
       <c r="A68" s="2" t="s">
         <v>95</v>
       </c>
@@ -5854,7 +5839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="29.25">
       <c r="A69" s="2" t="s">
         <v>95</v>
       </c>
@@ -5911,7 +5896,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" ht="29.25">
       <c r="A70" s="2" t="s">
         <v>95</v>
       </c>
@@ -5968,7 +5953,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" ht="29.25">
       <c r="A71" s="2" t="s">
         <v>95</v>
       </c>
@@ -6025,7 +6010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" ht="19.5">
       <c r="A72" s="2" t="s">
         <v>95</v>
       </c>
@@ -6080,7 +6065,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="19.5">
       <c r="A73" s="2" t="s">
         <v>95</v>
       </c>
@@ -6135,7 +6120,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="19.5">
       <c r="A74" s="2" t="s">
         <v>95</v>
       </c>
@@ -6190,7 +6175,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="19.5">
       <c r="A75" s="2" t="s">
         <v>95</v>
       </c>
@@ -6247,7 +6232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" ht="29.25">
       <c r="A76" s="2" t="s">
         <v>95</v>
       </c>
@@ -6304,7 +6289,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" ht="29.25">
       <c r="A77" s="2" t="s">
         <v>95</v>
       </c>
@@ -6343,7 +6328,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" ht="19.5">
       <c r="A78" s="2" t="s">
         <v>95</v>
       </c>
@@ -6400,7 +6385,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="19.5">
       <c r="A79" s="2" t="s">
         <v>95</v>
       </c>
@@ -6457,7 +6442,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" ht="19.5">
       <c r="A80" s="2" t="s">
         <v>95</v>
       </c>
@@ -6514,7 +6499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="19.5">
       <c r="A81" s="2" t="s">
         <v>95</v>
       </c>
@@ -6555,7 +6540,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="29.25">
       <c r="A82" s="2" t="s">
         <v>95</v>
       </c>
@@ -6600,7 +6585,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="29.25">
       <c r="A83" s="2" t="s">
         <v>95</v>
       </c>
@@ -6645,7 +6630,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="19.5">
       <c r="A84" s="2" t="s">
         <v>95</v>
       </c>
@@ -6680,7 +6665,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="29.25">
       <c r="A85" s="2" t="s">
         <v>95</v>
       </c>
@@ -6715,7 +6700,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="19.5">
       <c r="A86" s="2" t="s">
         <v>95</v>
       </c>
@@ -6770,7 +6755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="19.5">
       <c r="A87" s="2" t="s">
         <v>95</v>
       </c>
@@ -6809,7 +6794,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" ht="19.5">
       <c r="A88" s="2" t="s">
         <v>95</v>
       </c>
@@ -6866,7 +6851,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="19.5">
       <c r="A89" s="2" t="s">
         <v>95</v>
       </c>
@@ -6923,7 +6908,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="19.5">
       <c r="A90" s="2" t="s">
         <v>95</v>
       </c>
@@ -6964,7 +6949,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="29.25">
       <c r="A91" s="2" t="s">
         <v>95</v>
       </c>
@@ -7015,7 +7000,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" ht="19.5">
       <c r="A92" s="2" t="s">
         <v>95</v>
       </c>
@@ -7054,7 +7039,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" ht="19.5">
       <c r="A93" s="2" t="s">
         <v>95</v>
       </c>
@@ -7093,7 +7078,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" ht="19.5">
       <c r="A94" s="2" t="s">
         <v>95</v>
       </c>
@@ -7132,7 +7117,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" ht="19.5">
       <c r="A95" s="2" t="s">
         <v>95</v>
       </c>
@@ -7185,7 +7170,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" ht="48.75">
       <c r="A96" s="2" t="s">
         <v>149</v>
       </c>
@@ -7222,7 +7207,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" ht="48.75">
       <c r="A97" s="2" t="s">
         <v>149</v>
       </c>
@@ -7259,7 +7244,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" ht="48.75">
       <c r="A98" s="2" t="s">
         <v>149</v>
       </c>
@@ -7296,7 +7281,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" ht="48.75">
       <c r="A99" s="2" t="s">
         <v>149</v>
       </c>
@@ -7337,7 +7322,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" ht="48.75">
       <c r="A100" s="2" t="s">
         <v>149</v>
       </c>
@@ -7378,7 +7363,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" ht="48.75">
       <c r="A101" s="2" t="s">
         <v>149</v>
       </c>
@@ -7419,7 +7404,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" ht="48.75">
       <c r="A102" s="2" t="s">
         <v>149</v>
       </c>
@@ -7460,7 +7445,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" ht="48.75">
       <c r="A103" s="2" t="s">
         <v>149</v>
       </c>
@@ -7501,7 +7486,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" ht="48.75">
       <c r="A104" s="2" t="s">
         <v>149</v>
       </c>
@@ -7542,7 +7527,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" ht="29.25">
       <c r="A105" s="2" t="s">
         <v>149</v>
       </c>
@@ -7579,7 +7564,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" ht="19.5">
       <c r="A106" s="2" t="s">
         <v>149</v>
       </c>
@@ -7636,7 +7621,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" ht="19.5">
       <c r="A107" s="2" t="s">
         <v>149</v>
       </c>
@@ -7693,7 +7678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" ht="19.5">
       <c r="A108" s="2" t="s">
         <v>149</v>
       </c>
@@ -7750,7 +7735,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" ht="19.5">
       <c r="A109" s="2" t="s">
         <v>149</v>
       </c>
@@ -7787,7 +7772,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" ht="19.5">
       <c r="A110" s="2" t="s">
         <v>149</v>
       </c>
@@ -7824,7 +7809,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" ht="19.5">
       <c r="A111" s="2" t="s">
         <v>149</v>
       </c>
@@ -7861,7 +7846,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" ht="29.25">
       <c r="A112" s="2" t="s">
         <v>149</v>
       </c>
@@ -7906,7 +7891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" ht="19.5">
       <c r="A113" s="2" t="s">
         <v>149</v>
       </c>
@@ -7953,7 +7938,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" ht="39">
       <c r="A114" s="2" t="s">
         <v>149</v>
       </c>
@@ -8000,7 +7985,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" ht="48.75">
       <c r="A115" s="2" t="s">
         <v>149</v>
       </c>
@@ -8047,7 +8032,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" ht="58.5">
       <c r="A116" s="2" t="s">
         <v>149</v>
       </c>
@@ -8094,7 +8079,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" ht="29.25">
       <c r="A117" s="2" t="s">
         <v>149</v>
       </c>
@@ -8141,7 +8126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" ht="29.25">
       <c r="A118" s="2" t="s">
         <v>149</v>
       </c>
@@ -8186,7 +8171,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" ht="19.5">
       <c r="A119" s="2" t="s">
         <v>149</v>
       </c>
@@ -8233,7 +8218,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" ht="39">
       <c r="A120" s="2" t="s">
         <v>149</v>
       </c>
@@ -8280,7 +8265,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" ht="48.75">
       <c r="A121" s="2" t="s">
         <v>149</v>
       </c>
@@ -8327,7 +8312,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" ht="58.5">
       <c r="A122" s="2" t="s">
         <v>149</v>
       </c>
@@ -8374,7 +8359,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" ht="29.25">
       <c r="A123" s="2" t="s">
         <v>149</v>
       </c>
@@ -8421,7 +8406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" ht="48.75">
       <c r="A124" s="2" t="s">
         <v>149</v>
       </c>
@@ -8460,7 +8445,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" ht="48.75">
       <c r="A125" s="2" t="s">
         <v>149</v>
       </c>
@@ -8499,7 +8484,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" ht="29.25">
       <c r="A126" s="2" t="s">
         <v>149</v>
       </c>
@@ -8556,7 +8541,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" ht="29.25">
       <c r="A127" s="2" t="s">
         <v>149</v>
       </c>
@@ -8591,7 +8576,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" ht="29.25">
       <c r="A128" s="2" t="s">
         <v>149</v>
       </c>
@@ -8626,7 +8611,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" ht="29.25">
       <c r="A129" s="2" t="s">
         <v>149</v>
       </c>
@@ -8661,7 +8646,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" ht="29.25">
       <c r="A130" s="2" t="s">
         <v>149</v>
       </c>
@@ -8696,7 +8681,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" ht="29.25">
       <c r="A131" s="2" t="s">
         <v>149</v>
       </c>
@@ -8731,7 +8716,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" ht="29.25">
       <c r="A132" s="2" t="s">
         <v>149</v>
       </c>
@@ -8766,7 +8751,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" ht="29.25">
       <c r="A133" s="2" t="s">
         <v>149</v>
       </c>
@@ -8801,7 +8786,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" ht="29.25">
       <c r="A134" s="2" t="s">
         <v>149</v>
       </c>
@@ -8836,7 +8821,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" ht="29.25">
       <c r="A135" s="2" t="s">
         <v>149</v>
       </c>
@@ -8871,7 +8856,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" ht="29.25">
       <c r="A136" s="2" t="s">
         <v>149</v>
       </c>
@@ -8906,7 +8891,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" ht="29.25">
       <c r="A137" s="2" t="s">
         <v>149</v>
       </c>
@@ -8941,7 +8926,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" ht="29.25">
       <c r="A138" s="2" t="s">
         <v>149</v>
       </c>
@@ -8976,7 +8961,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" ht="29.25">
       <c r="A139" s="2" t="s">
         <v>149</v>
       </c>
@@ -9011,7 +8996,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" ht="29.25">
       <c r="A140" s="2" t="s">
         <v>149</v>
       </c>
@@ -9046,7 +9031,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" ht="29.25">
       <c r="A141" s="2" t="s">
         <v>149</v>
       </c>
@@ -9081,7 +9066,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" ht="29.25">
       <c r="A142" s="2" t="s">
         <v>149</v>
       </c>
@@ -9116,7 +9101,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" ht="48.75">
       <c r="A143" s="2" t="s">
         <v>149</v>
       </c>
@@ -9175,7 +9160,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" ht="58.5">
       <c r="A144" s="2" t="s">
         <v>149</v>
       </c>
@@ -9234,7 +9219,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" ht="58.5">
       <c r="A145" s="2" t="s">
         <v>149</v>
       </c>
@@ -9269,7 +9254,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" ht="58.5">
       <c r="A146" s="2" t="s">
         <v>149</v>
       </c>
@@ -9304,7 +9289,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" ht="58.5">
       <c r="A147" s="2" t="s">
         <v>149</v>
       </c>
@@ -9363,7 +9348,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" ht="58.5">
       <c r="A148" s="2" t="s">
         <v>149</v>
       </c>
@@ -9422,7 +9407,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" ht="58.5">
       <c r="A149" s="2" t="s">
         <v>149</v>
       </c>
@@ -9481,7 +9466,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" ht="29.25">
       <c r="A150" s="2" t="s">
         <v>149</v>
       </c>
@@ -9532,7 +9517,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" ht="58.5">
       <c r="A151" s="2" t="s">
         <v>149</v>
       </c>
@@ -9587,7 +9572,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" ht="58.5">
       <c r="A152" s="2" t="s">
         <v>149</v>
       </c>
@@ -9642,7 +9627,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" ht="58.5">
       <c r="A153" s="2" t="s">
         <v>149</v>
       </c>
@@ -9697,7 +9682,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" ht="58.5">
       <c r="A154" s="2" t="s">
         <v>149</v>
       </c>
@@ -9752,7 +9737,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" ht="29.25">
       <c r="A155" s="2" t="s">
         <v>205</v>
       </c>
@@ -9787,7 +9772,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" ht="19.5">
       <c r="A156" s="2" t="s">
         <v>205</v>
       </c>
@@ -9844,7 +9829,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" ht="39">
       <c r="A157" s="2" t="s">
         <v>205</v>
       </c>
@@ -9879,7 +9864,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" ht="39">
       <c r="A158" s="2" t="s">
         <v>205</v>
       </c>
@@ -9914,7 +9899,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" ht="39">
       <c r="A159" s="2" t="s">
         <v>205</v>
       </c>
@@ -9949,7 +9934,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="160" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" ht="39">
       <c r="A160" s="2" t="s">
         <v>205</v>
       </c>
@@ -9984,7 +9969,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" ht="39">
       <c r="A161" s="2" t="s">
         <v>205</v>
       </c>
@@ -10019,7 +10004,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" ht="19.5">
       <c r="A162" s="2" t="s">
         <v>205</v>
       </c>
@@ -10054,7 +10039,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:19" ht="19.5">
       <c r="A163" s="2" t="s">
         <v>205</v>
       </c>
@@ -10089,7 +10074,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" ht="19.5">
       <c r="A164" s="2" t="s">
         <v>205</v>
       </c>
@@ -10124,7 +10109,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:19" ht="19.5">
       <c r="A165" s="2" t="s">
         <v>205</v>
       </c>
@@ -10159,7 +10144,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" ht="19.5">
       <c r="A166" s="2" t="s">
         <v>205</v>
       </c>
@@ -10194,7 +10179,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" ht="19.5">
       <c r="A167" s="2" t="s">
         <v>205</v>
       </c>
@@ -10229,7 +10214,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:19" ht="19.5">
       <c r="A168" s="2" t="s">
         <v>205</v>
       </c>
@@ -10264,7 +10249,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" ht="19.5">
       <c r="A169" s="2" t="s">
         <v>205</v>
       </c>
@@ -10299,7 +10284,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:19" ht="29.25">
       <c r="A170" s="2" t="s">
         <v>205</v>
       </c>
@@ -10338,7 +10323,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:19" ht="29.25">
       <c r="A171" s="2" t="s">
         <v>205</v>
       </c>
@@ -10377,7 +10362,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:19" ht="29.25">
       <c r="A172" s="2" t="s">
         <v>205</v>
       </c>
@@ -10434,7 +10419,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:19" ht="29.25">
       <c r="A173" s="2" t="s">
         <v>205</v>
       </c>
@@ -10491,7 +10476,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:19" ht="29.25">
       <c r="A174" s="2" t="s">
         <v>205</v>
       </c>
@@ -10548,7 +10533,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:19" ht="29.25">
       <c r="A175" s="2" t="s">
         <v>205</v>
       </c>
@@ -10605,7 +10590,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:19" ht="29.25">
       <c r="A176" s="2" t="s">
         <v>205</v>
       </c>
@@ -10662,7 +10647,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="177" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:19" ht="19.5">
       <c r="A177" s="2" t="s">
         <v>205</v>
       </c>
@@ -10707,7 +10692,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="178" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:19" ht="39">
       <c r="A178" s="2" t="s">
         <v>205</v>
       </c>
@@ -10752,7 +10737,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:19" ht="19.5">
       <c r="A179" s="2" t="s">
         <v>205</v>
       </c>
@@ -10797,7 +10782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:19" ht="39">
       <c r="A180" s="2" t="s">
         <v>205</v>
       </c>
@@ -10842,7 +10827,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:19" ht="39">
       <c r="A181" s="2" t="s">
         <v>205</v>
       </c>
@@ -10887,7 +10872,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="182" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:19" ht="39">
       <c r="A182" s="2" t="s">
         <v>205</v>
       </c>
@@ -10932,7 +10917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:19" ht="39">
       <c r="A183" s="2" t="s">
         <v>205</v>
       </c>
@@ -10977,7 +10962,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:19" ht="39">
       <c r="A184" s="2" t="s">
         <v>205</v>
       </c>
@@ -11016,7 +11001,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:19" ht="39">
       <c r="A185" s="2" t="s">
         <v>205</v>
       </c>
@@ -11055,7 +11040,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="186" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:19" ht="39">
       <c r="A186" s="2" t="s">
         <v>205</v>
       </c>
@@ -11094,7 +11079,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:19" ht="39">
       <c r="A187" s="2" t="s">
         <v>205</v>
       </c>
@@ -11133,7 +11118,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:19" ht="39">
       <c r="A188" s="2" t="s">
         <v>205</v>
       </c>
@@ -11172,7 +11157,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:19" ht="39">
       <c r="A189" s="2" t="s">
         <v>205</v>
       </c>
@@ -11211,7 +11196,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:19" ht="39">
       <c r="A190" s="2" t="s">
         <v>205</v>
       </c>
@@ -11250,7 +11235,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:19" ht="39">
       <c r="A191" s="2" t="s">
         <v>205</v>
       </c>
@@ -11289,7 +11274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:19" ht="39">
       <c r="A192" s="2" t="s">
         <v>205</v>
       </c>
@@ -11328,7 +11313,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="193" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:19" ht="39">
       <c r="A193" s="2" t="s">
         <v>205</v>
       </c>
@@ -11367,7 +11352,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:19" ht="39">
       <c r="A194" s="2" t="s">
         <v>205</v>
       </c>
@@ -11406,7 +11391,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="195" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:19" ht="39">
       <c r="A195" s="2" t="s">
         <v>205</v>
       </c>
@@ -11445,7 +11430,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="196" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:19" ht="19.5">
       <c r="A196" s="2" t="s">
         <v>205</v>
       </c>
@@ -11486,7 +11471,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:19" ht="19.5">
       <c r="A197" s="2" t="s">
         <v>205</v>
       </c>
@@ -11541,7 +11526,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:19" ht="19.5">
       <c r="A198" s="2" t="s">
         <v>205</v>
       </c>
@@ -11596,7 +11581,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:19" ht="19.5">
       <c r="A199" s="2" t="s">
         <v>245</v>
       </c>
@@ -11653,7 +11638,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="200" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:19" ht="29.25">
       <c r="A200" s="2" t="s">
         <v>245</v>
       </c>
@@ -11710,7 +11695,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="201" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:19" ht="19.5">
       <c r="A201" s="2" t="s">
         <v>245</v>
       </c>
@@ -11767,7 +11752,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="202" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:19" ht="19.5">
       <c r="A202" s="2" t="s">
         <v>245</v>
       </c>
@@ -11802,7 +11787,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="203" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:19" ht="19.5">
       <c r="A203" s="2" t="s">
         <v>245</v>
       </c>
@@ -11837,7 +11822,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="204" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:19" ht="29.25">
       <c r="A204" s="2" t="s">
         <v>245</v>
       </c>
@@ -11892,7 +11877,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="205" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:19" ht="19.5">
       <c r="A205" s="2" t="s">
         <v>245</v>
       </c>
@@ -11947,7 +11932,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="206" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:19" ht="19.5">
       <c r="A206" s="2" t="s">
         <v>245</v>
       </c>
@@ -11992,7 +11977,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="207" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:19" ht="29.25">
       <c r="A207" s="2" t="s">
         <v>245</v>
       </c>
@@ -12047,7 +12032,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="208" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:19" ht="29.25">
       <c r="A208" s="2" t="s">
         <v>245</v>
       </c>
@@ -12098,7 +12083,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="209" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:19" ht="39">
       <c r="A209" s="2" t="s">
         <v>245</v>
       </c>
@@ -12155,7 +12140,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="210" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:19" ht="19.5">
       <c r="A210" s="2" t="s">
         <v>266</v>
       </c>
@@ -12190,7 +12175,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="211" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:19" ht="19.5">
       <c r="A211" s="2" t="s">
         <v>266</v>
       </c>
@@ -12247,7 +12232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="212" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:19" ht="29.25">
       <c r="A212" s="2" t="s">
         <v>266</v>
       </c>
@@ -12302,7 +12287,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="213" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:19" ht="29.25">
       <c r="A213" s="2" t="s">
         <v>266</v>
       </c>
@@ -12353,7 +12338,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="214" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:19" ht="29.25">
       <c r="A214" s="2" t="s">
         <v>272</v>
       </c>
@@ -12410,7 +12395,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:19" ht="29.25">
       <c r="A215" s="2" t="s">
         <v>272</v>
       </c>
@@ -12467,7 +12452,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="216" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:19" ht="29.25">
       <c r="A216" s="2" t="s">
         <v>272</v>
       </c>
@@ -12506,7 +12491,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="217" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:19" ht="29.25">
       <c r="A217" s="2" t="s">
         <v>272</v>
       </c>
@@ -12545,7 +12530,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="218" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:19" ht="29.25">
       <c r="A218" s="2" t="s">
         <v>272</v>
       </c>
@@ -12584,7 +12569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="219" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:19" ht="29.25">
       <c r="A219" s="2" t="s">
         <v>272</v>
       </c>
@@ -12641,7 +12626,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="220" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:19" ht="29.25">
       <c r="A220" s="2" t="s">
         <v>272</v>
       </c>
@@ -12698,7 +12683,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="221" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:19" ht="29.25">
       <c r="A221" s="2" t="s">
         <v>272</v>
       </c>
@@ -12755,7 +12740,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="222" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:19" ht="29.25">
       <c r="A222" s="2" t="s">
         <v>272</v>
       </c>
@@ -12800,7 +12785,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="223" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:19" ht="29.25">
       <c r="A223" s="2" t="s">
         <v>272</v>
       </c>
@@ -12845,7 +12830,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="224" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:19" ht="29.25">
       <c r="A224" s="2" t="s">
         <v>272</v>
       </c>
@@ -12890,7 +12875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="225" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:19" ht="29.25">
       <c r="A225" s="2" t="s">
         <v>272</v>
       </c>
@@ -12935,7 +12920,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="226" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:19" ht="29.25">
       <c r="A226" s="2" t="s">
         <v>272</v>
       </c>
@@ -12980,7 +12965,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="227" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:19" ht="29.25">
       <c r="A227" s="2" t="s">
         <v>272</v>
       </c>
@@ -13025,7 +13010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="228" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:19" ht="29.25">
       <c r="A228" s="2" t="s">
         <v>272</v>
       </c>
@@ -13070,7 +13055,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="229" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:19" ht="29.25">
       <c r="A229" s="2" t="s">
         <v>272</v>
       </c>
@@ -13115,7 +13100,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="230" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:19" ht="39">
       <c r="A230" s="2" t="s">
         <v>272</v>
       </c>
@@ -13160,7 +13145,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="231" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:19" ht="29.25">
       <c r="A231" s="2" t="s">
         <v>272</v>
       </c>
@@ -13205,7 +13190,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="232" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:19" ht="39">
       <c r="A232" s="2" t="s">
         <v>272</v>
       </c>
@@ -13250,7 +13235,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="233" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:19" ht="29.25">
       <c r="A233" s="2" t="s">
         <v>272</v>
       </c>
@@ -13295,7 +13280,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="234" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:19" ht="29.25">
       <c r="A234" s="2" t="s">
         <v>272</v>
       </c>
@@ -13340,7 +13325,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="235" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:19" ht="29.25">
       <c r="A235" s="2" t="s">
         <v>272</v>
       </c>
@@ -13385,7 +13370,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="236" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:19" ht="29.25">
       <c r="A236" s="2" t="s">
         <v>272</v>
       </c>
@@ -13430,7 +13415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="237" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:19" ht="29.25">
       <c r="A237" s="2" t="s">
         <v>272</v>
       </c>
@@ -13475,7 +13460,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="238" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:19" ht="29.25">
       <c r="A238" s="2" t="s">
         <v>272</v>
       </c>
@@ -13520,7 +13505,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:19" ht="29.25">
       <c r="A239" s="2" t="s">
         <v>272</v>
       </c>
@@ -13565,7 +13550,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="240" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:19" ht="29.25">
       <c r="A240" s="2" t="s">
         <v>272</v>
       </c>
@@ -13610,7 +13595,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="241" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:19" ht="29.25">
       <c r="A241" s="2" t="s">
         <v>272</v>
       </c>
@@ -13667,7 +13652,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="242" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:19" ht="29.25">
       <c r="A242" s="2" t="s">
         <v>272</v>
       </c>
@@ -13724,7 +13709,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="243" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:19" ht="29.25">
       <c r="A243" s="2" t="s">
         <v>272</v>
       </c>
@@ -13781,7 +13766,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="244" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:19" ht="29.25">
       <c r="A244" s="2" t="s">
         <v>272</v>
       </c>
@@ -13838,7 +13823,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="245" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:19" ht="29.25">
       <c r="A245" s="2" t="s">
         <v>272</v>
       </c>
@@ -13895,7 +13880,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="246" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:19" ht="29.25">
       <c r="A246" s="2" t="s">
         <v>272</v>
       </c>
@@ -13952,7 +13937,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="247" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:19" ht="29.25">
       <c r="A247" s="2" t="s">
         <v>272</v>
       </c>
@@ -14009,7 +13994,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="248" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:19" ht="29.25">
       <c r="A248" s="2" t="s">
         <v>272</v>
       </c>
@@ -14066,7 +14051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="249" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:19" ht="29.25">
       <c r="A249" s="2" t="s">
         <v>272</v>
       </c>
@@ -14123,7 +14108,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="250" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:19" ht="29.25">
       <c r="A250" s="2" t="s">
         <v>272</v>
       </c>
@@ -14180,7 +14165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="251" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:19" ht="29.25">
       <c r="A251" s="2" t="s">
         <v>272</v>
       </c>
@@ -14237,7 +14222,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="252" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:19" ht="29.25">
       <c r="A252" s="2" t="s">
         <v>272</v>
       </c>
@@ -14294,7 +14279,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="253" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:19" ht="39">
       <c r="A253" s="2" t="s">
         <v>272</v>
       </c>
@@ -14335,7 +14320,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="254" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:19" ht="39">
       <c r="A254" s="2" t="s">
         <v>272</v>
       </c>
@@ -14376,7 +14361,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="255" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:19" ht="39">
       <c r="A255" s="2" t="s">
         <v>272</v>
       </c>
@@ -14417,7 +14402,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="256" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:19" ht="29.25">
       <c r="A256" s="2" t="s">
         <v>272</v>
       </c>
@@ -14474,7 +14459,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="257" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:19" ht="48.75">
       <c r="A257" s="2" t="s">
         <v>272</v>
       </c>
@@ -14531,7 +14516,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="258" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:19" ht="29.25">
       <c r="A258" s="2" t="s">
         <v>272</v>
       </c>
@@ -14566,7 +14551,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="259" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:19" ht="29.25">
       <c r="A259" s="2" t="s">
         <v>272</v>
       </c>
@@ -14601,7 +14586,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="260" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:19" ht="29.25">
       <c r="A260" s="2" t="s">
         <v>272</v>
       </c>
@@ -14636,7 +14621,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="261" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:19" ht="29.25">
       <c r="A261" s="2" t="s">
         <v>272</v>
       </c>
@@ -14671,7 +14656,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="262" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:19" ht="29.25">
       <c r="A262" s="2" t="s">
         <v>272</v>
       </c>
@@ -14706,7 +14691,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="263" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:19" ht="29.25">
       <c r="A263" s="2" t="s">
         <v>272</v>
       </c>
@@ -14741,7 +14726,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="264" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:19" ht="29.25">
       <c r="A264" s="2" t="s">
         <v>272</v>
       </c>
@@ -14776,7 +14761,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="265" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:19" ht="29.25">
       <c r="A265" s="2" t="s">
         <v>272</v>
       </c>
@@ -14811,7 +14796,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="266" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:19" ht="29.25">
       <c r="A266" s="2" t="s">
         <v>272</v>
       </c>
@@ -14862,7 +14847,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="267" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:19" ht="29.25">
       <c r="A267" s="2" t="s">
         <v>318</v>
       </c>
@@ -14919,7 +14904,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="268" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:19" ht="29.25">
       <c r="A268" s="2" t="s">
         <v>318</v>
       </c>
@@ -14976,7 +14961,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="269" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:19" ht="29.25">
       <c r="A269" s="2" t="s">
         <v>318</v>
       </c>
@@ -15033,7 +15018,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="270" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:19" ht="29.25">
       <c r="A270" s="2" t="s">
         <v>318</v>
       </c>
@@ -15090,7 +15075,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="271" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:19" ht="29.25">
       <c r="A271" s="2" t="s">
         <v>318</v>
       </c>
@@ -15147,7 +15132,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="272" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:19" ht="29.25">
       <c r="A272" s="2" t="s">
         <v>318</v>
       </c>
@@ -15204,7 +15189,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="273" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:19" ht="29.25">
       <c r="A273" s="2" t="s">
         <v>318</v>
       </c>
@@ -15261,7 +15246,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="274" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:19" ht="29.25">
       <c r="A274" s="2" t="s">
         <v>318</v>
       </c>
@@ -15318,7 +15303,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="275" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:19" ht="29.25">
       <c r="A275" s="2" t="s">
         <v>318</v>
       </c>
@@ -15375,7 +15360,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="276" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:19" ht="29.25">
       <c r="A276" s="2" t="s">
         <v>318</v>
       </c>
@@ -15432,7 +15417,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="277" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:19" ht="29.25">
       <c r="A277" s="2" t="s">
         <v>318</v>
       </c>
@@ -15489,7 +15474,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="278" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:19" ht="29.25">
       <c r="A278" s="2" t="s">
         <v>318</v>
       </c>
@@ -15546,7 +15531,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="279" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:19" ht="29.25">
       <c r="A279" s="2" t="s">
         <v>318</v>
       </c>
@@ -15603,7 +15588,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="280" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:19" ht="29.25">
       <c r="A280" s="2" t="s">
         <v>318</v>
       </c>
@@ -15660,7 +15645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="281" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:19" ht="29.25">
       <c r="A281" s="2" t="s">
         <v>318</v>
       </c>
@@ -15717,7 +15702,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="282" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:19" ht="29.25">
       <c r="A282" s="2" t="s">
         <v>318</v>
       </c>
@@ -15774,7 +15759,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="283" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:19" ht="29.25">
       <c r="A283" s="2" t="s">
         <v>318</v>
       </c>
@@ -15831,7 +15816,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="284" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:19" ht="29.25">
       <c r="A284" s="2" t="s">
         <v>318</v>
       </c>
@@ -15888,7 +15873,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="285" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:19" ht="29.25">
       <c r="A285" s="2" t="s">
         <v>318</v>
       </c>
@@ -15945,7 +15930,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="286" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:19" ht="29.25">
       <c r="A286" s="2" t="s">
         <v>318</v>
       </c>
@@ -16002,7 +15987,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="287" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:19" ht="29.25">
       <c r="A287" s="2" t="s">
         <v>318</v>
       </c>
@@ -16053,7 +16038,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="288" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:19" ht="29.25">
       <c r="A288" s="2" t="s">
         <v>318</v>
       </c>
@@ -16110,7 +16095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="289" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:19" ht="29.25">
       <c r="A289" s="2" t="s">
         <v>318</v>
       </c>
@@ -16167,7 +16152,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="290" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:19" ht="29.25">
       <c r="A290" s="2" t="s">
         <v>318</v>
       </c>
@@ -16218,7 +16203,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="291" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:19" ht="29.25">
       <c r="A291" s="2" t="s">
         <v>318</v>
       </c>
@@ -16271,7 +16256,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="292" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:19" ht="39">
       <c r="A292" s="2" t="s">
         <v>318</v>
       </c>
@@ -16320,7 +16305,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="293" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:19" ht="39">
       <c r="A293" s="2" t="s">
         <v>318</v>
       </c>
@@ -16369,7 +16354,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="294" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:19" ht="19.5">
       <c r="A294" s="2" t="s">
         <v>350</v>
       </c>
@@ -16426,7 +16411,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="295" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:19" ht="68.25">
       <c r="A295" s="2" t="s">
         <v>350</v>
       </c>
@@ -16483,7 +16468,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="296" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:19" ht="19.5">
       <c r="A296" s="2" t="s">
         <v>350</v>
       </c>
@@ -16540,7 +16525,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="297" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:19" ht="19.5">
       <c r="A297" s="2" t="s">
         <v>350</v>
       </c>
@@ -16597,7 +16582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="298" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:19" ht="19.5">
       <c r="A298" s="2" t="s">
         <v>350</v>
       </c>
@@ -16654,7 +16639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="299" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:19" ht="19.5">
       <c r="A299" s="2" t="s">
         <v>350</v>
       </c>
@@ -16711,7 +16696,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="300" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:19" ht="19.5">
       <c r="A300" s="2" t="s">
         <v>350</v>
       </c>
@@ -16768,7 +16753,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="301" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:19" ht="19.5">
       <c r="A301" s="2" t="s">
         <v>350</v>
       </c>
@@ -16825,7 +16810,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="302" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:19" ht="19.5">
       <c r="A302" s="2" t="s">
         <v>350</v>
       </c>
@@ -16882,7 +16867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="303" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:19" ht="19.5">
       <c r="A303" s="2" t="s">
         <v>350</v>
       </c>
@@ -16939,7 +16924,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="304" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:19" ht="19.5">
       <c r="A304" s="2" t="s">
         <v>350</v>
       </c>
@@ -16996,7 +16981,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="305" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:19" ht="19.5">
       <c r="A305" s="2" t="s">
         <v>350</v>
       </c>
@@ -17035,7 +17020,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="306" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:19" ht="19.5">
       <c r="A306" s="2" t="s">
         <v>350</v>
       </c>
@@ -17092,7 +17077,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="307" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:19" ht="39">
       <c r="A307" s="2" t="s">
         <v>350</v>
       </c>
@@ -17149,7 +17134,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="308" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:19" ht="48.75">
       <c r="A308" s="2" t="s">
         <v>350</v>
       </c>
@@ -17206,7 +17191,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="309" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:19" ht="39">
       <c r="A309" s="2" t="s">
         <v>350</v>
       </c>
@@ -17263,7 +17248,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="310" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:19" ht="39">
       <c r="A310" s="2" t="s">
         <v>350</v>
       </c>
@@ -17320,7 +17305,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="311" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:19" ht="29.25">
       <c r="A311" s="2" t="s">
         <v>350</v>
       </c>
@@ -17377,7 +17362,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="312" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:19" ht="39">
       <c r="A312" s="2" t="s">
         <v>350</v>
       </c>
@@ -17432,7 +17417,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="313" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:19" ht="29.25">
       <c r="A313" s="2" t="s">
         <v>350</v>
       </c>
@@ -17489,7 +17474,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="314" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:19" ht="29.25">
       <c r="A314" s="2" t="s">
         <v>350</v>
       </c>
@@ -17546,7 +17531,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="315" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:19" ht="39">
       <c r="A315" s="2" t="s">
         <v>350</v>
       </c>
@@ -17603,7 +17588,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="316" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:19" ht="29.25">
       <c r="A316" s="2" t="s">
         <v>350</v>
       </c>
@@ -17660,7 +17645,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="317" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:19" ht="39">
       <c r="A317" s="2" t="s">
         <v>350</v>
       </c>
@@ -17717,7 +17702,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="318" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:19" ht="29.25">
       <c r="A318" s="2" t="s">
         <v>350</v>
       </c>
@@ -17774,7 +17759,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="319" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:19" ht="29.25">
       <c r="A319" s="2" t="s">
         <v>350</v>
       </c>
@@ -17831,7 +17816,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="320" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:19" ht="39">
       <c r="A320" s="2" t="s">
         <v>350</v>
       </c>
@@ -17888,7 +17873,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="321" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:19" ht="39">
       <c r="A321" s="2" t="s">
         <v>350</v>
       </c>
@@ -17945,7 +17930,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="322" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:19" ht="68.25">
       <c r="A322" s="2" t="s">
         <v>350</v>
       </c>
@@ -18002,7 +17987,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="323" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:19" ht="58.5">
       <c r="A323" s="2" t="s">
         <v>350</v>
       </c>
@@ -18059,7 +18044,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="324" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:19" ht="68.25">
       <c r="A324" s="2" t="s">
         <v>350</v>
       </c>
@@ -18116,7 +18101,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="325" spans="1:19" ht="72" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:19" ht="68.25">
       <c r="A325" s="2" t="s">
         <v>350</v>
       </c>
@@ -18173,7 +18158,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="326" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:19" ht="39">
       <c r="A326" s="2" t="s">
         <v>350</v>
       </c>
@@ -18230,7 +18215,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="327" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:19" ht="68.25">
       <c r="A327" s="2" t="s">
         <v>350</v>
       </c>
@@ -18287,7 +18272,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="328" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:19" ht="58.5">
       <c r="A328" s="2" t="s">
         <v>350</v>
       </c>
@@ -18344,7 +18329,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="329" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:19" ht="68.25">
       <c r="A329" s="2" t="s">
         <v>350</v>
       </c>
@@ -18401,7 +18386,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="330" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:19" ht="68.25">
       <c r="A330" s="2" t="s">
         <v>350</v>
       </c>
@@ -18458,7 +18443,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="331" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:19" ht="29.25">
       <c r="A331" s="2" t="s">
         <v>391</v>
       </c>
@@ -18513,7 +18498,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="332" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:19" ht="29.25">
       <c r="A332" s="2" t="s">
         <v>391</v>
       </c>
@@ -18568,7 +18553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="333" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:19" ht="29.25">
       <c r="A333" s="2" t="s">
         <v>391</v>
       </c>
@@ -18623,7 +18608,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="334" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:19" ht="29.25">
       <c r="A334" s="2" t="s">
         <v>391</v>
       </c>
@@ -18680,7 +18665,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="335" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:19" ht="29.25">
       <c r="A335" s="2" t="s">
         <v>391</v>
       </c>
@@ -18737,7 +18722,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="336" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:19" ht="29.25">
       <c r="A336" s="2" t="s">
         <v>391</v>
       </c>
@@ -18794,7 +18779,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="337" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:19" ht="29.25">
       <c r="A337" s="2" t="s">
         <v>391</v>
       </c>
@@ -18851,7 +18836,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="338" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:19" ht="29.25">
       <c r="A338" s="2" t="s">
         <v>391</v>
       </c>
@@ -18908,7 +18893,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="339" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:19" ht="29.25">
       <c r="A339" s="2" t="s">
         <v>391</v>
       </c>
@@ -18965,7 +18950,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="340" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:19" ht="29.25">
       <c r="A340" s="2" t="s">
         <v>391</v>
       </c>
@@ -19022,7 +19007,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="341" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:19" ht="29.25">
       <c r="A341" s="2" t="s">
         <v>391</v>
       </c>
@@ -19079,7 +19064,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="342" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:19" ht="29.25">
       <c r="A342" s="2" t="s">
         <v>391</v>
       </c>
@@ -19136,7 +19121,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="343" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:19" ht="29.25">
       <c r="A343" s="2" t="s">
         <v>391</v>
       </c>
@@ -19193,7 +19178,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="344" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:19" ht="29.25">
       <c r="A344" s="2" t="s">
         <v>391</v>
       </c>
@@ -19250,7 +19235,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="345" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:19" ht="29.25">
       <c r="A345" s="2" t="s">
         <v>391</v>
       </c>
@@ -19307,7 +19292,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="346" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:19" ht="29.25">
       <c r="A346" s="2" t="s">
         <v>391</v>
       </c>
@@ -19364,7 +19349,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="347" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:19" ht="29.25">
       <c r="A347" s="2" t="s">
         <v>391</v>
       </c>
@@ -19421,7 +19406,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="348" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:19" ht="29.25">
       <c r="A348" s="2" t="s">
         <v>391</v>
       </c>
@@ -19478,7 +19463,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="349" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:19" ht="29.25">
       <c r="A349" s="2" t="s">
         <v>391</v>
       </c>
@@ -19535,7 +19520,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="350" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:19" ht="29.25">
       <c r="A350" s="2" t="s">
         <v>391</v>
       </c>
@@ -19592,7 +19577,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="351" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:19" ht="29.25">
       <c r="A351" s="2" t="s">
         <v>391</v>
       </c>
@@ -19649,7 +19634,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="352" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:19" ht="29.25">
       <c r="A352" s="2" t="s">
         <v>391</v>
       </c>
@@ -19706,7 +19691,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="353" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:19" ht="29.25">
       <c r="A353" s="2" t="s">
         <v>391</v>
       </c>
@@ -19763,7 +19748,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="354" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:19" ht="29.25">
       <c r="A354" s="2" t="s">
         <v>391</v>
       </c>
@@ -19820,7 +19805,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="355" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:19" ht="29.25">
       <c r="A355" s="2" t="s">
         <v>391</v>
       </c>
@@ -19877,7 +19862,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="356" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:19" ht="29.25">
       <c r="A356" s="2" t="s">
         <v>391</v>
       </c>
@@ -19934,7 +19919,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="357" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:19" ht="29.25">
       <c r="A357" s="2" t="s">
         <v>391</v>
       </c>
@@ -19991,7 +19976,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="358" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:19" ht="29.25">
       <c r="A358" s="2" t="s">
         <v>391</v>
       </c>
@@ -20046,7 +20031,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="359" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:19" ht="29.25">
       <c r="A359" s="2" t="s">
         <v>391</v>
       </c>
@@ -20103,7 +20088,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="360" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:19" ht="29.25">
       <c r="A360" s="2" t="s">
         <v>391</v>
       </c>
@@ -20160,7 +20145,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="361" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:19" ht="29.25">
       <c r="A361" s="2" t="s">
         <v>391</v>
       </c>
@@ -20217,7 +20202,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="362" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:19" ht="29.25">
       <c r="A362" s="2" t="s">
         <v>391</v>
       </c>
@@ -20274,7 +20259,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="363" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:19" ht="29.25">
       <c r="A363" s="2" t="s">
         <v>391</v>
       </c>
@@ -20331,7 +20316,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="364" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:19" ht="39">
       <c r="A364" s="2" t="s">
         <v>391</v>
       </c>
@@ -20388,7 +20373,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="365" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:19" ht="39">
       <c r="A365" s="2" t="s">
         <v>391</v>
       </c>
@@ -20445,7 +20430,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="366" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:19" ht="39">
       <c r="A366" s="2" t="s">
         <v>391</v>
       </c>
@@ -20502,7 +20487,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="367" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:19" ht="39">
       <c r="A367" s="2" t="s">
         <v>391</v>
       </c>
@@ -20559,7 +20544,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="368" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:19" ht="39">
       <c r="A368" s="2" t="s">
         <v>391</v>
       </c>
@@ -20616,7 +20601,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="369" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:19" ht="39">
       <c r="A369" s="2" t="s">
         <v>391</v>
       </c>
@@ -20673,7 +20658,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="370" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:19" ht="39">
       <c r="A370" s="2" t="s">
         <v>391</v>
       </c>
@@ -20730,7 +20715,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="371" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:19" ht="39">
       <c r="A371" s="2" t="s">
         <v>391</v>
       </c>
@@ -20787,7 +20772,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="372" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:19" ht="39">
       <c r="A372" s="2" t="s">
         <v>424</v>
       </c>
@@ -20844,7 +20829,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="373" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:19" ht="39">
       <c r="A373" s="2" t="s">
         <v>424</v>
       </c>
@@ -20901,7 +20886,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="374" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:19" ht="39">
       <c r="A374" s="2" t="s">
         <v>424</v>
       </c>
@@ -20958,7 +20943,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="375" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:19" ht="48.75">
       <c r="A375" s="2" t="s">
         <v>424</v>
       </c>
@@ -21017,7 +21002,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="376" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:19" ht="39">
       <c r="A376" s="2" t="s">
         <v>424</v>
       </c>
@@ -21062,7 +21047,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="377" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:19" ht="39">
       <c r="A377" s="2" t="s">
         <v>424</v>
       </c>
@@ -21107,7 +21092,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="378" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:19" ht="39">
       <c r="A378" s="2" t="s">
         <v>424</v>
       </c>
@@ -21152,7 +21137,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="379" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:19" ht="39">
       <c r="A379" s="2" t="s">
         <v>424</v>
       </c>
@@ -21205,7 +21190,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="380" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:19" ht="39">
       <c r="A380" s="2" t="s">
         <v>424</v>
       </c>
@@ -21250,7 +21235,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="381" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:19" ht="39">
       <c r="A381" s="2" t="s">
         <v>424</v>
       </c>
@@ -21309,7 +21294,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="382" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:19" ht="48.75">
       <c r="A382" s="2" t="s">
         <v>424</v>
       </c>
@@ -21368,7 +21353,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="383" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:19" ht="29.25">
       <c r="A383" s="2" t="s">
         <v>444</v>
       </c>
@@ -21425,7 +21410,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="384" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:19" ht="29.25">
       <c r="A384" s="2" t="s">
         <v>444</v>
       </c>
@@ -21482,7 +21467,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="385" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:19" ht="39">
       <c r="A385" s="2" t="s">
         <v>444</v>
       </c>
@@ -21541,7 +21526,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="386" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:19" ht="39">
       <c r="A386" s="2" t="s">
         <v>444</v>
       </c>
@@ -21596,7 +21581,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="387" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:19" ht="48.75">
       <c r="A387" s="2" t="s">
         <v>444</v>
       </c>
@@ -21655,7 +21640,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="388" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:19" ht="29.25">
       <c r="A388" s="2" t="s">
         <v>444</v>
       </c>
@@ -21706,7 +21691,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="389" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:19" ht="39">
       <c r="A389" s="2" t="s">
         <v>454</v>
       </c>
@@ -21765,7 +21750,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="390" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:19" ht="48.75">
       <c r="A390" s="2" t="s">
         <v>454</v>
       </c>
@@ -21824,7 +21809,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="391" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:19" ht="48.75">
       <c r="A391" s="2" t="s">
         <v>454</v>
       </c>
@@ -21883,7 +21868,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="392" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:19" ht="58.5">
       <c r="A392" s="2" t="s">
         <v>454</v>
       </c>
@@ -21942,7 +21927,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="393" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:19" ht="58.5">
       <c r="A393" s="2" t="s">
         <v>454</v>
       </c>
@@ -21997,7 +21982,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="394" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:19" ht="19.5">
       <c r="A394" s="2" t="s">
         <v>464</v>
       </c>
@@ -22052,7 +22037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="395" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:19" ht="19.5">
       <c r="A395" s="2" t="s">
         <v>464</v>
       </c>
@@ -22107,7 +22092,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="396" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:19" ht="39">
       <c r="A396" s="2" t="s">
         <v>464</v>
       </c>
@@ -22164,7 +22149,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="397" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:19" ht="19.5">
       <c r="A397" s="2" t="s">
         <v>464</v>
       </c>
@@ -22203,7 +22188,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="398" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:19" ht="19.5">
       <c r="A398" s="2" t="s">
         <v>464</v>
       </c>
@@ -22236,7 +22221,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="399" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:19" ht="19.5">
       <c r="A399" s="2" t="s">
         <v>464</v>
       </c>
@@ -22269,7 +22254,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="400" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:19" ht="19.5">
       <c r="A400" s="2" t="s">
         <v>464</v>
       </c>
@@ -22302,7 +22287,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="401" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:19" ht="19.5">
       <c r="A401" s="2" t="s">
         <v>464</v>
       </c>
@@ -22341,7 +22326,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="402" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:19" ht="19.5">
       <c r="A402" s="2" t="s">
         <v>464</v>
       </c>
@@ -22380,7 +22365,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="403" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:19" ht="19.5">
       <c r="A403" s="2" t="s">
         <v>464</v>
       </c>
@@ -22419,7 +22404,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="404" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:19" ht="29.25">
       <c r="A404" s="2" t="s">
         <v>464</v>
       </c>
@@ -22478,7 +22463,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="405" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:19" ht="19.5">
       <c r="A405" s="2" t="s">
         <v>464</v>
       </c>
@@ -22535,7 +22520,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="406" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:19" ht="29.25">
       <c r="A406" s="2" t="s">
         <v>464</v>
       </c>
@@ -22594,7 +22579,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="407" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:19" ht="29.25">
       <c r="A407" s="2" t="s">
         <v>464</v>
       </c>
@@ -22645,7 +22630,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="408" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:19" ht="29.25">
       <c r="A408" s="2" t="s">
         <v>464</v>
       </c>
@@ -22696,7 +22681,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="409" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:19" ht="19.5">
       <c r="A409" s="2" t="s">
         <v>464</v>
       </c>
@@ -22753,7 +22738,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="410" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:19" ht="29.25">
       <c r="A410" s="2" t="s">
         <v>485</v>
       </c>
@@ -22808,7 +22793,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="411" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:19" ht="29.25">
       <c r="A411" s="2" t="s">
         <v>485</v>
       </c>
@@ -22867,7 +22852,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="412" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:19" ht="29.25">
       <c r="A412" s="2" t="s">
         <v>485</v>
       </c>
@@ -22910,7 +22895,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="413" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:19" ht="29.25">
       <c r="A413" s="2" t="s">
         <v>485</v>
       </c>
@@ -22963,7 +22948,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="414" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:19" ht="29.25">
       <c r="A414" s="2" t="s">
         <v>485</v>
       </c>
@@ -23008,7 +22993,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="415" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:19" ht="29.25">
       <c r="A415" s="2" t="s">
         <v>485</v>
       </c>
@@ -23053,7 +23038,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="416" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:19" ht="29.25">
       <c r="A416" s="2" t="s">
         <v>485</v>
       </c>
@@ -23098,7 +23083,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="417" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:19" ht="29.25">
       <c r="A417" s="2" t="s">
         <v>485</v>
       </c>
@@ -23143,7 +23128,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="418" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:19" ht="29.25">
       <c r="A418" s="2" t="s">
         <v>485</v>
       </c>
@@ -23188,7 +23173,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="419" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:19" ht="29.25">
       <c r="A419" s="2" t="s">
         <v>485</v>
       </c>
@@ -23233,7 +23218,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="420" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:19" ht="39">
       <c r="A420" s="2" t="s">
         <v>485</v>
       </c>
@@ -23278,7 +23263,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="421" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:19" ht="48.75">
       <c r="A421" s="2" t="s">
         <v>485</v>
       </c>
@@ -23323,7 +23308,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="422" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:19" ht="39">
       <c r="A422" s="2" t="s">
         <v>485</v>
       </c>
@@ -23368,7 +23353,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="423" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:19" ht="39">
       <c r="A423" s="2" t="s">
         <v>485</v>
       </c>
@@ -23413,7 +23398,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="424" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:19" ht="29.25">
       <c r="A424" s="2" t="s">
         <v>485</v>
       </c>
@@ -23470,7 +23455,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="425" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:19" ht="29.25">
       <c r="A425" s="2" t="s">
         <v>485</v>
       </c>
@@ -23525,7 +23510,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="426" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:19" ht="29.25">
       <c r="A426" s="2" t="s">
         <v>485</v>
       </c>
@@ -23580,7 +23565,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="427" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:19" ht="29.25">
       <c r="A427" s="2" t="s">
         <v>485</v>
       </c>
@@ -23635,7 +23620,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="428" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:19" ht="29.25">
       <c r="A428" s="2" t="s">
         <v>485</v>
       </c>
@@ -23692,7 +23677,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="429" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:19" ht="29.25">
       <c r="A429" s="2" t="s">
         <v>485</v>
       </c>
@@ -23749,7 +23734,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="430" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:19" ht="39">
       <c r="A430" s="2" t="s">
         <v>485</v>
       </c>
@@ -23788,7 +23773,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="431" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:19" ht="39">
       <c r="A431" s="2" t="s">
         <v>485</v>
       </c>
@@ -23827,7 +23812,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="432" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:19" ht="39">
       <c r="A432" s="2" t="s">
         <v>485</v>
       </c>
@@ -23866,7 +23851,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="433" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:19" ht="39">
       <c r="A433" s="2" t="s">
         <v>485</v>
       </c>
@@ -23905,7 +23890,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="434" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:19" ht="39">
       <c r="A434" s="2" t="s">
         <v>485</v>
       </c>
@@ -23944,7 +23929,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="435" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:19" ht="39">
       <c r="A435" s="2" t="s">
         <v>485</v>
       </c>
@@ -23983,7 +23968,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="436" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:19" ht="39">
       <c r="A436" s="2" t="s">
         <v>485</v>
       </c>
@@ -24022,7 +24007,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="437" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:19" ht="39">
       <c r="A437" s="2" t="s">
         <v>485</v>
       </c>
@@ -24061,7 +24046,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="438" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:19" ht="39">
       <c r="A438" s="2" t="s">
         <v>485</v>
       </c>
@@ -24100,7 +24085,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="439" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:19" ht="39">
       <c r="A439" s="2" t="s">
         <v>485</v>
       </c>
@@ -24139,7 +24124,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="440" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:19" ht="39">
       <c r="A440" s="2" t="s">
         <v>485</v>
       </c>
@@ -24178,7 +24163,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="441" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:19" ht="39">
       <c r="A441" s="2" t="s">
         <v>485</v>
       </c>
@@ -24217,7 +24202,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="442" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:19" ht="29.25">
       <c r="A442" s="2" t="s">
         <v>485</v>
       </c>
@@ -24276,7 +24261,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="443" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:19" ht="29.25">
       <c r="A443" s="2" t="s">
         <v>485</v>
       </c>
@@ -24315,7 +24300,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="444" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:19" ht="29.25">
       <c r="A444" s="2" t="s">
         <v>522</v>
       </c>
@@ -24372,7 +24357,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="445" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:19" ht="29.25">
       <c r="A445" s="2" t="s">
         <v>522</v>
       </c>
@@ -24429,7 +24414,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="446" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:19" ht="29.25">
       <c r="A446" s="2" t="s">
         <v>522</v>
       </c>
@@ -24486,7 +24471,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="447" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:19" ht="29.25">
       <c r="A447" s="2" t="s">
         <v>522</v>
       </c>
@@ -24543,7 +24528,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="448" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:19" ht="48.75">
       <c r="A448" s="2" t="s">
         <v>522</v>
       </c>
@@ -24600,7 +24585,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="449" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:19" ht="29.25">
       <c r="A449" s="2" t="s">
         <v>522</v>
       </c>
@@ -24657,7 +24642,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="450" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:19" ht="29.25">
       <c r="A450" s="2" t="s">
         <v>522</v>
       </c>
@@ -24714,7 +24699,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="451" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:19" ht="29.25">
       <c r="A451" s="2" t="s">
         <v>522</v>
       </c>
@@ -24773,7 +24758,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="452" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:19" ht="29.25">
       <c r="A452" s="2" t="s">
         <v>522</v>
       </c>
@@ -24832,7 +24817,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="453" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:19" ht="29.25">
       <c r="A453" s="2" t="s">
         <v>522</v>
       </c>
@@ -24891,7 +24876,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="454" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:19" ht="29.25">
       <c r="A454" s="2" t="s">
         <v>522</v>
       </c>
@@ -24948,7 +24933,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="455" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:19" ht="29.25">
       <c r="A455" s="2" t="s">
         <v>522</v>
       </c>
@@ -25005,7 +24990,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="456" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:19" ht="29.25">
       <c r="A456" s="2" t="s">
         <v>522</v>
       </c>
@@ -25062,7 +25047,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="457" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:19" ht="29.25">
       <c r="A457" s="2" t="s">
         <v>522</v>
       </c>
@@ -25119,7 +25104,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="458" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:19" ht="29.25">
       <c r="A458" s="2" t="s">
         <v>522</v>
       </c>
@@ -25178,7 +25163,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="459" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:19" ht="48.75">
       <c r="A459" s="2" t="s">
         <v>522</v>
       </c>
@@ -25237,7 +25222,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="460" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:19" ht="29.25">
       <c r="A460" s="2" t="s">
         <v>522</v>
       </c>
@@ -25296,7 +25281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="461" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:19" ht="39">
       <c r="A461" s="2" t="s">
         <v>522</v>
       </c>
@@ -25353,7 +25338,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="462" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:19" ht="39">
       <c r="A462" s="2" t="s">
         <v>522</v>
       </c>
@@ -25410,7 +25395,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="463" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:19" ht="29.25">
       <c r="A463" s="2" t="s">
         <v>522</v>
       </c>
@@ -25453,7 +25438,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="464" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:19" ht="29.25">
       <c r="A464" s="2" t="s">
         <v>522</v>
       </c>
@@ -25512,7 +25497,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="465" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:19" ht="29.25">
       <c r="A465" s="2" t="s">
         <v>522</v>
       </c>
@@ -25571,7 +25556,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="466" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:19" ht="29.25">
       <c r="A466" s="2" t="s">
         <v>522</v>
       </c>
@@ -25622,7 +25607,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="467" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:19" ht="39">
       <c r="A467" s="2" t="s">
         <v>522</v>
       </c>
@@ -25659,7 +25644,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="468" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:19" ht="39">
       <c r="A468" s="2" t="s">
         <v>522</v>
       </c>
@@ -25716,7 +25701,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="469" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:19" ht="39">
       <c r="A469" s="2" t="s">
         <v>522</v>
       </c>
@@ -25773,9 +25758,9 @@
         <v>557</v>
       </c>
     </row>
-    <row r="470" spans="1:19" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:19" ht="0" hidden="1" customHeight="1"/>
+    <row r="471" spans="1:19" ht="18" customHeight="1"/>
+    <row r="472" spans="1:19" ht="17.100000000000001" customHeight="1">
       <c r="A472" s="12" t="s">
         <v>560</v>
       </c>

</xml_diff>

<commit_message>
Zlecenie 18.05.23 zmiany w zakresie zestawu krajowego cz. 5 + 08.05.23 zmiany w zakresie zestawu krajowego cz. 4 - aktualizacja plików excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="18060" windowHeight="7050"/>
   </bookViews>
@@ -1705,13 +1700,13 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 09-05-2023, 13:26</t>
+    <t>Last update: 23-05-2023, 11:41</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$-10809]0.0;\-0.0;0.0"/>
     <numFmt numFmtId="165" formatCode="[$-10809]0.00;\-0.00;0.00"/>
@@ -1720,7 +1715,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1918,14 +1913,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1946,7 +1933,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="0" name="Picture 1"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2009,7 +1996,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2041,10 +2028,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2076,7 +2062,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -2252,15 +2237,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S472"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2272,17 +2257,17 @@
     <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="36" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2341,7 +2326,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="19.5">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2398,7 +2383,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="15">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2455,7 +2440,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -2512,7 +2497,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="15">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -2569,7 +2554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="15">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -2626,7 +2611,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="15">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -2683,7 +2668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -2740,7 +2725,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2797,7 +2782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -2854,7 +2839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2911,7 +2896,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="19.5">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -2968,7 +2953,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="19.5">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -3025,7 +3010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="15">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -3064,7 +3049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="29.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -3123,7 +3108,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="97.5">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -3178,7 +3163,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="97.5">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -3233,7 +3218,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="97.5">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -3288,7 +3273,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="19.5">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -3343,7 +3328,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="29.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -3400,7 +3385,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="29.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -3457,7 +3442,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="29.25">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -3506,7 +3491,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="68.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -3555,7 +3540,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="29.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
@@ -3604,7 +3589,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="29.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -3653,7 +3638,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="29.25">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
@@ -3704,7 +3689,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="39">
       <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
@@ -3761,7 +3746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="39">
       <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
@@ -3818,7 +3803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="39">
       <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
@@ -3875,7 +3860,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="39">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -3932,7 +3917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="19.5">
       <c r="A33" s="2" t="s">
         <v>66</v>
       </c>
@@ -3987,7 +3972,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="29.25">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -4032,7 +4017,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="29.25">
       <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
@@ -4077,7 +4062,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="29.25">
       <c r="A36" s="2" t="s">
         <v>66</v>
       </c>
@@ -4122,7 +4107,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="29.25">
       <c r="A37" s="2" t="s">
         <v>66</v>
       </c>
@@ -4167,7 +4152,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="29.25">
       <c r="A38" s="2" t="s">
         <v>66</v>
       </c>
@@ -4212,7 +4197,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="29.25">
       <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
@@ -4257,7 +4242,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="39">
       <c r="A40" s="2" t="s">
         <v>66</v>
       </c>
@@ -4296,7 +4281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="97.5">
       <c r="A41" s="2" t="s">
         <v>66</v>
       </c>
@@ -4355,7 +4340,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="97.5">
       <c r="A42" s="2" t="s">
         <v>66</v>
       </c>
@@ -4414,7 +4399,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="97.5">
       <c r="A43" s="2" t="s">
         <v>66</v>
       </c>
@@ -4473,7 +4458,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="97.5">
       <c r="A44" s="2" t="s">
         <v>66</v>
       </c>
@@ -4532,7 +4517,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="97.5">
       <c r="A45" s="2" t="s">
         <v>66</v>
       </c>
@@ -4591,7 +4576,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="97.5">
       <c r="A46" s="2" t="s">
         <v>66</v>
       </c>
@@ -4650,7 +4635,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="48.75">
       <c r="A47" s="2" t="s">
         <v>66</v>
       </c>
@@ -4699,7 +4684,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="48.75">
       <c r="A48" s="2" t="s">
         <v>66</v>
       </c>
@@ -4748,7 +4733,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="19.5">
       <c r="A49" s="2" t="s">
         <v>66</v>
       </c>
@@ -4805,7 +4790,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="29.25">
       <c r="A50" s="2" t="s">
         <v>66</v>
       </c>
@@ -4856,7 +4841,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="19.5">
       <c r="A51" s="2" t="s">
         <v>95</v>
       </c>
@@ -4913,7 +4898,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="19.5">
       <c r="A52" s="2" t="s">
         <v>95</v>
       </c>
@@ -4970,7 +4955,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>95</v>
       </c>
@@ -5027,7 +5012,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>95</v>
       </c>
@@ -5084,7 +5069,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>95</v>
       </c>
@@ -5141,7 +5126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>95</v>
       </c>
@@ -5198,7 +5183,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>95</v>
       </c>
@@ -5255,7 +5240,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>95</v>
       </c>
@@ -5312,7 +5297,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="29.25">
       <c r="A59" s="2" t="s">
         <v>95</v>
       </c>
@@ -5369,7 +5354,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>95</v>
       </c>
@@ -5426,7 +5411,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="29.25">
       <c r="A61" s="2" t="s">
         <v>95</v>
       </c>
@@ -5485,7 +5470,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="29.25">
       <c r="A62" s="2" t="s">
         <v>95</v>
       </c>
@@ -5544,7 +5529,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="29.25">
       <c r="A63" s="2" t="s">
         <v>95</v>
       </c>
@@ -5603,7 +5588,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="19.5">
       <c r="A64" s="2" t="s">
         <v>95</v>
       </c>
@@ -5660,7 +5645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="29.25">
       <c r="A65" s="2" t="s">
         <v>95</v>
       </c>
@@ -5719,7 +5704,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="29.25">
       <c r="A66" s="2" t="s">
         <v>95</v>
       </c>
@@ -5778,7 +5763,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="29.25">
       <c r="A67" s="2" t="s">
         <v>95</v>
       </c>
@@ -5837,7 +5822,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="29.25">
       <c r="A68" s="2" t="s">
         <v>95</v>
       </c>
@@ -5894,7 +5879,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="29.25">
       <c r="A69" s="2" t="s">
         <v>95</v>
       </c>
@@ -5951,7 +5936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" ht="29.25">
       <c r="A70" s="2" t="s">
         <v>95</v>
       </c>
@@ -6008,7 +5993,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" ht="29.25">
       <c r="A71" s="2" t="s">
         <v>95</v>
       </c>
@@ -6065,7 +6050,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" ht="19.5">
       <c r="A72" s="2" t="s">
         <v>95</v>
       </c>
@@ -6122,7 +6107,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="19.5">
       <c r="A73" s="2" t="s">
         <v>95</v>
       </c>
@@ -6179,7 +6164,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="19.5">
       <c r="A74" s="2" t="s">
         <v>95</v>
       </c>
@@ -6236,7 +6221,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="19.5">
       <c r="A75" s="2" t="s">
         <v>95</v>
       </c>
@@ -6293,7 +6278,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" ht="29.25">
       <c r="A76" s="2" t="s">
         <v>95</v>
       </c>
@@ -6350,7 +6335,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" ht="29.25">
       <c r="A77" s="2" t="s">
         <v>95</v>
       </c>
@@ -6389,7 +6374,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" ht="19.5">
       <c r="A78" s="2" t="s">
         <v>95</v>
       </c>
@@ -6446,7 +6431,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="19.5">
       <c r="A79" s="2" t="s">
         <v>95</v>
       </c>
@@ -6503,7 +6488,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" ht="19.5">
       <c r="A80" s="2" t="s">
         <v>95</v>
       </c>
@@ -6560,7 +6545,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="19.5">
       <c r="A81" s="2" t="s">
         <v>95</v>
       </c>
@@ -6601,7 +6586,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="29.25">
       <c r="A82" s="2" t="s">
         <v>95</v>
       </c>
@@ -6646,7 +6631,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="29.25">
       <c r="A83" s="2" t="s">
         <v>95</v>
       </c>
@@ -6691,7 +6676,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="19.5">
       <c r="A84" s="2" t="s">
         <v>95</v>
       </c>
@@ -6726,7 +6711,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="29.25">
       <c r="A85" s="2" t="s">
         <v>95</v>
       </c>
@@ -6761,7 +6746,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="19.5">
       <c r="A86" s="2" t="s">
         <v>95</v>
       </c>
@@ -6818,7 +6803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="19.5">
       <c r="A87" s="2" t="s">
         <v>95</v>
       </c>
@@ -6857,7 +6842,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" ht="19.5">
       <c r="A88" s="2" t="s">
         <v>95</v>
       </c>
@@ -6914,7 +6899,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="19.5">
       <c r="A89" s="2" t="s">
         <v>95</v>
       </c>
@@ -6971,7 +6956,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="19.5">
       <c r="A90" s="2" t="s">
         <v>95</v>
       </c>
@@ -7012,7 +6997,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="29.25">
       <c r="A91" s="2" t="s">
         <v>95</v>
       </c>
@@ -7063,7 +7048,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" ht="19.5">
       <c r="A92" s="2" t="s">
         <v>95</v>
       </c>
@@ -7102,7 +7087,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" ht="19.5">
       <c r="A93" s="2" t="s">
         <v>95</v>
       </c>
@@ -7141,7 +7126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" ht="19.5">
       <c r="A94" s="2" t="s">
         <v>95</v>
       </c>
@@ -7180,7 +7165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" ht="19.5">
       <c r="A95" s="2" t="s">
         <v>95</v>
       </c>
@@ -7233,7 +7218,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" ht="48.75">
       <c r="A96" s="2" t="s">
         <v>149</v>
       </c>
@@ -7270,7 +7255,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" ht="48.75">
       <c r="A97" s="2" t="s">
         <v>149</v>
       </c>
@@ -7307,7 +7292,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" ht="48.75">
       <c r="A98" s="2" t="s">
         <v>149</v>
       </c>
@@ -7344,7 +7329,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" ht="48.75">
       <c r="A99" s="2" t="s">
         <v>149</v>
       </c>
@@ -7385,7 +7370,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" ht="48.75">
       <c r="A100" s="2" t="s">
         <v>149</v>
       </c>
@@ -7426,7 +7411,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" ht="48.75">
       <c r="A101" s="2" t="s">
         <v>149</v>
       </c>
@@ -7467,7 +7452,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" ht="48.75">
       <c r="A102" s="2" t="s">
         <v>149</v>
       </c>
@@ -7508,7 +7493,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" ht="48.75">
       <c r="A103" s="2" t="s">
         <v>149</v>
       </c>
@@ -7549,7 +7534,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" ht="48.75">
       <c r="A104" s="2" t="s">
         <v>149</v>
       </c>
@@ -7590,7 +7575,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" ht="29.25">
       <c r="A105" s="2" t="s">
         <v>149</v>
       </c>
@@ -7627,7 +7612,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" ht="19.5">
       <c r="A106" s="2" t="s">
         <v>149</v>
       </c>
@@ -7684,7 +7669,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" ht="19.5">
       <c r="A107" s="2" t="s">
         <v>149</v>
       </c>
@@ -7741,7 +7726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" ht="19.5">
       <c r="A108" s="2" t="s">
         <v>149</v>
       </c>
@@ -7798,7 +7783,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" ht="19.5">
       <c r="A109" s="2" t="s">
         <v>149</v>
       </c>
@@ -7835,7 +7820,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" ht="19.5">
       <c r="A110" s="2" t="s">
         <v>149</v>
       </c>
@@ -7872,7 +7857,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" ht="19.5">
       <c r="A111" s="2" t="s">
         <v>149</v>
       </c>
@@ -7909,7 +7894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" ht="29.25">
       <c r="A112" s="2" t="s">
         <v>149</v>
       </c>
@@ -7954,7 +7939,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" ht="19.5">
       <c r="A113" s="2" t="s">
         <v>149</v>
       </c>
@@ -8001,7 +7986,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" ht="39">
       <c r="A114" s="2" t="s">
         <v>149</v>
       </c>
@@ -8048,7 +8033,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" ht="48.75">
       <c r="A115" s="2" t="s">
         <v>149</v>
       </c>
@@ -8095,7 +8080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" ht="58.5">
       <c r="A116" s="2" t="s">
         <v>149</v>
       </c>
@@ -8142,7 +8127,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" ht="29.25">
       <c r="A117" s="2" t="s">
         <v>149</v>
       </c>
@@ -8189,7 +8174,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" ht="29.25">
       <c r="A118" s="2" t="s">
         <v>149</v>
       </c>
@@ -8234,7 +8219,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" ht="19.5">
       <c r="A119" s="2" t="s">
         <v>149</v>
       </c>
@@ -8281,7 +8266,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" ht="39">
       <c r="A120" s="2" t="s">
         <v>149</v>
       </c>
@@ -8328,7 +8313,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" ht="48.75">
       <c r="A121" s="2" t="s">
         <v>149</v>
       </c>
@@ -8375,7 +8360,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" ht="58.5">
       <c r="A122" s="2" t="s">
         <v>149</v>
       </c>
@@ -8422,7 +8407,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" ht="29.25">
       <c r="A123" s="2" t="s">
         <v>149</v>
       </c>
@@ -8469,7 +8454,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" ht="48.75">
       <c r="A124" s="2" t="s">
         <v>149</v>
       </c>
@@ -8508,7 +8493,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" ht="48.75">
       <c r="A125" s="2" t="s">
         <v>149</v>
       </c>
@@ -8547,7 +8532,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" ht="29.25">
       <c r="A126" s="2" t="s">
         <v>149</v>
       </c>
@@ -8604,7 +8589,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" ht="29.25">
       <c r="A127" s="2" t="s">
         <v>149</v>
       </c>
@@ -8639,7 +8624,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" ht="29.25">
       <c r="A128" s="2" t="s">
         <v>149</v>
       </c>
@@ -8674,7 +8659,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" ht="29.25">
       <c r="A129" s="2" t="s">
         <v>149</v>
       </c>
@@ -8709,7 +8694,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" ht="29.25">
       <c r="A130" s="2" t="s">
         <v>149</v>
       </c>
@@ -8744,7 +8729,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" ht="29.25">
       <c r="A131" s="2" t="s">
         <v>149</v>
       </c>
@@ -8779,7 +8764,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" ht="29.25">
       <c r="A132" s="2" t="s">
         <v>149</v>
       </c>
@@ -8814,7 +8799,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" ht="29.25">
       <c r="A133" s="2" t="s">
         <v>149</v>
       </c>
@@ -8849,7 +8834,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" ht="29.25">
       <c r="A134" s="2" t="s">
         <v>149</v>
       </c>
@@ -8884,7 +8869,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" ht="29.25">
       <c r="A135" s="2" t="s">
         <v>149</v>
       </c>
@@ -8919,7 +8904,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" ht="29.25">
       <c r="A136" s="2" t="s">
         <v>149</v>
       </c>
@@ -8954,7 +8939,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" ht="29.25">
       <c r="A137" s="2" t="s">
         <v>149</v>
       </c>
@@ -8989,7 +8974,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" ht="29.25">
       <c r="A138" s="2" t="s">
         <v>149</v>
       </c>
@@ -9024,7 +9009,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" ht="29.25">
       <c r="A139" s="2" t="s">
         <v>149</v>
       </c>
@@ -9059,7 +9044,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" ht="29.25">
       <c r="A140" s="2" t="s">
         <v>149</v>
       </c>
@@ -9094,7 +9079,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" ht="29.25">
       <c r="A141" s="2" t="s">
         <v>149</v>
       </c>
@@ -9129,7 +9114,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" ht="29.25">
       <c r="A142" s="2" t="s">
         <v>149</v>
       </c>
@@ -9164,7 +9149,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" ht="48.75">
       <c r="A143" s="2" t="s">
         <v>149</v>
       </c>
@@ -9223,7 +9208,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" ht="58.5">
       <c r="A144" s="2" t="s">
         <v>149</v>
       </c>
@@ -9282,7 +9267,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" ht="58.5">
       <c r="A145" s="2" t="s">
         <v>149</v>
       </c>
@@ -9317,7 +9302,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" ht="58.5">
       <c r="A146" s="2" t="s">
         <v>149</v>
       </c>
@@ -9352,7 +9337,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" ht="58.5">
       <c r="A147" s="2" t="s">
         <v>149</v>
       </c>
@@ -9411,7 +9396,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" ht="58.5">
       <c r="A148" s="2" t="s">
         <v>149</v>
       </c>
@@ -9470,7 +9455,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" ht="58.5">
       <c r="A149" s="2" t="s">
         <v>149</v>
       </c>
@@ -9529,7 +9514,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" ht="29.25">
       <c r="A150" s="2" t="s">
         <v>149</v>
       </c>
@@ -9580,7 +9565,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" ht="58.5">
       <c r="A151" s="2" t="s">
         <v>149</v>
       </c>
@@ -9635,7 +9620,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" ht="58.5">
       <c r="A152" s="2" t="s">
         <v>149</v>
       </c>
@@ -9690,7 +9675,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" ht="58.5">
       <c r="A153" s="2" t="s">
         <v>149</v>
       </c>
@@ -9745,7 +9730,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" ht="58.5">
       <c r="A154" s="2" t="s">
         <v>149</v>
       </c>
@@ -9800,7 +9785,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" ht="29.25">
       <c r="A155" s="2" t="s">
         <v>205</v>
       </c>
@@ -9835,7 +9820,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" ht="19.5">
       <c r="A156" s="2" t="s">
         <v>205</v>
       </c>
@@ -9892,7 +9877,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" ht="39">
       <c r="A157" s="2" t="s">
         <v>205</v>
       </c>
@@ -9927,7 +9912,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" ht="39">
       <c r="A158" s="2" t="s">
         <v>205</v>
       </c>
@@ -9962,7 +9947,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" ht="39">
       <c r="A159" s="2" t="s">
         <v>205</v>
       </c>
@@ -9997,7 +9982,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="160" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" ht="39">
       <c r="A160" s="2" t="s">
         <v>205</v>
       </c>
@@ -10032,7 +10017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" ht="39">
       <c r="A161" s="2" t="s">
         <v>205</v>
       </c>
@@ -10067,7 +10052,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" ht="19.5">
       <c r="A162" s="2" t="s">
         <v>205</v>
       </c>
@@ -10102,7 +10087,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:19" ht="19.5">
       <c r="A163" s="2" t="s">
         <v>205</v>
       </c>
@@ -10137,7 +10122,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" ht="19.5">
       <c r="A164" s="2" t="s">
         <v>205</v>
       </c>
@@ -10172,7 +10157,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:19" ht="19.5">
       <c r="A165" s="2" t="s">
         <v>205</v>
       </c>
@@ -10207,7 +10192,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" ht="19.5">
       <c r="A166" s="2" t="s">
         <v>205</v>
       </c>
@@ -10242,7 +10227,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" ht="19.5">
       <c r="A167" s="2" t="s">
         <v>205</v>
       </c>
@@ -10277,7 +10262,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:19" ht="19.5">
       <c r="A168" s="2" t="s">
         <v>205</v>
       </c>
@@ -10312,7 +10297,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" ht="19.5">
       <c r="A169" s="2" t="s">
         <v>205</v>
       </c>
@@ -10347,7 +10332,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:19" ht="29.25">
       <c r="A170" s="2" t="s">
         <v>205</v>
       </c>
@@ -10386,7 +10371,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:19" ht="29.25">
       <c r="A171" s="2" t="s">
         <v>205</v>
       </c>
@@ -10425,7 +10410,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:19" ht="29.25">
       <c r="A172" s="2" t="s">
         <v>205</v>
       </c>
@@ -10482,7 +10467,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:19" ht="29.25">
       <c r="A173" s="2" t="s">
         <v>205</v>
       </c>
@@ -10539,7 +10524,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:19" ht="29.25">
       <c r="A174" s="2" t="s">
         <v>205</v>
       </c>
@@ -10596,7 +10581,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:19" ht="29.25">
       <c r="A175" s="2" t="s">
         <v>205</v>
       </c>
@@ -10653,7 +10638,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:19" ht="29.25">
       <c r="A176" s="2" t="s">
         <v>205</v>
       </c>
@@ -10710,7 +10695,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="177" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:19" ht="19.5">
       <c r="A177" s="2" t="s">
         <v>205</v>
       </c>
@@ -10755,7 +10740,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="178" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:19" ht="39">
       <c r="A178" s="2" t="s">
         <v>205</v>
       </c>
@@ -10800,7 +10785,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:19" ht="19.5">
       <c r="A179" s="2" t="s">
         <v>205</v>
       </c>
@@ -10845,7 +10830,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:19" ht="39">
       <c r="A180" s="2" t="s">
         <v>205</v>
       </c>
@@ -10890,7 +10875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:19" ht="39">
       <c r="A181" s="2" t="s">
         <v>205</v>
       </c>
@@ -10935,7 +10920,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="182" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:19" ht="39">
       <c r="A182" s="2" t="s">
         <v>205</v>
       </c>
@@ -10980,7 +10965,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:19" ht="39">
       <c r="A183" s="2" t="s">
         <v>205</v>
       </c>
@@ -11025,7 +11010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:19" ht="39">
       <c r="A184" s="2" t="s">
         <v>205</v>
       </c>
@@ -11064,7 +11049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:19" ht="39">
       <c r="A185" s="2" t="s">
         <v>205</v>
       </c>
@@ -11103,7 +11088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="186" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:19" ht="39">
       <c r="A186" s="2" t="s">
         <v>205</v>
       </c>
@@ -11142,7 +11127,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:19" ht="39">
       <c r="A187" s="2" t="s">
         <v>205</v>
       </c>
@@ -11181,7 +11166,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:19" ht="39">
       <c r="A188" s="2" t="s">
         <v>205</v>
       </c>
@@ -11220,7 +11205,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:19" ht="39">
       <c r="A189" s="2" t="s">
         <v>205</v>
       </c>
@@ -11259,7 +11244,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:19" ht="39">
       <c r="A190" s="2" t="s">
         <v>205</v>
       </c>
@@ -11298,7 +11283,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:19" ht="39">
       <c r="A191" s="2" t="s">
         <v>205</v>
       </c>
@@ -11337,7 +11322,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:19" ht="39">
       <c r="A192" s="2" t="s">
         <v>205</v>
       </c>
@@ -11376,7 +11361,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="193" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:19" ht="39">
       <c r="A193" s="2" t="s">
         <v>205</v>
       </c>
@@ -11415,7 +11400,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:19" ht="39">
       <c r="A194" s="2" t="s">
         <v>205</v>
       </c>
@@ -11454,7 +11439,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="195" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:19" ht="39">
       <c r="A195" s="2" t="s">
         <v>205</v>
       </c>
@@ -11493,7 +11478,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="196" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:19" ht="19.5">
       <c r="A196" s="2" t="s">
         <v>205</v>
       </c>
@@ -11534,7 +11519,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:19" ht="19.5">
       <c r="A197" s="2" t="s">
         <v>205</v>
       </c>
@@ -11589,7 +11574,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:19" ht="19.5">
       <c r="A198" s="2" t="s">
         <v>205</v>
       </c>
@@ -11644,7 +11629,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:19" ht="19.5">
       <c r="A199" s="2" t="s">
         <v>245</v>
       </c>
@@ -11701,7 +11686,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="200" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:19" ht="29.25">
       <c r="A200" s="2" t="s">
         <v>245</v>
       </c>
@@ -11758,7 +11743,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="201" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:19" ht="19.5">
       <c r="A201" s="2" t="s">
         <v>245</v>
       </c>
@@ -11815,7 +11800,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="202" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:19" ht="19.5">
       <c r="A202" s="2" t="s">
         <v>245</v>
       </c>
@@ -11850,7 +11835,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="203" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:19" ht="19.5">
       <c r="A203" s="2" t="s">
         <v>245</v>
       </c>
@@ -11885,7 +11870,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="204" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:19" ht="29.25">
       <c r="A204" s="2" t="s">
         <v>245</v>
       </c>
@@ -11940,7 +11925,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="205" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:19" ht="19.5">
       <c r="A205" s="2" t="s">
         <v>245</v>
       </c>
@@ -11995,7 +11980,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="206" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:19" ht="19.5">
       <c r="A206" s="2" t="s">
         <v>245</v>
       </c>
@@ -12040,7 +12025,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="207" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:19" ht="29.25">
       <c r="A207" s="2" t="s">
         <v>245</v>
       </c>
@@ -12099,7 +12084,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="208" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:19" ht="29.25">
       <c r="A208" s="2" t="s">
         <v>245</v>
       </c>
@@ -12150,7 +12135,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="209" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:19" ht="39">
       <c r="A209" s="2" t="s">
         <v>245</v>
       </c>
@@ -12207,7 +12192,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="210" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:19" ht="19.5">
       <c r="A210" s="2" t="s">
         <v>266</v>
       </c>
@@ -12242,7 +12227,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="211" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:19" ht="19.5">
       <c r="A211" s="2" t="s">
         <v>266</v>
       </c>
@@ -12299,7 +12284,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="212" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:19" ht="29.25">
       <c r="A212" s="2" t="s">
         <v>266</v>
       </c>
@@ -12354,7 +12339,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="213" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:19" ht="29.25">
       <c r="A213" s="2" t="s">
         <v>266</v>
       </c>
@@ -12405,7 +12390,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="214" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:19" ht="29.25">
       <c r="A214" s="2" t="s">
         <v>272</v>
       </c>
@@ -12462,7 +12447,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:19" ht="29.25">
       <c r="A215" s="2" t="s">
         <v>272</v>
       </c>
@@ -12519,7 +12504,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="216" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:19" ht="29.25">
       <c r="A216" s="2" t="s">
         <v>272</v>
       </c>
@@ -12558,7 +12543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="217" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:19" ht="29.25">
       <c r="A217" s="2" t="s">
         <v>272</v>
       </c>
@@ -12597,7 +12582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="218" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:19" ht="29.25">
       <c r="A218" s="2" t="s">
         <v>272</v>
       </c>
@@ -12636,7 +12621,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="219" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:19" ht="29.25">
       <c r="A219" s="2" t="s">
         <v>272</v>
       </c>
@@ -12693,7 +12678,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="220" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:19" ht="29.25">
       <c r="A220" s="2" t="s">
         <v>272</v>
       </c>
@@ -12750,7 +12735,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="221" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:19" ht="29.25">
       <c r="A221" s="2" t="s">
         <v>272</v>
       </c>
@@ -12807,7 +12792,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="222" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:19" ht="29.25">
       <c r="A222" s="2" t="s">
         <v>272</v>
       </c>
@@ -12852,7 +12837,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="223" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:19" ht="29.25">
       <c r="A223" s="2" t="s">
         <v>272</v>
       </c>
@@ -12897,7 +12882,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="224" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:19" ht="29.25">
       <c r="A224" s="2" t="s">
         <v>272</v>
       </c>
@@ -12942,7 +12927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="225" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:19" ht="29.25">
       <c r="A225" s="2" t="s">
         <v>272</v>
       </c>
@@ -12987,7 +12972,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="226" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:19" ht="29.25">
       <c r="A226" s="2" t="s">
         <v>272</v>
       </c>
@@ -13032,7 +13017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="227" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:19" ht="29.25">
       <c r="A227" s="2" t="s">
         <v>272</v>
       </c>
@@ -13077,7 +13062,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="228" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:19" ht="29.25">
       <c r="A228" s="2" t="s">
         <v>272</v>
       </c>
@@ -13122,7 +13107,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="229" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:19" ht="29.25">
       <c r="A229" s="2" t="s">
         <v>272</v>
       </c>
@@ -13167,7 +13152,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="230" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:19" ht="39">
       <c r="A230" s="2" t="s">
         <v>272</v>
       </c>
@@ -13212,7 +13197,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="231" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:19" ht="29.25">
       <c r="A231" s="2" t="s">
         <v>272</v>
       </c>
@@ -13257,7 +13242,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="232" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:19" ht="39">
       <c r="A232" s="2" t="s">
         <v>272</v>
       </c>
@@ -13302,7 +13287,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="233" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:19" ht="29.25">
       <c r="A233" s="2" t="s">
         <v>272</v>
       </c>
@@ -13347,7 +13332,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="234" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:19" ht="29.25">
       <c r="A234" s="2" t="s">
         <v>272</v>
       </c>
@@ -13392,7 +13377,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="235" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:19" ht="29.25">
       <c r="A235" s="2" t="s">
         <v>272</v>
       </c>
@@ -13437,7 +13422,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="236" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:19" ht="29.25">
       <c r="A236" s="2" t="s">
         <v>272</v>
       </c>
@@ -13482,7 +13467,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="237" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:19" ht="29.25">
       <c r="A237" s="2" t="s">
         <v>272</v>
       </c>
@@ -13527,7 +13512,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="238" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:19" ht="29.25">
       <c r="A238" s="2" t="s">
         <v>272</v>
       </c>
@@ -13572,7 +13557,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:19" ht="29.25">
       <c r="A239" s="2" t="s">
         <v>272</v>
       </c>
@@ -13617,7 +13602,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="240" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:19" ht="29.25">
       <c r="A240" s="2" t="s">
         <v>272</v>
       </c>
@@ -13662,7 +13647,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="241" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:19" ht="29.25">
       <c r="A241" s="2" t="s">
         <v>272</v>
       </c>
@@ -13721,7 +13706,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="242" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:19" ht="29.25">
       <c r="A242" s="2" t="s">
         <v>272</v>
       </c>
@@ -13780,7 +13765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="243" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:19" ht="29.25">
       <c r="A243" s="2" t="s">
         <v>272</v>
       </c>
@@ -13839,7 +13824,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="244" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:19" ht="29.25">
       <c r="A244" s="2" t="s">
         <v>272</v>
       </c>
@@ -13898,7 +13883,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="245" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:19" ht="29.25">
       <c r="A245" s="2" t="s">
         <v>272</v>
       </c>
@@ -13957,7 +13942,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="246" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:19" ht="29.25">
       <c r="A246" s="2" t="s">
         <v>272</v>
       </c>
@@ -14016,7 +14001,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="247" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:19" ht="29.25">
       <c r="A247" s="2" t="s">
         <v>272</v>
       </c>
@@ -14075,7 +14060,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="248" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:19" ht="29.25">
       <c r="A248" s="2" t="s">
         <v>272</v>
       </c>
@@ -14134,7 +14119,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="249" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:19" ht="29.25">
       <c r="A249" s="2" t="s">
         <v>272</v>
       </c>
@@ -14193,7 +14178,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="250" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:19" ht="29.25">
       <c r="A250" s="2" t="s">
         <v>272</v>
       </c>
@@ -14250,7 +14235,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="251" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:19" ht="29.25">
       <c r="A251" s="2" t="s">
         <v>272</v>
       </c>
@@ -14307,7 +14292,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="252" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:19" ht="29.25">
       <c r="A252" s="2" t="s">
         <v>272</v>
       </c>
@@ -14364,7 +14349,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="253" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:19" ht="39">
       <c r="A253" s="2" t="s">
         <v>272</v>
       </c>
@@ -14405,7 +14390,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="254" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:19" ht="39">
       <c r="A254" s="2" t="s">
         <v>272</v>
       </c>
@@ -14446,7 +14431,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="255" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:19" ht="39">
       <c r="A255" s="2" t="s">
         <v>272</v>
       </c>
@@ -14487,7 +14472,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="256" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:19" ht="29.25">
       <c r="A256" s="2" t="s">
         <v>272</v>
       </c>
@@ -14544,7 +14529,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="257" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:19" ht="48.75">
       <c r="A257" s="2" t="s">
         <v>272</v>
       </c>
@@ -14601,7 +14586,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="258" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:19" ht="29.25">
       <c r="A258" s="2" t="s">
         <v>272</v>
       </c>
@@ -14636,7 +14621,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="259" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:19" ht="29.25">
       <c r="A259" s="2" t="s">
         <v>272</v>
       </c>
@@ -14671,7 +14656,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="260" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:19" ht="29.25">
       <c r="A260" s="2" t="s">
         <v>272</v>
       </c>
@@ -14706,7 +14691,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="261" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:19" ht="29.25">
       <c r="A261" s="2" t="s">
         <v>272</v>
       </c>
@@ -14741,7 +14726,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="262" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:19" ht="29.25">
       <c r="A262" s="2" t="s">
         <v>272</v>
       </c>
@@ -14776,7 +14761,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="263" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:19" ht="29.25">
       <c r="A263" s="2" t="s">
         <v>272</v>
       </c>
@@ -14811,7 +14796,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="264" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:19" ht="29.25">
       <c r="A264" s="2" t="s">
         <v>272</v>
       </c>
@@ -14846,7 +14831,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="265" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:19" ht="29.25">
       <c r="A265" s="2" t="s">
         <v>272</v>
       </c>
@@ -14881,7 +14866,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="266" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:19" ht="29.25">
       <c r="A266" s="2" t="s">
         <v>272</v>
       </c>
@@ -14932,7 +14917,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="267" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:19" ht="29.25">
       <c r="A267" s="2" t="s">
         <v>318</v>
       </c>
@@ -14989,7 +14974,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="268" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:19" ht="29.25">
       <c r="A268" s="2" t="s">
         <v>318</v>
       </c>
@@ -15046,7 +15031,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="269" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:19" ht="29.25">
       <c r="A269" s="2" t="s">
         <v>318</v>
       </c>
@@ -15103,7 +15088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="270" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:19" ht="29.25">
       <c r="A270" s="2" t="s">
         <v>318</v>
       </c>
@@ -15160,7 +15145,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="271" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:19" ht="29.25">
       <c r="A271" s="2" t="s">
         <v>318</v>
       </c>
@@ -15217,7 +15202,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="272" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:19" ht="29.25">
       <c r="A272" s="2" t="s">
         <v>318</v>
       </c>
@@ -15274,7 +15259,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="273" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:19" ht="29.25">
       <c r="A273" s="2" t="s">
         <v>318</v>
       </c>
@@ -15331,7 +15316,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="274" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:19" ht="29.25">
       <c r="A274" s="2" t="s">
         <v>318</v>
       </c>
@@ -15388,7 +15373,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="275" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:19" ht="29.25">
       <c r="A275" s="2" t="s">
         <v>318</v>
       </c>
@@ -15445,7 +15430,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="276" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:19" ht="29.25">
       <c r="A276" s="2" t="s">
         <v>318</v>
       </c>
@@ -15502,7 +15487,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="277" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:19" ht="29.25">
       <c r="A277" s="2" t="s">
         <v>318</v>
       </c>
@@ -15559,7 +15544,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="278" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:19" ht="29.25">
       <c r="A278" s="2" t="s">
         <v>318</v>
       </c>
@@ -15616,7 +15601,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="279" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:19" ht="29.25">
       <c r="A279" s="2" t="s">
         <v>318</v>
       </c>
@@ -15673,7 +15658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="280" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:19" ht="29.25">
       <c r="A280" s="2" t="s">
         <v>318</v>
       </c>
@@ -15730,7 +15715,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="281" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:19" ht="29.25">
       <c r="A281" s="2" t="s">
         <v>318</v>
       </c>
@@ -15787,7 +15772,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="282" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:19" ht="29.25">
       <c r="A282" s="2" t="s">
         <v>318</v>
       </c>
@@ -15844,7 +15829,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="283" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:19" ht="29.25">
       <c r="A283" s="2" t="s">
         <v>318</v>
       </c>
@@ -15901,7 +15886,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="284" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:19" ht="29.25">
       <c r="A284" s="2" t="s">
         <v>318</v>
       </c>
@@ -15958,7 +15943,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="285" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:19" ht="29.25">
       <c r="A285" s="2" t="s">
         <v>318</v>
       </c>
@@ -16015,7 +16000,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="286" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:19" ht="29.25">
       <c r="A286" s="2" t="s">
         <v>318</v>
       </c>
@@ -16072,7 +16057,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="287" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:19" ht="29.25">
       <c r="A287" s="2" t="s">
         <v>318</v>
       </c>
@@ -16123,7 +16108,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="288" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:19" ht="29.25">
       <c r="A288" s="2" t="s">
         <v>318</v>
       </c>
@@ -16180,7 +16165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="289" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:19" ht="29.25">
       <c r="A289" s="2" t="s">
         <v>318</v>
       </c>
@@ -16237,7 +16222,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="290" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:19" ht="29.25">
       <c r="A290" s="2" t="s">
         <v>318</v>
       </c>
@@ -16288,7 +16273,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="291" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:19" ht="29.25">
       <c r="A291" s="2" t="s">
         <v>318</v>
       </c>
@@ -16341,7 +16326,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="292" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:19" ht="39">
       <c r="A292" s="2" t="s">
         <v>318</v>
       </c>
@@ -16390,7 +16375,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="293" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:19" ht="39">
       <c r="A293" s="2" t="s">
         <v>318</v>
       </c>
@@ -16439,7 +16424,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="294" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:19" ht="19.5">
       <c r="A294" s="2" t="s">
         <v>350</v>
       </c>
@@ -16496,7 +16481,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="295" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:19" ht="68.25">
       <c r="A295" s="2" t="s">
         <v>350</v>
       </c>
@@ -16553,7 +16538,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="296" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:19" ht="19.5">
       <c r="A296" s="2" t="s">
         <v>350</v>
       </c>
@@ -16610,7 +16595,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="297" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:19" ht="19.5">
       <c r="A297" s="2" t="s">
         <v>350</v>
       </c>
@@ -16667,7 +16652,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="298" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:19" ht="19.5">
       <c r="A298" s="2" t="s">
         <v>350</v>
       </c>
@@ -16724,7 +16709,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="299" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:19" ht="19.5">
       <c r="A299" s="2" t="s">
         <v>350</v>
       </c>
@@ -16781,7 +16766,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="300" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:19" ht="19.5">
       <c r="A300" s="2" t="s">
         <v>350</v>
       </c>
@@ -16838,7 +16823,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="301" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:19" ht="19.5">
       <c r="A301" s="2" t="s">
         <v>350</v>
       </c>
@@ -16895,7 +16880,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="302" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:19" ht="19.5">
       <c r="A302" s="2" t="s">
         <v>350</v>
       </c>
@@ -16952,7 +16937,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="303" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:19" ht="19.5">
       <c r="A303" s="2" t="s">
         <v>350</v>
       </c>
@@ -17009,7 +16994,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="304" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:19" ht="19.5">
       <c r="A304" s="2" t="s">
         <v>350</v>
       </c>
@@ -17066,7 +17051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="305" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:19" ht="19.5">
       <c r="A305" s="2" t="s">
         <v>350</v>
       </c>
@@ -17105,7 +17090,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="306" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:19" ht="19.5">
       <c r="A306" s="2" t="s">
         <v>350</v>
       </c>
@@ -17162,7 +17147,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="307" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:19" ht="39">
       <c r="A307" s="2" t="s">
         <v>350</v>
       </c>
@@ -17219,7 +17204,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="308" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:19" ht="48.75">
       <c r="A308" s="2" t="s">
         <v>350</v>
       </c>
@@ -17276,7 +17261,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="309" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:19" ht="39">
       <c r="A309" s="2" t="s">
         <v>350</v>
       </c>
@@ -17333,7 +17318,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="310" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:19" ht="39">
       <c r="A310" s="2" t="s">
         <v>350</v>
       </c>
@@ -17390,7 +17375,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="311" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:19" ht="29.25">
       <c r="A311" s="2" t="s">
         <v>350</v>
       </c>
@@ -17447,7 +17432,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="312" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:19" ht="39">
       <c r="A312" s="2" t="s">
         <v>350</v>
       </c>
@@ -17504,7 +17489,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="313" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:19" ht="29.25">
       <c r="A313" s="2" t="s">
         <v>350</v>
       </c>
@@ -17561,7 +17546,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="314" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:19" ht="29.25">
       <c r="A314" s="2" t="s">
         <v>350</v>
       </c>
@@ -17618,7 +17603,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="315" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:19" ht="39">
       <c r="A315" s="2" t="s">
         <v>350</v>
       </c>
@@ -17675,7 +17660,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="316" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:19" ht="29.25">
       <c r="A316" s="2" t="s">
         <v>350</v>
       </c>
@@ -17732,7 +17717,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="317" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:19" ht="39">
       <c r="A317" s="2" t="s">
         <v>350</v>
       </c>
@@ -17789,7 +17774,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="318" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:19" ht="29.25">
       <c r="A318" s="2" t="s">
         <v>350</v>
       </c>
@@ -17846,7 +17831,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="319" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:19" ht="29.25">
       <c r="A319" s="2" t="s">
         <v>350</v>
       </c>
@@ -17905,7 +17890,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="320" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:19" ht="39">
       <c r="A320" s="2" t="s">
         <v>350</v>
       </c>
@@ -17964,7 +17949,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="321" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:19" ht="39">
       <c r="A321" s="2" t="s">
         <v>350</v>
       </c>
@@ -18023,7 +18008,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="322" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:19" ht="68.25">
       <c r="A322" s="2" t="s">
         <v>350</v>
       </c>
@@ -18082,7 +18067,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="323" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:19" ht="58.5">
       <c r="A323" s="2" t="s">
         <v>350</v>
       </c>
@@ -18141,7 +18126,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="324" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:19" ht="68.25">
       <c r="A324" s="2" t="s">
         <v>350</v>
       </c>
@@ -18200,7 +18185,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="325" spans="1:19" ht="72" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:19" ht="68.25">
       <c r="A325" s="2" t="s">
         <v>350</v>
       </c>
@@ -18259,7 +18244,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="326" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:19" ht="39">
       <c r="A326" s="2" t="s">
         <v>350</v>
       </c>
@@ -18316,7 +18301,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="327" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:19" ht="68.25">
       <c r="A327" s="2" t="s">
         <v>350</v>
       </c>
@@ -18373,7 +18358,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="328" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:19" ht="58.5">
       <c r="A328" s="2" t="s">
         <v>350</v>
       </c>
@@ -18430,7 +18415,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="329" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:19" ht="68.25">
       <c r="A329" s="2" t="s">
         <v>350</v>
       </c>
@@ -18487,7 +18472,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="330" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:19" ht="68.25">
       <c r="A330" s="2" t="s">
         <v>350</v>
       </c>
@@ -18544,7 +18529,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="331" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:19" ht="29.25">
       <c r="A331" s="2" t="s">
         <v>391</v>
       </c>
@@ -18599,7 +18584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="332" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:19" ht="29.25">
       <c r="A332" s="2" t="s">
         <v>391</v>
       </c>
@@ -18654,7 +18639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="333" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:19" ht="29.25">
       <c r="A333" s="2" t="s">
         <v>391</v>
       </c>
@@ -18709,7 +18694,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="334" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:19" ht="29.25">
       <c r="A334" s="2" t="s">
         <v>391</v>
       </c>
@@ -18766,7 +18751,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="335" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:19" ht="29.25">
       <c r="A335" s="2" t="s">
         <v>391</v>
       </c>
@@ -18823,7 +18808,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="336" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:19" ht="29.25">
       <c r="A336" s="2" t="s">
         <v>391</v>
       </c>
@@ -18880,7 +18865,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="337" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:19" ht="29.25">
       <c r="A337" s="2" t="s">
         <v>391</v>
       </c>
@@ -18937,7 +18922,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="338" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:19" ht="29.25">
       <c r="A338" s="2" t="s">
         <v>391</v>
       </c>
@@ -18994,7 +18979,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="339" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:19" ht="29.25">
       <c r="A339" s="2" t="s">
         <v>391</v>
       </c>
@@ -19051,7 +19036,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="340" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:19" ht="29.25">
       <c r="A340" s="2" t="s">
         <v>391</v>
       </c>
@@ -19108,7 +19093,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="341" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:19" ht="29.25">
       <c r="A341" s="2" t="s">
         <v>391</v>
       </c>
@@ -19165,7 +19150,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="342" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:19" ht="29.25">
       <c r="A342" s="2" t="s">
         <v>391</v>
       </c>
@@ -19222,7 +19207,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="343" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:19" ht="29.25">
       <c r="A343" s="2" t="s">
         <v>391</v>
       </c>
@@ -19279,7 +19264,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="344" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:19" ht="29.25">
       <c r="A344" s="2" t="s">
         <v>391</v>
       </c>
@@ -19336,7 +19321,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="345" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:19" ht="29.25">
       <c r="A345" s="2" t="s">
         <v>391</v>
       </c>
@@ -19393,7 +19378,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="346" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:19" ht="29.25">
       <c r="A346" s="2" t="s">
         <v>391</v>
       </c>
@@ -19450,7 +19435,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="347" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:19" ht="29.25">
       <c r="A347" s="2" t="s">
         <v>391</v>
       </c>
@@ -19507,7 +19492,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="348" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:19" ht="29.25">
       <c r="A348" s="2" t="s">
         <v>391</v>
       </c>
@@ -19564,7 +19549,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="349" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:19" ht="29.25">
       <c r="A349" s="2" t="s">
         <v>391</v>
       </c>
@@ -19621,7 +19606,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="350" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:19" ht="29.25">
       <c r="A350" s="2" t="s">
         <v>391</v>
       </c>
@@ -19678,7 +19663,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="351" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:19" ht="29.25">
       <c r="A351" s="2" t="s">
         <v>391</v>
       </c>
@@ -19735,7 +19720,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="352" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:19" ht="29.25">
       <c r="A352" s="2" t="s">
         <v>391</v>
       </c>
@@ -19792,7 +19777,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="353" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:19" ht="29.25">
       <c r="A353" s="2" t="s">
         <v>391</v>
       </c>
@@ -19849,7 +19834,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="354" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:19" ht="29.25">
       <c r="A354" s="2" t="s">
         <v>391</v>
       </c>
@@ -19906,7 +19891,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="355" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:19" ht="29.25">
       <c r="A355" s="2" t="s">
         <v>391</v>
       </c>
@@ -19963,7 +19948,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="356" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:19" ht="29.25">
       <c r="A356" s="2" t="s">
         <v>391</v>
       </c>
@@ -20020,7 +20005,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="357" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:19" ht="29.25">
       <c r="A357" s="2" t="s">
         <v>391</v>
       </c>
@@ -20077,7 +20062,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="358" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:19" ht="29.25">
       <c r="A358" s="2" t="s">
         <v>391</v>
       </c>
@@ -20132,7 +20117,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="359" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:19" ht="29.25">
       <c r="A359" s="2" t="s">
         <v>391</v>
       </c>
@@ -20189,7 +20174,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="360" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:19" ht="29.25">
       <c r="A360" s="2" t="s">
         <v>391</v>
       </c>
@@ -20246,7 +20231,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="361" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:19" ht="29.25">
       <c r="A361" s="2" t="s">
         <v>391</v>
       </c>
@@ -20303,7 +20288,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="362" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:19" ht="29.25">
       <c r="A362" s="2" t="s">
         <v>391</v>
       </c>
@@ -20360,7 +20345,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="363" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:19" ht="29.25">
       <c r="A363" s="2" t="s">
         <v>391</v>
       </c>
@@ -20417,7 +20402,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="364" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:19" ht="39">
       <c r="A364" s="2" t="s">
         <v>391</v>
       </c>
@@ -20474,7 +20459,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="365" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:19" ht="39">
       <c r="A365" s="2" t="s">
         <v>391</v>
       </c>
@@ -20531,7 +20516,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="366" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:19" ht="39">
       <c r="A366" s="2" t="s">
         <v>391</v>
       </c>
@@ -20588,7 +20573,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="367" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:19" ht="39">
       <c r="A367" s="2" t="s">
         <v>391</v>
       </c>
@@ -20645,7 +20630,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="368" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:19" ht="39">
       <c r="A368" s="2" t="s">
         <v>391</v>
       </c>
@@ -20702,7 +20687,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="369" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:19" ht="39">
       <c r="A369" s="2" t="s">
         <v>391</v>
       </c>
@@ -20759,7 +20744,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="370" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:19" ht="39">
       <c r="A370" s="2" t="s">
         <v>391</v>
       </c>
@@ -20816,7 +20801,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="371" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:19" ht="39">
       <c r="A371" s="2" t="s">
         <v>391</v>
       </c>
@@ -20873,7 +20858,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="372" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:19" ht="39">
       <c r="A372" s="2" t="s">
         <v>424</v>
       </c>
@@ -20930,7 +20915,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="373" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:19" ht="39">
       <c r="A373" s="2" t="s">
         <v>424</v>
       </c>
@@ -20987,7 +20972,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="374" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:19" ht="39">
       <c r="A374" s="2" t="s">
         <v>424</v>
       </c>
@@ -21044,7 +21029,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="375" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:19" ht="48.75">
       <c r="A375" s="2" t="s">
         <v>424</v>
       </c>
@@ -21103,7 +21088,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="376" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:19" ht="39">
       <c r="A376" s="2" t="s">
         <v>424</v>
       </c>
@@ -21148,7 +21133,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="377" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:19" ht="39">
       <c r="A377" s="2" t="s">
         <v>424</v>
       </c>
@@ -21193,7 +21178,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="378" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:19" ht="39">
       <c r="A378" s="2" t="s">
         <v>424</v>
       </c>
@@ -21238,7 +21223,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="379" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:19" ht="39">
       <c r="A379" s="2" t="s">
         <v>424</v>
       </c>
@@ -21291,7 +21276,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="380" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:19" ht="39">
       <c r="A380" s="2" t="s">
         <v>424</v>
       </c>
@@ -21336,7 +21321,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="381" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:19" ht="39">
       <c r="A381" s="2" t="s">
         <v>424</v>
       </c>
@@ -21395,7 +21380,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="382" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:19" ht="48.75">
       <c r="A382" s="2" t="s">
         <v>424</v>
       </c>
@@ -21454,7 +21439,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="383" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:19" ht="29.25">
       <c r="A383" s="2" t="s">
         <v>444</v>
       </c>
@@ -21511,7 +21496,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="384" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:19" ht="29.25">
       <c r="A384" s="2" t="s">
         <v>444</v>
       </c>
@@ -21568,7 +21553,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="385" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:19" ht="39">
       <c r="A385" s="2" t="s">
         <v>444</v>
       </c>
@@ -21627,7 +21612,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="386" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:19" ht="39">
       <c r="A386" s="2" t="s">
         <v>444</v>
       </c>
@@ -21682,7 +21667,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="387" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:19" ht="48.75">
       <c r="A387" s="2" t="s">
         <v>444</v>
       </c>
@@ -21741,7 +21726,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="388" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:19" ht="29.25">
       <c r="A388" s="2" t="s">
         <v>444</v>
       </c>
@@ -21792,7 +21777,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="389" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:19" ht="39">
       <c r="A389" s="2" t="s">
         <v>454</v>
       </c>
@@ -21851,7 +21836,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="390" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:19" ht="48.75">
       <c r="A390" s="2" t="s">
         <v>454</v>
       </c>
@@ -21910,7 +21895,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="391" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:19" ht="48.75">
       <c r="A391" s="2" t="s">
         <v>454</v>
       </c>
@@ -21969,7 +21954,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="392" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:19" ht="58.5">
       <c r="A392" s="2" t="s">
         <v>454</v>
       </c>
@@ -22028,7 +22013,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="393" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:19" ht="58.5">
       <c r="A393" s="2" t="s">
         <v>454</v>
       </c>
@@ -22085,7 +22070,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="394" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:19" ht="19.5">
       <c r="A394" s="2" t="s">
         <v>464</v>
       </c>
@@ -22142,7 +22127,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="395" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:19" ht="19.5">
       <c r="A395" s="2" t="s">
         <v>464</v>
       </c>
@@ -22199,7 +22184,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="396" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:19" ht="39">
       <c r="A396" s="2" t="s">
         <v>464</v>
       </c>
@@ -22256,7 +22241,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="397" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:19" ht="19.5">
       <c r="A397" s="2" t="s">
         <v>464</v>
       </c>
@@ -22295,7 +22280,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="398" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:19" ht="19.5">
       <c r="A398" s="2" t="s">
         <v>464</v>
       </c>
@@ -22328,7 +22313,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="399" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:19" ht="19.5">
       <c r="A399" s="2" t="s">
         <v>464</v>
       </c>
@@ -22361,7 +22346,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="400" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:19" ht="19.5">
       <c r="A400" s="2" t="s">
         <v>464</v>
       </c>
@@ -22394,7 +22379,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="401" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:19" ht="19.5">
       <c r="A401" s="2" t="s">
         <v>464</v>
       </c>
@@ -22433,7 +22418,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="402" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:19" ht="19.5">
       <c r="A402" s="2" t="s">
         <v>464</v>
       </c>
@@ -22472,7 +22457,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="403" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:19" ht="19.5">
       <c r="A403" s="2" t="s">
         <v>464</v>
       </c>
@@ -22511,7 +22496,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="404" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:19" ht="29.25">
       <c r="A404" s="2" t="s">
         <v>464</v>
       </c>
@@ -22570,7 +22555,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="405" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:19" ht="19.5">
       <c r="A405" s="2" t="s">
         <v>464</v>
       </c>
@@ -22627,7 +22612,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="406" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:19" ht="29.25">
       <c r="A406" s="2" t="s">
         <v>464</v>
       </c>
@@ -22686,7 +22671,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="407" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:19" ht="29.25">
       <c r="A407" s="2" t="s">
         <v>464</v>
       </c>
@@ -22737,7 +22722,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="408" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:19" ht="29.25">
       <c r="A408" s="2" t="s">
         <v>464</v>
       </c>
@@ -22788,7 +22773,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="409" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:19" ht="19.5">
       <c r="A409" s="2" t="s">
         <v>464</v>
       </c>
@@ -22845,7 +22830,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="410" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:19" ht="29.25">
       <c r="A410" s="2" t="s">
         <v>485</v>
       </c>
@@ -22902,7 +22887,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="411" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:19" ht="29.25">
       <c r="A411" s="2" t="s">
         <v>485</v>
       </c>
@@ -22961,7 +22946,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="412" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:19" ht="29.25">
       <c r="A412" s="2" t="s">
         <v>485</v>
       </c>
@@ -23004,7 +22989,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="413" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:19" ht="29.25">
       <c r="A413" s="2" t="s">
         <v>485</v>
       </c>
@@ -23057,7 +23042,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="414" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:19" ht="29.25">
       <c r="A414" s="2" t="s">
         <v>485</v>
       </c>
@@ -23102,7 +23087,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="415" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:19" ht="29.25">
       <c r="A415" s="2" t="s">
         <v>485</v>
       </c>
@@ -23147,7 +23132,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="416" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:19" ht="29.25">
       <c r="A416" s="2" t="s">
         <v>485</v>
       </c>
@@ -23192,7 +23177,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="417" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:19" ht="29.25">
       <c r="A417" s="2" t="s">
         <v>485</v>
       </c>
@@ -23237,7 +23222,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="418" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:19" ht="29.25">
       <c r="A418" s="2" t="s">
         <v>485</v>
       </c>
@@ -23282,7 +23267,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="419" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:19" ht="29.25">
       <c r="A419" s="2" t="s">
         <v>485</v>
       </c>
@@ -23327,7 +23312,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="420" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:19" ht="39">
       <c r="A420" s="2" t="s">
         <v>485</v>
       </c>
@@ -23372,7 +23357,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="421" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:19" ht="48.75">
       <c r="A421" s="2" t="s">
         <v>485</v>
       </c>
@@ -23417,7 +23402,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="422" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:19" ht="39">
       <c r="A422" s="2" t="s">
         <v>485</v>
       </c>
@@ -23462,7 +23447,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="423" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:19" ht="39">
       <c r="A423" s="2" t="s">
         <v>485</v>
       </c>
@@ -23507,7 +23492,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="424" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:19" ht="29.25">
       <c r="A424" s="2" t="s">
         <v>485</v>
       </c>
@@ -23564,7 +23549,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="425" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:19" ht="29.25">
       <c r="A425" s="2" t="s">
         <v>485</v>
       </c>
@@ -23621,7 +23606,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="426" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:19" ht="29.25">
       <c r="A426" s="2" t="s">
         <v>485</v>
       </c>
@@ -23678,7 +23663,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="427" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:19" ht="29.25">
       <c r="A427" s="2" t="s">
         <v>485</v>
       </c>
@@ -23735,7 +23720,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="428" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:19" ht="29.25">
       <c r="A428" s="2" t="s">
         <v>485</v>
       </c>
@@ -23792,7 +23777,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="429" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:19" ht="29.25">
       <c r="A429" s="2" t="s">
         <v>485</v>
       </c>
@@ -23849,7 +23834,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="430" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:19" ht="39">
       <c r="A430" s="2" t="s">
         <v>485</v>
       </c>
@@ -23888,7 +23873,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="431" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:19" ht="39">
       <c r="A431" s="2" t="s">
         <v>485</v>
       </c>
@@ -23927,7 +23912,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="432" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:19" ht="39">
       <c r="A432" s="2" t="s">
         <v>485</v>
       </c>
@@ -23966,7 +23951,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="433" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:19" ht="39">
       <c r="A433" s="2" t="s">
         <v>485</v>
       </c>
@@ -24005,7 +23990,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="434" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:19" ht="39">
       <c r="A434" s="2" t="s">
         <v>485</v>
       </c>
@@ -24044,7 +24029,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="435" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:19" ht="39">
       <c r="A435" s="2" t="s">
         <v>485</v>
       </c>
@@ -24083,7 +24068,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="436" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:19" ht="39">
       <c r="A436" s="2" t="s">
         <v>485</v>
       </c>
@@ -24122,7 +24107,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="437" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:19" ht="39">
       <c r="A437" s="2" t="s">
         <v>485</v>
       </c>
@@ -24161,7 +24146,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="438" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:19" ht="39">
       <c r="A438" s="2" t="s">
         <v>485</v>
       </c>
@@ -24200,7 +24185,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="439" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:19" ht="39">
       <c r="A439" s="2" t="s">
         <v>485</v>
       </c>
@@ -24239,7 +24224,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="440" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:19" ht="39">
       <c r="A440" s="2" t="s">
         <v>485</v>
       </c>
@@ -24278,7 +24263,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="441" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:19" ht="39">
       <c r="A441" s="2" t="s">
         <v>485</v>
       </c>
@@ -24317,7 +24302,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="442" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:19" ht="29.25">
       <c r="A442" s="2" t="s">
         <v>485</v>
       </c>
@@ -24376,7 +24361,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="443" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:19" ht="29.25">
       <c r="A443" s="2" t="s">
         <v>485</v>
       </c>
@@ -24415,7 +24400,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="444" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:19" ht="29.25">
       <c r="A444" s="2" t="s">
         <v>522</v>
       </c>
@@ -24472,7 +24457,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="445" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:19" ht="29.25">
       <c r="A445" s="2" t="s">
         <v>522</v>
       </c>
@@ -24529,7 +24514,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="446" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:19" ht="29.25">
       <c r="A446" s="2" t="s">
         <v>522</v>
       </c>
@@ -24586,7 +24571,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="447" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:19" ht="29.25">
       <c r="A447" s="2" t="s">
         <v>522</v>
       </c>
@@ -24643,7 +24628,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="448" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:19" ht="48.75">
       <c r="A448" s="2" t="s">
         <v>522</v>
       </c>
@@ -24702,7 +24687,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="449" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:19" ht="29.25">
       <c r="A449" s="2" t="s">
         <v>522</v>
       </c>
@@ -24759,7 +24744,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="450" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:19" ht="29.25">
       <c r="A450" s="2" t="s">
         <v>522</v>
       </c>
@@ -24816,7 +24801,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="451" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:19" ht="29.25">
       <c r="A451" s="2" t="s">
         <v>522</v>
       </c>
@@ -24875,7 +24860,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="452" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:19" ht="29.25">
       <c r="A452" s="2" t="s">
         <v>522</v>
       </c>
@@ -24934,7 +24919,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="453" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:19" ht="29.25">
       <c r="A453" s="2" t="s">
         <v>522</v>
       </c>
@@ -24993,7 +24978,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="454" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:19" ht="29.25">
       <c r="A454" s="2" t="s">
         <v>522</v>
       </c>
@@ -25050,7 +25035,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="455" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:19" ht="29.25">
       <c r="A455" s="2" t="s">
         <v>522</v>
       </c>
@@ -25109,7 +25094,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="456" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:19" ht="29.25">
       <c r="A456" s="2" t="s">
         <v>522</v>
       </c>
@@ -25168,7 +25153,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="457" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:19" ht="29.25">
       <c r="A457" s="2" t="s">
         <v>522</v>
       </c>
@@ -25225,7 +25210,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="458" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:19" ht="29.25">
       <c r="A458" s="2" t="s">
         <v>522</v>
       </c>
@@ -25284,7 +25269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="459" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:19" ht="48.75">
       <c r="A459" s="2" t="s">
         <v>522</v>
       </c>
@@ -25343,7 +25328,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="460" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:19" ht="29.25">
       <c r="A460" s="2" t="s">
         <v>522</v>
       </c>
@@ -25402,7 +25387,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="461" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:19" ht="39">
       <c r="A461" s="2" t="s">
         <v>522</v>
       </c>
@@ -25461,7 +25446,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="462" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:19" ht="39">
       <c r="A462" s="2" t="s">
         <v>522</v>
       </c>
@@ -25520,7 +25505,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="463" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:19" ht="29.25">
       <c r="A463" s="2" t="s">
         <v>522</v>
       </c>
@@ -25563,7 +25548,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="464" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:19" ht="29.25">
       <c r="A464" s="2" t="s">
         <v>522</v>
       </c>
@@ -25622,7 +25607,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="465" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:19" ht="29.25">
       <c r="A465" s="2" t="s">
         <v>522</v>
       </c>
@@ -25681,7 +25666,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="466" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:19" ht="29.25">
       <c r="A466" s="2" t="s">
         <v>522</v>
       </c>
@@ -25732,7 +25717,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="467" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:19" ht="39">
       <c r="A467" s="2" t="s">
         <v>522</v>
       </c>
@@ -25769,7 +25754,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="468" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:19" ht="39">
       <c r="A468" s="2" t="s">
         <v>522</v>
       </c>
@@ -25828,7 +25813,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="469" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:19" ht="39">
       <c r="A469" s="2" t="s">
         <v>522</v>
       </c>
@@ -25887,9 +25872,9 @@
         <v>557</v>
       </c>
     </row>
-    <row r="470" spans="1:19" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:19" ht="0" hidden="1" customHeight="1"/>
+    <row r="471" spans="1:19" ht="18" customHeight="1"/>
+    <row r="472" spans="1:19" ht="17.100000000000001" customHeight="1">
       <c r="A472" s="12" t="s">
         <v>560</v>
       </c>

</xml_diff>

<commit_message>
Okno serwisowe 04.07.2023 - aktualizacja excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="18060" windowHeight="7050"/>
   </bookViews>
@@ -1705,13 +1700,13 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 20-06-2023, 09:32</t>
+    <t>Last update: 04-07-2023, 11:49</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$-10809]0.0;\-0.0;0.0"/>
     <numFmt numFmtId="165" formatCode="[$-10809]0.00;\-0.00;0.00"/>
@@ -1720,7 +1715,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1918,14 +1913,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1946,7 +1933,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="0" name="Picture 1"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2009,7 +1996,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2041,10 +2028,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2076,7 +2062,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -2252,15 +2237,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S472"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2272,17 +2257,17 @@
     <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="36" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2341,7 +2326,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="19.5">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2398,7 +2383,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="15">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2455,7 +2440,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -2512,7 +2497,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="15">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -2569,7 +2554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="15">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -2626,7 +2611,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="15">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -2683,7 +2668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -2740,7 +2725,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2797,7 +2782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -2854,7 +2839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2911,7 +2896,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="19.5">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -2968,7 +2953,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="19.5">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -3025,7 +3010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="15">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -3064,7 +3049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="29.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -3123,7 +3108,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="97.5">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -3178,7 +3163,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="97.5">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -3233,7 +3218,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="97.5">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -3288,7 +3273,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="19.5">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -3343,7 +3328,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="29.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -3400,7 +3385,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="29.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -3457,7 +3442,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="29.25">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -3506,7 +3491,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="68.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -3555,7 +3540,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="29.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
@@ -3604,7 +3589,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="29.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -3653,7 +3638,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="29.25">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
@@ -3704,7 +3689,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="39">
       <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
@@ -3761,7 +3746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="39">
       <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
@@ -3818,7 +3803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="39">
       <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
@@ -3875,7 +3860,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="39">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -3932,7 +3917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="19.5">
       <c r="A33" s="2" t="s">
         <v>66</v>
       </c>
@@ -3987,7 +3972,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="29.25">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -4032,7 +4017,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="29.25">
       <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
@@ -4077,7 +4062,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="29.25">
       <c r="A36" s="2" t="s">
         <v>66</v>
       </c>
@@ -4122,7 +4107,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="29.25">
       <c r="A37" s="2" t="s">
         <v>66</v>
       </c>
@@ -4167,7 +4152,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="29.25">
       <c r="A38" s="2" t="s">
         <v>66</v>
       </c>
@@ -4212,7 +4197,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="29.25">
       <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
@@ -4257,7 +4242,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="39">
       <c r="A40" s="2" t="s">
         <v>66</v>
       </c>
@@ -4296,7 +4281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="97.5">
       <c r="A41" s="2" t="s">
         <v>66</v>
       </c>
@@ -4355,7 +4340,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="97.5">
       <c r="A42" s="2" t="s">
         <v>66</v>
       </c>
@@ -4414,7 +4399,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="97.5">
       <c r="A43" s="2" t="s">
         <v>66</v>
       </c>
@@ -4473,7 +4458,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="97.5">
       <c r="A44" s="2" t="s">
         <v>66</v>
       </c>
@@ -4532,7 +4517,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="97.5">
       <c r="A45" s="2" t="s">
         <v>66</v>
       </c>
@@ -4591,7 +4576,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="97.5">
       <c r="A46" s="2" t="s">
         <v>66</v>
       </c>
@@ -4650,7 +4635,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="48.75">
       <c r="A47" s="2" t="s">
         <v>66</v>
       </c>
@@ -4699,7 +4684,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="48.75">
       <c r="A48" s="2" t="s">
         <v>66</v>
       </c>
@@ -4748,7 +4733,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="19.5">
       <c r="A49" s="2" t="s">
         <v>66</v>
       </c>
@@ -4805,7 +4790,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="29.25">
       <c r="A50" s="2" t="s">
         <v>66</v>
       </c>
@@ -4856,7 +4841,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="19.5">
       <c r="A51" s="2" t="s">
         <v>95</v>
       </c>
@@ -4913,7 +4898,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="19.5">
       <c r="A52" s="2" t="s">
         <v>95</v>
       </c>
@@ -4970,7 +4955,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>95</v>
       </c>
@@ -5027,7 +5012,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>95</v>
       </c>
@@ -5084,7 +5069,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>95</v>
       </c>
@@ -5141,7 +5126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>95</v>
       </c>
@@ -5198,7 +5183,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>95</v>
       </c>
@@ -5255,7 +5240,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>95</v>
       </c>
@@ -5312,7 +5297,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="29.25">
       <c r="A59" s="2" t="s">
         <v>95</v>
       </c>
@@ -5369,7 +5354,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>95</v>
       </c>
@@ -5426,7 +5411,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="29.25">
       <c r="A61" s="2" t="s">
         <v>95</v>
       </c>
@@ -5485,7 +5470,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="29.25">
       <c r="A62" s="2" t="s">
         <v>95</v>
       </c>
@@ -5544,7 +5529,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="29.25">
       <c r="A63" s="2" t="s">
         <v>95</v>
       </c>
@@ -5603,7 +5588,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="19.5">
       <c r="A64" s="2" t="s">
         <v>95</v>
       </c>
@@ -5660,7 +5645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="29.25">
       <c r="A65" s="2" t="s">
         <v>95</v>
       </c>
@@ -5719,7 +5704,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="29.25">
       <c r="A66" s="2" t="s">
         <v>95</v>
       </c>
@@ -5778,7 +5763,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="29.25">
       <c r="A67" s="2" t="s">
         <v>95</v>
       </c>
@@ -5837,7 +5822,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="29.25">
       <c r="A68" s="2" t="s">
         <v>95</v>
       </c>
@@ -5894,7 +5879,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="29.25">
       <c r="A69" s="2" t="s">
         <v>95</v>
       </c>
@@ -5951,7 +5936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" ht="29.25">
       <c r="A70" s="2" t="s">
         <v>95</v>
       </c>
@@ -6008,7 +5993,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" ht="29.25">
       <c r="A71" s="2" t="s">
         <v>95</v>
       </c>
@@ -6065,7 +6050,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" ht="19.5">
       <c r="A72" s="2" t="s">
         <v>95</v>
       </c>
@@ -6122,7 +6107,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="19.5">
       <c r="A73" s="2" t="s">
         <v>95</v>
       </c>
@@ -6179,7 +6164,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="19.5">
       <c r="A74" s="2" t="s">
         <v>95</v>
       </c>
@@ -6236,7 +6221,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="19.5">
       <c r="A75" s="2" t="s">
         <v>95</v>
       </c>
@@ -6293,7 +6278,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" ht="29.25">
       <c r="A76" s="2" t="s">
         <v>95</v>
       </c>
@@ -6350,7 +6335,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" ht="29.25">
       <c r="A77" s="2" t="s">
         <v>95</v>
       </c>
@@ -6389,7 +6374,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" ht="19.5">
       <c r="A78" s="2" t="s">
         <v>95</v>
       </c>
@@ -6446,7 +6431,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="19.5">
       <c r="A79" s="2" t="s">
         <v>95</v>
       </c>
@@ -6503,7 +6488,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" ht="19.5">
       <c r="A80" s="2" t="s">
         <v>95</v>
       </c>
@@ -6560,7 +6545,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="19.5">
       <c r="A81" s="2" t="s">
         <v>95</v>
       </c>
@@ -6601,7 +6586,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="29.25">
       <c r="A82" s="2" t="s">
         <v>95</v>
       </c>
@@ -6646,7 +6631,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="29.25">
       <c r="A83" s="2" t="s">
         <v>95</v>
       </c>
@@ -6691,7 +6676,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="19.5">
       <c r="A84" s="2" t="s">
         <v>95</v>
       </c>
@@ -6726,7 +6711,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="29.25">
       <c r="A85" s="2" t="s">
         <v>95</v>
       </c>
@@ -6761,7 +6746,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="19.5">
       <c r="A86" s="2" t="s">
         <v>95</v>
       </c>
@@ -6818,7 +6803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="19.5">
       <c r="A87" s="2" t="s">
         <v>95</v>
       </c>
@@ -6857,7 +6842,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" ht="19.5">
       <c r="A88" s="2" t="s">
         <v>95</v>
       </c>
@@ -6914,7 +6899,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="19.5">
       <c r="A89" s="2" t="s">
         <v>95</v>
       </c>
@@ -6971,7 +6956,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="19.5">
       <c r="A90" s="2" t="s">
         <v>95</v>
       </c>
@@ -7012,7 +6997,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="29.25">
       <c r="A91" s="2" t="s">
         <v>95</v>
       </c>
@@ -7063,7 +7048,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" ht="19.5">
       <c r="A92" s="2" t="s">
         <v>95</v>
       </c>
@@ -7102,7 +7087,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" ht="19.5">
       <c r="A93" s="2" t="s">
         <v>95</v>
       </c>
@@ -7141,7 +7126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" ht="19.5">
       <c r="A94" s="2" t="s">
         <v>95</v>
       </c>
@@ -7180,7 +7165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" ht="19.5">
       <c r="A95" s="2" t="s">
         <v>95</v>
       </c>
@@ -7233,7 +7218,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" ht="48.75">
       <c r="A96" s="2" t="s">
         <v>149</v>
       </c>
@@ -7270,7 +7255,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" ht="48.75">
       <c r="A97" s="2" t="s">
         <v>149</v>
       </c>
@@ -7307,7 +7292,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" ht="48.75">
       <c r="A98" s="2" t="s">
         <v>149</v>
       </c>
@@ -7344,7 +7329,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" ht="48.75">
       <c r="A99" s="2" t="s">
         <v>149</v>
       </c>
@@ -7385,7 +7370,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" ht="48.75">
       <c r="A100" s="2" t="s">
         <v>149</v>
       </c>
@@ -7426,7 +7411,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" ht="48.75">
       <c r="A101" s="2" t="s">
         <v>149</v>
       </c>
@@ -7467,7 +7452,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" ht="48.75">
       <c r="A102" s="2" t="s">
         <v>149</v>
       </c>
@@ -7508,7 +7493,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" ht="48.75">
       <c r="A103" s="2" t="s">
         <v>149</v>
       </c>
@@ -7549,7 +7534,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" ht="48.75">
       <c r="A104" s="2" t="s">
         <v>149</v>
       </c>
@@ -7590,7 +7575,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" ht="29.25">
       <c r="A105" s="2" t="s">
         <v>149</v>
       </c>
@@ -7627,7 +7612,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" ht="19.5">
       <c r="A106" s="2" t="s">
         <v>149</v>
       </c>
@@ -7684,7 +7669,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" ht="19.5">
       <c r="A107" s="2" t="s">
         <v>149</v>
       </c>
@@ -7741,7 +7726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" ht="19.5">
       <c r="A108" s="2" t="s">
         <v>149</v>
       </c>
@@ -7798,7 +7783,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" ht="19.5">
       <c r="A109" s="2" t="s">
         <v>149</v>
       </c>
@@ -7835,7 +7820,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" ht="19.5">
       <c r="A110" s="2" t="s">
         <v>149</v>
       </c>
@@ -7872,7 +7857,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" ht="19.5">
       <c r="A111" s="2" t="s">
         <v>149</v>
       </c>
@@ -7909,7 +7894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" ht="29.25">
       <c r="A112" s="2" t="s">
         <v>149</v>
       </c>
@@ -7954,7 +7939,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" ht="19.5">
       <c r="A113" s="2" t="s">
         <v>149</v>
       </c>
@@ -8001,7 +7986,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" ht="39">
       <c r="A114" s="2" t="s">
         <v>149</v>
       </c>
@@ -8048,7 +8033,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" ht="48.75">
       <c r="A115" s="2" t="s">
         <v>149</v>
       </c>
@@ -8095,7 +8080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" ht="58.5">
       <c r="A116" s="2" t="s">
         <v>149</v>
       </c>
@@ -8142,7 +8127,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" ht="29.25">
       <c r="A117" s="2" t="s">
         <v>149</v>
       </c>
@@ -8189,7 +8174,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" ht="29.25">
       <c r="A118" s="2" t="s">
         <v>149</v>
       </c>
@@ -8234,7 +8219,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" ht="19.5">
       <c r="A119" s="2" t="s">
         <v>149</v>
       </c>
@@ -8281,7 +8266,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" ht="39">
       <c r="A120" s="2" t="s">
         <v>149</v>
       </c>
@@ -8328,7 +8313,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" ht="48.75">
       <c r="A121" s="2" t="s">
         <v>149</v>
       </c>
@@ -8375,7 +8360,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" ht="58.5">
       <c r="A122" s="2" t="s">
         <v>149</v>
       </c>
@@ -8422,7 +8407,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" ht="29.25">
       <c r="A123" s="2" t="s">
         <v>149</v>
       </c>
@@ -8469,7 +8454,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" ht="48.75">
       <c r="A124" s="2" t="s">
         <v>149</v>
       </c>
@@ -8508,7 +8493,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" ht="48.75">
       <c r="A125" s="2" t="s">
         <v>149</v>
       </c>
@@ -8547,7 +8532,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" ht="29.25">
       <c r="A126" s="2" t="s">
         <v>149</v>
       </c>
@@ -8604,7 +8589,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" ht="29.25">
       <c r="A127" s="2" t="s">
         <v>149</v>
       </c>
@@ -8639,7 +8624,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" ht="29.25">
       <c r="A128" s="2" t="s">
         <v>149</v>
       </c>
@@ -8674,7 +8659,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" ht="29.25">
       <c r="A129" s="2" t="s">
         <v>149</v>
       </c>
@@ -8709,7 +8694,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" ht="29.25">
       <c r="A130" s="2" t="s">
         <v>149</v>
       </c>
@@ -8744,7 +8729,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" ht="29.25">
       <c r="A131" s="2" t="s">
         <v>149</v>
       </c>
@@ -8779,7 +8764,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" ht="29.25">
       <c r="A132" s="2" t="s">
         <v>149</v>
       </c>
@@ -8814,7 +8799,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" ht="29.25">
       <c r="A133" s="2" t="s">
         <v>149</v>
       </c>
@@ -8849,7 +8834,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" ht="29.25">
       <c r="A134" s="2" t="s">
         <v>149</v>
       </c>
@@ -8884,7 +8869,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" ht="29.25">
       <c r="A135" s="2" t="s">
         <v>149</v>
       </c>
@@ -8919,7 +8904,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" ht="29.25">
       <c r="A136" s="2" t="s">
         <v>149</v>
       </c>
@@ -8954,7 +8939,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" ht="29.25">
       <c r="A137" s="2" t="s">
         <v>149</v>
       </c>
@@ -8989,7 +8974,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" ht="29.25">
       <c r="A138" s="2" t="s">
         <v>149</v>
       </c>
@@ -9024,7 +9009,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" ht="29.25">
       <c r="A139" s="2" t="s">
         <v>149</v>
       </c>
@@ -9059,7 +9044,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" ht="29.25">
       <c r="A140" s="2" t="s">
         <v>149</v>
       </c>
@@ -9094,7 +9079,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" ht="29.25">
       <c r="A141" s="2" t="s">
         <v>149</v>
       </c>
@@ -9129,7 +9114,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" ht="29.25">
       <c r="A142" s="2" t="s">
         <v>149</v>
       </c>
@@ -9164,7 +9149,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" ht="48.75">
       <c r="A143" s="2" t="s">
         <v>149</v>
       </c>
@@ -9223,7 +9208,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" ht="58.5">
       <c r="A144" s="2" t="s">
         <v>149</v>
       </c>
@@ -9282,7 +9267,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" ht="58.5">
       <c r="A145" s="2" t="s">
         <v>149</v>
       </c>
@@ -9317,7 +9302,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" ht="58.5">
       <c r="A146" s="2" t="s">
         <v>149</v>
       </c>
@@ -9352,7 +9337,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" ht="58.5">
       <c r="A147" s="2" t="s">
         <v>149</v>
       </c>
@@ -9411,7 +9396,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" ht="58.5">
       <c r="A148" s="2" t="s">
         <v>149</v>
       </c>
@@ -9470,7 +9455,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" ht="58.5">
       <c r="A149" s="2" t="s">
         <v>149</v>
       </c>
@@ -9529,7 +9514,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" ht="29.25">
       <c r="A150" s="2" t="s">
         <v>149</v>
       </c>
@@ -9580,7 +9565,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" ht="58.5">
       <c r="A151" s="2" t="s">
         <v>149</v>
       </c>
@@ -9635,7 +9620,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" ht="58.5">
       <c r="A152" s="2" t="s">
         <v>149</v>
       </c>
@@ -9690,7 +9675,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" ht="58.5">
       <c r="A153" s="2" t="s">
         <v>149</v>
       </c>
@@ -9745,7 +9730,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" ht="58.5">
       <c r="A154" s="2" t="s">
         <v>149</v>
       </c>
@@ -9800,7 +9785,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" ht="29.25">
       <c r="A155" s="2" t="s">
         <v>205</v>
       </c>
@@ -9835,7 +9820,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" ht="19.5">
       <c r="A156" s="2" t="s">
         <v>205</v>
       </c>
@@ -9892,7 +9877,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" ht="39">
       <c r="A157" s="2" t="s">
         <v>205</v>
       </c>
@@ -9927,7 +9912,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" ht="39">
       <c r="A158" s="2" t="s">
         <v>205</v>
       </c>
@@ -9962,7 +9947,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" ht="39">
       <c r="A159" s="2" t="s">
         <v>205</v>
       </c>
@@ -9997,7 +9982,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="160" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" ht="39">
       <c r="A160" s="2" t="s">
         <v>205</v>
       </c>
@@ -10032,7 +10017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" ht="39">
       <c r="A161" s="2" t="s">
         <v>205</v>
       </c>
@@ -10067,7 +10052,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" ht="19.5">
       <c r="A162" s="2" t="s">
         <v>205</v>
       </c>
@@ -10102,7 +10087,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:19" ht="19.5">
       <c r="A163" s="2" t="s">
         <v>205</v>
       </c>
@@ -10137,7 +10122,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" ht="19.5">
       <c r="A164" s="2" t="s">
         <v>205</v>
       </c>
@@ -10172,7 +10157,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:19" ht="19.5">
       <c r="A165" s="2" t="s">
         <v>205</v>
       </c>
@@ -10207,7 +10192,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" ht="19.5">
       <c r="A166" s="2" t="s">
         <v>205</v>
       </c>
@@ -10242,7 +10227,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" ht="19.5">
       <c r="A167" s="2" t="s">
         <v>205</v>
       </c>
@@ -10277,7 +10262,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:19" ht="19.5">
       <c r="A168" s="2" t="s">
         <v>205</v>
       </c>
@@ -10312,7 +10297,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" ht="19.5">
       <c r="A169" s="2" t="s">
         <v>205</v>
       </c>
@@ -10347,7 +10332,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:19" ht="29.25">
       <c r="A170" s="2" t="s">
         <v>205</v>
       </c>
@@ -10386,7 +10371,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:19" ht="29.25">
       <c r="A171" s="2" t="s">
         <v>205</v>
       </c>
@@ -10425,7 +10410,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:19" ht="29.25">
       <c r="A172" s="2" t="s">
         <v>205</v>
       </c>
@@ -10482,7 +10467,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:19" ht="29.25">
       <c r="A173" s="2" t="s">
         <v>205</v>
       </c>
@@ -10539,7 +10524,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:19" ht="29.25">
       <c r="A174" s="2" t="s">
         <v>205</v>
       </c>
@@ -10596,7 +10581,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:19" ht="29.25">
       <c r="A175" s="2" t="s">
         <v>205</v>
       </c>
@@ -10653,7 +10638,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:19" ht="29.25">
       <c r="A176" s="2" t="s">
         <v>205</v>
       </c>
@@ -10710,7 +10695,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="177" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:19" ht="19.5">
       <c r="A177" s="2" t="s">
         <v>205</v>
       </c>
@@ -10755,7 +10740,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="178" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:19" ht="39">
       <c r="A178" s="2" t="s">
         <v>205</v>
       </c>
@@ -10800,7 +10785,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:19" ht="19.5">
       <c r="A179" s="2" t="s">
         <v>205</v>
       </c>
@@ -10845,7 +10830,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:19" ht="39">
       <c r="A180" s="2" t="s">
         <v>205</v>
       </c>
@@ -10890,7 +10875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:19" ht="39">
       <c r="A181" s="2" t="s">
         <v>205</v>
       </c>
@@ -10935,7 +10920,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="182" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:19" ht="39">
       <c r="A182" s="2" t="s">
         <v>205</v>
       </c>
@@ -10980,7 +10965,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:19" ht="39">
       <c r="A183" s="2" t="s">
         <v>205</v>
       </c>
@@ -11025,7 +11010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:19" ht="39">
       <c r="A184" s="2" t="s">
         <v>205</v>
       </c>
@@ -11064,7 +11049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:19" ht="39">
       <c r="A185" s="2" t="s">
         <v>205</v>
       </c>
@@ -11103,7 +11088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="186" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:19" ht="39">
       <c r="A186" s="2" t="s">
         <v>205</v>
       </c>
@@ -11142,7 +11127,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:19" ht="39">
       <c r="A187" s="2" t="s">
         <v>205</v>
       </c>
@@ -11181,7 +11166,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:19" ht="39">
       <c r="A188" s="2" t="s">
         <v>205</v>
       </c>
@@ -11220,7 +11205,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:19" ht="39">
       <c r="A189" s="2" t="s">
         <v>205</v>
       </c>
@@ -11259,7 +11244,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:19" ht="39">
       <c r="A190" s="2" t="s">
         <v>205</v>
       </c>
@@ -11298,7 +11283,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:19" ht="39">
       <c r="A191" s="2" t="s">
         <v>205</v>
       </c>
@@ -11337,7 +11322,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:19" ht="39">
       <c r="A192" s="2" t="s">
         <v>205</v>
       </c>
@@ -11376,7 +11361,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="193" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:19" ht="39">
       <c r="A193" s="2" t="s">
         <v>205</v>
       </c>
@@ -11415,7 +11400,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:19" ht="39">
       <c r="A194" s="2" t="s">
         <v>205</v>
       </c>
@@ -11454,7 +11439,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="195" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:19" ht="39">
       <c r="A195" s="2" t="s">
         <v>205</v>
       </c>
@@ -11493,7 +11478,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="196" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:19" ht="19.5">
       <c r="A196" s="2" t="s">
         <v>205</v>
       </c>
@@ -11534,7 +11519,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:19" ht="19.5">
       <c r="A197" s="2" t="s">
         <v>205</v>
       </c>
@@ -11589,7 +11574,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:19" ht="19.5">
       <c r="A198" s="2" t="s">
         <v>205</v>
       </c>
@@ -11644,7 +11629,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:19" ht="19.5">
       <c r="A199" s="2" t="s">
         <v>245</v>
       </c>
@@ -11701,7 +11686,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="200" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:19" ht="29.25">
       <c r="A200" s="2" t="s">
         <v>245</v>
       </c>
@@ -11758,7 +11743,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="201" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:19" ht="19.5">
       <c r="A201" s="2" t="s">
         <v>245</v>
       </c>
@@ -11815,7 +11800,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="202" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:19" ht="19.5">
       <c r="A202" s="2" t="s">
         <v>245</v>
       </c>
@@ -11850,7 +11835,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="203" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:19" ht="19.5">
       <c r="A203" s="2" t="s">
         <v>245</v>
       </c>
@@ -11885,7 +11870,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="204" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:19" ht="29.25">
       <c r="A204" s="2" t="s">
         <v>245</v>
       </c>
@@ -11940,7 +11925,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="205" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:19" ht="19.5">
       <c r="A205" s="2" t="s">
         <v>245</v>
       </c>
@@ -11995,7 +11980,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="206" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:19" ht="19.5">
       <c r="A206" s="2" t="s">
         <v>245</v>
       </c>
@@ -12040,7 +12025,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="207" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:19" ht="29.25">
       <c r="A207" s="2" t="s">
         <v>245</v>
       </c>
@@ -12099,7 +12084,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="208" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:19" ht="29.25">
       <c r="A208" s="2" t="s">
         <v>245</v>
       </c>
@@ -12150,7 +12135,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="209" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:19" ht="39">
       <c r="A209" s="2" t="s">
         <v>245</v>
       </c>
@@ -12207,7 +12192,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="210" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:19" ht="19.5">
       <c r="A210" s="2" t="s">
         <v>266</v>
       </c>
@@ -12242,7 +12227,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="211" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:19" ht="19.5">
       <c r="A211" s="2" t="s">
         <v>266</v>
       </c>
@@ -12299,7 +12284,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="212" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:19" ht="29.25">
       <c r="A212" s="2" t="s">
         <v>266</v>
       </c>
@@ -12354,7 +12339,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="213" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:19" ht="29.25">
       <c r="A213" s="2" t="s">
         <v>266</v>
       </c>
@@ -12405,7 +12390,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="214" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:19" ht="29.25">
       <c r="A214" s="2" t="s">
         <v>272</v>
       </c>
@@ -12462,7 +12447,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:19" ht="29.25">
       <c r="A215" s="2" t="s">
         <v>272</v>
       </c>
@@ -12519,7 +12504,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="216" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:19" ht="29.25">
       <c r="A216" s="2" t="s">
         <v>272</v>
       </c>
@@ -12558,7 +12543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="217" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:19" ht="29.25">
       <c r="A217" s="2" t="s">
         <v>272</v>
       </c>
@@ -12597,7 +12582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="218" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:19" ht="29.25">
       <c r="A218" s="2" t="s">
         <v>272</v>
       </c>
@@ -12636,7 +12621,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="219" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:19" ht="29.25">
       <c r="A219" s="2" t="s">
         <v>272</v>
       </c>
@@ -12693,7 +12678,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="220" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:19" ht="29.25">
       <c r="A220" s="2" t="s">
         <v>272</v>
       </c>
@@ -12750,7 +12735,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="221" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:19" ht="29.25">
       <c r="A221" s="2" t="s">
         <v>272</v>
       </c>
@@ -12807,7 +12792,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="222" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:19" ht="29.25">
       <c r="A222" s="2" t="s">
         <v>272</v>
       </c>
@@ -12852,7 +12837,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="223" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:19" ht="29.25">
       <c r="A223" s="2" t="s">
         <v>272</v>
       </c>
@@ -12897,7 +12882,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="224" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:19" ht="29.25">
       <c r="A224" s="2" t="s">
         <v>272</v>
       </c>
@@ -12942,7 +12927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="225" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:19" ht="29.25">
       <c r="A225" s="2" t="s">
         <v>272</v>
       </c>
@@ -12987,7 +12972,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="226" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:19" ht="29.25">
       <c r="A226" s="2" t="s">
         <v>272</v>
       </c>
@@ -13032,7 +13017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="227" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:19" ht="29.25">
       <c r="A227" s="2" t="s">
         <v>272</v>
       </c>
@@ -13077,7 +13062,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="228" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:19" ht="29.25">
       <c r="A228" s="2" t="s">
         <v>272</v>
       </c>
@@ -13122,7 +13107,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="229" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:19" ht="29.25">
       <c r="A229" s="2" t="s">
         <v>272</v>
       </c>
@@ -13167,7 +13152,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="230" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:19" ht="39">
       <c r="A230" s="2" t="s">
         <v>272</v>
       </c>
@@ -13212,7 +13197,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="231" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:19" ht="29.25">
       <c r="A231" s="2" t="s">
         <v>272</v>
       </c>
@@ -13257,7 +13242,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="232" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:19" ht="39">
       <c r="A232" s="2" t="s">
         <v>272</v>
       </c>
@@ -13302,7 +13287,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="233" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:19" ht="29.25">
       <c r="A233" s="2" t="s">
         <v>272</v>
       </c>
@@ -13347,7 +13332,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="234" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:19" ht="29.25">
       <c r="A234" s="2" t="s">
         <v>272</v>
       </c>
@@ -13392,7 +13377,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="235" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:19" ht="29.25">
       <c r="A235" s="2" t="s">
         <v>272</v>
       </c>
@@ -13437,7 +13422,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="236" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:19" ht="29.25">
       <c r="A236" s="2" t="s">
         <v>272</v>
       </c>
@@ -13482,7 +13467,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="237" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:19" ht="29.25">
       <c r="A237" s="2" t="s">
         <v>272</v>
       </c>
@@ -13527,7 +13512,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="238" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:19" ht="29.25">
       <c r="A238" s="2" t="s">
         <v>272</v>
       </c>
@@ -13572,7 +13557,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:19" ht="29.25">
       <c r="A239" s="2" t="s">
         <v>272</v>
       </c>
@@ -13617,7 +13602,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="240" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:19" ht="29.25">
       <c r="A240" s="2" t="s">
         <v>272</v>
       </c>
@@ -13662,7 +13647,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="241" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:19" ht="29.25">
       <c r="A241" s="2" t="s">
         <v>272</v>
       </c>
@@ -13721,7 +13706,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="242" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:19" ht="29.25">
       <c r="A242" s="2" t="s">
         <v>272</v>
       </c>
@@ -13780,7 +13765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="243" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:19" ht="29.25">
       <c r="A243" s="2" t="s">
         <v>272</v>
       </c>
@@ -13839,7 +13824,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="244" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:19" ht="29.25">
       <c r="A244" s="2" t="s">
         <v>272</v>
       </c>
@@ -13898,7 +13883,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="245" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:19" ht="29.25">
       <c r="A245" s="2" t="s">
         <v>272</v>
       </c>
@@ -13957,7 +13942,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="246" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:19" ht="29.25">
       <c r="A246" s="2" t="s">
         <v>272</v>
       </c>
@@ -14016,7 +14001,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="247" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:19" ht="29.25">
       <c r="A247" s="2" t="s">
         <v>272</v>
       </c>
@@ -14075,7 +14060,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="248" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:19" ht="29.25">
       <c r="A248" s="2" t="s">
         <v>272</v>
       </c>
@@ -14134,7 +14119,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="249" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:19" ht="29.25">
       <c r="A249" s="2" t="s">
         <v>272</v>
       </c>
@@ -14193,7 +14178,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="250" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:19" ht="29.25">
       <c r="A250" s="2" t="s">
         <v>272</v>
       </c>
@@ -14250,7 +14235,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="251" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:19" ht="29.25">
       <c r="A251" s="2" t="s">
         <v>272</v>
       </c>
@@ -14307,7 +14292,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="252" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:19" ht="29.25">
       <c r="A252" s="2" t="s">
         <v>272</v>
       </c>
@@ -14364,7 +14349,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="253" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:19" ht="39">
       <c r="A253" s="2" t="s">
         <v>272</v>
       </c>
@@ -14405,7 +14390,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="254" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:19" ht="39">
       <c r="A254" s="2" t="s">
         <v>272</v>
       </c>
@@ -14446,7 +14431,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="255" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:19" ht="39">
       <c r="A255" s="2" t="s">
         <v>272</v>
       </c>
@@ -14487,7 +14472,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="256" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:19" ht="29.25">
       <c r="A256" s="2" t="s">
         <v>272</v>
       </c>
@@ -14544,7 +14529,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="257" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:19" ht="48.75">
       <c r="A257" s="2" t="s">
         <v>272</v>
       </c>
@@ -14601,7 +14586,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="258" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:19" ht="29.25">
       <c r="A258" s="2" t="s">
         <v>272</v>
       </c>
@@ -14636,7 +14621,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="259" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:19" ht="29.25">
       <c r="A259" s="2" t="s">
         <v>272</v>
       </c>
@@ -14671,7 +14656,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="260" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:19" ht="29.25">
       <c r="A260" s="2" t="s">
         <v>272</v>
       </c>
@@ -14706,7 +14691,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="261" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:19" ht="29.25">
       <c r="A261" s="2" t="s">
         <v>272</v>
       </c>
@@ -14741,7 +14726,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="262" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:19" ht="29.25">
       <c r="A262" s="2" t="s">
         <v>272</v>
       </c>
@@ -14776,7 +14761,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="263" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:19" ht="29.25">
       <c r="A263" s="2" t="s">
         <v>272</v>
       </c>
@@ -14811,7 +14796,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="264" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:19" ht="29.25">
       <c r="A264" s="2" t="s">
         <v>272</v>
       </c>
@@ -14846,7 +14831,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="265" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:19" ht="29.25">
       <c r="A265" s="2" t="s">
         <v>272</v>
       </c>
@@ -14881,7 +14866,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="266" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:19" ht="29.25">
       <c r="A266" s="2" t="s">
         <v>272</v>
       </c>
@@ -14932,7 +14917,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="267" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:19" ht="29.25">
       <c r="A267" s="2" t="s">
         <v>318</v>
       </c>
@@ -14989,7 +14974,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="268" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:19" ht="29.25">
       <c r="A268" s="2" t="s">
         <v>318</v>
       </c>
@@ -15046,7 +15031,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="269" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:19" ht="29.25">
       <c r="A269" s="2" t="s">
         <v>318</v>
       </c>
@@ -15103,7 +15088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="270" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:19" ht="29.25">
       <c r="A270" s="2" t="s">
         <v>318</v>
       </c>
@@ -15160,7 +15145,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="271" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:19" ht="29.25">
       <c r="A271" s="2" t="s">
         <v>318</v>
       </c>
@@ -15217,7 +15202,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="272" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:19" ht="29.25">
       <c r="A272" s="2" t="s">
         <v>318</v>
       </c>
@@ -15274,7 +15259,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="273" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:19" ht="29.25">
       <c r="A273" s="2" t="s">
         <v>318</v>
       </c>
@@ -15331,7 +15316,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="274" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:19" ht="29.25">
       <c r="A274" s="2" t="s">
         <v>318</v>
       </c>
@@ -15388,7 +15373,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="275" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:19" ht="29.25">
       <c r="A275" s="2" t="s">
         <v>318</v>
       </c>
@@ -15445,7 +15430,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="276" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:19" ht="29.25">
       <c r="A276" s="2" t="s">
         <v>318</v>
       </c>
@@ -15502,7 +15487,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="277" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:19" ht="29.25">
       <c r="A277" s="2" t="s">
         <v>318</v>
       </c>
@@ -15559,7 +15544,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="278" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:19" ht="29.25">
       <c r="A278" s="2" t="s">
         <v>318</v>
       </c>
@@ -15616,7 +15601,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="279" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:19" ht="29.25">
       <c r="A279" s="2" t="s">
         <v>318</v>
       </c>
@@ -15673,7 +15658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="280" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:19" ht="29.25">
       <c r="A280" s="2" t="s">
         <v>318</v>
       </c>
@@ -15730,7 +15715,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="281" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:19" ht="29.25">
       <c r="A281" s="2" t="s">
         <v>318</v>
       </c>
@@ -15787,7 +15772,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="282" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:19" ht="29.25">
       <c r="A282" s="2" t="s">
         <v>318</v>
       </c>
@@ -15844,7 +15829,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="283" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:19" ht="29.25">
       <c r="A283" s="2" t="s">
         <v>318</v>
       </c>
@@ -15901,7 +15886,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="284" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:19" ht="29.25">
       <c r="A284" s="2" t="s">
         <v>318</v>
       </c>
@@ -15958,7 +15943,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="285" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:19" ht="29.25">
       <c r="A285" s="2" t="s">
         <v>318</v>
       </c>
@@ -16015,7 +16000,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="286" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:19" ht="29.25">
       <c r="A286" s="2" t="s">
         <v>318</v>
       </c>
@@ -16072,7 +16057,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="287" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:19" ht="29.25">
       <c r="A287" s="2" t="s">
         <v>318</v>
       </c>
@@ -16123,7 +16108,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="288" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:19" ht="29.25">
       <c r="A288" s="2" t="s">
         <v>318</v>
       </c>
@@ -16180,7 +16165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="289" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:19" ht="29.25">
       <c r="A289" s="2" t="s">
         <v>318</v>
       </c>
@@ -16237,7 +16222,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="290" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:19" ht="29.25">
       <c r="A290" s="2" t="s">
         <v>318</v>
       </c>
@@ -16288,7 +16273,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="291" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:19" ht="29.25">
       <c r="A291" s="2" t="s">
         <v>318</v>
       </c>
@@ -16341,7 +16326,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="292" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:19" ht="39">
       <c r="A292" s="2" t="s">
         <v>318</v>
       </c>
@@ -16390,7 +16375,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="293" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:19" ht="39">
       <c r="A293" s="2" t="s">
         <v>318</v>
       </c>
@@ -16439,7 +16424,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="294" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:19" ht="19.5">
       <c r="A294" s="2" t="s">
         <v>350</v>
       </c>
@@ -16496,7 +16481,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="295" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:19" ht="68.25">
       <c r="A295" s="2" t="s">
         <v>350</v>
       </c>
@@ -16553,7 +16538,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="296" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:19" ht="19.5">
       <c r="A296" s="2" t="s">
         <v>350</v>
       </c>
@@ -16610,7 +16595,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="297" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:19" ht="19.5">
       <c r="A297" s="2" t="s">
         <v>350</v>
       </c>
@@ -16667,7 +16652,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="298" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:19" ht="19.5">
       <c r="A298" s="2" t="s">
         <v>350</v>
       </c>
@@ -16724,7 +16709,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="299" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:19" ht="19.5">
       <c r="A299" s="2" t="s">
         <v>350</v>
       </c>
@@ -16781,7 +16766,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="300" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:19" ht="19.5">
       <c r="A300" s="2" t="s">
         <v>350</v>
       </c>
@@ -16838,7 +16823,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="301" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:19" ht="19.5">
       <c r="A301" s="2" t="s">
         <v>350</v>
       </c>
@@ -16895,7 +16880,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="302" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:19" ht="19.5">
       <c r="A302" s="2" t="s">
         <v>350</v>
       </c>
@@ -16952,7 +16937,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="303" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:19" ht="19.5">
       <c r="A303" s="2" t="s">
         <v>350</v>
       </c>
@@ -17009,7 +16994,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="304" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:19" ht="19.5">
       <c r="A304" s="2" t="s">
         <v>350</v>
       </c>
@@ -17066,7 +17051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="305" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:19" ht="19.5">
       <c r="A305" s="2" t="s">
         <v>350</v>
       </c>
@@ -17105,7 +17090,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="306" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:19" ht="19.5">
       <c r="A306" s="2" t="s">
         <v>350</v>
       </c>
@@ -17162,7 +17147,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="307" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:19" ht="39">
       <c r="A307" s="2" t="s">
         <v>350</v>
       </c>
@@ -17219,7 +17204,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="308" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:19" ht="48.75">
       <c r="A308" s="2" t="s">
         <v>350</v>
       </c>
@@ -17276,7 +17261,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="309" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:19" ht="39">
       <c r="A309" s="2" t="s">
         <v>350</v>
       </c>
@@ -17333,7 +17318,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="310" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:19" ht="39">
       <c r="A310" s="2" t="s">
         <v>350</v>
       </c>
@@ -17390,7 +17375,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="311" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:19" ht="29.25">
       <c r="A311" s="2" t="s">
         <v>350</v>
       </c>
@@ -17447,7 +17432,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="312" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:19" ht="39">
       <c r="A312" s="2" t="s">
         <v>350</v>
       </c>
@@ -17504,7 +17489,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="313" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:19" ht="29.25">
       <c r="A313" s="2" t="s">
         <v>350</v>
       </c>
@@ -17561,7 +17546,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="314" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:19" ht="29.25">
       <c r="A314" s="2" t="s">
         <v>350</v>
       </c>
@@ -17618,7 +17603,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="315" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:19" ht="39">
       <c r="A315" s="2" t="s">
         <v>350</v>
       </c>
@@ -17675,7 +17660,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="316" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:19" ht="29.25">
       <c r="A316" s="2" t="s">
         <v>350</v>
       </c>
@@ -17732,7 +17717,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="317" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:19" ht="39">
       <c r="A317" s="2" t="s">
         <v>350</v>
       </c>
@@ -17789,7 +17774,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="318" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:19" ht="29.25">
       <c r="A318" s="2" t="s">
         <v>350</v>
       </c>
@@ -17846,7 +17831,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="319" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:19" ht="29.25">
       <c r="A319" s="2" t="s">
         <v>350</v>
       </c>
@@ -17905,7 +17890,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="320" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:19" ht="39">
       <c r="A320" s="2" t="s">
         <v>350</v>
       </c>
@@ -17964,7 +17949,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="321" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:19" ht="39">
       <c r="A321" s="2" t="s">
         <v>350</v>
       </c>
@@ -18023,7 +18008,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="322" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:19" ht="68.25">
       <c r="A322" s="2" t="s">
         <v>350</v>
       </c>
@@ -18082,7 +18067,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="323" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:19" ht="58.5">
       <c r="A323" s="2" t="s">
         <v>350</v>
       </c>
@@ -18141,7 +18126,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="324" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:19" ht="68.25">
       <c r="A324" s="2" t="s">
         <v>350</v>
       </c>
@@ -18200,7 +18185,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="325" spans="1:19" ht="72" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:19" ht="68.25">
       <c r="A325" s="2" t="s">
         <v>350</v>
       </c>
@@ -18259,7 +18244,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="326" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:19" ht="39">
       <c r="A326" s="2" t="s">
         <v>350</v>
       </c>
@@ -18316,7 +18301,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="327" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:19" ht="68.25">
       <c r="A327" s="2" t="s">
         <v>350</v>
       </c>
@@ -18373,7 +18358,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="328" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:19" ht="58.5">
       <c r="A328" s="2" t="s">
         <v>350</v>
       </c>
@@ -18430,7 +18415,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="329" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:19" ht="68.25">
       <c r="A329" s="2" t="s">
         <v>350</v>
       </c>
@@ -18487,7 +18472,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="330" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:19" ht="68.25">
       <c r="A330" s="2" t="s">
         <v>350</v>
       </c>
@@ -18544,7 +18529,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="331" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:19" ht="29.25">
       <c r="A331" s="2" t="s">
         <v>391</v>
       </c>
@@ -18599,7 +18584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="332" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:19" ht="29.25">
       <c r="A332" s="2" t="s">
         <v>391</v>
       </c>
@@ -18654,7 +18639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="333" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:19" ht="29.25">
       <c r="A333" s="2" t="s">
         <v>391</v>
       </c>
@@ -18709,7 +18694,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="334" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:19" ht="29.25">
       <c r="A334" s="2" t="s">
         <v>391</v>
       </c>
@@ -18766,7 +18751,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="335" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:19" ht="29.25">
       <c r="A335" s="2" t="s">
         <v>391</v>
       </c>
@@ -18823,7 +18808,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="336" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:19" ht="29.25">
       <c r="A336" s="2" t="s">
         <v>391</v>
       </c>
@@ -18880,7 +18865,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="337" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:19" ht="29.25">
       <c r="A337" s="2" t="s">
         <v>391</v>
       </c>
@@ -18937,7 +18922,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="338" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:19" ht="29.25">
       <c r="A338" s="2" t="s">
         <v>391</v>
       </c>
@@ -18994,7 +18979,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="339" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:19" ht="29.25">
       <c r="A339" s="2" t="s">
         <v>391</v>
       </c>
@@ -19051,7 +19036,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="340" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:19" ht="29.25">
       <c r="A340" s="2" t="s">
         <v>391</v>
       </c>
@@ -19108,7 +19093,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="341" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:19" ht="29.25">
       <c r="A341" s="2" t="s">
         <v>391</v>
       </c>
@@ -19165,7 +19150,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="342" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:19" ht="29.25">
       <c r="A342" s="2" t="s">
         <v>391</v>
       </c>
@@ -19222,7 +19207,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="343" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:19" ht="29.25">
       <c r="A343" s="2" t="s">
         <v>391</v>
       </c>
@@ -19279,7 +19264,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="344" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:19" ht="29.25">
       <c r="A344" s="2" t="s">
         <v>391</v>
       </c>
@@ -19336,7 +19321,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="345" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:19" ht="29.25">
       <c r="A345" s="2" t="s">
         <v>391</v>
       </c>
@@ -19393,7 +19378,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="346" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:19" ht="29.25">
       <c r="A346" s="2" t="s">
         <v>391</v>
       </c>
@@ -19450,7 +19435,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="347" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:19" ht="29.25">
       <c r="A347" s="2" t="s">
         <v>391</v>
       </c>
@@ -19507,7 +19492,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="348" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:19" ht="29.25">
       <c r="A348" s="2" t="s">
         <v>391</v>
       </c>
@@ -19564,7 +19549,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="349" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:19" ht="29.25">
       <c r="A349" s="2" t="s">
         <v>391</v>
       </c>
@@ -19621,7 +19606,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="350" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:19" ht="29.25">
       <c r="A350" s="2" t="s">
         <v>391</v>
       </c>
@@ -19678,7 +19663,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="351" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:19" ht="29.25">
       <c r="A351" s="2" t="s">
         <v>391</v>
       </c>
@@ -19735,7 +19720,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="352" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:19" ht="29.25">
       <c r="A352" s="2" t="s">
         <v>391</v>
       </c>
@@ -19792,7 +19777,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="353" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:19" ht="29.25">
       <c r="A353" s="2" t="s">
         <v>391</v>
       </c>
@@ -19849,7 +19834,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="354" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:19" ht="29.25">
       <c r="A354" s="2" t="s">
         <v>391</v>
       </c>
@@ -19906,7 +19891,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="355" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:19" ht="29.25">
       <c r="A355" s="2" t="s">
         <v>391</v>
       </c>
@@ -19963,7 +19948,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="356" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:19" ht="29.25">
       <c r="A356" s="2" t="s">
         <v>391</v>
       </c>
@@ -20020,7 +20005,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="357" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:19" ht="29.25">
       <c r="A357" s="2" t="s">
         <v>391</v>
       </c>
@@ -20077,7 +20062,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="358" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:19" ht="29.25">
       <c r="A358" s="2" t="s">
         <v>391</v>
       </c>
@@ -20132,7 +20117,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="359" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:19" ht="29.25">
       <c r="A359" s="2" t="s">
         <v>391</v>
       </c>
@@ -20189,7 +20174,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="360" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:19" ht="29.25">
       <c r="A360" s="2" t="s">
         <v>391</v>
       </c>
@@ -20246,7 +20231,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="361" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:19" ht="29.25">
       <c r="A361" s="2" t="s">
         <v>391</v>
       </c>
@@ -20303,7 +20288,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="362" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:19" ht="29.25">
       <c r="A362" s="2" t="s">
         <v>391</v>
       </c>
@@ -20360,7 +20345,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="363" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:19" ht="29.25">
       <c r="A363" s="2" t="s">
         <v>391</v>
       </c>
@@ -20417,7 +20402,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="364" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:19" ht="39">
       <c r="A364" s="2" t="s">
         <v>391</v>
       </c>
@@ -20474,7 +20459,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="365" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:19" ht="39">
       <c r="A365" s="2" t="s">
         <v>391</v>
       </c>
@@ -20531,7 +20516,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="366" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:19" ht="39">
       <c r="A366" s="2" t="s">
         <v>391</v>
       </c>
@@ -20588,7 +20573,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="367" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:19" ht="39">
       <c r="A367" s="2" t="s">
         <v>391</v>
       </c>
@@ -20645,7 +20630,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="368" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:19" ht="39">
       <c r="A368" s="2" t="s">
         <v>391</v>
       </c>
@@ -20702,7 +20687,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="369" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:19" ht="39">
       <c r="A369" s="2" t="s">
         <v>391</v>
       </c>
@@ -20759,7 +20744,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="370" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:19" ht="39">
       <c r="A370" s="2" t="s">
         <v>391</v>
       </c>
@@ -20816,7 +20801,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="371" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:19" ht="39">
       <c r="A371" s="2" t="s">
         <v>391</v>
       </c>
@@ -20873,7 +20858,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="372" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:19" ht="39">
       <c r="A372" s="2" t="s">
         <v>424</v>
       </c>
@@ -20930,7 +20915,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="373" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:19" ht="39">
       <c r="A373" s="2" t="s">
         <v>424</v>
       </c>
@@ -20987,7 +20972,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="374" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:19" ht="39">
       <c r="A374" s="2" t="s">
         <v>424</v>
       </c>
@@ -21044,7 +21029,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="375" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:19" ht="48.75">
       <c r="A375" s="2" t="s">
         <v>424</v>
       </c>
@@ -21103,7 +21088,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="376" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:19" ht="39">
       <c r="A376" s="2" t="s">
         <v>424</v>
       </c>
@@ -21148,7 +21133,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="377" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:19" ht="39">
       <c r="A377" s="2" t="s">
         <v>424</v>
       </c>
@@ -21193,7 +21178,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="378" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:19" ht="39">
       <c r="A378" s="2" t="s">
         <v>424</v>
       </c>
@@ -21238,7 +21223,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="379" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:19" ht="39">
       <c r="A379" s="2" t="s">
         <v>424</v>
       </c>
@@ -21291,7 +21276,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="380" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:19" ht="39">
       <c r="A380" s="2" t="s">
         <v>424</v>
       </c>
@@ -21336,7 +21321,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="381" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:19" ht="39">
       <c r="A381" s="2" t="s">
         <v>424</v>
       </c>
@@ -21395,7 +21380,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="382" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:19" ht="48.75">
       <c r="A382" s="2" t="s">
         <v>424</v>
       </c>
@@ -21454,7 +21439,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="383" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:19" ht="29.25">
       <c r="A383" s="2" t="s">
         <v>444</v>
       </c>
@@ -21511,7 +21496,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="384" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:19" ht="29.25">
       <c r="A384" s="2" t="s">
         <v>444</v>
       </c>
@@ -21568,7 +21553,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="385" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:19" ht="39">
       <c r="A385" s="2" t="s">
         <v>444</v>
       </c>
@@ -21627,7 +21612,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="386" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:19" ht="39">
       <c r="A386" s="2" t="s">
         <v>444</v>
       </c>
@@ -21682,7 +21667,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="387" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:19" ht="48.75">
       <c r="A387" s="2" t="s">
         <v>444</v>
       </c>
@@ -21741,7 +21726,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="388" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:19" ht="29.25">
       <c r="A388" s="2" t="s">
         <v>444</v>
       </c>
@@ -21792,7 +21777,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="389" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:19" ht="58.5">
       <c r="A389" s="2" t="s">
         <v>454</v>
       </c>
@@ -21851,7 +21836,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="390" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:19" ht="39">
       <c r="A390" s="2" t="s">
         <v>454</v>
       </c>
@@ -21910,7 +21895,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="391" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:19" ht="48.75">
       <c r="A391" s="2" t="s">
         <v>454</v>
       </c>
@@ -21969,7 +21954,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="392" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:19" ht="48.75">
       <c r="A392" s="2" t="s">
         <v>454</v>
       </c>
@@ -22028,7 +22013,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="393" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:19" ht="58.5">
       <c r="A393" s="2" t="s">
         <v>454</v>
       </c>
@@ -22085,7 +22070,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="394" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:19" ht="19.5">
       <c r="A394" s="2" t="s">
         <v>464</v>
       </c>
@@ -22142,7 +22127,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="395" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:19" ht="19.5">
       <c r="A395" s="2" t="s">
         <v>464</v>
       </c>
@@ -22199,7 +22184,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="396" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:19" ht="39">
       <c r="A396" s="2" t="s">
         <v>464</v>
       </c>
@@ -22256,7 +22241,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="397" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:19" ht="19.5">
       <c r="A397" s="2" t="s">
         <v>464</v>
       </c>
@@ -22295,7 +22280,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="398" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:19" ht="19.5">
       <c r="A398" s="2" t="s">
         <v>464</v>
       </c>
@@ -22328,7 +22313,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="399" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:19" ht="19.5">
       <c r="A399" s="2" t="s">
         <v>464</v>
       </c>
@@ -22361,7 +22346,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="400" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:19" ht="19.5">
       <c r="A400" s="2" t="s">
         <v>464</v>
       </c>
@@ -22394,7 +22379,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="401" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:19" ht="19.5">
       <c r="A401" s="2" t="s">
         <v>464</v>
       </c>
@@ -22433,7 +22418,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="402" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:19" ht="19.5">
       <c r="A402" s="2" t="s">
         <v>464</v>
       </c>
@@ -22472,7 +22457,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="403" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:19" ht="19.5">
       <c r="A403" s="2" t="s">
         <v>464</v>
       </c>
@@ -22511,7 +22496,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="404" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:19" ht="29.25">
       <c r="A404" s="2" t="s">
         <v>464</v>
       </c>
@@ -22570,7 +22555,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="405" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:19" ht="19.5">
       <c r="A405" s="2" t="s">
         <v>464</v>
       </c>
@@ -22627,7 +22612,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="406" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:19" ht="29.25">
       <c r="A406" s="2" t="s">
         <v>464</v>
       </c>
@@ -22686,7 +22671,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="407" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:19" ht="29.25">
       <c r="A407" s="2" t="s">
         <v>464</v>
       </c>
@@ -22737,7 +22722,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="408" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:19" ht="29.25">
       <c r="A408" s="2" t="s">
         <v>464</v>
       </c>
@@ -22788,7 +22773,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="409" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:19" ht="19.5">
       <c r="A409" s="2" t="s">
         <v>464</v>
       </c>
@@ -22845,7 +22830,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="410" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:19" ht="29.25">
       <c r="A410" s="2" t="s">
         <v>485</v>
       </c>
@@ -22902,7 +22887,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="411" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:19" ht="29.25">
       <c r="A411" s="2" t="s">
         <v>485</v>
       </c>
@@ -22961,7 +22946,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="412" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:19" ht="29.25">
       <c r="A412" s="2" t="s">
         <v>485</v>
       </c>
@@ -23004,7 +22989,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="413" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:19" ht="29.25">
       <c r="A413" s="2" t="s">
         <v>485</v>
       </c>
@@ -23057,7 +23042,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="414" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:19" ht="29.25">
       <c r="A414" s="2" t="s">
         <v>485</v>
       </c>
@@ -23102,7 +23087,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="415" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:19" ht="29.25">
       <c r="A415" s="2" t="s">
         <v>485</v>
       </c>
@@ -23147,7 +23132,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="416" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:19" ht="29.25">
       <c r="A416" s="2" t="s">
         <v>485</v>
       </c>
@@ -23192,7 +23177,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="417" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:19" ht="29.25">
       <c r="A417" s="2" t="s">
         <v>485</v>
       </c>
@@ -23237,7 +23222,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="418" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:19" ht="29.25">
       <c r="A418" s="2" t="s">
         <v>485</v>
       </c>
@@ -23282,7 +23267,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="419" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:19" ht="29.25">
       <c r="A419" s="2" t="s">
         <v>485</v>
       </c>
@@ -23327,7 +23312,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="420" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:19" ht="39">
       <c r="A420" s="2" t="s">
         <v>485</v>
       </c>
@@ -23372,7 +23357,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="421" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:19" ht="48.75">
       <c r="A421" s="2" t="s">
         <v>485</v>
       </c>
@@ -23417,7 +23402,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="422" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:19" ht="39">
       <c r="A422" s="2" t="s">
         <v>485</v>
       </c>
@@ -23462,7 +23447,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="423" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:19" ht="39">
       <c r="A423" s="2" t="s">
         <v>485</v>
       </c>
@@ -23507,7 +23492,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="424" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:19" ht="29.25">
       <c r="A424" s="2" t="s">
         <v>485</v>
       </c>
@@ -23564,7 +23549,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="425" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:19" ht="29.25">
       <c r="A425" s="2" t="s">
         <v>485</v>
       </c>
@@ -23621,7 +23606,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="426" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:19" ht="29.25">
       <c r="A426" s="2" t="s">
         <v>485</v>
       </c>
@@ -23678,7 +23663,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="427" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:19" ht="29.25">
       <c r="A427" s="2" t="s">
         <v>485</v>
       </c>
@@ -23735,7 +23720,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="428" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:19" ht="29.25">
       <c r="A428" s="2" t="s">
         <v>485</v>
       </c>
@@ -23792,7 +23777,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="429" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:19" ht="29.25">
       <c r="A429" s="2" t="s">
         <v>485</v>
       </c>
@@ -23849,7 +23834,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="430" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:19" ht="39">
       <c r="A430" s="2" t="s">
         <v>485</v>
       </c>
@@ -23888,7 +23873,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="431" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:19" ht="39">
       <c r="A431" s="2" t="s">
         <v>485</v>
       </c>
@@ -23927,7 +23912,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="432" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:19" ht="39">
       <c r="A432" s="2" t="s">
         <v>485</v>
       </c>
@@ -23966,7 +23951,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="433" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:19" ht="39">
       <c r="A433" s="2" t="s">
         <v>485</v>
       </c>
@@ -24005,7 +23990,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="434" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:19" ht="39">
       <c r="A434" s="2" t="s">
         <v>485</v>
       </c>
@@ -24044,7 +24029,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="435" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:19" ht="39">
       <c r="A435" s="2" t="s">
         <v>485</v>
       </c>
@@ -24083,7 +24068,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="436" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:19" ht="39">
       <c r="A436" s="2" t="s">
         <v>485</v>
       </c>
@@ -24122,7 +24107,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="437" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:19" ht="39">
       <c r="A437" s="2" t="s">
         <v>485</v>
       </c>
@@ -24161,7 +24146,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="438" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:19" ht="39">
       <c r="A438" s="2" t="s">
         <v>485</v>
       </c>
@@ -24200,7 +24185,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="439" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:19" ht="39">
       <c r="A439" s="2" t="s">
         <v>485</v>
       </c>
@@ -24239,7 +24224,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="440" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:19" ht="39">
       <c r="A440" s="2" t="s">
         <v>485</v>
       </c>
@@ -24278,7 +24263,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="441" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:19" ht="39">
       <c r="A441" s="2" t="s">
         <v>485</v>
       </c>
@@ -24317,7 +24302,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="442" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:19" ht="29.25">
       <c r="A442" s="2" t="s">
         <v>485</v>
       </c>
@@ -24376,7 +24361,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="443" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:19" ht="29.25">
       <c r="A443" s="2" t="s">
         <v>485</v>
       </c>
@@ -24415,7 +24400,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="444" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:19" ht="29.25">
       <c r="A444" s="2" t="s">
         <v>522</v>
       </c>
@@ -24472,7 +24457,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="445" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:19" ht="29.25">
       <c r="A445" s="2" t="s">
         <v>522</v>
       </c>
@@ -24529,7 +24514,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="446" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:19" ht="29.25">
       <c r="A446" s="2" t="s">
         <v>522</v>
       </c>
@@ -24586,7 +24571,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="447" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:19" ht="29.25">
       <c r="A447" s="2" t="s">
         <v>522</v>
       </c>
@@ -24643,7 +24628,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="448" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:19" ht="48.75">
       <c r="A448" s="2" t="s">
         <v>522</v>
       </c>
@@ -24702,7 +24687,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="449" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:19" ht="29.25">
       <c r="A449" s="2" t="s">
         <v>522</v>
       </c>
@@ -24759,7 +24744,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="450" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:19" ht="29.25">
       <c r="A450" s="2" t="s">
         <v>522</v>
       </c>
@@ -24816,7 +24801,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="451" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:19" ht="29.25">
       <c r="A451" s="2" t="s">
         <v>522</v>
       </c>
@@ -24875,7 +24860,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="452" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:19" ht="29.25">
       <c r="A452" s="2" t="s">
         <v>522</v>
       </c>
@@ -24934,7 +24919,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="453" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:19" ht="29.25">
       <c r="A453" s="2" t="s">
         <v>522</v>
       </c>
@@ -24993,7 +24978,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="454" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:19" ht="29.25">
       <c r="A454" s="2" t="s">
         <v>522</v>
       </c>
@@ -25050,7 +25035,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="455" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:19" ht="29.25">
       <c r="A455" s="2" t="s">
         <v>522</v>
       </c>
@@ -25109,7 +25094,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="456" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:19" ht="29.25">
       <c r="A456" s="2" t="s">
         <v>522</v>
       </c>
@@ -25168,7 +25153,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="457" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:19" ht="29.25">
       <c r="A457" s="2" t="s">
         <v>522</v>
       </c>
@@ -25225,7 +25210,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="458" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:19" ht="29.25">
       <c r="A458" s="2" t="s">
         <v>522</v>
       </c>
@@ -25284,7 +25269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="459" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:19" ht="48.75">
       <c r="A459" s="2" t="s">
         <v>522</v>
       </c>
@@ -25343,7 +25328,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="460" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:19" ht="29.25">
       <c r="A460" s="2" t="s">
         <v>522</v>
       </c>
@@ -25402,7 +25387,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="461" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:19" ht="39">
       <c r="A461" s="2" t="s">
         <v>522</v>
       </c>
@@ -25461,7 +25446,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="462" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:19" ht="39">
       <c r="A462" s="2" t="s">
         <v>522</v>
       </c>
@@ -25520,7 +25505,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="463" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:19" ht="29.25">
       <c r="A463" s="2" t="s">
         <v>522</v>
       </c>
@@ -25563,7 +25548,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="464" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:19" ht="29.25">
       <c r="A464" s="2" t="s">
         <v>522</v>
       </c>
@@ -25622,7 +25607,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="465" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:19" ht="29.25">
       <c r="A465" s="2" t="s">
         <v>522</v>
       </c>
@@ -25681,7 +25666,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="466" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:19" ht="29.25">
       <c r="A466" s="2" t="s">
         <v>522</v>
       </c>
@@ -25732,7 +25717,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="467" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:19" ht="39">
       <c r="A467" s="2" t="s">
         <v>522</v>
       </c>
@@ -25769,7 +25754,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="468" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:19" ht="39">
       <c r="A468" s="2" t="s">
         <v>522</v>
       </c>
@@ -25828,7 +25813,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="469" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:19" ht="39">
       <c r="A469" s="2" t="s">
         <v>522</v>
       </c>
@@ -25887,9 +25872,9 @@
         <v>557</v>
       </c>
     </row>
-    <row r="470" spans="1:19" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:19" ht="0" hidden="1" customHeight="1"/>
+    <row r="471" spans="1:19" ht="18" customHeight="1"/>
+    <row r="472" spans="1:19" ht="17.100000000000001" customHeight="1">
       <c r="A472" s="12" t="s">
         <v>560</v>
       </c>
@@ -25906,7 +25891,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="75" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okno serwisowe 25.07.2023 pliki excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -15,7 +15,6 @@
     <sheet name="SDGs_1-17" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SDGs_1-17'!$A$3:$B$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'SDGs_1-17'!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2817" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="563">
   <si>
     <t>sdg.gov.pl/en</t>
   </si>
@@ -1705,7 +1704,13 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 25-07-2023, 10:38</t>
+    <t>Last update: 27-07-2023, 13:26</t>
+  </si>
+  <si>
+    <t>37,0</t>
+  </si>
+  <si>
+    <t>1,0</t>
   </si>
 </sst>
 </file>
@@ -1807,7 +1812,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
@@ -1834,6 +1839,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2255,9 +2263,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S472"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L202" sqref="L202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,14 +2281,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -11900,16 +11908,16 @@
       <c r="H202" s="3"/>
       <c r="I202" s="3"/>
       <c r="J202" s="3"/>
-      <c r="K202" s="6">
-        <v>37</v>
-      </c>
-      <c r="L202" s="3"/>
-      <c r="M202" s="3"/>
-      <c r="N202" s="3"/>
-      <c r="O202" s="3"/>
-      <c r="P202" s="3"/>
-      <c r="Q202" s="6">
-        <v>1</v>
+      <c r="K202" s="10" t="s">
+        <v>561</v>
+      </c>
+      <c r="L202" s="10"/>
+      <c r="M202" s="10"/>
+      <c r="N202" s="10"/>
+      <c r="O202" s="10"/>
+      <c r="P202" s="10"/>
+      <c r="Q202" s="10" t="s">
+        <v>562</v>
       </c>
       <c r="R202" s="3"/>
       <c r="S202" s="2" t="s">
@@ -26026,13 +26034,12 @@
     <row r="470" spans="1:19" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="471" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="472" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A472" s="12" t="s">
+      <c r="A472" s="13" t="s">
         <v>560</v>
       </c>
-      <c r="B472" s="10"/>
+      <c r="B472" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B3"/>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -26042,8 +26049,8 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="75" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Okno serwisowe 22.08.2023 - aktualizacja excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="18060" windowHeight="7050"/>
   </bookViews>
@@ -1705,13 +1700,13 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 08-08-2023, 09:41</t>
+    <t>Last update: 22-08-2023, 12:10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$-10809]0.0;\-0.0;0.0"/>
     <numFmt numFmtId="165" formatCode="[$-10809]0.00;\-0.00;0.00"/>
@@ -1720,7 +1715,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1918,14 +1913,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -2009,7 +1996,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2041,10 +2028,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2076,7 +2062,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -2252,7 +2237,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S472"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
@@ -2260,7 +2245,7 @@
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2272,17 +2257,17 @@
     <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="36" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2341,7 +2326,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="19.5">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2398,7 +2383,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2455,7 +2440,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -2512,7 +2497,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -2569,7 +2554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -2626,7 +2611,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -2683,7 +2668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -2740,7 +2725,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2797,7 +2782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -2854,7 +2839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2911,7 +2896,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="19.5">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -2968,7 +2953,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="19.5">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -3025,7 +3010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -3064,7 +3049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="29.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -3123,7 +3108,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="97.5">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -3178,7 +3163,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="97.5">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -3233,7 +3218,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="97.5">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -3288,7 +3273,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="19.5">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -3343,7 +3328,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="29.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -3400,7 +3385,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="29.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -3457,7 +3442,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="29.25">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -3506,7 +3491,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="68.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -3555,7 +3540,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="29.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
@@ -3604,7 +3589,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="29.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -3653,7 +3638,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="29.25">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
@@ -3704,7 +3689,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="39">
       <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
@@ -3761,7 +3746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="39">
       <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
@@ -3818,7 +3803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="39">
       <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
@@ -3875,7 +3860,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="39">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -3932,7 +3917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="19.5">
       <c r="A33" s="2" t="s">
         <v>66</v>
       </c>
@@ -3987,7 +3972,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="29.25">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -4032,7 +4017,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="29.25">
       <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
@@ -4077,7 +4062,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="29.25">
       <c r="A36" s="2" t="s">
         <v>66</v>
       </c>
@@ -4122,7 +4107,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="29.25">
       <c r="A37" s="2" t="s">
         <v>66</v>
       </c>
@@ -4167,7 +4152,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="29.25">
       <c r="A38" s="2" t="s">
         <v>66</v>
       </c>
@@ -4212,7 +4197,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="29.25">
       <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
@@ -4257,7 +4242,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="39">
       <c r="A40" s="2" t="s">
         <v>66</v>
       </c>
@@ -4296,7 +4281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="97.5">
       <c r="A41" s="2" t="s">
         <v>66</v>
       </c>
@@ -4355,7 +4340,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="97.5">
       <c r="A42" s="2" t="s">
         <v>66</v>
       </c>
@@ -4414,7 +4399,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="97.5">
       <c r="A43" s="2" t="s">
         <v>66</v>
       </c>
@@ -4473,7 +4458,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="97.5">
       <c r="A44" s="2" t="s">
         <v>66</v>
       </c>
@@ -4532,7 +4517,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="97.5">
       <c r="A45" s="2" t="s">
         <v>66</v>
       </c>
@@ -4591,7 +4576,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="97.5">
       <c r="A46" s="2" t="s">
         <v>66</v>
       </c>
@@ -4650,7 +4635,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="48.75">
       <c r="A47" s="2" t="s">
         <v>66</v>
       </c>
@@ -4699,7 +4684,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="48.75">
       <c r="A48" s="2" t="s">
         <v>66</v>
       </c>
@@ -4748,7 +4733,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="19.5">
       <c r="A49" s="2" t="s">
         <v>66</v>
       </c>
@@ -4805,7 +4790,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="29.25">
       <c r="A50" s="2" t="s">
         <v>66</v>
       </c>
@@ -4858,7 +4843,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="19.5">
       <c r="A51" s="2" t="s">
         <v>95</v>
       </c>
@@ -4915,7 +4900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="19.5">
       <c r="A52" s="2" t="s">
         <v>95</v>
       </c>
@@ -4974,7 +4959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>95</v>
       </c>
@@ -5033,7 +5018,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>95</v>
       </c>
@@ -5092,7 +5077,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>95</v>
       </c>
@@ -5151,7 +5136,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>95</v>
       </c>
@@ -5210,7 +5195,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>95</v>
       </c>
@@ -5269,7 +5254,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>95</v>
       </c>
@@ -5328,7 +5313,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="29.25">
       <c r="A59" s="2" t="s">
         <v>95</v>
       </c>
@@ -5385,7 +5370,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>95</v>
       </c>
@@ -5442,7 +5427,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="29.25">
       <c r="A61" s="2" t="s">
         <v>95</v>
       </c>
@@ -5501,7 +5486,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="29.25">
       <c r="A62" s="2" t="s">
         <v>95</v>
       </c>
@@ -5560,7 +5545,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="29.25">
       <c r="A63" s="2" t="s">
         <v>95</v>
       </c>
@@ -5619,7 +5604,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="19.5">
       <c r="A64" s="2" t="s">
         <v>95</v>
       </c>
@@ -5676,7 +5661,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="29.25">
       <c r="A65" s="2" t="s">
         <v>95</v>
       </c>
@@ -5735,7 +5720,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="29.25">
       <c r="A66" s="2" t="s">
         <v>95</v>
       </c>
@@ -5794,7 +5779,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="29.25">
       <c r="A67" s="2" t="s">
         <v>95</v>
       </c>
@@ -5853,7 +5838,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="29.25">
       <c r="A68" s="2" t="s">
         <v>95</v>
       </c>
@@ -5910,7 +5895,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="29.25">
       <c r="A69" s="2" t="s">
         <v>95</v>
       </c>
@@ -5967,7 +5952,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" ht="29.25">
       <c r="A70" s="2" t="s">
         <v>95</v>
       </c>
@@ -6024,7 +6009,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" ht="29.25">
       <c r="A71" s="2" t="s">
         <v>95</v>
       </c>
@@ -6081,7 +6066,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" ht="19.5">
       <c r="A72" s="2" t="s">
         <v>95</v>
       </c>
@@ -6138,7 +6123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="19.5">
       <c r="A73" s="2" t="s">
         <v>95</v>
       </c>
@@ -6195,7 +6180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="19.5">
       <c r="A74" s="2" t="s">
         <v>95</v>
       </c>
@@ -6252,7 +6237,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="19.5">
       <c r="A75" s="2" t="s">
         <v>95</v>
       </c>
@@ -6309,7 +6294,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" ht="29.25">
       <c r="A76" s="2" t="s">
         <v>95</v>
       </c>
@@ -6366,7 +6351,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" ht="29.25">
       <c r="A77" s="2" t="s">
         <v>95</v>
       </c>
@@ -6405,7 +6390,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" ht="19.5">
       <c r="A78" s="2" t="s">
         <v>95</v>
       </c>
@@ -6464,7 +6449,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="19.5">
       <c r="A79" s="2" t="s">
         <v>95</v>
       </c>
@@ -6523,7 +6508,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" ht="19.5">
       <c r="A80" s="2" t="s">
         <v>95</v>
       </c>
@@ -6582,7 +6567,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="19.5">
       <c r="A81" s="2" t="s">
         <v>95</v>
       </c>
@@ -6625,7 +6610,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="29.25">
       <c r="A82" s="2" t="s">
         <v>95</v>
       </c>
@@ -6682,7 +6667,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="29.25">
       <c r="A83" s="2" t="s">
         <v>95</v>
       </c>
@@ -6739,7 +6724,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="19.5">
       <c r="A84" s="2" t="s">
         <v>95</v>
       </c>
@@ -6774,7 +6759,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="29.25">
       <c r="A85" s="2" t="s">
         <v>95</v>
       </c>
@@ -6809,7 +6794,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="19.5">
       <c r="A86" s="2" t="s">
         <v>95</v>
       </c>
@@ -6866,7 +6851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="19.5">
       <c r="A87" s="2" t="s">
         <v>95</v>
       </c>
@@ -6905,7 +6890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" ht="19.5">
       <c r="A88" s="2" t="s">
         <v>95</v>
       </c>
@@ -6962,7 +6947,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="19.5">
       <c r="A89" s="2" t="s">
         <v>95</v>
       </c>
@@ -7019,7 +7004,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="19.5">
       <c r="A90" s="2" t="s">
         <v>95</v>
       </c>
@@ -7060,7 +7045,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="29.25">
       <c r="A91" s="2" t="s">
         <v>95</v>
       </c>
@@ -7113,7 +7098,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" ht="19.5">
       <c r="A92" s="2" t="s">
         <v>95</v>
       </c>
@@ -7152,7 +7137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" ht="19.5">
       <c r="A93" s="2" t="s">
         <v>95</v>
       </c>
@@ -7191,7 +7176,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" ht="19.5">
       <c r="A94" s="2" t="s">
         <v>95</v>
       </c>
@@ -7230,7 +7215,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" ht="19.5">
       <c r="A95" s="2" t="s">
         <v>95</v>
       </c>
@@ -7285,7 +7270,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" ht="48.75">
       <c r="A96" s="2" t="s">
         <v>149</v>
       </c>
@@ -7322,7 +7307,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" ht="48.75">
       <c r="A97" s="2" t="s">
         <v>149</v>
       </c>
@@ -7359,7 +7344,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" ht="48.75">
       <c r="A98" s="2" t="s">
         <v>149</v>
       </c>
@@ -7396,7 +7381,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" ht="48.75">
       <c r="A99" s="2" t="s">
         <v>149</v>
       </c>
@@ -7437,7 +7422,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" ht="48.75">
       <c r="A100" s="2" t="s">
         <v>149</v>
       </c>
@@ -7478,7 +7463,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" ht="48.75">
       <c r="A101" s="2" t="s">
         <v>149</v>
       </c>
@@ -7519,7 +7504,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" ht="48.75">
       <c r="A102" s="2" t="s">
         <v>149</v>
       </c>
@@ -7560,7 +7545,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" ht="48.75">
       <c r="A103" s="2" t="s">
         <v>149</v>
       </c>
@@ -7601,7 +7586,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" ht="48.75">
       <c r="A104" s="2" t="s">
         <v>149</v>
       </c>
@@ -7642,7 +7627,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" ht="29.25">
       <c r="A105" s="2" t="s">
         <v>149</v>
       </c>
@@ -7679,7 +7664,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" ht="19.5">
       <c r="A106" s="2" t="s">
         <v>149</v>
       </c>
@@ -7738,7 +7723,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" ht="19.5">
       <c r="A107" s="2" t="s">
         <v>149</v>
       </c>
@@ -7797,7 +7782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" ht="19.5">
       <c r="A108" s="2" t="s">
         <v>149</v>
       </c>
@@ -7856,7 +7841,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" ht="19.5">
       <c r="A109" s="2" t="s">
         <v>149</v>
       </c>
@@ -7893,7 +7878,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" ht="19.5">
       <c r="A110" s="2" t="s">
         <v>149</v>
       </c>
@@ -7930,7 +7915,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" ht="19.5">
       <c r="A111" s="2" t="s">
         <v>149</v>
       </c>
@@ -7967,7 +7952,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" ht="29.25">
       <c r="A112" s="2" t="s">
         <v>149</v>
       </c>
@@ -8012,7 +7997,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" ht="19.5">
       <c r="A113" s="2" t="s">
         <v>149</v>
       </c>
@@ -8059,7 +8044,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" ht="39">
       <c r="A114" s="2" t="s">
         <v>149</v>
       </c>
@@ -8106,7 +8091,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" ht="48.75">
       <c r="A115" s="2" t="s">
         <v>149</v>
       </c>
@@ -8153,7 +8138,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" ht="58.5">
       <c r="A116" s="2" t="s">
         <v>149</v>
       </c>
@@ -8200,7 +8185,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" ht="29.25">
       <c r="A117" s="2" t="s">
         <v>149</v>
       </c>
@@ -8247,7 +8232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" ht="29.25">
       <c r="A118" s="2" t="s">
         <v>149</v>
       </c>
@@ -8292,7 +8277,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" ht="19.5">
       <c r="A119" s="2" t="s">
         <v>149</v>
       </c>
@@ -8339,7 +8324,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" ht="39">
       <c r="A120" s="2" t="s">
         <v>149</v>
       </c>
@@ -8386,7 +8371,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" ht="48.75">
       <c r="A121" s="2" t="s">
         <v>149</v>
       </c>
@@ -8433,7 +8418,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" ht="58.5">
       <c r="A122" s="2" t="s">
         <v>149</v>
       </c>
@@ -8480,7 +8465,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" ht="29.25">
       <c r="A123" s="2" t="s">
         <v>149</v>
       </c>
@@ -8527,7 +8512,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" ht="48.75">
       <c r="A124" s="2" t="s">
         <v>149</v>
       </c>
@@ -8566,7 +8551,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" ht="48.75">
       <c r="A125" s="2" t="s">
         <v>149</v>
       </c>
@@ -8605,7 +8590,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" ht="29.25">
       <c r="A126" s="2" t="s">
         <v>149</v>
       </c>
@@ -8664,7 +8649,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" ht="29.25">
       <c r="A127" s="2" t="s">
         <v>149</v>
       </c>
@@ -8699,7 +8684,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" ht="29.25">
       <c r="A128" s="2" t="s">
         <v>149</v>
       </c>
@@ -8734,7 +8719,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" ht="29.25">
       <c r="A129" s="2" t="s">
         <v>149</v>
       </c>
@@ -8769,7 +8754,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" ht="29.25">
       <c r="A130" s="2" t="s">
         <v>149</v>
       </c>
@@ -8804,7 +8789,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" ht="29.25">
       <c r="A131" s="2" t="s">
         <v>149</v>
       </c>
@@ -8839,7 +8824,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" ht="29.25">
       <c r="A132" s="2" t="s">
         <v>149</v>
       </c>
@@ -8874,7 +8859,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" ht="29.25">
       <c r="A133" s="2" t="s">
         <v>149</v>
       </c>
@@ -8909,7 +8894,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" ht="29.25">
       <c r="A134" s="2" t="s">
         <v>149</v>
       </c>
@@ -8944,7 +8929,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" ht="29.25">
       <c r="A135" s="2" t="s">
         <v>149</v>
       </c>
@@ -8979,7 +8964,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" ht="29.25">
       <c r="A136" s="2" t="s">
         <v>149</v>
       </c>
@@ -9014,7 +8999,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" ht="29.25">
       <c r="A137" s="2" t="s">
         <v>149</v>
       </c>
@@ -9049,7 +9034,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" ht="29.25">
       <c r="A138" s="2" t="s">
         <v>149</v>
       </c>
@@ -9084,7 +9069,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" ht="29.25">
       <c r="A139" s="2" t="s">
         <v>149</v>
       </c>
@@ -9119,7 +9104,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" ht="29.25">
       <c r="A140" s="2" t="s">
         <v>149</v>
       </c>
@@ -9154,7 +9139,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" ht="29.25">
       <c r="A141" s="2" t="s">
         <v>149</v>
       </c>
@@ -9189,7 +9174,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" ht="29.25">
       <c r="A142" s="2" t="s">
         <v>149</v>
       </c>
@@ -9224,7 +9209,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" ht="48.75">
       <c r="A143" s="2" t="s">
         <v>149</v>
       </c>
@@ -9283,7 +9268,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" ht="58.5">
       <c r="A144" s="2" t="s">
         <v>149</v>
       </c>
@@ -9342,7 +9327,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" ht="58.5">
       <c r="A145" s="2" t="s">
         <v>149</v>
       </c>
@@ -9377,7 +9362,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" ht="58.5">
       <c r="A146" s="2" t="s">
         <v>149</v>
       </c>
@@ -9412,7 +9397,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" ht="58.5">
       <c r="A147" s="2" t="s">
         <v>149</v>
       </c>
@@ -9471,7 +9456,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" ht="58.5">
       <c r="A148" s="2" t="s">
         <v>149</v>
       </c>
@@ -9530,7 +9515,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" ht="58.5">
       <c r="A149" s="2" t="s">
         <v>149</v>
       </c>
@@ -9589,7 +9574,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" ht="29.25">
       <c r="A150" s="2" t="s">
         <v>149</v>
       </c>
@@ -9642,7 +9627,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" ht="58.5">
       <c r="A151" s="2" t="s">
         <v>149</v>
       </c>
@@ -9697,7 +9682,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" ht="58.5">
       <c r="A152" s="2" t="s">
         <v>149</v>
       </c>
@@ -9752,7 +9737,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" ht="58.5">
       <c r="A153" s="2" t="s">
         <v>149</v>
       </c>
@@ -9807,7 +9792,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" ht="58.5">
       <c r="A154" s="2" t="s">
         <v>149</v>
       </c>
@@ -9862,7 +9847,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" ht="29.25">
       <c r="A155" s="2" t="s">
         <v>205</v>
       </c>
@@ -9897,7 +9882,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" ht="19.5">
       <c r="A156" s="2" t="s">
         <v>205</v>
       </c>
@@ -9954,7 +9939,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" ht="39">
       <c r="A157" s="2" t="s">
         <v>205</v>
       </c>
@@ -9989,7 +9974,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" ht="39">
       <c r="A158" s="2" t="s">
         <v>205</v>
       </c>
@@ -10024,7 +10009,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" ht="39">
       <c r="A159" s="2" t="s">
         <v>205</v>
       </c>
@@ -10059,7 +10044,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="160" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" ht="39">
       <c r="A160" s="2" t="s">
         <v>205</v>
       </c>
@@ -10094,7 +10079,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" ht="39">
       <c r="A161" s="2" t="s">
         <v>205</v>
       </c>
@@ -10129,7 +10114,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" ht="19.5">
       <c r="A162" s="2" t="s">
         <v>205</v>
       </c>
@@ -10164,7 +10149,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:19" ht="19.5">
       <c r="A163" s="2" t="s">
         <v>205</v>
       </c>
@@ -10199,7 +10184,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" ht="19.5">
       <c r="A164" s="2" t="s">
         <v>205</v>
       </c>
@@ -10234,7 +10219,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:19" ht="19.5">
       <c r="A165" s="2" t="s">
         <v>205</v>
       </c>
@@ -10269,7 +10254,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" ht="19.5">
       <c r="A166" s="2" t="s">
         <v>205</v>
       </c>
@@ -10304,7 +10289,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" ht="19.5">
       <c r="A167" s="2" t="s">
         <v>205</v>
       </c>
@@ -10339,7 +10324,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:19" ht="19.5">
       <c r="A168" s="2" t="s">
         <v>205</v>
       </c>
@@ -10374,7 +10359,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" ht="19.5">
       <c r="A169" s="2" t="s">
         <v>205</v>
       </c>
@@ -10409,7 +10394,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:19" ht="29.25">
       <c r="A170" s="2" t="s">
         <v>205</v>
       </c>
@@ -10448,7 +10433,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:19" ht="29.25">
       <c r="A171" s="2" t="s">
         <v>205</v>
       </c>
@@ -10487,7 +10472,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:19" ht="29.25">
       <c r="A172" s="2" t="s">
         <v>205</v>
       </c>
@@ -10546,7 +10531,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:19" ht="29.25">
       <c r="A173" s="2" t="s">
         <v>205</v>
       </c>
@@ -10605,7 +10590,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:19" ht="29.25">
       <c r="A174" s="2" t="s">
         <v>205</v>
       </c>
@@ -10664,7 +10649,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:19" ht="29.25">
       <c r="A175" s="2" t="s">
         <v>205</v>
       </c>
@@ -10723,7 +10708,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:19" ht="29.25">
       <c r="A176" s="2" t="s">
         <v>205</v>
       </c>
@@ -10782,7 +10767,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="177" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:19" ht="19.5">
       <c r="A177" s="2" t="s">
         <v>205</v>
       </c>
@@ -10827,7 +10812,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="178" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:19" ht="39">
       <c r="A178" s="2" t="s">
         <v>205</v>
       </c>
@@ -10872,7 +10857,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:19" ht="19.5">
       <c r="A179" s="2" t="s">
         <v>205</v>
       </c>
@@ -10917,7 +10902,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:19" ht="39">
       <c r="A180" s="2" t="s">
         <v>205</v>
       </c>
@@ -10962,7 +10947,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:19" ht="39">
       <c r="A181" s="2" t="s">
         <v>205</v>
       </c>
@@ -11007,7 +10992,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="182" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:19" ht="39">
       <c r="A182" s="2" t="s">
         <v>205</v>
       </c>
@@ -11052,7 +11037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:19" ht="39">
       <c r="A183" s="2" t="s">
         <v>205</v>
       </c>
@@ -11097,7 +11082,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:19" ht="39">
       <c r="A184" s="2" t="s">
         <v>205</v>
       </c>
@@ -11136,7 +11121,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:19" ht="39">
       <c r="A185" s="2" t="s">
         <v>205</v>
       </c>
@@ -11175,7 +11160,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="186" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:19" ht="39">
       <c r="A186" s="2" t="s">
         <v>205</v>
       </c>
@@ -11214,7 +11199,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:19" ht="39">
       <c r="A187" s="2" t="s">
         <v>205</v>
       </c>
@@ -11253,7 +11238,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:19" ht="39">
       <c r="A188" s="2" t="s">
         <v>205</v>
       </c>
@@ -11292,7 +11277,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:19" ht="39">
       <c r="A189" s="2" t="s">
         <v>205</v>
       </c>
@@ -11331,7 +11316,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:19" ht="39">
       <c r="A190" s="2" t="s">
         <v>205</v>
       </c>
@@ -11370,7 +11355,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:19" ht="39">
       <c r="A191" s="2" t="s">
         <v>205</v>
       </c>
@@ -11409,7 +11394,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:19" ht="39">
       <c r="A192" s="2" t="s">
         <v>205</v>
       </c>
@@ -11448,7 +11433,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="193" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:19" ht="39">
       <c r="A193" s="2" t="s">
         <v>205</v>
       </c>
@@ -11487,7 +11472,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:19" ht="39">
       <c r="A194" s="2" t="s">
         <v>205</v>
       </c>
@@ -11526,7 +11511,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="195" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:19" ht="39">
       <c r="A195" s="2" t="s">
         <v>205</v>
       </c>
@@ -11565,7 +11550,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="196" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:19" ht="19.5">
       <c r="A196" s="2" t="s">
         <v>205</v>
       </c>
@@ -11606,7 +11591,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:19" ht="19.5">
       <c r="A197" s="2" t="s">
         <v>205</v>
       </c>
@@ -11661,7 +11646,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:19" ht="19.5">
       <c r="A198" s="2" t="s">
         <v>205</v>
       </c>
@@ -11716,7 +11701,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:19" ht="19.5">
       <c r="A199" s="2" t="s">
         <v>245</v>
       </c>
@@ -11773,7 +11758,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="200" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:19" ht="29.25">
       <c r="A200" s="2" t="s">
         <v>245</v>
       </c>
@@ -11830,7 +11815,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="201" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:19" ht="19.5">
       <c r="A201" s="2" t="s">
         <v>245</v>
       </c>
@@ -11887,7 +11872,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="202" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:19" ht="19.5">
       <c r="A202" s="2" t="s">
         <v>245</v>
       </c>
@@ -11924,7 +11909,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="203" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:19" ht="19.5">
       <c r="A203" s="2" t="s">
         <v>245</v>
       </c>
@@ -11961,7 +11946,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="204" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:19" ht="29.25">
       <c r="A204" s="2" t="s">
         <v>245</v>
       </c>
@@ -12016,7 +12001,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="205" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:19" ht="19.5">
       <c r="A205" s="2" t="s">
         <v>245</v>
       </c>
@@ -12071,7 +12056,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="206" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:19" ht="19.5">
       <c r="A206" s="2" t="s">
         <v>245</v>
       </c>
@@ -12116,7 +12101,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="207" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:19" ht="29.25">
       <c r="A207" s="2" t="s">
         <v>245</v>
       </c>
@@ -12175,7 +12160,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="208" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:19" ht="29.25">
       <c r="A208" s="2" t="s">
         <v>245</v>
       </c>
@@ -12228,7 +12213,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="209" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:19" ht="39">
       <c r="A209" s="2" t="s">
         <v>245</v>
       </c>
@@ -12285,7 +12270,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="210" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:19" ht="19.5">
       <c r="A210" s="2" t="s">
         <v>266</v>
       </c>
@@ -12320,7 +12305,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="211" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:19" ht="19.5">
       <c r="A211" s="2" t="s">
         <v>266</v>
       </c>
@@ -12377,7 +12362,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="212" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:19" ht="29.25">
       <c r="A212" s="2" t="s">
         <v>266</v>
       </c>
@@ -12432,7 +12417,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="213" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:19" ht="29.25">
       <c r="A213" s="2" t="s">
         <v>266</v>
       </c>
@@ -12485,7 +12470,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="214" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:19" ht="29.25">
       <c r="A214" s="2" t="s">
         <v>272</v>
       </c>
@@ -12542,7 +12527,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:19" ht="29.25">
       <c r="A215" s="2" t="s">
         <v>272</v>
       </c>
@@ -12599,7 +12584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="216" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:19" ht="29.25">
       <c r="A216" s="2" t="s">
         <v>272</v>
       </c>
@@ -12638,7 +12623,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="217" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:19" ht="29.25">
       <c r="A217" s="2" t="s">
         <v>272</v>
       </c>
@@ -12677,7 +12662,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="218" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:19" ht="29.25">
       <c r="A218" s="2" t="s">
         <v>272</v>
       </c>
@@ -12716,7 +12701,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="219" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:19" ht="29.25">
       <c r="A219" s="2" t="s">
         <v>272</v>
       </c>
@@ -12773,7 +12758,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="220" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:19" ht="29.25">
       <c r="A220" s="2" t="s">
         <v>272</v>
       </c>
@@ -12830,7 +12815,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="221" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:19" ht="29.25">
       <c r="A221" s="2" t="s">
         <v>272</v>
       </c>
@@ -12887,7 +12872,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="222" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:19" ht="29.25">
       <c r="A222" s="2" t="s">
         <v>272</v>
       </c>
@@ -12932,7 +12917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="223" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:19" ht="29.25">
       <c r="A223" s="2" t="s">
         <v>272</v>
       </c>
@@ -12977,7 +12962,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="224" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:19" ht="29.25">
       <c r="A224" s="2" t="s">
         <v>272</v>
       </c>
@@ -13022,7 +13007,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="225" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:19" ht="29.25">
       <c r="A225" s="2" t="s">
         <v>272</v>
       </c>
@@ -13067,7 +13052,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="226" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:19" ht="29.25">
       <c r="A226" s="2" t="s">
         <v>272</v>
       </c>
@@ -13112,7 +13097,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="227" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:19" ht="29.25">
       <c r="A227" s="2" t="s">
         <v>272</v>
       </c>
@@ -13157,7 +13142,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="228" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:19" ht="29.25">
       <c r="A228" s="2" t="s">
         <v>272</v>
       </c>
@@ -13202,7 +13187,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="229" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:19" ht="29.25">
       <c r="A229" s="2" t="s">
         <v>272</v>
       </c>
@@ -13247,7 +13232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="230" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:19" ht="39">
       <c r="A230" s="2" t="s">
         <v>272</v>
       </c>
@@ -13292,7 +13277,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="231" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:19" ht="29.25">
       <c r="A231" s="2" t="s">
         <v>272</v>
       </c>
@@ -13337,7 +13322,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="232" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:19" ht="39">
       <c r="A232" s="2" t="s">
         <v>272</v>
       </c>
@@ -13382,7 +13367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="233" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:19" ht="29.25">
       <c r="A233" s="2" t="s">
         <v>272</v>
       </c>
@@ -13427,7 +13412,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="234" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:19" ht="29.25">
       <c r="A234" s="2" t="s">
         <v>272</v>
       </c>
@@ -13472,7 +13457,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="235" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:19" ht="29.25">
       <c r="A235" s="2" t="s">
         <v>272</v>
       </c>
@@ -13517,7 +13502,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="236" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:19" ht="29.25">
       <c r="A236" s="2" t="s">
         <v>272</v>
       </c>
@@ -13562,7 +13547,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="237" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:19" ht="29.25">
       <c r="A237" s="2" t="s">
         <v>272</v>
       </c>
@@ -13607,7 +13592,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="238" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:19" ht="29.25">
       <c r="A238" s="2" t="s">
         <v>272</v>
       </c>
@@ -13652,7 +13637,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:19" ht="29.25">
       <c r="A239" s="2" t="s">
         <v>272</v>
       </c>
@@ -13697,7 +13682,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="240" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:19" ht="29.25">
       <c r="A240" s="2" t="s">
         <v>272</v>
       </c>
@@ -13742,7 +13727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="241" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:19" ht="29.25">
       <c r="A241" s="2" t="s">
         <v>272</v>
       </c>
@@ -13801,7 +13786,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="242" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:19" ht="29.25">
       <c r="A242" s="2" t="s">
         <v>272</v>
       </c>
@@ -13860,7 +13845,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="243" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:19" ht="29.25">
       <c r="A243" s="2" t="s">
         <v>272</v>
       </c>
@@ -13919,7 +13904,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="244" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:19" ht="29.25">
       <c r="A244" s="2" t="s">
         <v>272</v>
       </c>
@@ -13978,7 +13963,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="245" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:19" ht="29.25">
       <c r="A245" s="2" t="s">
         <v>272</v>
       </c>
@@ -14037,7 +14022,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="246" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:19" ht="29.25">
       <c r="A246" s="2" t="s">
         <v>272</v>
       </c>
@@ -14096,7 +14081,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="247" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:19" ht="29.25">
       <c r="A247" s="2" t="s">
         <v>272</v>
       </c>
@@ -14155,7 +14140,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="248" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:19" ht="29.25">
       <c r="A248" s="2" t="s">
         <v>272</v>
       </c>
@@ -14214,7 +14199,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="249" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:19" ht="29.25">
       <c r="A249" s="2" t="s">
         <v>272</v>
       </c>
@@ -14273,7 +14258,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="250" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:19" ht="29.25">
       <c r="A250" s="2" t="s">
         <v>272</v>
       </c>
@@ -14332,7 +14317,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="251" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:19" ht="29.25">
       <c r="A251" s="2" t="s">
         <v>272</v>
       </c>
@@ -14389,7 +14374,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="252" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:19" ht="29.25">
       <c r="A252" s="2" t="s">
         <v>272</v>
       </c>
@@ -14446,7 +14431,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="253" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:19" ht="39">
       <c r="A253" s="2" t="s">
         <v>272</v>
       </c>
@@ -14487,7 +14472,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="254" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:19" ht="39">
       <c r="A254" s="2" t="s">
         <v>272</v>
       </c>
@@ -14528,7 +14513,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="255" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:19" ht="39">
       <c r="A255" s="2" t="s">
         <v>272</v>
       </c>
@@ -14569,7 +14554,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="256" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:19" ht="29.25">
       <c r="A256" s="2" t="s">
         <v>272</v>
       </c>
@@ -14626,7 +14611,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="257" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:19" ht="48.75">
       <c r="A257" s="2" t="s">
         <v>272</v>
       </c>
@@ -14683,7 +14668,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="258" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:19" ht="29.25">
       <c r="A258" s="2" t="s">
         <v>272</v>
       </c>
@@ -14718,7 +14703,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="259" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:19" ht="29.25">
       <c r="A259" s="2" t="s">
         <v>272</v>
       </c>
@@ -14753,7 +14738,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="260" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:19" ht="29.25">
       <c r="A260" s="2" t="s">
         <v>272</v>
       </c>
@@ -14788,7 +14773,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="261" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:19" ht="29.25">
       <c r="A261" s="2" t="s">
         <v>272</v>
       </c>
@@ -14823,7 +14808,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="262" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:19" ht="29.25">
       <c r="A262" s="2" t="s">
         <v>272</v>
       </c>
@@ -14858,7 +14843,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="263" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:19" ht="29.25">
       <c r="A263" s="2" t="s">
         <v>272</v>
       </c>
@@ -14893,7 +14878,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="264" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:19" ht="29.25">
       <c r="A264" s="2" t="s">
         <v>272</v>
       </c>
@@ -14928,7 +14913,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="265" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:19" ht="29.25">
       <c r="A265" s="2" t="s">
         <v>272</v>
       </c>
@@ -14963,7 +14948,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="266" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:19" ht="29.25">
       <c r="A266" s="2" t="s">
         <v>272</v>
       </c>
@@ -15014,7 +14999,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="267" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:19" ht="29.25">
       <c r="A267" s="2" t="s">
         <v>318</v>
       </c>
@@ -15071,7 +15056,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="268" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:19" ht="29.25">
       <c r="A268" s="2" t="s">
         <v>318</v>
       </c>
@@ -15128,7 +15113,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="269" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:19" ht="29.25">
       <c r="A269" s="2" t="s">
         <v>318</v>
       </c>
@@ -15185,7 +15170,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="270" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:19" ht="29.25">
       <c r="A270" s="2" t="s">
         <v>318</v>
       </c>
@@ -15242,7 +15227,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="271" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:19" ht="29.25">
       <c r="A271" s="2" t="s">
         <v>318</v>
       </c>
@@ -15299,7 +15284,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="272" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:19" ht="29.25">
       <c r="A272" s="2" t="s">
         <v>318</v>
       </c>
@@ -15356,7 +15341,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="273" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:19" ht="29.25">
       <c r="A273" s="2" t="s">
         <v>318</v>
       </c>
@@ -15413,7 +15398,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="274" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:19" ht="29.25">
       <c r="A274" s="2" t="s">
         <v>318</v>
       </c>
@@ -15470,7 +15455,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="275" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:19" ht="29.25">
       <c r="A275" s="2" t="s">
         <v>318</v>
       </c>
@@ -15527,7 +15512,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="276" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:19" ht="29.25">
       <c r="A276" s="2" t="s">
         <v>318</v>
       </c>
@@ -15584,7 +15569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="277" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:19" ht="29.25">
       <c r="A277" s="2" t="s">
         <v>318</v>
       </c>
@@ -15641,7 +15626,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="278" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:19" ht="29.25">
       <c r="A278" s="2" t="s">
         <v>318</v>
       </c>
@@ -15698,7 +15683,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="279" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:19" ht="29.25">
       <c r="A279" s="2" t="s">
         <v>318</v>
       </c>
@@ -15755,7 +15740,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="280" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:19" ht="29.25">
       <c r="A280" s="2" t="s">
         <v>318</v>
       </c>
@@ -15812,7 +15797,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="281" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:19" ht="29.25">
       <c r="A281" s="2" t="s">
         <v>318</v>
       </c>
@@ -15869,7 +15854,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="282" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:19" ht="29.25">
       <c r="A282" s="2" t="s">
         <v>318</v>
       </c>
@@ -15926,7 +15911,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="283" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:19" ht="29.25">
       <c r="A283" s="2" t="s">
         <v>318</v>
       </c>
@@ -15983,7 +15968,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="284" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:19" ht="29.25">
       <c r="A284" s="2" t="s">
         <v>318</v>
       </c>
@@ -16040,7 +16025,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="285" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:19" ht="29.25">
       <c r="A285" s="2" t="s">
         <v>318</v>
       </c>
@@ -16097,7 +16082,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="286" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:19" ht="29.25">
       <c r="A286" s="2" t="s">
         <v>318</v>
       </c>
@@ -16154,7 +16139,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="287" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:19" ht="29.25">
       <c r="A287" s="2" t="s">
         <v>318</v>
       </c>
@@ -16205,7 +16190,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="288" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:19" ht="29.25">
       <c r="A288" s="2" t="s">
         <v>318</v>
       </c>
@@ -16262,7 +16247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="289" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:19" ht="29.25">
       <c r="A289" s="2" t="s">
         <v>318</v>
       </c>
@@ -16319,7 +16304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="290" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:19" ht="29.25">
       <c r="A290" s="2" t="s">
         <v>318</v>
       </c>
@@ -16372,7 +16357,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="291" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:19" ht="29.25">
       <c r="A291" s="2" t="s">
         <v>318</v>
       </c>
@@ -16425,7 +16410,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="292" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:19" ht="39">
       <c r="A292" s="2" t="s">
         <v>318</v>
       </c>
@@ -16476,7 +16461,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="293" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:19" ht="39">
       <c r="A293" s="2" t="s">
         <v>318</v>
       </c>
@@ -16527,7 +16512,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="294" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:19" ht="19.5">
       <c r="A294" s="2" t="s">
         <v>350</v>
       </c>
@@ -16584,7 +16569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="295" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:19" ht="68.25">
       <c r="A295" s="2" t="s">
         <v>350</v>
       </c>
@@ -16641,7 +16626,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="296" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:19" ht="19.5">
       <c r="A296" s="2" t="s">
         <v>350</v>
       </c>
@@ -16698,7 +16683,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="297" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:19" ht="19.5">
       <c r="A297" s="2" t="s">
         <v>350</v>
       </c>
@@ -16755,7 +16740,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="298" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:19" ht="19.5">
       <c r="A298" s="2" t="s">
         <v>350</v>
       </c>
@@ -16812,7 +16797,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="299" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:19" ht="19.5">
       <c r="A299" s="2" t="s">
         <v>350</v>
       </c>
@@ -16869,7 +16854,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="300" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:19" ht="19.5">
       <c r="A300" s="2" t="s">
         <v>350</v>
       </c>
@@ -16926,7 +16911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="301" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:19" ht="19.5">
       <c r="A301" s="2" t="s">
         <v>350</v>
       </c>
@@ -16983,7 +16968,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="302" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:19" ht="19.5">
       <c r="A302" s="2" t="s">
         <v>350</v>
       </c>
@@ -17040,7 +17025,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="303" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:19" ht="19.5">
       <c r="A303" s="2" t="s">
         <v>350</v>
       </c>
@@ -17097,7 +17082,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="304" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:19" ht="19.5">
       <c r="A304" s="2" t="s">
         <v>350</v>
       </c>
@@ -17154,7 +17139,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="305" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:19" ht="19.5">
       <c r="A305" s="2" t="s">
         <v>350</v>
       </c>
@@ -17193,7 +17178,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="306" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:19" ht="19.5">
       <c r="A306" s="2" t="s">
         <v>350</v>
       </c>
@@ -17250,7 +17235,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="307" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:19" ht="39">
       <c r="A307" s="2" t="s">
         <v>350</v>
       </c>
@@ -17307,7 +17292,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="308" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:19" ht="48.75">
       <c r="A308" s="2" t="s">
         <v>350</v>
       </c>
@@ -17364,7 +17349,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="309" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:19" ht="39">
       <c r="A309" s="2" t="s">
         <v>350</v>
       </c>
@@ -17421,7 +17406,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="310" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:19" ht="39">
       <c r="A310" s="2" t="s">
         <v>350</v>
       </c>
@@ -17478,7 +17463,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="311" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:19" ht="29.25">
       <c r="A311" s="2" t="s">
         <v>350</v>
       </c>
@@ -17535,7 +17520,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="312" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:19" ht="39">
       <c r="A312" s="2" t="s">
         <v>350</v>
       </c>
@@ -17592,7 +17577,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="313" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:19" ht="29.25">
       <c r="A313" s="2" t="s">
         <v>350</v>
       </c>
@@ -17649,7 +17634,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="314" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:19" ht="29.25">
       <c r="A314" s="2" t="s">
         <v>350</v>
       </c>
@@ -17706,7 +17691,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="315" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:19" ht="39">
       <c r="A315" s="2" t="s">
         <v>350</v>
       </c>
@@ -17763,7 +17748,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="316" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:19" ht="29.25">
       <c r="A316" s="2" t="s">
         <v>350</v>
       </c>
@@ -17820,7 +17805,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="317" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:19" ht="39">
       <c r="A317" s="2" t="s">
         <v>350</v>
       </c>
@@ -17877,7 +17862,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="318" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:19" ht="29.25">
       <c r="A318" s="2" t="s">
         <v>350</v>
       </c>
@@ -17934,7 +17919,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="319" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:19" ht="29.25">
       <c r="A319" s="2" t="s">
         <v>350</v>
       </c>
@@ -17993,7 +17978,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="320" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:19" ht="39">
       <c r="A320" s="2" t="s">
         <v>350</v>
       </c>
@@ -18052,7 +18037,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="321" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:19" ht="39">
       <c r="A321" s="2" t="s">
         <v>350</v>
       </c>
@@ -18111,7 +18096,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="322" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:19" ht="68.25">
       <c r="A322" s="2" t="s">
         <v>350</v>
       </c>
@@ -18170,7 +18155,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="323" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:19" ht="58.5">
       <c r="A323" s="2" t="s">
         <v>350</v>
       </c>
@@ -18229,7 +18214,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="324" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:19" ht="68.25">
       <c r="A324" s="2" t="s">
         <v>350</v>
       </c>
@@ -18288,7 +18273,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="325" spans="1:19" ht="72" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:19" ht="68.25">
       <c r="A325" s="2" t="s">
         <v>350</v>
       </c>
@@ -18347,7 +18332,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="326" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:19" ht="39">
       <c r="A326" s="2" t="s">
         <v>350</v>
       </c>
@@ -18404,7 +18389,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="327" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:19" ht="68.25">
       <c r="A327" s="2" t="s">
         <v>350</v>
       </c>
@@ -18461,7 +18446,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="328" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:19" ht="58.5">
       <c r="A328" s="2" t="s">
         <v>350</v>
       </c>
@@ -18518,7 +18503,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="329" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:19" ht="68.25">
       <c r="A329" s="2" t="s">
         <v>350</v>
       </c>
@@ -18575,7 +18560,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="330" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:19" ht="68.25">
       <c r="A330" s="2" t="s">
         <v>350</v>
       </c>
@@ -18632,7 +18617,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="331" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:19" ht="29.25">
       <c r="A331" s="2" t="s">
         <v>391</v>
       </c>
@@ -18687,7 +18672,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="332" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:19" ht="29.25">
       <c r="A332" s="2" t="s">
         <v>391</v>
       </c>
@@ -18742,7 +18727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="333" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:19" ht="29.25">
       <c r="A333" s="2" t="s">
         <v>391</v>
       </c>
@@ -18797,7 +18782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="334" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:19" ht="29.25">
       <c r="A334" s="2" t="s">
         <v>391</v>
       </c>
@@ -18854,7 +18839,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="335" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:19" ht="29.25">
       <c r="A335" s="2" t="s">
         <v>391</v>
       </c>
@@ -18911,7 +18896,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="336" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:19" ht="29.25">
       <c r="A336" s="2" t="s">
         <v>391</v>
       </c>
@@ -18968,7 +18953,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="337" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:19" ht="29.25">
       <c r="A337" s="2" t="s">
         <v>391</v>
       </c>
@@ -19025,7 +19010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="338" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:19" ht="29.25">
       <c r="A338" s="2" t="s">
         <v>391</v>
       </c>
@@ -19082,7 +19067,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="339" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:19" ht="29.25">
       <c r="A339" s="2" t="s">
         <v>391</v>
       </c>
@@ -19139,7 +19124,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="340" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:19" ht="29.25">
       <c r="A340" s="2" t="s">
         <v>391</v>
       </c>
@@ -19196,7 +19181,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="341" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:19" ht="29.25">
       <c r="A341" s="2" t="s">
         <v>391</v>
       </c>
@@ -19253,7 +19238,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="342" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:19" ht="29.25">
       <c r="A342" s="2" t="s">
         <v>391</v>
       </c>
@@ -19310,7 +19295,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="343" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:19" ht="29.25">
       <c r="A343" s="2" t="s">
         <v>391</v>
       </c>
@@ -19367,7 +19352,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="344" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:19" ht="29.25">
       <c r="A344" s="2" t="s">
         <v>391</v>
       </c>
@@ -19424,7 +19409,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="345" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:19" ht="29.25">
       <c r="A345" s="2" t="s">
         <v>391</v>
       </c>
@@ -19481,7 +19466,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="346" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:19" ht="29.25">
       <c r="A346" s="2" t="s">
         <v>391</v>
       </c>
@@ -19538,7 +19523,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="347" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:19" ht="29.25">
       <c r="A347" s="2" t="s">
         <v>391</v>
       </c>
@@ -19595,7 +19580,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="348" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:19" ht="29.25">
       <c r="A348" s="2" t="s">
         <v>391</v>
       </c>
@@ -19652,7 +19637,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="349" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:19" ht="29.25">
       <c r="A349" s="2" t="s">
         <v>391</v>
       </c>
@@ -19709,7 +19694,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="350" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:19" ht="29.25">
       <c r="A350" s="2" t="s">
         <v>391</v>
       </c>
@@ -19766,7 +19751,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="351" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:19" ht="29.25">
       <c r="A351" s="2" t="s">
         <v>391</v>
       </c>
@@ -19823,7 +19808,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="352" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:19" ht="29.25">
       <c r="A352" s="2" t="s">
         <v>391</v>
       </c>
@@ -19880,7 +19865,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="353" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:19" ht="29.25">
       <c r="A353" s="2" t="s">
         <v>391</v>
       </c>
@@ -19937,7 +19922,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="354" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:19" ht="29.25">
       <c r="A354" s="2" t="s">
         <v>391</v>
       </c>
@@ -19994,7 +19979,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="355" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:19" ht="29.25">
       <c r="A355" s="2" t="s">
         <v>391</v>
       </c>
@@ -20051,7 +20036,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="356" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:19" ht="29.25">
       <c r="A356" s="2" t="s">
         <v>391</v>
       </c>
@@ -20108,7 +20093,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="357" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:19" ht="29.25">
       <c r="A357" s="2" t="s">
         <v>391</v>
       </c>
@@ -20165,7 +20150,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="358" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:19" ht="29.25">
       <c r="A358" s="2" t="s">
         <v>391</v>
       </c>
@@ -20220,7 +20205,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="359" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:19" ht="29.25">
       <c r="A359" s="2" t="s">
         <v>391</v>
       </c>
@@ -20277,7 +20262,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="360" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:19" ht="29.25">
       <c r="A360" s="2" t="s">
         <v>391</v>
       </c>
@@ -20334,7 +20319,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="361" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:19" ht="29.25">
       <c r="A361" s="2" t="s">
         <v>391</v>
       </c>
@@ -20391,7 +20376,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="362" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:19" ht="29.25">
       <c r="A362" s="2" t="s">
         <v>391</v>
       </c>
@@ -20448,7 +20433,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="363" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:19" ht="29.25">
       <c r="A363" s="2" t="s">
         <v>391</v>
       </c>
@@ -20505,7 +20490,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="364" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:19" ht="39">
       <c r="A364" s="2" t="s">
         <v>391</v>
       </c>
@@ -20562,7 +20547,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="365" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:19" ht="39">
       <c r="A365" s="2" t="s">
         <v>391</v>
       </c>
@@ -20619,7 +20604,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="366" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:19" ht="39">
       <c r="A366" s="2" t="s">
         <v>391</v>
       </c>
@@ -20676,7 +20661,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="367" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:19" ht="39">
       <c r="A367" s="2" t="s">
         <v>391</v>
       </c>
@@ -20733,7 +20718,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="368" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:19" ht="39">
       <c r="A368" s="2" t="s">
         <v>391</v>
       </c>
@@ -20790,7 +20775,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="369" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:19" ht="39">
       <c r="A369" s="2" t="s">
         <v>391</v>
       </c>
@@ -20847,7 +20832,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="370" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:19" ht="39">
       <c r="A370" s="2" t="s">
         <v>391</v>
       </c>
@@ -20904,7 +20889,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="371" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:19" ht="39">
       <c r="A371" s="2" t="s">
         <v>391</v>
       </c>
@@ -20961,7 +20946,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="372" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:19" ht="39">
       <c r="A372" s="2" t="s">
         <v>424</v>
       </c>
@@ -21018,7 +21003,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="373" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:19" ht="39">
       <c r="A373" s="2" t="s">
         <v>424</v>
       </c>
@@ -21075,7 +21060,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="374" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:19" ht="39">
       <c r="A374" s="2" t="s">
         <v>424</v>
       </c>
@@ -21132,7 +21117,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="375" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:19" ht="48.75">
       <c r="A375" s="2" t="s">
         <v>424</v>
       </c>
@@ -21191,7 +21176,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="376" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:19" ht="39">
       <c r="A376" s="2" t="s">
         <v>424</v>
       </c>
@@ -21236,7 +21221,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="377" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:19" ht="39">
       <c r="A377" s="2" t="s">
         <v>424</v>
       </c>
@@ -21281,7 +21266,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="378" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:19" ht="39">
       <c r="A378" s="2" t="s">
         <v>424</v>
       </c>
@@ -21326,7 +21311,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="379" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:19" ht="39">
       <c r="A379" s="2" t="s">
         <v>424</v>
       </c>
@@ -21379,7 +21364,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="380" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:19" ht="39">
       <c r="A380" s="2" t="s">
         <v>424</v>
       </c>
@@ -21424,7 +21409,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="381" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:19" ht="39">
       <c r="A381" s="2" t="s">
         <v>424</v>
       </c>
@@ -21483,7 +21468,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="382" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:19" ht="48.75">
       <c r="A382" s="2" t="s">
         <v>424</v>
       </c>
@@ -21542,7 +21527,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="383" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:19" ht="29.25">
       <c r="A383" s="2" t="s">
         <v>444</v>
       </c>
@@ -21599,7 +21584,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="384" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:19" ht="29.25">
       <c r="A384" s="2" t="s">
         <v>444</v>
       </c>
@@ -21656,7 +21641,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="385" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:19" ht="39">
       <c r="A385" s="2" t="s">
         <v>444</v>
       </c>
@@ -21715,7 +21700,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="386" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:19" ht="39">
       <c r="A386" s="2" t="s">
         <v>444</v>
       </c>
@@ -21770,7 +21755,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="387" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:19" ht="48.75">
       <c r="A387" s="2" t="s">
         <v>444</v>
       </c>
@@ -21829,7 +21814,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="388" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:19" ht="29.25">
       <c r="A388" s="2" t="s">
         <v>444</v>
       </c>
@@ -21882,7 +21867,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="389" spans="1:19" ht="54" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:19" ht="58.5">
       <c r="A389" s="2" t="s">
         <v>454</v>
       </c>
@@ -21941,7 +21926,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="390" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:19" ht="39">
       <c r="A390" s="2" t="s">
         <v>454</v>
       </c>
@@ -22000,7 +21985,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="391" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:19" ht="48.75">
       <c r="A391" s="2" t="s">
         <v>454</v>
       </c>
@@ -22059,7 +22044,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="392" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:19" ht="48.75">
       <c r="A392" s="2" t="s">
         <v>454</v>
       </c>
@@ -22118,7 +22103,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="393" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:19" ht="58.5">
       <c r="A393" s="2" t="s">
         <v>454</v>
       </c>
@@ -22175,7 +22160,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="394" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:19" ht="19.5">
       <c r="A394" s="2" t="s">
         <v>464</v>
       </c>
@@ -22234,7 +22219,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="395" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:19" ht="19.5">
       <c r="A395" s="2" t="s">
         <v>464</v>
       </c>
@@ -22293,7 +22278,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="396" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:19" ht="39">
       <c r="A396" s="2" t="s">
         <v>464</v>
       </c>
@@ -22350,7 +22335,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="397" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:19" ht="19.5">
       <c r="A397" s="2" t="s">
         <v>464</v>
       </c>
@@ -22391,7 +22376,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="398" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:19" ht="19.5">
       <c r="A398" s="2" t="s">
         <v>464</v>
       </c>
@@ -22424,7 +22409,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="399" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:19" ht="19.5">
       <c r="A399" s="2" t="s">
         <v>464</v>
       </c>
@@ -22457,7 +22442,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="400" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:19" ht="19.5">
       <c r="A400" s="2" t="s">
         <v>464</v>
       </c>
@@ -22490,7 +22475,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="401" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:19" ht="19.5">
       <c r="A401" s="2" t="s">
         <v>464</v>
       </c>
@@ -22531,7 +22516,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="402" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:19" ht="19.5">
       <c r="A402" s="2" t="s">
         <v>464</v>
       </c>
@@ -22572,7 +22557,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="403" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:19" ht="19.5">
       <c r="A403" s="2" t="s">
         <v>464</v>
       </c>
@@ -22613,7 +22598,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="404" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:19" ht="29.25">
       <c r="A404" s="2" t="s">
         <v>464</v>
       </c>
@@ -22672,7 +22657,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="405" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:19" ht="19.5">
       <c r="A405" s="2" t="s">
         <v>464</v>
       </c>
@@ -22729,7 +22714,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="406" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:19" ht="29.25">
       <c r="A406" s="2" t="s">
         <v>464</v>
       </c>
@@ -22788,7 +22773,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="407" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:19" ht="29.25">
       <c r="A407" s="2" t="s">
         <v>464</v>
       </c>
@@ -22841,7 +22826,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="408" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:19" ht="29.25">
       <c r="A408" s="2" t="s">
         <v>464</v>
       </c>
@@ -22894,7 +22879,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="409" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:19" ht="19.5">
       <c r="A409" s="2" t="s">
         <v>464</v>
       </c>
@@ -22951,7 +22936,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="410" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:19" ht="29.25">
       <c r="A410" s="2" t="s">
         <v>485</v>
       </c>
@@ -23008,7 +22993,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="411" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:19" ht="29.25">
       <c r="A411" s="2" t="s">
         <v>485</v>
       </c>
@@ -23067,7 +23052,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="412" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:19" ht="29.25">
       <c r="A412" s="2" t="s">
         <v>485</v>
       </c>
@@ -23110,7 +23095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="413" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:19" ht="29.25">
       <c r="A413" s="2" t="s">
         <v>485</v>
       </c>
@@ -23163,7 +23148,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="414" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:19" ht="29.25">
       <c r="A414" s="2" t="s">
         <v>485</v>
       </c>
@@ -23210,7 +23195,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="415" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:19" ht="29.25">
       <c r="A415" s="2" t="s">
         <v>485</v>
       </c>
@@ -23257,7 +23242,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="416" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:19" ht="29.25">
       <c r="A416" s="2" t="s">
         <v>485</v>
       </c>
@@ -23304,7 +23289,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="417" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:19" ht="29.25">
       <c r="A417" s="2" t="s">
         <v>485</v>
       </c>
@@ -23351,7 +23336,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="418" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:19" ht="29.25">
       <c r="A418" s="2" t="s">
         <v>485</v>
       </c>
@@ -23398,7 +23383,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="419" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:19" ht="29.25">
       <c r="A419" s="2" t="s">
         <v>485</v>
       </c>
@@ -23445,7 +23430,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="420" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:19" ht="39">
       <c r="A420" s="2" t="s">
         <v>485</v>
       </c>
@@ -23492,7 +23477,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="421" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:19" ht="48.75">
       <c r="A421" s="2" t="s">
         <v>485</v>
       </c>
@@ -23539,7 +23524,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="422" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:19" ht="39">
       <c r="A422" s="2" t="s">
         <v>485</v>
       </c>
@@ -23586,7 +23571,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="423" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:19" ht="39">
       <c r="A423" s="2" t="s">
         <v>485</v>
       </c>
@@ -23633,7 +23618,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="424" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:19" ht="29.25">
       <c r="A424" s="2" t="s">
         <v>485</v>
       </c>
@@ -23690,7 +23675,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="425" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:19" ht="29.25">
       <c r="A425" s="2" t="s">
         <v>485</v>
       </c>
@@ -23747,7 +23732,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="426" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:19" ht="29.25">
       <c r="A426" s="2" t="s">
         <v>485</v>
       </c>
@@ -23804,7 +23789,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="427" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:19" ht="29.25">
       <c r="A427" s="2" t="s">
         <v>485</v>
       </c>
@@ -23861,7 +23846,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="428" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:19" ht="29.25">
       <c r="A428" s="2" t="s">
         <v>485</v>
       </c>
@@ -23918,7 +23903,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="429" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:19" ht="29.25">
       <c r="A429" s="2" t="s">
         <v>485</v>
       </c>
@@ -23977,7 +23962,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="430" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:19" ht="39">
       <c r="A430" s="2" t="s">
         <v>485</v>
       </c>
@@ -24016,7 +24001,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="431" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:19" ht="39">
       <c r="A431" s="2" t="s">
         <v>485</v>
       </c>
@@ -24055,7 +24040,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="432" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:19" ht="39">
       <c r="A432" s="2" t="s">
         <v>485</v>
       </c>
@@ -24094,7 +24079,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="433" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:19" ht="39">
       <c r="A433" s="2" t="s">
         <v>485</v>
       </c>
@@ -24133,7 +24118,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="434" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:19" ht="39">
       <c r="A434" s="2" t="s">
         <v>485</v>
       </c>
@@ -24172,7 +24157,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="435" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:19" ht="39">
       <c r="A435" s="2" t="s">
         <v>485</v>
       </c>
@@ -24211,7 +24196,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="436" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:19" ht="39">
       <c r="A436" s="2" t="s">
         <v>485</v>
       </c>
@@ -24250,7 +24235,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="437" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:19" ht="39">
       <c r="A437" s="2" t="s">
         <v>485</v>
       </c>
@@ -24289,7 +24274,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="438" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:19" ht="39">
       <c r="A438" s="2" t="s">
         <v>485</v>
       </c>
@@ -24328,7 +24313,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="439" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:19" ht="39">
       <c r="A439" s="2" t="s">
         <v>485</v>
       </c>
@@ -24367,7 +24352,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="440" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:19" ht="39">
       <c r="A440" s="2" t="s">
         <v>485</v>
       </c>
@@ -24406,7 +24391,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="441" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:19" ht="39">
       <c r="A441" s="2" t="s">
         <v>485</v>
       </c>
@@ -24445,7 +24430,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="442" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:19" ht="29.25">
       <c r="A442" s="2" t="s">
         <v>485</v>
       </c>
@@ -24504,7 +24489,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="443" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:19" ht="29.25">
       <c r="A443" s="2" t="s">
         <v>485</v>
       </c>
@@ -24543,7 +24528,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="444" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:19" ht="29.25">
       <c r="A444" s="2" t="s">
         <v>522</v>
       </c>
@@ -24602,7 +24587,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="445" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:19" ht="29.25">
       <c r="A445" s="2" t="s">
         <v>522</v>
       </c>
@@ -24661,7 +24646,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="446" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:19" ht="29.25">
       <c r="A446" s="2" t="s">
         <v>522</v>
       </c>
@@ -24720,7 +24705,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="447" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:19" ht="29.25">
       <c r="A447" s="2" t="s">
         <v>522</v>
       </c>
@@ -24779,7 +24764,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="448" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:19" ht="48.75">
       <c r="A448" s="2" t="s">
         <v>522</v>
       </c>
@@ -24838,7 +24823,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="449" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:19" ht="29.25">
       <c r="A449" s="2" t="s">
         <v>522</v>
       </c>
@@ -24897,7 +24882,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="450" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:19" ht="29.25">
       <c r="A450" s="2" t="s">
         <v>522</v>
       </c>
@@ -24954,7 +24939,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="451" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:19" ht="29.25">
       <c r="A451" s="2" t="s">
         <v>522</v>
       </c>
@@ -25013,7 +24998,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="452" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:19" ht="29.25">
       <c r="A452" s="2" t="s">
         <v>522</v>
       </c>
@@ -25072,7 +25057,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="453" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:19" ht="29.25">
       <c r="A453" s="2" t="s">
         <v>522</v>
       </c>
@@ -25131,7 +25116,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="454" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:19" ht="29.25">
       <c r="A454" s="2" t="s">
         <v>522</v>
       </c>
@@ -25188,7 +25173,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="455" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:19" ht="29.25">
       <c r="A455" s="2" t="s">
         <v>522</v>
       </c>
@@ -25247,7 +25232,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="456" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:19" ht="29.25">
       <c r="A456" s="2" t="s">
         <v>522</v>
       </c>
@@ -25306,7 +25291,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="457" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:19" ht="29.25">
       <c r="A457" s="2" t="s">
         <v>522</v>
       </c>
@@ -25365,7 +25350,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="458" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:19" ht="29.25">
       <c r="A458" s="2" t="s">
         <v>522</v>
       </c>
@@ -25424,7 +25409,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="459" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:19" ht="48.75">
       <c r="A459" s="2" t="s">
         <v>522</v>
       </c>
@@ -25483,7 +25468,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="460" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:19" ht="29.25">
       <c r="A460" s="2" t="s">
         <v>522</v>
       </c>
@@ -25542,7 +25527,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="461" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:19" ht="39">
       <c r="A461" s="2" t="s">
         <v>522</v>
       </c>
@@ -25601,7 +25586,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="462" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:19" ht="39">
       <c r="A462" s="2" t="s">
         <v>522</v>
       </c>
@@ -25660,7 +25645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="463" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:19" ht="29.25">
       <c r="A463" s="2" t="s">
         <v>522</v>
       </c>
@@ -25705,7 +25690,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="464" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:19" ht="29.25">
       <c r="A464" s="2" t="s">
         <v>522</v>
       </c>
@@ -25764,7 +25749,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="465" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:19" ht="29.25">
       <c r="A465" s="2" t="s">
         <v>522</v>
       </c>
@@ -25823,7 +25808,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="466" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:19" ht="29.25">
       <c r="A466" s="2" t="s">
         <v>522</v>
       </c>
@@ -25876,7 +25861,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="467" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:19" ht="39">
       <c r="A467" s="2" t="s">
         <v>522</v>
       </c>
@@ -25913,7 +25898,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="468" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:19" ht="39">
       <c r="A468" s="2" t="s">
         <v>522</v>
       </c>
@@ -25972,7 +25957,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="469" spans="1:19" ht="36" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:19" ht="39">
       <c r="A469" s="2" t="s">
         <v>522</v>
       </c>
@@ -26031,9 +26016,9 @@
         <v>557</v>
       </c>
     </row>
-    <row r="470" spans="1:19" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:19" ht="0" hidden="1" customHeight="1"/>
+    <row r="471" spans="1:19" ht="18" customHeight="1"/>
+    <row r="472" spans="1:19" ht="17.100000000000001" customHeight="1">
       <c r="A472" s="12" t="s">
         <v>560</v>
       </c>

</xml_diff>

<commit_message>
Zlecenie 25.10.2023 - aktualizacja plików excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -1705,7 +1705,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 24-10-2023, 11:45</t>
+    <t>Last update: 26-10-2023, 13:18</t>
   </si>
 </sst>
 </file>
@@ -25737,10 +25737,10 @@
         <v>51.3</v>
       </c>
       <c r="L461" s="4">
-        <v>54.2</v>
+        <v>54.5</v>
       </c>
       <c r="M461" s="4">
-        <v>50.6</v>
+        <v>50.8</v>
       </c>
       <c r="N461" s="4">
         <v>48.7</v>
@@ -25755,7 +25755,7 @@
         <v>53.6</v>
       </c>
       <c r="R461" s="4">
-        <v>49.1</v>
+        <v>49.3</v>
       </c>
       <c r="S461" s="2" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Okno serwisowe 27.02.2024 - aktualizacja API i plików excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dregerj\Documents\SDG\sdg_git_produkcja\sdg-indicators-pl\assets\excel\en\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1720,7 +1720,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 09-02-2024, 11:15</t>
+    <t>Last update: 27-02-2024, 09:05</t>
   </si>
 </sst>
 </file>
@@ -1735,7 +1735,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2272,10 +2272,10 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2287,17 +2287,17 @@
     <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="36" customHeight="1">
+    <row r="1" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:20" ht="25.5">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.5">
+    <row r="4" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.5">
+    <row r="14" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.5">
+    <row r="15" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="29.25">
+    <row r="17" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="97.5">
+    <row r="18" spans="1:20" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="97.5">
+    <row r="19" spans="1:20" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="97.5">
+    <row r="20" spans="1:20" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="19.5">
+    <row r="21" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="29.25">
+    <row r="22" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="29.25">
+    <row r="23" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="29.25">
+    <row r="24" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="68.25">
+    <row r="25" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="29.25">
+    <row r="26" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="29.25">
+    <row r="27" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>21</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="29.25">
+    <row r="28" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="39">
+    <row r="29" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="39">
+    <row r="30" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -3907,7 +3907,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="39">
+    <row r="31" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="39">
+    <row r="32" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="19.5">
+    <row r="33" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>67</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="29.25">
+    <row r="34" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>67</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="29.25">
+    <row r="35" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>67</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="29.25">
+    <row r="36" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="29.25">
+    <row r="37" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="29.25">
+    <row r="38" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>67</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="29.25">
+    <row r="39" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>67</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="39">
+    <row r="40" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>67</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="97.5">
+    <row r="41" spans="1:20" ht="81" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>67</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="97.5">
+    <row r="42" spans="1:20" ht="81" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>67</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="97.5">
+    <row r="43" spans="1:20" ht="81" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>67</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="97.5">
+    <row r="44" spans="1:20" ht="81" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>67</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="97.5">
+    <row r="45" spans="1:20" ht="81" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>67</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="97.5">
+    <row r="46" spans="1:20" ht="81" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>67</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="48.75">
+    <row r="47" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>67</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="48.75">
+    <row r="48" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>67</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="19.5">
+    <row r="49" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>67</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="29.25">
+    <row r="50" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>67</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="19.5">
+    <row r="51" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>96</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="19.5">
+    <row r="52" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>96</v>
       </c>
@@ -5115,7 +5115,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="19.5">
+    <row r="53" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>96</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="19.5">
+    <row r="54" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>96</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="19.5">
+    <row r="55" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>96</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="19.5">
+    <row r="56" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>96</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="19.5">
+    <row r="57" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>96</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="19.5">
+    <row r="58" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>96</v>
       </c>
@@ -5475,7 +5475,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="29.25">
+    <row r="59" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>96</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="19.5">
+    <row r="60" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>96</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="29.25">
+    <row r="61" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>96</v>
       </c>
@@ -5655,7 +5655,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="29.25">
+    <row r="62" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>96</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="29.25">
+    <row r="63" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>96</v>
       </c>
@@ -5775,7 +5775,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="19.5">
+    <row r="64" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>96</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="29.25">
+    <row r="65" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>96</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="29.25">
+    <row r="66" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>96</v>
       </c>
@@ -5955,7 +5955,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="29.25">
+    <row r="67" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>96</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="29.25">
+    <row r="68" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>96</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="29.25">
+    <row r="69" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>96</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="29.25">
+    <row r="70" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>96</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="29.25">
+    <row r="71" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>96</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="19.5">
+    <row r="72" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>96</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="19.5">
+    <row r="73" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>96</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="19.5">
+    <row r="74" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>96</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="19.5">
+    <row r="75" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>96</v>
       </c>
@@ -6481,7 +6481,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="29.25">
+    <row r="76" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>96</v>
       </c>
@@ -6541,7 +6541,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="29.25">
+    <row r="77" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>96</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="19.5">
+    <row r="78" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>96</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="19.5">
+    <row r="79" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>96</v>
       </c>
@@ -6701,7 +6701,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="19.5">
+    <row r="80" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>96</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="19.5">
+    <row r="81" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>96</v>
       </c>
@@ -6805,7 +6805,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="29.25">
+    <row r="82" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>96</v>
       </c>
@@ -6863,7 +6863,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="29.25">
+    <row r="83" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>96</v>
       </c>
@@ -6921,7 +6921,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="19.5">
+    <row r="84" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>96</v>
       </c>
@@ -6957,7 +6957,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="29.25">
+    <row r="85" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>96</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="19.5">
+    <row r="86" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>96</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="19.5">
+    <row r="87" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>96</v>
       </c>
@@ -7091,7 +7091,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="19.5">
+    <row r="88" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>96</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="19.5">
+    <row r="89" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>96</v>
       </c>
@@ -7211,7 +7211,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="19.5">
+    <row r="90" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>96</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="29.25">
+    <row r="91" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>96</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="19.5">
+    <row r="92" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>96</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="19.5">
+    <row r="93" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>96</v>
       </c>
@@ -7393,7 +7393,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="19.5">
+    <row r="94" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>96</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="19.5">
+    <row r="95" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>96</v>
       </c>
@@ -7491,7 +7491,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="78">
+    <row r="96" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>150</v>
       </c>
@@ -7522,14 +7522,16 @@
       <c r="N96" s="3"/>
       <c r="O96" s="3"/>
       <c r="P96" s="3"/>
-      <c r="Q96" s="3"/>
+      <c r="Q96" s="4">
+        <v>97.2</v>
+      </c>
       <c r="R96" s="3"/>
       <c r="S96" s="3"/>
       <c r="T96" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="78">
+    <row r="97" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>150</v>
       </c>
@@ -7560,14 +7562,16 @@
       <c r="N97" s="3"/>
       <c r="O97" s="3"/>
       <c r="P97" s="3"/>
-      <c r="Q97" s="3"/>
+      <c r="Q97" s="4">
+        <v>96.5</v>
+      </c>
       <c r="R97" s="3"/>
       <c r="S97" s="3"/>
       <c r="T97" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="78">
+    <row r="98" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>150</v>
       </c>
@@ -7598,14 +7602,16 @@
       <c r="N98" s="3"/>
       <c r="O98" s="3"/>
       <c r="P98" s="3"/>
-      <c r="Q98" s="3"/>
+      <c r="Q98" s="4">
+        <v>98.1</v>
+      </c>
       <c r="R98" s="3"/>
       <c r="S98" s="3"/>
       <c r="T98" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="78">
+    <row r="99" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>150</v>
       </c>
@@ -7641,13 +7647,15 @@
       <c r="O99" s="3"/>
       <c r="P99" s="3"/>
       <c r="Q99" s="3"/>
-      <c r="R99" s="3"/>
+      <c r="R99" s="4">
+        <v>77.8</v>
+      </c>
       <c r="S99" s="3"/>
       <c r="T99" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="78">
+    <row r="100" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>150</v>
       </c>
@@ -7683,13 +7691,15 @@
       <c r="O100" s="3"/>
       <c r="P100" s="3"/>
       <c r="Q100" s="3"/>
-      <c r="R100" s="3"/>
+      <c r="R100" s="4">
+        <v>72.5</v>
+      </c>
       <c r="S100" s="3"/>
       <c r="T100" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="78">
+    <row r="101" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>150</v>
       </c>
@@ -7725,13 +7735,15 @@
       <c r="O101" s="3"/>
       <c r="P101" s="3"/>
       <c r="Q101" s="3"/>
-      <c r="R101" s="3"/>
+      <c r="R101" s="4">
+        <v>83.2</v>
+      </c>
       <c r="S101" s="3"/>
       <c r="T101" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="78">
+    <row r="102" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>150</v>
       </c>
@@ -7767,13 +7779,15 @@
       <c r="O102" s="3"/>
       <c r="P102" s="3"/>
       <c r="Q102" s="3"/>
-      <c r="R102" s="3"/>
+      <c r="R102" s="4">
+        <v>77</v>
+      </c>
       <c r="S102" s="3"/>
       <c r="T102" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="78">
+    <row r="103" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>150</v>
       </c>
@@ -7809,13 +7823,15 @@
       <c r="O103" s="3"/>
       <c r="P103" s="3"/>
       <c r="Q103" s="3"/>
-      <c r="R103" s="3"/>
+      <c r="R103" s="4">
+        <v>76.2</v>
+      </c>
       <c r="S103" s="3"/>
       <c r="T103" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="78">
+    <row r="104" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>150</v>
       </c>
@@ -7851,13 +7867,15 @@
       <c r="O104" s="3"/>
       <c r="P104" s="3"/>
       <c r="Q104" s="3"/>
-      <c r="R104" s="3"/>
+      <c r="R104" s="4">
+        <v>77.8</v>
+      </c>
       <c r="S104" s="3"/>
       <c r="T104" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="29.25">
+    <row r="105" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>150</v>
       </c>
@@ -7895,7 +7913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="19.5">
+    <row r="106" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>150</v>
       </c>
@@ -7955,7 +7973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="19.5">
+    <row r="107" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>150</v>
       </c>
@@ -8015,7 +8033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="19.5">
+    <row r="108" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>150</v>
       </c>
@@ -8075,7 +8093,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="19.5">
+    <row r="109" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>150</v>
       </c>
@@ -8113,7 +8131,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="19.5">
+    <row r="110" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>150</v>
       </c>
@@ -8151,7 +8169,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="19.5">
+    <row r="111" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>150</v>
       </c>
@@ -8189,7 +8207,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="29.25">
+    <row r="112" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>150</v>
       </c>
@@ -8235,7 +8253,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="19.5">
+    <row r="113" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>150</v>
       </c>
@@ -8285,7 +8303,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="39">
+    <row r="114" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>150</v>
       </c>
@@ -8335,7 +8353,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="48.75">
+    <row r="115" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>150</v>
       </c>
@@ -8385,7 +8403,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="58.5">
+    <row r="116" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>150</v>
       </c>
@@ -8435,7 +8453,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="29.25">
+    <row r="117" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>150</v>
       </c>
@@ -8485,7 +8503,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="29.25">
+    <row r="118" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>150</v>
       </c>
@@ -8531,7 +8549,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="19.5">
+    <row r="119" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>150</v>
       </c>
@@ -8581,7 +8599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="39">
+    <row r="120" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>150</v>
       </c>
@@ -8631,7 +8649,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="48.75">
+    <row r="121" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>150</v>
       </c>
@@ -8681,7 +8699,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="58.5">
+    <row r="122" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>150</v>
       </c>
@@ -8731,7 +8749,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="29.25">
+    <row r="123" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>150</v>
       </c>
@@ -8781,7 +8799,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="48.75">
+    <row r="124" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>150</v>
       </c>
@@ -8815,13 +8833,15 @@
       <c r="O124" s="3"/>
       <c r="P124" s="3"/>
       <c r="Q124" s="3"/>
-      <c r="R124" s="3"/>
+      <c r="R124" s="5">
+        <v>1.02</v>
+      </c>
       <c r="S124" s="3"/>
       <c r="T124" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="48.75">
+    <row r="125" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>150</v>
       </c>
@@ -8855,13 +8875,15 @@
       <c r="O125" s="3"/>
       <c r="P125" s="3"/>
       <c r="Q125" s="3"/>
-      <c r="R125" s="3"/>
+      <c r="R125" s="5">
+        <v>1.1499999999999999</v>
+      </c>
       <c r="S125" s="3"/>
       <c r="T125" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="29.25">
+    <row r="126" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>150</v>
       </c>
@@ -8921,7 +8943,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="29.25">
+    <row r="127" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>150</v>
       </c>
@@ -8957,7 +8979,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="29.25">
+    <row r="128" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>150</v>
       </c>
@@ -8993,7 +9015,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="29.25">
+    <row r="129" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>150</v>
       </c>
@@ -9029,7 +9051,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="29.25">
+    <row r="130" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>150</v>
       </c>
@@ -9065,7 +9087,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="29.25">
+    <row r="131" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>150</v>
       </c>
@@ -9101,7 +9123,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="29.25">
+    <row r="132" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>150</v>
       </c>
@@ -9137,7 +9159,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="29.25">
+    <row r="133" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>150</v>
       </c>
@@ -9173,7 +9195,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="29.25">
+    <row r="134" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>150</v>
       </c>
@@ -9209,7 +9231,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="29.25">
+    <row r="135" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>150</v>
       </c>
@@ -9245,7 +9267,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="29.25">
+    <row r="136" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>150</v>
       </c>
@@ -9281,7 +9303,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="29.25">
+    <row r="137" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>150</v>
       </c>
@@ -9317,7 +9339,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="29.25">
+    <row r="138" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>150</v>
       </c>
@@ -9353,7 +9375,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="29.25">
+    <row r="139" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>150</v>
       </c>
@@ -9389,7 +9411,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="29.25">
+    <row r="140" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>150</v>
       </c>
@@ -9425,7 +9447,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="29.25">
+    <row r="141" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>150</v>
       </c>
@@ -9461,7 +9483,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="29.25">
+    <row r="142" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>150</v>
       </c>
@@ -9497,7 +9519,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="48.75">
+    <row r="143" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>150</v>
       </c>
@@ -9559,7 +9581,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="58.5">
+    <row r="144" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>150</v>
       </c>
@@ -9621,7 +9643,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="58.5">
+    <row r="145" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>150</v>
       </c>
@@ -9657,7 +9679,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="58.5">
+    <row r="146" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>150</v>
       </c>
@@ -9693,7 +9715,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="58.5">
+    <row r="147" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>150</v>
       </c>
@@ -9755,7 +9777,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="58.5">
+    <row r="148" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>150</v>
       </c>
@@ -9817,7 +9839,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="58.5">
+    <row r="149" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>150</v>
       </c>
@@ -9879,7 +9901,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="29.25">
+    <row r="150" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>150</v>
       </c>
@@ -9933,7 +9955,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="58.5">
+    <row r="151" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>150</v>
       </c>
@@ -9989,7 +10011,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="58.5">
+    <row r="152" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>150</v>
       </c>
@@ -10045,7 +10067,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="58.5">
+    <row r="153" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>150</v>
       </c>
@@ -10101,7 +10123,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="58.5">
+    <row r="154" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>150</v>
       </c>
@@ -10157,7 +10179,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="29.25">
+    <row r="155" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>206</v>
       </c>
@@ -10193,7 +10215,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="19.5">
+    <row r="156" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>206</v>
       </c>
@@ -10253,7 +10275,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="39">
+    <row r="157" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>206</v>
       </c>
@@ -10289,7 +10311,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="39">
+    <row r="158" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>206</v>
       </c>
@@ -10325,7 +10347,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="39">
+    <row r="159" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>206</v>
       </c>
@@ -10361,7 +10383,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="39">
+    <row r="160" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>206</v>
       </c>
@@ -10397,7 +10419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="39">
+    <row r="161" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>206</v>
       </c>
@@ -10433,7 +10455,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="19.5">
+    <row r="162" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>206</v>
       </c>
@@ -10469,7 +10491,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="19.5">
+    <row r="163" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>206</v>
       </c>
@@ -10505,7 +10527,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="19.5">
+    <row r="164" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>206</v>
       </c>
@@ -10541,7 +10563,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="19.5">
+    <row r="165" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>206</v>
       </c>
@@ -10577,7 +10599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="19.5">
+    <row r="166" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>206</v>
       </c>
@@ -10613,7 +10635,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="19.5">
+    <row r="167" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>206</v>
       </c>
@@ -10649,7 +10671,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="19.5">
+    <row r="168" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>206</v>
       </c>
@@ -10685,7 +10707,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="19.5">
+    <row r="169" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>206</v>
       </c>
@@ -10721,7 +10743,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="29.25">
+    <row r="170" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>206</v>
       </c>
@@ -10763,7 +10785,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="29.25">
+    <row r="171" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>206</v>
       </c>
@@ -10805,7 +10827,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="29.25">
+    <row r="172" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>206</v>
       </c>
@@ -10865,7 +10887,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="29.25">
+    <row r="173" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>206</v>
       </c>
@@ -10925,7 +10947,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="29.25">
+    <row r="174" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>206</v>
       </c>
@@ -10985,7 +11007,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="29.25">
+    <row r="175" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>206</v>
       </c>
@@ -11045,7 +11067,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="29.25">
+    <row r="176" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>206</v>
       </c>
@@ -11105,7 +11127,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="19.5">
+    <row r="177" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>206</v>
       </c>
@@ -11151,7 +11173,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="39">
+    <row r="178" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>206</v>
       </c>
@@ -11197,7 +11219,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="19.5">
+    <row r="179" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>206</v>
       </c>
@@ -11243,7 +11265,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="39">
+    <row r="180" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>206</v>
       </c>
@@ -11289,7 +11311,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="39">
+    <row r="181" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>206</v>
       </c>
@@ -11335,7 +11357,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="39">
+    <row r="182" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>206</v>
       </c>
@@ -11381,7 +11403,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="39">
+    <row r="183" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>206</v>
       </c>
@@ -11427,7 +11449,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="39">
+    <row r="184" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>206</v>
       </c>
@@ -11467,7 +11489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="39">
+    <row r="185" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>206</v>
       </c>
@@ -11507,7 +11529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="39">
+    <row r="186" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>206</v>
       </c>
@@ -11547,7 +11569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="39">
+    <row r="187" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>206</v>
       </c>
@@ -11587,7 +11609,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="39">
+    <row r="188" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>206</v>
       </c>
@@ -11627,7 +11649,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="39">
+    <row r="189" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>206</v>
       </c>
@@ -11667,7 +11689,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="39">
+    <row r="190" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>206</v>
       </c>
@@ -11707,7 +11729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="39">
+    <row r="191" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>206</v>
       </c>
@@ -11747,7 +11769,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="39">
+    <row r="192" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>206</v>
       </c>
@@ -11787,7 +11809,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="39">
+    <row r="193" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>206</v>
       </c>
@@ -11827,7 +11849,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="39">
+    <row r="194" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>206</v>
       </c>
@@ -11867,7 +11889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="39">
+    <row r="195" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>206</v>
       </c>
@@ -11907,7 +11929,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="19.5">
+    <row r="196" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>206</v>
       </c>
@@ -11949,7 +11971,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="19.5">
+    <row r="197" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>206</v>
       </c>
@@ -12007,7 +12029,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="19.5">
+    <row r="198" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>206</v>
       </c>
@@ -12065,7 +12087,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="19.5">
+    <row r="199" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>246</v>
       </c>
@@ -12123,7 +12145,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="29.25">
+    <row r="200" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>246</v>
       </c>
@@ -12181,7 +12203,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="19.5">
+    <row r="201" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>246</v>
       </c>
@@ -12241,7 +12263,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="19.5">
+    <row r="202" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>246</v>
       </c>
@@ -12279,7 +12301,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="19.5">
+    <row r="203" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>246</v>
       </c>
@@ -12317,7 +12339,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="29.25">
+    <row r="204" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>246</v>
       </c>
@@ -12375,7 +12397,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="19.5">
+    <row r="205" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>246</v>
       </c>
@@ -12431,7 +12453,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="19.5">
+    <row r="206" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>246</v>
       </c>
@@ -12477,7 +12499,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="29.25">
+    <row r="207" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>246</v>
       </c>
@@ -12537,7 +12559,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="29.25">
+    <row r="208" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>246</v>
       </c>
@@ -12591,7 +12613,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="39">
+    <row r="209" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>246</v>
       </c>
@@ -12651,7 +12673,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="19.5">
+    <row r="210" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>267</v>
       </c>
@@ -12687,7 +12709,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="19.5">
+    <row r="211" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>267</v>
       </c>
@@ -12745,7 +12767,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="29.25">
+    <row r="212" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>267</v>
       </c>
@@ -12801,7 +12823,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="29.25">
+    <row r="213" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>267</v>
       </c>
@@ -12855,7 +12877,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="29.25">
+    <row r="214" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>273</v>
       </c>
@@ -12915,7 +12937,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="29.25">
+    <row r="215" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>273</v>
       </c>
@@ -12975,7 +12997,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="29.25">
+    <row r="216" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>273</v>
       </c>
@@ -13015,7 +13037,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="29.25">
+    <row r="217" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>273</v>
       </c>
@@ -13055,7 +13077,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="29.25">
+    <row r="218" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>273</v>
       </c>
@@ -13095,7 +13117,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="29.25">
+    <row r="219" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>273</v>
       </c>
@@ -13155,7 +13177,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="29.25">
+    <row r="220" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>273</v>
       </c>
@@ -13215,7 +13237,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="29.25">
+    <row r="221" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>273</v>
       </c>
@@ -13275,7 +13297,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="29.25">
+    <row r="222" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>273</v>
       </c>
@@ -13321,7 +13343,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="29.25">
+    <row r="223" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>273</v>
       </c>
@@ -13367,7 +13389,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="29.25">
+    <row r="224" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>273</v>
       </c>
@@ -13413,7 +13435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="29.25">
+    <row r="225" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>273</v>
       </c>
@@ -13459,7 +13481,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="29.25">
+    <row r="226" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>273</v>
       </c>
@@ -13505,7 +13527,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="29.25">
+    <row r="227" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>273</v>
       </c>
@@ -13551,7 +13573,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="29.25">
+    <row r="228" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>273</v>
       </c>
@@ -13597,7 +13619,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="29.25">
+    <row r="229" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>273</v>
       </c>
@@ -13643,7 +13665,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="39">
+    <row r="230" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>273</v>
       </c>
@@ -13689,7 +13711,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="29.25">
+    <row r="231" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>273</v>
       </c>
@@ -13735,7 +13757,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="39">
+    <row r="232" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>273</v>
       </c>
@@ -13781,7 +13803,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="29.25">
+    <row r="233" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>273</v>
       </c>
@@ -13827,7 +13849,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="29.25">
+    <row r="234" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>273</v>
       </c>
@@ -13873,7 +13895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="29.25">
+    <row r="235" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>273</v>
       </c>
@@ -13919,7 +13941,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="29.25">
+    <row r="236" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>273</v>
       </c>
@@ -13965,7 +13987,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="29.25">
+    <row r="237" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>273</v>
       </c>
@@ -14011,7 +14033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="29.25">
+    <row r="238" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>273</v>
       </c>
@@ -14057,7 +14079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="29.25">
+    <row r="239" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>273</v>
       </c>
@@ -14103,7 +14125,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="29.25">
+    <row r="240" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>273</v>
       </c>
@@ -14149,7 +14171,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="29.25">
+    <row r="241" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>273</v>
       </c>
@@ -14209,7 +14231,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="29.25">
+    <row r="242" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>273</v>
       </c>
@@ -14269,7 +14291,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="243" spans="1:20" ht="29.25">
+    <row r="243" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>273</v>
       </c>
@@ -14329,7 +14351,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="29.25">
+    <row r="244" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>273</v>
       </c>
@@ -14389,7 +14411,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="29.25">
+    <row r="245" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>273</v>
       </c>
@@ -14449,7 +14471,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="29.25">
+    <row r="246" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>273</v>
       </c>
@@ -14509,7 +14531,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="29.25">
+    <row r="247" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>273</v>
       </c>
@@ -14569,7 +14591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="29.25">
+    <row r="248" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>273</v>
       </c>
@@ -14629,7 +14651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="29.25">
+    <row r="249" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>273</v>
       </c>
@@ -14689,7 +14711,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="29.25">
+    <row r="250" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>273</v>
       </c>
@@ -14749,7 +14771,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="29.25">
+    <row r="251" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>273</v>
       </c>
@@ -14809,7 +14831,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="29.25">
+    <row r="252" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>273</v>
       </c>
@@ -14869,7 +14891,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="39">
+    <row r="253" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>273</v>
       </c>
@@ -14911,7 +14933,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="39">
+    <row r="254" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>273</v>
       </c>
@@ -14953,7 +14975,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="39">
+    <row r="255" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>273</v>
       </c>
@@ -14995,7 +15017,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="29.25">
+    <row r="256" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>273</v>
       </c>
@@ -15055,7 +15077,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="48.75">
+    <row r="257" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>273</v>
       </c>
@@ -15113,7 +15135,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="29.25">
+    <row r="258" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>273</v>
       </c>
@@ -15149,7 +15171,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="29.25">
+    <row r="259" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>273</v>
       </c>
@@ -15185,7 +15207,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="29.25">
+    <row r="260" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>273</v>
       </c>
@@ -15221,7 +15243,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="29.25">
+    <row r="261" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>273</v>
       </c>
@@ -15257,7 +15279,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="29.25">
+    <row r="262" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>273</v>
       </c>
@@ -15293,7 +15315,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="29.25">
+    <row r="263" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>273</v>
       </c>
@@ -15329,7 +15351,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="29.25">
+    <row r="264" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>273</v>
       </c>
@@ -15365,7 +15387,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="29.25">
+    <row r="265" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>273</v>
       </c>
@@ -15401,7 +15423,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="29.25">
+    <row r="266" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>273</v>
       </c>
@@ -15453,7 +15475,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="29.25">
+    <row r="267" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>319</v>
       </c>
@@ -15513,7 +15535,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="29.25">
+    <row r="268" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>319</v>
       </c>
@@ -15573,7 +15595,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="29.25">
+    <row r="269" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>319</v>
       </c>
@@ -15633,7 +15655,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="29.25">
+    <row r="270" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>319</v>
       </c>
@@ -15693,7 +15715,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="29.25">
+    <row r="271" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>319</v>
       </c>
@@ -15753,7 +15775,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="272" spans="1:20" ht="29.25">
+    <row r="272" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>319</v>
       </c>
@@ -15813,7 +15835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="29.25">
+    <row r="273" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>319</v>
       </c>
@@ -15873,7 +15895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="29.25">
+    <row r="274" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>319</v>
       </c>
@@ -15933,7 +15955,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="275" spans="1:20" ht="29.25">
+    <row r="275" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>319</v>
       </c>
@@ -15993,7 +16015,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="276" spans="1:20" ht="29.25">
+    <row r="276" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>319</v>
       </c>
@@ -16053,7 +16075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="29.25">
+    <row r="277" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>319</v>
       </c>
@@ -16113,7 +16135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="29.25">
+    <row r="278" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>319</v>
       </c>
@@ -16173,7 +16195,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="29.25">
+    <row r="279" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>319</v>
       </c>
@@ -16233,7 +16255,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="29.25">
+    <row r="280" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>319</v>
       </c>
@@ -16291,7 +16313,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="281" spans="1:20" ht="29.25">
+    <row r="281" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>319</v>
       </c>
@@ -16351,7 +16373,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="282" spans="1:20" ht="29.25">
+    <row r="282" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>319</v>
       </c>
@@ -16411,7 +16433,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="29.25">
+    <row r="283" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>319</v>
       </c>
@@ -16471,7 +16493,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="29.25">
+    <row r="284" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>319</v>
       </c>
@@ -16531,7 +16553,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="29.25">
+    <row r="285" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>319</v>
       </c>
@@ -16591,7 +16613,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="29.25">
+    <row r="286" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>319</v>
       </c>
@@ -16651,7 +16673,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="29.25">
+    <row r="287" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>319</v>
       </c>
@@ -16703,7 +16725,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="29.25">
+    <row r="288" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>319</v>
       </c>
@@ -16763,7 +16785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="29.25">
+    <row r="289" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>319</v>
       </c>
@@ -16823,7 +16845,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="29.25">
+    <row r="290" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>319</v>
       </c>
@@ -16877,7 +16899,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="291" spans="1:20" ht="29.25">
+    <row r="291" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>319</v>
       </c>
@@ -16931,7 +16953,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="39">
+    <row r="292" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>319</v>
       </c>
@@ -16983,7 +17005,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="39">
+    <row r="293" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>319</v>
       </c>
@@ -17035,7 +17057,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="19.5">
+    <row r="294" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>351</v>
       </c>
@@ -17095,7 +17117,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="68.25">
+    <row r="295" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>351</v>
       </c>
@@ -17155,7 +17177,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="19.5">
+    <row r="296" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>351</v>
       </c>
@@ -17215,7 +17237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="19.5">
+    <row r="297" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>351</v>
       </c>
@@ -17275,7 +17297,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="19.5">
+    <row r="298" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>351</v>
       </c>
@@ -17335,7 +17357,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="19.5">
+    <row r="299" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>351</v>
       </c>
@@ -17395,7 +17417,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="19.5">
+    <row r="300" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>351</v>
       </c>
@@ -17455,7 +17477,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="19.5">
+    <row r="301" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>351</v>
       </c>
@@ -17515,7 +17537,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="19.5">
+    <row r="302" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
         <v>351</v>
       </c>
@@ -17575,7 +17597,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="19.5">
+    <row r="303" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
         <v>351</v>
       </c>
@@ -17635,7 +17657,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="304" spans="1:20" ht="19.5">
+    <row r="304" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>351</v>
       </c>
@@ -17695,7 +17717,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="305" spans="1:20" ht="19.5">
+    <row r="305" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>351</v>
       </c>
@@ -17735,7 +17757,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="306" spans="1:20" ht="19.5">
+    <row r="306" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
         <v>351</v>
       </c>
@@ -17795,7 +17817,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="307" spans="1:20" ht="39">
+    <row r="307" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
         <v>351</v>
       </c>
@@ -17855,7 +17877,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="308" spans="1:20" ht="48.75">
+    <row r="308" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
         <v>351</v>
       </c>
@@ -17915,7 +17937,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="309" spans="1:20" ht="39">
+    <row r="309" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
         <v>351</v>
       </c>
@@ -17975,7 +17997,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="310" spans="1:20" ht="39">
+    <row r="310" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
         <v>351</v>
       </c>
@@ -18035,7 +18057,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="311" spans="1:20" ht="29.25">
+    <row r="311" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
         <v>351</v>
       </c>
@@ -18095,7 +18117,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="312" spans="1:20" ht="39">
+    <row r="312" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
         <v>351</v>
       </c>
@@ -18155,7 +18177,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="313" spans="1:20" ht="29.25">
+    <row r="313" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
         <v>351</v>
       </c>
@@ -18215,7 +18237,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="314" spans="1:20" ht="29.25">
+    <row r="314" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
         <v>351</v>
       </c>
@@ -18275,7 +18297,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="315" spans="1:20" ht="39">
+    <row r="315" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
         <v>351</v>
       </c>
@@ -18335,7 +18357,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="316" spans="1:20" ht="29.25">
+    <row r="316" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
         <v>351</v>
       </c>
@@ -18395,7 +18417,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="317" spans="1:20" ht="39">
+    <row r="317" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
         <v>351</v>
       </c>
@@ -18455,7 +18477,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="318" spans="1:20" ht="29.25">
+    <row r="318" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
         <v>351</v>
       </c>
@@ -18515,7 +18537,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="319" spans="1:20" ht="29.25">
+    <row r="319" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
         <v>351</v>
       </c>
@@ -18575,7 +18597,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="320" spans="1:20" ht="39">
+    <row r="320" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
         <v>351</v>
       </c>
@@ -18635,7 +18657,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="321" spans="1:20" ht="39">
+    <row r="321" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
         <v>351</v>
       </c>
@@ -18695,7 +18717,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="322" spans="1:20" ht="68.25">
+    <row r="322" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
         <v>351</v>
       </c>
@@ -18755,7 +18777,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="323" spans="1:20" ht="58.5">
+    <row r="323" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
         <v>351</v>
       </c>
@@ -18815,7 +18837,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="324" spans="1:20" ht="68.25">
+    <row r="324" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
         <v>351</v>
       </c>
@@ -18875,7 +18897,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="325" spans="1:20" ht="68.25">
+    <row r="325" spans="1:20" ht="72" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>351</v>
       </c>
@@ -18935,7 +18957,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="326" spans="1:20" ht="39">
+    <row r="326" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
         <v>351</v>
       </c>
@@ -18995,7 +19017,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="327" spans="1:20" ht="68.25">
+    <row r="327" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
         <v>351</v>
       </c>
@@ -19055,7 +19077,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="328" spans="1:20" ht="58.5">
+    <row r="328" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
         <v>351</v>
       </c>
@@ -19115,7 +19137,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="329" spans="1:20" ht="68.25">
+    <row r="329" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
         <v>351</v>
       </c>
@@ -19175,7 +19197,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="330" spans="1:20" ht="68.25">
+    <row r="330" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
         <v>351</v>
       </c>
@@ -19235,7 +19257,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="331" spans="1:20" ht="29.25">
+    <row r="331" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
         <v>392</v>
       </c>
@@ -19291,7 +19313,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="332" spans="1:20" ht="29.25">
+    <row r="332" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
         <v>392</v>
       </c>
@@ -19347,7 +19369,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="333" spans="1:20" ht="29.25">
+    <row r="333" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
         <v>392</v>
       </c>
@@ -19403,7 +19425,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="29.25">
+    <row r="334" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
         <v>392</v>
       </c>
@@ -19463,7 +19485,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="335" spans="1:20" ht="29.25">
+    <row r="335" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
         <v>392</v>
       </c>
@@ -19523,7 +19545,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="336" spans="1:20" ht="29.25">
+    <row r="336" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
         <v>392</v>
       </c>
@@ -19583,7 +19605,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="337" spans="1:20" ht="29.25">
+    <row r="337" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
         <v>392</v>
       </c>
@@ -19643,7 +19665,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="338" spans="1:20" ht="29.25">
+    <row r="338" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
         <v>392</v>
       </c>
@@ -19703,7 +19725,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="339" spans="1:20" ht="29.25">
+    <row r="339" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
         <v>392</v>
       </c>
@@ -19763,7 +19785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="340" spans="1:20" ht="29.25">
+    <row r="340" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
         <v>392</v>
       </c>
@@ -19823,7 +19845,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="341" spans="1:20" ht="29.25">
+    <row r="341" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
         <v>392</v>
       </c>
@@ -19883,7 +19905,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="342" spans="1:20" ht="29.25">
+    <row r="342" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
         <v>392</v>
       </c>
@@ -19943,7 +19965,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="343" spans="1:20" ht="29.25">
+    <row r="343" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
         <v>392</v>
       </c>
@@ -20003,7 +20025,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="344" spans="1:20" ht="29.25">
+    <row r="344" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
         <v>392</v>
       </c>
@@ -20063,7 +20085,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="345" spans="1:20" ht="29.25">
+    <row r="345" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
         <v>392</v>
       </c>
@@ -20123,7 +20145,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="346" spans="1:20" ht="29.25">
+    <row r="346" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
         <v>392</v>
       </c>
@@ -20183,7 +20205,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="347" spans="1:20" ht="29.25">
+    <row r="347" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
         <v>392</v>
       </c>
@@ -20243,7 +20265,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="348" spans="1:20" ht="29.25">
+    <row r="348" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
         <v>392</v>
       </c>
@@ -20303,7 +20325,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="349" spans="1:20" ht="29.25">
+    <row r="349" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
         <v>392</v>
       </c>
@@ -20363,7 +20385,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="350" spans="1:20" ht="29.25">
+    <row r="350" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
         <v>392</v>
       </c>
@@ -20423,7 +20445,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="351" spans="1:20" ht="29.25">
+    <row r="351" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
         <v>392</v>
       </c>
@@ -20483,7 +20505,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="352" spans="1:20" ht="29.25">
+    <row r="352" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
         <v>392</v>
       </c>
@@ -20543,7 +20565,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="353" spans="1:20" ht="29.25">
+    <row r="353" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
         <v>392</v>
       </c>
@@ -20603,7 +20625,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="354" spans="1:20" ht="29.25">
+    <row r="354" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
         <v>392</v>
       </c>
@@ -20663,7 +20685,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="355" spans="1:20" ht="29.25">
+    <row r="355" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
         <v>392</v>
       </c>
@@ -20723,7 +20745,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="356" spans="1:20" ht="29.25">
+    <row r="356" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
         <v>392</v>
       </c>
@@ -20783,7 +20805,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="357" spans="1:20" ht="29.25">
+    <row r="357" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
         <v>392</v>
       </c>
@@ -20843,7 +20865,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="358" spans="1:20" ht="29.25">
+    <row r="358" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
         <v>392</v>
       </c>
@@ -20901,7 +20923,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="359" spans="1:20" ht="29.25">
+    <row r="359" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
         <v>392</v>
       </c>
@@ -20961,7 +20983,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="360" spans="1:20" ht="29.25">
+    <row r="360" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
         <v>392</v>
       </c>
@@ -21021,7 +21043,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="361" spans="1:20" ht="29.25">
+    <row r="361" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
         <v>392</v>
       </c>
@@ -21081,7 +21103,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="362" spans="1:20" ht="29.25">
+    <row r="362" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
         <v>392</v>
       </c>
@@ -21141,7 +21163,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="363" spans="1:20" ht="29.25">
+    <row r="363" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
         <v>392</v>
       </c>
@@ -21201,7 +21223,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="364" spans="1:20" ht="39">
+    <row r="364" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
         <v>392</v>
       </c>
@@ -21261,7 +21283,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="365" spans="1:20" ht="39">
+    <row r="365" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
         <v>392</v>
       </c>
@@ -21321,7 +21343,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="366" spans="1:20" ht="39">
+    <row r="366" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
         <v>392</v>
       </c>
@@ -21381,7 +21403,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="367" spans="1:20" ht="39">
+    <row r="367" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
         <v>392</v>
       </c>
@@ -21441,7 +21463,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="368" spans="1:20" ht="39">
+    <row r="368" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
         <v>392</v>
       </c>
@@ -21501,7 +21523,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="369" spans="1:20" ht="39">
+    <row r="369" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
         <v>392</v>
       </c>
@@ -21561,7 +21583,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="370" spans="1:20" ht="39">
+    <row r="370" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
         <v>392</v>
       </c>
@@ -21621,7 +21643,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="371" spans="1:20" ht="39">
+    <row r="371" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
         <v>392</v>
       </c>
@@ -21681,7 +21703,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="372" spans="1:20" ht="29.25">
+    <row r="372" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
         <v>392</v>
       </c>
@@ -21733,7 +21755,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="373" spans="1:20" ht="68.25">
+    <row r="373" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
         <v>392</v>
       </c>
@@ -21785,7 +21807,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="374" spans="1:20" ht="29.25">
+    <row r="374" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
         <v>392</v>
       </c>
@@ -21837,7 +21859,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="375" spans="1:20" ht="29.25">
+    <row r="375" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
         <v>392</v>
       </c>
@@ -21889,7 +21911,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="376" spans="1:20" ht="39">
+    <row r="376" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
         <v>427</v>
       </c>
@@ -21949,7 +21971,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="377" spans="1:20" ht="39">
+    <row r="377" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
         <v>427</v>
       </c>
@@ -22009,7 +22031,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="378" spans="1:20" ht="39">
+    <row r="378" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
         <v>427</v>
       </c>
@@ -22069,7 +22091,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="379" spans="1:20" ht="48.75">
+    <row r="379" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
         <v>427</v>
       </c>
@@ -22131,7 +22153,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="380" spans="1:20" ht="39">
+    <row r="380" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
         <v>427</v>
       </c>
@@ -22177,7 +22199,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="381" spans="1:20" ht="39">
+    <row r="381" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
         <v>427</v>
       </c>
@@ -22223,7 +22245,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="382" spans="1:20" ht="39">
+    <row r="382" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
         <v>427</v>
       </c>
@@ -22269,7 +22291,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="383" spans="1:20" ht="39">
+    <row r="383" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
         <v>427</v>
       </c>
@@ -22323,7 +22345,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="384" spans="1:20" ht="39">
+    <row r="384" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
         <v>427</v>
       </c>
@@ -22369,7 +22391,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="385" spans="1:20" ht="39">
+    <row r="385" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
         <v>427</v>
       </c>
@@ -22431,7 +22453,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="386" spans="1:20" ht="48.75">
+    <row r="386" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
         <v>427</v>
       </c>
@@ -22493,7 +22515,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="387" spans="1:20" ht="29.25">
+    <row r="387" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
         <v>447</v>
       </c>
@@ -22553,7 +22575,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="388" spans="1:20" ht="29.25">
+    <row r="388" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
         <v>447</v>
       </c>
@@ -22613,7 +22635,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="389" spans="1:20" ht="29.25">
+    <row r="389" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
         <v>447</v>
       </c>
@@ -22665,7 +22687,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="390" spans="1:20" ht="68.25">
+    <row r="390" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
         <v>447</v>
       </c>
@@ -22717,7 +22739,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="391" spans="1:20" ht="29.25">
+    <row r="391" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
         <v>447</v>
       </c>
@@ -22769,7 +22791,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="392" spans="1:20" ht="29.25">
+    <row r="392" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
         <v>447</v>
       </c>
@@ -22821,7 +22843,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="393" spans="1:20" ht="39">
+    <row r="393" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
         <v>447</v>
       </c>
@@ -22883,7 +22905,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="394" spans="1:20" ht="39">
+    <row r="394" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
         <v>447</v>
       </c>
@@ -22941,7 +22963,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="395" spans="1:20" ht="48.75">
+    <row r="395" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
         <v>447</v>
       </c>
@@ -23003,7 +23025,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="396" spans="1:20" ht="29.25">
+    <row r="396" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
         <v>447</v>
       </c>
@@ -23057,7 +23079,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="397" spans="1:20" ht="58.5">
+    <row r="397" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
         <v>459</v>
       </c>
@@ -23117,7 +23139,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="398" spans="1:20" ht="39">
+    <row r="398" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
         <v>459</v>
       </c>
@@ -23177,7 +23199,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="399" spans="1:20" ht="48.75">
+    <row r="399" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
         <v>459</v>
       </c>
@@ -23237,7 +23259,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="400" spans="1:20" ht="48.75">
+    <row r="400" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
         <v>459</v>
       </c>
@@ -23297,7 +23319,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="401" spans="1:20" ht="58.5">
+    <row r="401" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
         <v>459</v>
       </c>
@@ -23357,7 +23379,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="402" spans="1:20" ht="19.5">
+    <row r="402" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A402" s="2" t="s">
         <v>469</v>
       </c>
@@ -23417,7 +23439,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="403" spans="1:20" ht="19.5">
+    <row r="403" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
         <v>469</v>
       </c>
@@ -23477,7 +23499,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="404" spans="1:20" ht="39">
+    <row r="404" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
         <v>469</v>
       </c>
@@ -23537,7 +23559,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="405" spans="1:20" ht="19.5">
+    <row r="405" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
         <v>469</v>
       </c>
@@ -23579,7 +23601,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="406" spans="1:20" ht="19.5">
+    <row r="406" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
         <v>469</v>
       </c>
@@ -23613,7 +23635,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="407" spans="1:20" ht="19.5">
+    <row r="407" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
         <v>469</v>
       </c>
@@ -23647,7 +23669,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="408" spans="1:20" ht="19.5">
+    <row r="408" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
         <v>469</v>
       </c>
@@ -23681,7 +23703,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="409" spans="1:20" ht="19.5">
+    <row r="409" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
         <v>469</v>
       </c>
@@ -23723,7 +23745,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="410" spans="1:20" ht="19.5">
+    <row r="410" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
         <v>469</v>
       </c>
@@ -23765,7 +23787,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="411" spans="1:20" ht="19.5">
+    <row r="411" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A411" s="2" t="s">
         <v>469</v>
       </c>
@@ -23807,7 +23829,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="412" spans="1:20" ht="29.25">
+    <row r="412" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A412" s="2" t="s">
         <v>469</v>
       </c>
@@ -23869,7 +23891,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="413" spans="1:20" ht="19.5">
+    <row r="413" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
         <v>469</v>
       </c>
@@ -23929,7 +23951,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="414" spans="1:20" ht="29.25">
+    <row r="414" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
         <v>469</v>
       </c>
@@ -23991,7 +24013,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="415" spans="1:20" ht="29.25">
+    <row r="415" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
         <v>469</v>
       </c>
@@ -24045,7 +24067,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="416" spans="1:20" ht="29.25">
+    <row r="416" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
         <v>469</v>
       </c>
@@ -24099,7 +24121,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="417" spans="1:20" ht="19.5">
+    <row r="417" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A417" s="2" t="s">
         <v>469</v>
       </c>
@@ -24159,7 +24181,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="418" spans="1:20" ht="29.25">
+    <row r="418" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
         <v>490</v>
       </c>
@@ -24217,7 +24239,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="419" spans="1:20" ht="29.25">
+    <row r="419" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
         <v>490</v>
       </c>
@@ -24279,7 +24301,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="420" spans="1:20" ht="29.25">
+    <row r="420" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
         <v>490</v>
       </c>
@@ -24323,7 +24345,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="421" spans="1:20" ht="29.25">
+    <row r="421" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
         <v>490</v>
       </c>
@@ -24379,7 +24401,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="422" spans="1:20" ht="29.25">
+    <row r="422" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
         <v>490</v>
       </c>
@@ -24427,7 +24449,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="423" spans="1:20" ht="29.25">
+    <row r="423" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
         <v>490</v>
       </c>
@@ -24475,7 +24497,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="424" spans="1:20" ht="29.25">
+    <row r="424" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
         <v>490</v>
       </c>
@@ -24523,7 +24545,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="425" spans="1:20" ht="29.25">
+    <row r="425" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
         <v>490</v>
       </c>
@@ -24571,7 +24593,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="426" spans="1:20" ht="29.25">
+    <row r="426" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A426" s="2" t="s">
         <v>490</v>
       </c>
@@ -24619,7 +24641,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="427" spans="1:20" ht="29.25">
+    <row r="427" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
         <v>490</v>
       </c>
@@ -24667,7 +24689,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="428" spans="1:20" ht="39">
+    <row r="428" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
         <v>490</v>
       </c>
@@ -24715,7 +24737,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="429" spans="1:20" ht="48.75">
+    <row r="429" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A429" s="2" t="s">
         <v>490</v>
       </c>
@@ -24763,7 +24785,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="430" spans="1:20" ht="39">
+    <row r="430" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A430" s="2" t="s">
         <v>490</v>
       </c>
@@ -24811,7 +24833,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="431" spans="1:20" ht="39">
+    <row r="431" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
         <v>490</v>
       </c>
@@ -24859,7 +24881,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="432" spans="1:20" ht="29.25">
+    <row r="432" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A432" s="2" t="s">
         <v>490</v>
       </c>
@@ -24919,7 +24941,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="433" spans="1:20" ht="29.25">
+    <row r="433" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A433" s="2" t="s">
         <v>490</v>
       </c>
@@ -24979,7 +25001,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="434" spans="1:20" ht="29.25">
+    <row r="434" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A434" s="2" t="s">
         <v>490</v>
       </c>
@@ -25039,7 +25061,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="435" spans="1:20" ht="29.25">
+    <row r="435" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A435" s="2" t="s">
         <v>490</v>
       </c>
@@ -25099,7 +25121,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="436" spans="1:20" ht="29.25">
+    <row r="436" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A436" s="2" t="s">
         <v>490</v>
       </c>
@@ -25159,7 +25181,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="437" spans="1:20" ht="29.25">
+    <row r="437" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A437" s="2" t="s">
         <v>490</v>
       </c>
@@ -25219,7 +25241,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="438" spans="1:20" ht="39">
+    <row r="438" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A438" s="2" t="s">
         <v>490</v>
       </c>
@@ -25261,7 +25283,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="439" spans="1:20" ht="39">
+    <row r="439" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A439" s="2" t="s">
         <v>490</v>
       </c>
@@ -25303,7 +25325,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="440" spans="1:20" ht="39">
+    <row r="440" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
         <v>490</v>
       </c>
@@ -25345,7 +25367,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="441" spans="1:20" ht="39">
+    <row r="441" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
         <v>490</v>
       </c>
@@ -25387,7 +25409,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="442" spans="1:20" ht="39">
+    <row r="442" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
         <v>490</v>
       </c>
@@ -25429,7 +25451,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="443" spans="1:20" ht="39">
+    <row r="443" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A443" s="2" t="s">
         <v>490</v>
       </c>
@@ -25471,7 +25493,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="444" spans="1:20" ht="39">
+    <row r="444" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A444" s="2" t="s">
         <v>490</v>
       </c>
@@ -25513,7 +25535,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="445" spans="1:20" ht="39">
+    <row r="445" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A445" s="2" t="s">
         <v>490</v>
       </c>
@@ -25555,7 +25577,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="446" spans="1:20" ht="39">
+    <row r="446" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A446" s="2" t="s">
         <v>490</v>
       </c>
@@ -25597,7 +25619,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="447" spans="1:20" ht="39">
+    <row r="447" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
         <v>490</v>
       </c>
@@ -25639,7 +25661,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="448" spans="1:20" ht="39">
+    <row r="448" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
         <v>490</v>
       </c>
@@ -25681,7 +25703,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="449" spans="1:20" ht="39">
+    <row r="449" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A449" s="2" t="s">
         <v>490</v>
       </c>
@@ -25723,7 +25745,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="450" spans="1:20" ht="29.25">
+    <row r="450" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A450" s="2" t="s">
         <v>490</v>
       </c>
@@ -25785,7 +25807,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="451" spans="1:20" ht="29.25">
+    <row r="451" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A451" s="2" t="s">
         <v>490</v>
       </c>
@@ -25825,7 +25847,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="452" spans="1:20" ht="29.25">
+    <row r="452" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A452" s="2" t="s">
         <v>527</v>
       </c>
@@ -25885,7 +25907,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="453" spans="1:20" ht="29.25">
+    <row r="453" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A453" s="2" t="s">
         <v>527</v>
       </c>
@@ -25945,7 +25967,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="454" spans="1:20" ht="29.25">
+    <row r="454" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A454" s="2" t="s">
         <v>527</v>
       </c>
@@ -26005,7 +26027,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="455" spans="1:20" ht="29.25">
+    <row r="455" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A455" s="2" t="s">
         <v>527</v>
       </c>
@@ -26065,7 +26087,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="456" spans="1:20" ht="48.75">
+    <row r="456" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A456" s="2" t="s">
         <v>527</v>
       </c>
@@ -26125,7 +26147,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="457" spans="1:20" ht="29.25">
+    <row r="457" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
         <v>527</v>
       </c>
@@ -26185,7 +26207,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="458" spans="1:20" ht="29.25">
+    <row r="458" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A458" s="2" t="s">
         <v>527</v>
       </c>
@@ -26245,7 +26267,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="459" spans="1:20" ht="29.25">
+    <row r="459" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
         <v>527</v>
       </c>
@@ -26307,7 +26329,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="460" spans="1:20" ht="29.25">
+    <row r="460" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
         <v>527</v>
       </c>
@@ -26369,7 +26391,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="461" spans="1:20" ht="29.25">
+    <row r="461" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
         <v>527</v>
       </c>
@@ -26431,7 +26453,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="462" spans="1:20" ht="29.25">
+    <row r="462" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
         <v>527</v>
       </c>
@@ -26491,7 +26513,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="463" spans="1:20" ht="29.25">
+    <row r="463" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
         <v>527</v>
       </c>
@@ -26551,7 +26573,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="464" spans="1:20" ht="29.25">
+    <row r="464" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
         <v>527</v>
       </c>
@@ -26611,7 +26633,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="465" spans="1:20" ht="29.25">
+    <row r="465" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
         <v>527</v>
       </c>
@@ -26671,7 +26693,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="466" spans="1:20" ht="29.25">
+    <row r="466" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
         <v>527</v>
       </c>
@@ -26733,7 +26755,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="467" spans="1:20" ht="48.75">
+    <row r="467" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
         <v>527</v>
       </c>
@@ -26795,7 +26817,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="468" spans="1:20" ht="29.25">
+    <row r="468" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
         <v>527</v>
       </c>
@@ -26857,7 +26879,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="469" spans="1:20" ht="39">
+    <row r="469" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A469" s="2" t="s">
         <v>527</v>
       </c>
@@ -26917,7 +26939,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="470" spans="1:20" ht="39">
+    <row r="470" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
         <v>527</v>
       </c>
@@ -26977,7 +26999,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="471" spans="1:20" ht="29.25">
+    <row r="471" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A471" s="2" t="s">
         <v>527</v>
       </c>
@@ -27023,7 +27045,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="472" spans="1:20" ht="29.25">
+    <row r="472" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A472" s="2" t="s">
         <v>527</v>
       </c>
@@ -27085,7 +27107,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="473" spans="1:20" ht="29.25">
+    <row r="473" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
         <v>527</v>
       </c>
@@ -27147,7 +27169,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="474" spans="1:20" ht="29.25">
+    <row r="474" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A474" s="2" t="s">
         <v>527</v>
       </c>
@@ -27201,7 +27223,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="475" spans="1:20" ht="39">
+    <row r="475" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
         <v>527</v>
       </c>
@@ -27239,7 +27261,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="476" spans="1:20" ht="39">
+    <row r="476" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A476" s="2" t="s">
         <v>527</v>
       </c>
@@ -27301,7 +27323,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="477" spans="1:20" ht="39">
+    <row r="477" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A477" s="2" t="s">
         <v>527</v>
       </c>
@@ -27363,8 +27385,8 @@
         <v>562</v>
       </c>
     </row>
-    <row r="478" spans="1:20" ht="18" customHeight="1"/>
-    <row r="479" spans="1:20" ht="17.100000000000001" customHeight="1">
+    <row r="478" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A479" s="12" t="s">
         <v>565</v>
       </c>
@@ -27381,7 +27403,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="74" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="72" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okno serwisowe - 12.03.2024 Aktualizacja plików Excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1720,7 +1720,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 27-02-2024, 09:05</t>
+    <t>Last update: 12-03-2024, 08:17</t>
   </si>
 </sst>
 </file>
@@ -2272,7 +2272,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Okno serwisowe - 08.04.2024, aktualizacja API, PDF, XLS
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1720,7 +1720,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 12-03-2024, 08:17</t>
+    <t>Last update: 09-04-2024, 13:25</t>
   </si>
 </sst>
 </file>
@@ -2272,7 +2272,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27403,7 +27403,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="72" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="74" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okno serwisowe 23.04.2024 - Aktualizacja Excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1684,7 +1684,7 @@
     <t>general government result in relation to GDP</t>
   </si>
   <si>
-    <t>17.14.1 Number of countries with mechanisms in place to enhance policy coherence of sustainable development</t>
+    <t>17.14.1 Number of countries with mechanisms in place to enhance policy coherence of sustainable development - PROXY!</t>
   </si>
   <si>
     <t>17.18.2 Number of countries that have national statistical legislation that complies with the Fundamental Principles of Official Statistics</t>
@@ -1720,7 +1720,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 09-04-2024, 13:25</t>
+    <t>Last update: 23-04-2024, 13:07</t>
   </si>
 </sst>
 </file>
@@ -2272,7 +2272,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3174,7 +3174,9 @@
       <c r="R17" s="4">
         <v>14.2</v>
       </c>
-      <c r="S17" s="3"/>
+      <c r="S17" s="4">
+        <v>15.2</v>
+      </c>
       <c r="T17" s="2" t="s">
         <v>26</v>
       </c>
@@ -3843,7 +3845,9 @@
       <c r="Q29" s="4">
         <v>63.5</v>
       </c>
-      <c r="R29" s="3"/>
+      <c r="R29" s="4">
+        <v>61</v>
+      </c>
       <c r="S29" s="3"/>
       <c r="T29" s="2" t="s">
         <v>26</v>
@@ -3901,7 +3905,9 @@
       <c r="Q30" s="4">
         <v>13.1</v>
       </c>
-      <c r="R30" s="3"/>
+      <c r="R30" s="4">
+        <v>12</v>
+      </c>
       <c r="S30" s="3"/>
       <c r="T30" s="2" t="s">
         <v>26</v>
@@ -3959,7 +3965,9 @@
       <c r="Q31" s="4">
         <v>11.2</v>
       </c>
-      <c r="R31" s="3"/>
+      <c r="R31" s="4">
+        <v>10.5</v>
+      </c>
       <c r="S31" s="3"/>
       <c r="T31" s="2" t="s">
         <v>26</v>
@@ -4017,7 +4025,9 @@
       <c r="Q32" s="4">
         <v>39.200000000000003</v>
       </c>
-      <c r="R32" s="3"/>
+      <c r="R32" s="4">
+        <v>38.4</v>
+      </c>
       <c r="S32" s="3"/>
       <c r="T32" s="2" t="s">
         <v>26</v>
@@ -4935,9 +4945,11 @@
         <v>0.45</v>
       </c>
       <c r="Q49" s="5">
-        <v>0.41</v>
-      </c>
-      <c r="R49" s="3"/>
+        <v>0.46</v>
+      </c>
+      <c r="R49" s="5">
+        <v>0.82</v>
+      </c>
       <c r="S49" s="3"/>
       <c r="T49" s="2" t="s">
         <v>92</v>
@@ -5049,7 +5061,9 @@
       <c r="Q51" s="4">
         <v>2.1</v>
       </c>
-      <c r="R51" s="3"/>
+      <c r="R51" s="4">
+        <v>2</v>
+      </c>
       <c r="S51" s="3"/>
       <c r="T51" s="2" t="s">
         <v>26</v>
@@ -5650,7 +5664,9 @@
       <c r="R61" s="6">
         <v>26</v>
       </c>
-      <c r="S61" s="3"/>
+      <c r="S61" s="6">
+        <v>46</v>
+      </c>
       <c r="T61" s="2" t="s">
         <v>102</v>
       </c>
@@ -5710,7 +5726,9 @@
       <c r="R62" s="6">
         <v>11</v>
       </c>
-      <c r="S62" s="3"/>
+      <c r="S62" s="6">
+        <v>13</v>
+      </c>
       <c r="T62" s="2" t="s">
         <v>102</v>
       </c>
@@ -5770,7 +5788,9 @@
       <c r="R63" s="6">
         <v>15</v>
       </c>
-      <c r="S63" s="3"/>
+      <c r="S63" s="6">
+        <v>33</v>
+      </c>
       <c r="T63" s="2" t="s">
         <v>102</v>
       </c>
@@ -5888,9 +5908,11 @@
         <v>30</v>
       </c>
       <c r="R65" s="6">
-        <v>72</v>
-      </c>
-      <c r="S65" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="S65" s="6">
+        <v>140</v>
+      </c>
       <c r="T65" s="2" t="s">
         <v>102</v>
       </c>
@@ -5948,9 +5970,11 @@
         <v>21</v>
       </c>
       <c r="R66" s="6">
-        <v>39</v>
-      </c>
-      <c r="S66" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="S66" s="6">
+        <v>68</v>
+      </c>
       <c r="T66" s="2" t="s">
         <v>102</v>
       </c>
@@ -6010,7 +6034,9 @@
       <c r="R67" s="6">
         <v>33</v>
       </c>
-      <c r="S67" s="3"/>
+      <c r="S67" s="6">
+        <v>72</v>
+      </c>
       <c r="T67" s="2" t="s">
         <v>102</v>
       </c>
@@ -6067,7 +6093,9 @@
       <c r="Q68" s="4">
         <v>475.8</v>
       </c>
-      <c r="R68" s="3"/>
+      <c r="R68" s="4">
+        <v>426.2</v>
+      </c>
       <c r="S68" s="3"/>
       <c r="T68" s="2" t="s">
         <v>26</v>
@@ -6125,7 +6153,9 @@
       <c r="Q69" s="4">
         <v>28.5</v>
       </c>
-      <c r="R69" s="3"/>
+      <c r="R69" s="4">
+        <v>28.8</v>
+      </c>
       <c r="S69" s="3"/>
       <c r="T69" s="2" t="s">
         <v>26</v>
@@ -6183,7 +6213,9 @@
       <c r="Q70" s="4">
         <v>246.5</v>
       </c>
-      <c r="R70" s="3"/>
+      <c r="R70" s="4">
+        <v>253.9</v>
+      </c>
       <c r="S70" s="3"/>
       <c r="T70" s="2" t="s">
         <v>26</v>
@@ -6241,7 +6273,9 @@
       <c r="Q71" s="4">
         <v>25.4</v>
       </c>
-      <c r="R71" s="3"/>
+      <c r="R71" s="4">
+        <v>24.6</v>
+      </c>
       <c r="S71" s="3"/>
       <c r="T71" s="2" t="s">
         <v>26</v>
@@ -6299,7 +6333,9 @@
       <c r="Q72" s="4">
         <v>12.1</v>
       </c>
-      <c r="R72" s="3"/>
+      <c r="R72" s="4">
+        <v>11.9</v>
+      </c>
       <c r="S72" s="3"/>
       <c r="T72" s="2" t="s">
         <v>26</v>
@@ -6357,7 +6393,9 @@
       <c r="Q73" s="4">
         <v>21.4</v>
       </c>
-      <c r="R73" s="3"/>
+      <c r="R73" s="4">
+        <v>20.5</v>
+      </c>
       <c r="S73" s="3"/>
       <c r="T73" s="2" t="s">
         <v>26</v>
@@ -6415,7 +6453,9 @@
       <c r="Q74" s="4">
         <v>3.3</v>
       </c>
-      <c r="R74" s="3"/>
+      <c r="R74" s="4">
+        <v>3.4</v>
+      </c>
       <c r="S74" s="3"/>
       <c r="T74" s="2" t="s">
         <v>26</v>
@@ -7045,7 +7085,9 @@
       <c r="Q86" s="4">
         <v>1.3</v>
       </c>
-      <c r="R86" s="3"/>
+      <c r="R86" s="4">
+        <v>1.2</v>
+      </c>
       <c r="S86" s="3"/>
       <c r="T86" s="2" t="s">
         <v>26</v>
@@ -11167,7 +11209,9 @@
         <v>45</v>
       </c>
       <c r="Q177" s="3"/>
-      <c r="R177" s="3"/>
+      <c r="R177" s="4">
+        <v>46.1</v>
+      </c>
       <c r="S177" s="3"/>
       <c r="T177" s="2" t="s">
         <v>26</v>
@@ -11213,7 +11257,9 @@
         <v>31.4</v>
       </c>
       <c r="Q178" s="3"/>
-      <c r="R178" s="3"/>
+      <c r="R178" s="4">
+        <v>33.1</v>
+      </c>
       <c r="S178" s="3"/>
       <c r="T178" s="2" t="s">
         <v>26</v>
@@ -11259,7 +11305,9 @@
         <v>42.7</v>
       </c>
       <c r="Q179" s="3"/>
-      <c r="R179" s="3"/>
+      <c r="R179" s="4">
+        <v>42.4</v>
+      </c>
       <c r="S179" s="3"/>
       <c r="T179" s="2" t="s">
         <v>26</v>
@@ -11305,7 +11353,9 @@
         <v>30.3</v>
       </c>
       <c r="Q180" s="3"/>
-      <c r="R180" s="3"/>
+      <c r="R180" s="4">
+        <v>32.299999999999997</v>
+      </c>
       <c r="S180" s="3"/>
       <c r="T180" s="2" t="s">
         <v>26</v>
@@ -11351,7 +11401,9 @@
         <v>55.4</v>
       </c>
       <c r="Q181" s="3"/>
-      <c r="R181" s="3"/>
+      <c r="R181" s="4">
+        <v>56.3</v>
+      </c>
       <c r="S181" s="3"/>
       <c r="T181" s="2" t="s">
         <v>26</v>
@@ -11397,7 +11449,9 @@
         <v>35.1</v>
       </c>
       <c r="Q182" s="3"/>
-      <c r="R182" s="3"/>
+      <c r="R182" s="4">
+        <v>35.4</v>
+      </c>
       <c r="S182" s="3"/>
       <c r="T182" s="2" t="s">
         <v>26</v>
@@ -11443,7 +11497,9 @@
         <v>58.9</v>
       </c>
       <c r="Q183" s="3"/>
-      <c r="R183" s="3"/>
+      <c r="R183" s="4">
+        <v>59.7</v>
+      </c>
       <c r="S183" s="3"/>
       <c r="T183" s="2" t="s">
         <v>26</v>
@@ -12759,9 +12815,11 @@
         <v>16.100000000000001</v>
       </c>
       <c r="Q211" s="5">
-        <v>15.62</v>
-      </c>
-      <c r="R211" s="3"/>
+        <v>15.61</v>
+      </c>
+      <c r="R211" s="5">
+        <v>16.88</v>
+      </c>
       <c r="S211" s="3"/>
       <c r="T211" s="2" t="s">
         <v>26</v>
@@ -12930,7 +12988,7 @@
         <v>7.5</v>
       </c>
       <c r="R214" s="4">
-        <v>5.7</v>
+        <v>6.1</v>
       </c>
       <c r="S214" s="3"/>
       <c r="T214" s="2" t="s">
@@ -12990,7 +13048,7 @@
         <v>8.6</v>
       </c>
       <c r="R215" s="4">
-        <v>10.199999999999999</v>
+        <v>10.6</v>
       </c>
       <c r="S215" s="3"/>
       <c r="T215" s="2" t="s">
@@ -13025,13 +13083,15 @@
       <c r="K216" s="3"/>
       <c r="L216" s="3"/>
       <c r="M216" s="4">
-        <v>4.7</v>
+        <v>5.4</v>
       </c>
       <c r="N216" s="3"/>
       <c r="O216" s="3"/>
       <c r="P216" s="3"/>
       <c r="Q216" s="3"/>
-      <c r="R216" s="3"/>
+      <c r="R216" s="4">
+        <v>2</v>
+      </c>
       <c r="S216" s="3"/>
       <c r="T216" s="2" t="s">
         <v>26</v>
@@ -13065,13 +13125,15 @@
       <c r="K217" s="3"/>
       <c r="L217" s="3"/>
       <c r="M217" s="4">
-        <v>5.3</v>
+        <v>5.9</v>
       </c>
       <c r="N217" s="3"/>
       <c r="O217" s="3"/>
       <c r="P217" s="3"/>
       <c r="Q217" s="3"/>
-      <c r="R217" s="3"/>
+      <c r="R217" s="4">
+        <v>2.5</v>
+      </c>
       <c r="S217" s="3"/>
       <c r="T217" s="2" t="s">
         <v>26</v>
@@ -13105,13 +13167,15 @@
       <c r="K218" s="3"/>
       <c r="L218" s="3"/>
       <c r="M218" s="4">
-        <v>4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="N218" s="3"/>
       <c r="O218" s="3"/>
       <c r="P218" s="3"/>
       <c r="Q218" s="3"/>
-      <c r="R218" s="3"/>
+      <c r="R218" s="4">
+        <v>1.4</v>
+      </c>
       <c r="S218" s="3"/>
       <c r="T218" s="2" t="s">
         <v>26</v>
@@ -13337,7 +13401,9 @@
         <v>33.24</v>
       </c>
       <c r="Q222" s="3"/>
-      <c r="R222" s="3"/>
+      <c r="R222" s="5">
+        <v>42.3</v>
+      </c>
       <c r="S222" s="3"/>
       <c r="T222" s="2" t="s">
         <v>26</v>
@@ -13383,7 +13449,9 @@
         <v>34.57</v>
       </c>
       <c r="Q223" s="3"/>
-      <c r="R223" s="3"/>
+      <c r="R223" s="5">
+        <v>44.62</v>
+      </c>
       <c r="S223" s="3"/>
       <c r="T223" s="2" t="s">
         <v>26</v>
@@ -13429,7 +13497,9 @@
         <v>31.74</v>
       </c>
       <c r="Q224" s="3"/>
-      <c r="R224" s="3"/>
+      <c r="R224" s="5">
+        <v>39.799999999999997</v>
+      </c>
       <c r="S224" s="3"/>
       <c r="T224" s="2" t="s">
         <v>26</v>
@@ -13475,7 +13545,9 @@
         <v>59.25</v>
       </c>
       <c r="Q225" s="3"/>
-      <c r="R225" s="3"/>
+      <c r="R225" s="5">
+        <v>74.430000000000007</v>
+      </c>
       <c r="S225" s="3"/>
       <c r="T225" s="2" t="s">
         <v>26</v>
@@ -13521,7 +13593,9 @@
         <v>44.77</v>
       </c>
       <c r="Q226" s="3"/>
-      <c r="R226" s="3"/>
+      <c r="R226" s="5">
+        <v>55.29</v>
+      </c>
       <c r="S226" s="3"/>
       <c r="T226" s="2" t="s">
         <v>26</v>
@@ -13567,7 +13641,9 @@
         <v>31.69</v>
       </c>
       <c r="Q227" s="3"/>
-      <c r="R227" s="3"/>
+      <c r="R227" s="5">
+        <v>40.81</v>
+      </c>
       <c r="S227" s="3"/>
       <c r="T227" s="2" t="s">
         <v>26</v>
@@ -13613,7 +13689,9 @@
         <v>25.54</v>
       </c>
       <c r="Q228" s="3"/>
-      <c r="R228" s="3"/>
+      <c r="R228" s="5">
+        <v>32.590000000000003</v>
+      </c>
       <c r="S228" s="3"/>
       <c r="T228" s="2" t="s">
         <v>26</v>
@@ -13659,7 +13737,9 @@
         <v>20.77</v>
       </c>
       <c r="Q229" s="3"/>
-      <c r="R229" s="3"/>
+      <c r="R229" s="5">
+        <v>26.02</v>
+      </c>
       <c r="S229" s="3"/>
       <c r="T229" s="2" t="s">
         <v>26</v>
@@ -13705,7 +13785,9 @@
         <v>22.58</v>
       </c>
       <c r="Q230" s="3"/>
-      <c r="R230" s="3"/>
+      <c r="R230" s="5">
+        <v>28.35</v>
+      </c>
       <c r="S230" s="3"/>
       <c r="T230" s="2" t="s">
         <v>26</v>
@@ -13751,7 +13833,9 @@
         <v>25.78</v>
       </c>
       <c r="Q231" s="3"/>
-      <c r="R231" s="3"/>
+      <c r="R231" s="5">
+        <v>31.77</v>
+      </c>
       <c r="S231" s="3"/>
       <c r="T231" s="2" t="s">
         <v>26</v>
@@ -13797,7 +13881,9 @@
         <v>25.36</v>
       </c>
       <c r="Q232" s="3"/>
-      <c r="R232" s="3"/>
+      <c r="R232" s="5">
+        <v>34.49</v>
+      </c>
       <c r="S232" s="3"/>
       <c r="T232" s="2" t="s">
         <v>26</v>
@@ -13843,7 +13929,9 @@
         <v>20.14</v>
       </c>
       <c r="Q233" s="3"/>
-      <c r="R233" s="3"/>
+      <c r="R233" s="5">
+        <v>25.38</v>
+      </c>
       <c r="S233" s="3"/>
       <c r="T233" s="2" t="s">
         <v>26</v>
@@ -13889,7 +13977,9 @@
         <v>22.36</v>
       </c>
       <c r="Q234" s="3"/>
-      <c r="R234" s="3"/>
+      <c r="R234" s="5">
+        <v>29.22</v>
+      </c>
       <c r="S234" s="3"/>
       <c r="T234" s="2" t="s">
         <v>26</v>
@@ -13935,7 +14025,9 @@
         <v>30.54</v>
       </c>
       <c r="Q235" s="3"/>
-      <c r="R235" s="3"/>
+      <c r="R235" s="5">
+        <v>39.78</v>
+      </c>
       <c r="S235" s="3"/>
       <c r="T235" s="2" t="s">
         <v>26</v>
@@ -13981,7 +14073,9 @@
         <v>35.81</v>
       </c>
       <c r="Q236" s="3"/>
-      <c r="R236" s="3"/>
+      <c r="R236" s="5">
+        <v>45.09</v>
+      </c>
       <c r="S236" s="3"/>
       <c r="T236" s="2" t="s">
         <v>26</v>
@@ -14027,7 +14121,9 @@
         <v>35.159999999999997</v>
       </c>
       <c r="Q237" s="3"/>
-      <c r="R237" s="3"/>
+      <c r="R237" s="5">
+        <v>44.47</v>
+      </c>
       <c r="S237" s="3"/>
       <c r="T237" s="2" t="s">
         <v>26</v>
@@ -14073,7 +14169,9 @@
         <v>32.61</v>
       </c>
       <c r="Q238" s="3"/>
-      <c r="R238" s="3"/>
+      <c r="R238" s="5">
+        <v>40.81</v>
+      </c>
       <c r="S238" s="3"/>
       <c r="T238" s="2" t="s">
         <v>26</v>
@@ -14119,7 +14217,9 @@
         <v>32.770000000000003</v>
       </c>
       <c r="Q239" s="3"/>
-      <c r="R239" s="3"/>
+      <c r="R239" s="5">
+        <v>40.99</v>
+      </c>
       <c r="S239" s="3"/>
       <c r="T239" s="2" t="s">
         <v>26</v>
@@ -14165,7 +14265,9 @@
         <v>44.59</v>
       </c>
       <c r="Q240" s="3"/>
-      <c r="R240" s="3"/>
+      <c r="R240" s="5">
+        <v>57.5</v>
+      </c>
       <c r="S240" s="3"/>
       <c r="T240" s="2" t="s">
         <v>26</v>
@@ -14226,7 +14328,9 @@
       <c r="R241" s="4">
         <v>2.9</v>
       </c>
-      <c r="S241" s="3"/>
+      <c r="S241" s="4">
+        <v>2.8</v>
+      </c>
       <c r="T241" s="2" t="s">
         <v>26</v>
       </c>
@@ -14281,12 +14385,14 @@
         <v>3.1</v>
       </c>
       <c r="Q242" s="4">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="R242" s="4">
         <v>2.8</v>
       </c>
-      <c r="S242" s="3"/>
+      <c r="S242" s="4">
+        <v>2.8</v>
+      </c>
       <c r="T242" s="2" t="s">
         <v>26</v>
       </c>
@@ -14346,7 +14452,9 @@
       <c r="R243" s="4">
         <v>2.9</v>
       </c>
-      <c r="S243" s="3"/>
+      <c r="S243" s="4">
+        <v>2.9</v>
+      </c>
       <c r="T243" s="2" t="s">
         <v>26</v>
       </c>
@@ -14401,12 +14509,14 @@
         <v>10.9</v>
       </c>
       <c r="Q244" s="4">
-        <v>11.9</v>
+        <v>12</v>
       </c>
       <c r="R244" s="4">
         <v>10.8</v>
       </c>
-      <c r="S244" s="3"/>
+      <c r="S244" s="4">
+        <v>11.3</v>
+      </c>
       <c r="T244" s="2" t="s">
         <v>26</v>
       </c>
@@ -14461,12 +14571,14 @@
         <v>3.8</v>
       </c>
       <c r="Q245" s="4">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="R245" s="4">
-        <v>3.3</v>
-      </c>
-      <c r="S245" s="3"/>
+        <v>3.2</v>
+      </c>
+      <c r="S245" s="4">
+        <v>3</v>
+      </c>
       <c r="T245" s="2" t="s">
         <v>26</v>
       </c>
@@ -14521,12 +14633,14 @@
         <v>2.5</v>
       </c>
       <c r="Q246" s="4">
-        <v>2.7</v>
+        <v>2.6</v>
       </c>
       <c r="R246" s="4">
         <v>2.1</v>
       </c>
-      <c r="S246" s="3"/>
+      <c r="S246" s="4">
+        <v>2.1</v>
+      </c>
       <c r="T246" s="2" t="s">
         <v>26</v>
       </c>
@@ -14586,7 +14700,9 @@
       <c r="R247" s="4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="S247" s="3"/>
+      <c r="S247" s="4">
+        <v>2</v>
+      </c>
       <c r="T247" s="2" t="s">
         <v>26</v>
       </c>
@@ -14646,7 +14762,9 @@
       <c r="R248" s="4">
         <v>1.7</v>
       </c>
-      <c r="S248" s="3"/>
+      <c r="S248" s="4">
+        <v>1.7</v>
+      </c>
       <c r="T248" s="2" t="s">
         <v>26</v>
       </c>
@@ -14701,12 +14819,14 @@
         <v>4.8</v>
       </c>
       <c r="Q249" s="4">
-        <v>6</v>
+        <v>6.1</v>
       </c>
       <c r="R249" s="4">
-        <v>5.5</v>
-      </c>
-      <c r="S249" s="3"/>
+        <v>5.4</v>
+      </c>
+      <c r="S249" s="4">
+        <v>5.2</v>
+      </c>
       <c r="T249" s="2" t="s">
         <v>26</v>
       </c>
@@ -16188,7 +16308,7 @@
         <v>17.399999999999999</v>
       </c>
       <c r="R278" s="4">
-        <v>17.5</v>
+        <v>17.8</v>
       </c>
       <c r="S278" s="3"/>
       <c r="T278" s="2" t="s">
@@ -16307,7 +16427,9 @@
       <c r="Q280" s="5">
         <v>12.51</v>
       </c>
-      <c r="R280" s="3"/>
+      <c r="R280" s="5">
+        <v>9.7799999999999994</v>
+      </c>
       <c r="S280" s="3"/>
       <c r="T280" s="2" t="s">
         <v>26</v>
@@ -18578,7 +18700,7 @@
         <v>3.38</v>
       </c>
       <c r="N319" s="5">
-        <v>3.31</v>
+        <v>3.29</v>
       </c>
       <c r="O319" s="5">
         <v>3.77</v>
@@ -18587,12 +18709,14 @@
         <v>3.89</v>
       </c>
       <c r="Q319" s="5">
-        <v>3.99</v>
+        <v>3.98</v>
       </c>
       <c r="R319" s="5">
-        <v>4.12</v>
-      </c>
-      <c r="S319" s="3"/>
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="S319" s="5">
+        <v>4.0599999999999996</v>
+      </c>
       <c r="T319" s="2" t="s">
         <v>376</v>
       </c>
@@ -18652,7 +18776,9 @@
       <c r="R320" s="5">
         <v>3494.39</v>
       </c>
-      <c r="S320" s="3"/>
+      <c r="S320" s="5">
+        <v>2603.83</v>
+      </c>
       <c r="T320" s="2" t="s">
         <v>380</v>
       </c>
@@ -18712,7 +18838,9 @@
       <c r="R321" s="5">
         <v>2661.32</v>
       </c>
-      <c r="S321" s="3"/>
+      <c r="S321" s="5">
+        <v>1744.48</v>
+      </c>
       <c r="T321" s="2" t="s">
         <v>380</v>
       </c>
@@ -18772,7 +18900,9 @@
       <c r="R322" s="5">
         <v>14.33</v>
       </c>
-      <c r="S322" s="3"/>
+      <c r="S322" s="5">
+        <v>0.38</v>
+      </c>
       <c r="T322" s="2" t="s">
         <v>380</v>
       </c>
@@ -18832,7 +18962,9 @@
       <c r="R323" s="5">
         <v>1.25</v>
       </c>
-      <c r="S323" s="3"/>
+      <c r="S323" s="5">
+        <v>6.36</v>
+      </c>
       <c r="T323" s="2" t="s">
         <v>380</v>
       </c>
@@ -18892,7 +19024,9 @@
       <c r="R324" s="5">
         <v>344.04</v>
       </c>
-      <c r="S324" s="3"/>
+      <c r="S324" s="5">
+        <v>254.4</v>
+      </c>
       <c r="T324" s="2" t="s">
         <v>380</v>
       </c>
@@ -18952,7 +19086,9 @@
       <c r="R325" s="5">
         <v>100.6</v>
       </c>
-      <c r="S325" s="3"/>
+      <c r="S325" s="5">
+        <v>62.44</v>
+      </c>
       <c r="T325" s="2" t="s">
         <v>380</v>
       </c>
@@ -24233,7 +24369,9 @@
       <c r="Q418" s="5">
         <v>0.59</v>
       </c>
-      <c r="R418" s="3"/>
+      <c r="R418" s="5">
+        <v>0.49</v>
+      </c>
       <c r="S418" s="3"/>
       <c r="T418" s="2" t="s">
         <v>26</v>
@@ -26568,7 +26706,9 @@
       <c r="R463" s="4">
         <v>3494.4</v>
       </c>
-      <c r="S463" s="3"/>
+      <c r="S463" s="4">
+        <v>2603.8000000000002</v>
+      </c>
       <c r="T463" s="2" t="s">
         <v>95</v>
       </c>
@@ -26614,21 +26754,23 @@
         <v>1.4</v>
       </c>
       <c r="N464" s="5">
-        <v>1.47</v>
+        <v>1.51</v>
       </c>
       <c r="O464" s="5">
         <v>1.41</v>
       </c>
       <c r="P464" s="5">
-        <v>1.47</v>
+        <v>1.46</v>
       </c>
       <c r="Q464" s="5">
         <v>1.44</v>
       </c>
       <c r="R464" s="5">
-        <v>1.29</v>
-      </c>
-      <c r="S464" s="3"/>
+        <v>1.28</v>
+      </c>
+      <c r="S464" s="5">
+        <v>1.26</v>
+      </c>
       <c r="T464" s="2" t="s">
         <v>485</v>
       </c>
@@ -26932,9 +27074,11 @@
         <v>53.6</v>
       </c>
       <c r="R469" s="4">
-        <v>49.3</v>
-      </c>
-      <c r="S469" s="3"/>
+        <v>49.2</v>
+      </c>
+      <c r="S469" s="4">
+        <v>49.6</v>
+      </c>
       <c r="T469" s="2" t="s">
         <v>26</v>
       </c>
@@ -26992,9 +27136,11 @@
         <v>-1.8</v>
       </c>
       <c r="R470" s="4">
-        <v>-3.7</v>
-      </c>
-      <c r="S470" s="3"/>
+        <v>-3.4</v>
+      </c>
+      <c r="S470" s="4">
+        <v>-5.0999999999999996</v>
+      </c>
       <c r="T470" s="2" t="s">
         <v>26</v>
       </c>
@@ -27403,7 +27549,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="74" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="72" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okno serwisowe 07.05.2024 - aktualizacja plików EXCEL
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dregerj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -835,6 +835,9 @@
     <t>7.2.1 Renewable energy share in the gross final energy consumption</t>
   </si>
   <si>
+    <t>Eurostat</t>
+  </si>
+  <si>
     <t>7.3.1 Energy intensity measured in terms of primary energy and gross domestic product (GDP)</t>
   </si>
   <si>
@@ -862,9 +865,6 @@
     <t>euro per kilogram [euro/kg]</t>
   </si>
   <si>
-    <t>Eurostat</t>
-  </si>
-  <si>
     <t>8.4.2 Domestic material consumption (DMC)</t>
   </si>
   <si>
@@ -1720,7 +1720,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 23-04-2024, 13:07</t>
+    <t>Last update: 07-05-2024, 09:52</t>
   </si>
 </sst>
 </file>
@@ -1735,7 +1735,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2275,7 +2275,7 @@
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2287,17 +2287,17 @@
     <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="36" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.5">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.5">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.5">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="29.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="97.5">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="97.5">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="97.5">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="19.5">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="29.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="29.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="29.25">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="68.25">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="29.25">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="29.25">
       <c r="A27" s="2" t="s">
         <v>21</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="29.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="39">
       <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="39">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="39">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="39">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="19.5">
       <c r="A33" s="2" t="s">
         <v>67</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="29.25">
       <c r="A34" s="2" t="s">
         <v>67</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="29.25">
       <c r="A35" s="2" t="s">
         <v>67</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="29.25">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="29.25">
       <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="29.25">
       <c r="A38" s="2" t="s">
         <v>67</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="29.25">
       <c r="A39" s="2" t="s">
         <v>67</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="39">
       <c r="A40" s="2" t="s">
         <v>67</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="97.5">
       <c r="A41" s="2" t="s">
         <v>67</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="97.5">
       <c r="A42" s="2" t="s">
         <v>67</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="97.5">
       <c r="A43" s="2" t="s">
         <v>67</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="97.5">
       <c r="A44" s="2" t="s">
         <v>67</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="97.5">
       <c r="A45" s="2" t="s">
         <v>67</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="97.5">
       <c r="A46" s="2" t="s">
         <v>67</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="48.75">
       <c r="A47" s="2" t="s">
         <v>67</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="48.75">
       <c r="A48" s="2" t="s">
         <v>67</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="19.5">
       <c r="A49" s="2" t="s">
         <v>67</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="29.25">
       <c r="A50" s="2" t="s">
         <v>67</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="19.5">
       <c r="A51" s="2" t="s">
         <v>96</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="19.5">
       <c r="A52" s="2" t="s">
         <v>96</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>96</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>96</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>96</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>96</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>96</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>96</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="29.25">
       <c r="A59" s="2" t="s">
         <v>96</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>96</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="29.25">
       <c r="A61" s="2" t="s">
         <v>96</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="29.25">
       <c r="A62" s="2" t="s">
         <v>96</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="29.25">
       <c r="A63" s="2" t="s">
         <v>96</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="19.5">
       <c r="A64" s="2" t="s">
         <v>96</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="29.25">
       <c r="A65" s="2" t="s">
         <v>96</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="29.25">
       <c r="A66" s="2" t="s">
         <v>96</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="29.25">
       <c r="A67" s="2" t="s">
         <v>96</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="29.25">
       <c r="A68" s="2" t="s">
         <v>96</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="29.25">
       <c r="A69" s="2" t="s">
         <v>96</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="29.25">
       <c r="A70" s="2" t="s">
         <v>96</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="29.25">
       <c r="A71" s="2" t="s">
         <v>96</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="19.5">
       <c r="A72" s="2" t="s">
         <v>96</v>
       </c>
@@ -6341,7 +6341,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="19.5">
       <c r="A73" s="2" t="s">
         <v>96</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="19.5">
       <c r="A74" s="2" t="s">
         <v>96</v>
       </c>
@@ -6461,7 +6461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="19.5">
       <c r="A75" s="2" t="s">
         <v>96</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="29.25">
       <c r="A76" s="2" t="s">
         <v>96</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="29.25">
       <c r="A77" s="2" t="s">
         <v>96</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" ht="19.5">
       <c r="A78" s="2" t="s">
         <v>96</v>
       </c>
@@ -6681,7 +6681,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" ht="19.5">
       <c r="A79" s="2" t="s">
         <v>96</v>
       </c>
@@ -6741,7 +6741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="19.5">
       <c r="A80" s="2" t="s">
         <v>96</v>
       </c>
@@ -6801,7 +6801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" ht="19.5">
       <c r="A81" s="2" t="s">
         <v>96</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" ht="29.25">
       <c r="A82" s="2" t="s">
         <v>96</v>
       </c>
@@ -6903,7 +6903,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" ht="29.25">
       <c r="A83" s="2" t="s">
         <v>96</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" ht="19.5">
       <c r="A84" s="2" t="s">
         <v>96</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" ht="29.25">
       <c r="A85" s="2" t="s">
         <v>96</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" ht="19.5">
       <c r="A86" s="2" t="s">
         <v>96</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" ht="19.5">
       <c r="A87" s="2" t="s">
         <v>96</v>
       </c>
@@ -7133,7 +7133,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" ht="19.5">
       <c r="A88" s="2" t="s">
         <v>96</v>
       </c>
@@ -7193,7 +7193,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" ht="19.5">
       <c r="A89" s="2" t="s">
         <v>96</v>
       </c>
@@ -7253,7 +7253,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" ht="19.5">
       <c r="A90" s="2" t="s">
         <v>96</v>
       </c>
@@ -7297,7 +7297,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" ht="29.25">
       <c r="A91" s="2" t="s">
         <v>96</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" ht="19.5">
       <c r="A92" s="2" t="s">
         <v>96</v>
       </c>
@@ -7393,7 +7393,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" ht="19.5">
       <c r="A93" s="2" t="s">
         <v>96</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" ht="19.5">
       <c r="A94" s="2" t="s">
         <v>96</v>
       </c>
@@ -7477,7 +7477,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" ht="19.5">
       <c r="A95" s="2" t="s">
         <v>96</v>
       </c>
@@ -7533,7 +7533,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" ht="78">
       <c r="A96" s="2" t="s">
         <v>150</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" ht="78">
       <c r="A97" s="2" t="s">
         <v>150</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" ht="78">
       <c r="A98" s="2" t="s">
         <v>150</v>
       </c>
@@ -7653,7 +7653,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" ht="78">
       <c r="A99" s="2" t="s">
         <v>150</v>
       </c>
@@ -7697,7 +7697,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" ht="78">
       <c r="A100" s="2" t="s">
         <v>150</v>
       </c>
@@ -7741,7 +7741,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" ht="78">
       <c r="A101" s="2" t="s">
         <v>150</v>
       </c>
@@ -7785,7 +7785,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" ht="78">
       <c r="A102" s="2" t="s">
         <v>150</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" ht="78">
       <c r="A103" s="2" t="s">
         <v>150</v>
       </c>
@@ -7873,7 +7873,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" ht="78">
       <c r="A104" s="2" t="s">
         <v>150</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" ht="29.25">
       <c r="A105" s="2" t="s">
         <v>150</v>
       </c>
@@ -7955,7 +7955,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" ht="19.5">
       <c r="A106" s="2" t="s">
         <v>150</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" ht="19.5">
       <c r="A107" s="2" t="s">
         <v>150</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" ht="19.5">
       <c r="A108" s="2" t="s">
         <v>150</v>
       </c>
@@ -8135,7 +8135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" ht="19.5">
       <c r="A109" s="2" t="s">
         <v>150</v>
       </c>
@@ -8173,7 +8173,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" ht="19.5">
       <c r="A110" s="2" t="s">
         <v>150</v>
       </c>
@@ -8211,7 +8211,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" ht="19.5">
       <c r="A111" s="2" t="s">
         <v>150</v>
       </c>
@@ -8249,7 +8249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" ht="29.25">
       <c r="A112" s="2" t="s">
         <v>150</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" ht="19.5">
       <c r="A113" s="2" t="s">
         <v>150</v>
       </c>
@@ -8345,7 +8345,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" ht="39">
       <c r="A114" s="2" t="s">
         <v>150</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" ht="48.75">
       <c r="A115" s="2" t="s">
         <v>150</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" ht="58.5">
       <c r="A116" s="2" t="s">
         <v>150</v>
       </c>
@@ -8495,7 +8495,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" ht="29.25">
       <c r="A117" s="2" t="s">
         <v>150</v>
       </c>
@@ -8545,7 +8545,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" ht="29.25">
       <c r="A118" s="2" t="s">
         <v>150</v>
       </c>
@@ -8591,7 +8591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" ht="19.5">
       <c r="A119" s="2" t="s">
         <v>150</v>
       </c>
@@ -8641,7 +8641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" ht="39">
       <c r="A120" s="2" t="s">
         <v>150</v>
       </c>
@@ -8691,7 +8691,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" ht="48.75">
       <c r="A121" s="2" t="s">
         <v>150</v>
       </c>
@@ -8741,7 +8741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" ht="58.5">
       <c r="A122" s="2" t="s">
         <v>150</v>
       </c>
@@ -8791,7 +8791,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" ht="29.25">
       <c r="A123" s="2" t="s">
         <v>150</v>
       </c>
@@ -8841,7 +8841,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" ht="48.75">
       <c r="A124" s="2" t="s">
         <v>150</v>
       </c>
@@ -8883,7 +8883,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" ht="48.75">
       <c r="A125" s="2" t="s">
         <v>150</v>
       </c>
@@ -8925,7 +8925,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20" ht="29.25">
       <c r="A126" s="2" t="s">
         <v>150</v>
       </c>
@@ -8985,7 +8985,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20" ht="29.25">
       <c r="A127" s="2" t="s">
         <v>150</v>
       </c>
@@ -9021,7 +9021,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" ht="29.25">
       <c r="A128" s="2" t="s">
         <v>150</v>
       </c>
@@ -9057,7 +9057,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20" ht="29.25">
       <c r="A129" s="2" t="s">
         <v>150</v>
       </c>
@@ -9093,7 +9093,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20" ht="29.25">
       <c r="A130" s="2" t="s">
         <v>150</v>
       </c>
@@ -9129,7 +9129,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" ht="29.25">
       <c r="A131" s="2" t="s">
         <v>150</v>
       </c>
@@ -9165,7 +9165,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20" ht="29.25">
       <c r="A132" s="2" t="s">
         <v>150</v>
       </c>
@@ -9201,7 +9201,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" ht="29.25">
       <c r="A133" s="2" t="s">
         <v>150</v>
       </c>
@@ -9237,7 +9237,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20" ht="29.25">
       <c r="A134" s="2" t="s">
         <v>150</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:20" ht="29.25">
       <c r="A135" s="2" t="s">
         <v>150</v>
       </c>
@@ -9309,7 +9309,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20" ht="29.25">
       <c r="A136" s="2" t="s">
         <v>150</v>
       </c>
@@ -9345,7 +9345,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20" ht="29.25">
       <c r="A137" s="2" t="s">
         <v>150</v>
       </c>
@@ -9381,7 +9381,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:20" ht="29.25">
       <c r="A138" s="2" t="s">
         <v>150</v>
       </c>
@@ -9417,7 +9417,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" ht="29.25">
       <c r="A139" s="2" t="s">
         <v>150</v>
       </c>
@@ -9453,7 +9453,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20" ht="29.25">
       <c r="A140" s="2" t="s">
         <v>150</v>
       </c>
@@ -9489,7 +9489,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:20" ht="29.25">
       <c r="A141" s="2" t="s">
         <v>150</v>
       </c>
@@ -9525,7 +9525,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:20" ht="29.25">
       <c r="A142" s="2" t="s">
         <v>150</v>
       </c>
@@ -9561,7 +9561,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:20" ht="48.75">
       <c r="A143" s="2" t="s">
         <v>150</v>
       </c>
@@ -9623,7 +9623,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" ht="58.5">
       <c r="A144" s="2" t="s">
         <v>150</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" ht="58.5">
       <c r="A145" s="2" t="s">
         <v>150</v>
       </c>
@@ -9721,7 +9721,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" ht="58.5">
       <c r="A146" s="2" t="s">
         <v>150</v>
       </c>
@@ -9757,7 +9757,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" ht="58.5">
       <c r="A147" s="2" t="s">
         <v>150</v>
       </c>
@@ -9819,7 +9819,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:20" ht="58.5">
       <c r="A148" s="2" t="s">
         <v>150</v>
       </c>
@@ -9881,7 +9881,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:20" ht="58.5">
       <c r="A149" s="2" t="s">
         <v>150</v>
       </c>
@@ -9943,7 +9943,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:20" ht="29.25">
       <c r="A150" s="2" t="s">
         <v>150</v>
       </c>
@@ -9997,7 +9997,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:20" ht="58.5">
       <c r="A151" s="2" t="s">
         <v>150</v>
       </c>
@@ -10053,7 +10053,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:20" ht="58.5">
       <c r="A152" s="2" t="s">
         <v>150</v>
       </c>
@@ -10109,7 +10109,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:20" ht="58.5">
       <c r="A153" s="2" t="s">
         <v>150</v>
       </c>
@@ -10165,7 +10165,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:20" ht="58.5">
       <c r="A154" s="2" t="s">
         <v>150</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:20" ht="29.25">
       <c r="A155" s="2" t="s">
         <v>206</v>
       </c>
@@ -10257,7 +10257,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:20" ht="19.5">
       <c r="A156" s="2" t="s">
         <v>206</v>
       </c>
@@ -10317,7 +10317,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:20" ht="39">
       <c r="A157" s="2" t="s">
         <v>206</v>
       </c>
@@ -10353,7 +10353,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:20" ht="39">
       <c r="A158" s="2" t="s">
         <v>206</v>
       </c>
@@ -10389,7 +10389,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:20" ht="39">
       <c r="A159" s="2" t="s">
         <v>206</v>
       </c>
@@ -10425,7 +10425,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:20" ht="39">
       <c r="A160" s="2" t="s">
         <v>206</v>
       </c>
@@ -10461,7 +10461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:20" ht="39">
       <c r="A161" s="2" t="s">
         <v>206</v>
       </c>
@@ -10497,7 +10497,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:20" ht="19.5">
       <c r="A162" s="2" t="s">
         <v>206</v>
       </c>
@@ -10533,7 +10533,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:20" ht="19.5">
       <c r="A163" s="2" t="s">
         <v>206</v>
       </c>
@@ -10569,7 +10569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:20" ht="19.5">
       <c r="A164" s="2" t="s">
         <v>206</v>
       </c>
@@ -10605,7 +10605,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:20" ht="19.5">
       <c r="A165" s="2" t="s">
         <v>206</v>
       </c>
@@ -10641,7 +10641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:20" ht="19.5">
       <c r="A166" s="2" t="s">
         <v>206</v>
       </c>
@@ -10677,7 +10677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:20" ht="19.5">
       <c r="A167" s="2" t="s">
         <v>206</v>
       </c>
@@ -10713,7 +10713,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:20" ht="19.5">
       <c r="A168" s="2" t="s">
         <v>206</v>
       </c>
@@ -10749,7 +10749,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:20" ht="19.5">
       <c r="A169" s="2" t="s">
         <v>206</v>
       </c>
@@ -10785,7 +10785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:20" ht="29.25">
       <c r="A170" s="2" t="s">
         <v>206</v>
       </c>
@@ -10827,7 +10827,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:20" ht="29.25">
       <c r="A171" s="2" t="s">
         <v>206</v>
       </c>
@@ -10869,7 +10869,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:20" ht="29.25">
       <c r="A172" s="2" t="s">
         <v>206</v>
       </c>
@@ -10929,7 +10929,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:20" ht="29.25">
       <c r="A173" s="2" t="s">
         <v>206</v>
       </c>
@@ -10989,7 +10989,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:20" ht="29.25">
       <c r="A174" s="2" t="s">
         <v>206</v>
       </c>
@@ -11049,7 +11049,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:20" ht="29.25">
       <c r="A175" s="2" t="s">
         <v>206</v>
       </c>
@@ -11109,7 +11109,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" ht="29.25">
       <c r="A176" s="2" t="s">
         <v>206</v>
       </c>
@@ -11169,7 +11169,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:20" ht="19.5">
       <c r="A177" s="2" t="s">
         <v>206</v>
       </c>
@@ -11217,7 +11217,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:20" ht="39">
       <c r="A178" s="2" t="s">
         <v>206</v>
       </c>
@@ -11265,7 +11265,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:20" ht="19.5">
       <c r="A179" s="2" t="s">
         <v>206</v>
       </c>
@@ -11313,7 +11313,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:20" ht="39">
       <c r="A180" s="2" t="s">
         <v>206</v>
       </c>
@@ -11361,7 +11361,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:20" ht="39">
       <c r="A181" s="2" t="s">
         <v>206</v>
       </c>
@@ -11409,7 +11409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:20" ht="39">
       <c r="A182" s="2" t="s">
         <v>206</v>
       </c>
@@ -11457,7 +11457,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:20" ht="39">
       <c r="A183" s="2" t="s">
         <v>206</v>
       </c>
@@ -11505,7 +11505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:20" ht="39">
       <c r="A184" s="2" t="s">
         <v>206</v>
       </c>
@@ -11545,7 +11545,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:20" ht="39">
       <c r="A185" s="2" t="s">
         <v>206</v>
       </c>
@@ -11585,7 +11585,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:20" ht="39">
       <c r="A186" s="2" t="s">
         <v>206</v>
       </c>
@@ -11625,7 +11625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:20" ht="39">
       <c r="A187" s="2" t="s">
         <v>206</v>
       </c>
@@ -11665,7 +11665,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:20" ht="39">
       <c r="A188" s="2" t="s">
         <v>206</v>
       </c>
@@ -11705,7 +11705,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:20" ht="39">
       <c r="A189" s="2" t="s">
         <v>206</v>
       </c>
@@ -11745,7 +11745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:20" ht="39">
       <c r="A190" s="2" t="s">
         <v>206</v>
       </c>
@@ -11785,7 +11785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:20" ht="39">
       <c r="A191" s="2" t="s">
         <v>206</v>
       </c>
@@ -11825,7 +11825,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:20" ht="39">
       <c r="A192" s="2" t="s">
         <v>206</v>
       </c>
@@ -11865,7 +11865,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:20" ht="39">
       <c r="A193" s="2" t="s">
         <v>206</v>
       </c>
@@ -11905,7 +11905,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:20" ht="39">
       <c r="A194" s="2" t="s">
         <v>206</v>
       </c>
@@ -11945,7 +11945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:20" ht="39">
       <c r="A195" s="2" t="s">
         <v>206</v>
       </c>
@@ -11985,7 +11985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:20" ht="19.5">
       <c r="A196" s="2" t="s">
         <v>206</v>
       </c>
@@ -12027,7 +12027,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:20" ht="19.5">
       <c r="A197" s="2" t="s">
         <v>206</v>
       </c>
@@ -12085,7 +12085,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:20" ht="19.5">
       <c r="A198" s="2" t="s">
         <v>206</v>
       </c>
@@ -12143,7 +12143,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:20" ht="19.5">
       <c r="A199" s="2" t="s">
         <v>246</v>
       </c>
@@ -12201,7 +12201,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:20" ht="29.25">
       <c r="A200" s="2" t="s">
         <v>246</v>
       </c>
@@ -12259,7 +12259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:20" ht="19.5">
       <c r="A201" s="2" t="s">
         <v>246</v>
       </c>
@@ -12319,7 +12319,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:20" ht="19.5">
       <c r="A202" s="2" t="s">
         <v>246</v>
       </c>
@@ -12357,7 +12357,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:20" ht="19.5">
       <c r="A203" s="2" t="s">
         <v>246</v>
       </c>
@@ -12395,7 +12395,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:20" ht="29.25">
       <c r="A204" s="2" t="s">
         <v>246</v>
       </c>
@@ -12453,7 +12453,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:20" ht="19.5">
       <c r="A205" s="2" t="s">
         <v>246</v>
       </c>
@@ -12509,7 +12509,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:20" ht="19.5">
       <c r="A206" s="2" t="s">
         <v>246</v>
       </c>
@@ -12555,7 +12555,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:20" ht="29.25">
       <c r="A207" s="2" t="s">
         <v>246</v>
       </c>
@@ -12615,7 +12615,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:20" ht="29.25">
       <c r="A208" s="2" t="s">
         <v>246</v>
       </c>
@@ -12669,7 +12669,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:20" ht="39">
       <c r="A209" s="2" t="s">
         <v>246</v>
       </c>
@@ -12729,7 +12729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:20" ht="19.5">
       <c r="A210" s="2" t="s">
         <v>267</v>
       </c>
@@ -12765,7 +12765,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:20" ht="19.5">
       <c r="A211" s="2" t="s">
         <v>267</v>
       </c>
@@ -12822,15 +12822,15 @@
       </c>
       <c r="S211" s="3"/>
       <c r="T211" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="212" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="212" spans="1:20" ht="29.25">
       <c r="A212" s="2" t="s">
         <v>267</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>23</v>
@@ -12839,7 +12839,7 @@
         <v>24</v>
       </c>
       <c r="E212" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F212" s="7">
         <v>0.36799999999999999</v>
@@ -12881,12 +12881,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:20" ht="29.25">
       <c r="A213" s="2" t="s">
         <v>267</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>23</v>
@@ -12935,12 +12935,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:20" ht="29.25">
       <c r="A214" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C214" s="2" t="s">
         <v>23</v>
@@ -12995,12 +12995,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:20" ht="29.25">
       <c r="A215" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C215" s="2" t="s">
         <v>23</v>
@@ -13055,12 +13055,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:20" ht="29.25">
       <c r="A216" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C216" s="2" t="s">
         <v>31</v>
@@ -13097,12 +13097,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:20" ht="29.25">
       <c r="A217" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C217" s="2" t="s">
         <v>31</v>
@@ -13139,12 +13139,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:20" ht="29.25">
       <c r="A218" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C218" s="2" t="s">
         <v>31</v>
@@ -13181,12 +13181,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:20" ht="29.25">
       <c r="A219" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>23</v>
@@ -13195,7 +13195,7 @@
         <v>24</v>
       </c>
       <c r="E219" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F219" s="5">
         <v>0.56999999999999995</v>
@@ -13238,12 +13238,12 @@
       </c>
       <c r="S219" s="3"/>
       <c r="T219" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="220" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="220" spans="1:20" ht="29.25">
       <c r="A220" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>280</v>
@@ -13298,12 +13298,12 @@
       </c>
       <c r="S220" s="3"/>
       <c r="T220" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="221" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="221" spans="1:20" ht="29.25">
       <c r="A221" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B221" s="2" t="s">
         <v>280</v>
@@ -13358,12 +13358,12 @@
       </c>
       <c r="S221" s="3"/>
       <c r="T221" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="222" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="222" spans="1:20" ht="29.25">
       <c r="A222" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>283</v>
@@ -13409,9 +13409,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:20" ht="29.25">
       <c r="A223" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>283</v>
@@ -13457,9 +13457,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:20" ht="29.25">
       <c r="A224" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>283</v>
@@ -13505,9 +13505,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:20" ht="29.25">
       <c r="A225" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>283</v>
@@ -13553,9 +13553,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:20" ht="29.25">
       <c r="A226" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B226" s="2" t="s">
         <v>283</v>
@@ -13601,9 +13601,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:20" ht="29.25">
       <c r="A227" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>283</v>
@@ -13649,9 +13649,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:20" ht="29.25">
       <c r="A228" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>283</v>
@@ -13697,9 +13697,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:20" ht="29.25">
       <c r="A229" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>283</v>
@@ -13745,9 +13745,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:20" ht="39">
       <c r="A230" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>283</v>
@@ -13793,9 +13793,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:20" ht="29.25">
       <c r="A231" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B231" s="2" t="s">
         <v>283</v>
@@ -13841,9 +13841,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:20" ht="39">
       <c r="A232" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>283</v>
@@ -13889,9 +13889,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:20" ht="29.25">
       <c r="A233" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B233" s="2" t="s">
         <v>283</v>
@@ -13937,9 +13937,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:20" ht="29.25">
       <c r="A234" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B234" s="2" t="s">
         <v>283</v>
@@ -13985,9 +13985,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:20" ht="29.25">
       <c r="A235" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>283</v>
@@ -14033,9 +14033,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:20" ht="29.25">
       <c r="A236" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B236" s="2" t="s">
         <v>283</v>
@@ -14081,9 +14081,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:20" ht="29.25">
       <c r="A237" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B237" s="2" t="s">
         <v>283</v>
@@ -14129,9 +14129,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:20" ht="29.25">
       <c r="A238" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B238" s="2" t="s">
         <v>283</v>
@@ -14177,9 +14177,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:20" ht="29.25">
       <c r="A239" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B239" s="2" t="s">
         <v>283</v>
@@ -14225,9 +14225,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:20" ht="29.25">
       <c r="A240" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B240" s="2" t="s">
         <v>283</v>
@@ -14273,9 +14273,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:20" ht="29.25">
       <c r="A241" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B241" s="2" t="s">
         <v>298</v>
@@ -14335,9 +14335,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:20" ht="29.25">
       <c r="A242" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B242" s="2" t="s">
         <v>298</v>
@@ -14397,9 +14397,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="243" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:20" ht="29.25">
       <c r="A243" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B243" s="2" t="s">
         <v>298</v>
@@ -14459,9 +14459,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:20" ht="29.25">
       <c r="A244" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>298</v>
@@ -14521,9 +14521,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:20" ht="29.25">
       <c r="A245" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B245" s="2" t="s">
         <v>298</v>
@@ -14583,9 +14583,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:20" ht="29.25">
       <c r="A246" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B246" s="2" t="s">
         <v>298</v>
@@ -14645,9 +14645,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:20" ht="29.25">
       <c r="A247" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B247" s="2" t="s">
         <v>298</v>
@@ -14707,9 +14707,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:20" ht="29.25">
       <c r="A248" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B248" s="2" t="s">
         <v>298</v>
@@ -14769,9 +14769,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:20" ht="29.25">
       <c r="A249" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B249" s="2" t="s">
         <v>298</v>
@@ -14831,9 +14831,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:20" ht="29.25">
       <c r="A250" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B250" s="2" t="s">
         <v>302</v>
@@ -14891,9 +14891,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:20" ht="29.25">
       <c r="A251" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>303</v>
@@ -14951,9 +14951,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:20" ht="29.25">
       <c r="A252" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B252" s="2" t="s">
         <v>303</v>
@@ -15011,9 +15011,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:20" ht="39">
       <c r="A253" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B253" s="2" t="s">
         <v>305</v>
@@ -15053,9 +15053,9 @@
         <v>308</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:20" ht="39">
       <c r="A254" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B254" s="2" t="s">
         <v>305</v>
@@ -15095,9 +15095,9 @@
         <v>308</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:20" ht="39">
       <c r="A255" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B255" s="2" t="s">
         <v>305</v>
@@ -15137,9 +15137,9 @@
         <v>308</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:20" ht="29.25">
       <c r="A256" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B256" s="2" t="s">
         <v>311</v>
@@ -15197,9 +15197,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:20" ht="48.75">
       <c r="A257" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B257" s="2" t="s">
         <v>312</v>
@@ -15255,9 +15255,9 @@
         <v>314</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:20" ht="29.25">
       <c r="A258" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>315</v>
@@ -15291,9 +15291,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:20" ht="29.25">
       <c r="A259" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>315</v>
@@ -15327,9 +15327,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:20" ht="29.25">
       <c r="A260" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B260" s="2" t="s">
         <v>315</v>
@@ -15363,9 +15363,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:20" ht="29.25">
       <c r="A261" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B261" s="2" t="s">
         <v>315</v>
@@ -15399,9 +15399,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:20" ht="29.25">
       <c r="A262" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B262" s="2" t="s">
         <v>315</v>
@@ -15435,9 +15435,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:20" ht="29.25">
       <c r="A263" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>315</v>
@@ -15471,9 +15471,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:20" ht="29.25">
       <c r="A264" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>315</v>
@@ -15507,9 +15507,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:20" ht="29.25">
       <c r="A265" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>315</v>
@@ -15543,9 +15543,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:20" ht="29.25">
       <c r="A266" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B266" s="2" t="s">
         <v>318</v>
@@ -15595,7 +15595,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:20" ht="29.25">
       <c r="A267" s="2" t="s">
         <v>319</v>
       </c>
@@ -15655,7 +15655,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:20" ht="29.25">
       <c r="A268" s="2" t="s">
         <v>319</v>
       </c>
@@ -15715,7 +15715,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:20" ht="29.25">
       <c r="A269" s="2" t="s">
         <v>319</v>
       </c>
@@ -15775,7 +15775,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:20" ht="29.25">
       <c r="A270" s="2" t="s">
         <v>319</v>
       </c>
@@ -15835,7 +15835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:20" ht="29.25">
       <c r="A271" s="2" t="s">
         <v>319</v>
       </c>
@@ -15895,7 +15895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="272" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:20" ht="29.25">
       <c r="A272" s="2" t="s">
         <v>319</v>
       </c>
@@ -15955,7 +15955,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:20" ht="29.25">
       <c r="A273" s="2" t="s">
         <v>319</v>
       </c>
@@ -16015,7 +16015,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:20" ht="29.25">
       <c r="A274" s="2" t="s">
         <v>319</v>
       </c>
@@ -16075,7 +16075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="275" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:20" ht="29.25">
       <c r="A275" s="2" t="s">
         <v>319</v>
       </c>
@@ -16135,7 +16135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="276" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:20" ht="29.25">
       <c r="A276" s="2" t="s">
         <v>319</v>
       </c>
@@ -16195,7 +16195,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:20" ht="29.25">
       <c r="A277" s="2" t="s">
         <v>319</v>
       </c>
@@ -16255,7 +16255,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:20" ht="29.25">
       <c r="A278" s="2" t="s">
         <v>319</v>
       </c>
@@ -16315,7 +16315,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:20" ht="29.25">
       <c r="A279" s="2" t="s">
         <v>319</v>
       </c>
@@ -16375,7 +16375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:20" ht="29.25">
       <c r="A280" s="2" t="s">
         <v>319</v>
       </c>
@@ -16435,7 +16435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="281" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:20" ht="29.25">
       <c r="A281" s="2" t="s">
         <v>319</v>
       </c>
@@ -16495,7 +16495,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="282" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:20" ht="29.25">
       <c r="A282" s="2" t="s">
         <v>319</v>
       </c>
@@ -16555,7 +16555,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:20" ht="29.25">
       <c r="A283" s="2" t="s">
         <v>319</v>
       </c>
@@ -16615,7 +16615,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:20" ht="29.25">
       <c r="A284" s="2" t="s">
         <v>319</v>
       </c>
@@ -16675,7 +16675,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:20" ht="29.25">
       <c r="A285" s="2" t="s">
         <v>319</v>
       </c>
@@ -16735,7 +16735,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:20" ht="29.25">
       <c r="A286" s="2" t="s">
         <v>319</v>
       </c>
@@ -16795,7 +16795,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:20" ht="29.25">
       <c r="A287" s="2" t="s">
         <v>319</v>
       </c>
@@ -16847,7 +16847,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:20" ht="29.25">
       <c r="A288" s="2" t="s">
         <v>319</v>
       </c>
@@ -16907,7 +16907,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:20" ht="29.25">
       <c r="A289" s="2" t="s">
         <v>319</v>
       </c>
@@ -16967,7 +16967,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:20" ht="29.25">
       <c r="A290" s="2" t="s">
         <v>319</v>
       </c>
@@ -17021,7 +17021,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="291" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:20" ht="29.25">
       <c r="A291" s="2" t="s">
         <v>319</v>
       </c>
@@ -17075,7 +17075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:20" ht="39">
       <c r="A292" s="2" t="s">
         <v>319</v>
       </c>
@@ -17127,7 +17127,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:20" ht="39">
       <c r="A293" s="2" t="s">
         <v>319</v>
       </c>
@@ -17179,7 +17179,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:20" ht="19.5">
       <c r="A294" s="2" t="s">
         <v>351</v>
       </c>
@@ -17239,7 +17239,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:20" ht="68.25">
       <c r="A295" s="2" t="s">
         <v>351</v>
       </c>
@@ -17299,7 +17299,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:20" ht="19.5">
       <c r="A296" s="2" t="s">
         <v>351</v>
       </c>
@@ -17359,7 +17359,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:20" ht="19.5">
       <c r="A297" s="2" t="s">
         <v>351</v>
       </c>
@@ -17419,7 +17419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:20" ht="19.5">
       <c r="A298" s="2" t="s">
         <v>351</v>
       </c>
@@ -17479,7 +17479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:20" ht="19.5">
       <c r="A299" s="2" t="s">
         <v>351</v>
       </c>
@@ -17539,7 +17539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:20" ht="19.5">
       <c r="A300" s="2" t="s">
         <v>351</v>
       </c>
@@ -17599,7 +17599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:20" ht="19.5">
       <c r="A301" s="2" t="s">
         <v>351</v>
       </c>
@@ -17659,7 +17659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:20" ht="19.5">
       <c r="A302" s="2" t="s">
         <v>351</v>
       </c>
@@ -17719,7 +17719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:20" ht="19.5">
       <c r="A303" s="2" t="s">
         <v>351</v>
       </c>
@@ -17779,7 +17779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="304" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:20" ht="19.5">
       <c r="A304" s="2" t="s">
         <v>351</v>
       </c>
@@ -17839,7 +17839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="305" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:20" ht="19.5">
       <c r="A305" s="2" t="s">
         <v>351</v>
       </c>
@@ -17879,7 +17879,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="306" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:20" ht="19.5">
       <c r="A306" s="2" t="s">
         <v>351</v>
       </c>
@@ -17939,7 +17939,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="307" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:20" ht="39">
       <c r="A307" s="2" t="s">
         <v>351</v>
       </c>
@@ -17999,7 +17999,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="308" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:20" ht="48.75">
       <c r="A308" s="2" t="s">
         <v>351</v>
       </c>
@@ -18059,7 +18059,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="309" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:20" ht="39">
       <c r="A309" s="2" t="s">
         <v>351</v>
       </c>
@@ -18119,7 +18119,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="310" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:20" ht="39">
       <c r="A310" s="2" t="s">
         <v>351</v>
       </c>
@@ -18179,7 +18179,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="311" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:20" ht="29.25">
       <c r="A311" s="2" t="s">
         <v>351</v>
       </c>
@@ -18239,7 +18239,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="312" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:20" ht="39">
       <c r="A312" s="2" t="s">
         <v>351</v>
       </c>
@@ -18299,7 +18299,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="313" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:20" ht="29.25">
       <c r="A313" s="2" t="s">
         <v>351</v>
       </c>
@@ -18359,7 +18359,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="314" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:20" ht="29.25">
       <c r="A314" s="2" t="s">
         <v>351</v>
       </c>
@@ -18419,7 +18419,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="315" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:20" ht="39">
       <c r="A315" s="2" t="s">
         <v>351</v>
       </c>
@@ -18479,7 +18479,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="316" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:20" ht="29.25">
       <c r="A316" s="2" t="s">
         <v>351</v>
       </c>
@@ -18539,7 +18539,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="317" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:20" ht="39">
       <c r="A317" s="2" t="s">
         <v>351</v>
       </c>
@@ -18599,7 +18599,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="318" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:20" ht="29.25">
       <c r="A318" s="2" t="s">
         <v>351</v>
       </c>
@@ -18659,7 +18659,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="319" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:20" ht="29.25">
       <c r="A319" s="2" t="s">
         <v>351</v>
       </c>
@@ -18721,7 +18721,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="320" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:20" ht="39">
       <c r="A320" s="2" t="s">
         <v>351</v>
       </c>
@@ -18783,7 +18783,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="321" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:20" ht="39">
       <c r="A321" s="2" t="s">
         <v>351</v>
       </c>
@@ -18845,7 +18845,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="322" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:20" ht="68.25">
       <c r="A322" s="2" t="s">
         <v>351</v>
       </c>
@@ -18907,7 +18907,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="323" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:20" ht="58.5">
       <c r="A323" s="2" t="s">
         <v>351</v>
       </c>
@@ -18969,7 +18969,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="324" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:20" ht="68.25">
       <c r="A324" s="2" t="s">
         <v>351</v>
       </c>
@@ -19031,7 +19031,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="325" spans="1:20" ht="72" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:20" ht="68.25">
       <c r="A325" s="2" t="s">
         <v>351</v>
       </c>
@@ -19093,7 +19093,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="326" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:20" ht="39">
       <c r="A326" s="2" t="s">
         <v>351</v>
       </c>
@@ -19153,7 +19153,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="327" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:20" ht="68.25">
       <c r="A327" s="2" t="s">
         <v>351</v>
       </c>
@@ -19213,7 +19213,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="328" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:20" ht="58.5">
       <c r="A328" s="2" t="s">
         <v>351</v>
       </c>
@@ -19273,7 +19273,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="329" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:20" ht="68.25">
       <c r="A329" s="2" t="s">
         <v>351</v>
       </c>
@@ -19333,7 +19333,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="330" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:20" ht="68.25">
       <c r="A330" s="2" t="s">
         <v>351</v>
       </c>
@@ -19393,7 +19393,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="331" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:20" ht="29.25">
       <c r="A331" s="2" t="s">
         <v>392</v>
       </c>
@@ -19449,7 +19449,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="332" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:20" ht="29.25">
       <c r="A332" s="2" t="s">
         <v>392</v>
       </c>
@@ -19505,7 +19505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="333" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:20" ht="29.25">
       <c r="A333" s="2" t="s">
         <v>392</v>
       </c>
@@ -19561,7 +19561,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:20" ht="29.25">
       <c r="A334" s="2" t="s">
         <v>392</v>
       </c>
@@ -19621,7 +19621,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="335" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:20" ht="29.25">
       <c r="A335" s="2" t="s">
         <v>392</v>
       </c>
@@ -19681,7 +19681,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="336" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:20" ht="29.25">
       <c r="A336" s="2" t="s">
         <v>392</v>
       </c>
@@ -19741,7 +19741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="337" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:20" ht="29.25">
       <c r="A337" s="2" t="s">
         <v>392</v>
       </c>
@@ -19801,7 +19801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="338" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:20" ht="29.25">
       <c r="A338" s="2" t="s">
         <v>392</v>
       </c>
@@ -19861,7 +19861,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="339" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:20" ht="29.25">
       <c r="A339" s="2" t="s">
         <v>392</v>
       </c>
@@ -19921,7 +19921,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="340" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:20" ht="29.25">
       <c r="A340" s="2" t="s">
         <v>392</v>
       </c>
@@ -19981,7 +19981,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="341" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:20" ht="29.25">
       <c r="A341" s="2" t="s">
         <v>392</v>
       </c>
@@ -20041,7 +20041,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="342" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:20" ht="29.25">
       <c r="A342" s="2" t="s">
         <v>392</v>
       </c>
@@ -20101,7 +20101,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="343" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:20" ht="29.25">
       <c r="A343" s="2" t="s">
         <v>392</v>
       </c>
@@ -20161,7 +20161,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="344" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:20" ht="29.25">
       <c r="A344" s="2" t="s">
         <v>392</v>
       </c>
@@ -20221,7 +20221,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="345" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:20" ht="29.25">
       <c r="A345" s="2" t="s">
         <v>392</v>
       </c>
@@ -20281,7 +20281,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="346" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:20" ht="29.25">
       <c r="A346" s="2" t="s">
         <v>392</v>
       </c>
@@ -20341,7 +20341,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="347" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:20" ht="29.25">
       <c r="A347" s="2" t="s">
         <v>392</v>
       </c>
@@ -20401,7 +20401,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="348" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:20" ht="29.25">
       <c r="A348" s="2" t="s">
         <v>392</v>
       </c>
@@ -20461,7 +20461,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="349" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:20" ht="29.25">
       <c r="A349" s="2" t="s">
         <v>392</v>
       </c>
@@ -20521,7 +20521,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="350" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:20" ht="29.25">
       <c r="A350" s="2" t="s">
         <v>392</v>
       </c>
@@ -20581,7 +20581,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="351" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:20" ht="29.25">
       <c r="A351" s="2" t="s">
         <v>392</v>
       </c>
@@ -20641,7 +20641,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="352" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:20" ht="29.25">
       <c r="A352" s="2" t="s">
         <v>392</v>
       </c>
@@ -20701,7 +20701,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="353" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:20" ht="29.25">
       <c r="A353" s="2" t="s">
         <v>392</v>
       </c>
@@ -20761,7 +20761,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="354" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:20" ht="29.25">
       <c r="A354" s="2" t="s">
         <v>392</v>
       </c>
@@ -20821,7 +20821,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="355" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:20" ht="29.25">
       <c r="A355" s="2" t="s">
         <v>392</v>
       </c>
@@ -20881,7 +20881,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="356" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:20" ht="29.25">
       <c r="A356" s="2" t="s">
         <v>392</v>
       </c>
@@ -20941,7 +20941,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="357" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:20" ht="29.25">
       <c r="A357" s="2" t="s">
         <v>392</v>
       </c>
@@ -21001,7 +21001,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="358" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:20" ht="29.25">
       <c r="A358" s="2" t="s">
         <v>392</v>
       </c>
@@ -21059,7 +21059,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="359" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:20" ht="29.25">
       <c r="A359" s="2" t="s">
         <v>392</v>
       </c>
@@ -21119,7 +21119,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="360" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:20" ht="29.25">
       <c r="A360" s="2" t="s">
         <v>392</v>
       </c>
@@ -21179,7 +21179,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="361" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:20" ht="29.25">
       <c r="A361" s="2" t="s">
         <v>392</v>
       </c>
@@ -21239,7 +21239,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="362" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:20" ht="29.25">
       <c r="A362" s="2" t="s">
         <v>392</v>
       </c>
@@ -21299,7 +21299,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="363" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:20" ht="29.25">
       <c r="A363" s="2" t="s">
         <v>392</v>
       </c>
@@ -21359,7 +21359,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="364" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:20" ht="39">
       <c r="A364" s="2" t="s">
         <v>392</v>
       </c>
@@ -21419,7 +21419,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="365" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:20" ht="39">
       <c r="A365" s="2" t="s">
         <v>392</v>
       </c>
@@ -21479,7 +21479,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="366" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:20" ht="39">
       <c r="A366" s="2" t="s">
         <v>392</v>
       </c>
@@ -21539,7 +21539,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="367" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:20" ht="39">
       <c r="A367" s="2" t="s">
         <v>392</v>
       </c>
@@ -21599,7 +21599,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="368" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:20" ht="39">
       <c r="A368" s="2" t="s">
         <v>392</v>
       </c>
@@ -21659,7 +21659,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="369" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:20" ht="39">
       <c r="A369" s="2" t="s">
         <v>392</v>
       </c>
@@ -21719,7 +21719,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="370" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:20" ht="39">
       <c r="A370" s="2" t="s">
         <v>392</v>
       </c>
@@ -21779,7 +21779,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="371" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:20" ht="39">
       <c r="A371" s="2" t="s">
         <v>392</v>
       </c>
@@ -21839,7 +21839,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="372" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:20" ht="29.25">
       <c r="A372" s="2" t="s">
         <v>392</v>
       </c>
@@ -21891,7 +21891,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="373" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:20" ht="68.25">
       <c r="A373" s="2" t="s">
         <v>392</v>
       </c>
@@ -21943,7 +21943,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="374" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:20" ht="29.25">
       <c r="A374" s="2" t="s">
         <v>392</v>
       </c>
@@ -21995,7 +21995,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="375" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:20" ht="29.25">
       <c r="A375" s="2" t="s">
         <v>392</v>
       </c>
@@ -22047,7 +22047,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="376" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:20" ht="39">
       <c r="A376" s="2" t="s">
         <v>427</v>
       </c>
@@ -22061,7 +22061,7 @@
         <v>24</v>
       </c>
       <c r="E376" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F376" s="5">
         <v>0.56999999999999995</v>
@@ -22104,10 +22104,10 @@
       </c>
       <c r="S376" s="3"/>
       <c r="T376" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="377" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="377" spans="1:20" ht="39">
       <c r="A377" s="2" t="s">
         <v>427</v>
       </c>
@@ -22164,10 +22164,10 @@
       </c>
       <c r="S377" s="3"/>
       <c r="T377" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="378" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="378" spans="1:20" ht="39">
       <c r="A378" s="2" t="s">
         <v>427</v>
       </c>
@@ -22224,10 +22224,10 @@
       </c>
       <c r="S378" s="3"/>
       <c r="T378" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="379" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="379" spans="1:20" ht="48.75">
       <c r="A379" s="2" t="s">
         <v>427</v>
       </c>
@@ -22289,7 +22289,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="380" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:20" ht="39">
       <c r="A380" s="2" t="s">
         <v>427</v>
       </c>
@@ -22335,7 +22335,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="381" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:20" ht="39">
       <c r="A381" s="2" t="s">
         <v>427</v>
       </c>
@@ -22381,7 +22381,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="382" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:20" ht="39">
       <c r="A382" s="2" t="s">
         <v>427</v>
       </c>
@@ -22427,7 +22427,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="383" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:20" ht="39">
       <c r="A383" s="2" t="s">
         <v>427</v>
       </c>
@@ -22481,7 +22481,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="384" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:20" ht="39">
       <c r="A384" s="2" t="s">
         <v>427</v>
       </c>
@@ -22527,7 +22527,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="385" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:20" ht="39">
       <c r="A385" s="2" t="s">
         <v>427</v>
       </c>
@@ -22589,7 +22589,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="386" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:20" ht="48.75">
       <c r="A386" s="2" t="s">
         <v>427</v>
       </c>
@@ -22651,7 +22651,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="387" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:20" ht="29.25">
       <c r="A387" s="2" t="s">
         <v>447</v>
       </c>
@@ -22711,7 +22711,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="388" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:20" ht="29.25">
       <c r="A388" s="2" t="s">
         <v>447</v>
       </c>
@@ -22771,7 +22771,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="389" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:20" ht="29.25">
       <c r="A389" s="2" t="s">
         <v>447</v>
       </c>
@@ -22823,7 +22823,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="390" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:20" ht="68.25">
       <c r="A390" s="2" t="s">
         <v>447</v>
       </c>
@@ -22875,7 +22875,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="391" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:20" ht="29.25">
       <c r="A391" s="2" t="s">
         <v>447</v>
       </c>
@@ -22927,7 +22927,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="392" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:20" ht="29.25">
       <c r="A392" s="2" t="s">
         <v>447</v>
       </c>
@@ -22979,7 +22979,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="393" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:20" ht="39">
       <c r="A393" s="2" t="s">
         <v>447</v>
       </c>
@@ -23041,7 +23041,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="394" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:20" ht="39">
       <c r="A394" s="2" t="s">
         <v>447</v>
       </c>
@@ -23099,7 +23099,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="395" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:20" ht="48.75">
       <c r="A395" s="2" t="s">
         <v>447</v>
       </c>
@@ -23161,7 +23161,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="396" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:20" ht="29.25">
       <c r="A396" s="2" t="s">
         <v>447</v>
       </c>
@@ -23215,7 +23215,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="397" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:20" ht="58.5">
       <c r="A397" s="2" t="s">
         <v>459</v>
       </c>
@@ -23275,7 +23275,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="398" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:20" ht="39">
       <c r="A398" s="2" t="s">
         <v>459</v>
       </c>
@@ -23335,7 +23335,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="399" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:20" ht="48.75">
       <c r="A399" s="2" t="s">
         <v>459</v>
       </c>
@@ -23395,7 +23395,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="400" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:20" ht="48.75">
       <c r="A400" s="2" t="s">
         <v>459</v>
       </c>
@@ -23455,7 +23455,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="401" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:20" ht="58.5">
       <c r="A401" s="2" t="s">
         <v>459</v>
       </c>
@@ -23515,7 +23515,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="402" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:20" ht="19.5">
       <c r="A402" s="2" t="s">
         <v>469</v>
       </c>
@@ -23575,7 +23575,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="403" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:20" ht="19.5">
       <c r="A403" s="2" t="s">
         <v>469</v>
       </c>
@@ -23635,7 +23635,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="404" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:20" ht="39">
       <c r="A404" s="2" t="s">
         <v>469</v>
       </c>
@@ -23695,7 +23695,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="405" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:20" ht="19.5">
       <c r="A405" s="2" t="s">
         <v>469</v>
       </c>
@@ -23737,7 +23737,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="406" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:20" ht="19.5">
       <c r="A406" s="2" t="s">
         <v>469</v>
       </c>
@@ -23771,7 +23771,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="407" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:20" ht="19.5">
       <c r="A407" s="2" t="s">
         <v>469</v>
       </c>
@@ -23805,7 +23805,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="408" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:20" ht="19.5">
       <c r="A408" s="2" t="s">
         <v>469</v>
       </c>
@@ -23839,7 +23839,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="409" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:20" ht="19.5">
       <c r="A409" s="2" t="s">
         <v>469</v>
       </c>
@@ -23881,7 +23881,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="410" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:20" ht="19.5">
       <c r="A410" s="2" t="s">
         <v>469</v>
       </c>
@@ -23923,7 +23923,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="411" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:20" ht="19.5">
       <c r="A411" s="2" t="s">
         <v>469</v>
       </c>
@@ -23965,7 +23965,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="412" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:20" ht="29.25">
       <c r="A412" s="2" t="s">
         <v>469</v>
       </c>
@@ -24027,7 +24027,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="413" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:20" ht="19.5">
       <c r="A413" s="2" t="s">
         <v>469</v>
       </c>
@@ -24087,7 +24087,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="414" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:20" ht="29.25">
       <c r="A414" s="2" t="s">
         <v>469</v>
       </c>
@@ -24149,7 +24149,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="415" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:20" ht="29.25">
       <c r="A415" s="2" t="s">
         <v>469</v>
       </c>
@@ -24203,7 +24203,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="416" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:20" ht="29.25">
       <c r="A416" s="2" t="s">
         <v>469</v>
       </c>
@@ -24257,7 +24257,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="417" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:20" ht="19.5">
       <c r="A417" s="2" t="s">
         <v>469</v>
       </c>
@@ -24317,7 +24317,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="418" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:20" ht="29.25">
       <c r="A418" s="2" t="s">
         <v>490</v>
       </c>
@@ -24377,7 +24377,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="419" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:20" ht="29.25">
       <c r="A419" s="2" t="s">
         <v>490</v>
       </c>
@@ -24439,7 +24439,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="420" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:20" ht="29.25">
       <c r="A420" s="2" t="s">
         <v>490</v>
       </c>
@@ -24483,7 +24483,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="421" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:20" ht="29.25">
       <c r="A421" s="2" t="s">
         <v>490</v>
       </c>
@@ -24539,7 +24539,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="422" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:20" ht="29.25">
       <c r="A422" s="2" t="s">
         <v>490</v>
       </c>
@@ -24587,7 +24587,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="423" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:20" ht="29.25">
       <c r="A423" s="2" t="s">
         <v>490</v>
       </c>
@@ -24635,7 +24635,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="424" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:20" ht="29.25">
       <c r="A424" s="2" t="s">
         <v>490</v>
       </c>
@@ -24683,7 +24683,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="425" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:20" ht="29.25">
       <c r="A425" s="2" t="s">
         <v>490</v>
       </c>
@@ -24731,7 +24731,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="426" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:20" ht="29.25">
       <c r="A426" s="2" t="s">
         <v>490</v>
       </c>
@@ -24779,7 +24779,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="427" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:20" ht="29.25">
       <c r="A427" s="2" t="s">
         <v>490</v>
       </c>
@@ -24827,7 +24827,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="428" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:20" ht="39">
       <c r="A428" s="2" t="s">
         <v>490</v>
       </c>
@@ -24875,7 +24875,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="429" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:20" ht="48.75">
       <c r="A429" s="2" t="s">
         <v>490</v>
       </c>
@@ -24923,7 +24923,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="430" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:20" ht="39">
       <c r="A430" s="2" t="s">
         <v>490</v>
       </c>
@@ -24971,7 +24971,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="431" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:20" ht="39">
       <c r="A431" s="2" t="s">
         <v>490</v>
       </c>
@@ -25019,7 +25019,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="432" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:20" ht="29.25">
       <c r="A432" s="2" t="s">
         <v>490</v>
       </c>
@@ -25079,7 +25079,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="433" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:20" ht="29.25">
       <c r="A433" s="2" t="s">
         <v>490</v>
       </c>
@@ -25139,7 +25139,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="434" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:20" ht="29.25">
       <c r="A434" s="2" t="s">
         <v>490</v>
       </c>
@@ -25199,7 +25199,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="435" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:20" ht="29.25">
       <c r="A435" s="2" t="s">
         <v>490</v>
       </c>
@@ -25259,7 +25259,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="436" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:20" ht="29.25">
       <c r="A436" s="2" t="s">
         <v>490</v>
       </c>
@@ -25319,7 +25319,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="437" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:20" ht="29.25">
       <c r="A437" s="2" t="s">
         <v>490</v>
       </c>
@@ -25379,7 +25379,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="438" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:20" ht="39">
       <c r="A438" s="2" t="s">
         <v>490</v>
       </c>
@@ -25421,7 +25421,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="439" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:20" ht="39">
       <c r="A439" s="2" t="s">
         <v>490</v>
       </c>
@@ -25463,7 +25463,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="440" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:20" ht="39">
       <c r="A440" s="2" t="s">
         <v>490</v>
       </c>
@@ -25505,7 +25505,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="441" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:20" ht="39">
       <c r="A441" s="2" t="s">
         <v>490</v>
       </c>
@@ -25547,7 +25547,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="442" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:20" ht="39">
       <c r="A442" s="2" t="s">
         <v>490</v>
       </c>
@@ -25589,7 +25589,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="443" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:20" ht="39">
       <c r="A443" s="2" t="s">
         <v>490</v>
       </c>
@@ -25631,7 +25631,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="444" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:20" ht="39">
       <c r="A444" s="2" t="s">
         <v>490</v>
       </c>
@@ -25673,7 +25673,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="445" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:20" ht="39">
       <c r="A445" s="2" t="s">
         <v>490</v>
       </c>
@@ -25715,7 +25715,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="446" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:20" ht="39">
       <c r="A446" s="2" t="s">
         <v>490</v>
       </c>
@@ -25757,7 +25757,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="447" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:20" ht="39">
       <c r="A447" s="2" t="s">
         <v>490</v>
       </c>
@@ -25799,7 +25799,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="448" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:20" ht="39">
       <c r="A448" s="2" t="s">
         <v>490</v>
       </c>
@@ -25841,7 +25841,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="449" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:20" ht="39">
       <c r="A449" s="2" t="s">
         <v>490</v>
       </c>
@@ -25883,7 +25883,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="450" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:20" ht="29.25">
       <c r="A450" s="2" t="s">
         <v>490</v>
       </c>
@@ -25945,7 +25945,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="451" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:20" ht="29.25">
       <c r="A451" s="2" t="s">
         <v>490</v>
       </c>
@@ -25985,7 +25985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="452" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:20" ht="29.25">
       <c r="A452" s="2" t="s">
         <v>527</v>
       </c>
@@ -26045,7 +26045,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="453" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:20" ht="29.25">
       <c r="A453" s="2" t="s">
         <v>527</v>
       </c>
@@ -26105,7 +26105,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="454" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:20" ht="29.25">
       <c r="A454" s="2" t="s">
         <v>527</v>
       </c>
@@ -26165,7 +26165,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="455" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:20" ht="29.25">
       <c r="A455" s="2" t="s">
         <v>527</v>
       </c>
@@ -26225,7 +26225,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="456" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:20" ht="48.75">
       <c r="A456" s="2" t="s">
         <v>527</v>
       </c>
@@ -26285,7 +26285,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="457" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:20" ht="29.25">
       <c r="A457" s="2" t="s">
         <v>527</v>
       </c>
@@ -26345,7 +26345,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="458" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:20" ht="29.25">
       <c r="A458" s="2" t="s">
         <v>527</v>
       </c>
@@ -26405,7 +26405,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="459" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:20" ht="29.25">
       <c r="A459" s="2" t="s">
         <v>527</v>
       </c>
@@ -26467,7 +26467,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="460" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:20" ht="29.25">
       <c r="A460" s="2" t="s">
         <v>527</v>
       </c>
@@ -26529,7 +26529,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="461" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:20" ht="29.25">
       <c r="A461" s="2" t="s">
         <v>527</v>
       </c>
@@ -26591,7 +26591,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="462" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:20" ht="29.25">
       <c r="A462" s="2" t="s">
         <v>527</v>
       </c>
@@ -26651,7 +26651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="463" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:20" ht="29.25">
       <c r="A463" s="2" t="s">
         <v>527</v>
       </c>
@@ -26713,7 +26713,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="464" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:20" ht="29.25">
       <c r="A464" s="2" t="s">
         <v>527</v>
       </c>
@@ -26775,7 +26775,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="465" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:20" ht="29.25">
       <c r="A465" s="2" t="s">
         <v>527</v>
       </c>
@@ -26835,7 +26835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="466" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:20" ht="29.25">
       <c r="A466" s="2" t="s">
         <v>527</v>
       </c>
@@ -26897,7 +26897,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="467" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:20" ht="48.75">
       <c r="A467" s="2" t="s">
         <v>527</v>
       </c>
@@ -26959,7 +26959,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="468" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:20" ht="29.25">
       <c r="A468" s="2" t="s">
         <v>527</v>
       </c>
@@ -27021,7 +27021,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="469" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:20" ht="39">
       <c r="A469" s="2" t="s">
         <v>527</v>
       </c>
@@ -27083,7 +27083,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="470" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:20" ht="39">
       <c r="A470" s="2" t="s">
         <v>527</v>
       </c>
@@ -27145,7 +27145,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="471" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:20" ht="29.25">
       <c r="A471" s="2" t="s">
         <v>527</v>
       </c>
@@ -27191,7 +27191,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="472" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:20" ht="29.25">
       <c r="A472" s="2" t="s">
         <v>527</v>
       </c>
@@ -27253,7 +27253,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="473" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:20" ht="29.25">
       <c r="A473" s="2" t="s">
         <v>527</v>
       </c>
@@ -27315,7 +27315,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="474" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:20" ht="29.25">
       <c r="A474" s="2" t="s">
         <v>527</v>
       </c>
@@ -27369,7 +27369,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="475" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:20" ht="39">
       <c r="A475" s="2" t="s">
         <v>527</v>
       </c>
@@ -27407,7 +27407,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="476" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:20" ht="39">
       <c r="A476" s="2" t="s">
         <v>527</v>
       </c>
@@ -27469,7 +27469,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="477" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:20" ht="39">
       <c r="A477" s="2" t="s">
         <v>527</v>
       </c>
@@ -27531,8 +27531,8 @@
         <v>562</v>
       </c>
     </row>
-    <row r="478" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:20" ht="18" customHeight="1"/>
+    <row r="479" spans="1:20" ht="17.100000000000001" customHeight="1">
       <c r="A479" s="12" t="s">
         <v>565</v>
       </c>
@@ -27549,7 +27549,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="72" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="74" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
okienko serwisowe - 25.06.2024
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dregerj\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1720,7 +1720,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 07-05-2024, 09:52</t>
+    <t>Last update: 25-06-2024, 12:17</t>
   </si>
 </sst>
 </file>
@@ -1735,7 +1735,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2272,10 +2272,10 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2287,17 +2287,17 @@
     <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="36" customHeight="1">
+    <row r="1" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:20" ht="25.5">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="19.5">
+    <row r="4" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="19.5">
+    <row r="14" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="19.5">
+    <row r="15" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="29.25">
+    <row r="17" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="97.5">
+    <row r="18" spans="1:20" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="97.5">
+    <row r="19" spans="1:20" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="97.5">
+    <row r="20" spans="1:20" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="19.5">
+    <row r="21" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="29.25">
+    <row r="22" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="29.25">
+    <row r="23" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="29.25">
+    <row r="24" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="68.25">
+    <row r="25" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="29.25">
+    <row r="26" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="29.25">
+    <row r="27" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>21</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="29.25">
+    <row r="28" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="39">
+    <row r="29" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="39">
+    <row r="30" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="39">
+    <row r="31" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="39">
+    <row r="32" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="19.5">
+    <row r="33" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>67</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="29.25">
+    <row r="34" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>67</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="29.25">
+    <row r="35" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>67</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="29.25">
+    <row r="36" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="29.25">
+    <row r="37" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="29.25">
+    <row r="38" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>67</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="29.25">
+    <row r="39" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>67</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="39">
+    <row r="40" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>67</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="97.5">
+    <row r="41" spans="1:20" ht="81" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>67</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="97.5">
+    <row r="42" spans="1:20" ht="81" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>67</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="97.5">
+    <row r="43" spans="1:20" ht="81" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>67</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="97.5">
+    <row r="44" spans="1:20" ht="81" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>67</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="97.5">
+    <row r="45" spans="1:20" ht="81" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>67</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="97.5">
+    <row r="46" spans="1:20" ht="81" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>67</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="48.75">
+    <row r="47" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>67</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="48.75">
+    <row r="48" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>67</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="19.5">
+    <row r="49" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>67</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="29.25">
+    <row r="50" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>67</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="19.5">
+    <row r="51" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>96</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="19.5">
+    <row r="52" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>96</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="19.5">
+    <row r="53" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>96</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="19.5">
+    <row r="54" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>96</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="19.5">
+    <row r="55" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>96</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="19.5">
+    <row r="56" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>96</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="19.5">
+    <row r="57" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>96</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="19.5">
+    <row r="58" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>96</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="29.25">
+    <row r="59" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>96</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="19.5">
+    <row r="60" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>96</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="29.25">
+    <row r="61" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>96</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="29.25">
+    <row r="62" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>96</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="29.25">
+    <row r="63" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>96</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="19.5">
+    <row r="64" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>96</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="29.25">
+    <row r="65" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>96</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="29.25">
+    <row r="66" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>96</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="29.25">
+    <row r="67" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>96</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="29.25">
+    <row r="68" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>96</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="29.25">
+    <row r="69" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>96</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="29.25">
+    <row r="70" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>96</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="29.25">
+    <row r="71" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>96</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="19.5">
+    <row r="72" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>96</v>
       </c>
@@ -6341,7 +6341,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="19.5">
+    <row r="73" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>96</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="19.5">
+    <row r="74" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>96</v>
       </c>
@@ -6461,7 +6461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="19.5">
+    <row r="75" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>96</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="29.25">
+    <row r="76" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>96</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="29.25">
+    <row r="77" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>96</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="19.5">
+    <row r="78" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>96</v>
       </c>
@@ -6681,7 +6681,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="19.5">
+    <row r="79" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>96</v>
       </c>
@@ -6741,7 +6741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="19.5">
+    <row r="80" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>96</v>
       </c>
@@ -6801,7 +6801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="19.5">
+    <row r="81" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>96</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="29.25">
+    <row r="82" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>96</v>
       </c>
@@ -6903,7 +6903,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="29.25">
+    <row r="83" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>96</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="19.5">
+    <row r="84" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>96</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="29.25">
+    <row r="85" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>96</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="19.5">
+    <row r="86" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>96</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="19.5">
+    <row r="87" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>96</v>
       </c>
@@ -7133,7 +7133,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="19.5">
+    <row r="88" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>96</v>
       </c>
@@ -7193,7 +7193,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="19.5">
+    <row r="89" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>96</v>
       </c>
@@ -7253,7 +7253,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="19.5">
+    <row r="90" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>96</v>
       </c>
@@ -7297,7 +7297,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="29.25">
+    <row r="91" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>96</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="19.5">
+    <row r="92" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>96</v>
       </c>
@@ -7393,7 +7393,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="19.5">
+    <row r="93" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>96</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="19.5">
+    <row r="94" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>96</v>
       </c>
@@ -7477,7 +7477,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="19.5">
+    <row r="95" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>96</v>
       </c>
@@ -7533,7 +7533,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="78">
+    <row r="96" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>150</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="78">
+    <row r="97" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>150</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="78">
+    <row r="98" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>150</v>
       </c>
@@ -7653,7 +7653,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="78">
+    <row r="99" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>150</v>
       </c>
@@ -7697,7 +7697,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="78">
+    <row r="100" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>150</v>
       </c>
@@ -7741,7 +7741,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="78">
+    <row r="101" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>150</v>
       </c>
@@ -7785,7 +7785,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="78">
+    <row r="102" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>150</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="78">
+    <row r="103" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>150</v>
       </c>
@@ -7873,7 +7873,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="78">
+    <row r="104" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>150</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="29.25">
+    <row r="105" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>150</v>
       </c>
@@ -7955,7 +7955,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="19.5">
+    <row r="106" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>150</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="19.5">
+    <row r="107" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>150</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="19.5">
+    <row r="108" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>150</v>
       </c>
@@ -8135,7 +8135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="19.5">
+    <row r="109" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>150</v>
       </c>
@@ -8173,7 +8173,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="19.5">
+    <row r="110" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>150</v>
       </c>
@@ -8211,7 +8211,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="19.5">
+    <row r="111" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>150</v>
       </c>
@@ -8249,7 +8249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="29.25">
+    <row r="112" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>150</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="19.5">
+    <row r="113" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>150</v>
       </c>
@@ -8345,7 +8345,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="39">
+    <row r="114" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>150</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="48.75">
+    <row r="115" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>150</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="58.5">
+    <row r="116" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>150</v>
       </c>
@@ -8495,7 +8495,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="29.25">
+    <row r="117" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>150</v>
       </c>
@@ -8545,7 +8545,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="29.25">
+    <row r="118" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>150</v>
       </c>
@@ -8591,7 +8591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="19.5">
+    <row r="119" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>150</v>
       </c>
@@ -8641,7 +8641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="39">
+    <row r="120" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>150</v>
       </c>
@@ -8691,7 +8691,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="48.75">
+    <row r="121" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>150</v>
       </c>
@@ -8741,7 +8741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="58.5">
+    <row r="122" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>150</v>
       </c>
@@ -8791,7 +8791,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="29.25">
+    <row r="123" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>150</v>
       </c>
@@ -8841,7 +8841,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="48.75">
+    <row r="124" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>150</v>
       </c>
@@ -8883,7 +8883,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="48.75">
+    <row r="125" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>150</v>
       </c>
@@ -8925,7 +8925,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="29.25">
+    <row r="126" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>150</v>
       </c>
@@ -8985,7 +8985,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="29.25">
+    <row r="127" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>150</v>
       </c>
@@ -9021,7 +9021,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="29.25">
+    <row r="128" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>150</v>
       </c>
@@ -9057,7 +9057,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="29.25">
+    <row r="129" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>150</v>
       </c>
@@ -9093,7 +9093,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="29.25">
+    <row r="130" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>150</v>
       </c>
@@ -9129,7 +9129,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="29.25">
+    <row r="131" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>150</v>
       </c>
@@ -9165,7 +9165,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="29.25">
+    <row r="132" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>150</v>
       </c>
@@ -9201,7 +9201,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="29.25">
+    <row r="133" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>150</v>
       </c>
@@ -9237,7 +9237,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="29.25">
+    <row r="134" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>150</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="29.25">
+    <row r="135" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>150</v>
       </c>
@@ -9309,7 +9309,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="29.25">
+    <row r="136" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>150</v>
       </c>
@@ -9345,7 +9345,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="29.25">
+    <row r="137" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>150</v>
       </c>
@@ -9381,7 +9381,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="29.25">
+    <row r="138" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>150</v>
       </c>
@@ -9417,7 +9417,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="29.25">
+    <row r="139" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>150</v>
       </c>
@@ -9453,7 +9453,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="29.25">
+    <row r="140" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>150</v>
       </c>
@@ -9489,7 +9489,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="29.25">
+    <row r="141" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>150</v>
       </c>
@@ -9525,7 +9525,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="29.25">
+    <row r="142" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>150</v>
       </c>
@@ -9561,7 +9561,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="48.75">
+    <row r="143" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>150</v>
       </c>
@@ -9623,7 +9623,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="58.5">
+    <row r="144" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>150</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="58.5">
+    <row r="145" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>150</v>
       </c>
@@ -9721,7 +9721,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="58.5">
+    <row r="146" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>150</v>
       </c>
@@ -9757,7 +9757,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="58.5">
+    <row r="147" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>150</v>
       </c>
@@ -9819,7 +9819,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="58.5">
+    <row r="148" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>150</v>
       </c>
@@ -9881,7 +9881,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="58.5">
+    <row r="149" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>150</v>
       </c>
@@ -9943,7 +9943,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="29.25">
+    <row r="150" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>150</v>
       </c>
@@ -9997,7 +9997,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="58.5">
+    <row r="151" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>150</v>
       </c>
@@ -10053,7 +10053,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="58.5">
+    <row r="152" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>150</v>
       </c>
@@ -10109,7 +10109,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="58.5">
+    <row r="153" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>150</v>
       </c>
@@ -10165,7 +10165,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="58.5">
+    <row r="154" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>150</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="29.25">
+    <row r="155" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>206</v>
       </c>
@@ -10257,7 +10257,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="19.5">
+    <row r="156" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>206</v>
       </c>
@@ -10317,7 +10317,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="39">
+    <row r="157" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>206</v>
       </c>
@@ -10353,7 +10353,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="39">
+    <row r="158" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>206</v>
       </c>
@@ -10389,7 +10389,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="39">
+    <row r="159" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>206</v>
       </c>
@@ -10425,7 +10425,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="39">
+    <row r="160" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>206</v>
       </c>
@@ -10461,7 +10461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="39">
+    <row r="161" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>206</v>
       </c>
@@ -10497,7 +10497,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="19.5">
+    <row r="162" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>206</v>
       </c>
@@ -10533,7 +10533,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="19.5">
+    <row r="163" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>206</v>
       </c>
@@ -10569,7 +10569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="19.5">
+    <row r="164" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>206</v>
       </c>
@@ -10605,7 +10605,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="19.5">
+    <row r="165" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>206</v>
       </c>
@@ -10641,7 +10641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="19.5">
+    <row r="166" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>206</v>
       </c>
@@ -10677,7 +10677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="19.5">
+    <row r="167" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>206</v>
       </c>
@@ -10713,7 +10713,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="19.5">
+    <row r="168" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>206</v>
       </c>
@@ -10749,7 +10749,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="19.5">
+    <row r="169" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>206</v>
       </c>
@@ -10785,7 +10785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="29.25">
+    <row r="170" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>206</v>
       </c>
@@ -10827,7 +10827,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="29.25">
+    <row r="171" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>206</v>
       </c>
@@ -10869,7 +10869,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="29.25">
+    <row r="172" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>206</v>
       </c>
@@ -10929,7 +10929,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="29.25">
+    <row r="173" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>206</v>
       </c>
@@ -10989,7 +10989,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="29.25">
+    <row r="174" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>206</v>
       </c>
@@ -11049,7 +11049,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="29.25">
+    <row r="175" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>206</v>
       </c>
@@ -11109,7 +11109,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="29.25">
+    <row r="176" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>206</v>
       </c>
@@ -11169,7 +11169,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="19.5">
+    <row r="177" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>206</v>
       </c>
@@ -11217,7 +11217,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="39">
+    <row r="178" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>206</v>
       </c>
@@ -11265,7 +11265,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="19.5">
+    <row r="179" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>206</v>
       </c>
@@ -11313,7 +11313,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="39">
+    <row r="180" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>206</v>
       </c>
@@ -11361,7 +11361,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="39">
+    <row r="181" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>206</v>
       </c>
@@ -11409,7 +11409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="39">
+    <row r="182" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>206</v>
       </c>
@@ -11457,7 +11457,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="39">
+    <row r="183" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>206</v>
       </c>
@@ -11505,7 +11505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="39">
+    <row r="184" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>206</v>
       </c>
@@ -11545,7 +11545,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="39">
+    <row r="185" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>206</v>
       </c>
@@ -11585,7 +11585,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="39">
+    <row r="186" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>206</v>
       </c>
@@ -11625,7 +11625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="39">
+    <row r="187" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>206</v>
       </c>
@@ -11665,7 +11665,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="39">
+    <row r="188" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>206</v>
       </c>
@@ -11705,7 +11705,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="39">
+    <row r="189" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>206</v>
       </c>
@@ -11745,7 +11745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="39">
+    <row r="190" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>206</v>
       </c>
@@ -11785,7 +11785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="39">
+    <row r="191" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>206</v>
       </c>
@@ -11825,7 +11825,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="39">
+    <row r="192" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>206</v>
       </c>
@@ -11865,7 +11865,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="39">
+    <row r="193" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>206</v>
       </c>
@@ -11905,7 +11905,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="39">
+    <row r="194" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>206</v>
       </c>
@@ -11945,7 +11945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="39">
+    <row r="195" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>206</v>
       </c>
@@ -11985,7 +11985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="19.5">
+    <row r="196" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>206</v>
       </c>
@@ -12027,7 +12027,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="19.5">
+    <row r="197" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>206</v>
       </c>
@@ -12085,7 +12085,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="19.5">
+    <row r="198" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>206</v>
       </c>
@@ -12143,7 +12143,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="19.5">
+    <row r="199" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>246</v>
       </c>
@@ -12201,7 +12201,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="29.25">
+    <row r="200" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>246</v>
       </c>
@@ -12259,7 +12259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="19.5">
+    <row r="201" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>246</v>
       </c>
@@ -12319,7 +12319,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="19.5">
+    <row r="202" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>246</v>
       </c>
@@ -12357,7 +12357,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="19.5">
+    <row r="203" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>246</v>
       </c>
@@ -12395,7 +12395,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="29.25">
+    <row r="204" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>246</v>
       </c>
@@ -12453,7 +12453,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="19.5">
+    <row r="205" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>246</v>
       </c>
@@ -12509,7 +12509,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="19.5">
+    <row r="206" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>246</v>
       </c>
@@ -12555,7 +12555,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="29.25">
+    <row r="207" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>246</v>
       </c>
@@ -12615,7 +12615,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="29.25">
+    <row r="208" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>246</v>
       </c>
@@ -12669,7 +12669,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="39">
+    <row r="209" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>246</v>
       </c>
@@ -12729,7 +12729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="19.5">
+    <row r="210" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>267</v>
       </c>
@@ -12765,7 +12765,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="19.5">
+    <row r="211" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>267</v>
       </c>
@@ -12825,7 +12825,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="29.25">
+    <row r="212" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>267</v>
       </c>
@@ -12881,7 +12881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="29.25">
+    <row r="213" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>267</v>
       </c>
@@ -12935,7 +12935,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="29.25">
+    <row r="214" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>274</v>
       </c>
@@ -12995,7 +12995,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="29.25">
+    <row r="215" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>274</v>
       </c>
@@ -13055,7 +13055,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="29.25">
+    <row r="216" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>274</v>
       </c>
@@ -13097,7 +13097,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="29.25">
+    <row r="217" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>274</v>
       </c>
@@ -13139,7 +13139,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="29.25">
+    <row r="218" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>274</v>
       </c>
@@ -13181,7 +13181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="29.25">
+    <row r="219" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>274</v>
       </c>
@@ -13241,7 +13241,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="29.25">
+    <row r="220" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>274</v>
       </c>
@@ -13301,7 +13301,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="29.25">
+    <row r="221" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>274</v>
       </c>
@@ -13361,7 +13361,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="29.25">
+    <row r="222" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>274</v>
       </c>
@@ -13409,7 +13409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="29.25">
+    <row r="223" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>274</v>
       </c>
@@ -13457,7 +13457,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="29.25">
+    <row r="224" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>274</v>
       </c>
@@ -13505,7 +13505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="29.25">
+    <row r="225" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>274</v>
       </c>
@@ -13553,7 +13553,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="29.25">
+    <row r="226" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>274</v>
       </c>
@@ -13601,7 +13601,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="29.25">
+    <row r="227" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>274</v>
       </c>
@@ -13649,7 +13649,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="29.25">
+    <row r="228" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>274</v>
       </c>
@@ -13697,7 +13697,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="29.25">
+    <row r="229" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>274</v>
       </c>
@@ -13745,7 +13745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="39">
+    <row r="230" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>274</v>
       </c>
@@ -13793,7 +13793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="29.25">
+    <row r="231" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>274</v>
       </c>
@@ -13841,7 +13841,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="39">
+    <row r="232" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>274</v>
       </c>
@@ -13889,7 +13889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="29.25">
+    <row r="233" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>274</v>
       </c>
@@ -13937,7 +13937,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="29.25">
+    <row r="234" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>274</v>
       </c>
@@ -13985,7 +13985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="29.25">
+    <row r="235" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>274</v>
       </c>
@@ -14033,7 +14033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="29.25">
+    <row r="236" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>274</v>
       </c>
@@ -14081,7 +14081,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="29.25">
+    <row r="237" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>274</v>
       </c>
@@ -14129,7 +14129,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="29.25">
+    <row r="238" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>274</v>
       </c>
@@ -14177,7 +14177,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="29.25">
+    <row r="239" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>274</v>
       </c>
@@ -14225,7 +14225,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="29.25">
+    <row r="240" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>274</v>
       </c>
@@ -14273,7 +14273,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="29.25">
+    <row r="241" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>274</v>
       </c>
@@ -14335,7 +14335,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="29.25">
+    <row r="242" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>274</v>
       </c>
@@ -14397,7 +14397,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="243" spans="1:20" ht="29.25">
+    <row r="243" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>274</v>
       </c>
@@ -14459,7 +14459,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="29.25">
+    <row r="244" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>274</v>
       </c>
@@ -14521,7 +14521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="29.25">
+    <row r="245" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>274</v>
       </c>
@@ -14583,7 +14583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="29.25">
+    <row r="246" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>274</v>
       </c>
@@ -14645,7 +14645,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="29.25">
+    <row r="247" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>274</v>
       </c>
@@ -14707,7 +14707,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="29.25">
+    <row r="248" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>274</v>
       </c>
@@ -14769,7 +14769,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="29.25">
+    <row r="249" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>274</v>
       </c>
@@ -14831,7 +14831,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="29.25">
+    <row r="250" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>274</v>
       </c>
@@ -14891,7 +14891,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="29.25">
+    <row r="251" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>274</v>
       </c>
@@ -14951,7 +14951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="29.25">
+    <row r="252" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>274</v>
       </c>
@@ -15011,7 +15011,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="39">
+    <row r="253" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>274</v>
       </c>
@@ -15053,7 +15053,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="39">
+    <row r="254" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>274</v>
       </c>
@@ -15095,7 +15095,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="39">
+    <row r="255" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>274</v>
       </c>
@@ -15137,7 +15137,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="29.25">
+    <row r="256" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>274</v>
       </c>
@@ -15197,7 +15197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="48.75">
+    <row r="257" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>274</v>
       </c>
@@ -15255,7 +15255,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="29.25">
+    <row r="258" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>274</v>
       </c>
@@ -15291,7 +15291,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="29.25">
+    <row r="259" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>274</v>
       </c>
@@ -15327,7 +15327,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="29.25">
+    <row r="260" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>274</v>
       </c>
@@ -15363,7 +15363,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="29.25">
+    <row r="261" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>274</v>
       </c>
@@ -15399,7 +15399,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="29.25">
+    <row r="262" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>274</v>
       </c>
@@ -15435,7 +15435,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="29.25">
+    <row r="263" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>274</v>
       </c>
@@ -15471,7 +15471,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="29.25">
+    <row r="264" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>274</v>
       </c>
@@ -15507,7 +15507,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="29.25">
+    <row r="265" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>274</v>
       </c>
@@ -15543,7 +15543,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="29.25">
+    <row r="266" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>274</v>
       </c>
@@ -15595,7 +15595,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="29.25">
+    <row r="267" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>319</v>
       </c>
@@ -15655,7 +15655,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="29.25">
+    <row r="268" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>319</v>
       </c>
@@ -15715,7 +15715,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="29.25">
+    <row r="269" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>319</v>
       </c>
@@ -15775,7 +15775,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="29.25">
+    <row r="270" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>319</v>
       </c>
@@ -15835,7 +15835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="29.25">
+    <row r="271" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>319</v>
       </c>
@@ -15895,7 +15895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="272" spans="1:20" ht="29.25">
+    <row r="272" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>319</v>
       </c>
@@ -15955,7 +15955,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="29.25">
+    <row r="273" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>319</v>
       </c>
@@ -16015,7 +16015,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="29.25">
+    <row r="274" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>319</v>
       </c>
@@ -16075,7 +16075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="275" spans="1:20" ht="29.25">
+    <row r="275" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>319</v>
       </c>
@@ -16135,7 +16135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="276" spans="1:20" ht="29.25">
+    <row r="276" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>319</v>
       </c>
@@ -16195,7 +16195,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="29.25">
+    <row r="277" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>319</v>
       </c>
@@ -16255,7 +16255,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="29.25">
+    <row r="278" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>319</v>
       </c>
@@ -16315,7 +16315,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="29.25">
+    <row r="279" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>319</v>
       </c>
@@ -16375,7 +16375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="29.25">
+    <row r="280" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>319</v>
       </c>
@@ -16435,7 +16435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="281" spans="1:20" ht="29.25">
+    <row r="281" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>319</v>
       </c>
@@ -16495,7 +16495,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="282" spans="1:20" ht="29.25">
+    <row r="282" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>319</v>
       </c>
@@ -16555,7 +16555,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="29.25">
+    <row r="283" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>319</v>
       </c>
@@ -16615,7 +16615,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="29.25">
+    <row r="284" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>319</v>
       </c>
@@ -16675,7 +16675,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="29.25">
+    <row r="285" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>319</v>
       </c>
@@ -16735,7 +16735,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="29.25">
+    <row r="286" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>319</v>
       </c>
@@ -16795,7 +16795,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="29.25">
+    <row r="287" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>319</v>
       </c>
@@ -16847,7 +16847,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="29.25">
+    <row r="288" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>319</v>
       </c>
@@ -16907,7 +16907,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="29.25">
+    <row r="289" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>319</v>
       </c>
@@ -16967,7 +16967,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="29.25">
+    <row r="290" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>319</v>
       </c>
@@ -17021,7 +17021,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="291" spans="1:20" ht="29.25">
+    <row r="291" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>319</v>
       </c>
@@ -17075,7 +17075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="39">
+    <row r="292" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>319</v>
       </c>
@@ -17127,7 +17127,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="39">
+    <row r="293" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>319</v>
       </c>
@@ -17179,7 +17179,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="19.5">
+    <row r="294" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>351</v>
       </c>
@@ -17239,7 +17239,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="68.25">
+    <row r="295" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>351</v>
       </c>
@@ -17299,7 +17299,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="19.5">
+    <row r="296" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>351</v>
       </c>
@@ -17359,7 +17359,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="19.5">
+    <row r="297" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>351</v>
       </c>
@@ -17419,7 +17419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="19.5">
+    <row r="298" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>351</v>
       </c>
@@ -17479,7 +17479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="19.5">
+    <row r="299" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>351</v>
       </c>
@@ -17539,7 +17539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="19.5">
+    <row r="300" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>351</v>
       </c>
@@ -17599,7 +17599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="19.5">
+    <row r="301" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>351</v>
       </c>
@@ -17659,7 +17659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="19.5">
+    <row r="302" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
         <v>351</v>
       </c>
@@ -17719,7 +17719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="19.5">
+    <row r="303" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
         <v>351</v>
       </c>
@@ -17779,7 +17779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="304" spans="1:20" ht="19.5">
+    <row r="304" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>351</v>
       </c>
@@ -17839,7 +17839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="305" spans="1:20" ht="19.5">
+    <row r="305" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>351</v>
       </c>
@@ -17879,7 +17879,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="306" spans="1:20" ht="19.5">
+    <row r="306" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
         <v>351</v>
       </c>
@@ -17939,7 +17939,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="307" spans="1:20" ht="39">
+    <row r="307" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
         <v>351</v>
       </c>
@@ -17999,7 +17999,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="308" spans="1:20" ht="48.75">
+    <row r="308" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
         <v>351</v>
       </c>
@@ -18059,7 +18059,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="309" spans="1:20" ht="39">
+    <row r="309" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
         <v>351</v>
       </c>
@@ -18119,7 +18119,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="310" spans="1:20" ht="39">
+    <row r="310" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
         <v>351</v>
       </c>
@@ -18179,7 +18179,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="311" spans="1:20" ht="29.25">
+    <row r="311" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
         <v>351</v>
       </c>
@@ -18239,7 +18239,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="312" spans="1:20" ht="39">
+    <row r="312" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
         <v>351</v>
       </c>
@@ -18299,7 +18299,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="313" spans="1:20" ht="29.25">
+    <row r="313" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
         <v>351</v>
       </c>
@@ -18359,7 +18359,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="314" spans="1:20" ht="29.25">
+    <row r="314" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
         <v>351</v>
       </c>
@@ -18419,7 +18419,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="315" spans="1:20" ht="39">
+    <row r="315" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
         <v>351</v>
       </c>
@@ -18479,7 +18479,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="316" spans="1:20" ht="29.25">
+    <row r="316" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
         <v>351</v>
       </c>
@@ -18539,7 +18539,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="317" spans="1:20" ht="39">
+    <row r="317" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
         <v>351</v>
       </c>
@@ -18599,7 +18599,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="318" spans="1:20" ht="29.25">
+    <row r="318" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
         <v>351</v>
       </c>
@@ -18659,7 +18659,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="319" spans="1:20" ht="29.25">
+    <row r="319" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
         <v>351</v>
       </c>
@@ -18721,7 +18721,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="320" spans="1:20" ht="39">
+    <row r="320" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
         <v>351</v>
       </c>
@@ -18783,7 +18783,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="321" spans="1:20" ht="39">
+    <row r="321" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
         <v>351</v>
       </c>
@@ -18845,7 +18845,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="322" spans="1:20" ht="68.25">
+    <row r="322" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
         <v>351</v>
       </c>
@@ -18907,7 +18907,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="323" spans="1:20" ht="58.5">
+    <row r="323" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
         <v>351</v>
       </c>
@@ -18969,7 +18969,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="324" spans="1:20" ht="68.25">
+    <row r="324" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
         <v>351</v>
       </c>
@@ -19031,7 +19031,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="325" spans="1:20" ht="68.25">
+    <row r="325" spans="1:20" ht="72" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>351</v>
       </c>
@@ -19093,7 +19093,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="326" spans="1:20" ht="39">
+    <row r="326" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
         <v>351</v>
       </c>
@@ -19153,7 +19153,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="327" spans="1:20" ht="68.25">
+    <row r="327" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
         <v>351</v>
       </c>
@@ -19213,7 +19213,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="328" spans="1:20" ht="58.5">
+    <row r="328" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
         <v>351</v>
       </c>
@@ -19273,7 +19273,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="329" spans="1:20" ht="68.25">
+    <row r="329" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
         <v>351</v>
       </c>
@@ -19333,7 +19333,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="330" spans="1:20" ht="68.25">
+    <row r="330" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
         <v>351</v>
       </c>
@@ -19393,7 +19393,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="331" spans="1:20" ht="29.25">
+    <row r="331" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
         <v>392</v>
       </c>
@@ -19449,7 +19449,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="332" spans="1:20" ht="29.25">
+    <row r="332" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
         <v>392</v>
       </c>
@@ -19505,7 +19505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="333" spans="1:20" ht="29.25">
+    <row r="333" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
         <v>392</v>
       </c>
@@ -19561,7 +19561,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="29.25">
+    <row r="334" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
         <v>392</v>
       </c>
@@ -19621,7 +19621,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="335" spans="1:20" ht="29.25">
+    <row r="335" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
         <v>392</v>
       </c>
@@ -19681,7 +19681,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="336" spans="1:20" ht="29.25">
+    <row r="336" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
         <v>392</v>
       </c>
@@ -19741,7 +19741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="337" spans="1:20" ht="29.25">
+    <row r="337" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
         <v>392</v>
       </c>
@@ -19801,7 +19801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="338" spans="1:20" ht="29.25">
+    <row r="338" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
         <v>392</v>
       </c>
@@ -19861,7 +19861,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="339" spans="1:20" ht="29.25">
+    <row r="339" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
         <v>392</v>
       </c>
@@ -19921,7 +19921,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="340" spans="1:20" ht="29.25">
+    <row r="340" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
         <v>392</v>
       </c>
@@ -19981,7 +19981,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="341" spans="1:20" ht="29.25">
+    <row r="341" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
         <v>392</v>
       </c>
@@ -20041,7 +20041,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="342" spans="1:20" ht="29.25">
+    <row r="342" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
         <v>392</v>
       </c>
@@ -20101,7 +20101,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="343" spans="1:20" ht="29.25">
+    <row r="343" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
         <v>392</v>
       </c>
@@ -20161,7 +20161,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="344" spans="1:20" ht="29.25">
+    <row r="344" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
         <v>392</v>
       </c>
@@ -20221,7 +20221,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="345" spans="1:20" ht="29.25">
+    <row r="345" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
         <v>392</v>
       </c>
@@ -20281,7 +20281,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="346" spans="1:20" ht="29.25">
+    <row r="346" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
         <v>392</v>
       </c>
@@ -20341,7 +20341,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="347" spans="1:20" ht="29.25">
+    <row r="347" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
         <v>392</v>
       </c>
@@ -20401,7 +20401,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="348" spans="1:20" ht="29.25">
+    <row r="348" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
         <v>392</v>
       </c>
@@ -20461,7 +20461,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="349" spans="1:20" ht="29.25">
+    <row r="349" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
         <v>392</v>
       </c>
@@ -20521,7 +20521,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="350" spans="1:20" ht="29.25">
+    <row r="350" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
         <v>392</v>
       </c>
@@ -20581,7 +20581,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="351" spans="1:20" ht="29.25">
+    <row r="351" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
         <v>392</v>
       </c>
@@ -20641,7 +20641,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="352" spans="1:20" ht="29.25">
+    <row r="352" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
         <v>392</v>
       </c>
@@ -20701,7 +20701,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="353" spans="1:20" ht="29.25">
+    <row r="353" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
         <v>392</v>
       </c>
@@ -20761,7 +20761,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="354" spans="1:20" ht="29.25">
+    <row r="354" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
         <v>392</v>
       </c>
@@ -20821,7 +20821,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="355" spans="1:20" ht="29.25">
+    <row r="355" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
         <v>392</v>
       </c>
@@ -20881,7 +20881,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="356" spans="1:20" ht="29.25">
+    <row r="356" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
         <v>392</v>
       </c>
@@ -20941,7 +20941,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="357" spans="1:20" ht="29.25">
+    <row r="357" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
         <v>392</v>
       </c>
@@ -21001,7 +21001,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="358" spans="1:20" ht="29.25">
+    <row r="358" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
         <v>392</v>
       </c>
@@ -21059,7 +21059,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="359" spans="1:20" ht="29.25">
+    <row r="359" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
         <v>392</v>
       </c>
@@ -21119,7 +21119,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="360" spans="1:20" ht="29.25">
+    <row r="360" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
         <v>392</v>
       </c>
@@ -21179,7 +21179,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="361" spans="1:20" ht="29.25">
+    <row r="361" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
         <v>392</v>
       </c>
@@ -21239,7 +21239,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="362" spans="1:20" ht="29.25">
+    <row r="362" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
         <v>392</v>
       </c>
@@ -21299,7 +21299,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="363" spans="1:20" ht="29.25">
+    <row r="363" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
         <v>392</v>
       </c>
@@ -21359,7 +21359,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="364" spans="1:20" ht="39">
+    <row r="364" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
         <v>392</v>
       </c>
@@ -21419,7 +21419,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="365" spans="1:20" ht="39">
+    <row r="365" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
         <v>392</v>
       </c>
@@ -21479,7 +21479,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="366" spans="1:20" ht="39">
+    <row r="366" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
         <v>392</v>
       </c>
@@ -21539,7 +21539,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="367" spans="1:20" ht="39">
+    <row r="367" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
         <v>392</v>
       </c>
@@ -21599,7 +21599,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="368" spans="1:20" ht="39">
+    <row r="368" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
         <v>392</v>
       </c>
@@ -21659,7 +21659,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="369" spans="1:20" ht="39">
+    <row r="369" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
         <v>392</v>
       </c>
@@ -21719,7 +21719,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="370" spans="1:20" ht="39">
+    <row r="370" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
         <v>392</v>
       </c>
@@ -21779,7 +21779,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="371" spans="1:20" ht="39">
+    <row r="371" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
         <v>392</v>
       </c>
@@ -21839,7 +21839,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="372" spans="1:20" ht="29.25">
+    <row r="372" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
         <v>392</v>
       </c>
@@ -21891,7 +21891,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="373" spans="1:20" ht="68.25">
+    <row r="373" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
         <v>392</v>
       </c>
@@ -21943,7 +21943,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="374" spans="1:20" ht="29.25">
+    <row r="374" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
         <v>392</v>
       </c>
@@ -21995,7 +21995,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="375" spans="1:20" ht="29.25">
+    <row r="375" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
         <v>392</v>
       </c>
@@ -22047,7 +22047,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="376" spans="1:20" ht="39">
+    <row r="376" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
         <v>427</v>
       </c>
@@ -22107,7 +22107,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="377" spans="1:20" ht="39">
+    <row r="377" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
         <v>427</v>
       </c>
@@ -22167,7 +22167,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="378" spans="1:20" ht="39">
+    <row r="378" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
         <v>427</v>
       </c>
@@ -22227,7 +22227,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="379" spans="1:20" ht="48.75">
+    <row r="379" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
         <v>427</v>
       </c>
@@ -22289,7 +22289,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="380" spans="1:20" ht="39">
+    <row r="380" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
         <v>427</v>
       </c>
@@ -22335,7 +22335,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="381" spans="1:20" ht="39">
+    <row r="381" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
         <v>427</v>
       </c>
@@ -22381,7 +22381,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="382" spans="1:20" ht="39">
+    <row r="382" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
         <v>427</v>
       </c>
@@ -22427,7 +22427,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="383" spans="1:20" ht="39">
+    <row r="383" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
         <v>427</v>
       </c>
@@ -22481,7 +22481,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="384" spans="1:20" ht="39">
+    <row r="384" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
         <v>427</v>
       </c>
@@ -22527,7 +22527,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="385" spans="1:20" ht="39">
+    <row r="385" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
         <v>427</v>
       </c>
@@ -22589,7 +22589,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="386" spans="1:20" ht="48.75">
+    <row r="386" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
         <v>427</v>
       </c>
@@ -22651,7 +22651,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="387" spans="1:20" ht="29.25">
+    <row r="387" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
         <v>447</v>
       </c>
@@ -22711,7 +22711,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="388" spans="1:20" ht="29.25">
+    <row r="388" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
         <v>447</v>
       </c>
@@ -22771,7 +22771,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="389" spans="1:20" ht="29.25">
+    <row r="389" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
         <v>447</v>
       </c>
@@ -22823,7 +22823,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="390" spans="1:20" ht="68.25">
+    <row r="390" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
         <v>447</v>
       </c>
@@ -22875,7 +22875,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="391" spans="1:20" ht="29.25">
+    <row r="391" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
         <v>447</v>
       </c>
@@ -22927,7 +22927,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="392" spans="1:20" ht="29.25">
+    <row r="392" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
         <v>447</v>
       </c>
@@ -22979,7 +22979,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="393" spans="1:20" ht="39">
+    <row r="393" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
         <v>447</v>
       </c>
@@ -23041,7 +23041,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="394" spans="1:20" ht="39">
+    <row r="394" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
         <v>447</v>
       </c>
@@ -23099,7 +23099,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="395" spans="1:20" ht="48.75">
+    <row r="395" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
         <v>447</v>
       </c>
@@ -23161,7 +23161,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="396" spans="1:20" ht="29.25">
+    <row r="396" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
         <v>447</v>
       </c>
@@ -23215,7 +23215,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="397" spans="1:20" ht="58.5">
+    <row r="397" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
         <v>459</v>
       </c>
@@ -23275,7 +23275,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="398" spans="1:20" ht="39">
+    <row r="398" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
         <v>459</v>
       </c>
@@ -23335,7 +23335,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="399" spans="1:20" ht="48.75">
+    <row r="399" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
         <v>459</v>
       </c>
@@ -23395,7 +23395,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="400" spans="1:20" ht="48.75">
+    <row r="400" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
         <v>459</v>
       </c>
@@ -23455,7 +23455,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="401" spans="1:20" ht="58.5">
+    <row r="401" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
         <v>459</v>
       </c>
@@ -23515,7 +23515,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="402" spans="1:20" ht="19.5">
+    <row r="402" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A402" s="2" t="s">
         <v>469</v>
       </c>
@@ -23575,7 +23575,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="403" spans="1:20" ht="19.5">
+    <row r="403" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
         <v>469</v>
       </c>
@@ -23635,7 +23635,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="404" spans="1:20" ht="39">
+    <row r="404" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
         <v>469</v>
       </c>
@@ -23695,7 +23695,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="405" spans="1:20" ht="19.5">
+    <row r="405" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
         <v>469</v>
       </c>
@@ -23737,7 +23737,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="406" spans="1:20" ht="19.5">
+    <row r="406" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
         <v>469</v>
       </c>
@@ -23771,7 +23771,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="407" spans="1:20" ht="19.5">
+    <row r="407" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
         <v>469</v>
       </c>
@@ -23805,7 +23805,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="408" spans="1:20" ht="19.5">
+    <row r="408" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
         <v>469</v>
       </c>
@@ -23839,7 +23839,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="409" spans="1:20" ht="19.5">
+    <row r="409" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
         <v>469</v>
       </c>
@@ -23881,7 +23881,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="410" spans="1:20" ht="19.5">
+    <row r="410" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
         <v>469</v>
       </c>
@@ -23923,7 +23923,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="411" spans="1:20" ht="19.5">
+    <row r="411" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A411" s="2" t="s">
         <v>469</v>
       </c>
@@ -23965,7 +23965,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="412" spans="1:20" ht="29.25">
+    <row r="412" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A412" s="2" t="s">
         <v>469</v>
       </c>
@@ -24027,7 +24027,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="413" spans="1:20" ht="19.5">
+    <row r="413" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
         <v>469</v>
       </c>
@@ -24087,7 +24087,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="414" spans="1:20" ht="29.25">
+    <row r="414" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
         <v>469</v>
       </c>
@@ -24149,7 +24149,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="415" spans="1:20" ht="29.25">
+    <row r="415" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
         <v>469</v>
       </c>
@@ -24203,7 +24203,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="416" spans="1:20" ht="29.25">
+    <row r="416" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
         <v>469</v>
       </c>
@@ -24257,7 +24257,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="417" spans="1:20" ht="19.5">
+    <row r="417" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A417" s="2" t="s">
         <v>469</v>
       </c>
@@ -24317,7 +24317,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="418" spans="1:20" ht="29.25">
+    <row r="418" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
         <v>490</v>
       </c>
@@ -24377,7 +24377,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="419" spans="1:20" ht="29.25">
+    <row r="419" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
         <v>490</v>
       </c>
@@ -24439,7 +24439,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="420" spans="1:20" ht="29.25">
+    <row r="420" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
         <v>490</v>
       </c>
@@ -24483,7 +24483,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="421" spans="1:20" ht="29.25">
+    <row r="421" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
         <v>490</v>
       </c>
@@ -24539,7 +24539,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="422" spans="1:20" ht="29.25">
+    <row r="422" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
         <v>490</v>
       </c>
@@ -24587,7 +24587,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="423" spans="1:20" ht="29.25">
+    <row r="423" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
         <v>490</v>
       </c>
@@ -24635,7 +24635,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="424" spans="1:20" ht="29.25">
+    <row r="424" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
         <v>490</v>
       </c>
@@ -24683,7 +24683,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="425" spans="1:20" ht="29.25">
+    <row r="425" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
         <v>490</v>
       </c>
@@ -24731,7 +24731,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="426" spans="1:20" ht="29.25">
+    <row r="426" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A426" s="2" t="s">
         <v>490</v>
       </c>
@@ -24779,7 +24779,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="427" spans="1:20" ht="29.25">
+    <row r="427" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
         <v>490</v>
       </c>
@@ -24827,7 +24827,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="428" spans="1:20" ht="39">
+    <row r="428" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
         <v>490</v>
       </c>
@@ -24875,7 +24875,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="429" spans="1:20" ht="48.75">
+    <row r="429" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A429" s="2" t="s">
         <v>490</v>
       </c>
@@ -24923,7 +24923,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="430" spans="1:20" ht="39">
+    <row r="430" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A430" s="2" t="s">
         <v>490</v>
       </c>
@@ -24971,7 +24971,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="431" spans="1:20" ht="39">
+    <row r="431" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
         <v>490</v>
       </c>
@@ -25019,7 +25019,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="432" spans="1:20" ht="29.25">
+    <row r="432" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A432" s="2" t="s">
         <v>490</v>
       </c>
@@ -25079,7 +25079,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="433" spans="1:20" ht="29.25">
+    <row r="433" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A433" s="2" t="s">
         <v>490</v>
       </c>
@@ -25139,7 +25139,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="434" spans="1:20" ht="29.25">
+    <row r="434" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A434" s="2" t="s">
         <v>490</v>
       </c>
@@ -25199,7 +25199,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="435" spans="1:20" ht="29.25">
+    <row r="435" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A435" s="2" t="s">
         <v>490</v>
       </c>
@@ -25259,7 +25259,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="436" spans="1:20" ht="29.25">
+    <row r="436" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A436" s="2" t="s">
         <v>490</v>
       </c>
@@ -25319,7 +25319,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="437" spans="1:20" ht="29.25">
+    <row r="437" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A437" s="2" t="s">
         <v>490</v>
       </c>
@@ -25379,7 +25379,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="438" spans="1:20" ht="39">
+    <row r="438" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A438" s="2" t="s">
         <v>490</v>
       </c>
@@ -25421,7 +25421,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="439" spans="1:20" ht="39">
+    <row r="439" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A439" s="2" t="s">
         <v>490</v>
       </c>
@@ -25463,7 +25463,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="440" spans="1:20" ht="39">
+    <row r="440" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
         <v>490</v>
       </c>
@@ -25505,7 +25505,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="441" spans="1:20" ht="39">
+    <row r="441" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
         <v>490</v>
       </c>
@@ -25547,7 +25547,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="442" spans="1:20" ht="39">
+    <row r="442" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
         <v>490</v>
       </c>
@@ -25589,7 +25589,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="443" spans="1:20" ht="39">
+    <row r="443" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A443" s="2" t="s">
         <v>490</v>
       </c>
@@ -25631,7 +25631,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="444" spans="1:20" ht="39">
+    <row r="444" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A444" s="2" t="s">
         <v>490</v>
       </c>
@@ -25673,7 +25673,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="445" spans="1:20" ht="39">
+    <row r="445" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A445" s="2" t="s">
         <v>490</v>
       </c>
@@ -25715,7 +25715,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="446" spans="1:20" ht="39">
+    <row r="446" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A446" s="2" t="s">
         <v>490</v>
       </c>
@@ -25757,7 +25757,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="447" spans="1:20" ht="39">
+    <row r="447" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
         <v>490</v>
       </c>
@@ -25799,7 +25799,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="448" spans="1:20" ht="39">
+    <row r="448" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
         <v>490</v>
       </c>
@@ -25841,7 +25841,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="449" spans="1:20" ht="39">
+    <row r="449" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A449" s="2" t="s">
         <v>490</v>
       </c>
@@ -25883,7 +25883,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="450" spans="1:20" ht="29.25">
+    <row r="450" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A450" s="2" t="s">
         <v>490</v>
       </c>
@@ -25945,7 +25945,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="451" spans="1:20" ht="29.25">
+    <row r="451" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A451" s="2" t="s">
         <v>490</v>
       </c>
@@ -25985,7 +25985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="452" spans="1:20" ht="29.25">
+    <row r="452" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A452" s="2" t="s">
         <v>527</v>
       </c>
@@ -26045,7 +26045,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="453" spans="1:20" ht="29.25">
+    <row r="453" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A453" s="2" t="s">
         <v>527</v>
       </c>
@@ -26105,7 +26105,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="454" spans="1:20" ht="29.25">
+    <row r="454" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A454" s="2" t="s">
         <v>527</v>
       </c>
@@ -26165,7 +26165,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="455" spans="1:20" ht="29.25">
+    <row r="455" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A455" s="2" t="s">
         <v>527</v>
       </c>
@@ -26225,7 +26225,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="456" spans="1:20" ht="48.75">
+    <row r="456" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A456" s="2" t="s">
         <v>527</v>
       </c>
@@ -26285,7 +26285,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="457" spans="1:20" ht="29.25">
+    <row r="457" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
         <v>527</v>
       </c>
@@ -26345,7 +26345,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="458" spans="1:20" ht="29.25">
+    <row r="458" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A458" s="2" t="s">
         <v>527</v>
       </c>
@@ -26405,7 +26405,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="459" spans="1:20" ht="29.25">
+    <row r="459" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
         <v>527</v>
       </c>
@@ -26467,7 +26467,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="460" spans="1:20" ht="29.25">
+    <row r="460" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
         <v>527</v>
       </c>
@@ -26529,7 +26529,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="461" spans="1:20" ht="29.25">
+    <row r="461" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
         <v>527</v>
       </c>
@@ -26591,7 +26591,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="462" spans="1:20" ht="29.25">
+    <row r="462" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
         <v>527</v>
       </c>
@@ -26651,7 +26651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="463" spans="1:20" ht="29.25">
+    <row r="463" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
         <v>527</v>
       </c>
@@ -26713,7 +26713,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="464" spans="1:20" ht="29.25">
+    <row r="464" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
         <v>527</v>
       </c>
@@ -26775,7 +26775,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="465" spans="1:20" ht="29.25">
+    <row r="465" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
         <v>527</v>
       </c>
@@ -26835,7 +26835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="466" spans="1:20" ht="29.25">
+    <row r="466" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
         <v>527</v>
       </c>
@@ -26897,7 +26897,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="467" spans="1:20" ht="48.75">
+    <row r="467" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
         <v>527</v>
       </c>
@@ -26959,7 +26959,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="468" spans="1:20" ht="29.25">
+    <row r="468" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
         <v>527</v>
       </c>
@@ -27021,7 +27021,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="469" spans="1:20" ht="39">
+    <row r="469" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A469" s="2" t="s">
         <v>527</v>
       </c>
@@ -27083,7 +27083,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="470" spans="1:20" ht="39">
+    <row r="470" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
         <v>527</v>
       </c>
@@ -27145,7 +27145,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="471" spans="1:20" ht="29.25">
+    <row r="471" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A471" s="2" t="s">
         <v>527</v>
       </c>
@@ -27191,7 +27191,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="472" spans="1:20" ht="29.25">
+    <row r="472" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A472" s="2" t="s">
         <v>527</v>
       </c>
@@ -27253,7 +27253,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="473" spans="1:20" ht="29.25">
+    <row r="473" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
         <v>527</v>
       </c>
@@ -27315,7 +27315,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="474" spans="1:20" ht="29.25">
+    <row r="474" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A474" s="2" t="s">
         <v>527</v>
       </c>
@@ -27369,7 +27369,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="475" spans="1:20" ht="39">
+    <row r="475" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
         <v>527</v>
       </c>
@@ -27407,7 +27407,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="476" spans="1:20" ht="39">
+    <row r="476" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A476" s="2" t="s">
         <v>527</v>
       </c>
@@ -27469,7 +27469,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="477" spans="1:20" ht="39">
+    <row r="477" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A477" s="2" t="s">
         <v>527</v>
       </c>
@@ -27531,8 +27531,8 @@
         <v>562</v>
       </c>
     </row>
-    <row r="478" spans="1:20" ht="18" customHeight="1"/>
-    <row r="479" spans="1:20" ht="17.100000000000001" customHeight="1">
+    <row r="478" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A479" s="12" t="s">
         <v>565</v>
       </c>
@@ -27549,7 +27549,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="74" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="72" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okno 16.07.2024. - aktualizacja EXCEL
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dregerj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1720,7 +1720,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 25-06-2024, 12:17</t>
+    <t>Last update: 17-07-2024, 07:47</t>
   </si>
 </sst>
 </file>
@@ -1735,7 +1735,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2272,10 +2272,10 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2287,17 +2287,17 @@
     <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="36" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.5">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.5">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.5">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="29.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="97.5">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="97.5">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="97.5">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="19.5">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="29.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="29.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="29.25">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="68.25">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="29.25">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="29.25">
       <c r="A27" s="2" t="s">
         <v>21</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="29.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="39">
       <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="39">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="39">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="39">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="19.5">
       <c r="A33" s="2" t="s">
         <v>67</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="29.25">
       <c r="A34" s="2" t="s">
         <v>67</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="29.25">
       <c r="A35" s="2" t="s">
         <v>67</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="29.25">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="29.25">
       <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="29.25">
       <c r="A38" s="2" t="s">
         <v>67</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="29.25">
       <c r="A39" s="2" t="s">
         <v>67</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="39">
       <c r="A40" s="2" t="s">
         <v>67</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="97.5">
       <c r="A41" s="2" t="s">
         <v>67</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="97.5">
       <c r="A42" s="2" t="s">
         <v>67</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="97.5">
       <c r="A43" s="2" t="s">
         <v>67</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="97.5">
       <c r="A44" s="2" t="s">
         <v>67</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="97.5">
       <c r="A45" s="2" t="s">
         <v>67</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="97.5">
       <c r="A46" s="2" t="s">
         <v>67</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="48.75">
       <c r="A47" s="2" t="s">
         <v>67</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="48.75">
       <c r="A48" s="2" t="s">
         <v>67</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="19.5">
       <c r="A49" s="2" t="s">
         <v>67</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="29.25">
       <c r="A50" s="2" t="s">
         <v>67</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="19.5">
       <c r="A51" s="2" t="s">
         <v>96</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="19.5">
       <c r="A52" s="2" t="s">
         <v>96</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>96</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>96</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>96</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>96</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>96</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>96</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="29.25">
       <c r="A59" s="2" t="s">
         <v>96</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>96</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="29.25">
       <c r="A61" s="2" t="s">
         <v>96</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="29.25">
       <c r="A62" s="2" t="s">
         <v>96</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="29.25">
       <c r="A63" s="2" t="s">
         <v>96</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="19.5">
       <c r="A64" s="2" t="s">
         <v>96</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="29.25">
       <c r="A65" s="2" t="s">
         <v>96</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="29.25">
       <c r="A66" s="2" t="s">
         <v>96</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="29.25">
       <c r="A67" s="2" t="s">
         <v>96</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="29.25">
       <c r="A68" s="2" t="s">
         <v>96</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="29.25">
       <c r="A69" s="2" t="s">
         <v>96</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="29.25">
       <c r="A70" s="2" t="s">
         <v>96</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="29.25">
       <c r="A71" s="2" t="s">
         <v>96</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="19.5">
       <c r="A72" s="2" t="s">
         <v>96</v>
       </c>
@@ -6341,7 +6341,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="19.5">
       <c r="A73" s="2" t="s">
         <v>96</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="19.5">
       <c r="A74" s="2" t="s">
         <v>96</v>
       </c>
@@ -6461,7 +6461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="19.5">
       <c r="A75" s="2" t="s">
         <v>96</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="29.25">
       <c r="A76" s="2" t="s">
         <v>96</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="29.25">
       <c r="A77" s="2" t="s">
         <v>96</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" ht="19.5">
       <c r="A78" s="2" t="s">
         <v>96</v>
       </c>
@@ -6681,7 +6681,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" ht="19.5">
       <c r="A79" s="2" t="s">
         <v>96</v>
       </c>
@@ -6741,7 +6741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="19.5">
       <c r="A80" s="2" t="s">
         <v>96</v>
       </c>
@@ -6801,7 +6801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" ht="19.5">
       <c r="A81" s="2" t="s">
         <v>96</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" ht="29.25">
       <c r="A82" s="2" t="s">
         <v>96</v>
       </c>
@@ -6903,7 +6903,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" ht="29.25">
       <c r="A83" s="2" t="s">
         <v>96</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" ht="19.5">
       <c r="A84" s="2" t="s">
         <v>96</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" ht="29.25">
       <c r="A85" s="2" t="s">
         <v>96</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" ht="19.5">
       <c r="A86" s="2" t="s">
         <v>96</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" ht="19.5">
       <c r="A87" s="2" t="s">
         <v>96</v>
       </c>
@@ -7133,7 +7133,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" ht="19.5">
       <c r="A88" s="2" t="s">
         <v>96</v>
       </c>
@@ -7193,7 +7193,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" ht="19.5">
       <c r="A89" s="2" t="s">
         <v>96</v>
       </c>
@@ -7253,7 +7253,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" ht="19.5">
       <c r="A90" s="2" t="s">
         <v>96</v>
       </c>
@@ -7297,7 +7297,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" ht="29.25">
       <c r="A91" s="2" t="s">
         <v>96</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" ht="19.5">
       <c r="A92" s="2" t="s">
         <v>96</v>
       </c>
@@ -7393,7 +7393,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" ht="19.5">
       <c r="A93" s="2" t="s">
         <v>96</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" ht="19.5">
       <c r="A94" s="2" t="s">
         <v>96</v>
       </c>
@@ -7477,7 +7477,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" ht="19.5">
       <c r="A95" s="2" t="s">
         <v>96</v>
       </c>
@@ -7533,7 +7533,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" ht="78">
       <c r="A96" s="2" t="s">
         <v>150</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" ht="78">
       <c r="A97" s="2" t="s">
         <v>150</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" ht="78">
       <c r="A98" s="2" t="s">
         <v>150</v>
       </c>
@@ -7653,7 +7653,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" ht="78">
       <c r="A99" s="2" t="s">
         <v>150</v>
       </c>
@@ -7697,7 +7697,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" ht="78">
       <c r="A100" s="2" t="s">
         <v>150</v>
       </c>
@@ -7741,7 +7741,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" ht="78">
       <c r="A101" s="2" t="s">
         <v>150</v>
       </c>
@@ -7785,7 +7785,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" ht="78">
       <c r="A102" s="2" t="s">
         <v>150</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" ht="78">
       <c r="A103" s="2" t="s">
         <v>150</v>
       </c>
@@ -7873,7 +7873,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" ht="78">
       <c r="A104" s="2" t="s">
         <v>150</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" ht="29.25">
       <c r="A105" s="2" t="s">
         <v>150</v>
       </c>
@@ -7955,7 +7955,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" ht="19.5">
       <c r="A106" s="2" t="s">
         <v>150</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" ht="19.5">
       <c r="A107" s="2" t="s">
         <v>150</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" ht="19.5">
       <c r="A108" s="2" t="s">
         <v>150</v>
       </c>
@@ -8135,7 +8135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" ht="19.5">
       <c r="A109" s="2" t="s">
         <v>150</v>
       </c>
@@ -8173,7 +8173,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" ht="19.5">
       <c r="A110" s="2" t="s">
         <v>150</v>
       </c>
@@ -8211,7 +8211,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" ht="19.5">
       <c r="A111" s="2" t="s">
         <v>150</v>
       </c>
@@ -8249,7 +8249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" ht="29.25">
       <c r="A112" s="2" t="s">
         <v>150</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" ht="19.5">
       <c r="A113" s="2" t="s">
         <v>150</v>
       </c>
@@ -8345,7 +8345,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" ht="39">
       <c r="A114" s="2" t="s">
         <v>150</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" ht="48.75">
       <c r="A115" s="2" t="s">
         <v>150</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" ht="58.5">
       <c r="A116" s="2" t="s">
         <v>150</v>
       </c>
@@ -8495,7 +8495,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" ht="29.25">
       <c r="A117" s="2" t="s">
         <v>150</v>
       </c>
@@ -8545,7 +8545,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" ht="29.25">
       <c r="A118" s="2" t="s">
         <v>150</v>
       </c>
@@ -8591,7 +8591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" ht="19.5">
       <c r="A119" s="2" t="s">
         <v>150</v>
       </c>
@@ -8641,7 +8641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" ht="39">
       <c r="A120" s="2" t="s">
         <v>150</v>
       </c>
@@ -8691,7 +8691,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" ht="48.75">
       <c r="A121" s="2" t="s">
         <v>150</v>
       </c>
@@ -8741,7 +8741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" ht="58.5">
       <c r="A122" s="2" t="s">
         <v>150</v>
       </c>
@@ -8791,7 +8791,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" ht="29.25">
       <c r="A123" s="2" t="s">
         <v>150</v>
       </c>
@@ -8841,7 +8841,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" ht="48.75">
       <c r="A124" s="2" t="s">
         <v>150</v>
       </c>
@@ -8883,7 +8883,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" ht="48.75">
       <c r="A125" s="2" t="s">
         <v>150</v>
       </c>
@@ -8925,7 +8925,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20" ht="29.25">
       <c r="A126" s="2" t="s">
         <v>150</v>
       </c>
@@ -8985,7 +8985,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20" ht="29.25">
       <c r="A127" s="2" t="s">
         <v>150</v>
       </c>
@@ -9021,7 +9021,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" ht="29.25">
       <c r="A128" s="2" t="s">
         <v>150</v>
       </c>
@@ -9057,7 +9057,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20" ht="29.25">
       <c r="A129" s="2" t="s">
         <v>150</v>
       </c>
@@ -9093,7 +9093,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20" ht="29.25">
       <c r="A130" s="2" t="s">
         <v>150</v>
       </c>
@@ -9129,7 +9129,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" ht="29.25">
       <c r="A131" s="2" t="s">
         <v>150</v>
       </c>
@@ -9165,7 +9165,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20" ht="29.25">
       <c r="A132" s="2" t="s">
         <v>150</v>
       </c>
@@ -9201,7 +9201,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" ht="29.25">
       <c r="A133" s="2" t="s">
         <v>150</v>
       </c>
@@ -9237,7 +9237,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20" ht="29.25">
       <c r="A134" s="2" t="s">
         <v>150</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:20" ht="29.25">
       <c r="A135" s="2" t="s">
         <v>150</v>
       </c>
@@ -9309,7 +9309,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20" ht="29.25">
       <c r="A136" s="2" t="s">
         <v>150</v>
       </c>
@@ -9345,7 +9345,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20" ht="29.25">
       <c r="A137" s="2" t="s">
         <v>150</v>
       </c>
@@ -9381,7 +9381,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:20" ht="29.25">
       <c r="A138" s="2" t="s">
         <v>150</v>
       </c>
@@ -9417,7 +9417,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" ht="29.25">
       <c r="A139" s="2" t="s">
         <v>150</v>
       </c>
@@ -9453,7 +9453,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20" ht="29.25">
       <c r="A140" s="2" t="s">
         <v>150</v>
       </c>
@@ -9489,7 +9489,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:20" ht="29.25">
       <c r="A141" s="2" t="s">
         <v>150</v>
       </c>
@@ -9525,7 +9525,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:20" ht="29.25">
       <c r="A142" s="2" t="s">
         <v>150</v>
       </c>
@@ -9561,7 +9561,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:20" ht="48.75">
       <c r="A143" s="2" t="s">
         <v>150</v>
       </c>
@@ -9623,7 +9623,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" ht="58.5">
       <c r="A144" s="2" t="s">
         <v>150</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" ht="58.5">
       <c r="A145" s="2" t="s">
         <v>150</v>
       </c>
@@ -9721,7 +9721,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" ht="58.5">
       <c r="A146" s="2" t="s">
         <v>150</v>
       </c>
@@ -9757,7 +9757,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" ht="58.5">
       <c r="A147" s="2" t="s">
         <v>150</v>
       </c>
@@ -9819,7 +9819,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:20" ht="58.5">
       <c r="A148" s="2" t="s">
         <v>150</v>
       </c>
@@ -9881,7 +9881,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:20" ht="58.5">
       <c r="A149" s="2" t="s">
         <v>150</v>
       </c>
@@ -9943,7 +9943,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:20" ht="29.25">
       <c r="A150" s="2" t="s">
         <v>150</v>
       </c>
@@ -9997,7 +9997,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:20" ht="58.5">
       <c r="A151" s="2" t="s">
         <v>150</v>
       </c>
@@ -10053,7 +10053,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:20" ht="58.5">
       <c r="A152" s="2" t="s">
         <v>150</v>
       </c>
@@ -10109,7 +10109,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:20" ht="58.5">
       <c r="A153" s="2" t="s">
         <v>150</v>
       </c>
@@ -10165,7 +10165,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:20" ht="58.5">
       <c r="A154" s="2" t="s">
         <v>150</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:20" ht="29.25">
       <c r="A155" s="2" t="s">
         <v>206</v>
       </c>
@@ -10257,7 +10257,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:20" ht="19.5">
       <c r="A156" s="2" t="s">
         <v>206</v>
       </c>
@@ -10317,7 +10317,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:20" ht="39">
       <c r="A157" s="2" t="s">
         <v>206</v>
       </c>
@@ -10353,7 +10353,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:20" ht="39">
       <c r="A158" s="2" t="s">
         <v>206</v>
       </c>
@@ -10389,7 +10389,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:20" ht="39">
       <c r="A159" s="2" t="s">
         <v>206</v>
       </c>
@@ -10425,7 +10425,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:20" ht="39">
       <c r="A160" s="2" t="s">
         <v>206</v>
       </c>
@@ -10461,7 +10461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:20" ht="39">
       <c r="A161" s="2" t="s">
         <v>206</v>
       </c>
@@ -10497,7 +10497,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:20" ht="19.5">
       <c r="A162" s="2" t="s">
         <v>206</v>
       </c>
@@ -10533,7 +10533,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:20" ht="19.5">
       <c r="A163" s="2" t="s">
         <v>206</v>
       </c>
@@ -10569,7 +10569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:20" ht="19.5">
       <c r="A164" s="2" t="s">
         <v>206</v>
       </c>
@@ -10605,7 +10605,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:20" ht="19.5">
       <c r="A165" s="2" t="s">
         <v>206</v>
       </c>
@@ -10641,7 +10641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:20" ht="19.5">
       <c r="A166" s="2" t="s">
         <v>206</v>
       </c>
@@ -10677,7 +10677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:20" ht="19.5">
       <c r="A167" s="2" t="s">
         <v>206</v>
       </c>
@@ -10713,7 +10713,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:20" ht="19.5">
       <c r="A168" s="2" t="s">
         <v>206</v>
       </c>
@@ -10749,7 +10749,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:20" ht="19.5">
       <c r="A169" s="2" t="s">
         <v>206</v>
       </c>
@@ -10785,7 +10785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:20" ht="29.25">
       <c r="A170" s="2" t="s">
         <v>206</v>
       </c>
@@ -10827,7 +10827,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:20" ht="29.25">
       <c r="A171" s="2" t="s">
         <v>206</v>
       </c>
@@ -10869,7 +10869,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:20" ht="29.25">
       <c r="A172" s="2" t="s">
         <v>206</v>
       </c>
@@ -10929,7 +10929,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:20" ht="29.25">
       <c r="A173" s="2" t="s">
         <v>206</v>
       </c>
@@ -10989,7 +10989,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:20" ht="29.25">
       <c r="A174" s="2" t="s">
         <v>206</v>
       </c>
@@ -11049,7 +11049,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:20" ht="29.25">
       <c r="A175" s="2" t="s">
         <v>206</v>
       </c>
@@ -11109,7 +11109,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" ht="29.25">
       <c r="A176" s="2" t="s">
         <v>206</v>
       </c>
@@ -11169,7 +11169,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:20" ht="19.5">
       <c r="A177" s="2" t="s">
         <v>206</v>
       </c>
@@ -11217,7 +11217,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:20" ht="39">
       <c r="A178" s="2" t="s">
         <v>206</v>
       </c>
@@ -11265,7 +11265,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:20" ht="19.5">
       <c r="A179" s="2" t="s">
         <v>206</v>
       </c>
@@ -11313,7 +11313,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:20" ht="39">
       <c r="A180" s="2" t="s">
         <v>206</v>
       </c>
@@ -11361,7 +11361,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:20" ht="39">
       <c r="A181" s="2" t="s">
         <v>206</v>
       </c>
@@ -11409,7 +11409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:20" ht="39">
       <c r="A182" s="2" t="s">
         <v>206</v>
       </c>
@@ -11457,7 +11457,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:20" ht="39">
       <c r="A183" s="2" t="s">
         <v>206</v>
       </c>
@@ -11505,7 +11505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:20" ht="39">
       <c r="A184" s="2" t="s">
         <v>206</v>
       </c>
@@ -11545,7 +11545,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:20" ht="39">
       <c r="A185" s="2" t="s">
         <v>206</v>
       </c>
@@ -11585,7 +11585,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:20" ht="39">
       <c r="A186" s="2" t="s">
         <v>206</v>
       </c>
@@ -11625,7 +11625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:20" ht="39">
       <c r="A187" s="2" t="s">
         <v>206</v>
       </c>
@@ -11665,7 +11665,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:20" ht="39">
       <c r="A188" s="2" t="s">
         <v>206</v>
       </c>
@@ -11705,7 +11705,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:20" ht="39">
       <c r="A189" s="2" t="s">
         <v>206</v>
       </c>
@@ -11745,7 +11745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:20" ht="39">
       <c r="A190" s="2" t="s">
         <v>206</v>
       </c>
@@ -11785,7 +11785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:20" ht="39">
       <c r="A191" s="2" t="s">
         <v>206</v>
       </c>
@@ -11825,7 +11825,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:20" ht="39">
       <c r="A192" s="2" t="s">
         <v>206</v>
       </c>
@@ -11865,7 +11865,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:20" ht="39">
       <c r="A193" s="2" t="s">
         <v>206</v>
       </c>
@@ -11905,7 +11905,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:20" ht="39">
       <c r="A194" s="2" t="s">
         <v>206</v>
       </c>
@@ -11945,7 +11945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:20" ht="39">
       <c r="A195" s="2" t="s">
         <v>206</v>
       </c>
@@ -11985,7 +11985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:20" ht="19.5">
       <c r="A196" s="2" t="s">
         <v>206</v>
       </c>
@@ -12027,7 +12027,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:20" ht="19.5">
       <c r="A197" s="2" t="s">
         <v>206</v>
       </c>
@@ -12085,7 +12085,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:20" ht="19.5">
       <c r="A198" s="2" t="s">
         <v>206</v>
       </c>
@@ -12143,7 +12143,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:20" ht="19.5">
       <c r="A199" s="2" t="s">
         <v>246</v>
       </c>
@@ -12201,7 +12201,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:20" ht="29.25">
       <c r="A200" s="2" t="s">
         <v>246</v>
       </c>
@@ -12259,7 +12259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:20" ht="19.5">
       <c r="A201" s="2" t="s">
         <v>246</v>
       </c>
@@ -12319,7 +12319,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:20" ht="19.5">
       <c r="A202" s="2" t="s">
         <v>246</v>
       </c>
@@ -12357,7 +12357,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:20" ht="19.5">
       <c r="A203" s="2" t="s">
         <v>246</v>
       </c>
@@ -12395,7 +12395,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:20" ht="29.25">
       <c r="A204" s="2" t="s">
         <v>246</v>
       </c>
@@ -12453,7 +12453,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:20" ht="19.5">
       <c r="A205" s="2" t="s">
         <v>246</v>
       </c>
@@ -12509,7 +12509,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:20" ht="19.5">
       <c r="A206" s="2" t="s">
         <v>246</v>
       </c>
@@ -12555,7 +12555,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:20" ht="29.25">
       <c r="A207" s="2" t="s">
         <v>246</v>
       </c>
@@ -12615,7 +12615,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:20" ht="29.25">
       <c r="A208" s="2" t="s">
         <v>246</v>
       </c>
@@ -12669,7 +12669,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:20" ht="39">
       <c r="A209" s="2" t="s">
         <v>246</v>
       </c>
@@ -12729,7 +12729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:20" ht="19.5">
       <c r="A210" s="2" t="s">
         <v>267</v>
       </c>
@@ -12765,7 +12765,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:20" ht="19.5">
       <c r="A211" s="2" t="s">
         <v>267</v>
       </c>
@@ -12825,7 +12825,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:20" ht="29.25">
       <c r="A212" s="2" t="s">
         <v>267</v>
       </c>
@@ -12881,7 +12881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:20" ht="29.25">
       <c r="A213" s="2" t="s">
         <v>267</v>
       </c>
@@ -12935,7 +12935,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:20" ht="29.25">
       <c r="A214" s="2" t="s">
         <v>274</v>
       </c>
@@ -12995,7 +12995,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:20" ht="29.25">
       <c r="A215" s="2" t="s">
         <v>274</v>
       </c>
@@ -13055,7 +13055,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:20" ht="29.25">
       <c r="A216" s="2" t="s">
         <v>274</v>
       </c>
@@ -13097,7 +13097,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:20" ht="29.25">
       <c r="A217" s="2" t="s">
         <v>274</v>
       </c>
@@ -13139,7 +13139,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:20" ht="29.25">
       <c r="A218" s="2" t="s">
         <v>274</v>
       </c>
@@ -13181,7 +13181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:20" ht="29.25">
       <c r="A219" s="2" t="s">
         <v>274</v>
       </c>
@@ -13241,7 +13241,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:20" ht="29.25">
       <c r="A220" s="2" t="s">
         <v>274</v>
       </c>
@@ -13301,7 +13301,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:20" ht="29.25">
       <c r="A221" s="2" t="s">
         <v>274</v>
       </c>
@@ -13361,7 +13361,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:20" ht="29.25">
       <c r="A222" s="2" t="s">
         <v>274</v>
       </c>
@@ -13409,7 +13409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:20" ht="29.25">
       <c r="A223" s="2" t="s">
         <v>274</v>
       </c>
@@ -13457,7 +13457,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:20" ht="29.25">
       <c r="A224" s="2" t="s">
         <v>274</v>
       </c>
@@ -13505,7 +13505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:20" ht="29.25">
       <c r="A225" s="2" t="s">
         <v>274</v>
       </c>
@@ -13553,7 +13553,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:20" ht="29.25">
       <c r="A226" s="2" t="s">
         <v>274</v>
       </c>
@@ -13601,7 +13601,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:20" ht="29.25">
       <c r="A227" s="2" t="s">
         <v>274</v>
       </c>
@@ -13649,7 +13649,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:20" ht="29.25">
       <c r="A228" s="2" t="s">
         <v>274</v>
       </c>
@@ -13697,7 +13697,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:20" ht="29.25">
       <c r="A229" s="2" t="s">
         <v>274</v>
       </c>
@@ -13745,7 +13745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:20" ht="39">
       <c r="A230" s="2" t="s">
         <v>274</v>
       </c>
@@ -13793,7 +13793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:20" ht="29.25">
       <c r="A231" s="2" t="s">
         <v>274</v>
       </c>
@@ -13841,7 +13841,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:20" ht="39">
       <c r="A232" s="2" t="s">
         <v>274</v>
       </c>
@@ -13889,7 +13889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:20" ht="29.25">
       <c r="A233" s="2" t="s">
         <v>274</v>
       </c>
@@ -13937,7 +13937,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:20" ht="29.25">
       <c r="A234" s="2" t="s">
         <v>274</v>
       </c>
@@ -13985,7 +13985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:20" ht="29.25">
       <c r="A235" s="2" t="s">
         <v>274</v>
       </c>
@@ -14033,7 +14033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:20" ht="29.25">
       <c r="A236" s="2" t="s">
         <v>274</v>
       </c>
@@ -14081,7 +14081,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:20" ht="29.25">
       <c r="A237" s="2" t="s">
         <v>274</v>
       </c>
@@ -14129,7 +14129,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:20" ht="29.25">
       <c r="A238" s="2" t="s">
         <v>274</v>
       </c>
@@ -14177,7 +14177,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:20" ht="29.25">
       <c r="A239" s="2" t="s">
         <v>274</v>
       </c>
@@ -14225,7 +14225,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:20" ht="29.25">
       <c r="A240" s="2" t="s">
         <v>274</v>
       </c>
@@ -14273,7 +14273,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:20" ht="29.25">
       <c r="A241" s="2" t="s">
         <v>274</v>
       </c>
@@ -14335,7 +14335,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:20" ht="29.25">
       <c r="A242" s="2" t="s">
         <v>274</v>
       </c>
@@ -14397,7 +14397,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="243" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:20" ht="29.25">
       <c r="A243" s="2" t="s">
         <v>274</v>
       </c>
@@ -14459,7 +14459,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:20" ht="29.25">
       <c r="A244" s="2" t="s">
         <v>274</v>
       </c>
@@ -14521,7 +14521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:20" ht="29.25">
       <c r="A245" s="2" t="s">
         <v>274</v>
       </c>
@@ -14583,7 +14583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:20" ht="29.25">
       <c r="A246" s="2" t="s">
         <v>274</v>
       </c>
@@ -14645,7 +14645,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:20" ht="29.25">
       <c r="A247" s="2" t="s">
         <v>274</v>
       </c>
@@ -14707,7 +14707,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:20" ht="29.25">
       <c r="A248" s="2" t="s">
         <v>274</v>
       </c>
@@ -14769,7 +14769,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:20" ht="29.25">
       <c r="A249" s="2" t="s">
         <v>274</v>
       </c>
@@ -14831,7 +14831,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:20" ht="29.25">
       <c r="A250" s="2" t="s">
         <v>274</v>
       </c>
@@ -14891,7 +14891,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:20" ht="29.25">
       <c r="A251" s="2" t="s">
         <v>274</v>
       </c>
@@ -14951,7 +14951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:20" ht="29.25">
       <c r="A252" s="2" t="s">
         <v>274</v>
       </c>
@@ -15011,7 +15011,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:20" ht="39">
       <c r="A253" s="2" t="s">
         <v>274</v>
       </c>
@@ -15053,7 +15053,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:20" ht="39">
       <c r="A254" s="2" t="s">
         <v>274</v>
       </c>
@@ -15095,7 +15095,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:20" ht="39">
       <c r="A255" s="2" t="s">
         <v>274</v>
       </c>
@@ -15137,7 +15137,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:20" ht="29.25">
       <c r="A256" s="2" t="s">
         <v>274</v>
       </c>
@@ -15197,7 +15197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:20" ht="48.75">
       <c r="A257" s="2" t="s">
         <v>274</v>
       </c>
@@ -15255,7 +15255,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:20" ht="29.25">
       <c r="A258" s="2" t="s">
         <v>274</v>
       </c>
@@ -15291,7 +15291,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:20" ht="29.25">
       <c r="A259" s="2" t="s">
         <v>274</v>
       </c>
@@ -15327,7 +15327,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:20" ht="29.25">
       <c r="A260" s="2" t="s">
         <v>274</v>
       </c>
@@ -15363,7 +15363,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:20" ht="29.25">
       <c r="A261" s="2" t="s">
         <v>274</v>
       </c>
@@ -15399,7 +15399,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:20" ht="29.25">
       <c r="A262" s="2" t="s">
         <v>274</v>
       </c>
@@ -15435,7 +15435,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:20" ht="29.25">
       <c r="A263" s="2" t="s">
         <v>274</v>
       </c>
@@ -15471,7 +15471,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:20" ht="29.25">
       <c r="A264" s="2" t="s">
         <v>274</v>
       </c>
@@ -15507,7 +15507,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:20" ht="29.25">
       <c r="A265" s="2" t="s">
         <v>274</v>
       </c>
@@ -15543,7 +15543,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:20" ht="29.25">
       <c r="A266" s="2" t="s">
         <v>274</v>
       </c>
@@ -15595,7 +15595,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:20" ht="29.25">
       <c r="A267" s="2" t="s">
         <v>319</v>
       </c>
@@ -15655,7 +15655,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:20" ht="29.25">
       <c r="A268" s="2" t="s">
         <v>319</v>
       </c>
@@ -15715,7 +15715,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:20" ht="29.25">
       <c r="A269" s="2" t="s">
         <v>319</v>
       </c>
@@ -15775,7 +15775,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:20" ht="29.25">
       <c r="A270" s="2" t="s">
         <v>319</v>
       </c>
@@ -15835,7 +15835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:20" ht="29.25">
       <c r="A271" s="2" t="s">
         <v>319</v>
       </c>
@@ -15895,7 +15895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="272" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:20" ht="29.25">
       <c r="A272" s="2" t="s">
         <v>319</v>
       </c>
@@ -15955,7 +15955,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:20" ht="29.25">
       <c r="A273" s="2" t="s">
         <v>319</v>
       </c>
@@ -16015,7 +16015,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:20" ht="29.25">
       <c r="A274" s="2" t="s">
         <v>319</v>
       </c>
@@ -16075,7 +16075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="275" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:20" ht="29.25">
       <c r="A275" s="2" t="s">
         <v>319</v>
       </c>
@@ -16135,7 +16135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="276" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:20" ht="29.25">
       <c r="A276" s="2" t="s">
         <v>319</v>
       </c>
@@ -16195,7 +16195,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:20" ht="29.25">
       <c r="A277" s="2" t="s">
         <v>319</v>
       </c>
@@ -16255,7 +16255,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:20" ht="29.25">
       <c r="A278" s="2" t="s">
         <v>319</v>
       </c>
@@ -16315,7 +16315,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:20" ht="29.25">
       <c r="A279" s="2" t="s">
         <v>319</v>
       </c>
@@ -16375,7 +16375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:20" ht="29.25">
       <c r="A280" s="2" t="s">
         <v>319</v>
       </c>
@@ -16435,7 +16435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="281" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:20" ht="29.25">
       <c r="A281" s="2" t="s">
         <v>319</v>
       </c>
@@ -16495,7 +16495,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="282" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:20" ht="29.25">
       <c r="A282" s="2" t="s">
         <v>319</v>
       </c>
@@ -16555,7 +16555,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:20" ht="29.25">
       <c r="A283" s="2" t="s">
         <v>319</v>
       </c>
@@ -16615,7 +16615,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:20" ht="29.25">
       <c r="A284" s="2" t="s">
         <v>319</v>
       </c>
@@ -16675,7 +16675,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:20" ht="29.25">
       <c r="A285" s="2" t="s">
         <v>319</v>
       </c>
@@ -16735,7 +16735,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:20" ht="29.25">
       <c r="A286" s="2" t="s">
         <v>319</v>
       </c>
@@ -16795,7 +16795,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:20" ht="29.25">
       <c r="A287" s="2" t="s">
         <v>319</v>
       </c>
@@ -16847,7 +16847,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:20" ht="29.25">
       <c r="A288" s="2" t="s">
         <v>319</v>
       </c>
@@ -16907,7 +16907,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:20" ht="29.25">
       <c r="A289" s="2" t="s">
         <v>319</v>
       </c>
@@ -16967,7 +16967,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:20" ht="29.25">
       <c r="A290" s="2" t="s">
         <v>319</v>
       </c>
@@ -17021,7 +17021,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="291" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:20" ht="29.25">
       <c r="A291" s="2" t="s">
         <v>319</v>
       </c>
@@ -17075,7 +17075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:20" ht="39">
       <c r="A292" s="2" t="s">
         <v>319</v>
       </c>
@@ -17127,7 +17127,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:20" ht="39">
       <c r="A293" s="2" t="s">
         <v>319</v>
       </c>
@@ -17179,7 +17179,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:20" ht="19.5">
       <c r="A294" s="2" t="s">
         <v>351</v>
       </c>
@@ -17239,7 +17239,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:20" ht="68.25">
       <c r="A295" s="2" t="s">
         <v>351</v>
       </c>
@@ -17299,7 +17299,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:20" ht="19.5">
       <c r="A296" s="2" t="s">
         <v>351</v>
       </c>
@@ -17359,7 +17359,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:20" ht="19.5">
       <c r="A297" s="2" t="s">
         <v>351</v>
       </c>
@@ -17419,7 +17419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:20" ht="19.5">
       <c r="A298" s="2" t="s">
         <v>351</v>
       </c>
@@ -17479,7 +17479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:20" ht="19.5">
       <c r="A299" s="2" t="s">
         <v>351</v>
       </c>
@@ -17539,7 +17539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:20" ht="19.5">
       <c r="A300" s="2" t="s">
         <v>351</v>
       </c>
@@ -17599,7 +17599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:20" ht="19.5">
       <c r="A301" s="2" t="s">
         <v>351</v>
       </c>
@@ -17659,7 +17659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:20" ht="19.5">
       <c r="A302" s="2" t="s">
         <v>351</v>
       </c>
@@ -17719,7 +17719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:20" ht="19.5">
       <c r="A303" s="2" t="s">
         <v>351</v>
       </c>
@@ -17779,7 +17779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="304" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:20" ht="19.5">
       <c r="A304" s="2" t="s">
         <v>351</v>
       </c>
@@ -17839,7 +17839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="305" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:20" ht="19.5">
       <c r="A305" s="2" t="s">
         <v>351</v>
       </c>
@@ -17879,7 +17879,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="306" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:20" ht="19.5">
       <c r="A306" s="2" t="s">
         <v>351</v>
       </c>
@@ -17939,7 +17939,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="307" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:20" ht="39">
       <c r="A307" s="2" t="s">
         <v>351</v>
       </c>
@@ -17999,7 +17999,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="308" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:20" ht="48.75">
       <c r="A308" s="2" t="s">
         <v>351</v>
       </c>
@@ -18059,7 +18059,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="309" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:20" ht="39">
       <c r="A309" s="2" t="s">
         <v>351</v>
       </c>
@@ -18119,7 +18119,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="310" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:20" ht="39">
       <c r="A310" s="2" t="s">
         <v>351</v>
       </c>
@@ -18179,7 +18179,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="311" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:20" ht="29.25">
       <c r="A311" s="2" t="s">
         <v>351</v>
       </c>
@@ -18239,7 +18239,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="312" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:20" ht="39">
       <c r="A312" s="2" t="s">
         <v>351</v>
       </c>
@@ -18299,7 +18299,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="313" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:20" ht="29.25">
       <c r="A313" s="2" t="s">
         <v>351</v>
       </c>
@@ -18359,7 +18359,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="314" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:20" ht="29.25">
       <c r="A314" s="2" t="s">
         <v>351</v>
       </c>
@@ -18419,7 +18419,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="315" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:20" ht="39">
       <c r="A315" s="2" t="s">
         <v>351</v>
       </c>
@@ -18479,7 +18479,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="316" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:20" ht="29.25">
       <c r="A316" s="2" t="s">
         <v>351</v>
       </c>
@@ -18539,7 +18539,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="317" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:20" ht="39">
       <c r="A317" s="2" t="s">
         <v>351</v>
       </c>
@@ -18599,7 +18599,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="318" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:20" ht="29.25">
       <c r="A318" s="2" t="s">
         <v>351</v>
       </c>
@@ -18659,7 +18659,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="319" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:20" ht="29.25">
       <c r="A319" s="2" t="s">
         <v>351</v>
       </c>
@@ -18721,7 +18721,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="320" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:20" ht="39">
       <c r="A320" s="2" t="s">
         <v>351</v>
       </c>
@@ -18783,7 +18783,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="321" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:20" ht="39">
       <c r="A321" s="2" t="s">
         <v>351</v>
       </c>
@@ -18845,7 +18845,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="322" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:20" ht="68.25">
       <c r="A322" s="2" t="s">
         <v>351</v>
       </c>
@@ -18907,7 +18907,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="323" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:20" ht="58.5">
       <c r="A323" s="2" t="s">
         <v>351</v>
       </c>
@@ -18969,7 +18969,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="324" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:20" ht="68.25">
       <c r="A324" s="2" t="s">
         <v>351</v>
       </c>
@@ -19031,7 +19031,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="325" spans="1:20" ht="72" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:20" ht="68.25">
       <c r="A325" s="2" t="s">
         <v>351</v>
       </c>
@@ -19093,7 +19093,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="326" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:20" ht="39">
       <c r="A326" s="2" t="s">
         <v>351</v>
       </c>
@@ -19153,7 +19153,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="327" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:20" ht="68.25">
       <c r="A327" s="2" t="s">
         <v>351</v>
       </c>
@@ -19213,7 +19213,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="328" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:20" ht="58.5">
       <c r="A328" s="2" t="s">
         <v>351</v>
       </c>
@@ -19273,7 +19273,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="329" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:20" ht="68.25">
       <c r="A329" s="2" t="s">
         <v>351</v>
       </c>
@@ -19333,7 +19333,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="330" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:20" ht="68.25">
       <c r="A330" s="2" t="s">
         <v>351</v>
       </c>
@@ -19393,7 +19393,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="331" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:20" ht="29.25">
       <c r="A331" s="2" t="s">
         <v>392</v>
       </c>
@@ -19449,7 +19449,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="332" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:20" ht="29.25">
       <c r="A332" s="2" t="s">
         <v>392</v>
       </c>
@@ -19505,7 +19505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="333" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:20" ht="29.25">
       <c r="A333" s="2" t="s">
         <v>392</v>
       </c>
@@ -19561,7 +19561,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:20" ht="29.25">
       <c r="A334" s="2" t="s">
         <v>392</v>
       </c>
@@ -19621,7 +19621,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="335" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:20" ht="29.25">
       <c r="A335" s="2" t="s">
         <v>392</v>
       </c>
@@ -19681,7 +19681,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="336" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:20" ht="29.25">
       <c r="A336" s="2" t="s">
         <v>392</v>
       </c>
@@ -19741,7 +19741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="337" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:20" ht="29.25">
       <c r="A337" s="2" t="s">
         <v>392</v>
       </c>
@@ -19801,7 +19801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="338" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:20" ht="29.25">
       <c r="A338" s="2" t="s">
         <v>392</v>
       </c>
@@ -19861,7 +19861,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="339" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:20" ht="29.25">
       <c r="A339" s="2" t="s">
         <v>392</v>
       </c>
@@ -19921,7 +19921,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="340" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:20" ht="29.25">
       <c r="A340" s="2" t="s">
         <v>392</v>
       </c>
@@ -19981,7 +19981,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="341" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:20" ht="29.25">
       <c r="A341" s="2" t="s">
         <v>392</v>
       </c>
@@ -20041,7 +20041,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="342" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:20" ht="29.25">
       <c r="A342" s="2" t="s">
         <v>392</v>
       </c>
@@ -20101,7 +20101,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="343" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:20" ht="29.25">
       <c r="A343" s="2" t="s">
         <v>392</v>
       </c>
@@ -20161,7 +20161,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="344" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:20" ht="29.25">
       <c r="A344" s="2" t="s">
         <v>392</v>
       </c>
@@ -20221,7 +20221,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="345" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:20" ht="29.25">
       <c r="A345" s="2" t="s">
         <v>392</v>
       </c>
@@ -20281,7 +20281,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="346" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:20" ht="29.25">
       <c r="A346" s="2" t="s">
         <v>392</v>
       </c>
@@ -20341,7 +20341,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="347" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:20" ht="29.25">
       <c r="A347" s="2" t="s">
         <v>392</v>
       </c>
@@ -20401,7 +20401,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="348" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:20" ht="29.25">
       <c r="A348" s="2" t="s">
         <v>392</v>
       </c>
@@ -20461,7 +20461,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="349" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:20" ht="29.25">
       <c r="A349" s="2" t="s">
         <v>392</v>
       </c>
@@ -20521,7 +20521,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="350" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:20" ht="29.25">
       <c r="A350" s="2" t="s">
         <v>392</v>
       </c>
@@ -20581,7 +20581,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="351" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:20" ht="29.25">
       <c r="A351" s="2" t="s">
         <v>392</v>
       </c>
@@ -20641,7 +20641,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="352" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:20" ht="29.25">
       <c r="A352" s="2" t="s">
         <v>392</v>
       </c>
@@ -20701,7 +20701,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="353" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:20" ht="29.25">
       <c r="A353" s="2" t="s">
         <v>392</v>
       </c>
@@ -20761,7 +20761,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="354" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:20" ht="29.25">
       <c r="A354" s="2" t="s">
         <v>392</v>
       </c>
@@ -20821,7 +20821,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="355" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:20" ht="29.25">
       <c r="A355" s="2" t="s">
         <v>392</v>
       </c>
@@ -20881,7 +20881,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="356" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:20" ht="29.25">
       <c r="A356" s="2" t="s">
         <v>392</v>
       </c>
@@ -20941,7 +20941,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="357" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:20" ht="29.25">
       <c r="A357" s="2" t="s">
         <v>392</v>
       </c>
@@ -21001,7 +21001,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="358" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:20" ht="29.25">
       <c r="A358" s="2" t="s">
         <v>392</v>
       </c>
@@ -21059,7 +21059,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="359" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:20" ht="29.25">
       <c r="A359" s="2" t="s">
         <v>392</v>
       </c>
@@ -21119,7 +21119,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="360" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:20" ht="29.25">
       <c r="A360" s="2" t="s">
         <v>392</v>
       </c>
@@ -21179,7 +21179,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="361" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:20" ht="29.25">
       <c r="A361" s="2" t="s">
         <v>392</v>
       </c>
@@ -21239,7 +21239,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="362" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:20" ht="29.25">
       <c r="A362" s="2" t="s">
         <v>392</v>
       </c>
@@ -21299,7 +21299,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="363" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:20" ht="29.25">
       <c r="A363" s="2" t="s">
         <v>392</v>
       </c>
@@ -21359,7 +21359,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="364" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:20" ht="39">
       <c r="A364" s="2" t="s">
         <v>392</v>
       </c>
@@ -21419,7 +21419,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="365" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:20" ht="39">
       <c r="A365" s="2" t="s">
         <v>392</v>
       </c>
@@ -21479,7 +21479,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="366" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:20" ht="39">
       <c r="A366" s="2" t="s">
         <v>392</v>
       </c>
@@ -21539,7 +21539,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="367" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:20" ht="39">
       <c r="A367" s="2" t="s">
         <v>392</v>
       </c>
@@ -21599,7 +21599,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="368" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:20" ht="39">
       <c r="A368" s="2" t="s">
         <v>392</v>
       </c>
@@ -21659,7 +21659,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="369" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:20" ht="39">
       <c r="A369" s="2" t="s">
         <v>392</v>
       </c>
@@ -21719,7 +21719,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="370" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:20" ht="39">
       <c r="A370" s="2" t="s">
         <v>392</v>
       </c>
@@ -21779,7 +21779,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="371" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:20" ht="39">
       <c r="A371" s="2" t="s">
         <v>392</v>
       </c>
@@ -21839,7 +21839,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="372" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:20" ht="29.25">
       <c r="A372" s="2" t="s">
         <v>392</v>
       </c>
@@ -21891,7 +21891,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="373" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:20" ht="68.25">
       <c r="A373" s="2" t="s">
         <v>392</v>
       </c>
@@ -21943,7 +21943,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="374" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:20" ht="29.25">
       <c r="A374" s="2" t="s">
         <v>392</v>
       </c>
@@ -21995,7 +21995,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="375" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:20" ht="29.25">
       <c r="A375" s="2" t="s">
         <v>392</v>
       </c>
@@ -22047,7 +22047,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="376" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:20" ht="39">
       <c r="A376" s="2" t="s">
         <v>427</v>
       </c>
@@ -22107,7 +22107,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="377" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:20" ht="39">
       <c r="A377" s="2" t="s">
         <v>427</v>
       </c>
@@ -22167,7 +22167,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="378" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:20" ht="39">
       <c r="A378" s="2" t="s">
         <v>427</v>
       </c>
@@ -22227,7 +22227,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="379" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:20" ht="48.75">
       <c r="A379" s="2" t="s">
         <v>427</v>
       </c>
@@ -22289,7 +22289,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="380" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:20" ht="39">
       <c r="A380" s="2" t="s">
         <v>427</v>
       </c>
@@ -22335,7 +22335,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="381" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:20" ht="39">
       <c r="A381" s="2" t="s">
         <v>427</v>
       </c>
@@ -22381,7 +22381,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="382" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:20" ht="39">
       <c r="A382" s="2" t="s">
         <v>427</v>
       </c>
@@ -22427,7 +22427,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="383" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:20" ht="39">
       <c r="A383" s="2" t="s">
         <v>427</v>
       </c>
@@ -22481,7 +22481,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="384" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:20" ht="39">
       <c r="A384" s="2" t="s">
         <v>427</v>
       </c>
@@ -22527,7 +22527,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="385" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:20" ht="39">
       <c r="A385" s="2" t="s">
         <v>427</v>
       </c>
@@ -22589,7 +22589,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="386" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:20" ht="48.75">
       <c r="A386" s="2" t="s">
         <v>427</v>
       </c>
@@ -22651,7 +22651,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="387" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:20" ht="29.25">
       <c r="A387" s="2" t="s">
         <v>447</v>
       </c>
@@ -22711,7 +22711,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="388" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:20" ht="29.25">
       <c r="A388" s="2" t="s">
         <v>447</v>
       </c>
@@ -22771,7 +22771,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="389" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:20" ht="29.25">
       <c r="A389" s="2" t="s">
         <v>447</v>
       </c>
@@ -22823,7 +22823,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="390" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:20" ht="68.25">
       <c r="A390" s="2" t="s">
         <v>447</v>
       </c>
@@ -22875,7 +22875,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="391" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:20" ht="29.25">
       <c r="A391" s="2" t="s">
         <v>447</v>
       </c>
@@ -22927,7 +22927,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="392" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:20" ht="29.25">
       <c r="A392" s="2" t="s">
         <v>447</v>
       </c>
@@ -22979,7 +22979,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="393" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:20" ht="39">
       <c r="A393" s="2" t="s">
         <v>447</v>
       </c>
@@ -23041,7 +23041,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="394" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:20" ht="39">
       <c r="A394" s="2" t="s">
         <v>447</v>
       </c>
@@ -23099,7 +23099,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="395" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:20" ht="48.75">
       <c r="A395" s="2" t="s">
         <v>447</v>
       </c>
@@ -23161,7 +23161,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="396" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:20" ht="29.25">
       <c r="A396" s="2" t="s">
         <v>447</v>
       </c>
@@ -23215,7 +23215,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="397" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:20" ht="58.5">
       <c r="A397" s="2" t="s">
         <v>459</v>
       </c>
@@ -23275,7 +23275,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="398" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:20" ht="39">
       <c r="A398" s="2" t="s">
         <v>459</v>
       </c>
@@ -23335,7 +23335,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="399" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:20" ht="48.75">
       <c r="A399" s="2" t="s">
         <v>459</v>
       </c>
@@ -23395,7 +23395,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="400" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:20" ht="48.75">
       <c r="A400" s="2" t="s">
         <v>459</v>
       </c>
@@ -23455,7 +23455,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="401" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:20" ht="58.5">
       <c r="A401" s="2" t="s">
         <v>459</v>
       </c>
@@ -23515,7 +23515,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="402" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:20" ht="19.5">
       <c r="A402" s="2" t="s">
         <v>469</v>
       </c>
@@ -23575,7 +23575,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="403" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:20" ht="19.5">
       <c r="A403" s="2" t="s">
         <v>469</v>
       </c>
@@ -23635,7 +23635,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="404" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:20" ht="39">
       <c r="A404" s="2" t="s">
         <v>469</v>
       </c>
@@ -23695,7 +23695,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="405" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:20" ht="19.5">
       <c r="A405" s="2" t="s">
         <v>469</v>
       </c>
@@ -23737,7 +23737,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="406" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:20" ht="19.5">
       <c r="A406" s="2" t="s">
         <v>469</v>
       </c>
@@ -23771,7 +23771,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="407" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:20" ht="19.5">
       <c r="A407" s="2" t="s">
         <v>469</v>
       </c>
@@ -23805,7 +23805,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="408" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:20" ht="19.5">
       <c r="A408" s="2" t="s">
         <v>469</v>
       </c>
@@ -23839,7 +23839,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="409" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:20" ht="19.5">
       <c r="A409" s="2" t="s">
         <v>469</v>
       </c>
@@ -23881,7 +23881,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="410" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:20" ht="19.5">
       <c r="A410" s="2" t="s">
         <v>469</v>
       </c>
@@ -23923,7 +23923,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="411" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:20" ht="19.5">
       <c r="A411" s="2" t="s">
         <v>469</v>
       </c>
@@ -23965,7 +23965,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="412" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:20" ht="29.25">
       <c r="A412" s="2" t="s">
         <v>469</v>
       </c>
@@ -24027,7 +24027,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="413" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:20" ht="19.5">
       <c r="A413" s="2" t="s">
         <v>469</v>
       </c>
@@ -24087,7 +24087,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="414" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:20" ht="29.25">
       <c r="A414" s="2" t="s">
         <v>469</v>
       </c>
@@ -24149,7 +24149,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="415" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:20" ht="29.25">
       <c r="A415" s="2" t="s">
         <v>469</v>
       </c>
@@ -24203,7 +24203,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="416" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:20" ht="29.25">
       <c r="A416" s="2" t="s">
         <v>469</v>
       </c>
@@ -24257,7 +24257,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="417" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:20" ht="19.5">
       <c r="A417" s="2" t="s">
         <v>469</v>
       </c>
@@ -24317,7 +24317,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="418" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:20" ht="29.25">
       <c r="A418" s="2" t="s">
         <v>490</v>
       </c>
@@ -24377,7 +24377,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="419" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:20" ht="29.25">
       <c r="A419" s="2" t="s">
         <v>490</v>
       </c>
@@ -24439,7 +24439,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="420" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:20" ht="29.25">
       <c r="A420" s="2" t="s">
         <v>490</v>
       </c>
@@ -24483,7 +24483,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="421" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:20" ht="29.25">
       <c r="A421" s="2" t="s">
         <v>490</v>
       </c>
@@ -24539,7 +24539,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="422" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:20" ht="29.25">
       <c r="A422" s="2" t="s">
         <v>490</v>
       </c>
@@ -24587,7 +24587,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="423" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:20" ht="29.25">
       <c r="A423" s="2" t="s">
         <v>490</v>
       </c>
@@ -24635,7 +24635,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="424" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:20" ht="29.25">
       <c r="A424" s="2" t="s">
         <v>490</v>
       </c>
@@ -24683,7 +24683,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="425" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:20" ht="29.25">
       <c r="A425" s="2" t="s">
         <v>490</v>
       </c>
@@ -24731,7 +24731,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="426" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:20" ht="29.25">
       <c r="A426" s="2" t="s">
         <v>490</v>
       </c>
@@ -24779,7 +24779,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="427" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:20" ht="29.25">
       <c r="A427" s="2" t="s">
         <v>490</v>
       </c>
@@ -24827,7 +24827,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="428" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:20" ht="39">
       <c r="A428" s="2" t="s">
         <v>490</v>
       </c>
@@ -24875,7 +24875,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="429" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:20" ht="48.75">
       <c r="A429" s="2" t="s">
         <v>490</v>
       </c>
@@ -24923,7 +24923,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="430" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:20" ht="39">
       <c r="A430" s="2" t="s">
         <v>490</v>
       </c>
@@ -24971,7 +24971,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="431" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:20" ht="39">
       <c r="A431" s="2" t="s">
         <v>490</v>
       </c>
@@ -25019,7 +25019,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="432" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:20" ht="29.25">
       <c r="A432" s="2" t="s">
         <v>490</v>
       </c>
@@ -25079,7 +25079,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="433" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:20" ht="29.25">
       <c r="A433" s="2" t="s">
         <v>490</v>
       </c>
@@ -25139,7 +25139,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="434" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:20" ht="29.25">
       <c r="A434" s="2" t="s">
         <v>490</v>
       </c>
@@ -25199,7 +25199,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="435" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:20" ht="29.25">
       <c r="A435" s="2" t="s">
         <v>490</v>
       </c>
@@ -25259,7 +25259,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="436" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:20" ht="29.25">
       <c r="A436" s="2" t="s">
         <v>490</v>
       </c>
@@ -25319,7 +25319,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="437" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:20" ht="29.25">
       <c r="A437" s="2" t="s">
         <v>490</v>
       </c>
@@ -25379,7 +25379,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="438" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:20" ht="39">
       <c r="A438" s="2" t="s">
         <v>490</v>
       </c>
@@ -25421,7 +25421,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="439" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:20" ht="39">
       <c r="A439" s="2" t="s">
         <v>490</v>
       </c>
@@ -25463,7 +25463,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="440" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:20" ht="39">
       <c r="A440" s="2" t="s">
         <v>490</v>
       </c>
@@ -25505,7 +25505,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="441" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:20" ht="39">
       <c r="A441" s="2" t="s">
         <v>490</v>
       </c>
@@ -25547,7 +25547,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="442" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:20" ht="39">
       <c r="A442" s="2" t="s">
         <v>490</v>
       </c>
@@ -25589,7 +25589,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="443" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:20" ht="39">
       <c r="A443" s="2" t="s">
         <v>490</v>
       </c>
@@ -25631,7 +25631,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="444" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:20" ht="39">
       <c r="A444" s="2" t="s">
         <v>490</v>
       </c>
@@ -25673,7 +25673,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="445" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:20" ht="39">
       <c r="A445" s="2" t="s">
         <v>490</v>
       </c>
@@ -25715,7 +25715,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="446" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:20" ht="39">
       <c r="A446" s="2" t="s">
         <v>490</v>
       </c>
@@ -25757,7 +25757,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="447" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:20" ht="39">
       <c r="A447" s="2" t="s">
         <v>490</v>
       </c>
@@ -25799,7 +25799,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="448" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:20" ht="39">
       <c r="A448" s="2" t="s">
         <v>490</v>
       </c>
@@ -25841,7 +25841,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="449" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:20" ht="39">
       <c r="A449" s="2" t="s">
         <v>490</v>
       </c>
@@ -25883,7 +25883,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="450" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:20" ht="29.25">
       <c r="A450" s="2" t="s">
         <v>490</v>
       </c>
@@ -25945,7 +25945,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="451" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:20" ht="29.25">
       <c r="A451" s="2" t="s">
         <v>490</v>
       </c>
@@ -25985,7 +25985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="452" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:20" ht="29.25">
       <c r="A452" s="2" t="s">
         <v>527</v>
       </c>
@@ -26045,7 +26045,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="453" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:20" ht="29.25">
       <c r="A453" s="2" t="s">
         <v>527</v>
       </c>
@@ -26105,7 +26105,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="454" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:20" ht="29.25">
       <c r="A454" s="2" t="s">
         <v>527</v>
       </c>
@@ -26165,7 +26165,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="455" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:20" ht="29.25">
       <c r="A455" s="2" t="s">
         <v>527</v>
       </c>
@@ -26225,7 +26225,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="456" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:20" ht="48.75">
       <c r="A456" s="2" t="s">
         <v>527</v>
       </c>
@@ -26285,7 +26285,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="457" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:20" ht="29.25">
       <c r="A457" s="2" t="s">
         <v>527</v>
       </c>
@@ -26345,7 +26345,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="458" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:20" ht="29.25">
       <c r="A458" s="2" t="s">
         <v>527</v>
       </c>
@@ -26405,7 +26405,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="459" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:20" ht="29.25">
       <c r="A459" s="2" t="s">
         <v>527</v>
       </c>
@@ -26467,7 +26467,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="460" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:20" ht="29.25">
       <c r="A460" s="2" t="s">
         <v>527</v>
       </c>
@@ -26529,7 +26529,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="461" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:20" ht="29.25">
       <c r="A461" s="2" t="s">
         <v>527</v>
       </c>
@@ -26591,7 +26591,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="462" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:20" ht="29.25">
       <c r="A462" s="2" t="s">
         <v>527</v>
       </c>
@@ -26651,7 +26651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="463" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:20" ht="29.25">
       <c r="A463" s="2" t="s">
         <v>527</v>
       </c>
@@ -26713,7 +26713,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="464" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:20" ht="29.25">
       <c r="A464" s="2" t="s">
         <v>527</v>
       </c>
@@ -26775,7 +26775,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="465" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:20" ht="29.25">
       <c r="A465" s="2" t="s">
         <v>527</v>
       </c>
@@ -26835,7 +26835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="466" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:20" ht="29.25">
       <c r="A466" s="2" t="s">
         <v>527</v>
       </c>
@@ -26897,7 +26897,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="467" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:20" ht="48.75">
       <c r="A467" s="2" t="s">
         <v>527</v>
       </c>
@@ -26959,7 +26959,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="468" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:20" ht="29.25">
       <c r="A468" s="2" t="s">
         <v>527</v>
       </c>
@@ -27021,7 +27021,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="469" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:20" ht="39">
       <c r="A469" s="2" t="s">
         <v>527</v>
       </c>
@@ -27083,7 +27083,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="470" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:20" ht="39">
       <c r="A470" s="2" t="s">
         <v>527</v>
       </c>
@@ -27145,7 +27145,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="471" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:20" ht="29.25">
       <c r="A471" s="2" t="s">
         <v>527</v>
       </c>
@@ -27191,7 +27191,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="472" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:20" ht="29.25">
       <c r="A472" s="2" t="s">
         <v>527</v>
       </c>
@@ -27253,7 +27253,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="473" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:20" ht="29.25">
       <c r="A473" s="2" t="s">
         <v>527</v>
       </c>
@@ -27315,7 +27315,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="474" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:20" ht="29.25">
       <c r="A474" s="2" t="s">
         <v>527</v>
       </c>
@@ -27369,7 +27369,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="475" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:20" ht="39">
       <c r="A475" s="2" t="s">
         <v>527</v>
       </c>
@@ -27407,7 +27407,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="476" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:20" ht="39">
       <c r="A476" s="2" t="s">
         <v>527</v>
       </c>
@@ -27469,7 +27469,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="477" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:20" ht="39">
       <c r="A477" s="2" t="s">
         <v>527</v>
       </c>
@@ -27531,8 +27531,8 @@
         <v>562</v>
       </c>
     </row>
-    <row r="478" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:20" ht="18" customHeight="1"/>
+    <row r="479" spans="1:20" ht="17.100000000000001" customHeight="1">
       <c r="A479" s="12" t="s">
         <v>565</v>
       </c>
@@ -27549,7 +27549,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="72" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="74" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okienko 22.10.2024 - aktualizacja EXCEL
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dregerj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1720,7 +1720,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 30-07-2024, 13:15</t>
+    <t>Last update: 23-10-2024, 13:20</t>
   </si>
 </sst>
 </file>
@@ -1735,7 +1735,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2275,7 +2275,7 @@
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2287,17 +2287,17 @@
     <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="36" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="19.5">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="19.5">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="19.5">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="29.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="97.5">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="97.5">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="97.5">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="19.5">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="29.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="29.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="29.25">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="68.25">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="29.25">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="29.25">
       <c r="A27" s="2" t="s">
         <v>21</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="29.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="39">
       <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="39">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="39">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="39">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="19.5">
       <c r="A33" s="2" t="s">
         <v>67</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="29.25">
       <c r="A34" s="2" t="s">
         <v>67</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="29.25">
       <c r="A35" s="2" t="s">
         <v>67</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="29.25">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="29.25">
       <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="29.25">
       <c r="A38" s="2" t="s">
         <v>67</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="29.25">
       <c r="A39" s="2" t="s">
         <v>67</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="39">
       <c r="A40" s="2" t="s">
         <v>67</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="97.5">
       <c r="A41" s="2" t="s">
         <v>67</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="97.5">
       <c r="A42" s="2" t="s">
         <v>67</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="97.5">
       <c r="A43" s="2" t="s">
         <v>67</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="97.5">
       <c r="A44" s="2" t="s">
         <v>67</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="97.5">
       <c r="A45" s="2" t="s">
         <v>67</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="81" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="97.5">
       <c r="A46" s="2" t="s">
         <v>67</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="48.75">
       <c r="A47" s="2" t="s">
         <v>67</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="48.75">
       <c r="A48" s="2" t="s">
         <v>67</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="19.5">
       <c r="A49" s="2" t="s">
         <v>67</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="29.25">
       <c r="A50" s="2" t="s">
         <v>67</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="19.5">
       <c r="A51" s="2" t="s">
         <v>96</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="19.5">
       <c r="A52" s="2" t="s">
         <v>96</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>96</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>96</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>96</v>
       </c>
@@ -5319,7 +5319,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>96</v>
       </c>
@@ -5381,7 +5381,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>96</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>96</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="29.25">
       <c r="A59" s="2" t="s">
         <v>96</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>96</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="29.25">
       <c r="A61" s="2" t="s">
         <v>96</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="29.25">
       <c r="A62" s="2" t="s">
         <v>96</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="29.25">
       <c r="A63" s="2" t="s">
         <v>96</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="19.5">
       <c r="A64" s="2" t="s">
         <v>96</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="29.25">
       <c r="A65" s="2" t="s">
         <v>96</v>
       </c>
@@ -5935,7 +5935,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="29.25">
       <c r="A66" s="2" t="s">
         <v>96</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="29.25">
       <c r="A67" s="2" t="s">
         <v>96</v>
       </c>
@@ -6059,7 +6059,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="29.25">
       <c r="A68" s="2" t="s">
         <v>96</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="29.25">
       <c r="A69" s="2" t="s">
         <v>96</v>
       </c>
@@ -6179,7 +6179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="29.25">
       <c r="A70" s="2" t="s">
         <v>96</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="29.25">
       <c r="A71" s="2" t="s">
         <v>96</v>
       </c>
@@ -6299,7 +6299,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="19.5">
       <c r="A72" s="2" t="s">
         <v>96</v>
       </c>
@@ -6359,7 +6359,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="19.5">
       <c r="A73" s="2" t="s">
         <v>96</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="19.5">
       <c r="A74" s="2" t="s">
         <v>96</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="19.5">
       <c r="A75" s="2" t="s">
         <v>96</v>
       </c>
@@ -6539,7 +6539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="29.25">
       <c r="A76" s="2" t="s">
         <v>96</v>
       </c>
@@ -6599,7 +6599,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="29.25">
       <c r="A77" s="2" t="s">
         <v>96</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" ht="19.5">
       <c r="A78" s="2" t="s">
         <v>96</v>
       </c>
@@ -6701,7 +6701,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" ht="19.5">
       <c r="A79" s="2" t="s">
         <v>96</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="19.5">
       <c r="A80" s="2" t="s">
         <v>96</v>
       </c>
@@ -6825,7 +6825,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" ht="19.5">
       <c r="A81" s="2" t="s">
         <v>96</v>
       </c>
@@ -6869,7 +6869,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" ht="29.25">
       <c r="A82" s="2" t="s">
         <v>96</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" ht="29.25">
       <c r="A83" s="2" t="s">
         <v>96</v>
       </c>
@@ -6985,7 +6985,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" ht="19.5">
       <c r="A84" s="2" t="s">
         <v>96</v>
       </c>
@@ -7021,7 +7021,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" ht="29.25">
       <c r="A85" s="2" t="s">
         <v>96</v>
       </c>
@@ -7057,7 +7057,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" ht="19.5">
       <c r="A86" s="2" t="s">
         <v>96</v>
       </c>
@@ -7117,7 +7117,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" ht="19.5">
       <c r="A87" s="2" t="s">
         <v>96</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" ht="19.5">
       <c r="A88" s="2" t="s">
         <v>96</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" ht="19.5">
       <c r="A89" s="2" t="s">
         <v>96</v>
       </c>
@@ -7281,7 +7281,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" ht="19.5">
       <c r="A90" s="2" t="s">
         <v>96</v>
       </c>
@@ -7327,7 +7327,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" ht="29.25">
       <c r="A91" s="2" t="s">
         <v>96</v>
       </c>
@@ -7383,7 +7383,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" ht="19.5">
       <c r="A92" s="2" t="s">
         <v>96</v>
       </c>
@@ -7425,7 +7425,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" ht="19.5">
       <c r="A93" s="2" t="s">
         <v>96</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" ht="19.5">
       <c r="A94" s="2" t="s">
         <v>96</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" ht="19.5">
       <c r="A95" s="2" t="s">
         <v>96</v>
       </c>
@@ -7567,7 +7567,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" ht="78">
       <c r="A96" s="2" t="s">
         <v>150</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" ht="78">
       <c r="A97" s="2" t="s">
         <v>150</v>
       </c>
@@ -7647,7 +7647,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" ht="78">
       <c r="A98" s="2" t="s">
         <v>150</v>
       </c>
@@ -7687,7 +7687,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" ht="78">
       <c r="A99" s="2" t="s">
         <v>150</v>
       </c>
@@ -7731,7 +7731,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" ht="78">
       <c r="A100" s="2" t="s">
         <v>150</v>
       </c>
@@ -7775,7 +7775,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" ht="78">
       <c r="A101" s="2" t="s">
         <v>150</v>
       </c>
@@ -7819,7 +7819,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" ht="78">
       <c r="A102" s="2" t="s">
         <v>150</v>
       </c>
@@ -7863,7 +7863,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" ht="78">
       <c r="A103" s="2" t="s">
         <v>150</v>
       </c>
@@ -7907,7 +7907,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" ht="78">
       <c r="A104" s="2" t="s">
         <v>150</v>
       </c>
@@ -7951,7 +7951,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" ht="29.25">
       <c r="A105" s="2" t="s">
         <v>150</v>
       </c>
@@ -7989,7 +7989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" ht="19.5">
       <c r="A106" s="2" t="s">
         <v>150</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" ht="19.5">
       <c r="A107" s="2" t="s">
         <v>150</v>
       </c>
@@ -8113,7 +8113,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" ht="19.5">
       <c r="A108" s="2" t="s">
         <v>150</v>
       </c>
@@ -8175,7 +8175,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" ht="19.5">
       <c r="A109" s="2" t="s">
         <v>150</v>
       </c>
@@ -8213,7 +8213,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" ht="19.5">
       <c r="A110" s="2" t="s">
         <v>150</v>
       </c>
@@ -8251,7 +8251,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" ht="19.5">
       <c r="A111" s="2" t="s">
         <v>150</v>
       </c>
@@ -8289,7 +8289,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" ht="29.25">
       <c r="A112" s="2" t="s">
         <v>150</v>
       </c>
@@ -8335,7 +8335,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" ht="19.5">
       <c r="A113" s="2" t="s">
         <v>150</v>
       </c>
@@ -8385,7 +8385,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" ht="39">
       <c r="A114" s="2" t="s">
         <v>150</v>
       </c>
@@ -8435,7 +8435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" ht="48.75">
       <c r="A115" s="2" t="s">
         <v>150</v>
       </c>
@@ -8485,7 +8485,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" ht="58.5">
       <c r="A116" s="2" t="s">
         <v>150</v>
       </c>
@@ -8535,7 +8535,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" ht="29.25">
       <c r="A117" s="2" t="s">
         <v>150</v>
       </c>
@@ -8585,7 +8585,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" ht="29.25">
       <c r="A118" s="2" t="s">
         <v>150</v>
       </c>
@@ -8631,7 +8631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" ht="19.5">
       <c r="A119" s="2" t="s">
         <v>150</v>
       </c>
@@ -8681,7 +8681,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" ht="39">
       <c r="A120" s="2" t="s">
         <v>150</v>
       </c>
@@ -8731,7 +8731,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" ht="48.75">
       <c r="A121" s="2" t="s">
         <v>150</v>
       </c>
@@ -8781,7 +8781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" ht="58.5">
       <c r="A122" s="2" t="s">
         <v>150</v>
       </c>
@@ -8831,7 +8831,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" ht="29.25">
       <c r="A123" s="2" t="s">
         <v>150</v>
       </c>
@@ -8881,7 +8881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" ht="48.75">
       <c r="A124" s="2" t="s">
         <v>150</v>
       </c>
@@ -8923,7 +8923,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" ht="48.75">
       <c r="A125" s="2" t="s">
         <v>150</v>
       </c>
@@ -8965,7 +8965,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20" ht="29.25">
       <c r="A126" s="2" t="s">
         <v>150</v>
       </c>
@@ -9025,7 +9025,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20" ht="29.25">
       <c r="A127" s="2" t="s">
         <v>150</v>
       </c>
@@ -9061,7 +9061,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" ht="29.25">
       <c r="A128" s="2" t="s">
         <v>150</v>
       </c>
@@ -9097,7 +9097,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20" ht="29.25">
       <c r="A129" s="2" t="s">
         <v>150</v>
       </c>
@@ -9133,7 +9133,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20" ht="29.25">
       <c r="A130" s="2" t="s">
         <v>150</v>
       </c>
@@ -9169,7 +9169,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" ht="29.25">
       <c r="A131" s="2" t="s">
         <v>150</v>
       </c>
@@ -9205,7 +9205,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20" ht="29.25">
       <c r="A132" s="2" t="s">
         <v>150</v>
       </c>
@@ -9241,7 +9241,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" ht="29.25">
       <c r="A133" s="2" t="s">
         <v>150</v>
       </c>
@@ -9277,7 +9277,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20" ht="29.25">
       <c r="A134" s="2" t="s">
         <v>150</v>
       </c>
@@ -9313,7 +9313,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:20" ht="29.25">
       <c r="A135" s="2" t="s">
         <v>150</v>
       </c>
@@ -9349,7 +9349,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20" ht="29.25">
       <c r="A136" s="2" t="s">
         <v>150</v>
       </c>
@@ -9385,7 +9385,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20" ht="29.25">
       <c r="A137" s="2" t="s">
         <v>150</v>
       </c>
@@ -9421,7 +9421,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:20" ht="29.25">
       <c r="A138" s="2" t="s">
         <v>150</v>
       </c>
@@ -9457,7 +9457,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" ht="29.25">
       <c r="A139" s="2" t="s">
         <v>150</v>
       </c>
@@ -9493,7 +9493,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20" ht="29.25">
       <c r="A140" s="2" t="s">
         <v>150</v>
       </c>
@@ -9529,7 +9529,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:20" ht="29.25">
       <c r="A141" s="2" t="s">
         <v>150</v>
       </c>
@@ -9565,7 +9565,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:20" ht="29.25">
       <c r="A142" s="2" t="s">
         <v>150</v>
       </c>
@@ -9601,7 +9601,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:20" ht="48.75">
       <c r="A143" s="2" t="s">
         <v>150</v>
       </c>
@@ -9663,7 +9663,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" ht="58.5">
       <c r="A144" s="2" t="s">
         <v>150</v>
       </c>
@@ -9725,7 +9725,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" ht="58.5">
       <c r="A145" s="2" t="s">
         <v>150</v>
       </c>
@@ -9761,7 +9761,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" ht="58.5">
       <c r="A146" s="2" t="s">
         <v>150</v>
       </c>
@@ -9797,7 +9797,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" ht="58.5">
       <c r="A147" s="2" t="s">
         <v>150</v>
       </c>
@@ -9859,7 +9859,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:20" ht="58.5">
       <c r="A148" s="2" t="s">
         <v>150</v>
       </c>
@@ -9921,7 +9921,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:20" ht="58.5">
       <c r="A149" s="2" t="s">
         <v>150</v>
       </c>
@@ -9983,7 +9983,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:20" ht="29.25">
       <c r="A150" s="2" t="s">
         <v>150</v>
       </c>
@@ -10039,7 +10039,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:20" ht="58.5">
       <c r="A151" s="2" t="s">
         <v>150</v>
       </c>
@@ -10095,7 +10095,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:20" ht="58.5">
       <c r="A152" s="2" t="s">
         <v>150</v>
       </c>
@@ -10151,7 +10151,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:20" ht="58.5">
       <c r="A153" s="2" t="s">
         <v>150</v>
       </c>
@@ -10207,7 +10207,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:20" ht="58.5">
       <c r="A154" s="2" t="s">
         <v>150</v>
       </c>
@@ -10263,7 +10263,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:20" ht="29.25">
       <c r="A155" s="2" t="s">
         <v>206</v>
       </c>
@@ -10299,7 +10299,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:20" ht="19.5">
       <c r="A156" s="2" t="s">
         <v>206</v>
       </c>
@@ -10359,7 +10359,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:20" ht="39">
       <c r="A157" s="2" t="s">
         <v>206</v>
       </c>
@@ -10397,7 +10397,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:20" ht="39">
       <c r="A158" s="2" t="s">
         <v>206</v>
       </c>
@@ -10435,7 +10435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:20" ht="39">
       <c r="A159" s="2" t="s">
         <v>206</v>
       </c>
@@ -10473,7 +10473,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:20" ht="39">
       <c r="A160" s="2" t="s">
         <v>206</v>
       </c>
@@ -10511,7 +10511,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:20" ht="39">
       <c r="A161" s="2" t="s">
         <v>206</v>
       </c>
@@ -10549,7 +10549,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:20" ht="19.5">
       <c r="A162" s="2" t="s">
         <v>206</v>
       </c>
@@ -10587,7 +10587,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:20" ht="19.5">
       <c r="A163" s="2" t="s">
         <v>206</v>
       </c>
@@ -10625,7 +10625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:20" ht="19.5">
       <c r="A164" s="2" t="s">
         <v>206</v>
       </c>
@@ -10663,7 +10663,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:20" ht="19.5">
       <c r="A165" s="2" t="s">
         <v>206</v>
       </c>
@@ -10701,7 +10701,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:20" ht="19.5">
       <c r="A166" s="2" t="s">
         <v>206</v>
       </c>
@@ -10739,7 +10739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:20" ht="19.5">
       <c r="A167" s="2" t="s">
         <v>206</v>
       </c>
@@ -10777,7 +10777,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:20" ht="19.5">
       <c r="A168" s="2" t="s">
         <v>206</v>
       </c>
@@ -10815,7 +10815,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:20" ht="19.5">
       <c r="A169" s="2" t="s">
         <v>206</v>
       </c>
@@ -10853,7 +10853,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:20" ht="29.25">
       <c r="A170" s="2" t="s">
         <v>206</v>
       </c>
@@ -10895,7 +10895,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:20" ht="29.25">
       <c r="A171" s="2" t="s">
         <v>206</v>
       </c>
@@ -10937,7 +10937,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:20" ht="29.25">
       <c r="A172" s="2" t="s">
         <v>206</v>
       </c>
@@ -10999,7 +10999,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:20" ht="29.25">
       <c r="A173" s="2" t="s">
         <v>206</v>
       </c>
@@ -11061,7 +11061,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:20" ht="29.25">
       <c r="A174" s="2" t="s">
         <v>206</v>
       </c>
@@ -11123,7 +11123,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:20" ht="29.25">
       <c r="A175" s="2" t="s">
         <v>206</v>
       </c>
@@ -11185,7 +11185,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" ht="29.25">
       <c r="A176" s="2" t="s">
         <v>206</v>
       </c>
@@ -11247,7 +11247,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:20" ht="19.5">
       <c r="A177" s="2" t="s">
         <v>206</v>
       </c>
@@ -11295,7 +11295,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:20" ht="39">
       <c r="A178" s="2" t="s">
         <v>206</v>
       </c>
@@ -11343,7 +11343,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:20" ht="19.5">
       <c r="A179" s="2" t="s">
         <v>206</v>
       </c>
@@ -11391,7 +11391,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:20" ht="39">
       <c r="A180" s="2" t="s">
         <v>206</v>
       </c>
@@ -11439,7 +11439,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:20" ht="39">
       <c r="A181" s="2" t="s">
         <v>206</v>
       </c>
@@ -11487,7 +11487,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:20" ht="39">
       <c r="A182" s="2" t="s">
         <v>206</v>
       </c>
@@ -11535,7 +11535,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:20" ht="39">
       <c r="A183" s="2" t="s">
         <v>206</v>
       </c>
@@ -11583,7 +11583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:20" ht="39">
       <c r="A184" s="2" t="s">
         <v>206</v>
       </c>
@@ -11623,7 +11623,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:20" ht="39">
       <c r="A185" s="2" t="s">
         <v>206</v>
       </c>
@@ -11663,7 +11663,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:20" ht="39">
       <c r="A186" s="2" t="s">
         <v>206</v>
       </c>
@@ -11703,7 +11703,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:20" ht="39">
       <c r="A187" s="2" t="s">
         <v>206</v>
       </c>
@@ -11743,7 +11743,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:20" ht="39">
       <c r="A188" s="2" t="s">
         <v>206</v>
       </c>
@@ -11783,7 +11783,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:20" ht="39">
       <c r="A189" s="2" t="s">
         <v>206</v>
       </c>
@@ -11823,7 +11823,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:20" ht="39">
       <c r="A190" s="2" t="s">
         <v>206</v>
       </c>
@@ -11863,7 +11863,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:20" ht="39">
       <c r="A191" s="2" t="s">
         <v>206</v>
       </c>
@@ -11903,7 +11903,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:20" ht="39">
       <c r="A192" s="2" t="s">
         <v>206</v>
       </c>
@@ -11943,7 +11943,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:20" ht="39">
       <c r="A193" s="2" t="s">
         <v>206</v>
       </c>
@@ -11983,7 +11983,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:20" ht="39">
       <c r="A194" s="2" t="s">
         <v>206</v>
       </c>
@@ -12023,7 +12023,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:20" ht="39">
       <c r="A195" s="2" t="s">
         <v>206</v>
       </c>
@@ -12063,7 +12063,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:20" ht="19.5">
       <c r="A196" s="2" t="s">
         <v>206</v>
       </c>
@@ -12105,7 +12105,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:20" ht="19.5">
       <c r="A197" s="2" t="s">
         <v>206</v>
       </c>
@@ -12163,7 +12163,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:20" ht="19.5">
       <c r="A198" s="2" t="s">
         <v>206</v>
       </c>
@@ -12221,7 +12221,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:20" ht="19.5">
       <c r="A199" s="2" t="s">
         <v>246</v>
       </c>
@@ -12279,7 +12279,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:20" ht="29.25">
       <c r="A200" s="2" t="s">
         <v>246</v>
       </c>
@@ -12337,7 +12337,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:20" ht="19.5">
       <c r="A201" s="2" t="s">
         <v>246</v>
       </c>
@@ -12397,7 +12397,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:20" ht="19.5">
       <c r="A202" s="2" t="s">
         <v>246</v>
       </c>
@@ -12435,7 +12435,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:20" ht="19.5">
       <c r="A203" s="2" t="s">
         <v>246</v>
       </c>
@@ -12473,7 +12473,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:20" ht="29.25">
       <c r="A204" s="2" t="s">
         <v>246</v>
       </c>
@@ -12533,7 +12533,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:20" ht="19.5">
       <c r="A205" s="2" t="s">
         <v>246</v>
       </c>
@@ -12589,7 +12589,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:20" ht="19.5">
       <c r="A206" s="2" t="s">
         <v>246</v>
       </c>
@@ -12635,7 +12635,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:20" ht="29.25">
       <c r="A207" s="2" t="s">
         <v>246</v>
       </c>
@@ -12695,7 +12695,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:20" ht="29.25">
       <c r="A208" s="2" t="s">
         <v>246</v>
       </c>
@@ -12751,7 +12751,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:20" ht="39">
       <c r="A209" s="2" t="s">
         <v>246</v>
       </c>
@@ -12811,7 +12811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:20" ht="19.5">
       <c r="A210" s="2" t="s">
         <v>267</v>
       </c>
@@ -12847,7 +12847,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:20" ht="19.5">
       <c r="A211" s="2" t="s">
         <v>267</v>
       </c>
@@ -12907,7 +12907,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:20" ht="29.25">
       <c r="A212" s="2" t="s">
         <v>267</v>
       </c>
@@ -12963,7 +12963,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:20" ht="29.25">
       <c r="A213" s="2" t="s">
         <v>267</v>
       </c>
@@ -13019,7 +13019,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:20" ht="29.25">
       <c r="A214" s="2" t="s">
         <v>274</v>
       </c>
@@ -13079,7 +13079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:20" ht="29.25">
       <c r="A215" s="2" t="s">
         <v>274</v>
       </c>
@@ -13139,7 +13139,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:20" ht="29.25">
       <c r="A216" s="2" t="s">
         <v>274</v>
       </c>
@@ -13181,7 +13181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:20" ht="29.25">
       <c r="A217" s="2" t="s">
         <v>274</v>
       </c>
@@ -13223,7 +13223,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:20" ht="29.25">
       <c r="A218" s="2" t="s">
         <v>274</v>
       </c>
@@ -13265,7 +13265,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:20" ht="29.25">
       <c r="A219" s="2" t="s">
         <v>274</v>
       </c>
@@ -13325,7 +13325,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:20" ht="29.25">
       <c r="A220" s="2" t="s">
         <v>274</v>
       </c>
@@ -13385,7 +13385,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:20" ht="29.25">
       <c r="A221" s="2" t="s">
         <v>274</v>
       </c>
@@ -13445,7 +13445,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:20" ht="29.25">
       <c r="A222" s="2" t="s">
         <v>274</v>
       </c>
@@ -13493,7 +13493,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:20" ht="29.25">
       <c r="A223" s="2" t="s">
         <v>274</v>
       </c>
@@ -13541,7 +13541,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:20" ht="29.25">
       <c r="A224" s="2" t="s">
         <v>274</v>
       </c>
@@ -13589,7 +13589,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:20" ht="29.25">
       <c r="A225" s="2" t="s">
         <v>274</v>
       </c>
@@ -13637,7 +13637,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:20" ht="29.25">
       <c r="A226" s="2" t="s">
         <v>274</v>
       </c>
@@ -13685,7 +13685,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:20" ht="29.25">
       <c r="A227" s="2" t="s">
         <v>274</v>
       </c>
@@ -13733,7 +13733,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:20" ht="29.25">
       <c r="A228" s="2" t="s">
         <v>274</v>
       </c>
@@ -13781,7 +13781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:20" ht="29.25">
       <c r="A229" s="2" t="s">
         <v>274</v>
       </c>
@@ -13829,7 +13829,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:20" ht="39">
       <c r="A230" s="2" t="s">
         <v>274</v>
       </c>
@@ -13877,7 +13877,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:20" ht="29.25">
       <c r="A231" s="2" t="s">
         <v>274</v>
       </c>
@@ -13925,7 +13925,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:20" ht="39">
       <c r="A232" s="2" t="s">
         <v>274</v>
       </c>
@@ -13973,7 +13973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:20" ht="29.25">
       <c r="A233" s="2" t="s">
         <v>274</v>
       </c>
@@ -14021,7 +14021,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:20" ht="29.25">
       <c r="A234" s="2" t="s">
         <v>274</v>
       </c>
@@ -14069,7 +14069,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:20" ht="29.25">
       <c r="A235" s="2" t="s">
         <v>274</v>
       </c>
@@ -14117,7 +14117,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:20" ht="29.25">
       <c r="A236" s="2" t="s">
         <v>274</v>
       </c>
@@ -14165,7 +14165,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:20" ht="29.25">
       <c r="A237" s="2" t="s">
         <v>274</v>
       </c>
@@ -14213,7 +14213,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:20" ht="29.25">
       <c r="A238" s="2" t="s">
         <v>274</v>
       </c>
@@ -14261,7 +14261,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:20" ht="29.25">
       <c r="A239" s="2" t="s">
         <v>274</v>
       </c>
@@ -14309,7 +14309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:20" ht="29.25">
       <c r="A240" s="2" t="s">
         <v>274</v>
       </c>
@@ -14357,7 +14357,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:20" ht="29.25">
       <c r="A241" s="2" t="s">
         <v>274</v>
       </c>
@@ -14419,7 +14419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:20" ht="29.25">
       <c r="A242" s="2" t="s">
         <v>274</v>
       </c>
@@ -14481,7 +14481,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="243" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:20" ht="29.25">
       <c r="A243" s="2" t="s">
         <v>274</v>
       </c>
@@ -14543,7 +14543,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:20" ht="29.25">
       <c r="A244" s="2" t="s">
         <v>274</v>
       </c>
@@ -14605,7 +14605,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:20" ht="29.25">
       <c r="A245" s="2" t="s">
         <v>274</v>
       </c>
@@ -14667,7 +14667,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:20" ht="29.25">
       <c r="A246" s="2" t="s">
         <v>274</v>
       </c>
@@ -14729,7 +14729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:20" ht="29.25">
       <c r="A247" s="2" t="s">
         <v>274</v>
       </c>
@@ -14791,7 +14791,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:20" ht="29.25">
       <c r="A248" s="2" t="s">
         <v>274</v>
       </c>
@@ -14853,7 +14853,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:20" ht="29.25">
       <c r="A249" s="2" t="s">
         <v>274</v>
       </c>
@@ -14915,7 +14915,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:20" ht="29.25">
       <c r="A250" s="2" t="s">
         <v>274</v>
       </c>
@@ -14977,7 +14977,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:20" ht="29.25">
       <c r="A251" s="2" t="s">
         <v>274</v>
       </c>
@@ -15037,7 +15037,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:20" ht="29.25">
       <c r="A252" s="2" t="s">
         <v>274</v>
       </c>
@@ -15097,7 +15097,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:20" ht="39">
       <c r="A253" s="2" t="s">
         <v>274</v>
       </c>
@@ -15139,7 +15139,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:20" ht="39">
       <c r="A254" s="2" t="s">
         <v>274</v>
       </c>
@@ -15181,7 +15181,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:20" ht="39">
       <c r="A255" s="2" t="s">
         <v>274</v>
       </c>
@@ -15223,7 +15223,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:20" ht="29.25">
       <c r="A256" s="2" t="s">
         <v>274</v>
       </c>
@@ -15283,7 +15283,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:20" ht="48.75">
       <c r="A257" s="2" t="s">
         <v>274</v>
       </c>
@@ -15341,7 +15341,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:20" ht="29.25">
       <c r="A258" s="2" t="s">
         <v>274</v>
       </c>
@@ -15377,7 +15377,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:20" ht="29.25">
       <c r="A259" s="2" t="s">
         <v>274</v>
       </c>
@@ -15413,7 +15413,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:20" ht="29.25">
       <c r="A260" s="2" t="s">
         <v>274</v>
       </c>
@@ -15449,7 +15449,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:20" ht="29.25">
       <c r="A261" s="2" t="s">
         <v>274</v>
       </c>
@@ -15485,7 +15485,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:20" ht="29.25">
       <c r="A262" s="2" t="s">
         <v>274</v>
       </c>
@@ -15521,7 +15521,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:20" ht="29.25">
       <c r="A263" s="2" t="s">
         <v>274</v>
       </c>
@@ -15557,7 +15557,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:20" ht="29.25">
       <c r="A264" s="2" t="s">
         <v>274</v>
       </c>
@@ -15593,7 +15593,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:20" ht="29.25">
       <c r="A265" s="2" t="s">
         <v>274</v>
       </c>
@@ -15629,7 +15629,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:20" ht="29.25">
       <c r="A266" s="2" t="s">
         <v>274</v>
       </c>
@@ -15681,7 +15681,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:20" ht="29.25">
       <c r="A267" s="2" t="s">
         <v>319</v>
       </c>
@@ -15741,7 +15741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:20" ht="29.25">
       <c r="A268" s="2" t="s">
         <v>319</v>
       </c>
@@ -15801,7 +15801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:20" ht="29.25">
       <c r="A269" s="2" t="s">
         <v>319</v>
       </c>
@@ -15861,7 +15861,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:20" ht="29.25">
       <c r="A270" s="2" t="s">
         <v>319</v>
       </c>
@@ -15921,7 +15921,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:20" ht="29.25">
       <c r="A271" s="2" t="s">
         <v>319</v>
       </c>
@@ -15981,7 +15981,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="272" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:20" ht="29.25">
       <c r="A272" s="2" t="s">
         <v>319</v>
       </c>
@@ -16041,7 +16041,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:20" ht="29.25">
       <c r="A273" s="2" t="s">
         <v>319</v>
       </c>
@@ -16101,7 +16101,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:20" ht="29.25">
       <c r="A274" s="2" t="s">
         <v>319</v>
       </c>
@@ -16161,7 +16161,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="275" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:20" ht="29.25">
       <c r="A275" s="2" t="s">
         <v>319</v>
       </c>
@@ -16221,7 +16221,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="276" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:20" ht="29.25">
       <c r="A276" s="2" t="s">
         <v>319</v>
       </c>
@@ -16281,7 +16281,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:20" ht="29.25">
       <c r="A277" s="2" t="s">
         <v>319</v>
       </c>
@@ -16341,7 +16341,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:20" ht="29.25">
       <c r="A278" s="2" t="s">
         <v>319</v>
       </c>
@@ -16401,7 +16401,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:20" ht="29.25">
       <c r="A279" s="2" t="s">
         <v>319</v>
       </c>
@@ -16461,7 +16461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:20" ht="29.25">
       <c r="A280" s="2" t="s">
         <v>319</v>
       </c>
@@ -16521,7 +16521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="281" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:20" ht="29.25">
       <c r="A281" s="2" t="s">
         <v>319</v>
       </c>
@@ -16581,7 +16581,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="282" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:20" ht="29.25">
       <c r="A282" s="2" t="s">
         <v>319</v>
       </c>
@@ -16641,7 +16641,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:20" ht="29.25">
       <c r="A283" s="2" t="s">
         <v>319</v>
       </c>
@@ -16701,7 +16701,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:20" ht="29.25">
       <c r="A284" s="2" t="s">
         <v>319</v>
       </c>
@@ -16761,7 +16761,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:20" ht="29.25">
       <c r="A285" s="2" t="s">
         <v>319</v>
       </c>
@@ -16821,7 +16821,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:20" ht="29.25">
       <c r="A286" s="2" t="s">
         <v>319</v>
       </c>
@@ -16881,7 +16881,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:20" ht="29.25">
       <c r="A287" s="2" t="s">
         <v>319</v>
       </c>
@@ -16933,7 +16933,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:20" ht="29.25">
       <c r="A288" s="2" t="s">
         <v>319</v>
       </c>
@@ -16993,7 +16993,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:20" ht="29.25">
       <c r="A289" s="2" t="s">
         <v>319</v>
       </c>
@@ -17053,7 +17053,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:20" ht="29.25">
       <c r="A290" s="2" t="s">
         <v>319</v>
       </c>
@@ -17109,7 +17109,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="291" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:20" ht="29.25">
       <c r="A291" s="2" t="s">
         <v>319</v>
       </c>
@@ -17163,7 +17163,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:20" ht="39">
       <c r="A292" s="2" t="s">
         <v>319</v>
       </c>
@@ -17215,7 +17215,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:20" ht="39">
       <c r="A293" s="2" t="s">
         <v>319</v>
       </c>
@@ -17269,7 +17269,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:20" ht="19.5">
       <c r="A294" s="2" t="s">
         <v>351</v>
       </c>
@@ -17329,7 +17329,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:20" ht="68.25">
       <c r="A295" s="2" t="s">
         <v>351</v>
       </c>
@@ -17389,7 +17389,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:20" ht="19.5">
       <c r="A296" s="2" t="s">
         <v>351</v>
       </c>
@@ -17449,7 +17449,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:20" ht="19.5">
       <c r="A297" s="2" t="s">
         <v>351</v>
       </c>
@@ -17509,7 +17509,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:20" ht="19.5">
       <c r="A298" s="2" t="s">
         <v>351</v>
       </c>
@@ -17569,7 +17569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:20" ht="19.5">
       <c r="A299" s="2" t="s">
         <v>351</v>
       </c>
@@ -17629,7 +17629,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:20" ht="19.5">
       <c r="A300" s="2" t="s">
         <v>351</v>
       </c>
@@ -17689,7 +17689,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:20" ht="19.5">
       <c r="A301" s="2" t="s">
         <v>351</v>
       </c>
@@ -17749,7 +17749,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:20" ht="19.5">
       <c r="A302" s="2" t="s">
         <v>351</v>
       </c>
@@ -17809,7 +17809,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:20" ht="19.5">
       <c r="A303" s="2" t="s">
         <v>351</v>
       </c>
@@ -17869,7 +17869,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="304" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:20" ht="19.5">
       <c r="A304" s="2" t="s">
         <v>351</v>
       </c>
@@ -17929,7 +17929,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="305" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:20" ht="19.5">
       <c r="A305" s="2" t="s">
         <v>351</v>
       </c>
@@ -17969,7 +17969,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="306" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:20" ht="19.5">
       <c r="A306" s="2" t="s">
         <v>351</v>
       </c>
@@ -18029,7 +18029,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="307" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:20" ht="39">
       <c r="A307" s="2" t="s">
         <v>351</v>
       </c>
@@ -18089,7 +18089,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="308" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:20" ht="48.75">
       <c r="A308" s="2" t="s">
         <v>351</v>
       </c>
@@ -18149,7 +18149,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="309" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:20" ht="39">
       <c r="A309" s="2" t="s">
         <v>351</v>
       </c>
@@ -18209,7 +18209,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="310" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:20" ht="39">
       <c r="A310" s="2" t="s">
         <v>351</v>
       </c>
@@ -18269,7 +18269,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="311" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:20" ht="29.25">
       <c r="A311" s="2" t="s">
         <v>351</v>
       </c>
@@ -18329,7 +18329,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="312" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:20" ht="39">
       <c r="A312" s="2" t="s">
         <v>351</v>
       </c>
@@ -18389,7 +18389,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="313" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:20" ht="29.25">
       <c r="A313" s="2" t="s">
         <v>351</v>
       </c>
@@ -18449,7 +18449,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="314" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:20" ht="29.25">
       <c r="A314" s="2" t="s">
         <v>351</v>
       </c>
@@ -18509,7 +18509,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="315" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:20" ht="39">
       <c r="A315" s="2" t="s">
         <v>351</v>
       </c>
@@ -18569,7 +18569,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="316" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:20" ht="29.25">
       <c r="A316" s="2" t="s">
         <v>351</v>
       </c>
@@ -18629,7 +18629,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="317" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:20" ht="39">
       <c r="A317" s="2" t="s">
         <v>351</v>
       </c>
@@ -18689,7 +18689,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="318" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:20" ht="29.25">
       <c r="A318" s="2" t="s">
         <v>351</v>
       </c>
@@ -18749,7 +18749,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="319" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:20" ht="29.25">
       <c r="A319" s="2" t="s">
         <v>351</v>
       </c>
@@ -18811,7 +18811,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="320" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:20" ht="39">
       <c r="A320" s="2" t="s">
         <v>351</v>
       </c>
@@ -18873,7 +18873,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="321" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:20" ht="39">
       <c r="A321" s="2" t="s">
         <v>351</v>
       </c>
@@ -18935,7 +18935,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="322" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:20" ht="68.25">
       <c r="A322" s="2" t="s">
         <v>351</v>
       </c>
@@ -18997,7 +18997,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="323" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:20" ht="58.5">
       <c r="A323" s="2" t="s">
         <v>351</v>
       </c>
@@ -19059,7 +19059,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="324" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:20" ht="68.25">
       <c r="A324" s="2" t="s">
         <v>351</v>
       </c>
@@ -19121,7 +19121,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="325" spans="1:20" ht="72" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:20" ht="68.25">
       <c r="A325" s="2" t="s">
         <v>351</v>
       </c>
@@ -19183,7 +19183,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="326" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:20" ht="39">
       <c r="A326" s="2" t="s">
         <v>351</v>
       </c>
@@ -19243,7 +19243,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="327" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:20" ht="68.25">
       <c r="A327" s="2" t="s">
         <v>351</v>
       </c>
@@ -19303,7 +19303,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="328" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:20" ht="58.5">
       <c r="A328" s="2" t="s">
         <v>351</v>
       </c>
@@ -19363,7 +19363,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="329" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:20" ht="68.25">
       <c r="A329" s="2" t="s">
         <v>351</v>
       </c>
@@ -19423,7 +19423,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="330" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:20" ht="68.25">
       <c r="A330" s="2" t="s">
         <v>351</v>
       </c>
@@ -19483,7 +19483,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="331" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:20" ht="29.25">
       <c r="A331" s="2" t="s">
         <v>392</v>
       </c>
@@ -19539,7 +19539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="332" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:20" ht="29.25">
       <c r="A332" s="2" t="s">
         <v>392</v>
       </c>
@@ -19595,7 +19595,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="333" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:20" ht="29.25">
       <c r="A333" s="2" t="s">
         <v>392</v>
       </c>
@@ -19651,7 +19651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:20" ht="29.25">
       <c r="A334" s="2" t="s">
         <v>392</v>
       </c>
@@ -19711,7 +19711,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="335" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:20" ht="29.25">
       <c r="A335" s="2" t="s">
         <v>392</v>
       </c>
@@ -19771,7 +19771,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="336" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:20" ht="29.25">
       <c r="A336" s="2" t="s">
         <v>392</v>
       </c>
@@ -19831,7 +19831,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="337" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:20" ht="29.25">
       <c r="A337" s="2" t="s">
         <v>392</v>
       </c>
@@ -19891,7 +19891,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="338" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:20" ht="29.25">
       <c r="A338" s="2" t="s">
         <v>392</v>
       </c>
@@ -19951,7 +19951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="339" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:20" ht="29.25">
       <c r="A339" s="2" t="s">
         <v>392</v>
       </c>
@@ -20011,7 +20011,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="340" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:20" ht="29.25">
       <c r="A340" s="2" t="s">
         <v>392</v>
       </c>
@@ -20071,7 +20071,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="341" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:20" ht="29.25">
       <c r="A341" s="2" t="s">
         <v>392</v>
       </c>
@@ -20131,7 +20131,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="342" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:20" ht="29.25">
       <c r="A342" s="2" t="s">
         <v>392</v>
       </c>
@@ -20191,7 +20191,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="343" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:20" ht="29.25">
       <c r="A343" s="2" t="s">
         <v>392</v>
       </c>
@@ -20251,7 +20251,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="344" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:20" ht="29.25">
       <c r="A344" s="2" t="s">
         <v>392</v>
       </c>
@@ -20311,7 +20311,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="345" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:20" ht="29.25">
       <c r="A345" s="2" t="s">
         <v>392</v>
       </c>
@@ -20371,7 +20371,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="346" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:20" ht="29.25">
       <c r="A346" s="2" t="s">
         <v>392</v>
       </c>
@@ -20431,7 +20431,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="347" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:20" ht="29.25">
       <c r="A347" s="2" t="s">
         <v>392</v>
       </c>
@@ -20491,7 +20491,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="348" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:20" ht="29.25">
       <c r="A348" s="2" t="s">
         <v>392</v>
       </c>
@@ -20551,7 +20551,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="349" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:20" ht="29.25">
       <c r="A349" s="2" t="s">
         <v>392</v>
       </c>
@@ -20611,7 +20611,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="350" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:20" ht="29.25">
       <c r="A350" s="2" t="s">
         <v>392</v>
       </c>
@@ -20671,7 +20671,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="351" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:20" ht="29.25">
       <c r="A351" s="2" t="s">
         <v>392</v>
       </c>
@@ -20731,7 +20731,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="352" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:20" ht="29.25">
       <c r="A352" s="2" t="s">
         <v>392</v>
       </c>
@@ -20791,7 +20791,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="353" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:20" ht="29.25">
       <c r="A353" s="2" t="s">
         <v>392</v>
       </c>
@@ -20851,7 +20851,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="354" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:20" ht="29.25">
       <c r="A354" s="2" t="s">
         <v>392</v>
       </c>
@@ -20911,7 +20911,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="355" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:20" ht="29.25">
       <c r="A355" s="2" t="s">
         <v>392</v>
       </c>
@@ -20971,7 +20971,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="356" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:20" ht="29.25">
       <c r="A356" s="2" t="s">
         <v>392</v>
       </c>
@@ -21031,7 +21031,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="357" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:20" ht="29.25">
       <c r="A357" s="2" t="s">
         <v>392</v>
       </c>
@@ -21091,7 +21091,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="358" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:20" ht="29.25">
       <c r="A358" s="2" t="s">
         <v>392</v>
       </c>
@@ -21149,7 +21149,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="359" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:20" ht="29.25">
       <c r="A359" s="2" t="s">
         <v>392</v>
       </c>
@@ -21209,7 +21209,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="360" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:20" ht="29.25">
       <c r="A360" s="2" t="s">
         <v>392</v>
       </c>
@@ -21269,7 +21269,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="361" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:20" ht="29.25">
       <c r="A361" s="2" t="s">
         <v>392</v>
       </c>
@@ -21329,7 +21329,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="362" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:20" ht="29.25">
       <c r="A362" s="2" t="s">
         <v>392</v>
       </c>
@@ -21389,7 +21389,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="363" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:20" ht="29.25">
       <c r="A363" s="2" t="s">
         <v>392</v>
       </c>
@@ -21449,7 +21449,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="364" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:20" ht="39">
       <c r="A364" s="2" t="s">
         <v>392</v>
       </c>
@@ -21509,7 +21509,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="365" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:20" ht="39">
       <c r="A365" s="2" t="s">
         <v>392</v>
       </c>
@@ -21569,7 +21569,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="366" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:20" ht="39">
       <c r="A366" s="2" t="s">
         <v>392</v>
       </c>
@@ -21629,7 +21629,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="367" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:20" ht="39">
       <c r="A367" s="2" t="s">
         <v>392</v>
       </c>
@@ -21689,7 +21689,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="368" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:20" ht="39">
       <c r="A368" s="2" t="s">
         <v>392</v>
       </c>
@@ -21749,7 +21749,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="369" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:20" ht="39">
       <c r="A369" s="2" t="s">
         <v>392</v>
       </c>
@@ -21809,7 +21809,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="370" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:20" ht="39">
       <c r="A370" s="2" t="s">
         <v>392</v>
       </c>
@@ -21869,7 +21869,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="371" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:20" ht="39">
       <c r="A371" s="2" t="s">
         <v>392</v>
       </c>
@@ -21929,7 +21929,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="372" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:20" ht="29.25">
       <c r="A372" s="2" t="s">
         <v>392</v>
       </c>
@@ -21981,7 +21981,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="373" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:20" ht="68.25">
       <c r="A373" s="2" t="s">
         <v>392</v>
       </c>
@@ -22033,7 +22033,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="374" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:20" ht="29.25">
       <c r="A374" s="2" t="s">
         <v>392</v>
       </c>
@@ -22085,7 +22085,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="375" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:20" ht="29.25">
       <c r="A375" s="2" t="s">
         <v>392</v>
       </c>
@@ -22137,7 +22137,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="376" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:20" ht="39">
       <c r="A376" s="2" t="s">
         <v>427</v>
       </c>
@@ -22197,7 +22197,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="377" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:20" ht="39">
       <c r="A377" s="2" t="s">
         <v>427</v>
       </c>
@@ -22257,7 +22257,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="378" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:20" ht="39">
       <c r="A378" s="2" t="s">
         <v>427</v>
       </c>
@@ -22317,7 +22317,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="379" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:20" ht="48.75">
       <c r="A379" s="2" t="s">
         <v>427</v>
       </c>
@@ -22379,7 +22379,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="380" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:20" ht="39">
       <c r="A380" s="2" t="s">
         <v>427</v>
       </c>
@@ -22425,7 +22425,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="381" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:20" ht="39">
       <c r="A381" s="2" t="s">
         <v>427</v>
       </c>
@@ -22471,7 +22471,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="382" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:20" ht="39">
       <c r="A382" s="2" t="s">
         <v>427</v>
       </c>
@@ -22517,7 +22517,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="383" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:20" ht="39">
       <c r="A383" s="2" t="s">
         <v>427</v>
       </c>
@@ -22571,7 +22571,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="384" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:20" ht="39">
       <c r="A384" s="2" t="s">
         <v>427</v>
       </c>
@@ -22617,7 +22617,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="385" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:20" ht="39">
       <c r="A385" s="2" t="s">
         <v>427</v>
       </c>
@@ -22679,7 +22679,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="386" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:20" ht="48.75">
       <c r="A386" s="2" t="s">
         <v>427</v>
       </c>
@@ -22741,7 +22741,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="387" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:20" ht="29.25">
       <c r="A387" s="2" t="s">
         <v>447</v>
       </c>
@@ -22801,7 +22801,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="388" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:20" ht="29.25">
       <c r="A388" s="2" t="s">
         <v>447</v>
       </c>
@@ -22861,7 +22861,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="389" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:20" ht="29.25">
       <c r="A389" s="2" t="s">
         <v>447</v>
       </c>
@@ -22913,7 +22913,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="390" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:20" ht="68.25">
       <c r="A390" s="2" t="s">
         <v>447</v>
       </c>
@@ -22965,7 +22965,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="391" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:20" ht="29.25">
       <c r="A391" s="2" t="s">
         <v>447</v>
       </c>
@@ -23017,7 +23017,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="392" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:20" ht="29.25">
       <c r="A392" s="2" t="s">
         <v>447</v>
       </c>
@@ -23069,7 +23069,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="393" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:20" ht="39">
       <c r="A393" s="2" t="s">
         <v>447</v>
       </c>
@@ -23131,7 +23131,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="394" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:20" ht="39">
       <c r="A394" s="2" t="s">
         <v>447</v>
       </c>
@@ -23189,7 +23189,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="395" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:20" ht="48.75">
       <c r="A395" s="2" t="s">
         <v>447</v>
       </c>
@@ -23251,7 +23251,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="396" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:20" ht="29.25">
       <c r="A396" s="2" t="s">
         <v>447</v>
       </c>
@@ -23307,7 +23307,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="397" spans="1:20" ht="54" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:20" ht="58.5">
       <c r="A397" s="2" t="s">
         <v>459</v>
       </c>
@@ -23369,7 +23369,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="398" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:20" ht="39">
       <c r="A398" s="2" t="s">
         <v>459</v>
       </c>
@@ -23431,7 +23431,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="399" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:20" ht="48.75">
       <c r="A399" s="2" t="s">
         <v>459</v>
       </c>
@@ -23493,7 +23493,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="400" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:20" ht="48.75">
       <c r="A400" s="2" t="s">
         <v>459</v>
       </c>
@@ -23555,7 +23555,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="401" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:20" ht="58.5">
       <c r="A401" s="2" t="s">
         <v>459</v>
       </c>
@@ -23615,7 +23615,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="402" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:20" ht="19.5">
       <c r="A402" s="2" t="s">
         <v>469</v>
       </c>
@@ -23677,7 +23677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="403" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:20" ht="19.5">
       <c r="A403" s="2" t="s">
         <v>469</v>
       </c>
@@ -23739,7 +23739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="404" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:20" ht="39">
       <c r="A404" s="2" t="s">
         <v>469</v>
       </c>
@@ -23799,7 +23799,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="405" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:20" ht="19.5">
       <c r="A405" s="2" t="s">
         <v>469</v>
       </c>
@@ -23843,7 +23843,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="406" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:20" ht="19.5">
       <c r="A406" s="2" t="s">
         <v>469</v>
       </c>
@@ -23877,7 +23877,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="407" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:20" ht="19.5">
       <c r="A407" s="2" t="s">
         <v>469</v>
       </c>
@@ -23911,7 +23911,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="408" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:20" ht="19.5">
       <c r="A408" s="2" t="s">
         <v>469</v>
       </c>
@@ -23945,7 +23945,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="409" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:20" ht="19.5">
       <c r="A409" s="2" t="s">
         <v>469</v>
       </c>
@@ -23989,7 +23989,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="410" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:20" ht="19.5">
       <c r="A410" s="2" t="s">
         <v>469</v>
       </c>
@@ -24033,7 +24033,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="411" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:20" ht="19.5">
       <c r="A411" s="2" t="s">
         <v>469</v>
       </c>
@@ -24077,7 +24077,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="412" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:20" ht="29.25">
       <c r="A412" s="2" t="s">
         <v>469</v>
       </c>
@@ -24139,7 +24139,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="413" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:20" ht="19.5">
       <c r="A413" s="2" t="s">
         <v>469</v>
       </c>
@@ -24199,7 +24199,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="414" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:20" ht="29.25">
       <c r="A414" s="2" t="s">
         <v>469</v>
       </c>
@@ -24261,7 +24261,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="415" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:20" ht="29.25">
       <c r="A415" s="2" t="s">
         <v>469</v>
       </c>
@@ -24317,7 +24317,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="416" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:20" ht="29.25">
       <c r="A416" s="2" t="s">
         <v>469</v>
       </c>
@@ -24373,7 +24373,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="417" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:20" ht="19.5">
       <c r="A417" s="2" t="s">
         <v>469</v>
       </c>
@@ -24433,7 +24433,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="418" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:20" ht="29.25">
       <c r="A418" s="2" t="s">
         <v>490</v>
       </c>
@@ -24493,7 +24493,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="419" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:20" ht="29.25">
       <c r="A419" s="2" t="s">
         <v>490</v>
       </c>
@@ -24555,7 +24555,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="420" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:20" ht="29.25">
       <c r="A420" s="2" t="s">
         <v>490</v>
       </c>
@@ -24599,7 +24599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="421" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:20" ht="29.25">
       <c r="A421" s="2" t="s">
         <v>490</v>
       </c>
@@ -24655,7 +24655,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="422" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:20" ht="29.25">
       <c r="A422" s="2" t="s">
         <v>490</v>
       </c>
@@ -24705,7 +24705,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="423" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:20" ht="29.25">
       <c r="A423" s="2" t="s">
         <v>490</v>
       </c>
@@ -24755,7 +24755,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="424" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:20" ht="29.25">
       <c r="A424" s="2" t="s">
         <v>490</v>
       </c>
@@ -24805,7 +24805,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="425" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:20" ht="29.25">
       <c r="A425" s="2" t="s">
         <v>490</v>
       </c>
@@ -24855,7 +24855,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="426" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:20" ht="29.25">
       <c r="A426" s="2" t="s">
         <v>490</v>
       </c>
@@ -24905,7 +24905,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="427" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:20" ht="29.25">
       <c r="A427" s="2" t="s">
         <v>490</v>
       </c>
@@ -24955,7 +24955,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="428" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:20" ht="39">
       <c r="A428" s="2" t="s">
         <v>490</v>
       </c>
@@ -25005,7 +25005,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="429" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:20" ht="48.75">
       <c r="A429" s="2" t="s">
         <v>490</v>
       </c>
@@ -25055,7 +25055,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="430" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:20" ht="39">
       <c r="A430" s="2" t="s">
         <v>490</v>
       </c>
@@ -25105,7 +25105,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="431" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:20" ht="39">
       <c r="A431" s="2" t="s">
         <v>490</v>
       </c>
@@ -25155,7 +25155,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="432" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:20" ht="29.25">
       <c r="A432" s="2" t="s">
         <v>490</v>
       </c>
@@ -25215,7 +25215,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="433" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:20" ht="29.25">
       <c r="A433" s="2" t="s">
         <v>490</v>
       </c>
@@ -25275,7 +25275,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="434" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:20" ht="29.25">
       <c r="A434" s="2" t="s">
         <v>490</v>
       </c>
@@ -25335,7 +25335,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="435" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:20" ht="29.25">
       <c r="A435" s="2" t="s">
         <v>490</v>
       </c>
@@ -25395,7 +25395,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="436" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:20" ht="29.25">
       <c r="A436" s="2" t="s">
         <v>490</v>
       </c>
@@ -25455,7 +25455,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="437" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:20" ht="29.25">
       <c r="A437" s="2" t="s">
         <v>490</v>
       </c>
@@ -25515,7 +25515,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="438" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:20" ht="39">
       <c r="A438" s="2" t="s">
         <v>490</v>
       </c>
@@ -25557,7 +25557,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="439" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:20" ht="39">
       <c r="A439" s="2" t="s">
         <v>490</v>
       </c>
@@ -25599,7 +25599,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="440" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:20" ht="39">
       <c r="A440" s="2" t="s">
         <v>490</v>
       </c>
@@ -25641,7 +25641,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="441" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:20" ht="39">
       <c r="A441" s="2" t="s">
         <v>490</v>
       </c>
@@ -25683,7 +25683,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="442" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:20" ht="39">
       <c r="A442" s="2" t="s">
         <v>490</v>
       </c>
@@ -25725,7 +25725,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="443" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:20" ht="39">
       <c r="A443" s="2" t="s">
         <v>490</v>
       </c>
@@ -25767,7 +25767,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="444" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:20" ht="39">
       <c r="A444" s="2" t="s">
         <v>490</v>
       </c>
@@ -25809,7 +25809,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="445" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:20" ht="39">
       <c r="A445" s="2" t="s">
         <v>490</v>
       </c>
@@ -25851,7 +25851,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="446" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:20" ht="39">
       <c r="A446" s="2" t="s">
         <v>490</v>
       </c>
@@ -25893,7 +25893,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="447" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:20" ht="39">
       <c r="A447" s="2" t="s">
         <v>490</v>
       </c>
@@ -25935,7 +25935,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="448" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:20" ht="39">
       <c r="A448" s="2" t="s">
         <v>490</v>
       </c>
@@ -25977,7 +25977,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="449" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:20" ht="39">
       <c r="A449" s="2" t="s">
         <v>490</v>
       </c>
@@ -26019,7 +26019,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="450" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:20" ht="29.25">
       <c r="A450" s="2" t="s">
         <v>490</v>
       </c>
@@ -26081,7 +26081,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="451" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:20" ht="29.25">
       <c r="A451" s="2" t="s">
         <v>490</v>
       </c>
@@ -26121,7 +26121,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="452" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:20" ht="29.25">
       <c r="A452" s="2" t="s">
         <v>527</v>
       </c>
@@ -26183,7 +26183,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="453" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:20" ht="29.25">
       <c r="A453" s="2" t="s">
         <v>527</v>
       </c>
@@ -26245,7 +26245,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="454" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:20" ht="29.25">
       <c r="A454" s="2" t="s">
         <v>527</v>
       </c>
@@ -26307,7 +26307,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="455" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:20" ht="29.25">
       <c r="A455" s="2" t="s">
         <v>527</v>
       </c>
@@ -26369,7 +26369,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="456" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:20" ht="48.75">
       <c r="A456" s="2" t="s">
         <v>527</v>
       </c>
@@ -26431,7 +26431,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="457" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:20" ht="29.25">
       <c r="A457" s="2" t="s">
         <v>527</v>
       </c>
@@ -26493,7 +26493,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="458" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:20" ht="29.25">
       <c r="A458" s="2" t="s">
         <v>527</v>
       </c>
@@ -26555,7 +26555,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="459" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:20" ht="29.25">
       <c r="A459" s="2" t="s">
         <v>527</v>
       </c>
@@ -26617,7 +26617,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="460" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:20" ht="29.25">
       <c r="A460" s="2" t="s">
         <v>527</v>
       </c>
@@ -26679,7 +26679,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="461" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:20" ht="29.25">
       <c r="A461" s="2" t="s">
         <v>527</v>
       </c>
@@ -26741,7 +26741,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="462" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:20" ht="29.25">
       <c r="A462" s="2" t="s">
         <v>527</v>
       </c>
@@ -26801,7 +26801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="463" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:20" ht="29.25">
       <c r="A463" s="2" t="s">
         <v>527</v>
       </c>
@@ -26863,7 +26863,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="464" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:20" ht="29.25">
       <c r="A464" s="2" t="s">
         <v>527</v>
       </c>
@@ -26925,7 +26925,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="465" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:20" ht="29.25">
       <c r="A465" s="2" t="s">
         <v>527</v>
       </c>
@@ -26987,7 +26987,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="466" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:20" ht="29.25">
       <c r="A466" s="2" t="s">
         <v>527</v>
       </c>
@@ -27049,7 +27049,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="467" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:20" ht="48.75">
       <c r="A467" s="2" t="s">
         <v>527</v>
       </c>
@@ -27111,7 +27111,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="468" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:20" ht="29.25">
       <c r="A468" s="2" t="s">
         <v>527</v>
       </c>
@@ -27173,7 +27173,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="469" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:20" ht="39">
       <c r="A469" s="2" t="s">
         <v>527</v>
       </c>
@@ -27235,7 +27235,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="470" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:20" ht="39">
       <c r="A470" s="2" t="s">
         <v>527</v>
       </c>
@@ -27297,7 +27297,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="471" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:20" ht="29.25">
       <c r="A471" s="2" t="s">
         <v>527</v>
       </c>
@@ -27343,7 +27343,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="472" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:20" ht="29.25">
       <c r="A472" s="2" t="s">
         <v>527</v>
       </c>
@@ -27405,7 +27405,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="473" spans="1:20" ht="27" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:20" ht="29.25">
       <c r="A473" s="2" t="s">
         <v>527</v>
       </c>
@@ -27467,7 +27467,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="474" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:20" ht="29.25">
       <c r="A474" s="2" t="s">
         <v>527</v>
       </c>
@@ -27523,7 +27523,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="475" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:20" ht="39">
       <c r="A475" s="2" t="s">
         <v>527</v>
       </c>
@@ -27561,7 +27561,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="476" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:20" ht="39">
       <c r="A476" s="2" t="s">
         <v>527</v>
       </c>
@@ -27623,7 +27623,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="477" spans="1:20" ht="36" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:20" ht="39">
       <c r="A477" s="2" t="s">
         <v>527</v>
       </c>
@@ -27685,8 +27685,8 @@
         <v>562</v>
       </c>
     </row>
-    <row r="478" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:20" ht="18" customHeight="1"/>
+    <row r="479" spans="1:20" ht="17.100000000000001" customHeight="1">
       <c r="A479" s="12" t="s">
         <v>565</v>
       </c>
@@ -27703,7 +27703,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="72" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="74" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Aktualizacja Excel - nowe logo
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1723,7 +1723,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 28-02-2025, 08:52</t>
+    <t>Last update: 03-03-2025, 10:40</t>
   </si>
 </sst>
 </file>
@@ -1958,7 +1958,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1541068</xdr:colOff>
+      <xdr:colOff>2111654</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>457200</xdr:rowOff>
     </xdr:to>
@@ -2274,8 +2274,8 @@
   <dimension ref="A1:U479"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20427,7 +20427,9 @@
       <c r="R336" s="5">
         <v>26.72</v>
       </c>
-      <c r="S336" s="3"/>
+      <c r="S336" s="5">
+        <v>15.76</v>
+      </c>
       <c r="T336" s="3"/>
       <c r="U336" s="2" t="s">
         <v>27</v>
@@ -20488,7 +20490,9 @@
       <c r="R337" s="5">
         <v>14.15</v>
       </c>
-      <c r="S337" s="3"/>
+      <c r="S337" s="5">
+        <v>11.79</v>
+      </c>
       <c r="T337" s="3"/>
       <c r="U337" s="2" t="s">
         <v>27</v>
@@ -20549,7 +20553,9 @@
       <c r="R338" s="5">
         <v>21.07</v>
       </c>
-      <c r="S338" s="3"/>
+      <c r="S338" s="5">
+        <v>20.66</v>
+      </c>
       <c r="T338" s="3"/>
       <c r="U338" s="2" t="s">
         <v>27</v>
@@ -20610,7 +20616,9 @@
       <c r="R339" s="5">
         <v>38.06</v>
       </c>
-      <c r="S339" s="3"/>
+      <c r="S339" s="5">
+        <v>30.24</v>
+      </c>
       <c r="T339" s="3"/>
       <c r="U339" s="2" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Okno serwisowe 11.03. - aktualizacja excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dregerj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1723,7 +1723,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 03-03-2025, 10:40</t>
+    <t>Last update: 11-03-2025, 11:22</t>
   </si>
 </sst>
 </file>
@@ -1738,7 +1738,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2278,7 +2278,7 @@
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2289,17 +2289,17 @@
     <col min="21" max="21" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="36" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="19.5">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="19.5">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="19.5">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="29.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="97.5">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="97.5">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="97.5">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="19.5">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="29.25">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="29.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="29.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="68.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="29.25">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="29.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="29.25">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="39">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="39">
       <c r="A30" s="2" t="s">
         <v>22</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="39">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="39">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="19.5">
       <c r="A33" s="2" t="s">
         <v>68</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="29.25">
       <c r="A34" s="2" t="s">
         <v>68</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="29.25">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="29.25">
       <c r="A36" s="2" t="s">
         <v>68</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="29.25">
       <c r="A37" s="2" t="s">
         <v>68</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="29.25">
       <c r="A38" s="2" t="s">
         <v>68</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="29.25">
       <c r="A39" s="2" t="s">
         <v>68</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="39">
       <c r="A40" s="2" t="s">
         <v>68</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="97.5">
       <c r="A41" s="2" t="s">
         <v>68</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="97.5">
       <c r="A42" s="2" t="s">
         <v>68</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="97.5">
       <c r="A43" s="2" t="s">
         <v>68</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="97.5">
       <c r="A44" s="2" t="s">
         <v>68</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="97.5">
       <c r="A45" s="2" t="s">
         <v>68</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="97.5">
       <c r="A46" s="2" t="s">
         <v>68</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="48.75">
       <c r="A47" s="2" t="s">
         <v>68</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="48.75">
       <c r="A48" s="2" t="s">
         <v>68</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="19.5">
       <c r="A49" s="2" t="s">
         <v>68</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="29.25">
       <c r="A50" s="2" t="s">
         <v>68</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="19.5">
       <c r="A51" s="2" t="s">
         <v>97</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="19.5">
       <c r="A52" s="2" t="s">
         <v>97</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>97</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>97</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>97</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>97</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>97</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>97</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="29.25">
       <c r="A59" s="2" t="s">
         <v>97</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>97</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="29.25">
       <c r="A61" s="2" t="s">
         <v>97</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="29.25">
       <c r="A62" s="2" t="s">
         <v>97</v>
       </c>
@@ -5889,7 +5889,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="29.25">
       <c r="A63" s="2" t="s">
         <v>97</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="19.5">
       <c r="A64" s="2" t="s">
         <v>97</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" ht="29.25">
       <c r="A65" s="2" t="s">
         <v>97</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="29.25">
       <c r="A66" s="2" t="s">
         <v>97</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="29.25">
       <c r="A67" s="2" t="s">
         <v>97</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="29.25">
       <c r="A68" s="2" t="s">
         <v>97</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="29.25">
       <c r="A69" s="2" t="s">
         <v>97</v>
       </c>
@@ -6324,7 +6324,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="29.25">
       <c r="A70" s="2" t="s">
         <v>97</v>
       </c>
@@ -6385,7 +6385,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" ht="29.25">
       <c r="A71" s="2" t="s">
         <v>97</v>
       </c>
@@ -6446,7 +6446,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" ht="19.5">
       <c r="A72" s="2" t="s">
         <v>97</v>
       </c>
@@ -6507,7 +6507,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" ht="19.5">
       <c r="A73" s="2" t="s">
         <v>97</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="19.5">
       <c r="A74" s="2" t="s">
         <v>97</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" ht="19.5">
       <c r="A75" s="2" t="s">
         <v>97</v>
       </c>
@@ -6692,7 +6692,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" ht="29.25">
       <c r="A76" s="2" t="s">
         <v>97</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="77" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="29.25">
       <c r="A77" s="2" t="s">
         <v>97</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" ht="19.5">
       <c r="A78" s="2" t="s">
         <v>97</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" ht="19.5">
       <c r="A79" s="2" t="s">
         <v>97</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" ht="19.5">
       <c r="A80" s="2" t="s">
         <v>97</v>
       </c>
@@ -6985,7 +6985,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" ht="19.5">
       <c r="A81" s="2" t="s">
         <v>97</v>
       </c>
@@ -7030,7 +7030,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" ht="29.25">
       <c r="A82" s="2" t="s">
         <v>97</v>
       </c>
@@ -7089,7 +7089,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" ht="29.25">
       <c r="A83" s="2" t="s">
         <v>97</v>
       </c>
@@ -7148,7 +7148,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="84" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" ht="19.5">
       <c r="A84" s="2" t="s">
         <v>97</v>
       </c>
@@ -7185,7 +7185,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" ht="29.25">
       <c r="A85" s="2" t="s">
         <v>97</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="86" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" ht="19.5">
       <c r="A86" s="2" t="s">
         <v>97</v>
       </c>
@@ -7283,7 +7283,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" ht="19.5">
       <c r="A87" s="2" t="s">
         <v>97</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" ht="19.5">
       <c r="A88" s="2" t="s">
         <v>97</v>
       </c>
@@ -7387,7 +7387,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="89" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" ht="19.5">
       <c r="A89" s="2" t="s">
         <v>97</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="90" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" ht="19.5">
       <c r="A90" s="2" t="s">
         <v>97</v>
       </c>
@@ -7497,7 +7497,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="91" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" ht="29.25">
       <c r="A91" s="2" t="s">
         <v>97</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" ht="19.5">
       <c r="A92" s="2" t="s">
         <v>97</v>
       </c>
@@ -7599,7 +7599,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" ht="19.5">
       <c r="A93" s="2" t="s">
         <v>97</v>
       </c>
@@ -7644,7 +7644,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" ht="19.5">
       <c r="A94" s="2" t="s">
         <v>97</v>
       </c>
@@ -7689,7 +7689,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" ht="19.5">
       <c r="A95" s="2" t="s">
         <v>97</v>
       </c>
@@ -7748,7 +7748,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" ht="78">
       <c r="A96" s="2" t="s">
         <v>151</v>
       </c>
@@ -7789,7 +7789,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" ht="78">
       <c r="A97" s="2" t="s">
         <v>151</v>
       </c>
@@ -7830,7 +7830,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="98" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" ht="78">
       <c r="A98" s="2" t="s">
         <v>151</v>
       </c>
@@ -7871,7 +7871,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="99" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" ht="78">
       <c r="A99" s="2" t="s">
         <v>151</v>
       </c>
@@ -7916,7 +7916,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="100" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" ht="78">
       <c r="A100" s="2" t="s">
         <v>151</v>
       </c>
@@ -7961,7 +7961,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" ht="78">
       <c r="A101" s="2" t="s">
         <v>151</v>
       </c>
@@ -8006,7 +8006,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" ht="78">
       <c r="A102" s="2" t="s">
         <v>151</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="103" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" ht="78">
       <c r="A103" s="2" t="s">
         <v>151</v>
       </c>
@@ -8096,7 +8096,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" ht="78">
       <c r="A104" s="2" t="s">
         <v>151</v>
       </c>
@@ -8141,7 +8141,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" ht="29.25">
       <c r="A105" s="2" t="s">
         <v>151</v>
       </c>
@@ -8180,7 +8180,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="106" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" ht="19.5">
       <c r="A106" s="2" t="s">
         <v>151</v>
       </c>
@@ -8243,7 +8243,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" ht="19.5">
       <c r="A107" s="2" t="s">
         <v>151</v>
       </c>
@@ -8306,7 +8306,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" ht="19.5">
       <c r="A108" s="2" t="s">
         <v>151</v>
       </c>
@@ -8369,7 +8369,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" ht="19.5">
       <c r="A109" s="2" t="s">
         <v>151</v>
       </c>
@@ -8408,7 +8408,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" ht="19.5">
       <c r="A110" s="2" t="s">
         <v>151</v>
       </c>
@@ -8447,7 +8447,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="111" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" ht="19.5">
       <c r="A111" s="2" t="s">
         <v>151</v>
       </c>
@@ -8486,7 +8486,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" ht="29.25">
       <c r="A112" s="2" t="s">
         <v>151</v>
       </c>
@@ -8533,7 +8533,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" ht="19.5">
       <c r="A113" s="2" t="s">
         <v>151</v>
       </c>
@@ -8588,7 +8588,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" ht="39">
       <c r="A114" s="2" t="s">
         <v>151</v>
       </c>
@@ -8643,7 +8643,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" ht="48.75">
       <c r="A115" s="2" t="s">
         <v>151</v>
       </c>
@@ -8698,7 +8698,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" ht="58.5">
       <c r="A116" s="2" t="s">
         <v>151</v>
       </c>
@@ -8753,7 +8753,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="117" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" ht="29.25">
       <c r="A117" s="2" t="s">
         <v>151</v>
       </c>
@@ -8808,7 +8808,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="118" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" ht="29.25">
       <c r="A118" s="2" t="s">
         <v>151</v>
       </c>
@@ -8855,7 +8855,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" ht="19.5">
       <c r="A119" s="2" t="s">
         <v>151</v>
       </c>
@@ -8910,7 +8910,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" ht="39">
       <c r="A120" s="2" t="s">
         <v>151</v>
       </c>
@@ -8965,7 +8965,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" ht="48.75">
       <c r="A121" s="2" t="s">
         <v>151</v>
       </c>
@@ -9020,7 +9020,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="122" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" ht="58.5">
       <c r="A122" s="2" t="s">
         <v>151</v>
       </c>
@@ -9075,7 +9075,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="123" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" ht="29.25">
       <c r="A123" s="2" t="s">
         <v>151</v>
       </c>
@@ -9130,7 +9130,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="124" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" ht="48.75">
       <c r="A124" s="2" t="s">
         <v>151</v>
       </c>
@@ -9173,7 +9173,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="125" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:21" ht="48.75">
       <c r="A125" s="2" t="s">
         <v>151</v>
       </c>
@@ -9216,7 +9216,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="126" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:21" ht="29.25">
       <c r="A126" s="2" t="s">
         <v>151</v>
       </c>
@@ -9277,7 +9277,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="127" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:21" ht="29.25">
       <c r="A127" s="2" t="s">
         <v>151</v>
       </c>
@@ -9314,7 +9314,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:21" ht="29.25">
       <c r="A128" s="2" t="s">
         <v>151</v>
       </c>
@@ -9351,7 +9351,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="129" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:21" ht="29.25">
       <c r="A129" s="2" t="s">
         <v>151</v>
       </c>
@@ -9388,7 +9388,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:21" ht="29.25">
       <c r="A130" s="2" t="s">
         <v>151</v>
       </c>
@@ -9425,7 +9425,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="131" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:21" ht="29.25">
       <c r="A131" s="2" t="s">
         <v>151</v>
       </c>
@@ -9462,7 +9462,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="132" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:21" ht="29.25">
       <c r="A132" s="2" t="s">
         <v>151</v>
       </c>
@@ -9499,7 +9499,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="133" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:21" ht="29.25">
       <c r="A133" s="2" t="s">
         <v>151</v>
       </c>
@@ -9536,7 +9536,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="134" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:21" ht="29.25">
       <c r="A134" s="2" t="s">
         <v>151</v>
       </c>
@@ -9573,7 +9573,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="135" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:21" ht="29.25">
       <c r="A135" s="2" t="s">
         <v>151</v>
       </c>
@@ -9610,7 +9610,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="136" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:21" ht="29.25">
       <c r="A136" s="2" t="s">
         <v>151</v>
       </c>
@@ -9647,7 +9647,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="137" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:21" ht="29.25">
       <c r="A137" s="2" t="s">
         <v>151</v>
       </c>
@@ -9684,7 +9684,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="138" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:21" ht="29.25">
       <c r="A138" s="2" t="s">
         <v>151</v>
       </c>
@@ -9721,7 +9721,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="139" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:21" ht="29.25">
       <c r="A139" s="2" t="s">
         <v>151</v>
       </c>
@@ -9758,7 +9758,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="140" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:21" ht="29.25">
       <c r="A140" s="2" t="s">
         <v>151</v>
       </c>
@@ -9795,7 +9795,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="141" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:21" ht="29.25">
       <c r="A141" s="2" t="s">
         <v>151</v>
       </c>
@@ -9832,7 +9832,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="142" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:21" ht="29.25">
       <c r="A142" s="2" t="s">
         <v>151</v>
       </c>
@@ -9869,7 +9869,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="143" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:21" ht="48.75">
       <c r="A143" s="2" t="s">
         <v>151</v>
       </c>
@@ -9934,7 +9934,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="144" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:21" ht="58.5">
       <c r="A144" s="2" t="s">
         <v>151</v>
       </c>
@@ -9999,7 +9999,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:21" ht="58.5">
       <c r="A145" s="2" t="s">
         <v>151</v>
       </c>
@@ -10036,7 +10036,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="146" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:21" ht="58.5">
       <c r="A146" s="2" t="s">
         <v>151</v>
       </c>
@@ -10073,7 +10073,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="147" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:21" ht="58.5">
       <c r="A147" s="2" t="s">
         <v>151</v>
       </c>
@@ -10138,7 +10138,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="148" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:21" ht="58.5">
       <c r="A148" s="2" t="s">
         <v>151</v>
       </c>
@@ -10203,7 +10203,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="149" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:21" ht="58.5">
       <c r="A149" s="2" t="s">
         <v>151</v>
       </c>
@@ -10268,7 +10268,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="150" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:21" ht="29.25">
       <c r="A150" s="2" t="s">
         <v>151</v>
       </c>
@@ -10325,7 +10325,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="151" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" ht="58.5">
       <c r="A151" s="2" t="s">
         <v>151</v>
       </c>
@@ -10382,7 +10382,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="152" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:21" ht="58.5">
       <c r="A152" s="2" t="s">
         <v>151</v>
       </c>
@@ -10439,7 +10439,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="153" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:21" ht="58.5">
       <c r="A153" s="2" t="s">
         <v>151</v>
       </c>
@@ -10496,7 +10496,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="154" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:21" ht="58.5">
       <c r="A154" s="2" t="s">
         <v>151</v>
       </c>
@@ -10553,7 +10553,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="155" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:21" ht="29.25">
       <c r="A155" s="2" t="s">
         <v>207</v>
       </c>
@@ -10590,7 +10590,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="156" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:21" ht="19.5">
       <c r="A156" s="2" t="s">
         <v>207</v>
       </c>
@@ -10651,7 +10651,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="157" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:21" ht="39">
       <c r="A157" s="2" t="s">
         <v>207</v>
       </c>
@@ -10690,7 +10690,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="158" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:21" ht="39">
       <c r="A158" s="2" t="s">
         <v>207</v>
       </c>
@@ -10729,7 +10729,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="159" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:21" ht="39">
       <c r="A159" s="2" t="s">
         <v>207</v>
       </c>
@@ -10768,7 +10768,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="160" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:21" ht="39">
       <c r="A160" s="2" t="s">
         <v>207</v>
       </c>
@@ -10807,7 +10807,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="161" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" ht="39">
       <c r="A161" s="2" t="s">
         <v>207</v>
       </c>
@@ -10846,7 +10846,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="162" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:21" ht="19.5">
       <c r="A162" s="2" t="s">
         <v>207</v>
       </c>
@@ -10885,7 +10885,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="163" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:21" ht="19.5">
       <c r="A163" s="2" t="s">
         <v>207</v>
       </c>
@@ -10924,7 +10924,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="164" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:21" ht="19.5">
       <c r="A164" s="2" t="s">
         <v>207</v>
       </c>
@@ -10963,7 +10963,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="165" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:21" ht="19.5">
       <c r="A165" s="2" t="s">
         <v>207</v>
       </c>
@@ -11002,7 +11002,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="166" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:21" ht="19.5">
       <c r="A166" s="2" t="s">
         <v>207</v>
       </c>
@@ -11041,7 +11041,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="167" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:21" ht="19.5">
       <c r="A167" s="2" t="s">
         <v>207</v>
       </c>
@@ -11080,7 +11080,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="168" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:21" ht="19.5">
       <c r="A168" s="2" t="s">
         <v>207</v>
       </c>
@@ -11119,7 +11119,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="169" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:21" ht="19.5">
       <c r="A169" s="2" t="s">
         <v>207</v>
       </c>
@@ -11158,7 +11158,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="170" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:21" ht="29.25">
       <c r="A170" s="2" t="s">
         <v>207</v>
       </c>
@@ -11201,7 +11201,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="171" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:21" ht="29.25">
       <c r="A171" s="2" t="s">
         <v>207</v>
       </c>
@@ -11244,7 +11244,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="172" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:21" ht="29.25">
       <c r="A172" s="2" t="s">
         <v>207</v>
       </c>
@@ -11307,7 +11307,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="173" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:21" ht="29.25">
       <c r="A173" s="2" t="s">
         <v>207</v>
       </c>
@@ -11370,7 +11370,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="174" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:21" ht="29.25">
       <c r="A174" s="2" t="s">
         <v>207</v>
       </c>
@@ -11433,7 +11433,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="175" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:21" ht="29.25">
       <c r="A175" s="2" t="s">
         <v>207</v>
       </c>
@@ -11496,7 +11496,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="176" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:21" ht="29.25">
       <c r="A176" s="2" t="s">
         <v>207</v>
       </c>
@@ -11559,7 +11559,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="177" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:21" ht="19.5">
       <c r="A177" s="2" t="s">
         <v>207</v>
       </c>
@@ -11608,7 +11608,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="178" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:21" ht="39">
       <c r="A178" s="2" t="s">
         <v>207</v>
       </c>
@@ -11657,7 +11657,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="179" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:21" ht="19.5">
       <c r="A179" s="2" t="s">
         <v>207</v>
       </c>
@@ -11706,7 +11706,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="180" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:21" ht="39">
       <c r="A180" s="2" t="s">
         <v>207</v>
       </c>
@@ -11755,7 +11755,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="181" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:21" ht="39">
       <c r="A181" s="2" t="s">
         <v>207</v>
       </c>
@@ -11804,7 +11804,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="182" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:21" ht="39">
       <c r="A182" s="2" t="s">
         <v>207</v>
       </c>
@@ -11853,7 +11853,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="183" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:21" ht="39">
       <c r="A183" s="2" t="s">
         <v>207</v>
       </c>
@@ -11902,7 +11902,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="184" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:21" ht="39">
       <c r="A184" s="2" t="s">
         <v>207</v>
       </c>
@@ -11943,7 +11943,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="185" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:21" ht="39">
       <c r="A185" s="2" t="s">
         <v>207</v>
       </c>
@@ -11984,7 +11984,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="186" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:21" ht="39">
       <c r="A186" s="2" t="s">
         <v>207</v>
       </c>
@@ -12025,7 +12025,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="187" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:21" ht="39">
       <c r="A187" s="2" t="s">
         <v>207</v>
       </c>
@@ -12066,7 +12066,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="188" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:21" ht="39">
       <c r="A188" s="2" t="s">
         <v>207</v>
       </c>
@@ -12107,7 +12107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="189" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:21" ht="39">
       <c r="A189" s="2" t="s">
         <v>207</v>
       </c>
@@ -12148,7 +12148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="190" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:21" ht="39">
       <c r="A190" s="2" t="s">
         <v>207</v>
       </c>
@@ -12189,7 +12189,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="191" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:21" ht="39">
       <c r="A191" s="2" t="s">
         <v>207</v>
       </c>
@@ -12230,7 +12230,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="192" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:21" ht="39">
       <c r="A192" s="2" t="s">
         <v>207</v>
       </c>
@@ -12271,7 +12271,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="193" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:21" ht="39">
       <c r="A193" s="2" t="s">
         <v>207</v>
       </c>
@@ -12312,7 +12312,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="194" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:21" ht="39">
       <c r="A194" s="2" t="s">
         <v>207</v>
       </c>
@@ -12353,7 +12353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="195" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:21" ht="39">
       <c r="A195" s="2" t="s">
         <v>207</v>
       </c>
@@ -12394,7 +12394,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="196" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:21" ht="19.5">
       <c r="A196" s="2" t="s">
         <v>207</v>
       </c>
@@ -12437,7 +12437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="197" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:21" ht="19.5">
       <c r="A197" s="2" t="s">
         <v>207</v>
       </c>
@@ -12496,7 +12496,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="198" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:21" ht="19.5">
       <c r="A198" s="2" t="s">
         <v>207</v>
       </c>
@@ -12555,7 +12555,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="199" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:21" ht="19.5">
       <c r="A199" s="2" t="s">
         <v>247</v>
       </c>
@@ -12614,7 +12614,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="200" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:21" ht="29.25">
       <c r="A200" s="2" t="s">
         <v>247</v>
       </c>
@@ -12673,7 +12673,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="201" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:21" ht="19.5">
       <c r="A201" s="2" t="s">
         <v>247</v>
       </c>
@@ -12736,7 +12736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="202" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:21" ht="19.5">
       <c r="A202" s="2" t="s">
         <v>247</v>
       </c>
@@ -12775,7 +12775,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="203" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:21" ht="19.5">
       <c r="A203" s="2" t="s">
         <v>247</v>
       </c>
@@ -12814,7 +12814,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="204" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:21" ht="29.25">
       <c r="A204" s="2" t="s">
         <v>247</v>
       </c>
@@ -12875,7 +12875,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="205" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:21" ht="19.5">
       <c r="A205" s="2" t="s">
         <v>247</v>
       </c>
@@ -12936,7 +12936,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="206" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:21" ht="19.5">
       <c r="A206" s="2" t="s">
         <v>247</v>
       </c>
@@ -12983,7 +12983,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="207" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:21" ht="29.25">
       <c r="A207" s="2" t="s">
         <v>247</v>
       </c>
@@ -13044,7 +13044,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="208" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:21" ht="29.25">
       <c r="A208" s="2" t="s">
         <v>247</v>
       </c>
@@ -13101,7 +13101,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="209" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:21" ht="39">
       <c r="A209" s="2" t="s">
         <v>247</v>
       </c>
@@ -13164,7 +13164,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="210" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:21" ht="19.5">
       <c r="A210" s="2" t="s">
         <v>268</v>
       </c>
@@ -13201,7 +13201,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="211" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:21" ht="19.5">
       <c r="A211" s="2" t="s">
         <v>268</v>
       </c>
@@ -13264,7 +13264,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="212" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:21" ht="29.25">
       <c r="A212" s="2" t="s">
         <v>268</v>
       </c>
@@ -13321,7 +13321,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="213" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:21" ht="29.25">
       <c r="A213" s="2" t="s">
         <v>268</v>
       </c>
@@ -13378,7 +13378,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="214" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:21" ht="29.25">
       <c r="A214" s="2" t="s">
         <v>275</v>
       </c>
@@ -13441,7 +13441,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="215" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:21" ht="29.25">
       <c r="A215" s="2" t="s">
         <v>275</v>
       </c>
@@ -13504,7 +13504,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="216" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:21" ht="29.25">
       <c r="A216" s="2" t="s">
         <v>275</v>
       </c>
@@ -13547,7 +13547,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="217" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:21" ht="29.25">
       <c r="A217" s="2" t="s">
         <v>275</v>
       </c>
@@ -13590,7 +13590,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="218" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:21" ht="29.25">
       <c r="A218" s="2" t="s">
         <v>275</v>
       </c>
@@ -13633,7 +13633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:21" ht="29.25">
       <c r="A219" s="2" t="s">
         <v>275</v>
       </c>
@@ -13696,7 +13696,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="220" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:21" ht="29.25">
       <c r="A220" s="2" t="s">
         <v>275</v>
       </c>
@@ -13759,7 +13759,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="221" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:21" ht="29.25">
       <c r="A221" s="2" t="s">
         <v>275</v>
       </c>
@@ -13822,7 +13822,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="222" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:21" ht="29.25">
       <c r="A222" s="2" t="s">
         <v>275</v>
       </c>
@@ -13871,7 +13871,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="223" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:21" ht="29.25">
       <c r="A223" s="2" t="s">
         <v>275</v>
       </c>
@@ -13920,7 +13920,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="224" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:21" ht="29.25">
       <c r="A224" s="2" t="s">
         <v>275</v>
       </c>
@@ -13969,7 +13969,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="225" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:21" ht="29.25">
       <c r="A225" s="2" t="s">
         <v>275</v>
       </c>
@@ -14018,7 +14018,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="226" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:21" ht="29.25">
       <c r="A226" s="2" t="s">
         <v>275</v>
       </c>
@@ -14067,7 +14067,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="227" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:21" ht="29.25">
       <c r="A227" s="2" t="s">
         <v>275</v>
       </c>
@@ -14116,7 +14116,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="228" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:21" ht="29.25">
       <c r="A228" s="2" t="s">
         <v>275</v>
       </c>
@@ -14165,7 +14165,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="229" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:21" ht="29.25">
       <c r="A229" s="2" t="s">
         <v>275</v>
       </c>
@@ -14214,7 +14214,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="230" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:21" ht="39">
       <c r="A230" s="2" t="s">
         <v>275</v>
       </c>
@@ -14263,7 +14263,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="231" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:21" ht="29.25">
       <c r="A231" s="2" t="s">
         <v>275</v>
       </c>
@@ -14312,7 +14312,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="232" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:21" ht="39">
       <c r="A232" s="2" t="s">
         <v>275</v>
       </c>
@@ -14361,7 +14361,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="233" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:21" ht="29.25">
       <c r="A233" s="2" t="s">
         <v>275</v>
       </c>
@@ -14410,7 +14410,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="234" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:21" ht="29.25">
       <c r="A234" s="2" t="s">
         <v>275</v>
       </c>
@@ -14459,7 +14459,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="235" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:21" ht="29.25">
       <c r="A235" s="2" t="s">
         <v>275</v>
       </c>
@@ -14508,7 +14508,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="236" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:21" ht="29.25">
       <c r="A236" s="2" t="s">
         <v>275</v>
       </c>
@@ -14557,7 +14557,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="237" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:21" ht="29.25">
       <c r="A237" s="2" t="s">
         <v>275</v>
       </c>
@@ -14606,7 +14606,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="238" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:21" ht="29.25">
       <c r="A238" s="2" t="s">
         <v>275</v>
       </c>
@@ -14655,7 +14655,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="239" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:21" ht="29.25">
       <c r="A239" s="2" t="s">
         <v>275</v>
       </c>
@@ -14704,7 +14704,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="240" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:21" ht="29.25">
       <c r="A240" s="2" t="s">
         <v>275</v>
       </c>
@@ -14753,7 +14753,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="241" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:21" ht="29.25">
       <c r="A241" s="2" t="s">
         <v>275</v>
       </c>
@@ -14816,7 +14816,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="242" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:21" ht="29.25">
       <c r="A242" s="2" t="s">
         <v>275</v>
       </c>
@@ -14879,7 +14879,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="243" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:21" ht="29.25">
       <c r="A243" s="2" t="s">
         <v>275</v>
       </c>
@@ -14942,7 +14942,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="244" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:21" ht="29.25">
       <c r="A244" s="2" t="s">
         <v>275</v>
       </c>
@@ -15005,7 +15005,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="245" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:21" ht="29.25">
       <c r="A245" s="2" t="s">
         <v>275</v>
       </c>
@@ -15068,7 +15068,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="246" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:21" ht="29.25">
       <c r="A246" s="2" t="s">
         <v>275</v>
       </c>
@@ -15131,7 +15131,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="247" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:21" ht="29.25">
       <c r="A247" s="2" t="s">
         <v>275</v>
       </c>
@@ -15194,7 +15194,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="248" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:21" ht="29.25">
       <c r="A248" s="2" t="s">
         <v>275</v>
       </c>
@@ -15257,7 +15257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="249" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:21" ht="29.25">
       <c r="A249" s="2" t="s">
         <v>275</v>
       </c>
@@ -15320,7 +15320,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="250" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:21" ht="29.25">
       <c r="A250" s="2" t="s">
         <v>275</v>
       </c>
@@ -15383,7 +15383,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="251" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:21" ht="29.25">
       <c r="A251" s="2" t="s">
         <v>275</v>
       </c>
@@ -15446,7 +15446,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="252" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:21" ht="29.25">
       <c r="A252" s="2" t="s">
         <v>275</v>
       </c>
@@ -15509,7 +15509,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="253" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:21" ht="39">
       <c r="A253" s="2" t="s">
         <v>275</v>
       </c>
@@ -15552,7 +15552,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="254" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:21" ht="39">
       <c r="A254" s="2" t="s">
         <v>275</v>
       </c>
@@ -15595,7 +15595,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="255" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:21" ht="39">
       <c r="A255" s="2" t="s">
         <v>275</v>
       </c>
@@ -15638,7 +15638,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="256" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:21" ht="29.25">
       <c r="A256" s="2" t="s">
         <v>275</v>
       </c>
@@ -15701,7 +15701,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="257" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:21" ht="48.75">
       <c r="A257" s="2" t="s">
         <v>275</v>
       </c>
@@ -15760,7 +15760,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="258" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:21" ht="29.25">
       <c r="A258" s="2" t="s">
         <v>275</v>
       </c>
@@ -15797,7 +15797,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="259" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:21" ht="29.25">
       <c r="A259" s="2" t="s">
         <v>275</v>
       </c>
@@ -15834,7 +15834,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="260" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:21" ht="29.25">
       <c r="A260" s="2" t="s">
         <v>275</v>
       </c>
@@ -15871,7 +15871,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="261" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:21" ht="29.25">
       <c r="A261" s="2" t="s">
         <v>275</v>
       </c>
@@ -15908,7 +15908,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="262" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:21" ht="29.25">
       <c r="A262" s="2" t="s">
         <v>275</v>
       </c>
@@ -15945,7 +15945,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="263" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:21" ht="29.25">
       <c r="A263" s="2" t="s">
         <v>275</v>
       </c>
@@ -15982,7 +15982,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="264" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:21" ht="29.25">
       <c r="A264" s="2" t="s">
         <v>275</v>
       </c>
@@ -16019,7 +16019,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="265" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:21" ht="29.25">
       <c r="A265" s="2" t="s">
         <v>275</v>
       </c>
@@ -16056,7 +16056,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="266" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:21" ht="29.25">
       <c r="A266" s="2" t="s">
         <v>275</v>
       </c>
@@ -16109,7 +16109,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="267" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:21" ht="29.25">
       <c r="A267" s="2" t="s">
         <v>320</v>
       </c>
@@ -16172,7 +16172,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="268" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:21" ht="29.25">
       <c r="A268" s="2" t="s">
         <v>320</v>
       </c>
@@ -16235,7 +16235,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="269" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:21" ht="29.25">
       <c r="A269" s="2" t="s">
         <v>320</v>
       </c>
@@ -16298,7 +16298,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="270" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:21" ht="29.25">
       <c r="A270" s="2" t="s">
         <v>320</v>
       </c>
@@ -16361,7 +16361,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="271" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:21" ht="29.25">
       <c r="A271" s="2" t="s">
         <v>320</v>
       </c>
@@ -16424,7 +16424,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="272" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:21" ht="29.25">
       <c r="A272" s="2" t="s">
         <v>320</v>
       </c>
@@ -16487,7 +16487,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="273" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:21" ht="29.25">
       <c r="A273" s="2" t="s">
         <v>320</v>
       </c>
@@ -16550,7 +16550,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="274" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:21" ht="29.25">
       <c r="A274" s="2" t="s">
         <v>320</v>
       </c>
@@ -16613,7 +16613,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="275" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:21" ht="29.25">
       <c r="A275" s="2" t="s">
         <v>320</v>
       </c>
@@ -16676,7 +16676,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="276" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:21" ht="29.25">
       <c r="A276" s="2" t="s">
         <v>320</v>
       </c>
@@ -16739,7 +16739,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="277" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:21" ht="29.25">
       <c r="A277" s="2" t="s">
         <v>320</v>
       </c>
@@ -16802,7 +16802,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="278" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:21" ht="29.25">
       <c r="A278" s="2" t="s">
         <v>320</v>
       </c>
@@ -16865,7 +16865,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="279" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:21" ht="29.25">
       <c r="A279" s="2" t="s">
         <v>320</v>
       </c>
@@ -16928,7 +16928,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="280" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:21" ht="29.25">
       <c r="A280" s="2" t="s">
         <v>320</v>
       </c>
@@ -16991,7 +16991,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="281" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:21" ht="29.25">
       <c r="A281" s="2" t="s">
         <v>320</v>
       </c>
@@ -17054,7 +17054,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="282" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:21" ht="29.25">
       <c r="A282" s="2" t="s">
         <v>320</v>
       </c>
@@ -17117,7 +17117,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="283" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:21" ht="29.25">
       <c r="A283" s="2" t="s">
         <v>320</v>
       </c>
@@ -17180,7 +17180,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="284" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:21" ht="29.25">
       <c r="A284" s="2" t="s">
         <v>320</v>
       </c>
@@ -17243,7 +17243,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="285" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:21" ht="29.25">
       <c r="A285" s="2" t="s">
         <v>320</v>
       </c>
@@ -17306,7 +17306,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="286" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:21" ht="29.25">
       <c r="A286" s="2" t="s">
         <v>320</v>
       </c>
@@ -17369,7 +17369,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="287" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:21" ht="29.25">
       <c r="A287" s="2" t="s">
         <v>320</v>
       </c>
@@ -17422,7 +17422,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="288" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:21" ht="29.25">
       <c r="A288" s="2" t="s">
         <v>320</v>
       </c>
@@ -17485,7 +17485,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="289" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:21" ht="29.25">
       <c r="A289" s="2" t="s">
         <v>320</v>
       </c>
@@ -17548,7 +17548,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="290" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:21" ht="29.25">
       <c r="A290" s="2" t="s">
         <v>320</v>
       </c>
@@ -17605,7 +17605,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="291" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:21" ht="29.25">
       <c r="A291" s="2" t="s">
         <v>320</v>
       </c>
@@ -17660,7 +17660,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="292" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:21" ht="39">
       <c r="A292" s="2" t="s">
         <v>320</v>
       </c>
@@ -17713,7 +17713,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="293" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:21" ht="39">
       <c r="A293" s="2" t="s">
         <v>320</v>
       </c>
@@ -17768,7 +17768,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="294" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:21" ht="19.5">
       <c r="A294" s="2" t="s">
         <v>352</v>
       </c>
@@ -17831,7 +17831,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="295" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:21" ht="68.25">
       <c r="A295" s="2" t="s">
         <v>352</v>
       </c>
@@ -17894,7 +17894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="296" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:21" ht="19.5">
       <c r="A296" s="2" t="s">
         <v>352</v>
       </c>
@@ -17957,7 +17957,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="297" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:21" ht="19.5">
       <c r="A297" s="2" t="s">
         <v>352</v>
       </c>
@@ -18020,7 +18020,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="298" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:21" ht="19.5">
       <c r="A298" s="2" t="s">
         <v>352</v>
       </c>
@@ -18083,7 +18083,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="299" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:21" ht="19.5">
       <c r="A299" s="2" t="s">
         <v>352</v>
       </c>
@@ -18146,7 +18146,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="300" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:21" ht="19.5">
       <c r="A300" s="2" t="s">
         <v>352</v>
       </c>
@@ -18209,7 +18209,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="301" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:21" ht="19.5">
       <c r="A301" s="2" t="s">
         <v>352</v>
       </c>
@@ -18272,7 +18272,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="302" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:21" ht="19.5">
       <c r="A302" s="2" t="s">
         <v>352</v>
       </c>
@@ -18335,7 +18335,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="303" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:21" ht="19.5">
       <c r="A303" s="2" t="s">
         <v>352</v>
       </c>
@@ -18398,7 +18398,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="304" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:21" ht="19.5">
       <c r="A304" s="2" t="s">
         <v>352</v>
       </c>
@@ -18461,7 +18461,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="305" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:21" ht="19.5">
       <c r="A305" s="2" t="s">
         <v>352</v>
       </c>
@@ -18502,7 +18502,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="306" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:21" ht="19.5">
       <c r="A306" s="2" t="s">
         <v>352</v>
       </c>
@@ -18563,7 +18563,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="307" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:21" ht="39">
       <c r="A307" s="2" t="s">
         <v>352</v>
       </c>
@@ -18626,7 +18626,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="308" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:21" ht="48.75">
       <c r="A308" s="2" t="s">
         <v>352</v>
       </c>
@@ -18689,7 +18689,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="309" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:21" ht="39">
       <c r="A309" s="2" t="s">
         <v>352</v>
       </c>
@@ -18752,7 +18752,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="310" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:21" ht="39">
       <c r="A310" s="2" t="s">
         <v>352</v>
       </c>
@@ -18815,7 +18815,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="311" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:21" ht="29.25">
       <c r="A311" s="2" t="s">
         <v>352</v>
       </c>
@@ -18878,7 +18878,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="312" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:21" ht="39">
       <c r="A312" s="2" t="s">
         <v>352</v>
       </c>
@@ -18941,7 +18941,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="313" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:21" ht="29.25">
       <c r="A313" s="2" t="s">
         <v>352</v>
       </c>
@@ -19004,7 +19004,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="314" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:21" ht="29.25">
       <c r="A314" s="2" t="s">
         <v>352</v>
       </c>
@@ -19067,7 +19067,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="315" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:21" ht="39">
       <c r="A315" s="2" t="s">
         <v>352</v>
       </c>
@@ -19130,7 +19130,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="316" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:21" ht="29.25">
       <c r="A316" s="2" t="s">
         <v>352</v>
       </c>
@@ -19193,7 +19193,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="317" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:21" ht="39">
       <c r="A317" s="2" t="s">
         <v>352</v>
       </c>
@@ -19256,7 +19256,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="318" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:21" ht="29.25">
       <c r="A318" s="2" t="s">
         <v>352</v>
       </c>
@@ -19319,7 +19319,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="319" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:21" ht="29.25">
       <c r="A319" s="2" t="s">
         <v>352</v>
       </c>
@@ -19382,7 +19382,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="320" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:21" ht="39">
       <c r="A320" s="2" t="s">
         <v>352</v>
       </c>
@@ -19445,7 +19445,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="321" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:21" ht="39">
       <c r="A321" s="2" t="s">
         <v>352</v>
       </c>
@@ -19508,7 +19508,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="322" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:21" ht="68.25">
       <c r="A322" s="2" t="s">
         <v>352</v>
       </c>
@@ -19571,7 +19571,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="323" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:21" ht="58.5">
       <c r="A323" s="2" t="s">
         <v>352</v>
       </c>
@@ -19634,7 +19634,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="324" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:21" ht="68.25">
       <c r="A324" s="2" t="s">
         <v>352</v>
       </c>
@@ -19697,7 +19697,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="325" spans="1:21" ht="72" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:21" ht="68.25">
       <c r="A325" s="2" t="s">
         <v>352</v>
       </c>
@@ -19760,7 +19760,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="326" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:21" ht="39">
       <c r="A326" s="2" t="s">
         <v>352</v>
       </c>
@@ -19823,7 +19823,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="327" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:21" ht="68.25">
       <c r="A327" s="2" t="s">
         <v>352</v>
       </c>
@@ -19886,7 +19886,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="328" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:21" ht="58.5">
       <c r="A328" s="2" t="s">
         <v>352</v>
       </c>
@@ -19949,7 +19949,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="329" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:21" ht="68.25">
       <c r="A329" s="2" t="s">
         <v>352</v>
       </c>
@@ -20012,7 +20012,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="330" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:21" ht="68.25">
       <c r="A330" s="2" t="s">
         <v>352</v>
       </c>
@@ -20075,7 +20075,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="331" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:21" ht="29.25">
       <c r="A331" s="2" t="s">
         <v>393</v>
       </c>
@@ -20132,7 +20132,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="332" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:21" ht="29.25">
       <c r="A332" s="2" t="s">
         <v>393</v>
       </c>
@@ -20189,7 +20189,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="333" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:21" ht="29.25">
       <c r="A333" s="2" t="s">
         <v>393</v>
       </c>
@@ -20246,7 +20246,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="334" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:21" ht="29.25">
       <c r="A334" s="2" t="s">
         <v>393</v>
       </c>
@@ -20309,7 +20309,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="335" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:21" ht="29.25">
       <c r="A335" s="2" t="s">
         <v>393</v>
       </c>
@@ -20372,7 +20372,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="336" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:21" ht="29.25">
       <c r="A336" s="2" t="s">
         <v>393</v>
       </c>
@@ -20435,7 +20435,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="337" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:21" ht="29.25">
       <c r="A337" s="2" t="s">
         <v>393</v>
       </c>
@@ -20498,7 +20498,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="338" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:21" ht="29.25">
       <c r="A338" s="2" t="s">
         <v>393</v>
       </c>
@@ -20561,7 +20561,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="339" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:21" ht="29.25">
       <c r="A339" s="2" t="s">
         <v>393</v>
       </c>
@@ -20624,7 +20624,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="340" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:21" ht="29.25">
       <c r="A340" s="2" t="s">
         <v>393</v>
       </c>
@@ -20687,7 +20687,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="341" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:21" ht="29.25">
       <c r="A341" s="2" t="s">
         <v>393</v>
       </c>
@@ -20750,7 +20750,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="342" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:21" ht="29.25">
       <c r="A342" s="2" t="s">
         <v>393</v>
       </c>
@@ -20813,7 +20813,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="343" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:21" ht="29.25">
       <c r="A343" s="2" t="s">
         <v>393</v>
       </c>
@@ -20876,7 +20876,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="344" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:21" ht="29.25">
       <c r="A344" s="2" t="s">
         <v>393</v>
       </c>
@@ -20939,7 +20939,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="345" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:21" ht="29.25">
       <c r="A345" s="2" t="s">
         <v>393</v>
       </c>
@@ -21002,7 +21002,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="346" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:21" ht="29.25">
       <c r="A346" s="2" t="s">
         <v>393</v>
       </c>
@@ -21065,7 +21065,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="347" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:21" ht="29.25">
       <c r="A347" s="2" t="s">
         <v>393</v>
       </c>
@@ -21128,7 +21128,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="348" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:21" ht="29.25">
       <c r="A348" s="2" t="s">
         <v>393</v>
       </c>
@@ -21191,7 +21191,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="349" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:21" ht="29.25">
       <c r="A349" s="2" t="s">
         <v>393</v>
       </c>
@@ -21254,7 +21254,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="350" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:21" ht="29.25">
       <c r="A350" s="2" t="s">
         <v>393</v>
       </c>
@@ -21317,7 +21317,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="351" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:21" ht="29.25">
       <c r="A351" s="2" t="s">
         <v>393</v>
       </c>
@@ -21380,7 +21380,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="352" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:21" ht="29.25">
       <c r="A352" s="2" t="s">
         <v>393</v>
       </c>
@@ -21443,7 +21443,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="353" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:21" ht="29.25">
       <c r="A353" s="2" t="s">
         <v>393</v>
       </c>
@@ -21506,7 +21506,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="354" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:21" ht="29.25">
       <c r="A354" s="2" t="s">
         <v>393</v>
       </c>
@@ -21569,7 +21569,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="355" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:21" ht="29.25">
       <c r="A355" s="2" t="s">
         <v>393</v>
       </c>
@@ -21632,7 +21632,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="356" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:21" ht="29.25">
       <c r="A356" s="2" t="s">
         <v>393</v>
       </c>
@@ -21695,7 +21695,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="357" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:21" ht="29.25">
       <c r="A357" s="2" t="s">
         <v>393</v>
       </c>
@@ -21758,7 +21758,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="358" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:21" ht="29.25">
       <c r="A358" s="2" t="s">
         <v>393</v>
       </c>
@@ -21819,7 +21819,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="359" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:21" ht="29.25">
       <c r="A359" s="2" t="s">
         <v>393</v>
       </c>
@@ -21882,7 +21882,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="360" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:21" ht="29.25">
       <c r="A360" s="2" t="s">
         <v>393</v>
       </c>
@@ -21945,7 +21945,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="361" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:21" ht="29.25">
       <c r="A361" s="2" t="s">
         <v>393</v>
       </c>
@@ -22008,7 +22008,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="362" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:21" ht="29.25">
       <c r="A362" s="2" t="s">
         <v>393</v>
       </c>
@@ -22071,7 +22071,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="363" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:21" ht="29.25">
       <c r="A363" s="2" t="s">
         <v>393</v>
       </c>
@@ -22134,7 +22134,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="364" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:21" ht="39">
       <c r="A364" s="2" t="s">
         <v>393</v>
       </c>
@@ -22197,7 +22197,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="365" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:21" ht="39">
       <c r="A365" s="2" t="s">
         <v>393</v>
       </c>
@@ -22260,7 +22260,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="366" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:21" ht="39">
       <c r="A366" s="2" t="s">
         <v>393</v>
       </c>
@@ -22323,7 +22323,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="367" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:21" ht="39">
       <c r="A367" s="2" t="s">
         <v>393</v>
       </c>
@@ -22386,7 +22386,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="368" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:21" ht="39">
       <c r="A368" s="2" t="s">
         <v>393</v>
       </c>
@@ -22449,7 +22449,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="369" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:21" ht="39">
       <c r="A369" s="2" t="s">
         <v>393</v>
       </c>
@@ -22512,7 +22512,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="370" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:21" ht="39">
       <c r="A370" s="2" t="s">
         <v>393</v>
       </c>
@@ -22575,7 +22575,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="371" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:21" ht="39">
       <c r="A371" s="2" t="s">
         <v>393</v>
       </c>
@@ -22638,7 +22638,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="372" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:21" ht="29.25">
       <c r="A372" s="2" t="s">
         <v>393</v>
       </c>
@@ -22693,7 +22693,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="373" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:21" ht="68.25">
       <c r="A373" s="2" t="s">
         <v>393</v>
       </c>
@@ -22748,7 +22748,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="374" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:21" ht="29.25">
       <c r="A374" s="2" t="s">
         <v>393</v>
       </c>
@@ -22803,7 +22803,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="375" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:21" ht="29.25">
       <c r="A375" s="2" t="s">
         <v>393</v>
       </c>
@@ -22858,7 +22858,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="376" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:21" ht="39">
       <c r="A376" s="2" t="s">
         <v>428</v>
       </c>
@@ -22921,7 +22921,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="377" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:21" ht="39">
       <c r="A377" s="2" t="s">
         <v>428</v>
       </c>
@@ -22984,7 +22984,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="378" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:21" ht="39">
       <c r="A378" s="2" t="s">
         <v>428</v>
       </c>
@@ -23047,7 +23047,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="379" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:21" ht="48.75">
       <c r="A379" s="2" t="s">
         <v>428</v>
       </c>
@@ -23110,7 +23110,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="380" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:21" ht="39">
       <c r="A380" s="2" t="s">
         <v>428</v>
       </c>
@@ -23157,7 +23157,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="381" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:21" ht="39">
       <c r="A381" s="2" t="s">
         <v>428</v>
       </c>
@@ -23204,7 +23204,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="382" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:21" ht="39">
       <c r="A382" s="2" t="s">
         <v>428</v>
       </c>
@@ -23251,7 +23251,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="383" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:21" ht="39">
       <c r="A383" s="2" t="s">
         <v>428</v>
       </c>
@@ -23306,7 +23306,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="384" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:21" ht="39">
       <c r="A384" s="2" t="s">
         <v>428</v>
       </c>
@@ -23353,7 +23353,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="385" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:21" ht="39">
       <c r="A385" s="2" t="s">
         <v>428</v>
       </c>
@@ -23418,7 +23418,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="386" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:21" ht="48.75">
       <c r="A386" s="2" t="s">
         <v>428</v>
       </c>
@@ -23483,7 +23483,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="387" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:21" ht="29.25">
       <c r="A387" s="2" t="s">
         <v>448</v>
       </c>
@@ -23546,7 +23546,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="388" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:21" ht="29.25">
       <c r="A388" s="2" t="s">
         <v>448</v>
       </c>
@@ -23609,7 +23609,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="389" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:21" ht="29.25">
       <c r="A389" s="2" t="s">
         <v>448</v>
       </c>
@@ -23664,7 +23664,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="390" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:21" ht="68.25">
       <c r="A390" s="2" t="s">
         <v>448</v>
       </c>
@@ -23719,7 +23719,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="391" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:21" ht="29.25">
       <c r="A391" s="2" t="s">
         <v>448</v>
       </c>
@@ -23774,7 +23774,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="392" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:21" ht="29.25">
       <c r="A392" s="2" t="s">
         <v>448</v>
       </c>
@@ -23829,7 +23829,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="393" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:21" ht="39">
       <c r="A393" s="2" t="s">
         <v>448</v>
       </c>
@@ -23894,7 +23894,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="394" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:21" ht="39">
       <c r="A394" s="2" t="s">
         <v>448</v>
       </c>
@@ -23955,7 +23955,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="395" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:21" ht="48.75">
       <c r="A395" s="2" t="s">
         <v>448</v>
       </c>
@@ -24020,7 +24020,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="396" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:21" ht="29.25">
       <c r="A396" s="2" t="s">
         <v>448</v>
       </c>
@@ -24077,7 +24077,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="397" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:21" ht="58.5">
       <c r="A397" s="2" t="s">
         <v>460</v>
       </c>
@@ -24140,7 +24140,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="398" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:21" ht="39">
       <c r="A398" s="2" t="s">
         <v>460</v>
       </c>
@@ -24203,7 +24203,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="399" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:21" ht="48.75">
       <c r="A399" s="2" t="s">
         <v>460</v>
       </c>
@@ -24266,7 +24266,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="400" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:21" ht="48.75">
       <c r="A400" s="2" t="s">
         <v>460</v>
       </c>
@@ -24329,7 +24329,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="401" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:21" ht="58.5">
       <c r="A401" s="2" t="s">
         <v>460</v>
       </c>
@@ -24392,7 +24392,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="402" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:21" ht="19.5">
       <c r="A402" s="2" t="s">
         <v>470</v>
       </c>
@@ -24455,7 +24455,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="403" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:21" ht="19.5">
       <c r="A403" s="2" t="s">
         <v>470</v>
       </c>
@@ -24518,7 +24518,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="404" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:21" ht="39">
       <c r="A404" s="2" t="s">
         <v>470</v>
       </c>
@@ -24581,7 +24581,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="405" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:21" ht="19.5">
       <c r="A405" s="2" t="s">
         <v>470</v>
       </c>
@@ -24626,7 +24626,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="406" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:21" ht="19.5">
       <c r="A406" s="2" t="s">
         <v>470</v>
       </c>
@@ -24661,7 +24661,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="407" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:21" ht="19.5">
       <c r="A407" s="2" t="s">
         <v>470</v>
       </c>
@@ -24696,7 +24696,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="408" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:21" ht="19.5">
       <c r="A408" s="2" t="s">
         <v>470</v>
       </c>
@@ -24731,7 +24731,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="409" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:21" ht="19.5">
       <c r="A409" s="2" t="s">
         <v>470</v>
       </c>
@@ -24776,7 +24776,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="410" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:21" ht="19.5">
       <c r="A410" s="2" t="s">
         <v>470</v>
       </c>
@@ -24821,7 +24821,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="411" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:21" ht="19.5">
       <c r="A411" s="2" t="s">
         <v>470</v>
       </c>
@@ -24866,7 +24866,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="412" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:21" ht="29.25">
       <c r="A412" s="2" t="s">
         <v>470</v>
       </c>
@@ -24931,7 +24931,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="413" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:21" ht="19.5">
       <c r="A413" s="2" t="s">
         <v>470</v>
       </c>
@@ -24994,7 +24994,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="414" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:21" ht="29.25">
       <c r="A414" s="2" t="s">
         <v>470</v>
       </c>
@@ -25059,7 +25059,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="415" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:21" ht="29.25">
       <c r="A415" s="2" t="s">
         <v>470</v>
       </c>
@@ -25116,7 +25116,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="416" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:21" ht="29.25">
       <c r="A416" s="2" t="s">
         <v>470</v>
       </c>
@@ -25173,7 +25173,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="417" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:21" ht="19.5">
       <c r="A417" s="2" t="s">
         <v>470</v>
       </c>
@@ -25236,7 +25236,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="418" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:21" ht="29.25">
       <c r="A418" s="2" t="s">
         <v>491</v>
       </c>
@@ -25297,7 +25297,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="419" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:21" ht="29.25">
       <c r="A419" s="2" t="s">
         <v>491</v>
       </c>
@@ -25355,12 +25355,14 @@
       <c r="S419" s="6">
         <v>2</v>
       </c>
-      <c r="T419" s="3"/>
+      <c r="T419" s="6">
+        <v>0</v>
+      </c>
       <c r="U419" s="2" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="420" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:21" ht="29.25">
       <c r="A420" s="2" t="s">
         <v>491</v>
       </c>
@@ -25405,7 +25407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="421" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:21" ht="29.25">
       <c r="A421" s="2" t="s">
         <v>491</v>
       </c>
@@ -25464,7 +25466,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="422" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:21" ht="29.25">
       <c r="A422" s="2" t="s">
         <v>491</v>
       </c>
@@ -25515,7 +25517,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="423" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:21" ht="29.25">
       <c r="A423" s="2" t="s">
         <v>491</v>
       </c>
@@ -25566,7 +25568,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="424" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:21" ht="29.25">
       <c r="A424" s="2" t="s">
         <v>491</v>
       </c>
@@ -25617,7 +25619,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="425" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:21" ht="29.25">
       <c r="A425" s="2" t="s">
         <v>491</v>
       </c>
@@ -25668,7 +25670,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="426" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:21" ht="29.25">
       <c r="A426" s="2" t="s">
         <v>491</v>
       </c>
@@ -25719,7 +25721,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="427" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:21" ht="29.25">
       <c r="A427" s="2" t="s">
         <v>491</v>
       </c>
@@ -25770,7 +25772,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="428" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:21" ht="39">
       <c r="A428" s="2" t="s">
         <v>491</v>
       </c>
@@ -25821,7 +25823,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="429" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:21" ht="48.75">
       <c r="A429" s="2" t="s">
         <v>491</v>
       </c>
@@ -25872,7 +25874,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="430" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:21" ht="39">
       <c r="A430" s="2" t="s">
         <v>491</v>
       </c>
@@ -25923,7 +25925,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="431" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:21" ht="39">
       <c r="A431" s="2" t="s">
         <v>491</v>
       </c>
@@ -25974,7 +25976,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="432" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:21" ht="29.25">
       <c r="A432" s="2" t="s">
         <v>491</v>
       </c>
@@ -26037,7 +26039,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="433" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:21" ht="29.25">
       <c r="A433" s="2" t="s">
         <v>491</v>
       </c>
@@ -26100,7 +26102,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="434" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:21" ht="29.25">
       <c r="A434" s="2" t="s">
         <v>491</v>
       </c>
@@ -26163,7 +26165,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="435" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:21" ht="29.25">
       <c r="A435" s="2" t="s">
         <v>491</v>
       </c>
@@ -26226,7 +26228,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="436" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:21" ht="29.25">
       <c r="A436" s="2" t="s">
         <v>491</v>
       </c>
@@ -26289,7 +26291,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="437" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:21" ht="29.25">
       <c r="A437" s="2" t="s">
         <v>491</v>
       </c>
@@ -26352,7 +26354,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="438" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:21" ht="39">
       <c r="A438" s="2" t="s">
         <v>491</v>
       </c>
@@ -26395,7 +26397,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="439" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:21" ht="39">
       <c r="A439" s="2" t="s">
         <v>491</v>
       </c>
@@ -26438,7 +26440,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="440" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:21" ht="39">
       <c r="A440" s="2" t="s">
         <v>491</v>
       </c>
@@ -26481,7 +26483,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="441" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:21" ht="39">
       <c r="A441" s="2" t="s">
         <v>491</v>
       </c>
@@ -26524,7 +26526,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="442" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:21" ht="39">
       <c r="A442" s="2" t="s">
         <v>491</v>
       </c>
@@ -26567,7 +26569,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="443" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:21" ht="39">
       <c r="A443" s="2" t="s">
         <v>491</v>
       </c>
@@ -26610,7 +26612,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="444" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:21" ht="39">
       <c r="A444" s="2" t="s">
         <v>491</v>
       </c>
@@ -26653,7 +26655,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="445" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:21" ht="39">
       <c r="A445" s="2" t="s">
         <v>491</v>
       </c>
@@ -26696,7 +26698,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="446" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:21" ht="39">
       <c r="A446" s="2" t="s">
         <v>491</v>
       </c>
@@ -26739,7 +26741,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="447" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:21" ht="39">
       <c r="A447" s="2" t="s">
         <v>491</v>
       </c>
@@ -26782,7 +26784,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="448" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:21" ht="39">
       <c r="A448" s="2" t="s">
         <v>491</v>
       </c>
@@ -26825,7 +26827,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="449" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:21" ht="39">
       <c r="A449" s="2" t="s">
         <v>491</v>
       </c>
@@ -26868,7 +26870,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="450" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:21" ht="29.25">
       <c r="A450" s="2" t="s">
         <v>491</v>
       </c>
@@ -26933,7 +26935,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="451" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:21" ht="29.25">
       <c r="A451" s="2" t="s">
         <v>491</v>
       </c>
@@ -26974,7 +26976,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="452" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:21" ht="29.25">
       <c r="A452" s="2" t="s">
         <v>528</v>
       </c>
@@ -27037,7 +27039,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="453" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:21" ht="29.25">
       <c r="A453" s="2" t="s">
         <v>528</v>
       </c>
@@ -27100,7 +27102,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="454" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:21" ht="29.25">
       <c r="A454" s="2" t="s">
         <v>528</v>
       </c>
@@ -27163,7 +27165,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="455" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:21" ht="29.25">
       <c r="A455" s="2" t="s">
         <v>528</v>
       </c>
@@ -27226,7 +27228,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="456" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:21" ht="48.75">
       <c r="A456" s="2" t="s">
         <v>528</v>
       </c>
@@ -27289,7 +27291,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="457" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:21" ht="29.25">
       <c r="A457" s="2" t="s">
         <v>528</v>
       </c>
@@ -27352,7 +27354,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="458" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:21" ht="29.25">
       <c r="A458" s="2" t="s">
         <v>528</v>
       </c>
@@ -27415,7 +27417,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="459" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:21" ht="29.25">
       <c r="A459" s="2" t="s">
         <v>528</v>
       </c>
@@ -27480,7 +27482,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="460" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:21" ht="29.25">
       <c r="A460" s="2" t="s">
         <v>528</v>
       </c>
@@ -27545,7 +27547,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="461" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:21" ht="29.25">
       <c r="A461" s="2" t="s">
         <v>528</v>
       </c>
@@ -27610,7 +27612,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="462" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:21" ht="29.25">
       <c r="A462" s="2" t="s">
         <v>528</v>
       </c>
@@ -27673,7 +27675,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="463" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:21" ht="29.25">
       <c r="A463" s="2" t="s">
         <v>528</v>
       </c>
@@ -27736,7 +27738,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="464" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:21" ht="29.25">
       <c r="A464" s="2" t="s">
         <v>528</v>
       </c>
@@ -27799,7 +27801,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="465" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:21" ht="29.25">
       <c r="A465" s="2" t="s">
         <v>528</v>
       </c>
@@ -27862,7 +27864,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="466" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:21" ht="29.25">
       <c r="A466" s="2" t="s">
         <v>528</v>
       </c>
@@ -27927,7 +27929,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="467" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:21" ht="48.75">
       <c r="A467" s="2" t="s">
         <v>528</v>
       </c>
@@ -27992,7 +27994,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="468" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:21" ht="29.25">
       <c r="A468" s="2" t="s">
         <v>528</v>
       </c>
@@ -28057,7 +28059,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="469" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:21" ht="39">
       <c r="A469" s="2" t="s">
         <v>528</v>
       </c>
@@ -28120,7 +28122,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="470" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:21" ht="39">
       <c r="A470" s="2" t="s">
         <v>528</v>
       </c>
@@ -28183,7 +28185,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="471" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:21" ht="29.25">
       <c r="A471" s="2" t="s">
         <v>528</v>
       </c>
@@ -28234,7 +28236,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="472" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:21" ht="29.25">
       <c r="A472" s="2" t="s">
         <v>528</v>
       </c>
@@ -28299,7 +28301,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="473" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:21" ht="29.25">
       <c r="A473" s="2" t="s">
         <v>528</v>
       </c>
@@ -28364,7 +28366,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="474" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:21" ht="29.25">
       <c r="A474" s="2" t="s">
         <v>528</v>
       </c>
@@ -28421,7 +28423,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="475" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:21" ht="39">
       <c r="A475" s="2" t="s">
         <v>528</v>
       </c>
@@ -28460,7 +28462,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="476" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:21" ht="39">
       <c r="A476" s="2" t="s">
         <v>528</v>
       </c>
@@ -28525,7 +28527,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="477" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:21" ht="39">
       <c r="A477" s="2" t="s">
         <v>528</v>
       </c>
@@ -28590,8 +28592,8 @@
         <v>563</v>
       </c>
     </row>
-    <row r="478" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:21" ht="18" customHeight="1"/>
+    <row r="479" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A479" s="12" t="s">
         <v>566</v>
       </c>

</xml_diff>

<commit_message>
Okno serwisowe 08.04.2025 - aktualizacja plików Excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DregerJ\Documents\SDG\gitowy\sdg-indicators-pl\assets\excel\en\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1723,7 +1723,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 11-03-2025, 11:22</t>
+    <t>Last update: 08-04-2025, 08:10</t>
   </si>
 </sst>
 </file>
@@ -1949,7 +1949,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -1958,48 +1958,25 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1323975</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>1302105</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>457200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Obraz 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2219325" cy="457200"/>
-        </a:xfrm>
+      <xdr:spPr>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2298,7 +2275,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Okno serwisowe 29.04.2025 - aktualizacja EXCEL
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dregerj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1723,7 +1723,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 08-04-2025, 08:10</t>
+    <t>Last update: 29-04-2025, 08:07</t>
   </si>
 </sst>
 </file>
@@ -1738,7 +1738,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2275,10 +2275,10 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2289,17 +2289,17 @@
     <col min="21" max="21" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="36" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="19.5">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="19.5">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="19.5">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="29.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="97.5">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="97.5">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="97.5">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="19.5">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="29.25">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="29.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="29.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="68.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="29.25">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="29.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="29.25">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="39">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="39">
       <c r="A30" s="2" t="s">
         <v>22</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="39">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="39">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="19.5">
       <c r="A33" s="2" t="s">
         <v>68</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="29.25">
       <c r="A34" s="2" t="s">
         <v>68</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="29.25">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="29.25">
       <c r="A36" s="2" t="s">
         <v>68</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="29.25">
       <c r="A37" s="2" t="s">
         <v>68</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="29.25">
       <c r="A38" s="2" t="s">
         <v>68</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="29.25">
       <c r="A39" s="2" t="s">
         <v>68</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="39">
       <c r="A40" s="2" t="s">
         <v>68</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="97.5">
       <c r="A41" s="2" t="s">
         <v>68</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="97.5">
       <c r="A42" s="2" t="s">
         <v>68</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="97.5">
       <c r="A43" s="2" t="s">
         <v>68</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="97.5">
       <c r="A44" s="2" t="s">
         <v>68</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="97.5">
       <c r="A45" s="2" t="s">
         <v>68</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="97.5">
       <c r="A46" s="2" t="s">
         <v>68</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="48.75">
       <c r="A47" s="2" t="s">
         <v>68</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="48.75">
       <c r="A48" s="2" t="s">
         <v>68</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="19.5">
       <c r="A49" s="2" t="s">
         <v>68</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="29.25">
       <c r="A50" s="2" t="s">
         <v>68</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="19.5">
       <c r="A51" s="2" t="s">
         <v>97</v>
       </c>
@@ -5190,13 +5190,15 @@
       <c r="R51" s="4">
         <v>2</v>
       </c>
-      <c r="S51" s="3"/>
+      <c r="S51" s="4">
+        <v>2.6</v>
+      </c>
       <c r="T51" s="3"/>
       <c r="U51" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="19.5">
       <c r="A52" s="2" t="s">
         <v>97</v>
       </c>
@@ -5259,7 +5261,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>97</v>
       </c>
@@ -5322,7 +5324,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>97</v>
       </c>
@@ -5385,7 +5387,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>97</v>
       </c>
@@ -5448,7 +5450,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>97</v>
       </c>
@@ -5511,7 +5513,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>97</v>
       </c>
@@ -5574,7 +5576,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>97</v>
       </c>
@@ -5637,7 +5639,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="29.25">
       <c r="A59" s="2" t="s">
         <v>97</v>
       </c>
@@ -5700,7 +5702,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>97</v>
       </c>
@@ -5763,7 +5765,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="29.25">
       <c r="A61" s="2" t="s">
         <v>97</v>
       </c>
@@ -5821,12 +5823,14 @@
       <c r="S61" s="6">
         <v>46</v>
       </c>
-      <c r="T61" s="3"/>
+      <c r="T61" s="6">
+        <v>43</v>
+      </c>
       <c r="U61" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="29.25">
       <c r="A62" s="2" t="s">
         <v>97</v>
       </c>
@@ -5884,12 +5888,14 @@
       <c r="S62" s="6">
         <v>13</v>
       </c>
-      <c r="T62" s="3"/>
+      <c r="T62" s="6">
+        <v>16</v>
+      </c>
       <c r="U62" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="29.25">
       <c r="A63" s="2" t="s">
         <v>97</v>
       </c>
@@ -5947,12 +5953,14 @@
       <c r="S63" s="6">
         <v>33</v>
       </c>
-      <c r="T63" s="3"/>
+      <c r="T63" s="6">
+        <v>27</v>
+      </c>
       <c r="U63" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="19.5">
       <c r="A64" s="2" t="s">
         <v>97</v>
       </c>
@@ -6007,13 +6015,15 @@
       <c r="R64" s="4">
         <v>6.6</v>
       </c>
-      <c r="S64" s="3"/>
+      <c r="S64" s="4">
+        <v>8.3000000000000007</v>
+      </c>
       <c r="T64" s="3"/>
       <c r="U64" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" ht="29.25">
       <c r="A65" s="2" t="s">
         <v>97</v>
       </c>
@@ -6069,14 +6079,16 @@
         <v>69</v>
       </c>
       <c r="S65" s="6">
-        <v>140</v>
-      </c>
-      <c r="T65" s="3"/>
+        <v>138</v>
+      </c>
+      <c r="T65" s="6">
+        <v>200</v>
+      </c>
       <c r="U65" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="29.25">
       <c r="A66" s="2" t="s">
         <v>97</v>
       </c>
@@ -6132,14 +6144,16 @@
         <v>36</v>
       </c>
       <c r="S66" s="6">
-        <v>68</v>
-      </c>
-      <c r="T66" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="T66" s="6">
+        <v>102</v>
+      </c>
       <c r="U66" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="29.25">
       <c r="A67" s="2" t="s">
         <v>97</v>
       </c>
@@ -6195,14 +6209,16 @@
         <v>33</v>
       </c>
       <c r="S67" s="6">
-        <v>72</v>
-      </c>
-      <c r="T67" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="T67" s="6">
+        <v>98</v>
+      </c>
       <c r="U67" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="29.25">
       <c r="A68" s="2" t="s">
         <v>97</v>
       </c>
@@ -6257,13 +6273,15 @@
       <c r="R68" s="4">
         <v>426.2</v>
       </c>
-      <c r="S68" s="3"/>
+      <c r="S68" s="4">
+        <v>400.4</v>
+      </c>
       <c r="T68" s="3"/>
       <c r="U68" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="29.25">
       <c r="A69" s="2" t="s">
         <v>97</v>
       </c>
@@ -6318,13 +6336,15 @@
       <c r="R69" s="4">
         <v>28.8</v>
       </c>
-      <c r="S69" s="3"/>
+      <c r="S69" s="4">
+        <v>25.7</v>
+      </c>
       <c r="T69" s="3"/>
       <c r="U69" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="29.25">
       <c r="A70" s="2" t="s">
         <v>97</v>
       </c>
@@ -6379,13 +6399,15 @@
       <c r="R70" s="4">
         <v>253.9</v>
       </c>
-      <c r="S70" s="3"/>
+      <c r="S70" s="4">
+        <v>264.39999999999998</v>
+      </c>
       <c r="T70" s="3"/>
       <c r="U70" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" ht="29.25">
       <c r="A71" s="2" t="s">
         <v>97</v>
       </c>
@@ -6440,13 +6462,15 @@
       <c r="R71" s="4">
         <v>24.6</v>
       </c>
-      <c r="S71" s="3"/>
+      <c r="S71" s="4">
+        <v>25.7</v>
+      </c>
       <c r="T71" s="3"/>
       <c r="U71" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" ht="19.5">
       <c r="A72" s="2" t="s">
         <v>97</v>
       </c>
@@ -6499,15 +6523,17 @@
         <v>12.1</v>
       </c>
       <c r="R72" s="4">
-        <v>11.9</v>
-      </c>
-      <c r="S72" s="3"/>
+        <v>11.7</v>
+      </c>
+      <c r="S72" s="4">
+        <v>12.1</v>
+      </c>
       <c r="T72" s="3"/>
       <c r="U72" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" ht="19.5">
       <c r="A73" s="2" t="s">
         <v>97</v>
       </c>
@@ -6524,7 +6550,7 @@
         <v>49</v>
       </c>
       <c r="F73" s="4">
-        <v>29.5</v>
+        <v>29.6</v>
       </c>
       <c r="G73" s="4">
         <v>28.7</v>
@@ -6562,13 +6588,15 @@
       <c r="R73" s="4">
         <v>20.5</v>
       </c>
-      <c r="S73" s="3"/>
+      <c r="S73" s="4">
+        <v>21.4</v>
+      </c>
       <c r="T73" s="3"/>
       <c r="U73" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="19.5">
       <c r="A74" s="2" t="s">
         <v>97</v>
       </c>
@@ -6623,13 +6651,15 @@
       <c r="R74" s="4">
         <v>3.4</v>
       </c>
-      <c r="S74" s="3"/>
+      <c r="S74" s="4">
+        <v>3.4</v>
+      </c>
       <c r="T74" s="3"/>
       <c r="U74" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" ht="19.5">
       <c r="A75" s="2" t="s">
         <v>97</v>
       </c>
@@ -6692,7 +6722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" ht="29.25">
       <c r="A76" s="2" t="s">
         <v>97</v>
       </c>
@@ -6755,7 +6785,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="77" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="29.25">
       <c r="A77" s="2" t="s">
         <v>97</v>
       </c>
@@ -6796,7 +6826,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" ht="19.5">
       <c r="A78" s="2" t="s">
         <v>97</v>
       </c>
@@ -6859,7 +6889,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" ht="19.5">
       <c r="A79" s="2" t="s">
         <v>97</v>
       </c>
@@ -6922,7 +6952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" ht="19.5">
       <c r="A80" s="2" t="s">
         <v>97</v>
       </c>
@@ -6985,7 +7015,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" ht="19.5">
       <c r="A81" s="2" t="s">
         <v>97</v>
       </c>
@@ -7030,7 +7060,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" ht="29.25">
       <c r="A82" s="2" t="s">
         <v>97</v>
       </c>
@@ -7089,7 +7119,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" ht="29.25">
       <c r="A83" s="2" t="s">
         <v>97</v>
       </c>
@@ -7148,7 +7178,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="84" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" ht="19.5">
       <c r="A84" s="2" t="s">
         <v>97</v>
       </c>
@@ -7185,7 +7215,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" ht="29.25">
       <c r="A85" s="2" t="s">
         <v>97</v>
       </c>
@@ -7222,7 +7252,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="86" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" ht="19.5">
       <c r="A86" s="2" t="s">
         <v>97</v>
       </c>
@@ -7277,13 +7307,15 @@
       <c r="R86" s="4">
         <v>1.2</v>
       </c>
-      <c r="S86" s="3"/>
+      <c r="S86" s="4">
+        <v>1.2</v>
+      </c>
       <c r="T86" s="3"/>
       <c r="U86" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" ht="19.5">
       <c r="A87" s="2" t="s">
         <v>97</v>
       </c>
@@ -7324,7 +7356,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" ht="19.5">
       <c r="A88" s="2" t="s">
         <v>97</v>
       </c>
@@ -7387,7 +7419,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="89" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" ht="19.5">
       <c r="A89" s="2" t="s">
         <v>97</v>
       </c>
@@ -7450,7 +7482,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="90" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" ht="19.5">
       <c r="A90" s="2" t="s">
         <v>97</v>
       </c>
@@ -7497,7 +7529,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="91" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" ht="29.25">
       <c r="A91" s="2" t="s">
         <v>97</v>
       </c>
@@ -7554,7 +7586,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" ht="19.5">
       <c r="A92" s="2" t="s">
         <v>97</v>
       </c>
@@ -7599,7 +7631,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" ht="19.5">
       <c r="A93" s="2" t="s">
         <v>97</v>
       </c>
@@ -7644,7 +7676,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" ht="19.5">
       <c r="A94" s="2" t="s">
         <v>97</v>
       </c>
@@ -7689,7 +7721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" ht="19.5">
       <c r="A95" s="2" t="s">
         <v>97</v>
       </c>
@@ -7748,7 +7780,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" ht="78">
       <c r="A96" s="2" t="s">
         <v>151</v>
       </c>
@@ -7789,7 +7821,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" ht="78">
       <c r="A97" s="2" t="s">
         <v>151</v>
       </c>
@@ -7830,7 +7862,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="98" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" ht="78">
       <c r="A98" s="2" t="s">
         <v>151</v>
       </c>
@@ -7871,7 +7903,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="99" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" ht="78">
       <c r="A99" s="2" t="s">
         <v>151</v>
       </c>
@@ -7916,7 +7948,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="100" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" ht="78">
       <c r="A100" s="2" t="s">
         <v>151</v>
       </c>
@@ -7961,7 +7993,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" ht="78">
       <c r="A101" s="2" t="s">
         <v>151</v>
       </c>
@@ -8006,7 +8038,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" ht="78">
       <c r="A102" s="2" t="s">
         <v>151</v>
       </c>
@@ -8051,7 +8083,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="103" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" ht="78">
       <c r="A103" s="2" t="s">
         <v>151</v>
       </c>
@@ -8096,7 +8128,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" ht="78">
       <c r="A104" s="2" t="s">
         <v>151</v>
       </c>
@@ -8141,7 +8173,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" ht="29.25">
       <c r="A105" s="2" t="s">
         <v>151</v>
       </c>
@@ -8180,7 +8212,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="106" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" ht="19.5">
       <c r="A106" s="2" t="s">
         <v>151</v>
       </c>
@@ -8243,7 +8275,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" ht="19.5">
       <c r="A107" s="2" t="s">
         <v>151</v>
       </c>
@@ -8306,7 +8338,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" ht="19.5">
       <c r="A108" s="2" t="s">
         <v>151</v>
       </c>
@@ -8369,7 +8401,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" ht="19.5">
       <c r="A109" s="2" t="s">
         <v>151</v>
       </c>
@@ -8408,7 +8440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" ht="19.5">
       <c r="A110" s="2" t="s">
         <v>151</v>
       </c>
@@ -8447,7 +8479,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="111" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" ht="19.5">
       <c r="A111" s="2" t="s">
         <v>151</v>
       </c>
@@ -8486,7 +8518,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" ht="29.25">
       <c r="A112" s="2" t="s">
         <v>151</v>
       </c>
@@ -8533,7 +8565,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" ht="19.5">
       <c r="A113" s="2" t="s">
         <v>151</v>
       </c>
@@ -8588,7 +8620,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" ht="39">
       <c r="A114" s="2" t="s">
         <v>151</v>
       </c>
@@ -8643,7 +8675,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" ht="48.75">
       <c r="A115" s="2" t="s">
         <v>151</v>
       </c>
@@ -8698,7 +8730,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" ht="58.5">
       <c r="A116" s="2" t="s">
         <v>151</v>
       </c>
@@ -8753,7 +8785,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="117" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" ht="29.25">
       <c r="A117" s="2" t="s">
         <v>151</v>
       </c>
@@ -8808,7 +8840,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="118" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" ht="29.25">
       <c r="A118" s="2" t="s">
         <v>151</v>
       </c>
@@ -8855,7 +8887,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" ht="19.5">
       <c r="A119" s="2" t="s">
         <v>151</v>
       </c>
@@ -8910,7 +8942,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" ht="39">
       <c r="A120" s="2" t="s">
         <v>151</v>
       </c>
@@ -8965,7 +8997,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" ht="48.75">
       <c r="A121" s="2" t="s">
         <v>151</v>
       </c>
@@ -9020,7 +9052,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="122" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" ht="58.5">
       <c r="A122" s="2" t="s">
         <v>151</v>
       </c>
@@ -9075,7 +9107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="123" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" ht="29.25">
       <c r="A123" s="2" t="s">
         <v>151</v>
       </c>
@@ -9130,7 +9162,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="124" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" ht="48.75">
       <c r="A124" s="2" t="s">
         <v>151</v>
       </c>
@@ -9173,7 +9205,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="125" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:21" ht="48.75">
       <c r="A125" s="2" t="s">
         <v>151</v>
       </c>
@@ -9216,7 +9248,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="126" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:21" ht="29.25">
       <c r="A126" s="2" t="s">
         <v>151</v>
       </c>
@@ -9277,7 +9309,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="127" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:21" ht="29.25">
       <c r="A127" s="2" t="s">
         <v>151</v>
       </c>
@@ -9314,7 +9346,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:21" ht="29.25">
       <c r="A128" s="2" t="s">
         <v>151</v>
       </c>
@@ -9351,7 +9383,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="129" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:21" ht="29.25">
       <c r="A129" s="2" t="s">
         <v>151</v>
       </c>
@@ -9388,7 +9420,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:21" ht="29.25">
       <c r="A130" s="2" t="s">
         <v>151</v>
       </c>
@@ -9425,7 +9457,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="131" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:21" ht="29.25">
       <c r="A131" s="2" t="s">
         <v>151</v>
       </c>
@@ -9462,7 +9494,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="132" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:21" ht="29.25">
       <c r="A132" s="2" t="s">
         <v>151</v>
       </c>
@@ -9499,7 +9531,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="133" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:21" ht="29.25">
       <c r="A133" s="2" t="s">
         <v>151</v>
       </c>
@@ -9536,7 +9568,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="134" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:21" ht="29.25">
       <c r="A134" s="2" t="s">
         <v>151</v>
       </c>
@@ -9573,7 +9605,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="135" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:21" ht="29.25">
       <c r="A135" s="2" t="s">
         <v>151</v>
       </c>
@@ -9610,7 +9642,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="136" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:21" ht="29.25">
       <c r="A136" s="2" t="s">
         <v>151</v>
       </c>
@@ -9647,7 +9679,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="137" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:21" ht="29.25">
       <c r="A137" s="2" t="s">
         <v>151</v>
       </c>
@@ -9684,7 +9716,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="138" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:21" ht="29.25">
       <c r="A138" s="2" t="s">
         <v>151</v>
       </c>
@@ -9721,7 +9753,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="139" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:21" ht="29.25">
       <c r="A139" s="2" t="s">
         <v>151</v>
       </c>
@@ -9758,7 +9790,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="140" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:21" ht="29.25">
       <c r="A140" s="2" t="s">
         <v>151</v>
       </c>
@@ -9795,7 +9827,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="141" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:21" ht="29.25">
       <c r="A141" s="2" t="s">
         <v>151</v>
       </c>
@@ -9832,7 +9864,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="142" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:21" ht="29.25">
       <c r="A142" s="2" t="s">
         <v>151</v>
       </c>
@@ -9869,7 +9901,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="143" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:21" ht="48.75">
       <c r="A143" s="2" t="s">
         <v>151</v>
       </c>
@@ -9934,7 +9966,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="144" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:21" ht="58.5">
       <c r="A144" s="2" t="s">
         <v>151</v>
       </c>
@@ -9999,7 +10031,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:21" ht="58.5">
       <c r="A145" s="2" t="s">
         <v>151</v>
       </c>
@@ -10036,7 +10068,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="146" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:21" ht="58.5">
       <c r="A146" s="2" t="s">
         <v>151</v>
       </c>
@@ -10073,7 +10105,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="147" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:21" ht="58.5">
       <c r="A147" s="2" t="s">
         <v>151</v>
       </c>
@@ -10138,7 +10170,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="148" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:21" ht="58.5">
       <c r="A148" s="2" t="s">
         <v>151</v>
       </c>
@@ -10203,7 +10235,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="149" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:21" ht="58.5">
       <c r="A149" s="2" t="s">
         <v>151</v>
       </c>
@@ -10268,7 +10300,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="150" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:21" ht="29.25">
       <c r="A150" s="2" t="s">
         <v>151</v>
       </c>
@@ -10325,7 +10357,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="151" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" ht="58.5">
       <c r="A151" s="2" t="s">
         <v>151</v>
       </c>
@@ -10382,7 +10414,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="152" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:21" ht="58.5">
       <c r="A152" s="2" t="s">
         <v>151</v>
       </c>
@@ -10439,7 +10471,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="153" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:21" ht="58.5">
       <c r="A153" s="2" t="s">
         <v>151</v>
       </c>
@@ -10496,7 +10528,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="154" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:21" ht="58.5">
       <c r="A154" s="2" t="s">
         <v>151</v>
       </c>
@@ -10553,7 +10585,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="155" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:21" ht="29.25">
       <c r="A155" s="2" t="s">
         <v>207</v>
       </c>
@@ -10590,7 +10622,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="156" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:21" ht="19.5">
       <c r="A156" s="2" t="s">
         <v>207</v>
       </c>
@@ -10651,7 +10683,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="157" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:21" ht="39">
       <c r="A157" s="2" t="s">
         <v>207</v>
       </c>
@@ -10690,7 +10722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="158" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:21" ht="39">
       <c r="A158" s="2" t="s">
         <v>207</v>
       </c>
@@ -10729,7 +10761,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="159" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:21" ht="39">
       <c r="A159" s="2" t="s">
         <v>207</v>
       </c>
@@ -10768,7 +10800,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="160" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:21" ht="39">
       <c r="A160" s="2" t="s">
         <v>207</v>
       </c>
@@ -10807,7 +10839,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="161" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" ht="39">
       <c r="A161" s="2" t="s">
         <v>207</v>
       </c>
@@ -10846,7 +10878,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="162" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:21" ht="19.5">
       <c r="A162" s="2" t="s">
         <v>207</v>
       </c>
@@ -10885,7 +10917,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="163" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:21" ht="19.5">
       <c r="A163" s="2" t="s">
         <v>207</v>
       </c>
@@ -10924,7 +10956,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="164" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:21" ht="19.5">
       <c r="A164" s="2" t="s">
         <v>207</v>
       </c>
@@ -10963,7 +10995,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="165" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:21" ht="19.5">
       <c r="A165" s="2" t="s">
         <v>207</v>
       </c>
@@ -11002,7 +11034,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="166" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:21" ht="19.5">
       <c r="A166" s="2" t="s">
         <v>207</v>
       </c>
@@ -11041,7 +11073,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="167" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:21" ht="19.5">
       <c r="A167" s="2" t="s">
         <v>207</v>
       </c>
@@ -11080,7 +11112,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="168" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:21" ht="19.5">
       <c r="A168" s="2" t="s">
         <v>207</v>
       </c>
@@ -11119,7 +11151,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="169" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:21" ht="19.5">
       <c r="A169" s="2" t="s">
         <v>207</v>
       </c>
@@ -11158,7 +11190,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="170" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:21" ht="29.25">
       <c r="A170" s="2" t="s">
         <v>207</v>
       </c>
@@ -11201,7 +11233,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="171" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:21" ht="29.25">
       <c r="A171" s="2" t="s">
         <v>207</v>
       </c>
@@ -11244,7 +11276,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="172" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:21" ht="29.25">
       <c r="A172" s="2" t="s">
         <v>207</v>
       </c>
@@ -11307,7 +11339,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="173" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:21" ht="29.25">
       <c r="A173" s="2" t="s">
         <v>207</v>
       </c>
@@ -11370,7 +11402,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="174" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:21" ht="29.25">
       <c r="A174" s="2" t="s">
         <v>207</v>
       </c>
@@ -11433,7 +11465,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="175" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:21" ht="29.25">
       <c r="A175" s="2" t="s">
         <v>207</v>
       </c>
@@ -11496,7 +11528,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="176" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:21" ht="29.25">
       <c r="A176" s="2" t="s">
         <v>207</v>
       </c>
@@ -11559,7 +11591,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="177" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:21" ht="19.5">
       <c r="A177" s="2" t="s">
         <v>207</v>
       </c>
@@ -11608,7 +11640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="178" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:21" ht="39">
       <c r="A178" s="2" t="s">
         <v>207</v>
       </c>
@@ -11657,7 +11689,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="179" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:21" ht="19.5">
       <c r="A179" s="2" t="s">
         <v>207</v>
       </c>
@@ -11706,7 +11738,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="180" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:21" ht="39">
       <c r="A180" s="2" t="s">
         <v>207</v>
       </c>
@@ -11755,7 +11787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="181" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:21" ht="39">
       <c r="A181" s="2" t="s">
         <v>207</v>
       </c>
@@ -11804,7 +11836,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="182" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:21" ht="39">
       <c r="A182" s="2" t="s">
         <v>207</v>
       </c>
@@ -11853,7 +11885,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="183" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:21" ht="39">
       <c r="A183" s="2" t="s">
         <v>207</v>
       </c>
@@ -11902,7 +11934,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="184" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:21" ht="39">
       <c r="A184" s="2" t="s">
         <v>207</v>
       </c>
@@ -11943,7 +11975,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="185" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:21" ht="39">
       <c r="A185" s="2" t="s">
         <v>207</v>
       </c>
@@ -11984,7 +12016,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="186" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:21" ht="39">
       <c r="A186" s="2" t="s">
         <v>207</v>
       </c>
@@ -12025,7 +12057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="187" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:21" ht="39">
       <c r="A187" s="2" t="s">
         <v>207</v>
       </c>
@@ -12066,7 +12098,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="188" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:21" ht="39">
       <c r="A188" s="2" t="s">
         <v>207</v>
       </c>
@@ -12107,7 +12139,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="189" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:21" ht="39">
       <c r="A189" s="2" t="s">
         <v>207</v>
       </c>
@@ -12148,7 +12180,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="190" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:21" ht="39">
       <c r="A190" s="2" t="s">
         <v>207</v>
       </c>
@@ -12189,7 +12221,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="191" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:21" ht="39">
       <c r="A191" s="2" t="s">
         <v>207</v>
       </c>
@@ -12230,7 +12262,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="192" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:21" ht="39">
       <c r="A192" s="2" t="s">
         <v>207</v>
       </c>
@@ -12271,7 +12303,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="193" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:21" ht="39">
       <c r="A193" s="2" t="s">
         <v>207</v>
       </c>
@@ -12312,7 +12344,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="194" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:21" ht="39">
       <c r="A194" s="2" t="s">
         <v>207</v>
       </c>
@@ -12353,7 +12385,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="195" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:21" ht="39">
       <c r="A195" s="2" t="s">
         <v>207</v>
       </c>
@@ -12394,7 +12426,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="196" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:21" ht="19.5">
       <c r="A196" s="2" t="s">
         <v>207</v>
       </c>
@@ -12437,7 +12469,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="197" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:21" ht="19.5">
       <c r="A197" s="2" t="s">
         <v>207</v>
       </c>
@@ -12496,7 +12528,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="198" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:21" ht="19.5">
       <c r="A198" s="2" t="s">
         <v>207</v>
       </c>
@@ -12555,7 +12587,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="199" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:21" ht="19.5">
       <c r="A199" s="2" t="s">
         <v>247</v>
       </c>
@@ -12614,7 +12646,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="200" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:21" ht="29.25">
       <c r="A200" s="2" t="s">
         <v>247</v>
       </c>
@@ -12673,7 +12705,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="201" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:21" ht="19.5">
       <c r="A201" s="2" t="s">
         <v>247</v>
       </c>
@@ -12736,7 +12768,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="202" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:21" ht="19.5">
       <c r="A202" s="2" t="s">
         <v>247</v>
       </c>
@@ -12775,7 +12807,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="203" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:21" ht="19.5">
       <c r="A203" s="2" t="s">
         <v>247</v>
       </c>
@@ -12814,7 +12846,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="204" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:21" ht="29.25">
       <c r="A204" s="2" t="s">
         <v>247</v>
       </c>
@@ -12875,7 +12907,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="205" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:21" ht="19.5">
       <c r="A205" s="2" t="s">
         <v>247</v>
       </c>
@@ -12936,7 +12968,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="206" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:21" ht="19.5">
       <c r="A206" s="2" t="s">
         <v>247</v>
       </c>
@@ -12983,7 +13015,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="207" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:21" ht="29.25">
       <c r="A207" s="2" t="s">
         <v>247</v>
       </c>
@@ -13044,7 +13076,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="208" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:21" ht="29.25">
       <c r="A208" s="2" t="s">
         <v>247</v>
       </c>
@@ -13101,7 +13133,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="209" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:21" ht="39">
       <c r="A209" s="2" t="s">
         <v>247</v>
       </c>
@@ -13164,7 +13196,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="210" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:21" ht="19.5">
       <c r="A210" s="2" t="s">
         <v>268</v>
       </c>
@@ -13201,7 +13233,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="211" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:21" ht="19.5">
       <c r="A211" s="2" t="s">
         <v>268</v>
       </c>
@@ -13264,7 +13296,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="212" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:21" ht="29.25">
       <c r="A212" s="2" t="s">
         <v>268</v>
       </c>
@@ -13321,7 +13353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="213" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:21" ht="29.25">
       <c r="A213" s="2" t="s">
         <v>268</v>
       </c>
@@ -13378,7 +13410,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="214" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:21" ht="29.25">
       <c r="A214" s="2" t="s">
         <v>275</v>
       </c>
@@ -13395,10 +13427,10 @@
         <v>26</v>
       </c>
       <c r="F214" s="4">
-        <v>2.2000000000000002</v>
+        <v>3.1</v>
       </c>
       <c r="G214" s="4">
-        <v>6.5</v>
+        <v>5.2</v>
       </c>
       <c r="H214" s="4">
         <v>1.5</v>
@@ -13428,7 +13460,7 @@
         <v>-2</v>
       </c>
       <c r="Q214" s="4">
-        <v>9.6999999999999993</v>
+        <v>7.5</v>
       </c>
       <c r="R214" s="4">
         <v>3</v>
@@ -13436,12 +13468,14 @@
       <c r="S214" s="4">
         <v>0.6</v>
       </c>
-      <c r="T214" s="3"/>
+      <c r="T214" s="4">
+        <v>3.3</v>
+      </c>
       <c r="U214" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="215" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:21" ht="29.25">
       <c r="A215" s="2" t="s">
         <v>275</v>
       </c>
@@ -13504,7 +13538,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="216" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:21" ht="29.25">
       <c r="A216" s="2" t="s">
         <v>275</v>
       </c>
@@ -13547,7 +13581,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="217" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:21" ht="29.25">
       <c r="A217" s="2" t="s">
         <v>275</v>
       </c>
@@ -13590,7 +13624,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="218" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:21" ht="29.25">
       <c r="A218" s="2" t="s">
         <v>275</v>
       </c>
@@ -13633,7 +13667,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:21" ht="29.25">
       <c r="A219" s="2" t="s">
         <v>275</v>
       </c>
@@ -13696,7 +13730,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="220" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:21" ht="29.25">
       <c r="A220" s="2" t="s">
         <v>275</v>
       </c>
@@ -13759,7 +13793,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="221" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:21" ht="29.25">
       <c r="A221" s="2" t="s">
         <v>275</v>
       </c>
@@ -13822,7 +13856,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="222" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:21" ht="29.25">
       <c r="A222" s="2" t="s">
         <v>275</v>
       </c>
@@ -13871,7 +13905,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="223" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:21" ht="29.25">
       <c r="A223" s="2" t="s">
         <v>275</v>
       </c>
@@ -13920,7 +13954,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="224" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:21" ht="29.25">
       <c r="A224" s="2" t="s">
         <v>275</v>
       </c>
@@ -13969,7 +14003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="225" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:21" ht="29.25">
       <c r="A225" s="2" t="s">
         <v>275</v>
       </c>
@@ -14018,7 +14052,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="226" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:21" ht="29.25">
       <c r="A226" s="2" t="s">
         <v>275</v>
       </c>
@@ -14067,7 +14101,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="227" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:21" ht="29.25">
       <c r="A227" s="2" t="s">
         <v>275</v>
       </c>
@@ -14116,7 +14150,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="228" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:21" ht="29.25">
       <c r="A228" s="2" t="s">
         <v>275</v>
       </c>
@@ -14165,7 +14199,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="229" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:21" ht="29.25">
       <c r="A229" s="2" t="s">
         <v>275</v>
       </c>
@@ -14214,7 +14248,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="230" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:21" ht="39">
       <c r="A230" s="2" t="s">
         <v>275</v>
       </c>
@@ -14263,7 +14297,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="231" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:21" ht="29.25">
       <c r="A231" s="2" t="s">
         <v>275</v>
       </c>
@@ -14312,7 +14346,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="232" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:21" ht="39">
       <c r="A232" s="2" t="s">
         <v>275</v>
       </c>
@@ -14361,7 +14395,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="233" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:21" ht="29.25">
       <c r="A233" s="2" t="s">
         <v>275</v>
       </c>
@@ -14410,7 +14444,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="234" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:21" ht="29.25">
       <c r="A234" s="2" t="s">
         <v>275</v>
       </c>
@@ -14459,7 +14493,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="235" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:21" ht="29.25">
       <c r="A235" s="2" t="s">
         <v>275</v>
       </c>
@@ -14508,7 +14542,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="236" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:21" ht="29.25">
       <c r="A236" s="2" t="s">
         <v>275</v>
       </c>
@@ -14557,7 +14591,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="237" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:21" ht="29.25">
       <c r="A237" s="2" t="s">
         <v>275</v>
       </c>
@@ -14606,7 +14640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="238" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:21" ht="29.25">
       <c r="A238" s="2" t="s">
         <v>275</v>
       </c>
@@ -14655,7 +14689,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="239" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:21" ht="29.25">
       <c r="A239" s="2" t="s">
         <v>275</v>
       </c>
@@ -14704,7 +14738,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="240" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:21" ht="29.25">
       <c r="A240" s="2" t="s">
         <v>275</v>
       </c>
@@ -14753,7 +14787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="241" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:21" ht="29.25">
       <c r="A241" s="2" t="s">
         <v>275</v>
       </c>
@@ -14816,7 +14850,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="242" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:21" ht="29.25">
       <c r="A242" s="2" t="s">
         <v>275</v>
       </c>
@@ -14879,7 +14913,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="243" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:21" ht="29.25">
       <c r="A243" s="2" t="s">
         <v>275</v>
       </c>
@@ -14942,7 +14976,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="244" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:21" ht="29.25">
       <c r="A244" s="2" t="s">
         <v>275</v>
       </c>
@@ -15005,7 +15039,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="245" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:21" ht="29.25">
       <c r="A245" s="2" t="s">
         <v>275</v>
       </c>
@@ -15068,7 +15102,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="246" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:21" ht="29.25">
       <c r="A246" s="2" t="s">
         <v>275</v>
       </c>
@@ -15131,7 +15165,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="247" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:21" ht="29.25">
       <c r="A247" s="2" t="s">
         <v>275</v>
       </c>
@@ -15194,7 +15228,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="248" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:21" ht="29.25">
       <c r="A248" s="2" t="s">
         <v>275</v>
       </c>
@@ -15257,7 +15291,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="249" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:21" ht="29.25">
       <c r="A249" s="2" t="s">
         <v>275</v>
       </c>
@@ -15320,7 +15354,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="250" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:21" ht="29.25">
       <c r="A250" s="2" t="s">
         <v>275</v>
       </c>
@@ -15383,7 +15417,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="251" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:21" ht="29.25">
       <c r="A251" s="2" t="s">
         <v>275</v>
       </c>
@@ -15446,7 +15480,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="252" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:21" ht="29.25">
       <c r="A252" s="2" t="s">
         <v>275</v>
       </c>
@@ -15509,7 +15543,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="253" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:21" ht="39">
       <c r="A253" s="2" t="s">
         <v>275</v>
       </c>
@@ -15552,7 +15586,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="254" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:21" ht="39">
       <c r="A254" s="2" t="s">
         <v>275</v>
       </c>
@@ -15595,7 +15629,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="255" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:21" ht="39">
       <c r="A255" s="2" t="s">
         <v>275</v>
       </c>
@@ -15638,7 +15672,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="256" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:21" ht="29.25">
       <c r="A256" s="2" t="s">
         <v>275</v>
       </c>
@@ -15694,14 +15728,14 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="S256" s="5">
-        <v>0.09</v>
+        <v>0.03</v>
       </c>
       <c r="T256" s="3"/>
       <c r="U256" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="257" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:21" ht="48.75">
       <c r="A257" s="2" t="s">
         <v>275</v>
       </c>
@@ -15760,7 +15794,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="258" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:21" ht="29.25">
       <c r="A258" s="2" t="s">
         <v>275</v>
       </c>
@@ -15797,7 +15831,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="259" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:21" ht="29.25">
       <c r="A259" s="2" t="s">
         <v>275</v>
       </c>
@@ -15834,7 +15868,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="260" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:21" ht="29.25">
       <c r="A260" s="2" t="s">
         <v>275</v>
       </c>
@@ -15871,7 +15905,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="261" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:21" ht="29.25">
       <c r="A261" s="2" t="s">
         <v>275</v>
       </c>
@@ -15908,7 +15942,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="262" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:21" ht="29.25">
       <c r="A262" s="2" t="s">
         <v>275</v>
       </c>
@@ -15945,7 +15979,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="263" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:21" ht="29.25">
       <c r="A263" s="2" t="s">
         <v>275</v>
       </c>
@@ -15982,7 +16016,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="264" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:21" ht="29.25">
       <c r="A264" s="2" t="s">
         <v>275</v>
       </c>
@@ -16019,7 +16053,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="265" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:21" ht="29.25">
       <c r="A265" s="2" t="s">
         <v>275</v>
       </c>
@@ -16056,7 +16090,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="266" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:21" ht="29.25">
       <c r="A266" s="2" t="s">
         <v>275</v>
       </c>
@@ -16109,7 +16143,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="267" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:21" ht="29.25">
       <c r="A267" s="2" t="s">
         <v>320</v>
       </c>
@@ -16172,7 +16206,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="268" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:21" ht="29.25">
       <c r="A268" s="2" t="s">
         <v>320</v>
       </c>
@@ -16235,7 +16269,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="269" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:21" ht="29.25">
       <c r="A269" s="2" t="s">
         <v>320</v>
       </c>
@@ -16298,7 +16332,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="270" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:21" ht="29.25">
       <c r="A270" s="2" t="s">
         <v>320</v>
       </c>
@@ -16361,7 +16395,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="271" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:21" ht="29.25">
       <c r="A271" s="2" t="s">
         <v>320</v>
       </c>
@@ -16424,7 +16458,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="272" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:21" ht="29.25">
       <c r="A272" s="2" t="s">
         <v>320</v>
       </c>
@@ -16487,7 +16521,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="273" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:21" ht="29.25">
       <c r="A273" s="2" t="s">
         <v>320</v>
       </c>
@@ -16550,7 +16584,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="274" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:21" ht="29.25">
       <c r="A274" s="2" t="s">
         <v>320</v>
       </c>
@@ -16613,7 +16647,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="275" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:21" ht="29.25">
       <c r="A275" s="2" t="s">
         <v>320</v>
       </c>
@@ -16676,7 +16710,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="276" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:21" ht="29.25">
       <c r="A276" s="2" t="s">
         <v>320</v>
       </c>
@@ -16739,7 +16773,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="277" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:21" ht="29.25">
       <c r="A277" s="2" t="s">
         <v>320</v>
       </c>
@@ -16802,7 +16836,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="278" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:21" ht="29.25">
       <c r="A278" s="2" t="s">
         <v>320</v>
       </c>
@@ -16858,14 +16892,16 @@
         <v>17.7</v>
       </c>
       <c r="S278" s="4">
-        <v>16.8</v>
-      </c>
-      <c r="T278" s="3"/>
+        <v>17.5</v>
+      </c>
+      <c r="T278" s="4">
+        <v>15.4</v>
+      </c>
       <c r="U278" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="279" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:21" ht="29.25">
       <c r="A279" s="2" t="s">
         <v>320</v>
       </c>
@@ -16928,7 +16964,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="280" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:21" ht="29.25">
       <c r="A280" s="2" t="s">
         <v>320</v>
       </c>
@@ -16991,7 +17027,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="281" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:21" ht="29.25">
       <c r="A281" s="2" t="s">
         <v>320</v>
       </c>
@@ -17054,7 +17090,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="282" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:21" ht="29.25">
       <c r="A282" s="2" t="s">
         <v>320</v>
       </c>
@@ -17117,7 +17153,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="283" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:21" ht="29.25">
       <c r="A283" s="2" t="s">
         <v>320</v>
       </c>
@@ -17180,7 +17216,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="284" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:21" ht="29.25">
       <c r="A284" s="2" t="s">
         <v>320</v>
       </c>
@@ -17243,7 +17279,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="285" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:21" ht="29.25">
       <c r="A285" s="2" t="s">
         <v>320</v>
       </c>
@@ -17306,7 +17342,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="286" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:21" ht="29.25">
       <c r="A286" s="2" t="s">
         <v>320</v>
       </c>
@@ -17369,7 +17405,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="287" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:21" ht="29.25">
       <c r="A287" s="2" t="s">
         <v>320</v>
       </c>
@@ -17422,7 +17458,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="288" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:21" ht="29.25">
       <c r="A288" s="2" t="s">
         <v>320</v>
       </c>
@@ -17485,7 +17521,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="289" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:21" ht="29.25">
       <c r="A289" s="2" t="s">
         <v>320</v>
       </c>
@@ -17548,7 +17584,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="290" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:21" ht="29.25">
       <c r="A290" s="2" t="s">
         <v>320</v>
       </c>
@@ -17605,7 +17641,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="291" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:21" ht="29.25">
       <c r="A291" s="2" t="s">
         <v>320</v>
       </c>
@@ -17660,7 +17696,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="292" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:21" ht="39">
       <c r="A292" s="2" t="s">
         <v>320</v>
       </c>
@@ -17713,7 +17749,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="293" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:21" ht="39">
       <c r="A293" s="2" t="s">
         <v>320</v>
       </c>
@@ -17768,7 +17804,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="294" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:21" ht="19.5">
       <c r="A294" s="2" t="s">
         <v>352</v>
       </c>
@@ -17831,7 +17867,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="295" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:21" ht="68.25">
       <c r="A295" s="2" t="s">
         <v>352</v>
       </c>
@@ -17894,7 +17930,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="296" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:21" ht="19.5">
       <c r="A296" s="2" t="s">
         <v>352</v>
       </c>
@@ -17957,7 +17993,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="297" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:21" ht="19.5">
       <c r="A297" s="2" t="s">
         <v>352</v>
       </c>
@@ -18020,7 +18056,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="298" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:21" ht="19.5">
       <c r="A298" s="2" t="s">
         <v>352</v>
       </c>
@@ -18083,7 +18119,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="299" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:21" ht="19.5">
       <c r="A299" s="2" t="s">
         <v>352</v>
       </c>
@@ -18146,7 +18182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="300" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:21" ht="19.5">
       <c r="A300" s="2" t="s">
         <v>352</v>
       </c>
@@ -18209,7 +18245,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="301" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:21" ht="19.5">
       <c r="A301" s="2" t="s">
         <v>352</v>
       </c>
@@ -18272,7 +18308,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="302" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:21" ht="19.5">
       <c r="A302" s="2" t="s">
         <v>352</v>
       </c>
@@ -18335,7 +18371,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="303" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:21" ht="19.5">
       <c r="A303" s="2" t="s">
         <v>352</v>
       </c>
@@ -18398,7 +18434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="304" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:21" ht="19.5">
       <c r="A304" s="2" t="s">
         <v>352</v>
       </c>
@@ -18461,7 +18497,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="305" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:21" ht="19.5">
       <c r="A305" s="2" t="s">
         <v>352</v>
       </c>
@@ -18502,7 +18538,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="306" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:21" ht="19.5">
       <c r="A306" s="2" t="s">
         <v>352</v>
       </c>
@@ -18534,7 +18570,7 @@
         <v>38.299999999999997</v>
       </c>
       <c r="K306" s="4">
-        <v>37.700000000000003</v>
+        <v>37.4</v>
       </c>
       <c r="L306" s="4">
         <v>39</v>
@@ -18557,13 +18593,15 @@
       <c r="R306" s="4">
         <v>38.299999999999997</v>
       </c>
-      <c r="S306" s="3"/>
+      <c r="S306" s="4">
+        <v>38.9</v>
+      </c>
       <c r="T306" s="3"/>
       <c r="U306" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="307" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:21" ht="39">
       <c r="A307" s="2" t="s">
         <v>352</v>
       </c>
@@ -18626,7 +18664,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="308" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:21" ht="48.75">
       <c r="A308" s="2" t="s">
         <v>352</v>
       </c>
@@ -18689,7 +18727,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="309" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:21" ht="39">
       <c r="A309" s="2" t="s">
         <v>352</v>
       </c>
@@ -18752,7 +18790,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="310" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:21" ht="39">
       <c r="A310" s="2" t="s">
         <v>352</v>
       </c>
@@ -18815,7 +18853,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="311" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:21" ht="29.25">
       <c r="A311" s="2" t="s">
         <v>352</v>
       </c>
@@ -18878,7 +18916,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="312" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:21" ht="39">
       <c r="A312" s="2" t="s">
         <v>352</v>
       </c>
@@ -18941,7 +18979,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="313" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:21" ht="29.25">
       <c r="A313" s="2" t="s">
         <v>352</v>
       </c>
@@ -19004,7 +19042,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="314" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:21" ht="29.25">
       <c r="A314" s="2" t="s">
         <v>352</v>
       </c>
@@ -19067,7 +19105,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="315" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:21" ht="39">
       <c r="A315" s="2" t="s">
         <v>352</v>
       </c>
@@ -19130,7 +19168,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="316" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:21" ht="29.25">
       <c r="A316" s="2" t="s">
         <v>352</v>
       </c>
@@ -19193,7 +19231,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="317" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:21" ht="39">
       <c r="A317" s="2" t="s">
         <v>352</v>
       </c>
@@ -19256,7 +19294,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="318" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:21" ht="29.25">
       <c r="A318" s="2" t="s">
         <v>352</v>
       </c>
@@ -19319,7 +19357,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="319" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:21" ht="29.25">
       <c r="A319" s="2" t="s">
         <v>352</v>
       </c>
@@ -19375,14 +19413,16 @@
         <v>4.1100000000000003</v>
       </c>
       <c r="S319" s="5">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="T319" s="3"/>
+        <v>4.05</v>
+      </c>
+      <c r="T319" s="5">
+        <v>4.04</v>
+      </c>
       <c r="U319" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="320" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:21" ht="39">
       <c r="A320" s="2" t="s">
         <v>352</v>
       </c>
@@ -19445,7 +19485,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="321" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:21" ht="39">
       <c r="A321" s="2" t="s">
         <v>352</v>
       </c>
@@ -19508,7 +19548,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="322" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:21" ht="68.25">
       <c r="A322" s="2" t="s">
         <v>352</v>
       </c>
@@ -19571,7 +19611,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="323" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:21" ht="58.5">
       <c r="A323" s="2" t="s">
         <v>352</v>
       </c>
@@ -19634,7 +19674,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="324" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:21" ht="68.25">
       <c r="A324" s="2" t="s">
         <v>352</v>
       </c>
@@ -19697,7 +19737,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="325" spans="1:21" ht="72" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:21" ht="68.25">
       <c r="A325" s="2" t="s">
         <v>352</v>
       </c>
@@ -19760,7 +19800,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="326" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:21" ht="39">
       <c r="A326" s="2" t="s">
         <v>352</v>
       </c>
@@ -19823,7 +19863,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="327" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:21" ht="68.25">
       <c r="A327" s="2" t="s">
         <v>352</v>
       </c>
@@ -19886,7 +19926,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="328" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:21" ht="58.5">
       <c r="A328" s="2" t="s">
         <v>352</v>
       </c>
@@ -19949,7 +19989,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="329" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:21" ht="68.25">
       <c r="A329" s="2" t="s">
         <v>352</v>
       </c>
@@ -20012,7 +20052,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="330" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:21" ht="68.25">
       <c r="A330" s="2" t="s">
         <v>352</v>
       </c>
@@ -20075,7 +20115,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="331" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:21" ht="29.25">
       <c r="A331" s="2" t="s">
         <v>393</v>
       </c>
@@ -20126,13 +20166,15 @@
       </c>
       <c r="Q331" s="3"/>
       <c r="R331" s="3"/>
-      <c r="S331" s="3"/>
+      <c r="S331" s="4">
+        <v>5.8</v>
+      </c>
       <c r="T331" s="3"/>
       <c r="U331" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="332" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:21" ht="29.25">
       <c r="A332" s="2" t="s">
         <v>393</v>
       </c>
@@ -20183,13 +20225,15 @@
       </c>
       <c r="Q332" s="3"/>
       <c r="R332" s="3"/>
-      <c r="S332" s="3"/>
+      <c r="S332" s="4">
+        <v>6.1</v>
+      </c>
       <c r="T332" s="3"/>
       <c r="U332" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="333" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:21" ht="29.25">
       <c r="A333" s="2" t="s">
         <v>393</v>
       </c>
@@ -20240,13 +20284,15 @@
       </c>
       <c r="Q333" s="3"/>
       <c r="R333" s="3"/>
-      <c r="S333" s="3"/>
+      <c r="S333" s="4">
+        <v>5.4</v>
+      </c>
       <c r="T333" s="3"/>
       <c r="U333" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="334" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:21" ht="29.25">
       <c r="A334" s="2" t="s">
         <v>393</v>
       </c>
@@ -20309,7 +20355,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="335" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:21" ht="29.25">
       <c r="A335" s="2" t="s">
         <v>393</v>
       </c>
@@ -20372,7 +20418,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="336" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:21" ht="29.25">
       <c r="A336" s="2" t="s">
         <v>393</v>
       </c>
@@ -20435,7 +20481,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="337" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:21" ht="29.25">
       <c r="A337" s="2" t="s">
         <v>393</v>
       </c>
@@ -20498,7 +20544,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="338" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:21" ht="29.25">
       <c r="A338" s="2" t="s">
         <v>393</v>
       </c>
@@ -20561,7 +20607,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="339" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:21" ht="29.25">
       <c r="A339" s="2" t="s">
         <v>393</v>
       </c>
@@ -20624,7 +20670,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="340" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:21" ht="29.25">
       <c r="A340" s="2" t="s">
         <v>393</v>
       </c>
@@ -20687,7 +20733,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="341" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:21" ht="29.25">
       <c r="A341" s="2" t="s">
         <v>393</v>
       </c>
@@ -20750,7 +20796,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="342" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:21" ht="29.25">
       <c r="A342" s="2" t="s">
         <v>393</v>
       </c>
@@ -20813,7 +20859,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="343" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:21" ht="29.25">
       <c r="A343" s="2" t="s">
         <v>393</v>
       </c>
@@ -20876,7 +20922,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="344" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:21" ht="29.25">
       <c r="A344" s="2" t="s">
         <v>393</v>
       </c>
@@ -20939,7 +20985,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="345" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:21" ht="29.25">
       <c r="A345" s="2" t="s">
         <v>393</v>
       </c>
@@ -21002,7 +21048,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="346" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:21" ht="29.25">
       <c r="A346" s="2" t="s">
         <v>393</v>
       </c>
@@ -21065,7 +21111,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="347" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:21" ht="29.25">
       <c r="A347" s="2" t="s">
         <v>393</v>
       </c>
@@ -21128,7 +21174,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="348" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:21" ht="29.25">
       <c r="A348" s="2" t="s">
         <v>393</v>
       </c>
@@ -21191,7 +21237,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="349" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:21" ht="29.25">
       <c r="A349" s="2" t="s">
         <v>393</v>
       </c>
@@ -21254,7 +21300,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="350" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:21" ht="29.25">
       <c r="A350" s="2" t="s">
         <v>393</v>
       </c>
@@ -21317,7 +21363,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="351" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:21" ht="29.25">
       <c r="A351" s="2" t="s">
         <v>393</v>
       </c>
@@ -21380,7 +21426,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="352" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:21" ht="29.25">
       <c r="A352" s="2" t="s">
         <v>393</v>
       </c>
@@ -21443,7 +21489,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="353" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:21" ht="29.25">
       <c r="A353" s="2" t="s">
         <v>393</v>
       </c>
@@ -21506,7 +21552,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="354" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:21" ht="29.25">
       <c r="A354" s="2" t="s">
         <v>393</v>
       </c>
@@ -21569,7 +21615,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="355" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:21" ht="29.25">
       <c r="A355" s="2" t="s">
         <v>393</v>
       </c>
@@ -21632,7 +21678,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="356" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:21" ht="29.25">
       <c r="A356" s="2" t="s">
         <v>393</v>
       </c>
@@ -21695,7 +21741,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="357" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:21" ht="29.25">
       <c r="A357" s="2" t="s">
         <v>393</v>
       </c>
@@ -21758,7 +21804,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="358" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:21" ht="29.25">
       <c r="A358" s="2" t="s">
         <v>393</v>
       </c>
@@ -21819,7 +21865,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="359" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:21" ht="29.25">
       <c r="A359" s="2" t="s">
         <v>393</v>
       </c>
@@ -21882,7 +21928,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="360" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:21" ht="29.25">
       <c r="A360" s="2" t="s">
         <v>393</v>
       </c>
@@ -21945,7 +21991,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="361" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:21" ht="29.25">
       <c r="A361" s="2" t="s">
         <v>393</v>
       </c>
@@ -22008,7 +22054,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="362" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:21" ht="29.25">
       <c r="A362" s="2" t="s">
         <v>393</v>
       </c>
@@ -22071,7 +22117,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="363" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:21" ht="29.25">
       <c r="A363" s="2" t="s">
         <v>393</v>
       </c>
@@ -22134,7 +22180,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="364" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:21" ht="39">
       <c r="A364" s="2" t="s">
         <v>393</v>
       </c>
@@ -22197,7 +22243,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="365" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:21" ht="39">
       <c r="A365" s="2" t="s">
         <v>393</v>
       </c>
@@ -22260,7 +22306,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="366" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:21" ht="39">
       <c r="A366" s="2" t="s">
         <v>393</v>
       </c>
@@ -22323,7 +22369,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="367" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:21" ht="39">
       <c r="A367" s="2" t="s">
         <v>393</v>
       </c>
@@ -22386,7 +22432,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="368" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:21" ht="39">
       <c r="A368" s="2" t="s">
         <v>393</v>
       </c>
@@ -22449,7 +22495,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="369" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:21" ht="39">
       <c r="A369" s="2" t="s">
         <v>393</v>
       </c>
@@ -22512,7 +22558,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="370" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:21" ht="39">
       <c r="A370" s="2" t="s">
         <v>393</v>
       </c>
@@ -22575,7 +22621,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="371" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:21" ht="39">
       <c r="A371" s="2" t="s">
         <v>393</v>
       </c>
@@ -22638,7 +22684,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="372" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:21" ht="29.25">
       <c r="A372" s="2" t="s">
         <v>393</v>
       </c>
@@ -22693,7 +22739,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="373" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:21" ht="68.25">
       <c r="A373" s="2" t="s">
         <v>393</v>
       </c>
@@ -22748,7 +22794,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="374" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:21" ht="29.25">
       <c r="A374" s="2" t="s">
         <v>393</v>
       </c>
@@ -22803,7 +22849,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="375" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:21" ht="29.25">
       <c r="A375" s="2" t="s">
         <v>393</v>
       </c>
@@ -22858,7 +22904,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="376" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:21" ht="39">
       <c r="A376" s="2" t="s">
         <v>428</v>
       </c>
@@ -22921,7 +22967,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="377" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:21" ht="39">
       <c r="A377" s="2" t="s">
         <v>428</v>
       </c>
@@ -22984,7 +23030,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="378" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:21" ht="39">
       <c r="A378" s="2" t="s">
         <v>428</v>
       </c>
@@ -23047,7 +23093,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="379" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:21" ht="48.75">
       <c r="A379" s="2" t="s">
         <v>428</v>
       </c>
@@ -23110,7 +23156,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="380" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:21" ht="39">
       <c r="A380" s="2" t="s">
         <v>428</v>
       </c>
@@ -23157,7 +23203,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="381" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:21" ht="39">
       <c r="A381" s="2" t="s">
         <v>428</v>
       </c>
@@ -23204,7 +23250,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="382" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:21" ht="39">
       <c r="A382" s="2" t="s">
         <v>428</v>
       </c>
@@ -23251,7 +23297,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="383" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:21" ht="39">
       <c r="A383" s="2" t="s">
         <v>428</v>
       </c>
@@ -23306,7 +23352,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="384" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:21" ht="39">
       <c r="A384" s="2" t="s">
         <v>428</v>
       </c>
@@ -23353,7 +23399,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="385" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:21" ht="39">
       <c r="A385" s="2" t="s">
         <v>428</v>
       </c>
@@ -23418,7 +23464,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="386" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:21" ht="48.75">
       <c r="A386" s="2" t="s">
         <v>428</v>
       </c>
@@ -23483,7 +23529,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="387" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:21" ht="29.25">
       <c r="A387" s="2" t="s">
         <v>448</v>
       </c>
@@ -23546,7 +23592,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="388" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:21" ht="29.25">
       <c r="A388" s="2" t="s">
         <v>448</v>
       </c>
@@ -23609,7 +23655,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="389" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:21" ht="29.25">
       <c r="A389" s="2" t="s">
         <v>448</v>
       </c>
@@ -23664,7 +23710,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="390" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:21" ht="68.25">
       <c r="A390" s="2" t="s">
         <v>448</v>
       </c>
@@ -23719,7 +23765,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="391" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:21" ht="29.25">
       <c r="A391" s="2" t="s">
         <v>448</v>
       </c>
@@ -23774,7 +23820,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="392" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:21" ht="29.25">
       <c r="A392" s="2" t="s">
         <v>448</v>
       </c>
@@ -23829,7 +23875,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="393" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:21" ht="39">
       <c r="A393" s="2" t="s">
         <v>448</v>
       </c>
@@ -23894,7 +23940,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="394" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:21" ht="39">
       <c r="A394" s="2" t="s">
         <v>448</v>
       </c>
@@ -23955,7 +24001,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="395" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:21" ht="48.75">
       <c r="A395" s="2" t="s">
         <v>448</v>
       </c>
@@ -24020,7 +24066,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="396" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:21" ht="29.25">
       <c r="A396" s="2" t="s">
         <v>448</v>
       </c>
@@ -24077,7 +24123,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="397" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:21" ht="58.5">
       <c r="A397" s="2" t="s">
         <v>460</v>
       </c>
@@ -24140,7 +24186,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="398" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:21" ht="39">
       <c r="A398" s="2" t="s">
         <v>460</v>
       </c>
@@ -24203,7 +24249,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="399" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:21" ht="48.75">
       <c r="A399" s="2" t="s">
         <v>460</v>
       </c>
@@ -24266,7 +24312,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="400" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:21" ht="48.75">
       <c r="A400" s="2" t="s">
         <v>460</v>
       </c>
@@ -24329,7 +24375,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="401" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:21" ht="58.5">
       <c r="A401" s="2" t="s">
         <v>460</v>
       </c>
@@ -24392,7 +24438,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="402" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:21" ht="19.5">
       <c r="A402" s="2" t="s">
         <v>470</v>
       </c>
@@ -24455,7 +24501,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="403" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:21" ht="19.5">
       <c r="A403" s="2" t="s">
         <v>470</v>
       </c>
@@ -24518,7 +24564,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="404" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:21" ht="39">
       <c r="A404" s="2" t="s">
         <v>470</v>
       </c>
@@ -24581,7 +24627,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="405" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:21" ht="19.5">
       <c r="A405" s="2" t="s">
         <v>470</v>
       </c>
@@ -24626,7 +24672,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="406" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:21" ht="19.5">
       <c r="A406" s="2" t="s">
         <v>470</v>
       </c>
@@ -24661,7 +24707,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="407" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:21" ht="19.5">
       <c r="A407" s="2" t="s">
         <v>470</v>
       </c>
@@ -24696,7 +24742,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="408" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:21" ht="19.5">
       <c r="A408" s="2" t="s">
         <v>470</v>
       </c>
@@ -24731,7 +24777,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="409" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:21" ht="19.5">
       <c r="A409" s="2" t="s">
         <v>470</v>
       </c>
@@ -24776,7 +24822,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="410" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:21" ht="19.5">
       <c r="A410" s="2" t="s">
         <v>470</v>
       </c>
@@ -24821,7 +24867,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="411" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:21" ht="19.5">
       <c r="A411" s="2" t="s">
         <v>470</v>
       </c>
@@ -24866,7 +24912,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="412" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:21" ht="29.25">
       <c r="A412" s="2" t="s">
         <v>470</v>
       </c>
@@ -24931,7 +24977,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="413" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:21" ht="19.5">
       <c r="A413" s="2" t="s">
         <v>470</v>
       </c>
@@ -24994,7 +25040,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="414" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:21" ht="29.25">
       <c r="A414" s="2" t="s">
         <v>470</v>
       </c>
@@ -25059,7 +25105,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="415" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:21" ht="29.25">
       <c r="A415" s="2" t="s">
         <v>470</v>
       </c>
@@ -25116,7 +25162,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="416" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:21" ht="29.25">
       <c r="A416" s="2" t="s">
         <v>470</v>
       </c>
@@ -25173,7 +25219,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="417" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:21" ht="19.5">
       <c r="A417" s="2" t="s">
         <v>470</v>
       </c>
@@ -25236,7 +25282,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="418" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:21" ht="29.25">
       <c r="A418" s="2" t="s">
         <v>491</v>
       </c>
@@ -25291,13 +25337,15 @@
       <c r="R418" s="5">
         <v>0.49</v>
       </c>
-      <c r="S418" s="3"/>
+      <c r="S418" s="5">
+        <v>0.52</v>
+      </c>
       <c r="T418" s="3"/>
       <c r="U418" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="419" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:21" ht="29.25">
       <c r="A419" s="2" t="s">
         <v>491</v>
       </c>
@@ -25362,7 +25410,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="420" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:21" ht="29.25">
       <c r="A420" s="2" t="s">
         <v>491</v>
       </c>
@@ -25407,7 +25455,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="421" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:21" ht="29.25">
       <c r="A421" s="2" t="s">
         <v>491</v>
       </c>
@@ -25466,7 +25514,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="422" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:21" ht="29.25">
       <c r="A422" s="2" t="s">
         <v>491</v>
       </c>
@@ -25517,7 +25565,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="423" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:21" ht="29.25">
       <c r="A423" s="2" t="s">
         <v>491</v>
       </c>
@@ -25568,7 +25616,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="424" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:21" ht="29.25">
       <c r="A424" s="2" t="s">
         <v>491</v>
       </c>
@@ -25619,7 +25667,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="425" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:21" ht="29.25">
       <c r="A425" s="2" t="s">
         <v>491</v>
       </c>
@@ -25670,7 +25718,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="426" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:21" ht="29.25">
       <c r="A426" s="2" t="s">
         <v>491</v>
       </c>
@@ -25721,7 +25769,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="427" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:21" ht="29.25">
       <c r="A427" s="2" t="s">
         <v>491</v>
       </c>
@@ -25772,7 +25820,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="428" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:21" ht="39">
       <c r="A428" s="2" t="s">
         <v>491</v>
       </c>
@@ -25823,7 +25871,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="429" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:21" ht="48.75">
       <c r="A429" s="2" t="s">
         <v>491</v>
       </c>
@@ -25874,7 +25922,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="430" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:21" ht="39">
       <c r="A430" s="2" t="s">
         <v>491</v>
       </c>
@@ -25925,7 +25973,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="431" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:21" ht="39">
       <c r="A431" s="2" t="s">
         <v>491</v>
       </c>
@@ -25976,7 +26024,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="432" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:21" ht="29.25">
       <c r="A432" s="2" t="s">
         <v>491</v>
       </c>
@@ -26039,7 +26087,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="433" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:21" ht="29.25">
       <c r="A433" s="2" t="s">
         <v>491</v>
       </c>
@@ -26102,7 +26150,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="434" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:21" ht="29.25">
       <c r="A434" s="2" t="s">
         <v>491</v>
       </c>
@@ -26165,7 +26213,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="435" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:21" ht="29.25">
       <c r="A435" s="2" t="s">
         <v>491</v>
       </c>
@@ -26228,7 +26276,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="436" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:21" ht="29.25">
       <c r="A436" s="2" t="s">
         <v>491</v>
       </c>
@@ -26291,7 +26339,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="437" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:21" ht="29.25">
       <c r="A437" s="2" t="s">
         <v>491</v>
       </c>
@@ -26354,7 +26402,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="438" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:21" ht="39">
       <c r="A438" s="2" t="s">
         <v>491</v>
       </c>
@@ -26397,7 +26445,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="439" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:21" ht="39">
       <c r="A439" s="2" t="s">
         <v>491</v>
       </c>
@@ -26440,7 +26488,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="440" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:21" ht="39">
       <c r="A440" s="2" t="s">
         <v>491</v>
       </c>
@@ -26483,7 +26531,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="441" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:21" ht="39">
       <c r="A441" s="2" t="s">
         <v>491</v>
       </c>
@@ -26526,7 +26574,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="442" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:21" ht="39">
       <c r="A442" s="2" t="s">
         <v>491</v>
       </c>
@@ -26569,7 +26617,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="443" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:21" ht="39">
       <c r="A443" s="2" t="s">
         <v>491</v>
       </c>
@@ -26612,7 +26660,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="444" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:21" ht="39">
       <c r="A444" s="2" t="s">
         <v>491</v>
       </c>
@@ -26655,7 +26703,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="445" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:21" ht="39">
       <c r="A445" s="2" t="s">
         <v>491</v>
       </c>
@@ -26698,7 +26746,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="446" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:21" ht="39">
       <c r="A446" s="2" t="s">
         <v>491</v>
       </c>
@@ -26741,7 +26789,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="447" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:21" ht="39">
       <c r="A447" s="2" t="s">
         <v>491</v>
       </c>
@@ -26784,7 +26832,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="448" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:21" ht="39">
       <c r="A448" s="2" t="s">
         <v>491</v>
       </c>
@@ -26827,7 +26875,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="449" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:21" ht="39">
       <c r="A449" s="2" t="s">
         <v>491</v>
       </c>
@@ -26870,7 +26918,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="450" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:21" ht="29.25">
       <c r="A450" s="2" t="s">
         <v>491</v>
       </c>
@@ -26935,7 +26983,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="451" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:21" ht="29.25">
       <c r="A451" s="2" t="s">
         <v>491</v>
       </c>
@@ -26976,7 +27024,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="452" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:21" ht="29.25">
       <c r="A452" s="2" t="s">
         <v>528</v>
       </c>
@@ -27039,7 +27087,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="453" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:21" ht="29.25">
       <c r="A453" s="2" t="s">
         <v>528</v>
       </c>
@@ -27102,7 +27150,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="454" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:21" ht="29.25">
       <c r="A454" s="2" t="s">
         <v>528</v>
       </c>
@@ -27165,7 +27213,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="455" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:21" ht="29.25">
       <c r="A455" s="2" t="s">
         <v>528</v>
       </c>
@@ -27228,7 +27276,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="456" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:21" ht="48.75">
       <c r="A456" s="2" t="s">
         <v>528</v>
       </c>
@@ -27291,7 +27339,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="457" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:21" ht="29.25">
       <c r="A457" s="2" t="s">
         <v>528</v>
       </c>
@@ -27354,7 +27402,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="458" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:21" ht="29.25">
       <c r="A458" s="2" t="s">
         <v>528</v>
       </c>
@@ -27417,7 +27465,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="459" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:21" ht="29.25">
       <c r="A459" s="2" t="s">
         <v>528</v>
       </c>
@@ -27482,7 +27530,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="460" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:21" ht="29.25">
       <c r="A460" s="2" t="s">
         <v>528</v>
       </c>
@@ -27547,7 +27595,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="461" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:21" ht="29.25">
       <c r="A461" s="2" t="s">
         <v>528</v>
       </c>
@@ -27612,7 +27660,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="462" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:21" ht="29.25">
       <c r="A462" s="2" t="s">
         <v>528</v>
       </c>
@@ -27675,7 +27723,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="463" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:21" ht="29.25">
       <c r="A463" s="2" t="s">
         <v>528</v>
       </c>
@@ -27733,12 +27781,14 @@
       <c r="S463" s="4">
         <v>2580.4</v>
       </c>
-      <c r="T463" s="3"/>
+      <c r="T463" s="4">
+        <v>2064.6999999999998</v>
+      </c>
       <c r="U463" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="464" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:21" ht="29.25">
       <c r="A464" s="2" t="s">
         <v>528</v>
       </c>
@@ -27801,7 +27851,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="465" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:21" ht="29.25">
       <c r="A465" s="2" t="s">
         <v>528</v>
       </c>
@@ -27857,14 +27907,16 @@
         <v>82079</v>
       </c>
       <c r="S465" s="6">
-        <v>90396</v>
-      </c>
-      <c r="T465" s="3"/>
+        <v>90759</v>
+      </c>
+      <c r="T465" s="6">
+        <v>97120</v>
+      </c>
       <c r="U465" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="466" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:21" ht="29.25">
       <c r="A466" s="2" t="s">
         <v>528</v>
       </c>
@@ -27920,7 +27972,7 @@
         <v>105.3</v>
       </c>
       <c r="S466" s="4">
-        <v>100.1</v>
+        <v>100.2</v>
       </c>
       <c r="T466" s="4">
         <v>102.9</v>
@@ -27929,7 +27981,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="467" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:21" ht="48.75">
       <c r="A467" s="2" t="s">
         <v>528</v>
       </c>
@@ -27994,7 +28046,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="468" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:21" ht="29.25">
       <c r="A468" s="2" t="s">
         <v>528</v>
       </c>
@@ -28050,16 +28102,16 @@
         <v>16.399999999999999</v>
       </c>
       <c r="S468" s="4">
-        <v>17.7</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="T468" s="4">
-        <v>17.399999999999999</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="U468" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="469" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:21" ht="39">
       <c r="A469" s="2" t="s">
         <v>528</v>
       </c>
@@ -28115,14 +28167,16 @@
         <v>48.8</v>
       </c>
       <c r="S469" s="4">
-        <v>49.7</v>
-      </c>
-      <c r="T469" s="3"/>
+        <v>49.5</v>
+      </c>
+      <c r="T469" s="4">
+        <v>55.3</v>
+      </c>
       <c r="U469" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="470" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:21" ht="39">
       <c r="A470" s="2" t="s">
         <v>528</v>
       </c>
@@ -28180,12 +28234,14 @@
       <c r="S470" s="4">
         <v>-5.3</v>
       </c>
-      <c r="T470" s="3"/>
+      <c r="T470" s="4">
+        <v>-6.6</v>
+      </c>
       <c r="U470" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="471" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:21" ht="29.25">
       <c r="A471" s="2" t="s">
         <v>528</v>
       </c>
@@ -28236,7 +28292,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="472" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:21" ht="29.25">
       <c r="A472" s="2" t="s">
         <v>528</v>
       </c>
@@ -28301,7 +28357,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="473" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:21" ht="29.25">
       <c r="A473" s="2" t="s">
         <v>528</v>
       </c>
@@ -28366,7 +28422,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="474" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:21" ht="29.25">
       <c r="A474" s="2" t="s">
         <v>528</v>
       </c>
@@ -28423,7 +28479,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="475" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:21" ht="39">
       <c r="A475" s="2" t="s">
         <v>528</v>
       </c>
@@ -28462,7 +28518,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="476" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:21" ht="39">
       <c r="A476" s="2" t="s">
         <v>528</v>
       </c>
@@ -28527,7 +28583,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="477" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:21" ht="39">
       <c r="A477" s="2" t="s">
         <v>528</v>
       </c>
@@ -28592,8 +28648,8 @@
         <v>563</v>
       </c>
     </row>
-    <row r="478" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:21" ht="18" customHeight="1"/>
+    <row r="479" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A479" s="12" t="s">
         <v>566</v>
       </c>
@@ -28610,7 +28666,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="70" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="71" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okno serwisowe 29.04.2025. - aktualizacja EXCEL
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -1723,7 +1723,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 29-04-2025, 08:07</t>
+    <t>Last update: 29-04-2025, 13:45</t>
   </si>
 </sst>
 </file>
@@ -14845,7 +14845,9 @@
       <c r="S241" s="4">
         <v>2.8</v>
       </c>
-      <c r="T241" s="3"/>
+      <c r="T241" s="4">
+        <v>2.9</v>
+      </c>
       <c r="U241" s="2" t="s">
         <v>27</v>
       </c>
@@ -14908,7 +14910,9 @@
       <c r="S242" s="4">
         <v>2.8</v>
       </c>
-      <c r="T242" s="3"/>
+      <c r="T242" s="4">
+        <v>2.7</v>
+      </c>
       <c r="U242" s="2" t="s">
         <v>27</v>
       </c>
@@ -14971,7 +14975,9 @@
       <c r="S243" s="4">
         <v>2.9</v>
       </c>
-      <c r="T243" s="3"/>
+      <c r="T243" s="4">
+        <v>3.1</v>
+      </c>
       <c r="U243" s="2" t="s">
         <v>27</v>
       </c>
@@ -15034,7 +15040,9 @@
       <c r="S244" s="4">
         <v>11.3</v>
       </c>
-      <c r="T244" s="3"/>
+      <c r="T244" s="4">
+        <v>10.9</v>
+      </c>
       <c r="U244" s="2" t="s">
         <v>27</v>
       </c>
@@ -15097,7 +15105,9 @@
       <c r="S245" s="4">
         <v>3</v>
       </c>
-      <c r="T245" s="3"/>
+      <c r="T245" s="4">
+        <v>3.4</v>
+      </c>
       <c r="U245" s="2" t="s">
         <v>27</v>
       </c>
@@ -15160,7 +15170,9 @@
       <c r="S246" s="4">
         <v>2.1</v>
       </c>
-      <c r="T246" s="3"/>
+      <c r="T246" s="4">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="U246" s="2" t="s">
         <v>27</v>
       </c>
@@ -15223,7 +15235,9 @@
       <c r="S247" s="4">
         <v>2</v>
       </c>
-      <c r="T247" s="3"/>
+      <c r="T247" s="4">
+        <v>1.9</v>
+      </c>
       <c r="U247" s="2" t="s">
         <v>27</v>
       </c>
@@ -15286,7 +15300,9 @@
       <c r="S248" s="4">
         <v>1.7</v>
       </c>
-      <c r="T248" s="3"/>
+      <c r="T248" s="4">
+        <v>1.9</v>
+      </c>
       <c r="U248" s="2" t="s">
         <v>27</v>
       </c>
@@ -15349,7 +15365,9 @@
       <c r="S249" s="4">
         <v>5.2</v>
       </c>
-      <c r="T249" s="3"/>
+      <c r="T249" s="4">
+        <v>4.4000000000000004</v>
+      </c>
       <c r="U249" s="2" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Okno serwisowe 10.06.2025 - aktualizacja EXCEL
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dregerj\Documents\SDG\sdg_git_produkcja\sdg-indicators-pl\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1723,7 +1723,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 13-05-2025, 11:34</t>
+    <t>Last update: 10-06-2025, 12:31</t>
   </si>
 </sst>
 </file>
@@ -1738,7 +1738,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2278,7 +2278,7 @@
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2289,17 +2289,17 @@
     <col min="21" max="21" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="36" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="19.5">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="19.5">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="19.5">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="29.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="97.5">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="97.5">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="97.5">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="19.5">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="29.25">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="29.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="29.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="68.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="29.25">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="29.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="29.25">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="39">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="39">
       <c r="A30" s="2" t="s">
         <v>22</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="39">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="39">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="19.5">
       <c r="A33" s="2" t="s">
         <v>68</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="29.25">
       <c r="A34" s="2" t="s">
         <v>68</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="29.25">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="29.25">
       <c r="A36" s="2" t="s">
         <v>68</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="29.25">
       <c r="A37" s="2" t="s">
         <v>68</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="29.25">
       <c r="A38" s="2" t="s">
         <v>68</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="29.25">
       <c r="A39" s="2" t="s">
         <v>68</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="39">
       <c r="A40" s="2" t="s">
         <v>68</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="97.5">
       <c r="A41" s="2" t="s">
         <v>68</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="97.5">
       <c r="A42" s="2" t="s">
         <v>68</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="97.5">
       <c r="A43" s="2" t="s">
         <v>68</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="97.5">
       <c r="A44" s="2" t="s">
         <v>68</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="97.5">
       <c r="A45" s="2" t="s">
         <v>68</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="97.5">
       <c r="A46" s="2" t="s">
         <v>68</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="48.75">
       <c r="A47" s="2" t="s">
         <v>68</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="48.75">
       <c r="A48" s="2" t="s">
         <v>68</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="19.5">
       <c r="A49" s="2" t="s">
         <v>68</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="29.25">
       <c r="A50" s="2" t="s">
         <v>68</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="19.5">
       <c r="A51" s="2" t="s">
         <v>97</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="19.5">
       <c r="A52" s="2" t="s">
         <v>97</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>97</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>97</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>97</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>97</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>97</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>97</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="29.25">
       <c r="A59" s="2" t="s">
         <v>97</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>97</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="29.25">
       <c r="A61" s="2" t="s">
         <v>97</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="29.25">
       <c r="A62" s="2" t="s">
         <v>97</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="29.25">
       <c r="A63" s="2" t="s">
         <v>97</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="19.5">
       <c r="A64" s="2" t="s">
         <v>97</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" ht="29.25">
       <c r="A65" s="2" t="s">
         <v>97</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="29.25">
       <c r="A66" s="2" t="s">
         <v>97</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="29.25">
       <c r="A67" s="2" t="s">
         <v>97</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="29.25">
       <c r="A68" s="2" t="s">
         <v>97</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="29.25">
       <c r="A69" s="2" t="s">
         <v>97</v>
       </c>
@@ -6344,7 +6344,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="29.25">
       <c r="A70" s="2" t="s">
         <v>97</v>
       </c>
@@ -6407,7 +6407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" ht="29.25">
       <c r="A71" s="2" t="s">
         <v>97</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" ht="19.5">
       <c r="A72" s="2" t="s">
         <v>97</v>
       </c>
@@ -6533,7 +6533,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" ht="19.5">
       <c r="A73" s="2" t="s">
         <v>97</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="19.5">
       <c r="A74" s="2" t="s">
         <v>97</v>
       </c>
@@ -6659,7 +6659,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" ht="19.5">
       <c r="A75" s="2" t="s">
         <v>97</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" ht="29.25">
       <c r="A76" s="2" t="s">
         <v>97</v>
       </c>
@@ -6785,7 +6785,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="77" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="29.25">
       <c r="A77" s="2" t="s">
         <v>97</v>
       </c>
@@ -6826,7 +6826,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" ht="19.5">
       <c r="A78" s="2" t="s">
         <v>97</v>
       </c>
@@ -6889,7 +6889,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" ht="19.5">
       <c r="A79" s="2" t="s">
         <v>97</v>
       </c>
@@ -6952,7 +6952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" ht="19.5">
       <c r="A80" s="2" t="s">
         <v>97</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" ht="19.5">
       <c r="A81" s="2" t="s">
         <v>97</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" ht="29.25">
       <c r="A82" s="2" t="s">
         <v>97</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" ht="29.25">
       <c r="A83" s="2" t="s">
         <v>97</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="84" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" ht="19.5">
       <c r="A84" s="2" t="s">
         <v>97</v>
       </c>
@@ -7215,7 +7215,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" ht="29.25">
       <c r="A85" s="2" t="s">
         <v>97</v>
       </c>
@@ -7252,7 +7252,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="86" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" ht="19.5">
       <c r="A86" s="2" t="s">
         <v>97</v>
       </c>
@@ -7315,7 +7315,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" ht="19.5">
       <c r="A87" s="2" t="s">
         <v>97</v>
       </c>
@@ -7356,7 +7356,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" ht="19.5">
       <c r="A88" s="2" t="s">
         <v>97</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="89" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" ht="19.5">
       <c r="A89" s="2" t="s">
         <v>97</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="90" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" ht="19.5">
       <c r="A90" s="2" t="s">
         <v>97</v>
       </c>
@@ -7529,7 +7529,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="91" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" ht="29.25">
       <c r="A91" s="2" t="s">
         <v>97</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" ht="19.5">
       <c r="A92" s="2" t="s">
         <v>97</v>
       </c>
@@ -7631,7 +7631,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" ht="19.5">
       <c r="A93" s="2" t="s">
         <v>97</v>
       </c>
@@ -7676,7 +7676,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" ht="19.5">
       <c r="A94" s="2" t="s">
         <v>97</v>
       </c>
@@ -7721,7 +7721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" ht="19.5">
       <c r="A95" s="2" t="s">
         <v>97</v>
       </c>
@@ -7780,7 +7780,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" ht="78">
       <c r="A96" s="2" t="s">
         <v>151</v>
       </c>
@@ -7821,7 +7821,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" ht="78">
       <c r="A97" s="2" t="s">
         <v>151</v>
       </c>
@@ -7862,7 +7862,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="98" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" ht="78">
       <c r="A98" s="2" t="s">
         <v>151</v>
       </c>
@@ -7903,7 +7903,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="99" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" ht="78">
       <c r="A99" s="2" t="s">
         <v>151</v>
       </c>
@@ -7948,7 +7948,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="100" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" ht="78">
       <c r="A100" s="2" t="s">
         <v>151</v>
       </c>
@@ -7993,7 +7993,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" ht="78">
       <c r="A101" s="2" t="s">
         <v>151</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" ht="78">
       <c r="A102" s="2" t="s">
         <v>151</v>
       </c>
@@ -8083,7 +8083,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="103" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" ht="78">
       <c r="A103" s="2" t="s">
         <v>151</v>
       </c>
@@ -8128,7 +8128,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" ht="78">
       <c r="A104" s="2" t="s">
         <v>151</v>
       </c>
@@ -8173,7 +8173,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" ht="29.25">
       <c r="A105" s="2" t="s">
         <v>151</v>
       </c>
@@ -8212,7 +8212,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="106" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" ht="19.5">
       <c r="A106" s="2" t="s">
         <v>151</v>
       </c>
@@ -8275,7 +8275,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" ht="19.5">
       <c r="A107" s="2" t="s">
         <v>151</v>
       </c>
@@ -8338,7 +8338,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" ht="19.5">
       <c r="A108" s="2" t="s">
         <v>151</v>
       </c>
@@ -8401,7 +8401,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" ht="19.5">
       <c r="A109" s="2" t="s">
         <v>151</v>
       </c>
@@ -8440,7 +8440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" ht="19.5">
       <c r="A110" s="2" t="s">
         <v>151</v>
       </c>
@@ -8479,7 +8479,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="111" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" ht="19.5">
       <c r="A111" s="2" t="s">
         <v>151</v>
       </c>
@@ -8518,7 +8518,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" ht="29.25">
       <c r="A112" s="2" t="s">
         <v>151</v>
       </c>
@@ -8565,7 +8565,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" ht="19.5">
       <c r="A113" s="2" t="s">
         <v>151</v>
       </c>
@@ -8620,7 +8620,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" ht="39">
       <c r="A114" s="2" t="s">
         <v>151</v>
       </c>
@@ -8675,7 +8675,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" ht="48.75">
       <c r="A115" s="2" t="s">
         <v>151</v>
       </c>
@@ -8730,7 +8730,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" ht="58.5">
       <c r="A116" s="2" t="s">
         <v>151</v>
       </c>
@@ -8785,7 +8785,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="117" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" ht="29.25">
       <c r="A117" s="2" t="s">
         <v>151</v>
       </c>
@@ -8840,7 +8840,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="118" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" ht="29.25">
       <c r="A118" s="2" t="s">
         <v>151</v>
       </c>
@@ -8887,7 +8887,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" ht="19.5">
       <c r="A119" s="2" t="s">
         <v>151</v>
       </c>
@@ -8942,7 +8942,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" ht="39">
       <c r="A120" s="2" t="s">
         <v>151</v>
       </c>
@@ -8997,7 +8997,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" ht="48.75">
       <c r="A121" s="2" t="s">
         <v>151</v>
       </c>
@@ -9052,7 +9052,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="122" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" ht="58.5">
       <c r="A122" s="2" t="s">
         <v>151</v>
       </c>
@@ -9107,7 +9107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="123" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" ht="29.25">
       <c r="A123" s="2" t="s">
         <v>151</v>
       </c>
@@ -9162,7 +9162,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="124" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" ht="48.75">
       <c r="A124" s="2" t="s">
         <v>151</v>
       </c>
@@ -9205,7 +9205,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="125" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:21" ht="48.75">
       <c r="A125" s="2" t="s">
         <v>151</v>
       </c>
@@ -9248,7 +9248,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="126" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:21" ht="29.25">
       <c r="A126" s="2" t="s">
         <v>151</v>
       </c>
@@ -9309,7 +9309,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="127" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:21" ht="29.25">
       <c r="A127" s="2" t="s">
         <v>151</v>
       </c>
@@ -9346,7 +9346,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:21" ht="29.25">
       <c r="A128" s="2" t="s">
         <v>151</v>
       </c>
@@ -9383,7 +9383,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="129" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:21" ht="29.25">
       <c r="A129" s="2" t="s">
         <v>151</v>
       </c>
@@ -9420,7 +9420,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:21" ht="29.25">
       <c r="A130" s="2" t="s">
         <v>151</v>
       </c>
@@ -9457,7 +9457,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="131" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:21" ht="29.25">
       <c r="A131" s="2" t="s">
         <v>151</v>
       </c>
@@ -9494,7 +9494,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="132" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:21" ht="29.25">
       <c r="A132" s="2" t="s">
         <v>151</v>
       </c>
@@ -9531,7 +9531,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="133" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:21" ht="29.25">
       <c r="A133" s="2" t="s">
         <v>151</v>
       </c>
@@ -9568,7 +9568,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="134" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:21" ht="29.25">
       <c r="A134" s="2" t="s">
         <v>151</v>
       </c>
@@ -9605,7 +9605,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="135" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:21" ht="29.25">
       <c r="A135" s="2" t="s">
         <v>151</v>
       </c>
@@ -9642,7 +9642,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="136" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:21" ht="29.25">
       <c r="A136" s="2" t="s">
         <v>151</v>
       </c>
@@ -9679,7 +9679,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="137" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:21" ht="29.25">
       <c r="A137" s="2" t="s">
         <v>151</v>
       </c>
@@ -9716,7 +9716,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="138" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:21" ht="29.25">
       <c r="A138" s="2" t="s">
         <v>151</v>
       </c>
@@ -9753,7 +9753,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="139" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:21" ht="29.25">
       <c r="A139" s="2" t="s">
         <v>151</v>
       </c>
@@ -9790,7 +9790,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="140" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:21" ht="29.25">
       <c r="A140" s="2" t="s">
         <v>151</v>
       </c>
@@ -9827,7 +9827,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="141" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:21" ht="29.25">
       <c r="A141" s="2" t="s">
         <v>151</v>
       </c>
@@ -9864,7 +9864,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="142" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:21" ht="29.25">
       <c r="A142" s="2" t="s">
         <v>151</v>
       </c>
@@ -9901,7 +9901,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="143" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:21" ht="48.75">
       <c r="A143" s="2" t="s">
         <v>151</v>
       </c>
@@ -9966,7 +9966,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="144" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:21" ht="58.5">
       <c r="A144" s="2" t="s">
         <v>151</v>
       </c>
@@ -10031,7 +10031,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:21" ht="58.5">
       <c r="A145" s="2" t="s">
         <v>151</v>
       </c>
@@ -10068,7 +10068,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="146" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:21" ht="58.5">
       <c r="A146" s="2" t="s">
         <v>151</v>
       </c>
@@ -10105,7 +10105,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="147" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:21" ht="58.5">
       <c r="A147" s="2" t="s">
         <v>151</v>
       </c>
@@ -10170,7 +10170,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="148" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:21" ht="58.5">
       <c r="A148" s="2" t="s">
         <v>151</v>
       </c>
@@ -10235,7 +10235,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="149" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:21" ht="58.5">
       <c r="A149" s="2" t="s">
         <v>151</v>
       </c>
@@ -10300,7 +10300,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="150" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:21" ht="29.25">
       <c r="A150" s="2" t="s">
         <v>151</v>
       </c>
@@ -10357,7 +10357,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="151" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" ht="58.5">
       <c r="A151" s="2" t="s">
         <v>151</v>
       </c>
@@ -10414,7 +10414,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="152" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:21" ht="58.5">
       <c r="A152" s="2" t="s">
         <v>151</v>
       </c>
@@ -10471,7 +10471,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="153" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:21" ht="58.5">
       <c r="A153" s="2" t="s">
         <v>151</v>
       </c>
@@ -10528,7 +10528,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="154" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:21" ht="58.5">
       <c r="A154" s="2" t="s">
         <v>151</v>
       </c>
@@ -10585,7 +10585,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="155" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:21" ht="29.25">
       <c r="A155" s="2" t="s">
         <v>207</v>
       </c>
@@ -10622,7 +10622,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="156" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:21" ht="19.5">
       <c r="A156" s="2" t="s">
         <v>207</v>
       </c>
@@ -10683,7 +10683,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="157" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:21" ht="39">
       <c r="A157" s="2" t="s">
         <v>207</v>
       </c>
@@ -10722,7 +10722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="158" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:21" ht="39">
       <c r="A158" s="2" t="s">
         <v>207</v>
       </c>
@@ -10761,7 +10761,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="159" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:21" ht="39">
       <c r="A159" s="2" t="s">
         <v>207</v>
       </c>
@@ -10800,7 +10800,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="160" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:21" ht="39">
       <c r="A160" s="2" t="s">
         <v>207</v>
       </c>
@@ -10839,7 +10839,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="161" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" ht="39">
       <c r="A161" s="2" t="s">
         <v>207</v>
       </c>
@@ -10878,7 +10878,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="162" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:21" ht="19.5">
       <c r="A162" s="2" t="s">
         <v>207</v>
       </c>
@@ -10917,7 +10917,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="163" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:21" ht="19.5">
       <c r="A163" s="2" t="s">
         <v>207</v>
       </c>
@@ -10956,7 +10956,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="164" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:21" ht="19.5">
       <c r="A164" s="2" t="s">
         <v>207</v>
       </c>
@@ -10995,7 +10995,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="165" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:21" ht="19.5">
       <c r="A165" s="2" t="s">
         <v>207</v>
       </c>
@@ -11034,7 +11034,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="166" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:21" ht="19.5">
       <c r="A166" s="2" t="s">
         <v>207</v>
       </c>
@@ -11073,7 +11073,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="167" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:21" ht="19.5">
       <c r="A167" s="2" t="s">
         <v>207</v>
       </c>
@@ -11112,7 +11112,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="168" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:21" ht="19.5">
       <c r="A168" s="2" t="s">
         <v>207</v>
       </c>
@@ -11151,7 +11151,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="169" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:21" ht="19.5">
       <c r="A169" s="2" t="s">
         <v>207</v>
       </c>
@@ -11190,7 +11190,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="170" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:21" ht="29.25">
       <c r="A170" s="2" t="s">
         <v>207</v>
       </c>
@@ -11233,7 +11233,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="171" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:21" ht="29.25">
       <c r="A171" s="2" t="s">
         <v>207</v>
       </c>
@@ -11276,7 +11276,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="172" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:21" ht="29.25">
       <c r="A172" s="2" t="s">
         <v>207</v>
       </c>
@@ -11339,7 +11339,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="173" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:21" ht="29.25">
       <c r="A173" s="2" t="s">
         <v>207</v>
       </c>
@@ -11402,7 +11402,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="174" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:21" ht="29.25">
       <c r="A174" s="2" t="s">
         <v>207</v>
       </c>
@@ -11465,7 +11465,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="175" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:21" ht="29.25">
       <c r="A175" s="2" t="s">
         <v>207</v>
       </c>
@@ -11528,7 +11528,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="176" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:21" ht="29.25">
       <c r="A176" s="2" t="s">
         <v>207</v>
       </c>
@@ -11591,7 +11591,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="177" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:21" ht="19.5">
       <c r="A177" s="2" t="s">
         <v>207</v>
       </c>
@@ -11640,7 +11640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="178" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:21" ht="39">
       <c r="A178" s="2" t="s">
         <v>207</v>
       </c>
@@ -11689,7 +11689,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="179" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:21" ht="19.5">
       <c r="A179" s="2" t="s">
         <v>207</v>
       </c>
@@ -11738,7 +11738,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="180" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:21" ht="39">
       <c r="A180" s="2" t="s">
         <v>207</v>
       </c>
@@ -11787,7 +11787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="181" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:21" ht="39">
       <c r="A181" s="2" t="s">
         <v>207</v>
       </c>
@@ -11836,7 +11836,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="182" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:21" ht="39">
       <c r="A182" s="2" t="s">
         <v>207</v>
       </c>
@@ -11885,7 +11885,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="183" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:21" ht="39">
       <c r="A183" s="2" t="s">
         <v>207</v>
       </c>
@@ -11934,7 +11934,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="184" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:21" ht="39">
       <c r="A184" s="2" t="s">
         <v>207</v>
       </c>
@@ -11975,7 +11975,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="185" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:21" ht="39">
       <c r="A185" s="2" t="s">
         <v>207</v>
       </c>
@@ -12016,7 +12016,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="186" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:21" ht="39">
       <c r="A186" s="2" t="s">
         <v>207</v>
       </c>
@@ -12057,7 +12057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="187" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:21" ht="39">
       <c r="A187" s="2" t="s">
         <v>207</v>
       </c>
@@ -12098,7 +12098,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="188" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:21" ht="39">
       <c r="A188" s="2" t="s">
         <v>207</v>
       </c>
@@ -12139,7 +12139,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="189" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:21" ht="39">
       <c r="A189" s="2" t="s">
         <v>207</v>
       </c>
@@ -12180,7 +12180,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="190" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:21" ht="39">
       <c r="A190" s="2" t="s">
         <v>207</v>
       </c>
@@ -12221,7 +12221,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="191" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:21" ht="39">
       <c r="A191" s="2" t="s">
         <v>207</v>
       </c>
@@ -12262,7 +12262,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="192" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:21" ht="39">
       <c r="A192" s="2" t="s">
         <v>207</v>
       </c>
@@ -12303,7 +12303,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="193" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:21" ht="39">
       <c r="A193" s="2" t="s">
         <v>207</v>
       </c>
@@ -12344,7 +12344,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="194" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:21" ht="39">
       <c r="A194" s="2" t="s">
         <v>207</v>
       </c>
@@ -12385,7 +12385,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="195" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:21" ht="39">
       <c r="A195" s="2" t="s">
         <v>207</v>
       </c>
@@ -12426,7 +12426,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="196" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:21" ht="19.5">
       <c r="A196" s="2" t="s">
         <v>207</v>
       </c>
@@ -12469,7 +12469,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="197" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:21" ht="19.5">
       <c r="A197" s="2" t="s">
         <v>207</v>
       </c>
@@ -12528,7 +12528,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="198" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:21" ht="19.5">
       <c r="A198" s="2" t="s">
         <v>207</v>
       </c>
@@ -12587,7 +12587,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="199" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:21" ht="19.5">
       <c r="A199" s="2" t="s">
         <v>247</v>
       </c>
@@ -12646,7 +12646,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="200" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:21" ht="29.25">
       <c r="A200" s="2" t="s">
         <v>247</v>
       </c>
@@ -12705,7 +12705,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="201" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:21" ht="19.5">
       <c r="A201" s="2" t="s">
         <v>247</v>
       </c>
@@ -12768,7 +12768,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="202" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:21" ht="19.5">
       <c r="A202" s="2" t="s">
         <v>247</v>
       </c>
@@ -12807,7 +12807,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="203" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:21" ht="19.5">
       <c r="A203" s="2" t="s">
         <v>247</v>
       </c>
@@ -12846,7 +12846,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="204" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:21" ht="29.25">
       <c r="A204" s="2" t="s">
         <v>247</v>
       </c>
@@ -12907,7 +12907,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="205" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:21" ht="19.5">
       <c r="A205" s="2" t="s">
         <v>247</v>
       </c>
@@ -12968,7 +12968,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="206" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:21" ht="19.5">
       <c r="A206" s="2" t="s">
         <v>247</v>
       </c>
@@ -13015,7 +13015,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="207" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:21" ht="29.25">
       <c r="A207" s="2" t="s">
         <v>247</v>
       </c>
@@ -13076,7 +13076,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="208" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:21" ht="29.25">
       <c r="A208" s="2" t="s">
         <v>247</v>
       </c>
@@ -13133,7 +13133,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="209" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:21" ht="39">
       <c r="A209" s="2" t="s">
         <v>247</v>
       </c>
@@ -13196,7 +13196,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="210" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:21" ht="19.5">
       <c r="A210" s="2" t="s">
         <v>268</v>
       </c>
@@ -13233,7 +13233,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="211" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:21" ht="19.5">
       <c r="A211" s="2" t="s">
         <v>268</v>
       </c>
@@ -13296,7 +13296,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="212" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:21" ht="29.25">
       <c r="A212" s="2" t="s">
         <v>268</v>
       </c>
@@ -13353,7 +13353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="213" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:21" ht="29.25">
       <c r="A213" s="2" t="s">
         <v>268</v>
       </c>
@@ -13410,7 +13410,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="214" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:21" ht="29.25">
       <c r="A214" s="2" t="s">
         <v>275</v>
       </c>
@@ -13475,7 +13475,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="215" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:21" ht="29.25">
       <c r="A215" s="2" t="s">
         <v>275</v>
       </c>
@@ -13538,7 +13538,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="216" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:21" ht="29.25">
       <c r="A216" s="2" t="s">
         <v>275</v>
       </c>
@@ -13581,7 +13581,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="217" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:21" ht="29.25">
       <c r="A217" s="2" t="s">
         <v>275</v>
       </c>
@@ -13624,7 +13624,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="218" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:21" ht="29.25">
       <c r="A218" s="2" t="s">
         <v>275</v>
       </c>
@@ -13667,7 +13667,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:21" ht="29.25">
       <c r="A219" s="2" t="s">
         <v>275</v>
       </c>
@@ -13730,7 +13730,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="220" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:21" ht="29.25">
       <c r="A220" s="2" t="s">
         <v>275</v>
       </c>
@@ -13793,7 +13793,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="221" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:21" ht="29.25">
       <c r="A221" s="2" t="s">
         <v>275</v>
       </c>
@@ -13856,7 +13856,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="222" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:21" ht="29.25">
       <c r="A222" s="2" t="s">
         <v>275</v>
       </c>
@@ -13905,7 +13905,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="223" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:21" ht="29.25">
       <c r="A223" s="2" t="s">
         <v>275</v>
       </c>
@@ -13954,7 +13954,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="224" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:21" ht="29.25">
       <c r="A224" s="2" t="s">
         <v>275</v>
       </c>
@@ -14003,7 +14003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="225" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:21" ht="29.25">
       <c r="A225" s="2" t="s">
         <v>275</v>
       </c>
@@ -14052,7 +14052,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="226" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:21" ht="29.25">
       <c r="A226" s="2" t="s">
         <v>275</v>
       </c>
@@ -14101,7 +14101,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="227" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:21" ht="29.25">
       <c r="A227" s="2" t="s">
         <v>275</v>
       </c>
@@ -14150,7 +14150,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="228" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:21" ht="29.25">
       <c r="A228" s="2" t="s">
         <v>275</v>
       </c>
@@ -14199,7 +14199,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="229" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:21" ht="29.25">
       <c r="A229" s="2" t="s">
         <v>275</v>
       </c>
@@ -14248,7 +14248,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="230" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:21" ht="39">
       <c r="A230" s="2" t="s">
         <v>275</v>
       </c>
@@ -14297,7 +14297,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="231" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:21" ht="29.25">
       <c r="A231" s="2" t="s">
         <v>275</v>
       </c>
@@ -14346,7 +14346,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="232" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:21" ht="39">
       <c r="A232" s="2" t="s">
         <v>275</v>
       </c>
@@ -14395,7 +14395,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="233" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:21" ht="29.25">
       <c r="A233" s="2" t="s">
         <v>275</v>
       </c>
@@ -14444,7 +14444,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="234" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:21" ht="29.25">
       <c r="A234" s="2" t="s">
         <v>275</v>
       </c>
@@ -14493,7 +14493,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="235" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:21" ht="29.25">
       <c r="A235" s="2" t="s">
         <v>275</v>
       </c>
@@ -14542,7 +14542,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="236" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:21" ht="29.25">
       <c r="A236" s="2" t="s">
         <v>275</v>
       </c>
@@ -14591,7 +14591,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="237" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:21" ht="29.25">
       <c r="A237" s="2" t="s">
         <v>275</v>
       </c>
@@ -14640,7 +14640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="238" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:21" ht="29.25">
       <c r="A238" s="2" t="s">
         <v>275</v>
       </c>
@@ -14689,7 +14689,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="239" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:21" ht="29.25">
       <c r="A239" s="2" t="s">
         <v>275</v>
       </c>
@@ -14738,7 +14738,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="240" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:21" ht="29.25">
       <c r="A240" s="2" t="s">
         <v>275</v>
       </c>
@@ -14787,7 +14787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="241" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:21" ht="29.25">
       <c r="A241" s="2" t="s">
         <v>275</v>
       </c>
@@ -14852,7 +14852,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="242" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:21" ht="29.25">
       <c r="A242" s="2" t="s">
         <v>275</v>
       </c>
@@ -14917,7 +14917,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="243" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:21" ht="29.25">
       <c r="A243" s="2" t="s">
         <v>275</v>
       </c>
@@ -14982,7 +14982,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="244" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:21" ht="29.25">
       <c r="A244" s="2" t="s">
         <v>275</v>
       </c>
@@ -15047,7 +15047,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="245" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:21" ht="29.25">
       <c r="A245" s="2" t="s">
         <v>275</v>
       </c>
@@ -15112,7 +15112,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="246" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:21" ht="29.25">
       <c r="A246" s="2" t="s">
         <v>275</v>
       </c>
@@ -15177,7 +15177,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="247" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:21" ht="29.25">
       <c r="A247" s="2" t="s">
         <v>275</v>
       </c>
@@ -15242,7 +15242,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="248" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:21" ht="29.25">
       <c r="A248" s="2" t="s">
         <v>275</v>
       </c>
@@ -15307,7 +15307,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="249" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:21" ht="29.25">
       <c r="A249" s="2" t="s">
         <v>275</v>
       </c>
@@ -15372,7 +15372,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="250" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:21" ht="29.25">
       <c r="A250" s="2" t="s">
         <v>275</v>
       </c>
@@ -15435,7 +15435,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="251" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:21" ht="29.25">
       <c r="A251" s="2" t="s">
         <v>275</v>
       </c>
@@ -15498,7 +15498,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="252" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:21" ht="29.25">
       <c r="A252" s="2" t="s">
         <v>275</v>
       </c>
@@ -15561,7 +15561,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="253" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:21" ht="39">
       <c r="A253" s="2" t="s">
         <v>275</v>
       </c>
@@ -15604,7 +15604,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="254" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:21" ht="39">
       <c r="A254" s="2" t="s">
         <v>275</v>
       </c>
@@ -15647,7 +15647,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="255" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:21" ht="39">
       <c r="A255" s="2" t="s">
         <v>275</v>
       </c>
@@ -15690,7 +15690,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="256" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:21" ht="29.25">
       <c r="A256" s="2" t="s">
         <v>275</v>
       </c>
@@ -15753,7 +15753,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="257" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:21" ht="48.75">
       <c r="A257" s="2" t="s">
         <v>275</v>
       </c>
@@ -15812,7 +15812,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="258" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:21" ht="29.25">
       <c r="A258" s="2" t="s">
         <v>275</v>
       </c>
@@ -15849,7 +15849,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="259" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:21" ht="29.25">
       <c r="A259" s="2" t="s">
         <v>275</v>
       </c>
@@ -15886,7 +15886,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="260" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:21" ht="29.25">
       <c r="A260" s="2" t="s">
         <v>275</v>
       </c>
@@ -15923,7 +15923,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="261" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:21" ht="29.25">
       <c r="A261" s="2" t="s">
         <v>275</v>
       </c>
@@ -15960,7 +15960,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="262" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:21" ht="29.25">
       <c r="A262" s="2" t="s">
         <v>275</v>
       </c>
@@ -15997,7 +15997,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="263" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:21" ht="29.25">
       <c r="A263" s="2" t="s">
         <v>275</v>
       </c>
@@ -16034,7 +16034,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="264" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:21" ht="29.25">
       <c r="A264" s="2" t="s">
         <v>275</v>
       </c>
@@ -16071,7 +16071,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="265" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:21" ht="29.25">
       <c r="A265" s="2" t="s">
         <v>275</v>
       </c>
@@ -16108,7 +16108,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="266" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:21" ht="29.25">
       <c r="A266" s="2" t="s">
         <v>275</v>
       </c>
@@ -16161,7 +16161,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="267" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:21" ht="29.25">
       <c r="A267" s="2" t="s">
         <v>320</v>
       </c>
@@ -16224,7 +16224,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="268" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:21" ht="29.25">
       <c r="A268" s="2" t="s">
         <v>320</v>
       </c>
@@ -16287,7 +16287,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="269" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:21" ht="29.25">
       <c r="A269" s="2" t="s">
         <v>320</v>
       </c>
@@ -16350,7 +16350,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="270" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:21" ht="29.25">
       <c r="A270" s="2" t="s">
         <v>320</v>
       </c>
@@ -16413,7 +16413,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="271" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:21" ht="29.25">
       <c r="A271" s="2" t="s">
         <v>320</v>
       </c>
@@ -16476,7 +16476,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="272" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:21" ht="29.25">
       <c r="A272" s="2" t="s">
         <v>320</v>
       </c>
@@ -16539,7 +16539,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="273" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:21" ht="29.25">
       <c r="A273" s="2" t="s">
         <v>320</v>
       </c>
@@ -16602,7 +16602,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="274" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:21" ht="29.25">
       <c r="A274" s="2" t="s">
         <v>320</v>
       </c>
@@ -16665,7 +16665,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="275" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:21" ht="29.25">
       <c r="A275" s="2" t="s">
         <v>320</v>
       </c>
@@ -16728,7 +16728,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="276" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:21" ht="29.25">
       <c r="A276" s="2" t="s">
         <v>320</v>
       </c>
@@ -16791,7 +16791,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="277" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:21" ht="29.25">
       <c r="A277" s="2" t="s">
         <v>320</v>
       </c>
@@ -16854,7 +16854,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="278" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:21" ht="29.25">
       <c r="A278" s="2" t="s">
         <v>320</v>
       </c>
@@ -16919,7 +16919,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="279" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:21" ht="29.25">
       <c r="A279" s="2" t="s">
         <v>320</v>
       </c>
@@ -16982,7 +16982,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="280" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:21" ht="29.25">
       <c r="A280" s="2" t="s">
         <v>320</v>
       </c>
@@ -17045,7 +17045,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="281" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:21" ht="29.25">
       <c r="A281" s="2" t="s">
         <v>320</v>
       </c>
@@ -17108,7 +17108,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="282" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:21" ht="29.25">
       <c r="A282" s="2" t="s">
         <v>320</v>
       </c>
@@ -17171,7 +17171,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="283" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:21" ht="29.25">
       <c r="A283" s="2" t="s">
         <v>320</v>
       </c>
@@ -17234,7 +17234,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="284" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:21" ht="29.25">
       <c r="A284" s="2" t="s">
         <v>320</v>
       </c>
@@ -17297,7 +17297,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="285" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:21" ht="29.25">
       <c r="A285" s="2" t="s">
         <v>320</v>
       </c>
@@ -17360,7 +17360,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="286" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:21" ht="29.25">
       <c r="A286" s="2" t="s">
         <v>320</v>
       </c>
@@ -17423,7 +17423,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="287" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:21" ht="29.25">
       <c r="A287" s="2" t="s">
         <v>320</v>
       </c>
@@ -17476,7 +17476,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="288" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:21" ht="29.25">
       <c r="A288" s="2" t="s">
         <v>320</v>
       </c>
@@ -17539,7 +17539,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="289" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:21" ht="29.25">
       <c r="A289" s="2" t="s">
         <v>320</v>
       </c>
@@ -17602,7 +17602,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="290" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:21" ht="29.25">
       <c r="A290" s="2" t="s">
         <v>320</v>
       </c>
@@ -17659,7 +17659,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="291" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:21" ht="29.25">
       <c r="A291" s="2" t="s">
         <v>320</v>
       </c>
@@ -17714,7 +17714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="292" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:21" ht="39">
       <c r="A292" s="2" t="s">
         <v>320</v>
       </c>
@@ -17767,7 +17767,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="293" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:21" ht="39">
       <c r="A293" s="2" t="s">
         <v>320</v>
       </c>
@@ -17822,7 +17822,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="294" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:21" ht="19.5">
       <c r="A294" s="2" t="s">
         <v>352</v>
       </c>
@@ -17885,7 +17885,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="295" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:21" ht="68.25">
       <c r="A295" s="2" t="s">
         <v>352</v>
       </c>
@@ -17948,7 +17948,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="296" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:21" ht="19.5">
       <c r="A296" s="2" t="s">
         <v>352</v>
       </c>
@@ -18011,7 +18011,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="297" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:21" ht="19.5">
       <c r="A297" s="2" t="s">
         <v>352</v>
       </c>
@@ -18074,7 +18074,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="298" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:21" ht="19.5">
       <c r="A298" s="2" t="s">
         <v>352</v>
       </c>
@@ -18137,7 +18137,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="299" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:21" ht="19.5">
       <c r="A299" s="2" t="s">
         <v>352</v>
       </c>
@@ -18200,7 +18200,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="300" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:21" ht="19.5">
       <c r="A300" s="2" t="s">
         <v>352</v>
       </c>
@@ -18263,7 +18263,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="301" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:21" ht="19.5">
       <c r="A301" s="2" t="s">
         <v>352</v>
       </c>
@@ -18326,7 +18326,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="302" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:21" ht="19.5">
       <c r="A302" s="2" t="s">
         <v>352</v>
       </c>
@@ -18389,7 +18389,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="303" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:21" ht="19.5">
       <c r="A303" s="2" t="s">
         <v>352</v>
       </c>
@@ -18452,7 +18452,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="304" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:21" ht="19.5">
       <c r="A304" s="2" t="s">
         <v>352</v>
       </c>
@@ -18515,7 +18515,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="305" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:21" ht="19.5">
       <c r="A305" s="2" t="s">
         <v>352</v>
       </c>
@@ -18556,7 +18556,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="306" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:21" ht="19.5">
       <c r="A306" s="2" t="s">
         <v>352</v>
       </c>
@@ -18619,7 +18619,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="307" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:21" ht="39">
       <c r="A307" s="2" t="s">
         <v>352</v>
       </c>
@@ -18682,7 +18682,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="308" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:21" ht="48.75">
       <c r="A308" s="2" t="s">
         <v>352</v>
       </c>
@@ -18745,7 +18745,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="309" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:21" ht="39">
       <c r="A309" s="2" t="s">
         <v>352</v>
       </c>
@@ -18808,7 +18808,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="310" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:21" ht="39">
       <c r="A310" s="2" t="s">
         <v>352</v>
       </c>
@@ -18871,7 +18871,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="311" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:21" ht="29.25">
       <c r="A311" s="2" t="s">
         <v>352</v>
       </c>
@@ -18934,7 +18934,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="312" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:21" ht="39">
       <c r="A312" s="2" t="s">
         <v>352</v>
       </c>
@@ -18997,7 +18997,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="313" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:21" ht="29.25">
       <c r="A313" s="2" t="s">
         <v>352</v>
       </c>
@@ -19060,7 +19060,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="314" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:21" ht="29.25">
       <c r="A314" s="2" t="s">
         <v>352</v>
       </c>
@@ -19123,7 +19123,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="315" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:21" ht="39">
       <c r="A315" s="2" t="s">
         <v>352</v>
       </c>
@@ -19186,7 +19186,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="316" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:21" ht="29.25">
       <c r="A316" s="2" t="s">
         <v>352</v>
       </c>
@@ -19249,7 +19249,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="317" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:21" ht="39">
       <c r="A317" s="2" t="s">
         <v>352</v>
       </c>
@@ -19312,7 +19312,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="318" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:21" ht="29.25">
       <c r="A318" s="2" t="s">
         <v>352</v>
       </c>
@@ -19375,7 +19375,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="319" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:21" ht="29.25">
       <c r="A319" s="2" t="s">
         <v>352</v>
       </c>
@@ -19440,7 +19440,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="320" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:21" ht="39">
       <c r="A320" s="2" t="s">
         <v>352</v>
       </c>
@@ -19503,7 +19503,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="321" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:21" ht="39">
       <c r="A321" s="2" t="s">
         <v>352</v>
       </c>
@@ -19566,7 +19566,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="322" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:21" ht="68.25">
       <c r="A322" s="2" t="s">
         <v>352</v>
       </c>
@@ -19629,7 +19629,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="323" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:21" ht="58.5">
       <c r="A323" s="2" t="s">
         <v>352</v>
       </c>
@@ -19692,7 +19692,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="324" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:21" ht="68.25">
       <c r="A324" s="2" t="s">
         <v>352</v>
       </c>
@@ -19755,7 +19755,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="325" spans="1:21" ht="72" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:21" ht="68.25">
       <c r="A325" s="2" t="s">
         <v>352</v>
       </c>
@@ -19818,7 +19818,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="326" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:21" ht="39">
       <c r="A326" s="2" t="s">
         <v>352</v>
       </c>
@@ -19881,7 +19881,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="327" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:21" ht="68.25">
       <c r="A327" s="2" t="s">
         <v>352</v>
       </c>
@@ -19944,7 +19944,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="328" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:21" ht="58.5">
       <c r="A328" s="2" t="s">
         <v>352</v>
       </c>
@@ -20007,7 +20007,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="329" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:21" ht="68.25">
       <c r="A329" s="2" t="s">
         <v>352</v>
       </c>
@@ -20070,7 +20070,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="330" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:21" ht="68.25">
       <c r="A330" s="2" t="s">
         <v>352</v>
       </c>
@@ -20133,7 +20133,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="331" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:21" ht="29.25">
       <c r="A331" s="2" t="s">
         <v>393</v>
       </c>
@@ -20192,7 +20192,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="332" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:21" ht="29.25">
       <c r="A332" s="2" t="s">
         <v>393</v>
       </c>
@@ -20251,7 +20251,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="333" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:21" ht="29.25">
       <c r="A333" s="2" t="s">
         <v>393</v>
       </c>
@@ -20310,7 +20310,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="334" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:21" ht="29.25">
       <c r="A334" s="2" t="s">
         <v>393</v>
       </c>
@@ -20373,7 +20373,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="335" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:21" ht="29.25">
       <c r="A335" s="2" t="s">
         <v>393</v>
       </c>
@@ -20436,7 +20436,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="336" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:21" ht="29.25">
       <c r="A336" s="2" t="s">
         <v>393</v>
       </c>
@@ -20499,7 +20499,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="337" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:21" ht="29.25">
       <c r="A337" s="2" t="s">
         <v>393</v>
       </c>
@@ -20562,7 +20562,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="338" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:21" ht="29.25">
       <c r="A338" s="2" t="s">
         <v>393</v>
       </c>
@@ -20625,7 +20625,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="339" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:21" ht="29.25">
       <c r="A339" s="2" t="s">
         <v>393</v>
       </c>
@@ -20688,7 +20688,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="340" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:21" ht="29.25">
       <c r="A340" s="2" t="s">
         <v>393</v>
       </c>
@@ -20751,7 +20751,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="341" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:21" ht="29.25">
       <c r="A341" s="2" t="s">
         <v>393</v>
       </c>
@@ -20814,7 +20814,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="342" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:21" ht="29.25">
       <c r="A342" s="2" t="s">
         <v>393</v>
       </c>
@@ -20877,7 +20877,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="343" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:21" ht="29.25">
       <c r="A343" s="2" t="s">
         <v>393</v>
       </c>
@@ -20940,7 +20940,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="344" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:21" ht="29.25">
       <c r="A344" s="2" t="s">
         <v>393</v>
       </c>
@@ -21003,7 +21003,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="345" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:21" ht="29.25">
       <c r="A345" s="2" t="s">
         <v>393</v>
       </c>
@@ -21066,7 +21066,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="346" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:21" ht="29.25">
       <c r="A346" s="2" t="s">
         <v>393</v>
       </c>
@@ -21129,7 +21129,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="347" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:21" ht="29.25">
       <c r="A347" s="2" t="s">
         <v>393</v>
       </c>
@@ -21192,7 +21192,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="348" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:21" ht="29.25">
       <c r="A348" s="2" t="s">
         <v>393</v>
       </c>
@@ -21255,7 +21255,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="349" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:21" ht="29.25">
       <c r="A349" s="2" t="s">
         <v>393</v>
       </c>
@@ -21318,7 +21318,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="350" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:21" ht="29.25">
       <c r="A350" s="2" t="s">
         <v>393</v>
       </c>
@@ -21381,7 +21381,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="351" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:21" ht="29.25">
       <c r="A351" s="2" t="s">
         <v>393</v>
       </c>
@@ -21444,7 +21444,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="352" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:21" ht="29.25">
       <c r="A352" s="2" t="s">
         <v>393</v>
       </c>
@@ -21507,7 +21507,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="353" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:21" ht="29.25">
       <c r="A353" s="2" t="s">
         <v>393</v>
       </c>
@@ -21570,7 +21570,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="354" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:21" ht="29.25">
       <c r="A354" s="2" t="s">
         <v>393</v>
       </c>
@@ -21633,7 +21633,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="355" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:21" ht="29.25">
       <c r="A355" s="2" t="s">
         <v>393</v>
       </c>
@@ -21696,7 +21696,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="356" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:21" ht="29.25">
       <c r="A356" s="2" t="s">
         <v>393</v>
       </c>
@@ -21759,7 +21759,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="357" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:21" ht="29.25">
       <c r="A357" s="2" t="s">
         <v>393</v>
       </c>
@@ -21822,7 +21822,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="358" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:21" ht="29.25">
       <c r="A358" s="2" t="s">
         <v>393</v>
       </c>
@@ -21883,7 +21883,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="359" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:21" ht="29.25">
       <c r="A359" s="2" t="s">
         <v>393</v>
       </c>
@@ -21946,7 +21946,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="360" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:21" ht="29.25">
       <c r="A360" s="2" t="s">
         <v>393</v>
       </c>
@@ -22009,7 +22009,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="361" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:21" ht="29.25">
       <c r="A361" s="2" t="s">
         <v>393</v>
       </c>
@@ -22072,7 +22072,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="362" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:21" ht="29.25">
       <c r="A362" s="2" t="s">
         <v>393</v>
       </c>
@@ -22135,7 +22135,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="363" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:21" ht="29.25">
       <c r="A363" s="2" t="s">
         <v>393</v>
       </c>
@@ -22198,7 +22198,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="364" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:21" ht="39">
       <c r="A364" s="2" t="s">
         <v>393</v>
       </c>
@@ -22261,7 +22261,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="365" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:21" ht="39">
       <c r="A365" s="2" t="s">
         <v>393</v>
       </c>
@@ -22324,7 +22324,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="366" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:21" ht="39">
       <c r="A366" s="2" t="s">
         <v>393</v>
       </c>
@@ -22387,7 +22387,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="367" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:21" ht="39">
       <c r="A367" s="2" t="s">
         <v>393</v>
       </c>
@@ -22450,7 +22450,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="368" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:21" ht="39">
       <c r="A368" s="2" t="s">
         <v>393</v>
       </c>
@@ -22513,7 +22513,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="369" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:21" ht="39">
       <c r="A369" s="2" t="s">
         <v>393</v>
       </c>
@@ -22576,7 +22576,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="370" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:21" ht="39">
       <c r="A370" s="2" t="s">
         <v>393</v>
       </c>
@@ -22639,7 +22639,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="371" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:21" ht="39">
       <c r="A371" s="2" t="s">
         <v>393</v>
       </c>
@@ -22702,7 +22702,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="372" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:21" ht="29.25">
       <c r="A372" s="2" t="s">
         <v>393</v>
       </c>
@@ -22757,7 +22757,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="373" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:21" ht="68.25">
       <c r="A373" s="2" t="s">
         <v>393</v>
       </c>
@@ -22812,7 +22812,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="374" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:21" ht="29.25">
       <c r="A374" s="2" t="s">
         <v>393</v>
       </c>
@@ -22867,7 +22867,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="375" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:21" ht="29.25">
       <c r="A375" s="2" t="s">
         <v>393</v>
       </c>
@@ -22922,7 +22922,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="376" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:21" ht="39">
       <c r="A376" s="2" t="s">
         <v>428</v>
       </c>
@@ -22985,7 +22985,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="377" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:21" ht="39">
       <c r="A377" s="2" t="s">
         <v>428</v>
       </c>
@@ -23048,7 +23048,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="378" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:21" ht="39">
       <c r="A378" s="2" t="s">
         <v>428</v>
       </c>
@@ -23111,7 +23111,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="379" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:21" ht="48.75">
       <c r="A379" s="2" t="s">
         <v>428</v>
       </c>
@@ -23174,7 +23174,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="380" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:21" ht="39">
       <c r="A380" s="2" t="s">
         <v>428</v>
       </c>
@@ -23221,7 +23221,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="381" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:21" ht="39">
       <c r="A381" s="2" t="s">
         <v>428</v>
       </c>
@@ -23268,7 +23268,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="382" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:21" ht="39">
       <c r="A382" s="2" t="s">
         <v>428</v>
       </c>
@@ -23315,7 +23315,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="383" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:21" ht="39">
       <c r="A383" s="2" t="s">
         <v>428</v>
       </c>
@@ -23370,7 +23370,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="384" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:21" ht="39">
       <c r="A384" s="2" t="s">
         <v>428</v>
       </c>
@@ -23417,7 +23417,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="385" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:21" ht="39">
       <c r="A385" s="2" t="s">
         <v>428</v>
       </c>
@@ -23482,7 +23482,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="386" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:21" ht="48.75">
       <c r="A386" s="2" t="s">
         <v>428</v>
       </c>
@@ -23547,7 +23547,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="387" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:21" ht="29.25">
       <c r="A387" s="2" t="s">
         <v>448</v>
       </c>
@@ -23610,7 +23610,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="388" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:21" ht="29.25">
       <c r="A388" s="2" t="s">
         <v>448</v>
       </c>
@@ -23673,7 +23673,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="389" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:21" ht="29.25">
       <c r="A389" s="2" t="s">
         <v>448</v>
       </c>
@@ -23728,7 +23728,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="390" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:21" ht="68.25">
       <c r="A390" s="2" t="s">
         <v>448</v>
       </c>
@@ -23783,7 +23783,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="391" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:21" ht="29.25">
       <c r="A391" s="2" t="s">
         <v>448</v>
       </c>
@@ -23838,7 +23838,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="392" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:21" ht="29.25">
       <c r="A392" s="2" t="s">
         <v>448</v>
       </c>
@@ -23893,7 +23893,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="393" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:21" ht="39">
       <c r="A393" s="2" t="s">
         <v>448</v>
       </c>
@@ -23958,7 +23958,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="394" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:21" ht="39">
       <c r="A394" s="2" t="s">
         <v>448</v>
       </c>
@@ -24019,7 +24019,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="395" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:21" ht="48.75">
       <c r="A395" s="2" t="s">
         <v>448</v>
       </c>
@@ -24084,7 +24084,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="396" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:21" ht="29.25">
       <c r="A396" s="2" t="s">
         <v>448</v>
       </c>
@@ -24141,7 +24141,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="397" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:21" ht="58.5">
       <c r="A397" s="2" t="s">
         <v>460</v>
       </c>
@@ -24204,7 +24204,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="398" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:21" ht="39">
       <c r="A398" s="2" t="s">
         <v>460</v>
       </c>
@@ -24267,7 +24267,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="399" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:21" ht="48.75">
       <c r="A399" s="2" t="s">
         <v>460</v>
       </c>
@@ -24330,7 +24330,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="400" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:21" ht="48.75">
       <c r="A400" s="2" t="s">
         <v>460</v>
       </c>
@@ -24393,7 +24393,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="401" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:21" ht="58.5">
       <c r="A401" s="2" t="s">
         <v>460</v>
       </c>
@@ -24456,7 +24456,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="402" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:21" ht="19.5">
       <c r="A402" s="2" t="s">
         <v>470</v>
       </c>
@@ -24519,7 +24519,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="403" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:21" ht="19.5">
       <c r="A403" s="2" t="s">
         <v>470</v>
       </c>
@@ -24582,7 +24582,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="404" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:21" ht="39">
       <c r="A404" s="2" t="s">
         <v>470</v>
       </c>
@@ -24645,7 +24645,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="405" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:21" ht="19.5">
       <c r="A405" s="2" t="s">
         <v>470</v>
       </c>
@@ -24690,7 +24690,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="406" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:21" ht="19.5">
       <c r="A406" s="2" t="s">
         <v>470</v>
       </c>
@@ -24725,7 +24725,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="407" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:21" ht="19.5">
       <c r="A407" s="2" t="s">
         <v>470</v>
       </c>
@@ -24760,7 +24760,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="408" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:21" ht="19.5">
       <c r="A408" s="2" t="s">
         <v>470</v>
       </c>
@@ -24795,7 +24795,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="409" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:21" ht="19.5">
       <c r="A409" s="2" t="s">
         <v>470</v>
       </c>
@@ -24840,7 +24840,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="410" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:21" ht="19.5">
       <c r="A410" s="2" t="s">
         <v>470</v>
       </c>
@@ -24885,7 +24885,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="411" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:21" ht="19.5">
       <c r="A411" s="2" t="s">
         <v>470</v>
       </c>
@@ -24930,7 +24930,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="412" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:21" ht="29.25">
       <c r="A412" s="2" t="s">
         <v>470</v>
       </c>
@@ -24995,7 +24995,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="413" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:21" ht="19.5">
       <c r="A413" s="2" t="s">
         <v>470</v>
       </c>
@@ -25058,7 +25058,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="414" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:21" ht="29.25">
       <c r="A414" s="2" t="s">
         <v>470</v>
       </c>
@@ -25123,7 +25123,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="415" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:21" ht="29.25">
       <c r="A415" s="2" t="s">
         <v>470</v>
       </c>
@@ -25180,7 +25180,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="416" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:21" ht="29.25">
       <c r="A416" s="2" t="s">
         <v>470</v>
       </c>
@@ -25237,7 +25237,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="417" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:21" ht="19.5">
       <c r="A417" s="2" t="s">
         <v>470</v>
       </c>
@@ -25300,7 +25300,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="418" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:21" ht="29.25">
       <c r="A418" s="2" t="s">
         <v>491</v>
       </c>
@@ -25363,7 +25363,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="419" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:21" ht="29.25">
       <c r="A419" s="2" t="s">
         <v>491</v>
       </c>
@@ -25428,7 +25428,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="420" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:21" ht="29.25">
       <c r="A420" s="2" t="s">
         <v>491</v>
       </c>
@@ -25473,7 +25473,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="421" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:21" ht="29.25">
       <c r="A421" s="2" t="s">
         <v>491</v>
       </c>
@@ -25532,7 +25532,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="422" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:21" ht="29.25">
       <c r="A422" s="2" t="s">
         <v>491</v>
       </c>
@@ -25583,7 +25583,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="423" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:21" ht="29.25">
       <c r="A423" s="2" t="s">
         <v>491</v>
       </c>
@@ -25634,7 +25634,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="424" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:21" ht="29.25">
       <c r="A424" s="2" t="s">
         <v>491</v>
       </c>
@@ -25685,7 +25685,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="425" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:21" ht="29.25">
       <c r="A425" s="2" t="s">
         <v>491</v>
       </c>
@@ -25736,7 +25736,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="426" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:21" ht="29.25">
       <c r="A426" s="2" t="s">
         <v>491</v>
       </c>
@@ -25787,7 +25787,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="427" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:21" ht="29.25">
       <c r="A427" s="2" t="s">
         <v>491</v>
       </c>
@@ -25838,7 +25838,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="428" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:21" ht="39">
       <c r="A428" s="2" t="s">
         <v>491</v>
       </c>
@@ -25889,7 +25889,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="429" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:21" ht="48.75">
       <c r="A429" s="2" t="s">
         <v>491</v>
       </c>
@@ -25940,7 +25940,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="430" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:21" ht="39">
       <c r="A430" s="2" t="s">
         <v>491</v>
       </c>
@@ -25991,7 +25991,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="431" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:21" ht="39">
       <c r="A431" s="2" t="s">
         <v>491</v>
       </c>
@@ -26042,7 +26042,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="432" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:21" ht="29.25">
       <c r="A432" s="2" t="s">
         <v>491</v>
       </c>
@@ -26105,7 +26105,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="433" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:21" ht="29.25">
       <c r="A433" s="2" t="s">
         <v>491</v>
       </c>
@@ -26168,7 +26168,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="434" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:21" ht="29.25">
       <c r="A434" s="2" t="s">
         <v>491</v>
       </c>
@@ -26231,7 +26231,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="435" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:21" ht="29.25">
       <c r="A435" s="2" t="s">
         <v>491</v>
       </c>
@@ -26294,7 +26294,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="436" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:21" ht="29.25">
       <c r="A436" s="2" t="s">
         <v>491</v>
       </c>
@@ -26357,7 +26357,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="437" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:21" ht="29.25">
       <c r="A437" s="2" t="s">
         <v>491</v>
       </c>
@@ -26420,7 +26420,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="438" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:21" ht="39">
       <c r="A438" s="2" t="s">
         <v>491</v>
       </c>
@@ -26463,7 +26463,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="439" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:21" ht="39">
       <c r="A439" s="2" t="s">
         <v>491</v>
       </c>
@@ -26506,7 +26506,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="440" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:21" ht="39">
       <c r="A440" s="2" t="s">
         <v>491</v>
       </c>
@@ -26549,7 +26549,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="441" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:21" ht="39">
       <c r="A441" s="2" t="s">
         <v>491</v>
       </c>
@@ -26592,7 +26592,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="442" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:21" ht="39">
       <c r="A442" s="2" t="s">
         <v>491</v>
       </c>
@@ -26635,7 +26635,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="443" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:21" ht="39">
       <c r="A443" s="2" t="s">
         <v>491</v>
       </c>
@@ -26678,7 +26678,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="444" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:21" ht="39">
       <c r="A444" s="2" t="s">
         <v>491</v>
       </c>
@@ -26721,7 +26721,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="445" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:21" ht="39">
       <c r="A445" s="2" t="s">
         <v>491</v>
       </c>
@@ -26764,7 +26764,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="446" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:21" ht="39">
       <c r="A446" s="2" t="s">
         <v>491</v>
       </c>
@@ -26807,7 +26807,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="447" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:21" ht="39">
       <c r="A447" s="2" t="s">
         <v>491</v>
       </c>
@@ -26850,7 +26850,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="448" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:21" ht="39">
       <c r="A448" s="2" t="s">
         <v>491</v>
       </c>
@@ -26893,7 +26893,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="449" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:21" ht="39">
       <c r="A449" s="2" t="s">
         <v>491</v>
       </c>
@@ -26936,7 +26936,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="450" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:21" ht="29.25">
       <c r="A450" s="2" t="s">
         <v>491</v>
       </c>
@@ -27001,7 +27001,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="451" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:21" ht="29.25">
       <c r="A451" s="2" t="s">
         <v>491</v>
       </c>
@@ -27042,7 +27042,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="452" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:21" ht="29.25">
       <c r="A452" s="2" t="s">
         <v>528</v>
       </c>
@@ -27105,7 +27105,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="453" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:21" ht="29.25">
       <c r="A453" s="2" t="s">
         <v>528</v>
       </c>
@@ -27168,7 +27168,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="454" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:21" ht="29.25">
       <c r="A454" s="2" t="s">
         <v>528</v>
       </c>
@@ -27231,7 +27231,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="455" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:21" ht="29.25">
       <c r="A455" s="2" t="s">
         <v>528</v>
       </c>
@@ -27294,7 +27294,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="456" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:21" ht="48.75">
       <c r="A456" s="2" t="s">
         <v>528</v>
       </c>
@@ -27357,7 +27357,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="457" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:21" ht="29.25">
       <c r="A457" s="2" t="s">
         <v>528</v>
       </c>
@@ -27420,7 +27420,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="458" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:21" ht="29.25">
       <c r="A458" s="2" t="s">
         <v>528</v>
       </c>
@@ -27483,7 +27483,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="459" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:21" ht="29.25">
       <c r="A459" s="2" t="s">
         <v>528</v>
       </c>
@@ -27548,7 +27548,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="460" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:21" ht="29.25">
       <c r="A460" s="2" t="s">
         <v>528</v>
       </c>
@@ -27613,7 +27613,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="461" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:21" ht="29.25">
       <c r="A461" s="2" t="s">
         <v>528</v>
       </c>
@@ -27678,7 +27678,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="462" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:21" ht="29.25">
       <c r="A462" s="2" t="s">
         <v>528</v>
       </c>
@@ -27741,7 +27741,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="463" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:21" ht="29.25">
       <c r="A463" s="2" t="s">
         <v>528</v>
       </c>
@@ -27806,7 +27806,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="464" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:21" ht="29.25">
       <c r="A464" s="2" t="s">
         <v>528</v>
       </c>
@@ -27871,7 +27871,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="465" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:21" ht="29.25">
       <c r="A465" s="2" t="s">
         <v>528</v>
       </c>
@@ -27936,7 +27936,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="466" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:21" ht="29.25">
       <c r="A466" s="2" t="s">
         <v>528</v>
       </c>
@@ -28001,7 +28001,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="467" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:21" ht="48.75">
       <c r="A467" s="2" t="s">
         <v>528</v>
       </c>
@@ -28066,7 +28066,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="468" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:21" ht="29.25">
       <c r="A468" s="2" t="s">
         <v>528</v>
       </c>
@@ -28131,7 +28131,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="469" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:21" ht="39">
       <c r="A469" s="2" t="s">
         <v>528</v>
       </c>
@@ -28196,7 +28196,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="470" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:21" ht="39">
       <c r="A470" s="2" t="s">
         <v>528</v>
       </c>
@@ -28261,7 +28261,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="471" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:21" ht="29.25">
       <c r="A471" s="2" t="s">
         <v>528</v>
       </c>
@@ -28312,7 +28312,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="472" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:21" ht="29.25">
       <c r="A472" s="2" t="s">
         <v>528</v>
       </c>
@@ -28377,7 +28377,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="473" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:21" ht="29.25">
       <c r="A473" s="2" t="s">
         <v>528</v>
       </c>
@@ -28442,7 +28442,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="474" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:21" ht="29.25">
       <c r="A474" s="2" t="s">
         <v>528</v>
       </c>
@@ -28499,7 +28499,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="475" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:21" ht="39">
       <c r="A475" s="2" t="s">
         <v>528</v>
       </c>
@@ -28538,7 +28538,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="476" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:21" ht="39">
       <c r="A476" s="2" t="s">
         <v>528</v>
       </c>
@@ -28603,7 +28603,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="477" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:21" ht="39">
       <c r="A477" s="2" t="s">
         <v>528</v>
       </c>
@@ -28668,8 +28668,8 @@
         <v>563</v>
       </c>
     </row>
-    <row r="478" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:21" ht="18" customHeight="1"/>
+    <row r="479" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A479" s="12" t="s">
         <v>566</v>
       </c>
@@ -28686,7 +28686,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="70" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="71" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okno serwisowe - aktualizacja Excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -1723,7 +1723,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 22-07-2025, 09:54</t>
+    <t>Last update: 26-08-2025, 09:18</t>
   </si>
 </sst>
 </file>
@@ -3219,7 +3219,9 @@
       <c r="S17" s="4">
         <v>15.2</v>
       </c>
-      <c r="T17" s="3"/>
+      <c r="T17" s="4">
+        <v>15.5</v>
+      </c>
       <c r="U17" s="2" t="s">
         <v>27</v>
       </c>
@@ -4162,7 +4164,9 @@
       <c r="R33" s="4">
         <v>2.5</v>
       </c>
-      <c r="S33" s="3"/>
+      <c r="S33" s="4">
+        <v>2.5</v>
+      </c>
       <c r="T33" s="3"/>
       <c r="U33" s="2" t="s">
         <v>70</v>
@@ -4208,12 +4212,14 @@
         <v>7.4</v>
       </c>
       <c r="Q34" s="4">
-        <v>7.5</v>
+        <v>7.6</v>
       </c>
       <c r="R34" s="4">
-        <v>5.4</v>
-      </c>
-      <c r="S34" s="3"/>
+        <v>5.5</v>
+      </c>
+      <c r="S34" s="4">
+        <v>3.4</v>
+      </c>
       <c r="T34" s="3"/>
       <c r="U34" s="2" t="s">
         <v>73</v>
@@ -4259,12 +4265,14 @@
         <v>9.1</v>
       </c>
       <c r="Q35" s="4">
-        <v>9.1</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="R35" s="4">
         <v>6.5</v>
       </c>
-      <c r="S35" s="3"/>
+      <c r="S35" s="4">
+        <v>4.2</v>
+      </c>
       <c r="T35" s="3"/>
       <c r="U35" s="2" t="s">
         <v>73</v>
@@ -4310,12 +4318,14 @@
         <v>5.7</v>
       </c>
       <c r="Q36" s="4">
-        <v>5.9</v>
+        <v>6</v>
       </c>
       <c r="R36" s="4">
         <v>4.4000000000000004</v>
       </c>
-      <c r="S36" s="3"/>
+      <c r="S36" s="4">
+        <v>2.7</v>
+      </c>
       <c r="T36" s="3"/>
       <c r="U36" s="2" t="s">
         <v>73</v>
@@ -4366,7 +4376,9 @@
       <c r="R37" s="4">
         <v>0.9</v>
       </c>
-      <c r="S37" s="3"/>
+      <c r="S37" s="4">
+        <v>0.5</v>
+      </c>
       <c r="T37" s="3"/>
       <c r="U37" s="2" t="s">
         <v>73</v>
@@ -4415,9 +4427,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="R38" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="S38" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="S38" s="4">
+        <v>0.5</v>
+      </c>
       <c r="T38" s="3"/>
       <c r="U38" s="2" t="s">
         <v>73</v>
@@ -4468,7 +4482,9 @@
       <c r="R39" s="4">
         <v>0.8</v>
       </c>
-      <c r="S39" s="3"/>
+      <c r="S39" s="4">
+        <v>0.5</v>
+      </c>
       <c r="T39" s="3"/>
       <c r="U39" s="2" t="s">
         <v>73</v>
@@ -5319,7 +5335,9 @@
       <c r="S53" s="4">
         <v>4.5999999999999996</v>
       </c>
-      <c r="T53" s="3"/>
+      <c r="T53" s="4">
+        <v>4.4000000000000004</v>
+      </c>
       <c r="U53" s="2" t="s">
         <v>27</v>
       </c>
@@ -5382,7 +5400,9 @@
       <c r="S54" s="4">
         <v>4</v>
       </c>
-      <c r="T54" s="3"/>
+      <c r="T54" s="4">
+        <v>4.9000000000000004</v>
+      </c>
       <c r="U54" s="2" t="s">
         <v>27</v>
       </c>
@@ -5445,7 +5465,9 @@
       <c r="S55" s="4">
         <v>5.2</v>
       </c>
-      <c r="T55" s="3"/>
+      <c r="T55" s="4">
+        <v>3.9</v>
+      </c>
       <c r="U55" s="2" t="s">
         <v>27</v>
       </c>
@@ -5508,7 +5530,9 @@
       <c r="S56" s="4">
         <v>2.6</v>
       </c>
-      <c r="T56" s="3"/>
+      <c r="T56" s="4">
+        <v>2.4</v>
+      </c>
       <c r="U56" s="2" t="s">
         <v>27</v>
       </c>
@@ -5571,7 +5595,9 @@
       <c r="S57" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="T57" s="3"/>
+      <c r="T57" s="4">
+        <v>2.8</v>
+      </c>
       <c r="U57" s="2" t="s">
         <v>27</v>
       </c>
@@ -5634,7 +5660,9 @@
       <c r="S58" s="4">
         <v>3</v>
       </c>
-      <c r="T58" s="3"/>
+      <c r="T58" s="4">
+        <v>2</v>
+      </c>
       <c r="U58" s="2" t="s">
         <v>27</v>
       </c>
@@ -6884,7 +6912,9 @@
       <c r="S78" s="4">
         <v>2.4</v>
       </c>
-      <c r="T78" s="3"/>
+      <c r="T78" s="4">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="U78" s="2" t="s">
         <v>27</v>
       </c>
@@ -6947,7 +6977,9 @@
       <c r="S79" s="4">
         <v>0</v>
       </c>
-      <c r="T79" s="3"/>
+      <c r="T79" s="4">
+        <v>0</v>
+      </c>
       <c r="U79" s="2" t="s">
         <v>27</v>
       </c>
@@ -7010,7 +7042,9 @@
       <c r="S80" s="4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="T80" s="3"/>
+      <c r="T80" s="4">
+        <v>4.5</v>
+      </c>
       <c r="U80" s="2" t="s">
         <v>27</v>
       </c>
@@ -7581,7 +7615,9 @@
       <c r="S91" s="5">
         <v>3.11</v>
       </c>
-      <c r="T91" s="3"/>
+      <c r="T91" s="5">
+        <v>6.03</v>
+      </c>
       <c r="U91" s="2" t="s">
         <v>96</v>
       </c>
@@ -8270,7 +8306,9 @@
       <c r="S106" s="4">
         <v>102.5</v>
       </c>
-      <c r="T106" s="3"/>
+      <c r="T106" s="4">
+        <v>103</v>
+      </c>
       <c r="U106" s="2" t="s">
         <v>27</v>
       </c>
@@ -8333,7 +8371,9 @@
       <c r="S107" s="4">
         <v>102.4</v>
       </c>
-      <c r="T107" s="3"/>
+      <c r="T107" s="4">
+        <v>103</v>
+      </c>
       <c r="U107" s="2" t="s">
         <v>27</v>
       </c>
@@ -8396,7 +8436,9 @@
       <c r="S108" s="4">
         <v>102.6</v>
       </c>
-      <c r="T108" s="3"/>
+      <c r="T108" s="4">
+        <v>103.1</v>
+      </c>
       <c r="U108" s="2" t="s">
         <v>27</v>
       </c>
@@ -9303,7 +9345,9 @@
       <c r="R126" s="5">
         <v>1</v>
       </c>
-      <c r="S126" s="3"/>
+      <c r="S126" s="5">
+        <v>1</v>
+      </c>
       <c r="T126" s="3"/>
       <c r="U126" s="2" t="s">
         <v>174</v>
@@ -10352,7 +10396,9 @@
       <c r="S150" s="5">
         <v>7.99</v>
       </c>
-      <c r="T150" s="3"/>
+      <c r="T150" s="5">
+        <v>9.7899999999999991</v>
+      </c>
       <c r="U150" s="2" t="s">
         <v>96</v>
       </c>
@@ -10677,7 +10723,9 @@
       <c r="R156" s="6">
         <v>87</v>
       </c>
-      <c r="S156" s="3"/>
+      <c r="S156" s="6">
+        <v>77</v>
+      </c>
       <c r="T156" s="3"/>
       <c r="U156" s="2" t="s">
         <v>27</v>
@@ -12634,13 +12682,17 @@
         <v>92.2</v>
       </c>
       <c r="P199" s="4">
-        <v>92.7</v>
+        <v>92.2</v>
       </c>
       <c r="Q199" s="4">
-        <v>92.8</v>
-      </c>
-      <c r="R199" s="3"/>
-      <c r="S199" s="3"/>
+        <v>92.4</v>
+      </c>
+      <c r="R199" s="4">
+        <v>92.5</v>
+      </c>
+      <c r="S199" s="4">
+        <v>92.6</v>
+      </c>
       <c r="T199" s="3"/>
       <c r="U199" s="2" t="s">
         <v>27</v>
@@ -12693,13 +12745,17 @@
         <v>71.2</v>
       </c>
       <c r="P200" s="4">
-        <v>71.5</v>
+        <v>71.599999999999994</v>
       </c>
       <c r="Q200" s="4">
         <v>71.900000000000006</v>
       </c>
-      <c r="R200" s="3"/>
-      <c r="S200" s="3"/>
+      <c r="R200" s="4">
+        <v>72.3</v>
+      </c>
+      <c r="S200" s="4">
+        <v>72.599999999999994</v>
+      </c>
       <c r="T200" s="3"/>
       <c r="U200" s="2" t="s">
         <v>27</v>
@@ -12901,7 +12957,9 @@
       <c r="R204" s="4">
         <v>56.9</v>
       </c>
-      <c r="S204" s="3"/>
+      <c r="S204" s="4">
+        <v>64.5</v>
+      </c>
       <c r="T204" s="3"/>
       <c r="U204" s="2" t="s">
         <v>258</v>
@@ -12962,7 +13020,9 @@
       <c r="R205" s="4">
         <v>17</v>
       </c>
-      <c r="S205" s="3"/>
+      <c r="S205" s="4">
+        <v>15</v>
+      </c>
       <c r="T205" s="3"/>
       <c r="U205" s="2" t="s">
         <v>260</v>
@@ -13070,7 +13130,9 @@
       <c r="R207" s="6">
         <v>152963</v>
       </c>
-      <c r="S207" s="3"/>
+      <c r="S207" s="6">
+        <v>152964</v>
+      </c>
       <c r="T207" s="3"/>
       <c r="U207" s="2" t="s">
         <v>265</v>
@@ -13128,7 +13190,9 @@
       <c r="S208" s="5">
         <v>0.51</v>
       </c>
-      <c r="T208" s="3"/>
+      <c r="T208" s="5">
+        <v>0.69</v>
+      </c>
       <c r="U208" s="2" t="s">
         <v>96</v>
       </c>
@@ -13405,7 +13469,9 @@
       <c r="S213" s="5">
         <v>4.2699999999999996</v>
       </c>
-      <c r="T213" s="3"/>
+      <c r="T213" s="5">
+        <v>8.32</v>
+      </c>
       <c r="U213" s="2" t="s">
         <v>96</v>
       </c>
@@ -15430,7 +15496,9 @@
       <c r="S250" s="4">
         <v>6.9</v>
       </c>
-      <c r="T250" s="3"/>
+      <c r="T250" s="4">
+        <v>7</v>
+      </c>
       <c r="U250" s="2" t="s">
         <v>27</v>
       </c>
@@ -17654,7 +17722,9 @@
       <c r="S290" s="5">
         <v>37.71</v>
       </c>
-      <c r="T290" s="3"/>
+      <c r="T290" s="5">
+        <v>46.56</v>
+      </c>
       <c r="U290" s="2" t="s">
         <v>96</v>
       </c>
@@ -19498,7 +19568,9 @@
       <c r="S320" s="5">
         <v>2580.38</v>
       </c>
-      <c r="T320" s="3"/>
+      <c r="T320" s="5">
+        <v>1840.15</v>
+      </c>
       <c r="U320" s="2" t="s">
         <v>381</v>
       </c>
@@ -19561,7 +19633,9 @@
       <c r="S321" s="5">
         <v>1701.94</v>
       </c>
-      <c r="T321" s="3"/>
+      <c r="T321" s="5">
+        <v>705.25</v>
+      </c>
       <c r="U321" s="2" t="s">
         <v>381</v>
       </c>
@@ -19624,7 +19698,9 @@
       <c r="S322" s="5">
         <v>8.06</v>
       </c>
-      <c r="T322" s="3"/>
+      <c r="T322" s="5">
+        <v>12.96</v>
+      </c>
       <c r="U322" s="2" t="s">
         <v>381</v>
       </c>
@@ -19687,7 +19763,9 @@
       <c r="S323" s="5">
         <v>6.36</v>
       </c>
-      <c r="T323" s="3"/>
+      <c r="T323" s="5">
+        <v>1.79</v>
+      </c>
       <c r="U323" s="2" t="s">
         <v>381</v>
       </c>
@@ -19750,7 +19828,9 @@
       <c r="S324" s="5">
         <v>254.4</v>
       </c>
-      <c r="T324" s="3"/>
+      <c r="T324" s="5">
+        <v>199.97</v>
+      </c>
       <c r="U324" s="2" t="s">
         <v>381</v>
       </c>
@@ -19813,7 +19893,9 @@
       <c r="S325" s="5">
         <v>62.44</v>
       </c>
-      <c r="T325" s="3"/>
+      <c r="T325" s="5">
+        <v>87.2</v>
+      </c>
       <c r="U325" s="2" t="s">
         <v>381</v>
       </c>
@@ -23359,12 +23441,16 @@
         <v>58.7</v>
       </c>
       <c r="O383" s="4">
-        <v>55.5</v>
+        <v>58.2</v>
       </c>
       <c r="P383" s="3"/>
       <c r="Q383" s="3"/>
-      <c r="R383" s="3"/>
-      <c r="S383" s="3"/>
+      <c r="R383" s="4">
+        <v>64</v>
+      </c>
+      <c r="S383" s="4">
+        <v>67.400000000000006</v>
+      </c>
       <c r="T383" s="3"/>
       <c r="U383" s="2" t="s">
         <v>442</v>
@@ -24134,9 +24220,11 @@
         <v>9.59</v>
       </c>
       <c r="S396" s="5">
-        <v>4.22</v>
-      </c>
-      <c r="T396" s="3"/>
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="T396" s="5">
+        <v>8.32</v>
+      </c>
       <c r="U396" s="2" t="s">
         <v>96</v>
       </c>
@@ -24199,7 +24287,9 @@
       <c r="S397" s="6">
         <v>67</v>
       </c>
-      <c r="T397" s="3"/>
+      <c r="T397" s="6">
+        <v>67</v>
+      </c>
       <c r="U397" s="2" t="s">
         <v>464</v>
       </c>
@@ -24262,7 +24352,9 @@
       <c r="S398" s="6">
         <v>17</v>
       </c>
-      <c r="T398" s="3"/>
+      <c r="T398" s="6">
+        <v>0</v>
+      </c>
       <c r="U398" s="2" t="s">
         <v>464</v>
       </c>
@@ -24325,7 +24417,9 @@
       <c r="S399" s="6">
         <v>17</v>
       </c>
-      <c r="T399" s="3"/>
+      <c r="T399" s="6">
+        <v>50</v>
+      </c>
       <c r="U399" s="2" t="s">
         <v>464</v>
       </c>
@@ -24388,7 +24482,9 @@
       <c r="S400" s="6">
         <v>17</v>
       </c>
-      <c r="T400" s="3"/>
+      <c r="T400" s="6">
+        <v>25</v>
+      </c>
       <c r="U400" s="2" t="s">
         <v>464</v>
       </c>
@@ -24577,7 +24673,9 @@
       <c r="S403" s="4">
         <v>98.3</v>
       </c>
-      <c r="T403" s="3"/>
+      <c r="T403" s="4">
+        <v>98.3</v>
+      </c>
       <c r="U403" s="2" t="s">
         <v>27</v>
       </c>
@@ -24685,7 +24783,9 @@
       <c r="S405" s="6">
         <v>95</v>
       </c>
-      <c r="T405" s="3"/>
+      <c r="T405" s="6">
+        <v>95</v>
+      </c>
       <c r="U405" s="2" t="s">
         <v>477</v>
       </c>
@@ -24835,7 +24935,9 @@
       <c r="S409" s="4">
         <v>66.599999999999994</v>
       </c>
-      <c r="T409" s="3"/>
+      <c r="T409" s="4">
+        <v>66.599999999999994</v>
+      </c>
       <c r="U409" s="2" t="s">
         <v>477</v>
       </c>
@@ -24880,7 +24982,9 @@
       <c r="S410" s="4">
         <v>99.2</v>
       </c>
-      <c r="T410" s="3"/>
+      <c r="T410" s="4">
+        <v>99.1</v>
+      </c>
       <c r="U410" s="2" t="s">
         <v>477</v>
       </c>
@@ -24925,7 +25029,9 @@
       <c r="S411" s="4">
         <v>94.3</v>
       </c>
-      <c r="T411" s="3"/>
+      <c r="T411" s="4">
+        <v>93.5</v>
+      </c>
       <c r="U411" s="2" t="s">
         <v>477</v>
       </c>
@@ -25175,7 +25281,9 @@
       <c r="S415" s="5">
         <v>1.41</v>
       </c>
-      <c r="T415" s="3"/>
+      <c r="T415" s="5">
+        <v>1.93</v>
+      </c>
       <c r="U415" s="2" t="s">
         <v>96</v>
       </c>
@@ -25232,7 +25340,9 @@
       <c r="S416" s="5">
         <v>1.41</v>
       </c>
-      <c r="T416" s="3"/>
+      <c r="T416" s="5">
+        <v>1.93</v>
+      </c>
       <c r="U416" s="2" t="s">
         <v>96</v>
       </c>
@@ -27059,48 +27169,50 @@
         <v>26</v>
       </c>
       <c r="F452" s="4">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G452" s="4">
+        <v>17.7</v>
+      </c>
+      <c r="H452" s="4">
+        <v>17.7</v>
+      </c>
+      <c r="I452" s="4">
+        <v>17</v>
+      </c>
+      <c r="J452" s="4">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="K452" s="4">
+        <v>16</v>
+      </c>
+      <c r="L452" s="4">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="M452" s="4">
         <v>17.5</v>
       </c>
-      <c r="G452" s="4">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="H452" s="4">
+      <c r="N452" s="4">
+        <v>17.7</v>
+      </c>
+      <c r="O452" s="4">
+        <v>17.3</v>
+      </c>
+      <c r="P452" s="4">
         <v>17.8</v>
       </c>
-      <c r="I452" s="4">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="J452" s="4">
-        <v>16.7</v>
-      </c>
-      <c r="K452" s="4">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="L452" s="4">
-        <v>17</v>
-      </c>
-      <c r="M452" s="4">
-        <v>17.7</v>
-      </c>
-      <c r="N452" s="4">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="O452" s="4">
-        <v>17.5</v>
-      </c>
-      <c r="P452" s="4">
-        <v>18</v>
-      </c>
       <c r="Q452" s="4">
-        <v>18.8</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="R452" s="4">
-        <v>16.399999999999999</v>
+        <v>16.3</v>
       </c>
       <c r="S452" s="4">
         <v>16.8</v>
       </c>
-      <c r="T452" s="3"/>
+      <c r="T452" s="4">
+        <v>17.100000000000001</v>
+      </c>
       <c r="U452" s="2" t="s">
         <v>486</v>
       </c>
@@ -27163,7 +27275,9 @@
       <c r="S453" s="4">
         <v>88.3</v>
       </c>
-      <c r="T453" s="3"/>
+      <c r="T453" s="4">
+        <v>89.2</v>
+      </c>
       <c r="U453" s="2" t="s">
         <v>486</v>
       </c>
@@ -27226,7 +27340,9 @@
       <c r="S454" s="5">
         <v>0.33</v>
       </c>
-      <c r="T454" s="3"/>
+      <c r="T454" s="5">
+        <v>0.21</v>
+      </c>
       <c r="U454" s="2" t="s">
         <v>96</v>
       </c>
@@ -27289,7 +27405,9 @@
       <c r="S455" s="9">
         <v>1E-3</v>
       </c>
-      <c r="T455" s="3"/>
+      <c r="T455" s="9">
+        <v>1.5E-3</v>
+      </c>
       <c r="U455" s="2" t="s">
         <v>96</v>
       </c>
@@ -27352,7 +27470,9 @@
       <c r="S456" s="4">
         <v>1.9</v>
       </c>
-      <c r="T456" s="3"/>
+      <c r="T456" s="4">
+        <v>1.2</v>
+      </c>
       <c r="U456" s="2" t="s">
         <v>535</v>
       </c>
@@ -27415,7 +27535,9 @@
       <c r="S457" s="4">
         <v>1</v>
       </c>
-      <c r="T457" s="3"/>
+      <c r="T457" s="4">
+        <v>1</v>
+      </c>
       <c r="U457" s="2" t="s">
         <v>317</v>
       </c>
@@ -27478,7 +27600,9 @@
       <c r="S458" s="4">
         <v>3.1</v>
       </c>
-      <c r="T458" s="3"/>
+      <c r="T458" s="4">
+        <v>3.5</v>
+      </c>
       <c r="U458" s="2" t="s">
         <v>538</v>
       </c>
@@ -28494,7 +28618,9 @@
       <c r="S474" s="5">
         <v>0</v>
       </c>
-      <c r="T474" s="3"/>
+      <c r="T474" s="5">
+        <v>0</v>
+      </c>
       <c r="U474" s="2" t="s">
         <v>559</v>
       </c>

</xml_diff>

<commit_message>
Okienko 09.09.2025 - aktualizacja EXCEL
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dregerj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1723,7 +1723,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 26-08-2025, 09:18</t>
+    <t>Last update: 09-09-2025, 14:17</t>
   </si>
 </sst>
 </file>
@@ -1738,7 +1738,7 @@
     <numFmt numFmtId="168" formatCode="[$-10809]0.000000;\-0.000000;0.000000"/>
     <numFmt numFmtId="169" formatCode="[$-10809]0.0000;\-0.0000;0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2278,7 +2278,7 @@
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -2289,17 +2289,17 @@
     <col min="21" max="21" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="36" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="19.5">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="19.5">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="19.5">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="29.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="97.5">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="97.5">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="97.5">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="19.5">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="29.25">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="29.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="29.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="68.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="29.25">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="29.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="29.25">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="39">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="39">
       <c r="A30" s="2" t="s">
         <v>22</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="39">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="39">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="19.5">
       <c r="A33" s="2" t="s">
         <v>68</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="29.25">
       <c r="A34" s="2" t="s">
         <v>68</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="29.25">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="29.25">
       <c r="A36" s="2" t="s">
         <v>68</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="29.25">
       <c r="A37" s="2" t="s">
         <v>68</v>
       </c>
@@ -4384,7 +4384,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="29.25">
       <c r="A38" s="2" t="s">
         <v>68</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="29.25">
       <c r="A39" s="2" t="s">
         <v>68</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="39">
       <c r="A40" s="2" t="s">
         <v>68</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="97.5">
       <c r="A41" s="2" t="s">
         <v>68</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="97.5">
       <c r="A42" s="2" t="s">
         <v>68</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="97.5">
       <c r="A43" s="2" t="s">
         <v>68</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="97.5">
       <c r="A44" s="2" t="s">
         <v>68</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="97.5">
       <c r="A45" s="2" t="s">
         <v>68</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="81" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="97.5">
       <c r="A46" s="2" t="s">
         <v>68</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="48.75">
       <c r="A47" s="2" t="s">
         <v>68</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="48.75">
       <c r="A48" s="2" t="s">
         <v>68</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="19.5">
       <c r="A49" s="2" t="s">
         <v>68</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="29.25">
       <c r="A50" s="2" t="s">
         <v>68</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="19.5">
       <c r="A51" s="2" t="s">
         <v>97</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="19.5">
       <c r="A52" s="2" t="s">
         <v>97</v>
       </c>
@@ -5277,7 +5277,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>97</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>97</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>97</v>
       </c>
@@ -5472,7 +5472,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>97</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>97</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>97</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="29.25">
       <c r="A59" s="2" t="s">
         <v>97</v>
       </c>
@@ -5684,53 +5684,55 @@
         <v>49</v>
       </c>
       <c r="F59" s="6">
-        <v>1070</v>
+        <v>1146</v>
       </c>
       <c r="G59" s="6">
-        <v>1079</v>
+        <v>1185</v>
       </c>
       <c r="H59" s="6">
-        <v>1085</v>
+        <v>1200</v>
       </c>
       <c r="I59" s="6">
-        <v>1093</v>
+        <v>1233</v>
       </c>
       <c r="J59" s="6">
-        <v>1109</v>
+        <v>1264</v>
       </c>
       <c r="K59" s="6">
-        <v>1134</v>
+        <v>1291</v>
       </c>
       <c r="L59" s="6">
-        <v>1167</v>
+        <v>1290</v>
       </c>
       <c r="M59" s="6">
-        <v>1208</v>
+        <v>1278</v>
       </c>
       <c r="N59" s="6">
-        <v>1256</v>
+        <v>1282</v>
       </c>
       <c r="O59" s="6">
-        <v>1311</v>
+        <v>1293</v>
       </c>
       <c r="P59" s="6">
-        <v>1375</v>
+        <v>1296</v>
       </c>
       <c r="Q59" s="6">
-        <v>1453</v>
+        <v>1259</v>
       </c>
       <c r="R59" s="6">
-        <v>1548</v>
+        <v>1259</v>
       </c>
       <c r="S59" s="6">
-        <v>1664</v>
-      </c>
-      <c r="T59" s="3"/>
+        <v>1259</v>
+      </c>
+      <c r="T59" s="6">
+        <v>1259</v>
+      </c>
       <c r="U59" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>97</v>
       </c>
@@ -5793,7 +5795,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="29.25">
       <c r="A61" s="2" t="s">
         <v>97</v>
       </c>
@@ -5858,7 +5860,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="29.25">
       <c r="A62" s="2" t="s">
         <v>97</v>
       </c>
@@ -5923,7 +5925,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="29.25">
       <c r="A63" s="2" t="s">
         <v>97</v>
       </c>
@@ -5988,7 +5990,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="19.5">
       <c r="A64" s="2" t="s">
         <v>97</v>
       </c>
@@ -6051,7 +6053,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" ht="29.25">
       <c r="A65" s="2" t="s">
         <v>97</v>
       </c>
@@ -6116,7 +6118,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="29.25">
       <c r="A66" s="2" t="s">
         <v>97</v>
       </c>
@@ -6181,7 +6183,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="29.25">
       <c r="A67" s="2" t="s">
         <v>97</v>
       </c>
@@ -6246,7 +6248,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="29.25">
       <c r="A68" s="2" t="s">
         <v>97</v>
       </c>
@@ -6309,7 +6311,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="29.25">
       <c r="A69" s="2" t="s">
         <v>97</v>
       </c>
@@ -6372,7 +6374,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="29.25">
       <c r="A70" s="2" t="s">
         <v>97</v>
       </c>
@@ -6435,7 +6437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" ht="29.25">
       <c r="A71" s="2" t="s">
         <v>97</v>
       </c>
@@ -6498,7 +6500,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" ht="19.5">
       <c r="A72" s="2" t="s">
         <v>97</v>
       </c>
@@ -6561,7 +6563,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" ht="19.5">
       <c r="A73" s="2" t="s">
         <v>97</v>
       </c>
@@ -6624,7 +6626,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="19.5">
       <c r="A74" s="2" t="s">
         <v>97</v>
       </c>
@@ -6687,7 +6689,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" ht="19.5">
       <c r="A75" s="2" t="s">
         <v>97</v>
       </c>
@@ -6750,7 +6752,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" ht="29.25">
       <c r="A76" s="2" t="s">
         <v>97</v>
       </c>
@@ -6813,7 +6815,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="77" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="29.25">
       <c r="A77" s="2" t="s">
         <v>97</v>
       </c>
@@ -6854,7 +6856,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" ht="19.5">
       <c r="A78" s="2" t="s">
         <v>97</v>
       </c>
@@ -6919,7 +6921,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" ht="19.5">
       <c r="A79" s="2" t="s">
         <v>97</v>
       </c>
@@ -6984,7 +6986,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" ht="19.5">
       <c r="A80" s="2" t="s">
         <v>97</v>
       </c>
@@ -7049,7 +7051,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" ht="19.5">
       <c r="A81" s="2" t="s">
         <v>97</v>
       </c>
@@ -7094,7 +7096,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" ht="29.25">
       <c r="A82" s="2" t="s">
         <v>97</v>
       </c>
@@ -7153,7 +7155,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" ht="29.25">
       <c r="A83" s="2" t="s">
         <v>97</v>
       </c>
@@ -7212,7 +7214,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="84" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" ht="19.5">
       <c r="A84" s="2" t="s">
         <v>97</v>
       </c>
@@ -7249,7 +7251,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" ht="29.25">
       <c r="A85" s="2" t="s">
         <v>97</v>
       </c>
@@ -7286,7 +7288,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="86" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" ht="19.5">
       <c r="A86" s="2" t="s">
         <v>97</v>
       </c>
@@ -7349,7 +7351,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" ht="19.5">
       <c r="A87" s="2" t="s">
         <v>97</v>
       </c>
@@ -7390,7 +7392,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" ht="19.5">
       <c r="A88" s="2" t="s">
         <v>97</v>
       </c>
@@ -7453,7 +7455,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="89" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" ht="19.5">
       <c r="A89" s="2" t="s">
         <v>97</v>
       </c>
@@ -7516,7 +7518,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="90" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" ht="19.5">
       <c r="A90" s="2" t="s">
         <v>97</v>
       </c>
@@ -7563,7 +7565,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="91" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" ht="29.25">
       <c r="A91" s="2" t="s">
         <v>97</v>
       </c>
@@ -7622,7 +7624,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" ht="19.5">
       <c r="A92" s="2" t="s">
         <v>97</v>
       </c>
@@ -7667,7 +7669,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" ht="19.5">
       <c r="A93" s="2" t="s">
         <v>97</v>
       </c>
@@ -7712,7 +7714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" ht="19.5">
       <c r="A94" s="2" t="s">
         <v>97</v>
       </c>
@@ -7757,7 +7759,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" ht="19.5">
       <c r="A95" s="2" t="s">
         <v>97</v>
       </c>
@@ -7816,7 +7818,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" ht="78">
       <c r="A96" s="2" t="s">
         <v>151</v>
       </c>
@@ -7857,7 +7859,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" ht="78">
       <c r="A97" s="2" t="s">
         <v>151</v>
       </c>
@@ -7898,7 +7900,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="98" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" ht="78">
       <c r="A98" s="2" t="s">
         <v>151</v>
       </c>
@@ -7939,7 +7941,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="99" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" ht="78">
       <c r="A99" s="2" t="s">
         <v>151</v>
       </c>
@@ -7984,7 +7986,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="100" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" ht="78">
       <c r="A100" s="2" t="s">
         <v>151</v>
       </c>
@@ -8029,7 +8031,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" ht="78">
       <c r="A101" s="2" t="s">
         <v>151</v>
       </c>
@@ -8074,7 +8076,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" ht="78">
       <c r="A102" s="2" t="s">
         <v>151</v>
       </c>
@@ -8119,7 +8121,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="103" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" ht="78">
       <c r="A103" s="2" t="s">
         <v>151</v>
       </c>
@@ -8164,7 +8166,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" ht="78">
       <c r="A104" s="2" t="s">
         <v>151</v>
       </c>
@@ -8209,7 +8211,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" ht="29.25">
       <c r="A105" s="2" t="s">
         <v>151</v>
       </c>
@@ -8248,7 +8250,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="106" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" ht="19.5">
       <c r="A106" s="2" t="s">
         <v>151</v>
       </c>
@@ -8313,7 +8315,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" ht="19.5">
       <c r="A107" s="2" t="s">
         <v>151</v>
       </c>
@@ -8378,7 +8380,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" ht="19.5">
       <c r="A108" s="2" t="s">
         <v>151</v>
       </c>
@@ -8443,7 +8445,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" ht="19.5">
       <c r="A109" s="2" t="s">
         <v>151</v>
       </c>
@@ -8482,7 +8484,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" ht="19.5">
       <c r="A110" s="2" t="s">
         <v>151</v>
       </c>
@@ -8521,7 +8523,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="111" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" ht="19.5">
       <c r="A111" s="2" t="s">
         <v>151</v>
       </c>
@@ -8560,7 +8562,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" ht="29.25">
       <c r="A112" s="2" t="s">
         <v>151</v>
       </c>
@@ -8607,7 +8609,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" ht="19.5">
       <c r="A113" s="2" t="s">
         <v>151</v>
       </c>
@@ -8662,7 +8664,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" ht="39">
       <c r="A114" s="2" t="s">
         <v>151</v>
       </c>
@@ -8717,7 +8719,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" ht="48.75">
       <c r="A115" s="2" t="s">
         <v>151</v>
       </c>
@@ -8772,7 +8774,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" ht="58.5">
       <c r="A116" s="2" t="s">
         <v>151</v>
       </c>
@@ -8827,7 +8829,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="117" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" ht="29.25">
       <c r="A117" s="2" t="s">
         <v>151</v>
       </c>
@@ -8882,7 +8884,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="118" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" ht="29.25">
       <c r="A118" s="2" t="s">
         <v>151</v>
       </c>
@@ -8929,7 +8931,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" ht="19.5">
       <c r="A119" s="2" t="s">
         <v>151</v>
       </c>
@@ -8984,7 +8986,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" ht="39">
       <c r="A120" s="2" t="s">
         <v>151</v>
       </c>
@@ -9039,7 +9041,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" ht="48.75">
       <c r="A121" s="2" t="s">
         <v>151</v>
       </c>
@@ -9094,7 +9096,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="122" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" ht="58.5">
       <c r="A122" s="2" t="s">
         <v>151</v>
       </c>
@@ -9149,7 +9151,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="123" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" ht="29.25">
       <c r="A123" s="2" t="s">
         <v>151</v>
       </c>
@@ -9204,7 +9206,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="124" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" ht="48.75">
       <c r="A124" s="2" t="s">
         <v>151</v>
       </c>
@@ -9247,7 +9249,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="125" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:21" ht="48.75">
       <c r="A125" s="2" t="s">
         <v>151</v>
       </c>
@@ -9290,7 +9292,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="126" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:21" ht="29.25">
       <c r="A126" s="2" t="s">
         <v>151</v>
       </c>
@@ -9353,7 +9355,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="127" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:21" ht="29.25">
       <c r="A127" s="2" t="s">
         <v>151</v>
       </c>
@@ -9390,7 +9392,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:21" ht="29.25">
       <c r="A128" s="2" t="s">
         <v>151</v>
       </c>
@@ -9427,7 +9429,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="129" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:21" ht="29.25">
       <c r="A129" s="2" t="s">
         <v>151</v>
       </c>
@@ -9464,7 +9466,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:21" ht="29.25">
       <c r="A130" s="2" t="s">
         <v>151</v>
       </c>
@@ -9501,7 +9503,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="131" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:21" ht="29.25">
       <c r="A131" s="2" t="s">
         <v>151</v>
       </c>
@@ -9538,7 +9540,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="132" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:21" ht="29.25">
       <c r="A132" s="2" t="s">
         <v>151</v>
       </c>
@@ -9575,7 +9577,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="133" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:21" ht="29.25">
       <c r="A133" s="2" t="s">
         <v>151</v>
       </c>
@@ -9612,7 +9614,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="134" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:21" ht="29.25">
       <c r="A134" s="2" t="s">
         <v>151</v>
       </c>
@@ -9649,7 +9651,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="135" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:21" ht="29.25">
       <c r="A135" s="2" t="s">
         <v>151</v>
       </c>
@@ -9686,7 +9688,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="136" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:21" ht="29.25">
       <c r="A136" s="2" t="s">
         <v>151</v>
       </c>
@@ -9723,7 +9725,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="137" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:21" ht="29.25">
       <c r="A137" s="2" t="s">
         <v>151</v>
       </c>
@@ -9760,7 +9762,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="138" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:21" ht="29.25">
       <c r="A138" s="2" t="s">
         <v>151</v>
       </c>
@@ -9797,7 +9799,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="139" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:21" ht="29.25">
       <c r="A139" s="2" t="s">
         <v>151</v>
       </c>
@@ -9834,7 +9836,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="140" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:21" ht="29.25">
       <c r="A140" s="2" t="s">
         <v>151</v>
       </c>
@@ -9871,7 +9873,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="141" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:21" ht="29.25">
       <c r="A141" s="2" t="s">
         <v>151</v>
       </c>
@@ -9908,7 +9910,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="142" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:21" ht="29.25">
       <c r="A142" s="2" t="s">
         <v>151</v>
       </c>
@@ -9945,7 +9947,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="143" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:21" ht="48.75">
       <c r="A143" s="2" t="s">
         <v>151</v>
       </c>
@@ -10010,7 +10012,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="144" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:21" ht="58.5">
       <c r="A144" s="2" t="s">
         <v>151</v>
       </c>
@@ -10075,7 +10077,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:21" ht="58.5">
       <c r="A145" s="2" t="s">
         <v>151</v>
       </c>
@@ -10112,7 +10114,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="146" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:21" ht="58.5">
       <c r="A146" s="2" t="s">
         <v>151</v>
       </c>
@@ -10149,7 +10151,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="147" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:21" ht="58.5">
       <c r="A147" s="2" t="s">
         <v>151</v>
       </c>
@@ -10214,7 +10216,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="148" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:21" ht="58.5">
       <c r="A148" s="2" t="s">
         <v>151</v>
       </c>
@@ -10279,7 +10281,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="149" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:21" ht="58.5">
       <c r="A149" s="2" t="s">
         <v>151</v>
       </c>
@@ -10344,7 +10346,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="150" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:21" ht="29.25">
       <c r="A150" s="2" t="s">
         <v>151</v>
       </c>
@@ -10403,7 +10405,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="151" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" ht="58.5">
       <c r="A151" s="2" t="s">
         <v>151</v>
       </c>
@@ -10460,7 +10462,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="152" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:21" ht="58.5">
       <c r="A152" s="2" t="s">
         <v>151</v>
       </c>
@@ -10517,7 +10519,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="153" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:21" ht="58.5">
       <c r="A153" s="2" t="s">
         <v>151</v>
       </c>
@@ -10574,7 +10576,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="154" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:21" ht="58.5">
       <c r="A154" s="2" t="s">
         <v>151</v>
       </c>
@@ -10631,7 +10633,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="155" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:21" ht="29.25">
       <c r="A155" s="2" t="s">
         <v>207</v>
       </c>
@@ -10668,7 +10670,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="156" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:21" ht="19.5">
       <c r="A156" s="2" t="s">
         <v>207</v>
       </c>
@@ -10731,7 +10733,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="157" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:21" ht="39">
       <c r="A157" s="2" t="s">
         <v>207</v>
       </c>
@@ -10770,7 +10772,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="158" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:21" ht="39">
       <c r="A158" s="2" t="s">
         <v>207</v>
       </c>
@@ -10809,7 +10811,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="159" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:21" ht="39">
       <c r="A159" s="2" t="s">
         <v>207</v>
       </c>
@@ -10848,7 +10850,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="160" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:21" ht="39">
       <c r="A160" s="2" t="s">
         <v>207</v>
       </c>
@@ -10887,7 +10889,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="161" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" ht="39">
       <c r="A161" s="2" t="s">
         <v>207</v>
       </c>
@@ -10926,7 +10928,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="162" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:21" ht="19.5">
       <c r="A162" s="2" t="s">
         <v>207</v>
       </c>
@@ -10965,7 +10967,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="163" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:21" ht="19.5">
       <c r="A163" s="2" t="s">
         <v>207</v>
       </c>
@@ -11004,7 +11006,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="164" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:21" ht="19.5">
       <c r="A164" s="2" t="s">
         <v>207</v>
       </c>
@@ -11043,7 +11045,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="165" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:21" ht="19.5">
       <c r="A165" s="2" t="s">
         <v>207</v>
       </c>
@@ -11082,7 +11084,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="166" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:21" ht="19.5">
       <c r="A166" s="2" t="s">
         <v>207</v>
       </c>
@@ -11121,7 +11123,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="167" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:21" ht="19.5">
       <c r="A167" s="2" t="s">
         <v>207</v>
       </c>
@@ -11160,7 +11162,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="168" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:21" ht="19.5">
       <c r="A168" s="2" t="s">
         <v>207</v>
       </c>
@@ -11199,7 +11201,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="169" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:21" ht="19.5">
       <c r="A169" s="2" t="s">
         <v>207</v>
       </c>
@@ -11238,7 +11240,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="170" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:21" ht="29.25">
       <c r="A170" s="2" t="s">
         <v>207</v>
       </c>
@@ -11281,7 +11283,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="171" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:21" ht="29.25">
       <c r="A171" s="2" t="s">
         <v>207</v>
       </c>
@@ -11324,7 +11326,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="172" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:21" ht="29.25">
       <c r="A172" s="2" t="s">
         <v>207</v>
       </c>
@@ -11387,7 +11389,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="173" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:21" ht="29.25">
       <c r="A173" s="2" t="s">
         <v>207</v>
       </c>
@@ -11450,7 +11452,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="174" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:21" ht="29.25">
       <c r="A174" s="2" t="s">
         <v>207</v>
       </c>
@@ -11513,7 +11515,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="175" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:21" ht="29.25">
       <c r="A175" s="2" t="s">
         <v>207</v>
       </c>
@@ -11576,7 +11578,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="176" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:21" ht="29.25">
       <c r="A176" s="2" t="s">
         <v>207</v>
       </c>
@@ -11639,7 +11641,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="177" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:21" ht="19.5">
       <c r="A177" s="2" t="s">
         <v>207</v>
       </c>
@@ -11688,7 +11690,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="178" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:21" ht="39">
       <c r="A178" s="2" t="s">
         <v>207</v>
       </c>
@@ -11737,7 +11739,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="179" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:21" ht="19.5">
       <c r="A179" s="2" t="s">
         <v>207</v>
       </c>
@@ -11786,7 +11788,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="180" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:21" ht="39">
       <c r="A180" s="2" t="s">
         <v>207</v>
       </c>
@@ -11835,7 +11837,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="181" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:21" ht="39">
       <c r="A181" s="2" t="s">
         <v>207</v>
       </c>
@@ -11884,7 +11886,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="182" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:21" ht="39">
       <c r="A182" s="2" t="s">
         <v>207</v>
       </c>
@@ -11933,7 +11935,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="183" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:21" ht="39">
       <c r="A183" s="2" t="s">
         <v>207</v>
       </c>
@@ -11982,7 +11984,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="184" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:21" ht="39">
       <c r="A184" s="2" t="s">
         <v>207</v>
       </c>
@@ -12023,7 +12025,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="185" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:21" ht="39">
       <c r="A185" s="2" t="s">
         <v>207</v>
       </c>
@@ -12064,7 +12066,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="186" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:21" ht="39">
       <c r="A186" s="2" t="s">
         <v>207</v>
       </c>
@@ -12105,7 +12107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="187" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:21" ht="39">
       <c r="A187" s="2" t="s">
         <v>207</v>
       </c>
@@ -12146,7 +12148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="188" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:21" ht="39">
       <c r="A188" s="2" t="s">
         <v>207</v>
       </c>
@@ -12187,7 +12189,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="189" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:21" ht="39">
       <c r="A189" s="2" t="s">
         <v>207</v>
       </c>
@@ -12228,7 +12230,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="190" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:21" ht="39">
       <c r="A190" s="2" t="s">
         <v>207</v>
       </c>
@@ -12269,7 +12271,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="191" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:21" ht="39">
       <c r="A191" s="2" t="s">
         <v>207</v>
       </c>
@@ -12310,7 +12312,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="192" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:21" ht="39">
       <c r="A192" s="2" t="s">
         <v>207</v>
       </c>
@@ -12351,7 +12353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="193" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:21" ht="39">
       <c r="A193" s="2" t="s">
         <v>207</v>
       </c>
@@ -12392,7 +12394,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="194" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:21" ht="39">
       <c r="A194" s="2" t="s">
         <v>207</v>
       </c>
@@ -12433,7 +12435,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="195" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:21" ht="39">
       <c r="A195" s="2" t="s">
         <v>207</v>
       </c>
@@ -12474,7 +12476,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="196" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:21" ht="19.5">
       <c r="A196" s="2" t="s">
         <v>207</v>
       </c>
@@ -12517,7 +12519,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="197" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:21" ht="19.5">
       <c r="A197" s="2" t="s">
         <v>207</v>
       </c>
@@ -12576,7 +12578,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="198" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:21" ht="19.5">
       <c r="A198" s="2" t="s">
         <v>207</v>
       </c>
@@ -12635,7 +12637,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="199" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:21" ht="19.5">
       <c r="A199" s="2" t="s">
         <v>247</v>
       </c>
@@ -12698,7 +12700,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="200" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:21" ht="29.25">
       <c r="A200" s="2" t="s">
         <v>247</v>
       </c>
@@ -12761,7 +12763,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="201" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:21" ht="19.5">
       <c r="A201" s="2" t="s">
         <v>247</v>
       </c>
@@ -12824,7 +12826,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="202" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:21" ht="19.5">
       <c r="A202" s="2" t="s">
         <v>247</v>
       </c>
@@ -12863,7 +12865,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="203" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:21" ht="19.5">
       <c r="A203" s="2" t="s">
         <v>247</v>
       </c>
@@ -12902,7 +12904,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="204" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:21" ht="29.25">
       <c r="A204" s="2" t="s">
         <v>247</v>
       </c>
@@ -12965,7 +12967,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="205" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:21" ht="19.5">
       <c r="A205" s="2" t="s">
         <v>247</v>
       </c>
@@ -13028,7 +13030,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="206" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:21" ht="19.5">
       <c r="A206" s="2" t="s">
         <v>247</v>
       </c>
@@ -13075,7 +13077,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="207" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:21" ht="29.25">
       <c r="A207" s="2" t="s">
         <v>247</v>
       </c>
@@ -13138,7 +13140,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="208" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:21" ht="29.25">
       <c r="A208" s="2" t="s">
         <v>247</v>
       </c>
@@ -13197,7 +13199,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="209" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:21" ht="39">
       <c r="A209" s="2" t="s">
         <v>247</v>
       </c>
@@ -13260,7 +13262,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="210" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:21" ht="19.5">
       <c r="A210" s="2" t="s">
         <v>268</v>
       </c>
@@ -13297,7 +13299,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="211" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:21" ht="19.5">
       <c r="A211" s="2" t="s">
         <v>268</v>
       </c>
@@ -13360,7 +13362,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="212" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:21" ht="29.25">
       <c r="A212" s="2" t="s">
         <v>268</v>
       </c>
@@ -13417,7 +13419,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="213" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:21" ht="29.25">
       <c r="A213" s="2" t="s">
         <v>268</v>
       </c>
@@ -13476,7 +13478,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="214" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:21" ht="29.25">
       <c r="A214" s="2" t="s">
         <v>275</v>
       </c>
@@ -13541,7 +13543,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="215" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:21" ht="29.25">
       <c r="A215" s="2" t="s">
         <v>275</v>
       </c>
@@ -13604,7 +13606,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="216" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:21" ht="29.25">
       <c r="A216" s="2" t="s">
         <v>275</v>
       </c>
@@ -13647,7 +13649,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="217" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:21" ht="29.25">
       <c r="A217" s="2" t="s">
         <v>275</v>
       </c>
@@ -13690,7 +13692,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="218" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:21" ht="29.25">
       <c r="A218" s="2" t="s">
         <v>275</v>
       </c>
@@ -13733,7 +13735,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:21" ht="29.25">
       <c r="A219" s="2" t="s">
         <v>275</v>
       </c>
@@ -13796,7 +13798,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="220" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:21" ht="29.25">
       <c r="A220" s="2" t="s">
         <v>275</v>
       </c>
@@ -13859,7 +13861,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="221" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:21" ht="29.25">
       <c r="A221" s="2" t="s">
         <v>275</v>
       </c>
@@ -13922,7 +13924,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="222" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:21" ht="29.25">
       <c r="A222" s="2" t="s">
         <v>275</v>
       </c>
@@ -13971,7 +13973,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="223" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:21" ht="29.25">
       <c r="A223" s="2" t="s">
         <v>275</v>
       </c>
@@ -14020,7 +14022,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="224" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:21" ht="29.25">
       <c r="A224" s="2" t="s">
         <v>275</v>
       </c>
@@ -14069,7 +14071,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="225" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:21" ht="29.25">
       <c r="A225" s="2" t="s">
         <v>275</v>
       </c>
@@ -14118,7 +14120,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="226" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:21" ht="29.25">
       <c r="A226" s="2" t="s">
         <v>275</v>
       </c>
@@ -14167,7 +14169,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="227" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:21" ht="29.25">
       <c r="A227" s="2" t="s">
         <v>275</v>
       </c>
@@ -14216,7 +14218,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="228" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:21" ht="29.25">
       <c r="A228" s="2" t="s">
         <v>275</v>
       </c>
@@ -14265,7 +14267,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="229" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:21" ht="29.25">
       <c r="A229" s="2" t="s">
         <v>275</v>
       </c>
@@ -14314,7 +14316,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="230" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:21" ht="39">
       <c r="A230" s="2" t="s">
         <v>275</v>
       </c>
@@ -14363,7 +14365,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="231" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:21" ht="29.25">
       <c r="A231" s="2" t="s">
         <v>275</v>
       </c>
@@ -14412,7 +14414,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="232" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:21" ht="39">
       <c r="A232" s="2" t="s">
         <v>275</v>
       </c>
@@ -14461,7 +14463,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="233" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:21" ht="29.25">
       <c r="A233" s="2" t="s">
         <v>275</v>
       </c>
@@ -14510,7 +14512,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="234" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:21" ht="29.25">
       <c r="A234" s="2" t="s">
         <v>275</v>
       </c>
@@ -14559,7 +14561,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="235" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:21" ht="29.25">
       <c r="A235" s="2" t="s">
         <v>275</v>
       </c>
@@ -14608,7 +14610,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="236" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:21" ht="29.25">
       <c r="A236" s="2" t="s">
         <v>275</v>
       </c>
@@ -14657,7 +14659,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="237" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:21" ht="29.25">
       <c r="A237" s="2" t="s">
         <v>275</v>
       </c>
@@ -14706,7 +14708,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="238" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:21" ht="29.25">
       <c r="A238" s="2" t="s">
         <v>275</v>
       </c>
@@ -14755,7 +14757,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="239" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:21" ht="29.25">
       <c r="A239" s="2" t="s">
         <v>275</v>
       </c>
@@ -14804,7 +14806,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="240" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:21" ht="29.25">
       <c r="A240" s="2" t="s">
         <v>275</v>
       </c>
@@ -14853,7 +14855,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="241" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:21" ht="29.25">
       <c r="A241" s="2" t="s">
         <v>275</v>
       </c>
@@ -14918,7 +14920,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="242" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:21" ht="29.25">
       <c r="A242" s="2" t="s">
         <v>275</v>
       </c>
@@ -14983,7 +14985,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="243" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:21" ht="29.25">
       <c r="A243" s="2" t="s">
         <v>275</v>
       </c>
@@ -15048,7 +15050,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="244" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:21" ht="29.25">
       <c r="A244" s="2" t="s">
         <v>275</v>
       </c>
@@ -15113,7 +15115,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="245" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:21" ht="29.25">
       <c r="A245" s="2" t="s">
         <v>275</v>
       </c>
@@ -15178,7 +15180,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="246" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:21" ht="29.25">
       <c r="A246" s="2" t="s">
         <v>275</v>
       </c>
@@ -15243,7 +15245,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="247" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:21" ht="29.25">
       <c r="A247" s="2" t="s">
         <v>275</v>
       </c>
@@ -15308,7 +15310,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="248" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:21" ht="29.25">
       <c r="A248" s="2" t="s">
         <v>275</v>
       </c>
@@ -15373,7 +15375,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="249" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:21" ht="29.25">
       <c r="A249" s="2" t="s">
         <v>275</v>
       </c>
@@ -15438,7 +15440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="250" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:21" ht="29.25">
       <c r="A250" s="2" t="s">
         <v>275</v>
       </c>
@@ -15503,7 +15505,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="251" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:21" ht="29.25">
       <c r="A251" s="2" t="s">
         <v>275</v>
       </c>
@@ -15566,7 +15568,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="252" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:21" ht="29.25">
       <c r="A252" s="2" t="s">
         <v>275</v>
       </c>
@@ -15629,7 +15631,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="253" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:21" ht="39">
       <c r="A253" s="2" t="s">
         <v>275</v>
       </c>
@@ -15672,7 +15674,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="254" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:21" ht="39">
       <c r="A254" s="2" t="s">
         <v>275</v>
       </c>
@@ -15715,7 +15717,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="255" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:21" ht="39">
       <c r="A255" s="2" t="s">
         <v>275</v>
       </c>
@@ -15758,7 +15760,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="256" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:21" ht="29.25">
       <c r="A256" s="2" t="s">
         <v>275</v>
       </c>
@@ -15821,7 +15823,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="257" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:21" ht="48.75">
       <c r="A257" s="2" t="s">
         <v>275</v>
       </c>
@@ -15880,7 +15882,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="258" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:21" ht="29.25">
       <c r="A258" s="2" t="s">
         <v>275</v>
       </c>
@@ -15917,7 +15919,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="259" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:21" ht="29.25">
       <c r="A259" s="2" t="s">
         <v>275</v>
       </c>
@@ -15954,7 +15956,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="260" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:21" ht="29.25">
       <c r="A260" s="2" t="s">
         <v>275</v>
       </c>
@@ -15991,7 +15993,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="261" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:21" ht="29.25">
       <c r="A261" s="2" t="s">
         <v>275</v>
       </c>
@@ -16028,7 +16030,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="262" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:21" ht="29.25">
       <c r="A262" s="2" t="s">
         <v>275</v>
       </c>
@@ -16065,7 +16067,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="263" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:21" ht="29.25">
       <c r="A263" s="2" t="s">
         <v>275</v>
       </c>
@@ -16102,7 +16104,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="264" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:21" ht="29.25">
       <c r="A264" s="2" t="s">
         <v>275</v>
       </c>
@@ -16139,7 +16141,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="265" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:21" ht="29.25">
       <c r="A265" s="2" t="s">
         <v>275</v>
       </c>
@@ -16176,7 +16178,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="266" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:21" ht="29.25">
       <c r="A266" s="2" t="s">
         <v>275</v>
       </c>
@@ -16229,7 +16231,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="267" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:21" ht="29.25">
       <c r="A267" s="2" t="s">
         <v>320</v>
       </c>
@@ -16292,7 +16294,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="268" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:21" ht="29.25">
       <c r="A268" s="2" t="s">
         <v>320</v>
       </c>
@@ -16355,7 +16357,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="269" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:21" ht="29.25">
       <c r="A269" s="2" t="s">
         <v>320</v>
       </c>
@@ -16418,7 +16420,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="270" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:21" ht="29.25">
       <c r="A270" s="2" t="s">
         <v>320</v>
       </c>
@@ -16481,7 +16483,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="271" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:21" ht="29.25">
       <c r="A271" s="2" t="s">
         <v>320</v>
       </c>
@@ -16544,7 +16546,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="272" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:21" ht="29.25">
       <c r="A272" s="2" t="s">
         <v>320</v>
       </c>
@@ -16607,7 +16609,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="273" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:21" ht="29.25">
       <c r="A273" s="2" t="s">
         <v>320</v>
       </c>
@@ -16670,7 +16672,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="274" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:21" ht="29.25">
       <c r="A274" s="2" t="s">
         <v>320</v>
       </c>
@@ -16733,7 +16735,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="275" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:21" ht="29.25">
       <c r="A275" s="2" t="s">
         <v>320</v>
       </c>
@@ -16796,7 +16798,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="276" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:21" ht="29.25">
       <c r="A276" s="2" t="s">
         <v>320</v>
       </c>
@@ -16859,7 +16861,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="277" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:21" ht="29.25">
       <c r="A277" s="2" t="s">
         <v>320</v>
       </c>
@@ -16922,7 +16924,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="278" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:21" ht="29.25">
       <c r="A278" s="2" t="s">
         <v>320</v>
       </c>
@@ -16987,7 +16989,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="279" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:21" ht="29.25">
       <c r="A279" s="2" t="s">
         <v>320</v>
       </c>
@@ -17050,7 +17052,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="280" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:21" ht="29.25">
       <c r="A280" s="2" t="s">
         <v>320</v>
       </c>
@@ -17113,7 +17115,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="281" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:21" ht="29.25">
       <c r="A281" s="2" t="s">
         <v>320</v>
       </c>
@@ -17176,7 +17178,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="282" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:21" ht="29.25">
       <c r="A282" s="2" t="s">
         <v>320</v>
       </c>
@@ -17239,7 +17241,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="283" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:21" ht="29.25">
       <c r="A283" s="2" t="s">
         <v>320</v>
       </c>
@@ -17302,7 +17304,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="284" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:21" ht="29.25">
       <c r="A284" s="2" t="s">
         <v>320</v>
       </c>
@@ -17365,7 +17367,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="285" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:21" ht="29.25">
       <c r="A285" s="2" t="s">
         <v>320</v>
       </c>
@@ -17428,7 +17430,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="286" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:21" ht="29.25">
       <c r="A286" s="2" t="s">
         <v>320</v>
       </c>
@@ -17491,7 +17493,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="287" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:21" ht="29.25">
       <c r="A287" s="2" t="s">
         <v>320</v>
       </c>
@@ -17544,7 +17546,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="288" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:21" ht="29.25">
       <c r="A288" s="2" t="s">
         <v>320</v>
       </c>
@@ -17607,7 +17609,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="289" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:21" ht="29.25">
       <c r="A289" s="2" t="s">
         <v>320</v>
       </c>
@@ -17670,7 +17672,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="290" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:21" ht="29.25">
       <c r="A290" s="2" t="s">
         <v>320</v>
       </c>
@@ -17729,7 +17731,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="291" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:21" ht="29.25">
       <c r="A291" s="2" t="s">
         <v>320</v>
       </c>
@@ -17784,7 +17786,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="292" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:21" ht="39">
       <c r="A292" s="2" t="s">
         <v>320</v>
       </c>
@@ -17837,7 +17839,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="293" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:21" ht="39">
       <c r="A293" s="2" t="s">
         <v>320</v>
       </c>
@@ -17892,7 +17894,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="294" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:21" ht="19.5">
       <c r="A294" s="2" t="s">
         <v>352</v>
       </c>
@@ -17955,7 +17957,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="295" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:21" ht="68.25">
       <c r="A295" s="2" t="s">
         <v>352</v>
       </c>
@@ -18018,7 +18020,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="296" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:21" ht="19.5">
       <c r="A296" s="2" t="s">
         <v>352</v>
       </c>
@@ -18081,7 +18083,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="297" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:21" ht="19.5">
       <c r="A297" s="2" t="s">
         <v>352</v>
       </c>
@@ -18144,7 +18146,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="298" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:21" ht="19.5">
       <c r="A298" s="2" t="s">
         <v>352</v>
       </c>
@@ -18207,7 +18209,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="299" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:21" ht="19.5">
       <c r="A299" s="2" t="s">
         <v>352</v>
       </c>
@@ -18270,7 +18272,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="300" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:21" ht="19.5">
       <c r="A300" s="2" t="s">
         <v>352</v>
       </c>
@@ -18333,7 +18335,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="301" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:21" ht="19.5">
       <c r="A301" s="2" t="s">
         <v>352</v>
       </c>
@@ -18396,7 +18398,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="302" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:21" ht="19.5">
       <c r="A302" s="2" t="s">
         <v>352</v>
       </c>
@@ -18459,7 +18461,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="303" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:21" ht="19.5">
       <c r="A303" s="2" t="s">
         <v>352</v>
       </c>
@@ -18522,7 +18524,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="304" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:21" ht="19.5">
       <c r="A304" s="2" t="s">
         <v>352</v>
       </c>
@@ -18585,7 +18587,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="305" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:21" ht="19.5">
       <c r="A305" s="2" t="s">
         <v>352</v>
       </c>
@@ -18626,7 +18628,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="306" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:21" ht="19.5">
       <c r="A306" s="2" t="s">
         <v>352</v>
       </c>
@@ -18689,7 +18691,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="307" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:21" ht="39">
       <c r="A307" s="2" t="s">
         <v>352</v>
       </c>
@@ -18752,7 +18754,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="308" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:21" ht="48.75">
       <c r="A308" s="2" t="s">
         <v>352</v>
       </c>
@@ -18815,7 +18817,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="309" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:21" ht="39">
       <c r="A309" s="2" t="s">
         <v>352</v>
       </c>
@@ -18878,7 +18880,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="310" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:21" ht="39">
       <c r="A310" s="2" t="s">
         <v>352</v>
       </c>
@@ -18941,7 +18943,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="311" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:21" ht="29.25">
       <c r="A311" s="2" t="s">
         <v>352</v>
       </c>
@@ -19004,7 +19006,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="312" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:21" ht="39">
       <c r="A312" s="2" t="s">
         <v>352</v>
       </c>
@@ -19067,7 +19069,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="313" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:21" ht="29.25">
       <c r="A313" s="2" t="s">
         <v>352</v>
       </c>
@@ -19130,7 +19132,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="314" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:21" ht="29.25">
       <c r="A314" s="2" t="s">
         <v>352</v>
       </c>
@@ -19193,7 +19195,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="315" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:21" ht="39">
       <c r="A315" s="2" t="s">
         <v>352</v>
       </c>
@@ -19256,7 +19258,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="316" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:21" ht="29.25">
       <c r="A316" s="2" t="s">
         <v>352</v>
       </c>
@@ -19319,7 +19321,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="317" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:21" ht="39">
       <c r="A317" s="2" t="s">
         <v>352</v>
       </c>
@@ -19382,7 +19384,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="318" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:21" ht="29.25">
       <c r="A318" s="2" t="s">
         <v>352</v>
       </c>
@@ -19445,7 +19447,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="319" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:21" ht="29.25">
       <c r="A319" s="2" t="s">
         <v>352</v>
       </c>
@@ -19510,7 +19512,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="320" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:21" ht="39">
       <c r="A320" s="2" t="s">
         <v>352</v>
       </c>
@@ -19575,7 +19577,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="321" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:21" ht="39">
       <c r="A321" s="2" t="s">
         <v>352</v>
       </c>
@@ -19640,7 +19642,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="322" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:21" ht="68.25">
       <c r="A322" s="2" t="s">
         <v>352</v>
       </c>
@@ -19705,7 +19707,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="323" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:21" ht="58.5">
       <c r="A323" s="2" t="s">
         <v>352</v>
       </c>
@@ -19770,7 +19772,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="324" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:21" ht="68.25">
       <c r="A324" s="2" t="s">
         <v>352</v>
       </c>
@@ -19835,7 +19837,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="325" spans="1:21" ht="72" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:21" ht="68.25">
       <c r="A325" s="2" t="s">
         <v>352</v>
       </c>
@@ -19900,7 +19902,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="326" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:21" ht="39">
       <c r="A326" s="2" t="s">
         <v>352</v>
       </c>
@@ -19963,7 +19965,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="327" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:21" ht="68.25">
       <c r="A327" s="2" t="s">
         <v>352</v>
       </c>
@@ -20026,7 +20028,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="328" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:21" ht="58.5">
       <c r="A328" s="2" t="s">
         <v>352</v>
       </c>
@@ -20089,7 +20091,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="329" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:21" ht="68.25">
       <c r="A329" s="2" t="s">
         <v>352</v>
       </c>
@@ -20152,7 +20154,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="330" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:21" ht="68.25">
       <c r="A330" s="2" t="s">
         <v>352</v>
       </c>
@@ -20215,7 +20217,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="331" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:21" ht="29.25">
       <c r="A331" s="2" t="s">
         <v>393</v>
       </c>
@@ -20274,7 +20276,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="332" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:21" ht="29.25">
       <c r="A332" s="2" t="s">
         <v>393</v>
       </c>
@@ -20333,7 +20335,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="333" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:21" ht="29.25">
       <c r="A333" s="2" t="s">
         <v>393</v>
       </c>
@@ -20392,7 +20394,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="334" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:21" ht="29.25">
       <c r="A334" s="2" t="s">
         <v>393</v>
       </c>
@@ -20455,7 +20457,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="335" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:21" ht="29.25">
       <c r="A335" s="2" t="s">
         <v>393</v>
       </c>
@@ -20518,7 +20520,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="336" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:21" ht="29.25">
       <c r="A336" s="2" t="s">
         <v>393</v>
       </c>
@@ -20581,7 +20583,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="337" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:21" ht="29.25">
       <c r="A337" s="2" t="s">
         <v>393</v>
       </c>
@@ -20644,7 +20646,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="338" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:21" ht="29.25">
       <c r="A338" s="2" t="s">
         <v>393</v>
       </c>
@@ -20707,7 +20709,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="339" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:21" ht="29.25">
       <c r="A339" s="2" t="s">
         <v>393</v>
       </c>
@@ -20770,7 +20772,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="340" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:21" ht="29.25">
       <c r="A340" s="2" t="s">
         <v>393</v>
       </c>
@@ -20833,7 +20835,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="341" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:21" ht="29.25">
       <c r="A341" s="2" t="s">
         <v>393</v>
       </c>
@@ -20896,7 +20898,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="342" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:21" ht="29.25">
       <c r="A342" s="2" t="s">
         <v>393</v>
       </c>
@@ -20959,7 +20961,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="343" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:21" ht="29.25">
       <c r="A343" s="2" t="s">
         <v>393</v>
       </c>
@@ -21022,7 +21024,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="344" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:21" ht="29.25">
       <c r="A344" s="2" t="s">
         <v>393</v>
       </c>
@@ -21085,7 +21087,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="345" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:21" ht="29.25">
       <c r="A345" s="2" t="s">
         <v>393</v>
       </c>
@@ -21148,7 +21150,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="346" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:21" ht="29.25">
       <c r="A346" s="2" t="s">
         <v>393</v>
       </c>
@@ -21211,7 +21213,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="347" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:21" ht="29.25">
       <c r="A347" s="2" t="s">
         <v>393</v>
       </c>
@@ -21274,7 +21276,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="348" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:21" ht="29.25">
       <c r="A348" s="2" t="s">
         <v>393</v>
       </c>
@@ -21337,7 +21339,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="349" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:21" ht="29.25">
       <c r="A349" s="2" t="s">
         <v>393</v>
       </c>
@@ -21400,7 +21402,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="350" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:21" ht="29.25">
       <c r="A350" s="2" t="s">
         <v>393</v>
       </c>
@@ -21463,7 +21465,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="351" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:21" ht="29.25">
       <c r="A351" s="2" t="s">
         <v>393</v>
       </c>
@@ -21526,7 +21528,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="352" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:21" ht="29.25">
       <c r="A352" s="2" t="s">
         <v>393</v>
       </c>
@@ -21589,7 +21591,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="353" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:21" ht="29.25">
       <c r="A353" s="2" t="s">
         <v>393</v>
       </c>
@@ -21652,7 +21654,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="354" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:21" ht="29.25">
       <c r="A354" s="2" t="s">
         <v>393</v>
       </c>
@@ -21715,7 +21717,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="355" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:21" ht="29.25">
       <c r="A355" s="2" t="s">
         <v>393</v>
       </c>
@@ -21778,7 +21780,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="356" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:21" ht="29.25">
       <c r="A356" s="2" t="s">
         <v>393</v>
       </c>
@@ -21841,7 +21843,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="357" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:21" ht="29.25">
       <c r="A357" s="2" t="s">
         <v>393</v>
       </c>
@@ -21904,7 +21906,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="358" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:21" ht="29.25">
       <c r="A358" s="2" t="s">
         <v>393</v>
       </c>
@@ -21965,7 +21967,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="359" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:21" ht="29.25">
       <c r="A359" s="2" t="s">
         <v>393</v>
       </c>
@@ -22028,7 +22030,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="360" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:21" ht="29.25">
       <c r="A360" s="2" t="s">
         <v>393</v>
       </c>
@@ -22091,7 +22093,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="361" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:21" ht="29.25">
       <c r="A361" s="2" t="s">
         <v>393</v>
       </c>
@@ -22154,7 +22156,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="362" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:21" ht="29.25">
       <c r="A362" s="2" t="s">
         <v>393</v>
       </c>
@@ -22217,7 +22219,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="363" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:21" ht="29.25">
       <c r="A363" s="2" t="s">
         <v>393</v>
       </c>
@@ -22280,7 +22282,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="364" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:21" ht="39">
       <c r="A364" s="2" t="s">
         <v>393</v>
       </c>
@@ -22343,7 +22345,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="365" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:21" ht="39">
       <c r="A365" s="2" t="s">
         <v>393</v>
       </c>
@@ -22406,7 +22408,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="366" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:21" ht="39">
       <c r="A366" s="2" t="s">
         <v>393</v>
       </c>
@@ -22469,7 +22471,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="367" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:21" ht="39">
       <c r="A367" s="2" t="s">
         <v>393</v>
       </c>
@@ -22532,7 +22534,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="368" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:21" ht="39">
       <c r="A368" s="2" t="s">
         <v>393</v>
       </c>
@@ -22595,7 +22597,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="369" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:21" ht="39">
       <c r="A369" s="2" t="s">
         <v>393</v>
       </c>
@@ -22658,7 +22660,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="370" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:21" ht="39">
       <c r="A370" s="2" t="s">
         <v>393</v>
       </c>
@@ -22721,7 +22723,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="371" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:21" ht="39">
       <c r="A371" s="2" t="s">
         <v>393</v>
       </c>
@@ -22784,7 +22786,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="372" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:21" ht="29.25">
       <c r="A372" s="2" t="s">
         <v>393</v>
       </c>
@@ -22839,7 +22841,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="373" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:21" ht="68.25">
       <c r="A373" s="2" t="s">
         <v>393</v>
       </c>
@@ -22894,7 +22896,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="374" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:21" ht="29.25">
       <c r="A374" s="2" t="s">
         <v>393</v>
       </c>
@@ -22949,7 +22951,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="375" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:21" ht="29.25">
       <c r="A375" s="2" t="s">
         <v>393</v>
       </c>
@@ -23004,7 +23006,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="376" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:21" ht="39">
       <c r="A376" s="2" t="s">
         <v>428</v>
       </c>
@@ -23067,7 +23069,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="377" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:21" ht="39">
       <c r="A377" s="2" t="s">
         <v>428</v>
       </c>
@@ -23130,7 +23132,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="378" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:21" ht="39">
       <c r="A378" s="2" t="s">
         <v>428</v>
       </c>
@@ -23193,7 +23195,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="379" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:21" ht="48.75">
       <c r="A379" s="2" t="s">
         <v>428</v>
       </c>
@@ -23256,7 +23258,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="380" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:21" ht="39">
       <c r="A380" s="2" t="s">
         <v>428</v>
       </c>
@@ -23303,7 +23305,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="381" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:21" ht="39">
       <c r="A381" s="2" t="s">
         <v>428</v>
       </c>
@@ -23350,7 +23352,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="382" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:21" ht="39">
       <c r="A382" s="2" t="s">
         <v>428</v>
       </c>
@@ -23397,7 +23399,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="383" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:21" ht="39">
       <c r="A383" s="2" t="s">
         <v>428</v>
       </c>
@@ -23456,7 +23458,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="384" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:21" ht="39">
       <c r="A384" s="2" t="s">
         <v>428</v>
       </c>
@@ -23503,7 +23505,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="385" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:21" ht="39">
       <c r="A385" s="2" t="s">
         <v>428</v>
       </c>
@@ -23568,7 +23570,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="386" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:21" ht="48.75">
       <c r="A386" s="2" t="s">
         <v>428</v>
       </c>
@@ -23633,7 +23635,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="387" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:21" ht="29.25">
       <c r="A387" s="2" t="s">
         <v>448</v>
       </c>
@@ -23696,7 +23698,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="388" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:21" ht="29.25">
       <c r="A388" s="2" t="s">
         <v>448</v>
       </c>
@@ -23759,7 +23761,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="389" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:21" ht="29.25">
       <c r="A389" s="2" t="s">
         <v>448</v>
       </c>
@@ -23814,7 +23816,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="390" spans="1:21" ht="63" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:21" ht="68.25">
       <c r="A390" s="2" t="s">
         <v>448</v>
       </c>
@@ -23869,7 +23871,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="391" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:21" ht="29.25">
       <c r="A391" s="2" t="s">
         <v>448</v>
       </c>
@@ -23924,7 +23926,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="392" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:21" ht="29.25">
       <c r="A392" s="2" t="s">
         <v>448</v>
       </c>
@@ -23979,7 +23981,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="393" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:21" ht="39">
       <c r="A393" s="2" t="s">
         <v>448</v>
       </c>
@@ -24044,7 +24046,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="394" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:21" ht="39">
       <c r="A394" s="2" t="s">
         <v>448</v>
       </c>
@@ -24105,7 +24107,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="395" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:21" ht="48.75">
       <c r="A395" s="2" t="s">
         <v>448</v>
       </c>
@@ -24170,7 +24172,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="396" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:21" ht="29.25">
       <c r="A396" s="2" t="s">
         <v>448</v>
       </c>
@@ -24229,7 +24231,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="397" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:21" ht="58.5">
       <c r="A397" s="2" t="s">
         <v>460</v>
       </c>
@@ -24294,7 +24296,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="398" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:21" ht="39">
       <c r="A398" s="2" t="s">
         <v>460</v>
       </c>
@@ -24359,7 +24361,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="399" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:21" ht="48.75">
       <c r="A399" s="2" t="s">
         <v>460</v>
       </c>
@@ -24424,7 +24426,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="400" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:21" ht="48.75">
       <c r="A400" s="2" t="s">
         <v>460</v>
       </c>
@@ -24489,7 +24491,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="401" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:21" ht="58.5">
       <c r="A401" s="2" t="s">
         <v>460</v>
       </c>
@@ -24552,7 +24554,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="402" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:21" ht="19.5">
       <c r="A402" s="2" t="s">
         <v>470</v>
       </c>
@@ -24610,12 +24612,14 @@
       <c r="S402" s="4">
         <v>31</v>
       </c>
-      <c r="T402" s="3"/>
+      <c r="T402" s="4">
+        <v>31</v>
+      </c>
       <c r="U402" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="403" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:21" ht="19.5">
       <c r="A403" s="2" t="s">
         <v>470</v>
       </c>
@@ -24680,7 +24684,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="404" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:21" ht="39">
       <c r="A404" s="2" t="s">
         <v>470</v>
       </c>
@@ -24743,7 +24747,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="405" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:21" ht="19.5">
       <c r="A405" s="2" t="s">
         <v>470</v>
       </c>
@@ -24790,7 +24794,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="406" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:21" ht="19.5">
       <c r="A406" s="2" t="s">
         <v>470</v>
       </c>
@@ -24825,7 +24829,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="407" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:21" ht="19.5">
       <c r="A407" s="2" t="s">
         <v>470</v>
       </c>
@@ -24860,7 +24864,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="408" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:21" ht="19.5">
       <c r="A408" s="2" t="s">
         <v>470</v>
       </c>
@@ -24895,7 +24899,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="409" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:21" ht="19.5">
       <c r="A409" s="2" t="s">
         <v>470</v>
       </c>
@@ -24942,7 +24946,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="410" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:21" ht="19.5">
       <c r="A410" s="2" t="s">
         <v>470</v>
       </c>
@@ -24989,7 +24993,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="411" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:21" ht="19.5">
       <c r="A411" s="2" t="s">
         <v>470</v>
       </c>
@@ -25036,7 +25040,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="412" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:21" ht="29.25">
       <c r="A412" s="2" t="s">
         <v>470</v>
       </c>
@@ -25101,7 +25105,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="413" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:21" ht="19.5">
       <c r="A413" s="2" t="s">
         <v>470</v>
       </c>
@@ -25164,7 +25168,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="414" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:21" ht="29.25">
       <c r="A414" s="2" t="s">
         <v>470</v>
       </c>
@@ -25229,7 +25233,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="415" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:21" ht="29.25">
       <c r="A415" s="2" t="s">
         <v>470</v>
       </c>
@@ -25288,7 +25292,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="416" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:21" ht="29.25">
       <c r="A416" s="2" t="s">
         <v>470</v>
       </c>
@@ -25347,7 +25351,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="417" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:21" ht="19.5">
       <c r="A417" s="2" t="s">
         <v>470</v>
       </c>
@@ -25410,7 +25414,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="418" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:21" ht="29.25">
       <c r="A418" s="2" t="s">
         <v>491</v>
       </c>
@@ -25473,7 +25477,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="419" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:21" ht="29.25">
       <c r="A419" s="2" t="s">
         <v>491</v>
       </c>
@@ -25538,7 +25542,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="420" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:21" ht="29.25">
       <c r="A420" s="2" t="s">
         <v>491</v>
       </c>
@@ -25583,7 +25587,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="421" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:21" ht="29.25">
       <c r="A421" s="2" t="s">
         <v>491</v>
       </c>
@@ -25642,7 +25646,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="422" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:21" ht="29.25">
       <c r="A422" s="2" t="s">
         <v>491</v>
       </c>
@@ -25688,12 +25692,14 @@
       <c r="S422" s="6">
         <v>1311</v>
       </c>
-      <c r="T422" s="3"/>
+      <c r="T422" s="6">
+        <v>1278</v>
+      </c>
       <c r="U422" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="423" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:21" ht="29.25">
       <c r="A423" s="2" t="s">
         <v>491</v>
       </c>
@@ -25739,12 +25745,14 @@
       <c r="S423" s="6">
         <v>156</v>
       </c>
-      <c r="T423" s="3"/>
+      <c r="T423" s="6">
+        <v>115</v>
+      </c>
       <c r="U423" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="424" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:21" ht="29.25">
       <c r="A424" s="2" t="s">
         <v>491</v>
       </c>
@@ -25790,12 +25798,14 @@
       <c r="S424" s="6">
         <v>1147</v>
       </c>
-      <c r="T424" s="3"/>
+      <c r="T424" s="6">
+        <v>1157</v>
+      </c>
       <c r="U424" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="425" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:21" ht="29.25">
       <c r="A425" s="2" t="s">
         <v>491</v>
       </c>
@@ -25841,12 +25851,14 @@
       <c r="S425" s="6">
         <v>1107</v>
       </c>
-      <c r="T425" s="3"/>
+      <c r="T425" s="6">
+        <v>1126</v>
+      </c>
       <c r="U425" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="426" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:21" ht="29.25">
       <c r="A426" s="2" t="s">
         <v>491</v>
       </c>
@@ -25892,12 +25904,14 @@
       <c r="S426" s="6">
         <v>141</v>
       </c>
-      <c r="T426" s="3"/>
+      <c r="T426" s="6">
+        <v>106</v>
+      </c>
       <c r="U426" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="427" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:21" ht="29.25">
       <c r="A427" s="2" t="s">
         <v>491</v>
       </c>
@@ -25943,12 +25957,14 @@
       <c r="S427" s="6">
         <v>958</v>
       </c>
-      <c r="T427" s="3"/>
+      <c r="T427" s="6">
+        <v>1014</v>
+      </c>
       <c r="U427" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="428" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:21" ht="39">
       <c r="A428" s="2" t="s">
         <v>491</v>
       </c>
@@ -25994,12 +26010,14 @@
       <c r="S428" s="6">
         <v>163</v>
       </c>
-      <c r="T428" s="3"/>
+      <c r="T428" s="6">
+        <v>104</v>
+      </c>
       <c r="U428" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="429" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:21" ht="48.75">
       <c r="A429" s="2" t="s">
         <v>491</v>
       </c>
@@ -26045,12 +26063,14 @@
       <c r="S429" s="6">
         <v>1</v>
       </c>
-      <c r="T429" s="3"/>
+      <c r="T429" s="6">
+        <v>0</v>
+      </c>
       <c r="U429" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="430" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:21" ht="39">
       <c r="A430" s="2" t="s">
         <v>491</v>
       </c>
@@ -26096,12 +26116,14 @@
       <c r="S430" s="6">
         <v>1093</v>
       </c>
-      <c r="T430" s="3"/>
+      <c r="T430" s="6">
+        <v>1125</v>
+      </c>
       <c r="U430" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="431" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:21" ht="39">
       <c r="A431" s="2" t="s">
         <v>491</v>
       </c>
@@ -26147,12 +26169,14 @@
       <c r="S431" s="6">
         <v>55</v>
       </c>
-      <c r="T431" s="3"/>
+      <c r="T431" s="6">
+        <v>49</v>
+      </c>
       <c r="U431" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="432" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:21" ht="29.25">
       <c r="A432" s="2" t="s">
         <v>491</v>
       </c>
@@ -26215,7 +26239,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="433" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:21" ht="29.25">
       <c r="A433" s="2" t="s">
         <v>491</v>
       </c>
@@ -26278,7 +26302,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="434" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:21" ht="29.25">
       <c r="A434" s="2" t="s">
         <v>491</v>
       </c>
@@ -26341,7 +26365,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="435" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:21" ht="29.25">
       <c r="A435" s="2" t="s">
         <v>491</v>
       </c>
@@ -26404,7 +26428,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="436" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:21" ht="29.25">
       <c r="A436" s="2" t="s">
         <v>491</v>
       </c>
@@ -26467,7 +26491,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="437" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:21" ht="29.25">
       <c r="A437" s="2" t="s">
         <v>491</v>
       </c>
@@ -26530,7 +26554,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="438" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:21" ht="39">
       <c r="A438" s="2" t="s">
         <v>491</v>
       </c>
@@ -26573,7 +26597,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="439" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:21" ht="39">
       <c r="A439" s="2" t="s">
         <v>491</v>
       </c>
@@ -26616,7 +26640,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="440" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:21" ht="39">
       <c r="A440" s="2" t="s">
         <v>491</v>
       </c>
@@ -26659,7 +26683,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="441" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:21" ht="39">
       <c r="A441" s="2" t="s">
         <v>491</v>
       </c>
@@ -26702,7 +26726,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="442" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:21" ht="39">
       <c r="A442" s="2" t="s">
         <v>491</v>
       </c>
@@ -26745,7 +26769,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="443" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:21" ht="39">
       <c r="A443" s="2" t="s">
         <v>491</v>
       </c>
@@ -26788,7 +26812,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="444" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:21" ht="39">
       <c r="A444" s="2" t="s">
         <v>491</v>
       </c>
@@ -26831,7 +26855,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="445" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:21" ht="39">
       <c r="A445" s="2" t="s">
         <v>491</v>
       </c>
@@ -26874,7 +26898,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="446" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:21" ht="39">
       <c r="A446" s="2" t="s">
         <v>491</v>
       </c>
@@ -26917,7 +26941,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="447" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:21" ht="39">
       <c r="A447" s="2" t="s">
         <v>491</v>
       </c>
@@ -26960,7 +26984,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="448" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:21" ht="39">
       <c r="A448" s="2" t="s">
         <v>491</v>
       </c>
@@ -27003,7 +27027,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="449" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:21" ht="39">
       <c r="A449" s="2" t="s">
         <v>491</v>
       </c>
@@ -27046,7 +27070,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="450" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:21" ht="29.25">
       <c r="A450" s="2" t="s">
         <v>491</v>
       </c>
@@ -27111,7 +27135,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="451" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:21" ht="29.25">
       <c r="A451" s="2" t="s">
         <v>491</v>
       </c>
@@ -27152,7 +27176,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="452" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:21" ht="29.25">
       <c r="A452" s="2" t="s">
         <v>528</v>
       </c>
@@ -27217,7 +27241,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="453" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:21" ht="29.25">
       <c r="A453" s="2" t="s">
         <v>528</v>
       </c>
@@ -27282,7 +27306,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="454" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:21" ht="29.25">
       <c r="A454" s="2" t="s">
         <v>528</v>
       </c>
@@ -27347,7 +27371,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="455" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:21" ht="29.25">
       <c r="A455" s="2" t="s">
         <v>528</v>
       </c>
@@ -27412,7 +27436,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="456" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:21" ht="48.75">
       <c r="A456" s="2" t="s">
         <v>528</v>
       </c>
@@ -27477,7 +27501,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="457" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:21" ht="29.25">
       <c r="A457" s="2" t="s">
         <v>528</v>
       </c>
@@ -27542,7 +27566,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="458" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:21" ht="29.25">
       <c r="A458" s="2" t="s">
         <v>528</v>
       </c>
@@ -27607,7 +27631,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="459" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:21" ht="29.25">
       <c r="A459" s="2" t="s">
         <v>528</v>
       </c>
@@ -27672,7 +27696,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="460" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:21" ht="29.25">
       <c r="A460" s="2" t="s">
         <v>528</v>
       </c>
@@ -27737,7 +27761,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="461" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:21" ht="29.25">
       <c r="A461" s="2" t="s">
         <v>528</v>
       </c>
@@ -27802,7 +27826,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="462" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:21" ht="29.25">
       <c r="A462" s="2" t="s">
         <v>528</v>
       </c>
@@ -27865,7 +27889,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="463" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:21" ht="29.25">
       <c r="A463" s="2" t="s">
         <v>528</v>
       </c>
@@ -27930,7 +27954,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="464" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:21" ht="29.25">
       <c r="A464" s="2" t="s">
         <v>528</v>
       </c>
@@ -27995,7 +28019,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="465" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:21" ht="29.25">
       <c r="A465" s="2" t="s">
         <v>528</v>
       </c>
@@ -28060,7 +28084,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="466" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:21" ht="29.25">
       <c r="A466" s="2" t="s">
         <v>528</v>
       </c>
@@ -28125,7 +28149,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="467" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:21" ht="48.75">
       <c r="A467" s="2" t="s">
         <v>528</v>
       </c>
@@ -28190,7 +28214,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="468" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:21" ht="29.25">
       <c r="A468" s="2" t="s">
         <v>528</v>
       </c>
@@ -28255,7 +28279,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="469" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:21" ht="39">
       <c r="A469" s="2" t="s">
         <v>528</v>
       </c>
@@ -28320,7 +28344,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="470" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:21" ht="39">
       <c r="A470" s="2" t="s">
         <v>528</v>
       </c>
@@ -28385,7 +28409,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="471" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:21" ht="29.25">
       <c r="A471" s="2" t="s">
         <v>528</v>
       </c>
@@ -28436,7 +28460,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="472" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:21" ht="29.25">
       <c r="A472" s="2" t="s">
         <v>528</v>
       </c>
@@ -28501,7 +28525,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="473" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:21" ht="29.25">
       <c r="A473" s="2" t="s">
         <v>528</v>
       </c>
@@ -28566,7 +28590,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="474" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:21" ht="29.25">
       <c r="A474" s="2" t="s">
         <v>528</v>
       </c>
@@ -28625,7 +28649,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="475" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:21" ht="39">
       <c r="A475" s="2" t="s">
         <v>528</v>
       </c>
@@ -28664,7 +28688,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="476" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:21" ht="39">
       <c r="A476" s="2" t="s">
         <v>528</v>
       </c>
@@ -28729,7 +28753,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="477" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:21" ht="39">
       <c r="A477" s="2" t="s">
         <v>528</v>
       </c>
@@ -28794,8 +28818,8 @@
         <v>563</v>
       </c>
     </row>
-    <row r="478" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:21" ht="18" customHeight="1"/>
+    <row r="479" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A479" s="12" t="s">
         <v>566</v>
       </c>
@@ -28812,7 +28836,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="70" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="71" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okno 02.12.2025 - aktualizacja EXCEL
</commit_message>
<xml_diff>
--- a/assets/excel/en/global_sdg_indicators.xlsx
+++ b/assets/excel/en/global_sdg_indicators.xlsx
@@ -1723,7 +1723,7 @@
     <t>100% deaths registration</t>
   </si>
   <si>
-    <t>Last update: 09-09-2025, 14:17</t>
+    <t>Last update: 03-12-2025, 09:18</t>
   </si>
 </sst>
 </file>
@@ -2274,7 +2274,7 @@
   <dimension ref="A1:U479"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -3279,7 +3279,9 @@
       <c r="R18" s="4">
         <v>79.900000000000006</v>
       </c>
-      <c r="S18" s="3"/>
+      <c r="S18" s="4">
+        <v>80.400000000000006</v>
+      </c>
       <c r="T18" s="3"/>
       <c r="U18" s="2" t="s">
         <v>45</v>
@@ -3338,7 +3340,9 @@
       <c r="R19" s="4">
         <v>90.3</v>
       </c>
-      <c r="S19" s="3"/>
+      <c r="S19" s="4">
+        <v>90.6</v>
+      </c>
       <c r="T19" s="3"/>
       <c r="U19" s="2" t="s">
         <v>45</v>
@@ -3397,7 +3401,9 @@
       <c r="R20" s="4">
         <v>74.5</v>
       </c>
-      <c r="S20" s="3"/>
+      <c r="S20" s="4">
+        <v>75</v>
+      </c>
       <c r="T20" s="3"/>
       <c r="U20" s="2" t="s">
         <v>45</v>
@@ -3520,7 +3526,9 @@
       <c r="S22" s="5">
         <v>2.36</v>
       </c>
-      <c r="T22" s="3"/>
+      <c r="T22" s="5">
+        <v>2.73</v>
+      </c>
       <c r="U22" s="2" t="s">
         <v>50</v>
       </c>
@@ -3583,7 +3591,9 @@
       <c r="S23" s="5">
         <v>0.63</v>
       </c>
-      <c r="T23" s="3"/>
+      <c r="T23" s="5">
+        <v>0.55000000000000004</v>
+      </c>
       <c r="U23" s="2" t="s">
         <v>50</v>
       </c>
@@ -3860,7 +3870,9 @@
       <c r="S28" s="8">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="T28" s="3"/>
+      <c r="T28" s="8">
+        <v>7.9999999999999996E-6</v>
+      </c>
       <c r="U28" s="2" t="s">
         <v>62</v>
       </c>
@@ -6747,7 +6759,9 @@
       <c r="S75" s="4">
         <v>10</v>
       </c>
-      <c r="T75" s="3"/>
+      <c r="T75" s="4">
+        <v>9.8000000000000007</v>
+      </c>
       <c r="U75" s="2" t="s">
         <v>27</v>
       </c>
@@ -12695,7 +12709,9 @@
       <c r="S199" s="4">
         <v>92.6</v>
       </c>
-      <c r="T199" s="3"/>
+      <c r="T199" s="4">
+        <v>92.7</v>
+      </c>
       <c r="U199" s="2" t="s">
         <v>27</v>
       </c>
@@ -12758,7 +12774,9 @@
       <c r="S200" s="4">
         <v>72.599999999999994</v>
       </c>
-      <c r="T200" s="3"/>
+      <c r="T200" s="4">
+        <v>72.900000000000006</v>
+      </c>
       <c r="U200" s="2" t="s">
         <v>27</v>
       </c>
@@ -12821,7 +12839,9 @@
       <c r="S201" s="5">
         <v>78.11</v>
       </c>
-      <c r="T201" s="3"/>
+      <c r="T201" s="5">
+        <v>78.599999999999994</v>
+      </c>
       <c r="U201" s="2" t="s">
         <v>27</v>
       </c>
@@ -13135,7 +13155,9 @@
       <c r="S207" s="6">
         <v>152964</v>
       </c>
-      <c r="T207" s="3"/>
+      <c r="T207" s="6">
+        <v>152964</v>
+      </c>
       <c r="U207" s="2" t="s">
         <v>265</v>
       </c>
@@ -13257,7 +13279,9 @@
       <c r="S209" s="6">
         <v>100</v>
       </c>
-      <c r="T209" s="3"/>
+      <c r="T209" s="6">
+        <v>100</v>
+      </c>
       <c r="U209" s="2" t="s">
         <v>27</v>
       </c>
@@ -13599,9 +13623,11 @@
         <v>9.6</v>
       </c>
       <c r="S215" s="4">
-        <v>11</v>
-      </c>
-      <c r="T215" s="3"/>
+        <v>10.8</v>
+      </c>
+      <c r="T215" s="4">
+        <v>14</v>
+      </c>
       <c r="U215" s="2" t="s">
         <v>27</v>
       </c>
@@ -13755,7 +13781,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="G219" s="5">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
       <c r="H219" s="5">
         <v>0.57999999999999996</v>
@@ -13764,36 +13790,38 @@
         <v>0.61</v>
       </c>
       <c r="J219" s="5">
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
       <c r="K219" s="5">
         <v>0.69</v>
       </c>
       <c r="L219" s="5">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="M219" s="5">
-        <v>0.68</v>
+        <v>0.69</v>
       </c>
       <c r="N219" s="5">
-        <v>0.71</v>
+        <v>0.72</v>
       </c>
       <c r="O219" s="5">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
       <c r="P219" s="5">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
       <c r="Q219" s="5">
-        <v>0.85</v>
+        <v>0.86</v>
       </c>
       <c r="R219" s="5">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="S219" s="5">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="T219" s="3"/>
+        <v>1.18</v>
+      </c>
+      <c r="T219" s="5">
+        <v>1.38</v>
+      </c>
       <c r="U219" s="2" t="s">
         <v>271</v>
       </c>
@@ -13845,18 +13873,20 @@
         <v>667673.9</v>
       </c>
       <c r="P220" s="4">
-        <v>659543.30000000005</v>
+        <v>659532.30000000005</v>
       </c>
       <c r="Q220" s="4">
-        <v>674961.3</v>
+        <v>674950.4</v>
       </c>
       <c r="R220" s="4">
-        <v>674136.7</v>
+        <v>674125.7</v>
       </c>
       <c r="S220" s="4">
-        <v>661399.69999999995</v>
-      </c>
-      <c r="T220" s="3"/>
+        <v>635992.6</v>
+      </c>
+      <c r="T220" s="4">
+        <v>610837.9</v>
+      </c>
       <c r="U220" s="2" t="s">
         <v>271</v>
       </c>
@@ -13908,7 +13938,7 @@
         <v>17.59</v>
       </c>
       <c r="P221" s="5">
-        <v>17.399999999999999</v>
+        <v>17.579999999999998</v>
       </c>
       <c r="Q221" s="5">
         <v>18.25</v>
@@ -13917,9 +13947,11 @@
         <v>18.309999999999999</v>
       </c>
       <c r="S221" s="5">
-        <v>18.03</v>
-      </c>
-      <c r="T221" s="3"/>
+        <v>17.34</v>
+      </c>
+      <c r="T221" s="5">
+        <v>16.68</v>
+      </c>
       <c r="U221" s="2" t="s">
         <v>271</v>
       </c>
@@ -15818,7 +15850,9 @@
       <c r="S256" s="5">
         <v>0.03</v>
       </c>
-      <c r="T256" s="3"/>
+      <c r="T256" s="5">
+        <v>0.1</v>
+      </c>
       <c r="U256" s="2" t="s">
         <v>27</v>
       </c>
@@ -16289,7 +16323,9 @@
       <c r="S267" s="6">
         <v>373745</v>
       </c>
-      <c r="T267" s="3"/>
+      <c r="T267" s="6">
+        <v>406614</v>
+      </c>
       <c r="U267" s="2" t="s">
         <v>27</v>
       </c>
@@ -16352,7 +16388,9 @@
       <c r="S268" s="6">
         <v>256935</v>
       </c>
-      <c r="T268" s="3"/>
+      <c r="T268" s="6">
+        <v>272753</v>
+      </c>
       <c r="U268" s="2" t="s">
         <v>27</v>
       </c>
@@ -16415,7 +16453,9 @@
       <c r="S269" s="6">
         <v>722</v>
       </c>
-      <c r="T269" s="3"/>
+      <c r="T269" s="6">
+        <v>664</v>
+      </c>
       <c r="U269" s="2" t="s">
         <v>27</v>
       </c>
@@ -16478,7 +16518,9 @@
       <c r="S270" s="6">
         <v>1128</v>
       </c>
-      <c r="T270" s="3"/>
+      <c r="T270" s="6">
+        <v>1097</v>
+      </c>
       <c r="U270" s="2" t="s">
         <v>27</v>
       </c>
@@ -16541,7 +16583,9 @@
       <c r="S271" s="6">
         <v>16257</v>
       </c>
-      <c r="T271" s="3"/>
+      <c r="T271" s="6">
+        <v>17375</v>
+      </c>
       <c r="U271" s="2" t="s">
         <v>27</v>
       </c>
@@ -16604,7 +16648,9 @@
       <c r="S272" s="6">
         <v>229935</v>
       </c>
-      <c r="T272" s="3"/>
+      <c r="T272" s="6">
+        <v>222028</v>
+      </c>
       <c r="U272" s="2" t="s">
         <v>27</v>
       </c>
@@ -16667,7 +16713,9 @@
       <c r="S273" s="6">
         <v>1942800</v>
       </c>
-      <c r="T273" s="3"/>
+      <c r="T273" s="6">
+        <v>1861777</v>
+      </c>
       <c r="U273" s="2" t="s">
         <v>27</v>
       </c>
@@ -16730,7 +16778,9 @@
       <c r="S274" s="6">
         <v>44433</v>
       </c>
-      <c r="T274" s="3"/>
+      <c r="T274" s="6">
+        <v>46217</v>
+      </c>
       <c r="U274" s="2" t="s">
         <v>27</v>
       </c>
@@ -16793,7 +16843,9 @@
       <c r="S275" s="6">
         <v>7363</v>
       </c>
-      <c r="T275" s="3"/>
+      <c r="T275" s="6">
+        <v>6684</v>
+      </c>
       <c r="U275" s="2" t="s">
         <v>27</v>
       </c>
@@ -16856,7 +16908,9 @@
       <c r="S276" s="6">
         <v>1689</v>
       </c>
-      <c r="T276" s="3"/>
+      <c r="T276" s="6">
+        <v>1674</v>
+      </c>
       <c r="U276" s="2" t="s">
         <v>27</v>
       </c>
@@ -16919,7 +16973,9 @@
       <c r="S277" s="6">
         <v>89</v>
       </c>
-      <c r="T277" s="3"/>
+      <c r="T277" s="6">
+        <v>93</v>
+      </c>
       <c r="U277" s="2" t="s">
         <v>27</v>
       </c>
@@ -16983,7 +17039,7 @@
         <v>17.5</v>
       </c>
       <c r="T278" s="4">
-        <v>15.4</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="U278" s="2" t="s">
         <v>27</v>
@@ -18078,7 +18134,9 @@
       <c r="S296" s="4">
         <v>14</v>
       </c>
-      <c r="T296" s="3"/>
+      <c r="T296" s="4">
+        <v>13.8</v>
+      </c>
       <c r="U296" s="2" t="s">
         <v>27</v>
       </c>
@@ -18141,7 +18199,9 @@
       <c r="S297" s="4">
         <v>13.5</v>
       </c>
-      <c r="T297" s="3"/>
+      <c r="T297" s="4">
+        <v>13.3</v>
+      </c>
       <c r="U297" s="2" t="s">
         <v>27</v>
       </c>
@@ -18204,7 +18264,9 @@
       <c r="S298" s="4">
         <v>14.5</v>
       </c>
-      <c r="T298" s="3"/>
+      <c r="T298" s="4">
+        <v>14.3</v>
+      </c>
       <c r="U298" s="2" t="s">
         <v>27</v>
       </c>
@@ -18267,7 +18329,9 @@
       <c r="S299" s="4">
         <v>12.9</v>
       </c>
-      <c r="T299" s="3"/>
+      <c r="T299" s="4">
+        <v>12.6</v>
+      </c>
       <c r="U299" s="2" t="s">
         <v>27</v>
       </c>
@@ -18330,7 +18394,9 @@
       <c r="S300" s="4">
         <v>14.1</v>
       </c>
-      <c r="T300" s="3"/>
+      <c r="T300" s="4">
+        <v>13.6</v>
+      </c>
       <c r="U300" s="2" t="s">
         <v>27</v>
       </c>
@@ -18393,7 +18459,9 @@
       <c r="S301" s="4">
         <v>17.600000000000001</v>
       </c>
-      <c r="T301" s="3"/>
+      <c r="T301" s="4">
+        <v>19.2</v>
+      </c>
       <c r="U301" s="2" t="s">
         <v>27</v>
       </c>
@@ -18456,7 +18524,9 @@
       <c r="S302" s="4">
         <v>13.2</v>
       </c>
-      <c r="T302" s="3"/>
+      <c r="T302" s="4">
+        <v>13.4</v>
+      </c>
       <c r="U302" s="2" t="s">
         <v>27</v>
       </c>
@@ -18519,7 +18589,9 @@
       <c r="S303" s="4">
         <v>16.2</v>
       </c>
-      <c r="T303" s="3"/>
+      <c r="T303" s="4">
+        <v>15.1</v>
+      </c>
       <c r="U303" s="2" t="s">
         <v>27</v>
       </c>
@@ -18582,7 +18654,9 @@
       <c r="S304" s="4">
         <v>16.5</v>
       </c>
-      <c r="T304" s="3"/>
+      <c r="T304" s="4">
+        <v>15.2</v>
+      </c>
       <c r="U304" s="2" t="s">
         <v>27</v>
       </c>
@@ -18749,7 +18823,9 @@
       <c r="S307" s="4">
         <v>20.399999999999999</v>
       </c>
-      <c r="T307" s="3"/>
+      <c r="T307" s="4">
+        <v>20.3</v>
+      </c>
       <c r="U307" s="2" t="s">
         <v>364</v>
       </c>
@@ -18812,7 +18888,9 @@
       <c r="S308" s="4">
         <v>-0.7</v>
       </c>
-      <c r="T308" s="3"/>
+      <c r="T308" s="4">
+        <v>-1</v>
+      </c>
       <c r="U308" s="2" t="s">
         <v>364</v>
       </c>
@@ -18875,7 +18953,9 @@
       <c r="S309" s="4">
         <v>18.7</v>
       </c>
-      <c r="T309" s="3"/>
+      <c r="T309" s="4">
+        <v>18.899999999999999</v>
+      </c>
       <c r="U309" s="2" t="s">
         <v>364</v>
       </c>
@@ -18938,7 +19018,9 @@
       <c r="S310" s="4">
         <v>4.9000000000000004</v>
       </c>
-      <c r="T310" s="3"/>
+      <c r="T310" s="4">
+        <v>4.2</v>
+      </c>
       <c r="U310" s="2" t="s">
         <v>364</v>
       </c>
@@ -19001,7 +19083,9 @@
       <c r="S311" s="4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="T311" s="3"/>
+      <c r="T311" s="4">
+        <v>1.8</v>
+      </c>
       <c r="U311" s="2" t="s">
         <v>364</v>
       </c>
@@ -19064,7 +19148,9 @@
       <c r="S312" s="4">
         <v>57.8</v>
       </c>
-      <c r="T312" s="3"/>
+      <c r="T312" s="4">
+        <v>57.2</v>
+      </c>
       <c r="U312" s="2" t="s">
         <v>364</v>
       </c>
@@ -19127,7 +19213,9 @@
       <c r="S313" s="4">
         <v>1.4</v>
       </c>
-      <c r="T313" s="3"/>
+      <c r="T313" s="4">
+        <v>1.7</v>
+      </c>
       <c r="U313" s="2" t="s">
         <v>364</v>
       </c>
@@ -19190,7 +19278,9 @@
       <c r="S314" s="4">
         <v>11.8</v>
       </c>
-      <c r="T314" s="3"/>
+      <c r="T314" s="4">
+        <v>14.7</v>
+      </c>
       <c r="U314" s="2" t="s">
         <v>364</v>
       </c>
@@ -19253,7 +19343,9 @@
       <c r="S315" s="4">
         <v>70.099999999999994</v>
       </c>
-      <c r="T315" s="3"/>
+      <c r="T315" s="4">
+        <v>72.099999999999994</v>
+      </c>
       <c r="U315" s="2" t="s">
         <v>364</v>
       </c>
@@ -19316,7 +19408,9 @@
       <c r="S316" s="4">
         <v>57.3</v>
       </c>
-      <c r="T316" s="3"/>
+      <c r="T316" s="4">
+        <v>49.8</v>
+      </c>
       <c r="U316" s="2" t="s">
         <v>364</v>
       </c>
@@ -19379,7 +19473,9 @@
       <c r="S317" s="4">
         <v>27.6</v>
       </c>
-      <c r="T317" s="3"/>
+      <c r="T317" s="4">
+        <v>28</v>
+      </c>
       <c r="U317" s="2" t="s">
         <v>364</v>
       </c>
@@ -19442,7 +19538,9 @@
       <c r="S318" s="4">
         <v>45.5</v>
       </c>
-      <c r="T318" s="3"/>
+      <c r="T318" s="4">
+        <v>48</v>
+      </c>
       <c r="U318" s="2" t="s">
         <v>364</v>
       </c>
@@ -19960,7 +20058,9 @@
       <c r="S326" s="5">
         <v>8385.5</v>
       </c>
-      <c r="T326" s="3"/>
+      <c r="T326" s="5">
+        <v>3699.5</v>
+      </c>
       <c r="U326" s="2" t="s">
         <v>381</v>
       </c>
@@ -20023,7 +20123,9 @@
       <c r="S327" s="5">
         <v>6.2</v>
       </c>
-      <c r="T327" s="3"/>
+      <c r="T327" s="5">
+        <v>3.2</v>
+      </c>
       <c r="U327" s="2" t="s">
         <v>381</v>
       </c>
@@ -20086,7 +20188,9 @@
       <c r="S328" s="5">
         <v>0</v>
       </c>
-      <c r="T328" s="3"/>
+      <c r="T328" s="5">
+        <v>0</v>
+      </c>
       <c r="U328" s="2" t="s">
         <v>381</v>
       </c>
@@ -20149,7 +20253,9 @@
       <c r="S329" s="5">
         <v>321.5</v>
       </c>
-      <c r="T329" s="3"/>
+      <c r="T329" s="5">
+        <v>338.9</v>
+      </c>
       <c r="U329" s="2" t="s">
         <v>381</v>
       </c>
@@ -20212,7 +20318,9 @@
       <c r="S330" s="5">
         <v>128.19999999999999</v>
       </c>
-      <c r="T330" s="3"/>
+      <c r="T330" s="5">
+        <v>405.8</v>
+      </c>
       <c r="U330" s="2" t="s">
         <v>381</v>
       </c>
@@ -20452,7 +20560,9 @@
       <c r="S334" s="5">
         <v>2.36</v>
       </c>
-      <c r="T334" s="3"/>
+      <c r="T334" s="5">
+        <v>2.73</v>
+      </c>
       <c r="U334" s="2" t="s">
         <v>396</v>
       </c>
@@ -20515,7 +20625,9 @@
       <c r="S335" s="5">
         <v>0.63</v>
       </c>
-      <c r="T335" s="3"/>
+      <c r="T335" s="5">
+        <v>0.55000000000000004</v>
+      </c>
       <c r="U335" s="2" t="s">
         <v>396</v>
       </c>
@@ -20578,7 +20690,9 @@
       <c r="S336" s="5">
         <v>15.76</v>
       </c>
-      <c r="T336" s="3"/>
+      <c r="T336" s="5">
+        <v>18.34</v>
+      </c>
       <c r="U336" s="2" t="s">
         <v>27</v>
       </c>
@@ -20641,7 +20755,9 @@
       <c r="S337" s="5">
         <v>11.79</v>
       </c>
-      <c r="T337" s="3"/>
+      <c r="T337" s="5">
+        <v>12.81</v>
+      </c>
       <c r="U337" s="2" t="s">
         <v>27</v>
       </c>
@@ -20704,7 +20820,9 @@
       <c r="S338" s="5">
         <v>20.66</v>
       </c>
-      <c r="T338" s="3"/>
+      <c r="T338" s="5">
+        <v>21.92</v>
+      </c>
       <c r="U338" s="2" t="s">
         <v>27</v>
       </c>
@@ -20767,7 +20885,9 @@
       <c r="S339" s="5">
         <v>30.24</v>
       </c>
-      <c r="T339" s="3"/>
+      <c r="T339" s="5">
+        <v>30.07</v>
+      </c>
       <c r="U339" s="2" t="s">
         <v>27</v>
       </c>
@@ -20830,7 +20950,9 @@
       <c r="S340" s="4">
         <v>17.399999999999999</v>
       </c>
-      <c r="T340" s="3"/>
+      <c r="T340" s="4">
+        <v>19</v>
+      </c>
       <c r="U340" s="2" t="s">
         <v>254</v>
       </c>
@@ -20893,7 +21015,9 @@
       <c r="S341" s="4">
         <v>21.3</v>
       </c>
-      <c r="T341" s="3"/>
+      <c r="T341" s="4">
+        <v>20.7</v>
+      </c>
       <c r="U341" s="2" t="s">
         <v>254</v>
       </c>
@@ -20956,7 +21080,9 @@
       <c r="S342" s="4">
         <v>23.6</v>
       </c>
-      <c r="T342" s="3"/>
+      <c r="T342" s="4">
+        <v>27.6</v>
+      </c>
       <c r="U342" s="2" t="s">
         <v>254</v>
       </c>
@@ -21019,7 +21145,9 @@
       <c r="S343" s="4">
         <v>25.2</v>
       </c>
-      <c r="T343" s="3"/>
+      <c r="T343" s="4">
+        <v>26.4</v>
+      </c>
       <c r="U343" s="2" t="s">
         <v>254</v>
       </c>
@@ -21082,7 +21210,9 @@
       <c r="S344" s="4">
         <v>20.8</v>
       </c>
-      <c r="T344" s="3"/>
+      <c r="T344" s="4">
+        <v>22</v>
+      </c>
       <c r="U344" s="2" t="s">
         <v>254</v>
       </c>
@@ -21145,7 +21275,9 @@
       <c r="S345" s="4">
         <v>24.1</v>
       </c>
-      <c r="T345" s="3"/>
+      <c r="T345" s="4">
+        <v>24.8</v>
+      </c>
       <c r="U345" s="2" t="s">
         <v>254</v>
       </c>
@@ -21208,7 +21340,9 @@
       <c r="S346" s="4">
         <v>19.600000000000001</v>
       </c>
-      <c r="T346" s="3"/>
+      <c r="T346" s="4">
+        <v>21.4</v>
+      </c>
       <c r="U346" s="2" t="s">
         <v>254</v>
       </c>
@@ -21271,7 +21405,9 @@
       <c r="S347" s="4">
         <v>25.4</v>
       </c>
-      <c r="T347" s="3"/>
+      <c r="T347" s="4">
+        <v>27.5</v>
+      </c>
       <c r="U347" s="2" t="s">
         <v>254</v>
       </c>
@@ -21334,7 +21470,9 @@
       <c r="S348" s="4">
         <v>18.600000000000001</v>
       </c>
-      <c r="T348" s="3"/>
+      <c r="T348" s="4">
+        <v>19.600000000000001</v>
+      </c>
       <c r="U348" s="2" t="s">
         <v>254</v>
       </c>
@@ -21397,7 +21535,9 @@
       <c r="S349" s="4">
         <v>15.8</v>
       </c>
-      <c r="T349" s="3"/>
+      <c r="T349" s="4">
+        <v>17.3</v>
+      </c>
       <c r="U349" s="2" t="s">
         <v>254</v>
       </c>
@@ -21460,7 +21600,9 @@
       <c r="S350" s="4">
         <v>22.2</v>
       </c>
-      <c r="T350" s="3"/>
+      <c r="T350" s="4">
+        <v>23.1</v>
+      </c>
       <c r="U350" s="2" t="s">
         <v>254</v>
       </c>
@@ -21523,7 +21665,9 @@
       <c r="S351" s="4">
         <v>20.8</v>
       </c>
-      <c r="T351" s="3"/>
+      <c r="T351" s="4">
+        <v>23.4</v>
+      </c>
       <c r="U351" s="2" t="s">
         <v>254</v>
       </c>
@@ -21586,7 +21730,9 @@
       <c r="S352" s="4">
         <v>11.9</v>
       </c>
-      <c r="T352" s="3"/>
+      <c r="T352" s="4">
+        <v>12.8</v>
+      </c>
       <c r="U352" s="2" t="s">
         <v>254</v>
       </c>
@@ -21649,7 +21795,9 @@
       <c r="S353" s="4">
         <v>13.3</v>
       </c>
-      <c r="T353" s="3"/>
+      <c r="T353" s="4">
+        <v>13.4</v>
+      </c>
       <c r="U353" s="2" t="s">
         <v>254</v>
       </c>
@@ -21712,7 +21860,9 @@
       <c r="S354" s="4">
         <v>18.100000000000001</v>
       </c>
-      <c r="T354" s="3"/>
+      <c r="T354" s="4">
+        <v>20.3</v>
+      </c>
       <c r="U354" s="2" t="s">
         <v>254</v>
       </c>
@@ -21775,7 +21925,9 @@
       <c r="S355" s="4">
         <v>17.100000000000001</v>
       </c>
-      <c r="T355" s="3"/>
+      <c r="T355" s="4">
+        <v>17.5</v>
+      </c>
       <c r="U355" s="2" t="s">
         <v>254</v>
       </c>
@@ -21838,7 +21990,9 @@
       <c r="S356" s="4">
         <v>15</v>
       </c>
-      <c r="T356" s="3"/>
+      <c r="T356" s="4">
+        <v>15.5</v>
+      </c>
       <c r="U356" s="2" t="s">
         <v>254</v>
       </c>
@@ -21901,7 +22055,9 @@
       <c r="S357" s="4">
         <v>15</v>
       </c>
-      <c r="T357" s="3"/>
+      <c r="T357" s="4">
+        <v>15.8</v>
+      </c>
       <c r="U357" s="2" t="s">
         <v>254</v>
       </c>
@@ -21962,7 +22118,9 @@
       <c r="S358" s="4">
         <v>14.6</v>
       </c>
-      <c r="T358" s="3"/>
+      <c r="T358" s="4">
+        <v>15.8</v>
+      </c>
       <c r="U358" s="2" t="s">
         <v>254</v>
       </c>
@@ -22025,7 +22183,9 @@
       <c r="S359" s="4">
         <v>19.100000000000001</v>
       </c>
-      <c r="T359" s="3"/>
+      <c r="T359" s="4">
+        <v>20.100000000000001</v>
+      </c>
       <c r="U359" s="2" t="s">
         <v>254</v>
       </c>
@@ -22088,7 +22248,9 @@
       <c r="S360" s="4">
         <v>12.6</v>
       </c>
-      <c r="T360" s="3"/>
+      <c r="T360" s="4">
+        <v>13.4</v>
+      </c>
       <c r="U360" s="2" t="s">
         <v>254</v>
       </c>
@@ -22151,7 +22313,9 @@
       <c r="S361" s="4">
         <v>11.5</v>
       </c>
-      <c r="T361" s="3"/>
+      <c r="T361" s="4">
+        <v>13.2</v>
+      </c>
       <c r="U361" s="2" t="s">
         <v>254</v>
       </c>
@@ -22214,7 +22378,9 @@
       <c r="S362" s="4">
         <v>15.4</v>
       </c>
-      <c r="T362" s="3"/>
+      <c r="T362" s="4">
+        <v>14.7</v>
+      </c>
       <c r="U362" s="2" t="s">
         <v>254</v>
       </c>
@@ -22277,7 +22443,9 @@
       <c r="S363" s="4">
         <v>14.8</v>
       </c>
-      <c r="T363" s="3"/>
+      <c r="T363" s="4">
+        <v>15.5</v>
+      </c>
       <c r="U363" s="2" t="s">
         <v>254</v>
       </c>
@@ -22340,7 +22508,9 @@
       <c r="S364" s="5">
         <v>98.68</v>
       </c>
-      <c r="T364" s="3"/>
+      <c r="T364" s="5">
+        <v>98.72</v>
+      </c>
       <c r="U364" s="2" t="s">
         <v>421</v>
       </c>
@@ -22403,7 +22573,9 @@
       <c r="S365" s="5">
         <v>100</v>
       </c>
-      <c r="T365" s="3"/>
+      <c r="T365" s="5">
+        <v>100</v>
+      </c>
       <c r="U365" s="2" t="s">
         <v>421</v>
       </c>
@@ -22466,7 +22638,9 @@
       <c r="S366" s="5">
         <v>95.85</v>
       </c>
-      <c r="T366" s="3"/>
+      <c r="T366" s="5">
+        <v>96.13</v>
+      </c>
       <c r="U366" s="2" t="s">
         <v>421</v>
       </c>
@@ -22529,7 +22703,9 @@
       <c r="S367" s="5">
         <v>99.38</v>
       </c>
-      <c r="T367" s="3"/>
+      <c r="T367" s="5">
+        <v>99.18</v>
+      </c>
       <c r="U367" s="2" t="s">
         <v>421</v>
       </c>
@@ -22592,7 +22768,9 @@
       <c r="S368" s="4">
         <v>100</v>
       </c>
-      <c r="T368" s="3"/>
+      <c r="T368" s="4">
+        <v>99.8</v>
+      </c>
       <c r="U368" s="2" t="s">
         <v>421</v>
       </c>
@@ -22655,7 +22833,9 @@
       <c r="S369" s="4">
         <v>100</v>
       </c>
-      <c r="T369" s="3"/>
+      <c r="T369" s="4">
+        <v>99.8</v>
+      </c>
       <c r="U369" s="2" t="s">
         <v>421</v>
       </c>
@@ -22718,7 +22898,9 @@
       <c r="S370" s="4">
         <v>99.9</v>
       </c>
-      <c r="T370" s="3"/>
+      <c r="T370" s="4">
+        <v>99.8</v>
+      </c>
       <c r="U370" s="2" t="s">
         <v>421</v>
       </c>
@@ -22781,7 +22963,9 @@
       <c r="S371" s="4">
         <v>100</v>
       </c>
-      <c r="T371" s="3"/>
+      <c r="T371" s="4">
+        <v>99.6</v>
+      </c>
       <c r="U371" s="2" t="s">
         <v>421</v>
       </c>
@@ -23026,7 +23210,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="G376" s="5">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
       <c r="H376" s="5">
         <v>0.57999999999999996</v>
@@ -23035,36 +23219,38 @@
         <v>0.61</v>
       </c>
       <c r="J376" s="5">
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
       <c r="K376" s="5">
         <v>0.69</v>
       </c>
       <c r="L376" s="5">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="M376" s="5">
-        <v>0.68</v>
+        <v>0.69</v>
       </c>
       <c r="N376" s="5">
-        <v>0.71</v>
+        <v>0.72</v>
       </c>
       <c r="O376" s="5">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
       <c r="P376" s="5">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
       <c r="Q376" s="5">
-        <v>0.85</v>
+        <v>0.86</v>
       </c>
       <c r="R376" s="5">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="S376" s="5">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="T376" s="3"/>
+        <v>1.18</v>
+      </c>
+      <c r="T376" s="5">
+        <v>1.38</v>
+      </c>
       <c r="U376" s="2" t="s">
         <v>271</v>
       </c>
@@ -23116,18 +23302,20 @@
         <v>667673.9</v>
       </c>
       <c r="P377" s="4">
-        <v>659543.30000000005</v>
+        <v>659532.30000000005</v>
       </c>
       <c r="Q377" s="4">
-        <v>674961.3</v>
+        <v>674950.4</v>
       </c>
       <c r="R377" s="4">
-        <v>674136.7</v>
+        <v>674125.7</v>
       </c>
       <c r="S377" s="4">
-        <v>661399.69999999995</v>
-      </c>
-      <c r="T377" s="3"/>
+        <v>635992.6</v>
+      </c>
+      <c r="T377" s="4">
+        <v>610837.9</v>
+      </c>
       <c r="U377" s="2" t="s">
         <v>271</v>
       </c>
@@ -23179,7 +23367,7 @@
         <v>17.59</v>
       </c>
       <c r="P378" s="5">
-        <v>17.399999999999999</v>
+        <v>17.579999999999998</v>
       </c>
       <c r="Q378" s="5">
         <v>18.25</v>
@@ -23188,9 +23376,11 @@
         <v>18.309999999999999</v>
       </c>
       <c r="S378" s="5">
-        <v>18.03</v>
-      </c>
-      <c r="T378" s="3"/>
+        <v>17.34</v>
+      </c>
+      <c r="T378" s="5">
+        <v>16.68</v>
+      </c>
       <c r="U378" s="2" t="s">
         <v>271</v>
       </c>
@@ -23253,7 +23443,9 @@
       <c r="S379" s="6">
         <v>1</v>
       </c>
-      <c r="T379" s="3"/>
+      <c r="T379" s="6">
+        <v>1</v>
+      </c>
       <c r="U379" s="2" t="s">
         <v>433</v>
       </c>
@@ -23499,8 +23691,12 @@
       <c r="R384" s="6">
         <v>151</v>
       </c>
-      <c r="S384" s="3"/>
-      <c r="T384" s="3"/>
+      <c r="S384" s="6">
+        <v>163</v>
+      </c>
+      <c r="T384" s="6">
+        <v>163</v>
+      </c>
       <c r="U384" s="2" t="s">
         <v>444</v>
       </c>
@@ -23693,7 +23889,9 @@
       <c r="S387" s="5">
         <v>2.36</v>
       </c>
-      <c r="T387" s="3"/>
+      <c r="T387" s="5">
+        <v>2.73</v>
+      </c>
       <c r="U387" s="2" t="s">
         <v>50</v>
       </c>
@@ -23756,7 +23954,9 @@
       <c r="S388" s="5">
         <v>0.63</v>
       </c>
-      <c r="T388" s="3"/>
+      <c r="T388" s="5">
+        <v>0.55000000000000004</v>
+      </c>
       <c r="U388" s="2" t="s">
         <v>50</v>
       </c>
@@ -24549,7 +24749,9 @@
       <c r="S401" s="5">
         <v>1.58</v>
       </c>
-      <c r="T401" s="3"/>
+      <c r="T401" s="5">
+        <v>1.58</v>
+      </c>
       <c r="U401" s="2" t="s">
         <v>469</v>
       </c>
@@ -24742,7 +24944,9 @@
       <c r="S404" s="7">
         <v>0.192</v>
       </c>
-      <c r="T404" s="3"/>
+      <c r="T404" s="7">
+        <v>0.192</v>
+      </c>
       <c r="U404" s="2" t="s">
         <v>474</v>
       </c>
@@ -25163,7 +25367,9 @@
       <c r="S413" s="6">
         <v>4169</v>
       </c>
-      <c r="T413" s="3"/>
+      <c r="T413" s="6">
+        <v>24104</v>
+      </c>
       <c r="U413" s="2" t="s">
         <v>486</v>
       </c>
@@ -25409,7 +25615,9 @@
       <c r="S417" s="6">
         <v>4169</v>
       </c>
-      <c r="T417" s="3"/>
+      <c r="T417" s="6">
+        <v>24104</v>
+      </c>
       <c r="U417" s="2" t="s">
         <v>486</v>
       </c>
@@ -26549,7 +26757,9 @@
       <c r="S437" s="6">
         <v>5189</v>
       </c>
-      <c r="T437" s="3"/>
+      <c r="T437" s="6">
+        <v>5356</v>
+      </c>
       <c r="U437" s="2" t="s">
         <v>515</v>
       </c>
@@ -27884,7 +28094,9 @@
       <c r="S462" s="4">
         <v>86.4</v>
       </c>
-      <c r="T462" s="3"/>
+      <c r="T462" s="4">
+        <v>88.6</v>
+      </c>
       <c r="U462" s="2" t="s">
         <v>27</v>
       </c>
@@ -28078,7 +28290,7 @@
         <v>90759</v>
       </c>
       <c r="T465" s="6">
-        <v>97120</v>
+        <v>97357</v>
       </c>
       <c r="U465" s="2" t="s">
         <v>27</v>
@@ -28143,7 +28355,7 @@
         <v>100.2</v>
       </c>
       <c r="T466" s="4">
-        <v>102.9</v>
+        <v>103</v>
       </c>
       <c r="U466" s="2" t="s">
         <v>27</v>
@@ -28273,7 +28485,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="T468" s="4">
-        <v>16.899999999999999</v>
+        <v>17</v>
       </c>
       <c r="U468" s="2" t="s">
         <v>27</v>
@@ -28338,7 +28550,7 @@
         <v>49.5</v>
       </c>
       <c r="T469" s="4">
-        <v>55.3</v>
+        <v>55.1</v>
       </c>
       <c r="U469" s="2" t="s">
         <v>27</v>
@@ -28400,10 +28612,10 @@
         <v>-3.4</v>
       </c>
       <c r="S470" s="4">
-        <v>-5.3</v>
+        <v>-5.2</v>
       </c>
       <c r="T470" s="4">
-        <v>-6.6</v>
+        <v>-6.5</v>
       </c>
       <c r="U470" s="2" t="s">
         <v>27</v>

</xml_diff>